<commit_message>
Thử in ra không- kiếp
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFA53E1-AD12-4CB3-A6DA-538399176D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435FE222-2708-41F3-9CA4-1F8A0401D82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4185" yWindow="4185" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>Tâm lý của bạn hay bị ảnh hưởng bên ngoài nhưng thực chất đó cũng chỉ là do bạn muốn tiếp thu ý kiến mọi người.</t>
+  </si>
+  <si>
+    <t>Mệnh Không Thân Kiếp</t>
+  </si>
+  <si>
+    <t>Bạn là người khôn ngoan, sắc sảo nên ông trời thử thách bạn với những hoàn cảnh trớ trêu.</t>
+  </si>
+  <si>
+    <t>Bạn cũng là tuýp người nhiệt tình 5 phút, cả thèm mau chán.</t>
   </si>
 </sst>
 </file>
@@ -357,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -384,6 +393,17 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tìm ra các thế luận: độc tọa tại cung sau đó hợp chiếu với các sao, đồng cung với sao khác tại cung sau đó hội hộp với các sao khác, độc tọa tại chi sau đó hội hộp với các sao khác, đồng chi với sao khác sau đó hợp với sao khác độc tọa tại cung tại chi
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A66159-3353-4D40-A0F5-DB061978670E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA6B99F-C1AC-465F-95ED-AE0014AE6C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -124,6 +124,15 @@
   </si>
   <si>
     <t>Bạn là người có bằng cấp, đỗ đạt cao.</t>
+  </si>
+  <si>
+    <t>Bạn là người can đảm, cương nghị, ương ngạch.</t>
+  </si>
+  <si>
+    <t>Mệnh Tý Ngọ có Thiên Khốc Thiên Hư đồng cung</t>
+  </si>
+  <si>
+    <t>Thiếu thời nghèo túng, trung niên khá giả, về già giàu có.</t>
   </si>
 </sst>
 </file>
@@ -441,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,6 +557,9 @@
       <c r="C11" t="s">
         <v>20</v>
       </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -584,6 +596,14 @@
       </c>
       <c r="B16" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Luận giải cách cục tử vi tại mệnh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1727A2EC-A4C0-4E23-9964-5F362B1D7BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D02B2C5-87A3-4AF3-BE43-01F621757749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="68">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -81,12 +81,6 @@
     <t>Bạn sẽ gặp nhiều may mắn</t>
   </si>
   <si>
-    <t>Tang Hổ</t>
-  </si>
-  <si>
-    <t>Bạch Hổ</t>
-  </si>
-  <si>
     <t>Bạn là người hay suy nghĩ lo lắng, tuy nhiên sự lo lắng của bạn là có cơ sở.</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
     <t>Linh Tinh</t>
   </si>
   <si>
-    <t>Hỏa Tinh</t>
-  </si>
-  <si>
     <t>Tính tình nóng giận</t>
   </si>
   <si>
@@ -148,6 +139,96 @@
   </si>
   <si>
     <t>Tính tình nóng giận, liều lĩnh, bướng</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh hội chiếu tại mệnh</t>
+  </si>
+  <si>
+    <t>Sát Phá Tham hội chiếu tại mệnh</t>
+  </si>
+  <si>
+    <t>Tang Hổ hội chiếu tại Mệnh</t>
+  </si>
+  <si>
+    <t>Bạch Hổ tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Tỵ, Ngọ, Dần, Thân</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Thìn, Tuất</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Sửu, Mùi</t>
+  </si>
+  <si>
+    <t>Bạn là người Thông minh, trung hậu.</t>
+  </si>
+  <si>
+    <t>Bạn là người đa mưu, túc trí nhưng vì cái lợi bản thân là phần nhiều.</t>
+  </si>
+  <si>
+    <t>Bạn là người thông minh, mưu lược, nhưng có phần liều lĩnh.</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Tý, Hợi, Mão, Dậu</t>
+  </si>
+  <si>
+    <t>Bạn hơi kém thông minh, nhưng bản tính đôn hậu.</t>
+  </si>
+  <si>
+    <t>Quyền uy kém rực rỡ, khả năng tiêu giảm tai ách bị giảm nhiều.</t>
+  </si>
+  <si>
+    <t>Bạn là người có uy quyền khiến người khác nể trọng và giúp đỡ. Bản thân ra ngoài gặp nhiều may mắn.</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh và hội chiếu các sao Thiên Tướng, Văn Khúc, Văn Xương, Thiên Khôi, Thiên Việt, Tả Phù, Hữu Bật</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh và hội chiếu Thiên Phủ</t>
+  </si>
+  <si>
+    <t>Bạn có nhiều tiền bạc, của cải.</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh và gặp Thiên Mã, Lộc Tồn</t>
+  </si>
+  <si>
+    <t>Độ số quyền lực của bạn được tăng thêm.</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Thất Sát</t>
+  </si>
+  <si>
+    <t>Độ số quyền lực của bạn là tuyệt đối.</t>
+  </si>
+  <si>
+    <t>Chế ác được sự tác họa của Hỏa Linh</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh và gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh và gặp Địa Không, Địa Kiếp</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh gặp Kình Dương hoặc Đà La hoặc Địa Không hoặc Địa Kiếp</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh và gặp Kình Dương, Đà La, Địa Không, Địa Kiếp</t>
+  </si>
+  <si>
+    <t>Bạn như vị vua bị vây hãm không lối thoát.</t>
+  </si>
+  <si>
+    <t>Bạn như vị vua bị vây hãm.</t>
+  </si>
+  <si>
+    <t>Bạn như vị vua bị vậy hãm.</t>
+  </si>
+  <si>
+    <t>Bị tiểu nhân làm hại.</t>
   </si>
 </sst>
 </file>
@@ -163,12 +244,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -183,8 +270,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,15 +553,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -516,7 +604,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -553,98 +641,212 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="B19" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>40</v>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Luận hoàn thiện cách cục tử vi tại mệnh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D02B2C5-87A3-4AF3-BE43-01F621757749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40F52F3-83A1-4225-BD2B-6934D8808721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="79">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -153,15 +153,6 @@
     <t>Bạch Hổ tọa thủ tại Mệnh</t>
   </si>
   <si>
-    <t>Tử Vi tọa thủ cung Mệnh ở Tỵ, Ngọ, Dần, Thân</t>
-  </si>
-  <si>
-    <t>Tử Vi tọa thủ cung Mệnh ở Thìn, Tuất</t>
-  </si>
-  <si>
-    <t>Tử Vi tọa thủ cung Mệnh ở Sửu, Mùi</t>
-  </si>
-  <si>
     <t>Bạn là người Thông minh, trung hậu.</t>
   </si>
   <si>
@@ -171,9 +162,6 @@
     <t>Bạn là người thông minh, mưu lược, nhưng có phần liều lĩnh.</t>
   </si>
   <si>
-    <t>Tử Vi tọa thủ cung Mệnh ở Tý, Hợi, Mão, Dậu</t>
-  </si>
-  <si>
     <t>Bạn hơi kém thông minh, nhưng bản tính đôn hậu.</t>
   </si>
   <si>
@@ -213,9 +201,6 @@
     <t>Tử Vi tọa thủ cung Mệnh và gặp Địa Không, Địa Kiếp</t>
   </si>
   <si>
-    <t>Tử Vi tọa thủ cung Mệnh gặp Kình Dương hoặc Đà La hoặc Địa Không hoặc Địa Kiếp</t>
-  </si>
-  <si>
     <t>Tử Vi tọa thủ cung Mệnh và gặp Kình Dương, Đà La, Địa Không, Địa Kiếp</t>
   </si>
   <si>
@@ -229,6 +214,54 @@
   </si>
   <si>
     <t>Bị tiểu nhân làm hại.</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh gặp Kình Dương</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh gặp Đà La</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh gặp Địa Không</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh gặp Địa Kiếp</t>
   </si>
 </sst>
 </file>
@@ -553,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,23 +770,23 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
         <v>42</v>
-      </c>
-      <c r="B22" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B23" t="s">
         <v>43</v>
-      </c>
-      <c r="B23" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
         <v>47</v>
@@ -761,21 +794,18 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
         <v>52</v>
-      </c>
-      <c r="B26" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -785,13 +815,19 @@
       <c r="B27" t="s">
         <v>54</v>
       </c>
+      <c r="C27" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>56</v>
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -799,54 +835,157 @@
         <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B33" t="s">
-        <v>64</v>
-      </c>
-      <c r="C33" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Luận Mệnh các cách cục khác
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40F52F3-83A1-4225-BD2B-6934D8808721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B155230D-23B5-4CC0-9BDA-8CE0EF60D349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -262,6 +262,42 @@
   </si>
   <si>
     <t>Tử Vi tọa thủ cung Mệnh gặp Địa Kiếp</t>
+  </si>
+  <si>
+    <t>Anh sinh năm Mùi, Mệnh an tại Sửu</t>
+  </si>
+  <si>
+    <t>Anh sinh năm Ngọ, Mệnh an tại Sửu</t>
+  </si>
+  <si>
+    <t>Anh sinh năm Mùi, Mệnh an tại Tý</t>
+  </si>
+  <si>
+    <t>Anh sinh năm Ngọ, Mệnh an tại Tý</t>
+  </si>
+  <si>
+    <t>Cuộc đời vất vả,ít có điều xứng ý toại lòng.</t>
+  </si>
+  <si>
+    <t>Cung Mệnh của chị được an tại ví trí Tứ Mộ</t>
+  </si>
+  <si>
+    <t>Chị là một người khôn ngoan, đảm đang.</t>
+  </si>
+  <si>
+    <t>Cung Mệnh của chị được an tại ví trí cung Dậu</t>
+  </si>
+  <si>
+    <t>Chị đi ra ngoài được rất nhiều người  yêu mến và tôn trọng.</t>
+  </si>
+  <si>
+    <t>Cung Mệnh của chị được an tại ví trí cung Ngọ</t>
+  </si>
+  <si>
+    <t>Cung Mệnh của chị được an tại ví trí cung Tý</t>
+  </si>
+  <si>
+    <t>Cuộc đời chị an nhàn.</t>
   </si>
 </sst>
 </file>
@@ -586,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,6 +1024,70 @@
         <v>62</v>
       </c>
     </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B48" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B49" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Luận Cung Mệnh Vô chính Diệu, Thân Mệnh đồng cung
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B155230D-23B5-4CC0-9BDA-8CE0EF60D349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2A95CD-0944-4AA5-A463-EA0D6F61E57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="93">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -297,7 +297,13 @@
     <t>Cung Mệnh của chị được an tại ví trí cung Tý</t>
   </si>
   <si>
-    <t>Cuộc đời chị an nhàn.</t>
+    <t>Thân và Mệnh đồng cung Vô Chính Diệu</t>
+  </si>
+  <si>
+    <t>Cuộc đời cực kỳ vất vả, khổ cực. Không cậy nhờ được sự giúp đỡ của người khác, tự thân lập nghiệp.</t>
+  </si>
+  <si>
+    <t>Độ số an nhàn gia tăng.</t>
   </si>
 </sst>
 </file>
@@ -622,10 +628,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1083,7 @@
         <v>88</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -1085,7 +1091,15 @@
         <v>89</v>
       </c>
       <c r="B52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>90</v>
+      </c>
+      <c r="B53" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add thêm tứ chiếu, tam hợp, nhị hợp)
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2A95CD-0944-4AA5-A463-EA0D6F61E57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF882FF9-B2FC-434E-A021-C9B2C6752722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="102">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Tham Hỏa Linh</t>
   </si>
   <si>
-    <t>Cơ Nguyệt Đồng Lương</t>
-  </si>
-  <si>
     <t>Bạn là tuýp người nhẹ nhàng, có nội tâm sâu sắc, phù hợp với môi trường giáo dục, công việc cần chuyên lý thuyết và tư duy cao.</t>
   </si>
   <si>
@@ -304,6 +301,36 @@
   </si>
   <si>
     <t>Độ số an nhàn gia tăng.</t>
+  </si>
+  <si>
+    <t>Thân và Mệnh đồng cung Vô Chính Diệu tại Thìn</t>
+  </si>
+  <si>
+    <t>Thân và Mệnh đồng cung Vô Chính Diệu tại Tuất</t>
+  </si>
+  <si>
+    <t>Thân và Mệnh đồng cung Vô Chính Diệu tại Sửu</t>
+  </si>
+  <si>
+    <t>Thân và Mệnh đồng cung Vô Chính Diệu tại Mùi</t>
+  </si>
+  <si>
+    <t>Thọ mạng kém.</t>
+  </si>
+  <si>
+    <t>Độ số hậu vận an nhàn gia tăng.</t>
+  </si>
+  <si>
+    <t>Tuy ít có cơ hội học tập nhưng vẫn lập được sự nghiệp vẻ vang.</t>
+  </si>
+  <si>
+    <t>Cơ Nguyệt Đồng Lương hội chiếu tại Mệnh</t>
+  </si>
+  <si>
+    <t>Song Hao hội chiếu tại Mệnh</t>
+  </si>
+  <si>
+    <t>Cự Nhật hội chiếu tại Mệnh</t>
   </si>
 </sst>
 </file>
@@ -628,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +706,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
@@ -700,409 +727,473 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
-        <v>15</v>
+      <c r="C8" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
         <v>27</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
         <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
         <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
         <v>36</v>
-      </c>
-      <c r="B21" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
         <v>49</v>
-      </c>
-      <c r="B25" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
         <v>51</v>
-      </c>
-      <c r="B26" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
         <v>53</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>54</v>
-      </c>
-      <c r="C27" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
         <v>61</v>
-      </c>
-      <c r="C28" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
         <v>58</v>
       </c>
-      <c r="B30" t="s">
-        <v>59</v>
-      </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" t="s">
         <v>45</v>
-      </c>
-      <c r="C37" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B38" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" t="s">
         <v>45</v>
-      </c>
-      <c r="C38" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" t="s">
         <v>45</v>
-      </c>
-      <c r="C39" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" t="s">
         <v>45</v>
-      </c>
-      <c r="C40" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" t="s">
         <v>82</v>
       </c>
-      <c r="B48" t="s">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="B49" t="s">
         <v>84</v>
       </c>
-      <c r="B49" t="s">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="B50" t="s">
         <v>86</v>
       </c>
-      <c r="B50" t="s">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="B51" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B53" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B52" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="B54" t="s">
         <v>90</v>
       </c>
-      <c r="B53" t="s">
-        <v>91</v>
+      <c r="C54" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B56" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B57" t="s">
+        <v>90</v>
+      </c>
+      <c r="C57" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B58" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Hiển thị sao chính, sao phụ, các cách cục
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF882FF9-B2FC-434E-A021-C9B2C6752722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF34BD9-D87B-4A01-9D84-04967CC3CC7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="104">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -331,6 +331,12 @@
   </si>
   <si>
     <t>Cự Nhật hội chiếu tại Mệnh</t>
+  </si>
+  <si>
+    <t>Không Kiếp</t>
+  </si>
+  <si>
+    <t>Không Kiếp hội chiếu tại Mệnh</t>
   </si>
 </sst>
 </file>
@@ -655,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,6 +1198,14 @@
         <v>101</v>
       </c>
     </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Hiển thị cách cục tử vi ở Mệnh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D84983-1727-4A10-B155-CF8563654046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E095547-1521-47C8-94E1-D083888464E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="131">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -403,6 +403,21 @@
   </si>
   <si>
     <t>Bạn có duyên tu hành và từ đó có cuộc sống tốt hơn</t>
+  </si>
+  <si>
+    <t>Sinh năm Giáp có Tử Vi tọa thủ cung Mệnh ở Ngọ và không gặp Thiên Hình, Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Sinh năm Đinh có Tử Vi tọa thủ cung Mệnh ở Ngọ và không gặp Thiên Hình, Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Sinh năm Kỷ có Tử Vi tọa thủ cung Mệnh ở Ngọ và không gặp Thiên Hình, Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Nam mệnh sinh năm Nhâm có Tử Vi tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Nam mệnh sinh năm Giáp có Tử Vi tọa thủ cung Mệnh ở Hợi</t>
   </si>
 </sst>
 </file>
@@ -727,10 +742,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E68"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,6 +1378,46 @@
         <v>125</v>
       </c>
     </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Hoàn thiện luận giải sao tử Vi tại Mệnh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E095547-1521-47C8-94E1-D083888464E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7A8A8A-B512-464D-9319-0C3174A22BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="158">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -418,6 +418,87 @@
   </si>
   <si>
     <t>Nam mệnh sinh năm Giáp có Tử Vi tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Sinh năm Giáp có Tử Vi đồng cung Thiên Phủ tại Dần</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Thiên Phủ tại Dần</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Thiên Phủ tại Thân</t>
+  </si>
+  <si>
+    <t>Sinh năm Giáp có Tử Vi đồng cung Thiên Phủ tại Thân</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh và hội chiếu Thiên Phủ gặp Tả Phù, Hữu Bật</t>
+  </si>
+  <si>
+    <t>Được hưởng phú quý trọn đời.</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh và hội chiếu Thiên Phủ có Kình Dương đồng cung</t>
+  </si>
+  <si>
+    <t>Kinh doanh buôn bán đại phú.</t>
+  </si>
+  <si>
+    <t>ử Phủ Vũ Tướng Tả Hữu Khoa Quyền Lộc Long Phượng</t>
+  </si>
+  <si>
+    <t>Hưởng đại phú đến cực độ, tuổi thọ gia tăng.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tử Vi tọa thủ cung Mệnh và gặp Thiên Phủ, Vũ Khúc, Thiên Tướng, Tả Phù, Hữu Bật, Long Trì, Phượng Các, Hóa Khoa, Hóa Quyền, Hóa Lộc không gặp Kình Dương, Thiên Kiếp</t>
+  </si>
+  <si>
+    <t>Sinh năm Kỷ có Tử Vi đồng cung Thiên Phủ tại Dần tại Mệnh gặp Hóa Quyền</t>
+  </si>
+  <si>
+    <t>Tử Vi Thất Sát đồng cung tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Tử Vi Thất Sát đồng cung tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Tử Vi Thất Sát đồng cung tọa thủ cung Mệnh ở Hợi gặp Hóa Quyền</t>
+  </si>
+  <si>
+    <t>Tử Vi Thất Sát đồng cung tọa thủ cung Mệnh ở Tỵ gặp Hóa Quyền</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh và gặp Vũ Khúc, Phá Quân, Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Thìn có Phá Toái đồng cung</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Tuất có Phá Toái đồng cung</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Sửu có Phá Toái đồng cung</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh có Phá Toái đồng cung với Địa Không, Địa Kiếp</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh có Đào Hoa, Hồng Loan, Địa Không, Địa Kiếp</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh và hội chiếu các sao Văn Khúc, Văn Xương</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Tả Phù Hữu Bật</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Tý gặp Quyền, Lộc, Khoa</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Ngọ gặp Quyền, Lộc, Khoa</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh gặp Quyền, Lộc, Khoa, Kình, Đà</t>
   </si>
 </sst>
 </file>
@@ -742,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,6 +1499,214 @@
         <v>130</v>
       </c>
     </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Nhận xét vị trí sinh của mệnh so với bản mênh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7A8A8A-B512-464D-9319-0C3174A22BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE74A2F-6C71-4A44-A2D7-9BDA9BEF008A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="166">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -499,6 +499,30 @@
   </si>
   <si>
     <t>Tử Vi tọa thủ cung Mệnh gặp Quyền, Lộc, Khoa, Kình, Đà</t>
+  </si>
+  <si>
+    <t>Vị trí địa sinh cung Mệnh tại Sinh Địa</t>
+  </si>
+  <si>
+    <t>Vị trí địa sinh cung Mệnh tại Vượng Địa</t>
+  </si>
+  <si>
+    <t>Vị trí địa sinh cung Mệnh tại Sinh địa</t>
+  </si>
+  <si>
+    <t>Vị trí địa sinh cung Mệnh tại Bại địa</t>
+  </si>
+  <si>
+    <t>Vị trí địa sinh cung Mệnh tại Tuyệt địa</t>
+  </si>
+  <si>
+    <t>Vị trí địa sinh cung Mệnh tại Vượng địa</t>
+  </si>
+  <si>
+    <t>Vị trí địa sinh cung Mệnh tại Bình Thường</t>
+  </si>
+  <si>
+    <t>Vị trí địa sinh cung Mệnh tại Bình thường</t>
   </si>
 </sst>
 </file>
@@ -823,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1707,6 +1731,46 @@
         <v>157</v>
       </c>
     </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Liêm Trinh Toạ Thủ và hội họp cát tinh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE74A2F-6C71-4A44-A2D7-9BDA9BEF008A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE82DDD-88B5-4484-8189-4B8794F6D833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="185">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -523,6 +523,63 @@
   </si>
   <si>
     <t>Vị trí địa sinh cung Mệnh tại Bình thường</t>
+  </si>
+  <si>
+    <t>Liêm Trinh</t>
+  </si>
+  <si>
+    <t>Thân hình to lớn, xương thô, lông mày dầy.</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>Con người thẳng thắn, can đảm, dũng mãnh, nghiêm nghị, nóng tính.</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tý gặp Quyền, Lộc, Khoa, Phủ, Tả, Hữu, Tướng, Xương, Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Ngọ gặp Quyền, Lộc, Khoa, Phủ, Tả, Hữu, Tướng, Xương, Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Dần gặp Quyền, Lộc, Khoa, Phủ, Tả, Hữu, Tướng, Xương, Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Thân gặp Quyền, Lộc, Khoa, Phủ, Tả, Hữu, Tướng, Xương, Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Thìn gặp Quyền, Lộc, Khoa, Phủ, Tả, Hữu, Tướng, Xương, Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tuất gặp Quyền, Lộc, Khoa, Phủ, Tả, Hữu, Tướng, Xương, Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp Quyền, Lộc, Khoa, Phủ, Tướng, Xương, Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp Quyền, Lộc, Khoa, Phủ, Tướng, Xương, Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp Quyền, Lộc, Khoa, Phủ, Tả, Hữu, Tướng, Xương, Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp Quyền, Lộc, Khoa, Phủ, Tả, Hữu, Tướng, Xương, Khúc</t>
   </si>
 </sst>
 </file>
@@ -847,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E104"/>
+  <dimension ref="A1:E121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,6 +1828,142 @@
         <v>164</v>
       </c>
     </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Liêm Trinh miếu vượng đắc địa gặp Sát Hình Kỵ
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE82DDD-88B5-4484-8189-4B8794F6D833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90971508-6721-477B-A1C9-190A3671308C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="193">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -580,6 +580,30 @@
   </si>
   <si>
     <t>Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp Quyền, Lộc, Khoa, Phủ, Tả, Hữu, Tướng, Xương, Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tý gặp Kình Dương, Đà La, Địa Không, Địa Kiếp, Hoả Tinh, Linh Tinh, Hoá Kỵ, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Ngọ gặp Kình Dương, Đà La, Địa Không, Địa Kiếp, Hoả Tinh, Linh Tinh, Hoá Kỵ, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Dần gặp Kình Dương, Đà La, Địa Không, Địa Kiếp, Hoả Tinh, Linh Tinh, Hoá Kỵ, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Thân gặp Kình Dương, Đà La, Địa Không, Địa Kiếp, Hoả Tinh, Linh Tinh, Hoá Kỵ, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Thìn gặp Kình Dương, Đà La, Địa Không, Địa Kiếp, Hoả Tinh, Linh Tinh, Hoá Kỵ, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tuất gặp Kình Dương, Đà La, Địa Không, Địa Kiếp, Hoả Tinh, Linh Tinh, Hoá Kỵ, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp Kình Dương, Đà La, Địa Không, Địa Kiếp, Hoả Tinh, Linh Tinh, Hoá Kỵ, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp Kình Dương, Đà La, Địa Không, Địa Kiếp, Hoả Tinh, Linh Tinh, Hoá Kỵ, Thiên Hình</t>
   </si>
 </sst>
 </file>
@@ -904,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:E129"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="B121" sqref="B121"/>
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,6 +1988,70 @@
         <v>184</v>
       </c>
     </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Liêm Trinh Hoàn Thiện
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90971508-6721-477B-A1C9-190A3671308C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F295875E-5E89-4DF9-AFBF-8D771BE1B31D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="232">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -604,6 +604,123 @@
   </si>
   <si>
     <t>Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp Kình Dương, Đà La, Địa Không, Địa Kiếp, Hoả Tinh, Linh Tinh, Hoá Kỵ, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tỵ gặp Kình Dương, Đà La, Địa Không, Địa Kiếp, Hoả Tinh, Linh Tinh, Hoá Kỵ, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Hợi gặp Kình Dương, Đà La, Địa Không, Địa Kiếp, Hoả Tinh, Linh Tinh, Hoá Kỵ, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Mão gặp Kình Dương, Đà La, Địa Không, Địa Kiếp, Hoả Tinh, Linh Tinh, Hoá Kỵ, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Dậu gặp Kình Dương, Đà La, Địa Không, Địa Kiếp, Hoả Tinh, Linh Tinh, Hoá Kỵ, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Hoá Kỵ tại Tỵ, Văn Xương, Văn Khúc tại Mệnh và sinh năm Bính</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Hoá Kỵ tại Hợi, Văn Xương, Văn Khúc tại Mệnh và sinh năm Bính</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Dậu gặp Hoả Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Mão gặp Hoả Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Anh có Liêm Trinh tọa thủ cung Mệnh ở Tý gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Anh có Liêm Trinh tọa thủ cung Mệnh ở Ngọ gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Anh có Liêm Trinh tọa thủ cung Mệnh ở Dần gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Anh có Liêm Trinh tọa thủ cung Mệnh ở Thân gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Anh có Liêm Trinh tọa thủ cung Mệnh ở Thìn gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Anh có Liêm Trinh tọa thủ cung Mệnh ở Tuất gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Anh có Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Anh có Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Chị có Liêm Trinh tọa thủ cung Mệnh ở Tý gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Chị có Liêm Trinh tọa thủ cung Mệnh ở Ngọ gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Chị có Liêm Trinh tọa thủ cung Mệnh ở Dần gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Chị có Liêm Trinh tọa thủ cung Mệnh ở Thân gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Chị có Liêm Trinh tọa thủ cung Mệnh ở Thìn gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Chị có Liêm Trinh tọa thủ cung Mệnh ở Tuất gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Chị có Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Chị có Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Bạch Hổ tại Tỵ</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Bạch Hổ tại Hợi</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Bạch Hổ tại Mão</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Bạch Hổ tại Dậu</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Thiên Tướng tại Thân</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Thiên Tướng tại Dần</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Thiên Tướng tại Ngọ</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Thiên Tướng tại Tý</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Thiên Tướng tại Mùi</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Thiên Tướng tại Sửu</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Thiên Tướng tại Tuất</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung Thiên Tướng tại Thìn</t>
   </si>
 </sst>
 </file>
@@ -928,10 +1045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E129"/>
+  <dimension ref="A1:E173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="B131" sqref="B131"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="K158" sqref="K158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2052,6 +2169,358 @@
         <v>192</v>
       </c>
     </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="B164" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Luận cung Mệnh sao tử vi
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98F77A4E-89D8-4616-8611-9C0F8DFF603F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450A146B-6D7A-43D9-99A4-ECA44B1DEA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="240">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -724,7 +724,28 @@
     <t>Liêm Trinh đồng cung Thiên Tướng tại Thìn</t>
   </si>
   <si>
-    <t>Thiên Đồng</t>
+    <t>Tử Vi tọa thủ cung Mệnh và hội chiếu các sao: Thiên Phủ, Vũ Khúc, Thiên Tướng, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Long Trì, Phượng Các</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh và hội chiếu các sao: Kình Dương, Đà La, Không Kiếp, Kiếp Sát, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh và hội chiếu  Không Kiếp, Kiếp Sát</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Tham Lang tại Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Tham Lang tại Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Người sinh năm Giáp có Tử Vi tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Người sinh năm Đinh có Tử Vi tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Người sinh năm Kỷ có Tử Vi tọa thủ cung Mệnh ở Ngọ</t>
   </si>
 </sst>
 </file>
@@ -773,7 +794,178 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2533,18 +2725,198 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>232</v>
       </c>
+      <c r="B13" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>233</v>
+      </c>
+      <c r="B14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>235</v>
+      </c>
+      <c r="B16" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>236</v>
+      </c>
+      <c r="B17" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>237</v>
+      </c>
+      <c r="B18" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>238</v>
+      </c>
+      <c r="B19" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>239</v>
+      </c>
+      <c r="B20" t="s">
+        <v>239</v>
+      </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B17 B21:B1048576">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Tử vi đông cung kinh đương
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{450A146B-6D7A-43D9-99A4-ECA44B1DEA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E650A09-BDDC-44F4-B2A0-7F84442AD292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="249">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -739,13 +739,40 @@
     <t>Tử Vi đồng cung với Tham Lang tại Mệnh ở Dậu</t>
   </si>
   <si>
-    <t>Người sinh năm Giáp có Tử Vi tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>Người sinh năm Đinh có Tử Vi tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>Người sinh năm Kỷ có Tử Vi tọa thủ cung Mệnh ở Ngọ</t>
+    <t>Sinh năm Giáp có Tử Vi tọa thủ cung Mệnh ở Ngọ và không gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Sinh năm Đinh có Tử Vi tọa thủ cung Mệnh ở Ngọ và không gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Sinh năm Kỷ có Tử Vi tọa thủ cung Mệnh ở Ngọ và không gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Nữ mệnh sinh năm Nhâm có Tử Vi tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Nữ mệnh sinh năm Giáp có Tử Vi tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh đồng cung Thiên Phủ gặp Tả Phù, Hữu Bật</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh gặp Tả Phù, Hữu Bật</t>
+  </si>
+  <si>
+    <t>Thiên Phủ tọa thủ cung Mệnh gặp Tả Phù, Hữu Bật</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh đồng cung Kình Dương</t>
+  </si>
+  <si>
+    <t>Thiên Phủ tọa thủ cung Mệnh đồng cung Kình Dương</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh và hội chiếu các sao: Thiên Phủ, Vũ Khúc, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Long Trì, Phượng Các, Tả Phù, Hữu Bật, Quốc Ấn</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh và hội chiếu Địa Kiếp, Địa Không</t>
   </si>
 </sst>
 </file>
@@ -794,87 +821,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2725,10 +2672,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2896,26 +2843,130 @@
         <v>239</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>129</v>
+      </c>
+      <c r="B21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>240</v>
+      </c>
+      <c r="B22" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>241</v>
+      </c>
+      <c r="B24" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>242</v>
+      </c>
+      <c r="B27" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B28" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>244</v>
+      </c>
+      <c r="B29" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>245</v>
+      </c>
+      <c r="B30" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>246</v>
+      </c>
+      <c r="B31" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>247</v>
+      </c>
+      <c r="B32" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>248</v>
+      </c>
+      <c r="B33" t="s">
+        <v>248</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B17 B21:B1048576">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Tử vi quân thần khánh hội không gặp không kiếp
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E650A09-BDDC-44F4-B2A0-7F84442AD292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F83722-B2EB-481B-8EBB-72BDD82A5037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -769,10 +769,10 @@
     <t>Thiên Phủ tọa thủ cung Mệnh đồng cung Kình Dương</t>
   </si>
   <si>
-    <t>Tử Vi tọa thủ cung Mệnh và hội chiếu các sao: Thiên Phủ, Vũ Khúc, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Long Trì, Phượng Các, Tả Phù, Hữu Bật, Quốc Ấn</t>
-  </si>
-  <si>
-    <t>Tử Vi tọa thủ cung Mệnh và hội chiếu Địa Kiếp, Địa Không</t>
+    <t>Tử Vi tọa thủ cung Mệnh gặp cát tinh: Thiên Phủ, Vũ Khúc, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Long Trì, Phượng Các, Quốc Ấn</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh gặp cát tinh: Thiên Phủ, Vũ Khúc, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Long Trì, Phượng Các, Quốc Ấn Không gặp Địa Kiếp, Địa Không, Kình Dương</t>
   </si>
 </sst>
 </file>
@@ -821,7 +821,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2674,8 +2704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2933,40 +2963,47 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B32" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B33" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  <conditionalFormatting sqref="A1:A32 A34:A1048576">
+    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B17 B21:B1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  <conditionalFormatting sqref="B1:B17 B21:B32 B34:B1048576">
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A33">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Luận tử vi tại mệnh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F83722-B2EB-481B-8EBB-72BDD82A5037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031881CB-01D9-4333-B1E6-4C96F4EA5E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="258">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -773,6 +773,33 @@
   </si>
   <si>
     <t>Tử Vi tọa thủ cung Mệnh gặp cát tinh: Thiên Phủ, Vũ Khúc, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Long Trì, Phượng Các, Quốc Ấn Không gặp Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh đồng cung Thiên Tướng, Phá toại tại cung thân hợp chiếu với sao Kình Dương</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Thất Sát tại Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Thất Sát tại Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Thất Sát tại tại Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Thất Sát tại Mệnh gặp Hóa Quyền</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Vũ Khúc tại Mệnh gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Phá Quân tại Mệnh gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
   </si>
 </sst>
 </file>
@@ -821,7 +848,87 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2702,10 +2809,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2977,33 +3084,113 @@
         <v>247</v>
       </c>
     </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>249</v>
+      </c>
+      <c r="B34" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>250</v>
+      </c>
+      <c r="B35" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>251</v>
+      </c>
+      <c r="B36" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>253</v>
+      </c>
+      <c r="B37" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>255</v>
+      </c>
+      <c r="B38" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>254</v>
+      </c>
+      <c r="B39" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>256</v>
+      </c>
+      <c r="B40" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>257</v>
+      </c>
+      <c r="B41" t="s">
+        <v>257</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A1:A32 A34:A1048576">
-    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B17 B21:B32 B34:B1048576">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+  <conditionalFormatting sqref="B1:B17 B21:B32 B34 B37 B40:B1048576">
+    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B35">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Phá Quân tọa thủ cung Mệnh tại Sửu gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031881CB-01D9-4333-B1E6-4C96F4EA5E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0469B7-84B0-4992-AE89-AA6E56AB9B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="274">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -800,6 +800,54 @@
   </si>
   <si>
     <t>Vũ Khúc tọa thủ cung Mệnh gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh tại Thìn</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh tại Thìn</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh tại Tuất</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh tại Tuất</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh tại Mùi</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh tại Mùi</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh tại Sửu</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh tại Sửu</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh tại Thìn gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh tại Thìn gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh tại Tuất gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh tại Tuất gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh tại Mùi gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh tại Mùi gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh tại Sửu gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh tại Sửu gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
   </si>
 </sst>
 </file>
@@ -2809,10 +2857,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B41"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3146,6 +3194,110 @@
       </c>
       <c r="B41" t="s">
         <v>257</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>258</v>
+      </c>
+      <c r="B42" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>259</v>
+      </c>
+      <c r="B43" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>260</v>
+      </c>
+      <c r="B44" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>262</v>
+      </c>
+      <c r="B45" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>264</v>
+      </c>
+      <c r="B46" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>266</v>
+      </c>
+      <c r="B47" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>267</v>
+      </c>
+      <c r="B48" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>268</v>
+      </c>
+      <c r="B49" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>269</v>
+      </c>
+      <c r="B50" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>270</v>
+      </c>
+      <c r="B51" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>271</v>
+      </c>
+      <c r="B52" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>272</v>
+      </c>
+      <c r="B53" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>273</v>
+      </c>
+      <c r="B54" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>
@@ -3177,20 +3329,20 @@
     <cfRule type="duplicateValues" dxfId="8" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
An tử vi tại mệnh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0469B7-84B0-4992-AE89-AA6E56AB9B2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B8D131-2957-4B1C-BDB2-B10215F3344D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="296">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -848,6 +848,72 @@
   </si>
   <si>
     <t>Phá Quân tọa thủ cung Mệnh tại Sửu gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh tại Thìn gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh tại Thìn gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh tại Tuất gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh tại Tuất gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh tại Mùi gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh tại Mùi gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh tại Sửu gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh tại Sửu gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh tại Thìn gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh tại Thìn gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh tại Tuất gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh tại Tuất gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh tại Mùi gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh tại Mùi gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh tại Sửu gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh tại Sửu gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Mão gặp Địa Kiếp, Địa Không</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Dậu gặp Địa Kiếp, Địa Không</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh đồng cung Địa Không, Đào Hoa, Hồng Loan gặp Địa Kiếp</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh đồng cung Tả Phù, Hữu Bật</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Tý gặp Hóa Khoa, Hóa Lộc, Hóa Quyền</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh ở Ngọ gặp Hóa Khoa, Hóa Lộc, Hóa Quyền</t>
   </si>
 </sst>
 </file>
@@ -896,7 +962,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2857,10 +2963,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="O45" sqref="O45"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="U62" sqref="U62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3300,49 +3406,233 @@
         <v>273</v>
       </c>
     </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>274</v>
+      </c>
+      <c r="B55" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>275</v>
+      </c>
+      <c r="B56" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>276</v>
+      </c>
+      <c r="B57" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>277</v>
+      </c>
+      <c r="B58" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>278</v>
+      </c>
+      <c r="B59" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>279</v>
+      </c>
+      <c r="B60" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>280</v>
+      </c>
+      <c r="B61" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>281</v>
+      </c>
+      <c r="B62" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>282</v>
+      </c>
+      <c r="B63" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>283</v>
+      </c>
+      <c r="B64" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>284</v>
+      </c>
+      <c r="B65" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>285</v>
+      </c>
+      <c r="B66" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>286</v>
+      </c>
+      <c r="B67" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>287</v>
+      </c>
+      <c r="B68" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>288</v>
+      </c>
+      <c r="B69" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>289</v>
+      </c>
+      <c r="B70" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>290</v>
+      </c>
+      <c r="B71" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>291</v>
+      </c>
+      <c r="B72" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>292</v>
+      </c>
+      <c r="B73" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>293</v>
+      </c>
+      <c r="B74" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>294</v>
+      </c>
+      <c r="B75" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>295</v>
+      </c>
+      <c r="B76" t="s">
+        <v>295</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A1:A32 A34:A1048576">
-    <cfRule type="duplicateValues" dxfId="19" priority="21"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B17 B21:B32 B34 B37 B40:B1048576">
-    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
+  <conditionalFormatting sqref="B1:B17 B21:B32 B34 B37 B40:B74 B77:B1048576">
+    <cfRule type="duplicateValues" dxfId="21" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
+    <cfRule type="duplicateValues" dxfId="20" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B20">
+    <cfRule type="duplicateValues" dxfId="18" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18">
     <cfRule type="duplicateValues" dxfId="16" priority="16"/>
     <cfRule type="duplicateValues" dxfId="15" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
+  <conditionalFormatting sqref="A33">
     <cfRule type="duplicateValues" dxfId="14" priority="14"/>
     <cfRule type="duplicateValues" dxfId="13" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
+    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36">
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B38">
     <cfRule type="duplicateValues" dxfId="7" priority="7"/>
     <cfRule type="duplicateValues" dxfId="6" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B36">
+  <conditionalFormatting sqref="B39">
     <cfRule type="duplicateValues" dxfId="5" priority="5"/>
     <cfRule type="duplicateValues" dxfId="4" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B38">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  <conditionalFormatting sqref="B75">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  <conditionalFormatting sqref="B76">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Luận hòan thiện cung Mệnh có tử vi
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B8D131-2957-4B1C-BDB2-B10215F3344D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321281AA-4A63-4FFE-A1A5-92F15CA58DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="299">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -914,6 +914,15 @@
   </si>
   <si>
     <t>Tử Vi tọa thủ cung Mệnh ở Ngọ gặp Hóa Khoa, Hóa Lộc, Hóa Quyền</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh gặp Hóa Quyền, Hóa Lộc, Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh đồng cung Hóa Lộc gặp Tả Phù, Hữu Bật</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh hội chiếu Thiên Phủ</t>
   </si>
 </sst>
 </file>
@@ -2963,10 +2972,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B76"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="U62" sqref="U62"/>
+      <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3580,6 +3589,30 @@
       </c>
       <c r="B76" t="s">
         <v>295</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>296</v>
+      </c>
+      <c r="B77" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>297</v>
+      </c>
+      <c r="B78" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>298</v>
+      </c>
+      <c r="B79" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -3627,12 +3660,12 @@
     <cfRule type="duplicateValues" dxfId="4" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Liêm Trinh hãm gặp Hoả Linh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\New\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E98A05E-09FF-412A-9EDC-3C84A3740AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37390511-40FF-452D-843F-B50830A4845E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="329">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -1008,6 +1008,20 @@
   </si>
   <si>
     <t>Liêm Trinh tọa thủ cung Mệnh ở Hợi đồng cung Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuổi Bính Liêm Trinh tọa thủ cung Mệnh ở Tỵ đồng cung Hóa Kỵ gặp Văn Xương, Văn Khúc
+</t>
+  </si>
+  <si>
+    <t>Tuổi Bính Liêm Trinh tọa thủ cung Mệnh ở Hợi đồng cung Hóa Kỵ gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liêm Trinh tọa thủ cung Mệnh ở Mão gặp Hỏa Tinh, Linh Tinh
+</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Dậu gặp Hỏa Tinh, Linh Tinh</t>
   </si>
 </sst>
 </file>
@@ -1049,9 +1063,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -3098,863 +3115,895 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B107"/>
+  <dimension ref="A1:B111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+      <selection activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="29.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="3" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="3" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="3" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="3" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="3" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="3" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="3" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="3" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="3" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="3" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="3" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="3" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="3" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="3" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="3" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="3" t="s">
         <v>274</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="3" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="3" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="3" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="3" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="3" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="3" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="3" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="3" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="3" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="3" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B65" s="3" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="3" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="3" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="3" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="3" t="s">
         <v>288</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="3" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="3" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="3" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="3" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="3" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="3" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="3" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="3" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" s="3" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="3" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="3" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="3" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+      <c r="A82" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" s="3" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
+      <c r="A83" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="3" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B84" s="3" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B85" s="3" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
+      <c r="A86" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="3" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
+      <c r="A87" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="B87" s="2" t="s">
+      <c r="B87" s="3" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
+      <c r="A88" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" s="3" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
+      <c r="A89" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" s="3" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="B90" s="3" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B91" s="3" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
+      <c r="A92" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B92" s="3" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
+      <c r="A93" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B93" s="3" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B94" s="3" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B95" s="3" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
+      <c r="A96" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B96" s="3" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
+      <c r="A97" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B97" s="3" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
+      <c r="A98" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B98" s="3" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
+      <c r="A99" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B99" s="3" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
+      <c r="A100" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B100" s="3" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
+      <c r="A101" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B101" s="3" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
+      <c r="A102" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B102" s="3" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
+      <c r="A103" s="3" t="s">
         <v>319</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B103" s="3" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
+      <c r="A104" s="3" t="s">
         <v>321</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B104" s="3" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
+      <c r="A105" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B105" s="3" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
+      <c r="A106" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B106" s="3" t="s">
         <v>323</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
+      <c r="A107" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B107" s="3" t="s">
         <v>324</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="B109" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Luận Hoàn thiện cung mệnh tại Liêm Trinh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2DA20A-BFCD-472D-8E0E-D3CA1127A8EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FA9A41-CB2B-4BEE-B9EA-F27FD1666C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="353">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -1079,6 +1079,12 @@
   </si>
   <si>
     <t>Liêm Trinh tọa thủ cung Mệnh ở Mão gặp Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh gặp tứ sát Kình Đà Hỏa Linh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh gặp tứ sát Kình Đà Hỏa Linh và Bạch Hổ</t>
   </si>
 </sst>
 </file>
@@ -1128,47 +1134,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="26">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3189,10 +3155,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B135"/>
+  <dimension ref="A1:B137"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="G80" sqref="G80"/>
+      <selection activeCell="B140" sqref="B140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4272,62 +4238,79 @@
         <v>319</v>
       </c>
     </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A1:A32 A34:A1048576">
-    <cfRule type="duplicateValues" dxfId="29" priority="29"/>
-    <cfRule type="duplicateValues" dxfId="28" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33">
-    <cfRule type="duplicateValues" dxfId="27" priority="20"/>
-    <cfRule type="duplicateValues" dxfId="26" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B17 B21:B32 B34 B37 B40:B74 B77:B80 B136:B1048576">
-    <cfRule type="duplicateValues" dxfId="25" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="24" priority="22"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="22" priority="26"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="20" priority="24"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="duplicateValues" dxfId="17" priority="17"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="15" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="duplicateValues" dxfId="13" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B75">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81:B135">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sửa lại file excel luận mệnh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,25 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FA9A41-CB2B-4BEE-B9EA-F27FD1666C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DDB19E-1304-4CFA-A2E5-CBC6812BA412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="513">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -727,18 +737,6 @@
     <t>Tử Vi tọa thủ cung Mệnh và hội chiếu các sao: Thiên Phủ, Vũ Khúc, Thiên Tướng, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Long Trì, Phượng Các</t>
   </si>
   <si>
-    <t>Tử Vi tọa thủ cung Mệnh và hội chiếu các sao: Kình Dương, Đà La, Không Kiếp, Kiếp Sát, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>Tử Vi tọa thủ cung Mệnh và hội chiếu  Không Kiếp, Kiếp Sát</t>
-  </si>
-  <si>
-    <t>Tử Vi đồng cung với Tham Lang tại Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>Tử Vi đồng cung với Tham Lang tại Mệnh ở Dậu</t>
-  </si>
-  <si>
     <t>Sinh năm Giáp có Tử Vi tọa thủ cung Mệnh ở Ngọ và không gặp Thiên Hình, Hóa Kỵ</t>
   </si>
   <si>
@@ -784,9 +782,6 @@
     <t>Tử Vi đồng cung với Thất Sát tại Mệnh ở Hợi</t>
   </si>
   <si>
-    <t>Tử Vi đồng cung với Thất Sát tại tại Mệnh ở Hợi</t>
-  </si>
-  <si>
     <t>Tử Vi đồng cung với Thất Sát tại Mệnh gặp Hóa Quyền</t>
   </si>
   <si>
@@ -928,163 +923,658 @@
     <t>Liêm Trinh tọa thủ cung Mệnh</t>
   </si>
   <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Thìn gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Tuất gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Tý gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Ngọ gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Dần gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Thân gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Sửu đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Mùi đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Thìn gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Tuất gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Tỵ đồng cung Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Hợi đồng cung Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>Tuổi Bính Liêm Trinh tọa thủ cung Mệnh ở Hợi đồng cung Hóa Kỵ gặp Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Dậu gặp Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Mão gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Tỵ gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Tý gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Ngọ gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Thân gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Hợi gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t>Tuổi Bính Liêm Trinh tọa thủ cung Mệnh ở Tỵ đồng cung Hóa Kỵ gặp Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh ở Mão gặp Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh gặp tứ sát Kình Đà Hỏa Linh</t>
-  </si>
-  <si>
-    <t>Liêm Trinh tọa thủ cung Mệnh gặp tứ sát Kình Đà Hỏa Linh và Bạch Hổ</t>
+    <t>Thiên Đồng tọa thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Dần gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Dần gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Thân gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tý gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Mão gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tỵ gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Hợi gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Lương ở Dần</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Lương ở Dần gặp các sao cát tinh: Hóa Lộc, Hóa Quyền, Lộc Tồn, Hỏa Linh, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Lương ở Thân</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Lương ở Thân gặp các sao cát tinh: Hóa Lộc, Hóa Quyền, Lộc Tồn, Hỏa Linh, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Ngọ đồng cung Thái Âm gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tý đồng cung Thái Âm gặp các sao Bạch Hổ, Thiên Khốc, Thiên Riêu, Tang Môn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Việt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Việt gặp các sao cát tinh: Hóa Lộc, Hóa Quyền, Lộc Tồn, Hỏa Linh, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Ngọ gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Sửu gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Mùi gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tuất gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Thìn gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Dậu gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Người tuổi Ấ. có Thiên Đồng tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Người tuổi Ấ. có Thiên Đồng tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Thìn gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Thìn gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tuất gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tuất gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tý gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tý gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Ngọ gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Ngọ gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Dần gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Thân gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Thân gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Sửu đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Mùi đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tỵ gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Hợi gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Mão gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tỵ đồng cung Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tuổi Bính Liêm Trinh tọa thủ cung Mệnh ở Tỵ đồng cung Hóa Kỵ gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Hợi đồng cung Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tuổi Bính Liêm Trinh tọa thủ cung Mệnh ở Hợi đồng cung Hóa Kỵ gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Mão gặp Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Dậu gặp Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh gặp tứ sát Kình Đà Hỏa Linh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh gặp tứ sát Kình Đà Hỏa Linh và Bạch Hổ</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:380 Tử Vi tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:380 Tử Vi tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:380 Tử Vi tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:380 Tử Vi tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:380 Tử Vi tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:380 Tử Vi tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:380 Tử Vi tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:380 Tử Vi tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:388 Tử Vi tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:388 Tử Vi tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:388 Tử Vi tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:388 Tử Vi tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:388 Tử Vi tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:388 Tử Vi tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:388 Tử Vi tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:388 Tử Vi tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:395 Tử Vi tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:395 Tử Vi tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:395 Tử Vi tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:395 Tử Vi tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:404 Tử Vi tọa thủ cung Mệnh và hội chiếu các sao: Thiên Phủ, Vũ Khúc, Thiên Tướng, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Long Trì, Phượng Các</t>
+  </si>
+  <si>
+    <t>luanmenh.js:412 Tử Vi tọa thủ cung Mệnh và hội chiếu  Địa Kiếp, Địa Không</t>
+  </si>
+  <si>
+    <t>luanmenh.js:415 Tử Vi tọa thủ cung Mệnh và hội chiếu các sao: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:426 Tử Vi đồng cung với Tham Lang tại Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:429 Tử Vi tọa thủ cung Mệnh ở Mão gặp Địa Kiếp, Địa Không</t>
+  </si>
+  <si>
+    <t>luanmenh.js:429 Tử Vi tọa thủ cung Mệnh ở Dậu gặp Địa Kiếp, Địa Không</t>
+  </si>
+  <si>
+    <t>luanmenh.js:440 Sinh năm Giáp có Tử Vi tọa thủ cung Mệnh ở Ngọ và không gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:440 Sinh năm Đinh có Tử Vi tọa thủ cung Mệnh ở Ngọ và không gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:440 Sinh năm Kỷ có Tử Vi tọa thủ cung Mệnh ở Ngọ và không gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:453 Nam mệnh sinh năm Nhâm có Tử Vi tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:456 Nữ mệnh sinh năm Nhâm có Tử Vi tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:453 Nam mệnh sinh năm Giáp có Tử Vi tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:456 Nữ mệnh sinh năm Giáp có Tử Vi tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:466 Sinh năm Giáp có Tử Vi đồng cung Thiên Phủ tại Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:466 Sinh năm Giáp có Tử Vi đồng cung Thiên Phủ tại Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:477 Tử Vi tọa thủ cung Mệnh đồng cung Thiên Phủ gặp Tả Phù, Hữu Bật</t>
+  </si>
+  <si>
+    <t>luanmenh.js:483 Tử Vi tọa thủ cung Mệnh gặp Tả Phù, Hữu Bật</t>
+  </si>
+  <si>
+    <t>luanmenh.js:483 Thiên Phủ tọa thủ cung Mệnh gặp Tả Phù, Hữu Bật</t>
+  </si>
+  <si>
+    <t>luanmenh.js:492 Tử Vi tọa thủ cung Mệnh đồng cung Kình Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:492 Thiên Phủ tọa thủ cung Mệnh đồng cung Kình Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:501 Tử Vi tọa thủ cung Mệnh gặp cát tinh: Thiên Phủ, Vũ Khúc, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Long Trì, Phượng Các, Quốc Ấn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:506 Tử Vi tọa thủ cung Mệnh gặp cát tinh: Thiên Phủ, Vũ Khúc, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Long Trì, Phượng Các, Quốc Ấn Không gặp Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:510 Phu Thê</t>
+  </si>
+  <si>
+    <t>luanmenh.js:513 Tử Vi tọa thủ cung Mệnh đồng cung Thiên Tướng, Phá toại tại cung thân hợp chiếu với sao Kình Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:519 Tử Vi đồng cung với Thất Sát tại Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:519 Tử Vi đồng cung với Thất Sát tại Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:526 Tử Vi đồng cung với Thất Sát tại Mệnh gặp Hóa Quyền</t>
+  </si>
+  <si>
+    <t>luanmenh.js:533 Tử Vi đồng cung với Vũ Khúc tại Mệnh gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:533 Tử Vi đồng cung với Phá Quân tại Mệnh gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:541 Tử Vi tọa thủ cung Mệnh gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:541 Vũ Khúc tọa thủ cung Mệnh gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:549 Tử Vi tọa thủ cung Mệnh tại Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:552 Tử Vi tọa thủ cung Mệnh tại Thìn gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:556 Tử Vi tọa thủ cung Mệnh tại Thìn gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:561 Tử Vi tọa thủ cung Mệnh tại Thìn gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>luanmenh.js:549 Phá Quân tọa thủ cung Mệnh tại Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:552 Phá Quân tọa thủ cung Mệnh tại Thìn gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:556 Phá Quân tọa thủ cung Mệnh tại Thìn gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:561 Phá Quân tọa thủ cung Mệnh tại Thìn gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>luanmenh.js:549 Tử Vi tọa thủ cung Mệnh tại Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:552 Tử Vi tọa thủ cung Mệnh tại Tuất gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:556 Tử Vi tọa thủ cung Mệnh tại Tuất gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:561 Tử Vi tọa thủ cung Mệnh tại Tuất gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>luanmenh.js:549 Phá Quân tọa thủ cung Mệnh tại Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:552 Phá Quân tọa thủ cung Mệnh tại Tuất gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:556 Phá Quân tọa thủ cung Mệnh tại Tuất gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:561 Phá Quân tọa thủ cung Mệnh tại Tuất gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>luanmenh.js:549 Tử Vi tọa thủ cung Mệnh tại Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:552 Tử Vi tọa thủ cung Mệnh tại Mùi gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:556 Tử Vi tọa thủ cung Mệnh tại Mùi gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:561 Tử Vi tọa thủ cung Mệnh tại Mùi gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>luanmenh.js:549 Phá Quân tọa thủ cung Mệnh tại Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:552 Phá Quân tọa thủ cung Mệnh tại Mùi gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:556 Phá Quân tọa thủ cung Mệnh tại Mùi gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:561 Phá Quân tọa thủ cung Mệnh tại Mùi gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>luanmenh.js:549 Tử Vi tọa thủ cung Mệnh tại Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:552 Tử Vi tọa thủ cung Mệnh tại Sửu gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:556 Tử Vi tọa thủ cung Mệnh tại Sửu gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:561 Tử Vi tọa thủ cung Mệnh tại Sửu gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>luanmenh.js:549 Phá Quân tọa thủ cung Mệnh tại Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:552 Phá Quân tọa thủ cung Mệnh tại Sửu gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:556 Phá Quân tọa thủ cung Mệnh tại Sửu gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:561 Phá Quân tọa thủ cung Mệnh tại Sửu gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
+  </si>
+  <si>
+    <t>luanmenh.js:570 Tử Vi tọa thủ cung Mệnh đồng cung Địa Không, Đào Hoa, Hồng Loan gặp Địa Kiếp</t>
+  </si>
+  <si>
+    <t>luanmenh.js:576 Tử Vi tọa thủ cung Mệnh đồng cung Tả Phù, Hữu Bật</t>
+  </si>
+  <si>
+    <t>luanmenh.js:583 Tử Vi tọa thủ cung Mệnh ở Tý gặp Hóa Khoa, Hóa Lộc, Hóa Quyền</t>
+  </si>
+  <si>
+    <t>luanmenh.js:583 Tử Vi tọa thủ cung Mệnh ở Ngọ gặp Hóa Khoa, Hóa Lộc, Hóa Quyền</t>
+  </si>
+  <si>
+    <t>luanmenh.js:589 Tử Vi tọa thủ cung Mệnh gặp Hóa Quyền, Hóa Lộc, Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:594 Tử Vi tọa thủ cung Mệnh đồng cung Hóa Lộc gặp Tả Phù, Hữu Bật</t>
+  </si>
+  <si>
+    <t>luanmenh.js:599 Tử Vi tọa thủ cung Mệnh hội chiếu Thiên Phủ</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh và hội chiếu  Địa Kiếp, Địa Không</t>
+  </si>
+  <si>
+    <t>Tử Vi tọa thủ cung Mệnh và hội chiếu các sao: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Tham Lang tại Mệnh</t>
+  </si>
+  <si>
+    <t>Phu Thê</t>
   </si>
 </sst>
 </file>
@@ -1134,37 +1624,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="23">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3155,10 +3615,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B137"/>
+  <dimension ref="A1:B214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="B140" sqref="B140"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3166,1151 +3626,2260 @@
     <col min="1" max="2" width="29.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>69</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>62</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>70</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>232</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>233</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>234</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>235</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>236</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>237</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>238</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>239</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>240</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>241</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>242</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>243</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>244</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>245</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>246</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>248</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>249</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>250</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>251</v>
       </c>
-      <c r="B36" s="2" t="s">
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>253</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>255</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>256</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>257</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>258</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>259</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>260</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
-        <v>266</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>267</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>268</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>272</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>276</v>
       </c>
-      <c r="B57" s="2" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>284</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>287</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>288</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>289</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>290</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>291</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>292</v>
       </c>
-      <c r="B73" s="2" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>293</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>294</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B84" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>360</v>
+      </c>
+      <c r="B85" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>361</v>
+      </c>
+      <c r="B86" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>362</v>
+      </c>
+      <c r="B87" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>363</v>
+      </c>
+      <c r="B88" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>364</v>
+      </c>
+      <c r="B89" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>365</v>
+      </c>
+      <c r="B90" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>366</v>
+      </c>
+      <c r="B91" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>367</v>
+      </c>
+      <c r="B92" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>368</v>
+      </c>
+      <c r="B93" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>369</v>
+      </c>
+      <c r="B94" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>370</v>
+      </c>
+      <c r="B95" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>371</v>
+      </c>
+      <c r="B96" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>372</v>
+      </c>
+      <c r="B97" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>373</v>
+      </c>
+      <c r="B98" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>374</v>
+      </c>
+      <c r="B99" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>375</v>
+      </c>
+      <c r="B100" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>376</v>
+      </c>
+      <c r="B101" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>377</v>
+      </c>
+      <c r="B102" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>378</v>
+      </c>
+      <c r="B103" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>379</v>
+      </c>
+      <c r="B104" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>380</v>
+      </c>
+      <c r="B105" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>381</v>
+      </c>
+      <c r="B106" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>382</v>
+      </c>
+      <c r="B107" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>383</v>
+      </c>
+      <c r="B108" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>384</v>
+      </c>
+      <c r="B109" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>385</v>
+      </c>
+      <c r="B110" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>386</v>
+      </c>
+      <c r="B111" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>387</v>
+      </c>
+      <c r="B112" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>388</v>
+      </c>
+      <c r="B113" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>389</v>
+      </c>
+      <c r="B114" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>390</v>
+      </c>
+      <c r="B115" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>391</v>
+      </c>
+      <c r="B116" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>392</v>
+      </c>
+      <c r="B117" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>393</v>
+      </c>
+      <c r="B118" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>394</v>
+      </c>
+      <c r="B119" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>395</v>
+      </c>
+      <c r="B120" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>396</v>
+      </c>
+      <c r="B121" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>397</v>
+      </c>
+      <c r="B122" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>398</v>
+      </c>
+      <c r="B123" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>399</v>
+      </c>
+      <c r="B124" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>400</v>
+      </c>
+      <c r="B125" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>401</v>
+      </c>
+      <c r="B126" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>402</v>
+      </c>
+      <c r="B127" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>403</v>
+      </c>
+      <c r="B128" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>404</v>
+      </c>
+      <c r="B129" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>405</v>
+      </c>
+      <c r="B130" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>406</v>
+      </c>
+      <c r="B131" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>407</v>
+      </c>
+      <c r="B132" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>408</v>
+      </c>
+      <c r="B133" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>409</v>
+      </c>
+      <c r="B134" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>410</v>
+      </c>
+      <c r="B135" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>411</v>
+      </c>
+      <c r="B136" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>412</v>
+      </c>
+      <c r="B137" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>413</v>
+      </c>
+      <c r="B138" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>414</v>
+      </c>
+      <c r="B139" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>415</v>
+      </c>
+      <c r="B140" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>416</v>
+      </c>
+      <c r="B141" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>417</v>
+      </c>
+      <c r="B142" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B144" s="2" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B145" s="2" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B146" s="2" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B147" s="2" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B148" s="2" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B149" s="2" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="2" t="s">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
         <v>308</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B157" s="2" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="2" t="s">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B159" s="2" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="2" t="s">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B85" s="2" t="s">
+      <c r="B170" s="2" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>301</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="2" t="s">
-        <v>311</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="B175" s="2" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B176" s="2" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="2" t="s">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="B177" s="2" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="2" t="s">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="B178" s="2" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="2" t="s">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B179" s="2" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="B180" s="2" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="2" t="s">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B181" s="2" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="2" t="s">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="B101" s="2" t="s">
+      <c r="B182" s="2" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="B102" s="2" t="s">
+      <c r="B183" s="2" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B103" s="2" t="s">
+      <c r="B184" s="2" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="2" t="s">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B185" s="2" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="2" t="s">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B186" s="2" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="2" t="s">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
         <v>338</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B187" s="2" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
         <v>339</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B188" s="2" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B109" s="2" t="s">
+      <c r="B189" s="2" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B110" s="2" t="s">
+      <c r="B190" s="2" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B191" s="2" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="2" t="s">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B192" s="2" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B210" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B211" s="2" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="B212" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B214" s="2" t="s">
         <v>323</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="B122" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="B123" s="2" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="2" t="s">
-        <v>322</v>
-      </c>
-      <c r="B124" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
-        <v>347</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="2" t="s">
-        <v>348</v>
-      </c>
-      <c r="B129" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
-        <v>317</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
-        <v>352</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>352</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1:A32 A34:A1048576">
-    <cfRule type="duplicateValues" dxfId="25" priority="29"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="31"/>
+  <conditionalFormatting sqref="A215:A1048576 A1:A23 A25:A143">
+    <cfRule type="duplicateValues" dxfId="22" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="40"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A33">
-    <cfRule type="duplicateValues" dxfId="23" priority="20"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="21"/>
+  <conditionalFormatting sqref="A24">
+    <cfRule type="duplicateValues" dxfId="20" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="30"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B17 B21:B32 B34 B37 B40:B74 B77:B80 B136:B1048576">
-    <cfRule type="duplicateValues" dxfId="21" priority="28"/>
+  <conditionalFormatting sqref="B145:B1048576 B1:B23 B25 B28 B31:B83">
+    <cfRule type="duplicateValues" dxfId="18" priority="37"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="20" priority="22"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="23"/>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="duplicateValues" dxfId="17" priority="28"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="18" priority="26"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="27"/>
+  <conditionalFormatting sqref="B26">
+    <cfRule type="duplicateValues" dxfId="16" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="27"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
-    <cfRule type="duplicateValues" dxfId="16" priority="24"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="25"/>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="duplicateValues" dxfId="14" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="25"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B33">
-    <cfRule type="duplicateValues" dxfId="14" priority="19"/>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="duplicateValues" dxfId="12" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="23"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35">
-    <cfRule type="duplicateValues" dxfId="13" priority="17"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="18"/>
+  <conditionalFormatting sqref="B30">
+    <cfRule type="duplicateValues" dxfId="10" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="21"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="11" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="16"/>
+  <conditionalFormatting sqref="B144">
+    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B38">
-    <cfRule type="duplicateValues" dxfId="9" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="14"/>
+  <conditionalFormatting sqref="A145:A214">
+    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39">
-    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="12"/>
+  <conditionalFormatting sqref="A144">
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B75">
-    <cfRule type="duplicateValues" dxfId="5" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="10"/>
+  <conditionalFormatting sqref="B143">
+    <cfRule type="duplicateValues" dxfId="3" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="52"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B76">
-    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B81:B135">
+  <conditionalFormatting sqref="B84:B142">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBE4172-FC39-45CE-BD67-BA23D6FB1A86}">
+  <dimension ref="A1:B92"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B92"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B1" t="str">
+        <f>A1</f>
+        <v>Tử Vi tọa thủ cung Mệnh</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>419</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>420</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>421</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>422</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>423</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>424</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>425</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>426</v>
+      </c>
+      <c r="B9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>427</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>428</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>429</v>
+      </c>
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>430</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>431</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>432</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>433</v>
+      </c>
+      <c r="B16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>434</v>
+      </c>
+      <c r="B17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>435</v>
+      </c>
+      <c r="B18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>436</v>
+      </c>
+      <c r="B19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>437</v>
+      </c>
+      <c r="B20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>438</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>439</v>
+      </c>
+      <c r="B22" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>440</v>
+      </c>
+      <c r="B23" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>441</v>
+      </c>
+      <c r="B24" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>442</v>
+      </c>
+      <c r="B25" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>443</v>
+      </c>
+      <c r="B26" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>442</v>
+      </c>
+      <c r="B27" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>444</v>
+      </c>
+      <c r="B28" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>445</v>
+      </c>
+      <c r="B29" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>446</v>
+      </c>
+      <c r="B30" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>447</v>
+      </c>
+      <c r="B31" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>448</v>
+      </c>
+      <c r="B32" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>449</v>
+      </c>
+      <c r="B33" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>450</v>
+      </c>
+      <c r="B34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>451</v>
+      </c>
+      <c r="B35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>452</v>
+      </c>
+      <c r="B36" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>453</v>
+      </c>
+      <c r="B37" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>454</v>
+      </c>
+      <c r="B38" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>455</v>
+      </c>
+      <c r="B39" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>456</v>
+      </c>
+      <c r="B40" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>457</v>
+      </c>
+      <c r="B41" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>458</v>
+      </c>
+      <c r="B42" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>459</v>
+      </c>
+      <c r="B43" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>460</v>
+      </c>
+      <c r="B44" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>461</v>
+      </c>
+      <c r="B45" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>462</v>
+      </c>
+      <c r="B46" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>463</v>
+      </c>
+      <c r="B47" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>464</v>
+      </c>
+      <c r="B48" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>465</v>
+      </c>
+      <c r="B49" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>466</v>
+      </c>
+      <c r="B50" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>467</v>
+      </c>
+      <c r="B51" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>468</v>
+      </c>
+      <c r="B52" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>469</v>
+      </c>
+      <c r="B53" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>470</v>
+      </c>
+      <c r="B54" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>471</v>
+      </c>
+      <c r="B55" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>472</v>
+      </c>
+      <c r="B56" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>473</v>
+      </c>
+      <c r="B57" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>474</v>
+      </c>
+      <c r="B58" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>475</v>
+      </c>
+      <c r="B59" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>476</v>
+      </c>
+      <c r="B60" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>477</v>
+      </c>
+      <c r="B61" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>478</v>
+      </c>
+      <c r="B62" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>479</v>
+      </c>
+      <c r="B63" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>480</v>
+      </c>
+      <c r="B64" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>481</v>
+      </c>
+      <c r="B65" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>482</v>
+      </c>
+      <c r="B66" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>483</v>
+      </c>
+      <c r="B67" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>484</v>
+      </c>
+      <c r="B68" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>485</v>
+      </c>
+      <c r="B69" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>486</v>
+      </c>
+      <c r="B70" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>487</v>
+      </c>
+      <c r="B71" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>488</v>
+      </c>
+      <c r="B72" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>489</v>
+      </c>
+      <c r="B73" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>490</v>
+      </c>
+      <c r="B74" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>491</v>
+      </c>
+      <c r="B75" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>492</v>
+      </c>
+      <c r="B76" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>493</v>
+      </c>
+      <c r="B77" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>494</v>
+      </c>
+      <c r="B78" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>495</v>
+      </c>
+      <c r="B79" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>496</v>
+      </c>
+      <c r="B80" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>497</v>
+      </c>
+      <c r="B81" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>498</v>
+      </c>
+      <c r="B82" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>499</v>
+      </c>
+      <c r="B83" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>500</v>
+      </c>
+      <c r="B84" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>501</v>
+      </c>
+      <c r="B85" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>502</v>
+      </c>
+      <c r="B86" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>503</v>
+      </c>
+      <c r="B87" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>504</v>
+      </c>
+      <c r="B88" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>505</v>
+      </c>
+      <c r="B89" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>506</v>
+      </c>
+      <c r="B90" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>507</v>
+      </c>
+      <c r="B91" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>508</v>
+      </c>
+      <c r="B92" t="s">
+        <v>293</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Luận xong Vũ Khúc
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DDB19E-1304-4CFA-A2E5-CBC6812BA412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39478FF8-4D35-43E3-817D-1DA56060E2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="552">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -1292,279 +1292,6 @@
     <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh gặp tứ sát Kình Đà Hỏa Linh và Bạch Hổ</t>
   </si>
   <si>
-    <t>Tử Vi tọa thủ cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:380 Tử Vi tọa thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:380 Tử Vi tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:380 Tử Vi tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:380 Tử Vi tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:380 Tử Vi tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:380 Tử Vi tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:380 Tử Vi tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:380 Tử Vi tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:388 Tử Vi tọa thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:388 Tử Vi tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:388 Tử Vi tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:388 Tử Vi tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:388 Tử Vi tọa thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:388 Tử Vi tọa thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:388 Tử Vi tọa thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>luanmenh.js:388 Tử Vi tọa thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:395 Tử Vi tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:395 Tử Vi tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:395 Tử Vi tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:395 Tử Vi tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:404 Tử Vi tọa thủ cung Mệnh và hội chiếu các sao: Thiên Phủ, Vũ Khúc, Thiên Tướng, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Long Trì, Phượng Các</t>
-  </si>
-  <si>
-    <t>luanmenh.js:412 Tử Vi tọa thủ cung Mệnh và hội chiếu  Địa Kiếp, Địa Không</t>
-  </si>
-  <si>
-    <t>luanmenh.js:415 Tử Vi tọa thủ cung Mệnh và hội chiếu các sao: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:426 Tử Vi đồng cung với Tham Lang tại Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:429 Tử Vi tọa thủ cung Mệnh ở Mão gặp Địa Kiếp, Địa Không</t>
-  </si>
-  <si>
-    <t>luanmenh.js:429 Tử Vi tọa thủ cung Mệnh ở Dậu gặp Địa Kiếp, Địa Không</t>
-  </si>
-  <si>
-    <t>luanmenh.js:440 Sinh năm Giáp có Tử Vi tọa thủ cung Mệnh ở Ngọ và không gặp Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:440 Sinh năm Đinh có Tử Vi tọa thủ cung Mệnh ở Ngọ và không gặp Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:440 Sinh năm Kỷ có Tử Vi tọa thủ cung Mệnh ở Ngọ và không gặp Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:453 Nam mệnh sinh năm Nhâm có Tử Vi tọa thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:456 Nữ mệnh sinh năm Nhâm có Tử Vi tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:453 Nam mệnh sinh năm Giáp có Tử Vi tọa thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:456 Nữ mệnh sinh năm Giáp có Tử Vi tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:466 Sinh năm Giáp có Tử Vi đồng cung Thiên Phủ tại Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:466 Sinh năm Giáp có Tử Vi đồng cung Thiên Phủ tại Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:477 Tử Vi tọa thủ cung Mệnh đồng cung Thiên Phủ gặp Tả Phù, Hữu Bật</t>
-  </si>
-  <si>
-    <t>luanmenh.js:483 Tử Vi tọa thủ cung Mệnh gặp Tả Phù, Hữu Bật</t>
-  </si>
-  <si>
-    <t>luanmenh.js:483 Thiên Phủ tọa thủ cung Mệnh gặp Tả Phù, Hữu Bật</t>
-  </si>
-  <si>
-    <t>luanmenh.js:492 Tử Vi tọa thủ cung Mệnh đồng cung Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:492 Thiên Phủ tọa thủ cung Mệnh đồng cung Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:501 Tử Vi tọa thủ cung Mệnh gặp cát tinh: Thiên Phủ, Vũ Khúc, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Long Trì, Phượng Các, Quốc Ấn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:506 Tử Vi tọa thủ cung Mệnh gặp cát tinh: Thiên Phủ, Vũ Khúc, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Long Trì, Phượng Các, Quốc Ấn Không gặp Địa Kiếp, Địa Không, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:510 Phu Thê</t>
-  </si>
-  <si>
-    <t>luanmenh.js:513 Tử Vi tọa thủ cung Mệnh đồng cung Thiên Tướng, Phá toại tại cung thân hợp chiếu với sao Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:519 Tử Vi đồng cung với Thất Sát tại Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:519 Tử Vi đồng cung với Thất Sát tại Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:526 Tử Vi đồng cung với Thất Sát tại Mệnh gặp Hóa Quyền</t>
-  </si>
-  <si>
-    <t>luanmenh.js:533 Tử Vi đồng cung với Vũ Khúc tại Mệnh gặp Kình Dương, Đà La</t>
-  </si>
-  <si>
-    <t>luanmenh.js:533 Tử Vi đồng cung với Phá Quân tại Mệnh gặp Kình Dương, Đà La</t>
-  </si>
-  <si>
-    <t>luanmenh.js:541 Tử Vi tọa thủ cung Mệnh gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:541 Vũ Khúc tọa thủ cung Mệnh gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:549 Tử Vi tọa thủ cung Mệnh tại Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:552 Tử Vi tọa thủ cung Mệnh tại Thìn gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:556 Tử Vi tọa thủ cung Mệnh tại Thìn gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:561 Tử Vi tọa thủ cung Mệnh tại Thìn gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
-  </si>
-  <si>
-    <t>luanmenh.js:549 Phá Quân tọa thủ cung Mệnh tại Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:552 Phá Quân tọa thủ cung Mệnh tại Thìn gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:556 Phá Quân tọa thủ cung Mệnh tại Thìn gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:561 Phá Quân tọa thủ cung Mệnh tại Thìn gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
-  </si>
-  <si>
-    <t>luanmenh.js:549 Tử Vi tọa thủ cung Mệnh tại Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:552 Tử Vi tọa thủ cung Mệnh tại Tuất gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:556 Tử Vi tọa thủ cung Mệnh tại Tuất gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:561 Tử Vi tọa thủ cung Mệnh tại Tuất gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
-  </si>
-  <si>
-    <t>luanmenh.js:549 Phá Quân tọa thủ cung Mệnh tại Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:552 Phá Quân tọa thủ cung Mệnh tại Tuất gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:556 Phá Quân tọa thủ cung Mệnh tại Tuất gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:561 Phá Quân tọa thủ cung Mệnh tại Tuất gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
-  </si>
-  <si>
-    <t>luanmenh.js:549 Tử Vi tọa thủ cung Mệnh tại Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:552 Tử Vi tọa thủ cung Mệnh tại Mùi gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:556 Tử Vi tọa thủ cung Mệnh tại Mùi gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:561 Tử Vi tọa thủ cung Mệnh tại Mùi gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
-  </si>
-  <si>
-    <t>luanmenh.js:549 Phá Quân tọa thủ cung Mệnh tại Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:552 Phá Quân tọa thủ cung Mệnh tại Mùi gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:556 Phá Quân tọa thủ cung Mệnh tại Mùi gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:561 Phá Quân tọa thủ cung Mệnh tại Mùi gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
-  </si>
-  <si>
-    <t>luanmenh.js:549 Tử Vi tọa thủ cung Mệnh tại Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:552 Tử Vi tọa thủ cung Mệnh tại Sửu gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:556 Tử Vi tọa thủ cung Mệnh tại Sửu gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:561 Tử Vi tọa thủ cung Mệnh tại Sửu gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
-  </si>
-  <si>
-    <t>luanmenh.js:549 Phá Quân tọa thủ cung Mệnh tại Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:552 Phá Quân tọa thủ cung Mệnh tại Sửu gặp các sao cát tinh: Hóa Quyền, Hóa Lộc, Hóa Khoa, Thiên Phủ, Tả Phù, Hữu Bật, Thiên Tướng, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:556 Phá Quân tọa thủ cung Mệnh tại Sửu gặp các sao Sát tinh: Địa Kiếp, Địa Không, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:561 Phá Quân tọa thủ cung Mệnh tại Sửu gặp Địa Kiếp, Địa Không, Kình Dương mà không gặp Văn Xương, Văn Khúc, Long Trì Phượng Các</t>
-  </si>
-  <si>
-    <t>luanmenh.js:570 Tử Vi tọa thủ cung Mệnh đồng cung Địa Không, Đào Hoa, Hồng Loan gặp Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:576 Tử Vi tọa thủ cung Mệnh đồng cung Tả Phù, Hữu Bật</t>
-  </si>
-  <si>
-    <t>luanmenh.js:583 Tử Vi tọa thủ cung Mệnh ở Tý gặp Hóa Khoa, Hóa Lộc, Hóa Quyền</t>
-  </si>
-  <si>
-    <t>luanmenh.js:583 Tử Vi tọa thủ cung Mệnh ở Ngọ gặp Hóa Khoa, Hóa Lộc, Hóa Quyền</t>
-  </si>
-  <si>
-    <t>luanmenh.js:589 Tử Vi tọa thủ cung Mệnh gặp Hóa Quyền, Hóa Lộc, Kình Dương, Đà La</t>
-  </si>
-  <si>
-    <t>luanmenh.js:594 Tử Vi tọa thủ cung Mệnh đồng cung Hóa Lộc gặp Tả Phù, Hữu Bật</t>
-  </si>
-  <si>
-    <t>luanmenh.js:599 Tử Vi tọa thủ cung Mệnh hội chiếu Thiên Phủ</t>
-  </si>
-  <si>
     <t>Tử Vi tọa thủ cung Mệnh và hội chiếu  Địa Kiếp, Địa Không</t>
   </si>
   <si>
@@ -1575,6 +1302,396 @@
   </si>
   <si>
     <t>Phu Thê</t>
+  </si>
+  <si>
+    <t>luanmenh.js:722 Vũ Khúc tọa thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Thìn đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Tuất đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Sửu đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Mùi đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Tý gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Tý gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Tý đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Ngọ đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Dần gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Dần đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Thân gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Thân gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Thân đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Mão gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Mão gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Mão đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Dậu đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:749 Vũ Khúc tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:749 Vũ Khúc tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:755 Vũ Khúc tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:760 Vũ Khúc tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:766 Vũ Khúc tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:769 Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:772 Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:775 Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:778 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:766 Vũ Khúc tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:769 Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:772 Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:775 Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:778 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Thìn đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tuất đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Sửu đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mùi đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tý gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tý gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tý đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Ngọ đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dần gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dần đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Thân gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Thân gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Thân đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mão gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mão gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mão đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dậu đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Hợi</t>
   </si>
 </sst>
 </file>
@@ -3615,10 +3732,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B214"/>
+  <dimension ref="A1:B280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
+      <selection activeCell="B216" sqref="B216:B280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3693,12 +3810,12 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>509</v>
+        <v>418</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>510</v>
+        <v>419</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
@@ -3708,7 +3825,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>511</v>
+        <v>420</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -3798,7 +3915,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>512</v>
+        <v>421</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -5074,6 +5191,526 @@
       </c>
       <c r="B214" s="2" t="s">
         <v>323</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>487</v>
+      </c>
+      <c r="B216" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>488</v>
+      </c>
+      <c r="B217" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>489</v>
+      </c>
+      <c r="B218" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>490</v>
+      </c>
+      <c r="B219" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>491</v>
+      </c>
+      <c r="B220" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>492</v>
+      </c>
+      <c r="B221" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>493</v>
+      </c>
+      <c r="B222" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>494</v>
+      </c>
+      <c r="B223" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>495</v>
+      </c>
+      <c r="B224" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>496</v>
+      </c>
+      <c r="B225" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>497</v>
+      </c>
+      <c r="B226" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>498</v>
+      </c>
+      <c r="B227" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>499</v>
+      </c>
+      <c r="B228" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>500</v>
+      </c>
+      <c r="B229" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>501</v>
+      </c>
+      <c r="B230" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>502</v>
+      </c>
+      <c r="B231" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>503</v>
+      </c>
+      <c r="B232" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>504</v>
+      </c>
+      <c r="B233" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>505</v>
+      </c>
+      <c r="B234" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>506</v>
+      </c>
+      <c r="B235" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>507</v>
+      </c>
+      <c r="B236" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>508</v>
+      </c>
+      <c r="B237" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>509</v>
+      </c>
+      <c r="B238" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>510</v>
+      </c>
+      <c r="B239" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>511</v>
+      </c>
+      <c r="B240" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>512</v>
+      </c>
+      <c r="B241" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>513</v>
+      </c>
+      <c r="B242" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>514</v>
+      </c>
+      <c r="B243" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>515</v>
+      </c>
+      <c r="B244" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>516</v>
+      </c>
+      <c r="B245" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" t="s">
+        <v>517</v>
+      </c>
+      <c r="B246" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>518</v>
+      </c>
+      <c r="B247" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" t="s">
+        <v>519</v>
+      </c>
+      <c r="B248" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>520</v>
+      </c>
+      <c r="B249" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" t="s">
+        <v>521</v>
+      </c>
+      <c r="B250" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>522</v>
+      </c>
+      <c r="B251" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" t="s">
+        <v>523</v>
+      </c>
+      <c r="B252" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>524</v>
+      </c>
+      <c r="B253" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" t="s">
+        <v>525</v>
+      </c>
+      <c r="B254" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>526</v>
+      </c>
+      <c r="B255" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>527</v>
+      </c>
+      <c r="B256" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>528</v>
+      </c>
+      <c r="B257" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>529</v>
+      </c>
+      <c r="B258" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>530</v>
+      </c>
+      <c r="B259" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>531</v>
+      </c>
+      <c r="B260" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>532</v>
+      </c>
+      <c r="B261" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>533</v>
+      </c>
+      <c r="B262" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>534</v>
+      </c>
+      <c r="B263" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>535</v>
+      </c>
+      <c r="B264" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>536</v>
+      </c>
+      <c r="B265" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>537</v>
+      </c>
+      <c r="B266" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>538</v>
+      </c>
+      <c r="B267" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>539</v>
+      </c>
+      <c r="B268" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>540</v>
+      </c>
+      <c r="B269" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>541</v>
+      </c>
+      <c r="B270" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>542</v>
+      </c>
+      <c r="B271" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>543</v>
+      </c>
+      <c r="B272" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>544</v>
+      </c>
+      <c r="B273" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>545</v>
+      </c>
+      <c r="B274" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>546</v>
+      </c>
+      <c r="B275" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>547</v>
+      </c>
+      <c r="B276" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>548</v>
+      </c>
+      <c r="B277" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>549</v>
+      </c>
+      <c r="B278" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>550</v>
+      </c>
+      <c r="B279" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>551</v>
+      </c>
+      <c r="B280" t="s">
+        <v>551</v>
       </c>
     </row>
   </sheetData>
@@ -5134,749 +5771,532 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBE4172-FC39-45CE-BD67-BA23D6FB1A86}">
-  <dimension ref="A1:B92"/>
+  <dimension ref="A2:B66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B92"/>
+      <selection activeCell="B2" sqref="B2:B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>418</v>
-      </c>
-      <c r="B1" t="str">
-        <f>A1</f>
-        <v>Tử Vi tọa thủ cung Mệnh</v>
-      </c>
-    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>487</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>488</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>489</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>490</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>491</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>492</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>493</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>494</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>495</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>496</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>497</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>498</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="B14" t="s">
-        <v>71</v>
+        <v>499</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>500</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="B16" t="s">
-        <v>72</v>
+        <v>501</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>502</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>503</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="B19" t="s">
-        <v>68</v>
+        <v>504</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>505</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>506</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="B22" t="s">
-        <v>232</v>
+        <v>507</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="B23" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="B24" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="B25" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="B26" t="s">
-        <v>285</v>
+        <v>511</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="B27" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="B28" t="s">
-        <v>286</v>
+        <v>513</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="B29" t="s">
-        <v>233</v>
+        <v>514</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="B30" t="s">
-        <v>234</v>
+        <v>515</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="B31" t="s">
-        <v>235</v>
+        <v>516</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="B32" t="s">
-        <v>129</v>
+        <v>517</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="B33" t="s">
-        <v>236</v>
+        <v>518</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="B34" t="s">
-        <v>130</v>
+        <v>519</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="B35" t="s">
-        <v>237</v>
+        <v>520</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>521</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
       <c r="B37" t="s">
-        <v>134</v>
+        <v>522</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="B38" t="s">
-        <v>238</v>
+        <v>523</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
       <c r="B39" t="s">
-        <v>239</v>
+        <v>524</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="B40" t="s">
-        <v>240</v>
+        <v>525</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
       <c r="B41" t="s">
-        <v>241</v>
+        <v>526</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
       <c r="B42" t="s">
-        <v>242</v>
+        <v>527</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="B43" t="s">
-        <v>243</v>
+        <v>528</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="B44" t="s">
-        <v>244</v>
+        <v>529</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="B45" t="s">
-        <v>512</v>
+        <v>530</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
       <c r="B46" t="s">
-        <v>245</v>
+        <v>531</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="B47" t="s">
-        <v>246</v>
+        <v>532</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="B48" t="s">
-        <v>247</v>
+        <v>533</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
       <c r="B49" t="s">
-        <v>248</v>
+        <v>534</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="B50" t="s">
-        <v>249</v>
+        <v>535</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="B51" t="s">
-        <v>250</v>
+        <v>536</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="B52" t="s">
-        <v>251</v>
+        <v>537</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="B53" t="s">
-        <v>252</v>
+        <v>538</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="B54" t="s">
-        <v>253</v>
+        <v>539</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="B55" t="s">
-        <v>261</v>
+        <v>540</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="B56" t="s">
-        <v>269</v>
+        <v>541</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="B57" t="s">
-        <v>277</v>
+        <v>542</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
       <c r="B58" t="s">
-        <v>254</v>
+        <v>543</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="B59" t="s">
-        <v>262</v>
+        <v>544</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B60" t="s">
-        <v>270</v>
+        <v>545</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="B61" t="s">
-        <v>278</v>
+        <v>546</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="B62" t="s">
-        <v>255</v>
+        <v>547</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="B63" t="s">
-        <v>263</v>
+        <v>548</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="B64" t="s">
-        <v>271</v>
+        <v>549</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
       <c r="B65" t="s">
-        <v>279</v>
+        <v>550</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="B66" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>483</v>
-      </c>
-      <c r="B67" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>484</v>
-      </c>
-      <c r="B68" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>485</v>
-      </c>
-      <c r="B69" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>486</v>
-      </c>
-      <c r="B70" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>487</v>
-      </c>
-      <c r="B71" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>488</v>
-      </c>
-      <c r="B72" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>489</v>
-      </c>
-      <c r="B73" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>490</v>
-      </c>
-      <c r="B74" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>491</v>
-      </c>
-      <c r="B75" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>492</v>
-      </c>
-      <c r="B76" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>493</v>
-      </c>
-      <c r="B77" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>494</v>
-      </c>
-      <c r="B78" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>495</v>
-      </c>
-      <c r="B79" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>496</v>
-      </c>
-      <c r="B80" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>497</v>
-      </c>
-      <c r="B81" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>498</v>
-      </c>
-      <c r="B82" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>499</v>
-      </c>
-      <c r="B83" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>500</v>
-      </c>
-      <c r="B84" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>501</v>
-      </c>
-      <c r="B85" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>502</v>
-      </c>
-      <c r="B86" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>503</v>
-      </c>
-      <c r="B87" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>504</v>
-      </c>
-      <c r="B88" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>505</v>
-      </c>
-      <c r="B89" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>506</v>
-      </c>
-      <c r="B90" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>507</v>
-      </c>
-      <c r="B91" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>508</v>
-      </c>
-      <c r="B92" t="s">
-        <v>293</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Luận Phú về Vũ Khúc
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39478FF8-4D35-43E3-817D-1DA56060E2E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319D9890-F3C2-4F67-8C8F-DC61C1118924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="633">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -926,372 +926,6 @@
     <t>Thiên Đồng tọa thủ cung Mệnh</t>
   </si>
   <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Dần gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Dần gặp Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Thân gặp Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tý gặp Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Mão gặp Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tỵ gặp Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Hợi gặp Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Lương ở Dần</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Lương ở Dần gặp các sao cát tinh: Hóa Lộc, Hóa Quyền, Lộc Tồn, Hỏa Linh, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Lương ở Thân</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Lương ở Thân gặp các sao cát tinh: Hóa Lộc, Hóa Quyền, Lộc Tồn, Hỏa Linh, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Ngọ đồng cung Thái Âm gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tý đồng cung Thái Âm gặp các sao Bạch Hổ, Thiên Khốc, Thiên Riêu, Tang Môn</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Việt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Việt gặp các sao cát tinh: Hóa Lộc, Hóa Quyền, Lộc Tồn, Hỏa Linh, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Ngọ gặp Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Sửu gặp Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Mùi gặp Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Tuất gặp Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Thìn gặp Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Thiên Đồng tọa thủ cung Mệnh ở Dậu gặp Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Người tuổi Ấ. có Thiên Đồng tọa thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Người tuổi Ấ. có Thiên Đồng tọa thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Thìn gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Thìn gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tuất gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tuất gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tý gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tý gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Ngọ gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Ngọ gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Dần gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Thân gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Thân gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Sửu đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Mùi đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tỵ gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Hợi gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Mão gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Tỵ đồng cung Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tuổi Bính Liêm Trinh tọa thủ cung Mệnh ở Tỵ đồng cung Hóa Kỵ gặp Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Hợi đồng cung Hóa Kỵ</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tuổi Bính Liêm Trinh tọa thủ cung Mệnh ở Hợi đồng cung Hóa Kỵ gặp Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Mão gặp Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh ở Dậu gặp Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh gặp tứ sát Kình Đà Hỏa Linh</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Liêm Trinh tọa thủ cung Mệnh gặp tứ sát Kình Đà Hỏa Linh và Bạch Hổ</t>
-  </si>
-  <si>
     <t>Tử Vi tọa thủ cung Mệnh và hội chiếu  Địa Kiếp, Địa Không</t>
   </si>
   <si>
@@ -1304,201 +938,6 @@
     <t>Phu Thê</t>
   </si>
   <si>
-    <t>luanmenh.js:722 Vũ Khúc tọa thủ cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Thìn đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Tuất đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Sửu đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Mùi đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Tý gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Tý gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Tý đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Ngọ đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Dần gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Dần đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Thân gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Thân gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Thân đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Mão gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Mão gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Mão đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>luanmenh.js:729 Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:732 Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:735 Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:738 Vũ Khúc tọa thủ cung Mệnh ở Dậu đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:741 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:749 Vũ Khúc tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:749 Vũ Khúc tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:755 Vũ Khúc tọa thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>luanmenh.js:760 Vũ Khúc tọa thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:766 Vũ Khúc tọa thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:769 Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:772 Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:775 Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:778 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:766 Vũ Khúc tọa thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:769 Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:772 Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:775 Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:778 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
     <t>Vũ Khúc tọa thủ cung Mệnh</t>
   </si>
   <si>
@@ -1692,6 +1131,810 @@
   </si>
   <si>
     <t>Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tỵ đồng cung Phá Quân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:826 Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp Phá Quân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:830 Vũ Khúc tọa thủ cung Mệnh ở Tỵ đồng cung Phá Quân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:834 Vũ Khúc tọa thủ cung Mệnh ở Tỵ đồng cung Phá Quân gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:840 Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp Kình Đà Quả Tú</t>
+  </si>
+  <si>
+    <t>luanmenh.js:845 Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp Kình Dương Kiếp Sát</t>
+  </si>
+  <si>
+    <t>luanmenh.js:822 Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:826 Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp Phá Quân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:830 Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:834 Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:840 Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp Kình Đà Quả Tú</t>
+  </si>
+  <si>
+    <t>luanmenh.js:845 Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp Kình Dương Kiếp Sát</t>
+  </si>
+  <si>
+    <t>luanmenh.js:854 Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân gặp Thái Âm, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:862 Người tuổi Giáp có Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân và Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:862 Người tuổi Kỷ có Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân và Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:862 Người tuổi Nhâm có Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân và Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:870 Vũ Khúc tọa thủ cung Mệnh đồng cung Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:877 Vũ Khúc tọa thủ cung Mệnh ở Sửu đồng cung Tham Lang, Kiếp Sát</t>
+  </si>
+  <si>
+    <t>luanmenh.js:877 Vũ Khúc tọa thủ cung Mệnh ở Mùi đồng cung Tham Lang, Kiếp Sát</t>
+  </si>
+  <si>
+    <t>luanmenh.js:884 Vũ Khúc tọa thủ cung Mệnh ở Dần gặp các sao cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền</t>
+  </si>
+  <si>
+    <t>luanmenh.js:884 Vũ Khúc tọa thủ cung Mệnh ở Thân gặp các sao cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền</t>
+  </si>
+  <si>
+    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Thìn đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Thìn đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Thìn đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Tuất đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Tuất đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Tuất đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Sửu đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Sửu đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Sửu đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Mùi đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Mùi đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Mùi đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Tý gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Tý gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Tý đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Tý đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Tý đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Tý gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Ngọ đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Ngọ đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Ngọ đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Dần gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Dần đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Dần đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Dần đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Dần gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Thân gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Thân gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Thân đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Thân đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Thân đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Thân gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Mão gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Mão gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Mão đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Mão đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Mão đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Mão gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Dậu đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Dậu đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Dậu đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp Phá Quân</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tỵ đồng cung Phá Quân gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp Kình Đà Quả Tú</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp Kình Dương Kiếp Sát</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp Phá Quân</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp Kình Đà Quả Tú</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp Kình Dương Kiếp Sát</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân gặp Thái Âm, Tham Lang</t>
+  </si>
+  <si>
+    <t>Người tuổi Giáp có Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân và Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>Người tuổi Kỷ có Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân và Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>Người tuổi Nhâm có Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân và Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh đồng cung Tham Lang</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Sửu đồng cung Tham Lang, Kiếp Sát</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mùi đồng cung Tham Lang, Kiếp Sát</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dần gặp các sao cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Thân gặp các sao cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Thìn đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Thìn đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tuất đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tuất đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Sửu đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Sửu đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mùi đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mùi đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tý đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tý đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Tý gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Ngọ đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Ngọ đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dần đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dần đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dần gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Thân đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Thân đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Thân gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mão đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mão đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Mão gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dậu đồng cung Văn Khúc</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dậu đồng cung Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp Thiên Mã, Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Thìn gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Thìn gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tuất gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tuất gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tý gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tý gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Ngọ gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Ngọ gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Dần gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Thân gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Thân gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Sửu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Sửu đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp cát tinh: Thiên Phủ, Thiên Tướng, Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Mùi gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Mùi đồng cung Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tỵ gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Hợi gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Mão gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Liêm Trinh tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Tỵ đồng cung Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Tuổi Bính Liêm Trinh tọa thủ cung Mệnh ở Tỵ đồng cung Hóa Kỵ gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Hợi đồng cung Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Tuổi Bính Liêm Trinh tọa thủ cung Mệnh ở Hợi đồng cung Hóa Kỵ gặp Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Mão gặp Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh ở Dậu gặp Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh gặp tứ sát Kình Đà Hỏa Linh</t>
+  </si>
+  <si>
+    <t>Liêm Trinh tọa thủ cung Mệnh gặp tứ sát Kình Đà Hỏa Linh và Bạch Hổ</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Dần gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Dần gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Thân gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Tý gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Mão gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Tỵ gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Hợi gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Đồng tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Lương ở Dần</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Lương ở Dần gặp các sao cát tinh: Hóa Lộc, Hóa Quyền, Lộc Tồn, Hỏa Linh, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Lương ở Thân</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Lương ở Thân gặp các sao cát tinh: Hóa Lộc, Hóa Quyền, Lộc Tồn, Hỏa Linh, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Ngọ đồng cung Thái Âm gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Tý đồng cung Thái Âm gặp các sao Bạch Hổ, Thiên Khốc, Thiên Riêu, Tang Môn</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Việt</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh đồng cung Thiên Việt gặp các sao cát tinh: Hóa Lộc, Hóa Quyền, Lộc Tồn, Hỏa Linh, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Ngọ gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Sửu gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Mùi gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Tuất gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Thìn gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Đồng tọa thủ cung Mệnh ở Dậu gặp Thiên Hình, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Người tuổi Đ. có Thiên Đồng tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Người tuổi C. có Thiên Đồng tọa thủ cung Mệnh ở Hợi</t>
   </si>
 </sst>
 </file>
@@ -1741,7 +1984,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3732,10 +4015,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B280"/>
+  <dimension ref="A1:B323"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A206" workbookViewId="0">
-      <selection activeCell="B216" sqref="B216:B280"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="B211" sqref="B211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3810,12 +4093,12 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>418</v>
+        <v>296</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>419</v>
+        <v>297</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
@@ -3825,7 +4108,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>420</v>
+        <v>298</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -3915,7 +4198,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>421</v>
+        <v>299</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -4163,466 +4446,466 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>360</v>
+        <v>514</v>
       </c>
       <c r="B85" t="s">
-        <v>360</v>
+        <v>514</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>361</v>
+        <v>515</v>
       </c>
       <c r="B86" t="s">
-        <v>361</v>
+        <v>515</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>362</v>
+        <v>516</v>
       </c>
       <c r="B87" t="s">
-        <v>362</v>
+        <v>516</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>363</v>
+        <v>517</v>
       </c>
       <c r="B88" t="s">
-        <v>363</v>
+        <v>517</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>364</v>
+        <v>518</v>
       </c>
       <c r="B89" t="s">
-        <v>364</v>
+        <v>518</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>365</v>
+        <v>519</v>
       </c>
       <c r="B90" t="s">
-        <v>365</v>
+        <v>519</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>366</v>
+        <v>520</v>
       </c>
       <c r="B91" t="s">
-        <v>366</v>
+        <v>520</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>367</v>
+        <v>521</v>
       </c>
       <c r="B92" t="s">
-        <v>367</v>
+        <v>521</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>368</v>
+        <v>522</v>
       </c>
       <c r="B93" t="s">
-        <v>368</v>
+        <v>522</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>369</v>
+        <v>523</v>
       </c>
       <c r="B94" t="s">
-        <v>369</v>
+        <v>523</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>370</v>
+        <v>524</v>
       </c>
       <c r="B95" t="s">
-        <v>370</v>
+        <v>524</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>371</v>
+        <v>525</v>
       </c>
       <c r="B96" t="s">
-        <v>371</v>
+        <v>525</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>372</v>
+        <v>526</v>
       </c>
       <c r="B97" t="s">
-        <v>372</v>
+        <v>526</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>373</v>
+        <v>527</v>
       </c>
       <c r="B98" t="s">
-        <v>373</v>
+        <v>527</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>374</v>
+        <v>528</v>
       </c>
       <c r="B99" t="s">
-        <v>374</v>
+        <v>528</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>375</v>
+        <v>529</v>
       </c>
       <c r="B100" t="s">
-        <v>375</v>
+        <v>529</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>376</v>
+        <v>530</v>
       </c>
       <c r="B101" t="s">
-        <v>376</v>
+        <v>530</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>377</v>
+        <v>531</v>
       </c>
       <c r="B102" t="s">
-        <v>377</v>
+        <v>531</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>378</v>
+        <v>532</v>
       </c>
       <c r="B103" t="s">
-        <v>378</v>
+        <v>532</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>379</v>
+        <v>533</v>
       </c>
       <c r="B104" t="s">
-        <v>379</v>
+        <v>533</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>380</v>
+        <v>534</v>
       </c>
       <c r="B105" t="s">
-        <v>380</v>
+        <v>534</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>381</v>
+        <v>535</v>
       </c>
       <c r="B106" t="s">
-        <v>381</v>
+        <v>535</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>382</v>
+        <v>536</v>
       </c>
       <c r="B107" t="s">
-        <v>382</v>
+        <v>536</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>383</v>
+        <v>537</v>
       </c>
       <c r="B108" t="s">
-        <v>383</v>
+        <v>537</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>384</v>
+        <v>538</v>
       </c>
       <c r="B109" t="s">
-        <v>384</v>
+        <v>538</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>385</v>
+        <v>539</v>
       </c>
       <c r="B110" t="s">
-        <v>385</v>
+        <v>539</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>386</v>
+        <v>540</v>
       </c>
       <c r="B111" t="s">
-        <v>386</v>
+        <v>540</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>387</v>
+        <v>541</v>
       </c>
       <c r="B112" t="s">
-        <v>387</v>
+        <v>541</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>388</v>
+        <v>542</v>
       </c>
       <c r="B113" t="s">
-        <v>388</v>
+        <v>542</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>389</v>
+        <v>543</v>
       </c>
       <c r="B114" t="s">
-        <v>389</v>
+        <v>543</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>390</v>
+        <v>544</v>
       </c>
       <c r="B115" t="s">
-        <v>390</v>
+        <v>544</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>391</v>
+        <v>545</v>
       </c>
       <c r="B116" t="s">
-        <v>391</v>
+        <v>545</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>392</v>
+        <v>546</v>
       </c>
       <c r="B117" t="s">
-        <v>392</v>
+        <v>546</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>393</v>
+        <v>547</v>
       </c>
       <c r="B118" t="s">
-        <v>393</v>
+        <v>547</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>394</v>
+        <v>197</v>
       </c>
       <c r="B119" t="s">
-        <v>394</v>
+        <v>197</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>395</v>
+        <v>548</v>
       </c>
       <c r="B120" t="s">
-        <v>395</v>
+        <v>548</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>396</v>
+        <v>549</v>
       </c>
       <c r="B121" t="s">
-        <v>396</v>
+        <v>549</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>397</v>
+        <v>550</v>
       </c>
       <c r="B122" t="s">
-        <v>397</v>
+        <v>550</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>398</v>
+        <v>198</v>
       </c>
       <c r="B123" t="s">
-        <v>398</v>
+        <v>198</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>399</v>
+        <v>551</v>
       </c>
       <c r="B124" t="s">
-        <v>399</v>
+        <v>551</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>400</v>
+        <v>552</v>
       </c>
       <c r="B125" t="s">
-        <v>400</v>
+        <v>552</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>401</v>
+        <v>553</v>
       </c>
       <c r="B126" t="s">
-        <v>401</v>
+        <v>553</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>402</v>
+        <v>199</v>
       </c>
       <c r="B127" t="s">
-        <v>402</v>
+        <v>199</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>403</v>
+        <v>554</v>
       </c>
       <c r="B128" t="s">
-        <v>403</v>
+        <v>554</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>404</v>
+        <v>555</v>
       </c>
       <c r="B129" t="s">
-        <v>404</v>
+        <v>555</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>405</v>
+        <v>556</v>
       </c>
       <c r="B130" t="s">
-        <v>405</v>
+        <v>556</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>406</v>
+        <v>557</v>
       </c>
       <c r="B131" t="s">
-        <v>406</v>
+        <v>557</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>407</v>
+        <v>558</v>
       </c>
       <c r="B132" t="s">
-        <v>407</v>
+        <v>558</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>408</v>
+        <v>559</v>
       </c>
       <c r="B133" t="s">
-        <v>408</v>
+        <v>559</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>409</v>
+        <v>560</v>
       </c>
       <c r="B134" t="s">
-        <v>409</v>
+        <v>560</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>410</v>
+        <v>561</v>
       </c>
       <c r="B135" t="s">
-        <v>410</v>
+        <v>561</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>411</v>
+        <v>562</v>
       </c>
       <c r="B136" t="s">
-        <v>411</v>
+        <v>562</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>412</v>
+        <v>563</v>
       </c>
       <c r="B137" t="s">
-        <v>412</v>
+        <v>563</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>413</v>
+        <v>564</v>
       </c>
       <c r="B138" t="s">
-        <v>413</v>
+        <v>564</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>414</v>
+        <v>565</v>
       </c>
       <c r="B139" t="s">
-        <v>414</v>
+        <v>565</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>415</v>
+        <v>566</v>
       </c>
       <c r="B140" t="s">
-        <v>415</v>
+        <v>566</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>416</v>
+        <v>567</v>
       </c>
       <c r="B141" t="s">
-        <v>416</v>
+        <v>567</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>417</v>
+        <v>568</v>
       </c>
       <c r="B142" t="s">
-        <v>417</v>
+        <v>568</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -4635,1134 +4918,1482 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>296</v>
+        <v>569</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>296</v>
+        <v>569</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>297</v>
+        <v>570</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>297</v>
+        <v>570</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>298</v>
+        <v>571</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>298</v>
+        <v>571</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>299</v>
+        <v>572</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>299</v>
+        <v>572</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>300</v>
+        <v>573</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>300</v>
+        <v>573</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>301</v>
+        <v>574</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>301</v>
+        <v>574</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>302</v>
+        <v>575</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>302</v>
+        <v>575</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>303</v>
+        <v>576</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>303</v>
+        <v>576</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>304</v>
+        <v>577</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>304</v>
+        <v>577</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>305</v>
+        <v>578</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>305</v>
+        <v>578</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>306</v>
+        <v>579</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>306</v>
+        <v>579</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>307</v>
+        <v>580</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>307</v>
+        <v>580</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>308</v>
+        <v>581</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>308</v>
+        <v>581</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>309</v>
+        <v>582</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>309</v>
+        <v>582</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>310</v>
+        <v>583</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>310</v>
+        <v>583</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>311</v>
+        <v>584</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>311</v>
+        <v>584</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>312</v>
+        <v>585</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>312</v>
+        <v>585</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>313</v>
+        <v>586</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>313</v>
+        <v>586</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>314</v>
+        <v>587</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>314</v>
+        <v>587</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>315</v>
+        <v>588</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>315</v>
+        <v>588</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>316</v>
+        <v>589</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>316</v>
+        <v>589</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>317</v>
+        <v>590</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>317</v>
+        <v>590</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>318</v>
+        <v>591</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>318</v>
+        <v>591</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>319</v>
+        <v>592</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>319</v>
+        <v>592</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>320</v>
+        <v>593</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>320</v>
+        <v>593</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>321</v>
+        <v>594</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>321</v>
+        <v>594</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>322</v>
+        <v>595</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>322</v>
+        <v>595</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>323</v>
+        <v>596</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>323</v>
+        <v>596</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>324</v>
+        <v>597</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>324</v>
+        <v>597</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>325</v>
+        <v>598</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>325</v>
+        <v>598</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>326</v>
+        <v>599</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>326</v>
+        <v>599</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>327</v>
+        <v>600</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>327</v>
+        <v>600</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>328</v>
+        <v>601</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>328</v>
+        <v>601</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>329</v>
+        <v>602</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>329</v>
+        <v>602</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>330</v>
+        <v>603</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>330</v>
+        <v>603</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>331</v>
+        <v>604</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>331</v>
+        <v>604</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>332</v>
+        <v>605</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>332</v>
+        <v>605</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>333</v>
+        <v>606</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>333</v>
+        <v>606</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>334</v>
+        <v>607</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>334</v>
+        <v>607</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>335</v>
+        <v>608</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>335</v>
+        <v>608</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>336</v>
+        <v>609</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>336</v>
+        <v>609</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>337</v>
+        <v>610</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>337</v>
+        <v>610</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>338</v>
+        <v>611</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>338</v>
+        <v>611</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>339</v>
+        <v>612</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>339</v>
+        <v>612</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>340</v>
+        <v>613</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>340</v>
+        <v>613</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>341</v>
+        <v>614</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>341</v>
+        <v>614</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>342</v>
+        <v>615</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>342</v>
+        <v>615</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>343</v>
+        <v>616</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>343</v>
+        <v>616</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>344</v>
+        <v>617</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>344</v>
+        <v>617</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>345</v>
+        <v>618</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>345</v>
+        <v>618</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>346</v>
+        <v>619</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>346</v>
+        <v>619</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>347</v>
+        <v>620</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>347</v>
+        <v>620</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>348</v>
+        <v>621</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>348</v>
+        <v>621</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>349</v>
+        <v>622</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>349</v>
+        <v>622</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>350</v>
+        <v>623</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>350</v>
+        <v>623</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>351</v>
+        <v>624</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>351</v>
+        <v>624</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>352</v>
+        <v>625</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>352</v>
+        <v>625</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>353</v>
+        <v>626</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>353</v>
+        <v>626</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>354</v>
+        <v>627</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>354</v>
+        <v>627</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>355</v>
+        <v>628</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>355</v>
+        <v>628</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>356</v>
+        <v>629</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>356</v>
+        <v>629</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>357</v>
+        <v>630</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>357</v>
+        <v>630</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>346</v>
+        <v>631</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>346</v>
+        <v>631</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>334</v>
+        <v>632</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A209" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="B209" s="2" t="s">
-        <v>316</v>
+        <v>632</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A210" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="B210" s="2" t="s">
-        <v>358</v>
+      <c r="A210" t="s">
+        <v>300</v>
+      </c>
+      <c r="B210" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A211" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="B211" s="2" t="s">
-        <v>318</v>
+      <c r="A211" t="s">
+        <v>301</v>
+      </c>
+      <c r="B211" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A212" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="B212" s="2" t="s">
-        <v>321</v>
+      <c r="A212" t="s">
+        <v>302</v>
+      </c>
+      <c r="B212" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A213" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="B213" s="2" t="s">
-        <v>359</v>
+      <c r="A213" t="s">
+        <v>303</v>
+      </c>
+      <c r="B213" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A214" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="B214" s="2" t="s">
-        <v>323</v>
+      <c r="A214" t="s">
+        <v>304</v>
+      </c>
+      <c r="B214" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>305</v>
+      </c>
+      <c r="B215" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>487</v>
+        <v>306</v>
       </c>
       <c r="B216" t="s">
-        <v>487</v>
+        <v>306</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>488</v>
+        <v>307</v>
       </c>
       <c r="B217" t="s">
-        <v>488</v>
+        <v>307</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>489</v>
+        <v>308</v>
       </c>
       <c r="B218" t="s">
-        <v>489</v>
+        <v>308</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>490</v>
+        <v>309</v>
       </c>
       <c r="B219" t="s">
-        <v>490</v>
+        <v>309</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>491</v>
+        <v>310</v>
       </c>
       <c r="B220" t="s">
-        <v>491</v>
+        <v>310</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>492</v>
+        <v>311</v>
       </c>
       <c r="B221" t="s">
-        <v>492</v>
+        <v>311</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>493</v>
+        <v>312</v>
       </c>
       <c r="B222" t="s">
-        <v>493</v>
+        <v>312</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>494</v>
+        <v>313</v>
       </c>
       <c r="B223" t="s">
-        <v>494</v>
+        <v>313</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>495</v>
+        <v>314</v>
       </c>
       <c r="B224" t="s">
-        <v>495</v>
+        <v>314</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>496</v>
+        <v>315</v>
       </c>
       <c r="B225" t="s">
-        <v>496</v>
+        <v>315</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>497</v>
+        <v>316</v>
       </c>
       <c r="B226" t="s">
-        <v>497</v>
+        <v>316</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>498</v>
+        <v>317</v>
       </c>
       <c r="B227" t="s">
-        <v>498</v>
+        <v>317</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>499</v>
+        <v>318</v>
       </c>
       <c r="B228" t="s">
-        <v>499</v>
+        <v>318</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>500</v>
+        <v>319</v>
       </c>
       <c r="B229" t="s">
-        <v>500</v>
+        <v>319</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>501</v>
+        <v>320</v>
       </c>
       <c r="B230" t="s">
-        <v>501</v>
+        <v>320</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>502</v>
+        <v>321</v>
       </c>
       <c r="B231" t="s">
-        <v>502</v>
+        <v>321</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>503</v>
+        <v>322</v>
       </c>
       <c r="B232" t="s">
-        <v>503</v>
+        <v>322</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>504</v>
+        <v>323</v>
       </c>
       <c r="B233" t="s">
-        <v>504</v>
+        <v>323</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>505</v>
+        <v>324</v>
       </c>
       <c r="B234" t="s">
-        <v>505</v>
+        <v>324</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>506</v>
+        <v>325</v>
       </c>
       <c r="B235" t="s">
-        <v>506</v>
+        <v>325</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>507</v>
+        <v>326</v>
       </c>
       <c r="B236" t="s">
-        <v>507</v>
+        <v>326</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>508</v>
+        <v>327</v>
       </c>
       <c r="B237" t="s">
-        <v>508</v>
+        <v>327</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>509</v>
+        <v>328</v>
       </c>
       <c r="B238" t="s">
-        <v>509</v>
+        <v>328</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>510</v>
+        <v>329</v>
       </c>
       <c r="B239" t="s">
-        <v>510</v>
+        <v>329</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>511</v>
+        <v>330</v>
       </c>
       <c r="B240" t="s">
-        <v>511</v>
+        <v>330</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>512</v>
+        <v>331</v>
       </c>
       <c r="B241" t="s">
-        <v>512</v>
+        <v>331</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>513</v>
+        <v>332</v>
       </c>
       <c r="B242" t="s">
-        <v>513</v>
+        <v>332</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>514</v>
+        <v>333</v>
       </c>
       <c r="B243" t="s">
-        <v>514</v>
+        <v>333</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>515</v>
+        <v>334</v>
       </c>
       <c r="B244" t="s">
-        <v>515</v>
+        <v>334</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>516</v>
+        <v>335</v>
       </c>
       <c r="B245" t="s">
-        <v>516</v>
+        <v>335</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>517</v>
+        <v>336</v>
       </c>
       <c r="B246" t="s">
-        <v>517</v>
+        <v>336</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>518</v>
+        <v>337</v>
       </c>
       <c r="B247" t="s">
-        <v>518</v>
+        <v>337</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>519</v>
+        <v>338</v>
       </c>
       <c r="B248" t="s">
-        <v>519</v>
+        <v>338</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>520</v>
+        <v>339</v>
       </c>
       <c r="B249" t="s">
-        <v>520</v>
+        <v>339</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>521</v>
+        <v>340</v>
       </c>
       <c r="B250" t="s">
-        <v>521</v>
+        <v>340</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>522</v>
+        <v>341</v>
       </c>
       <c r="B251" t="s">
-        <v>522</v>
+        <v>341</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>523</v>
+        <v>342</v>
       </c>
       <c r="B252" t="s">
-        <v>523</v>
+        <v>342</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>524</v>
+        <v>343</v>
       </c>
       <c r="B253" t="s">
-        <v>524</v>
+        <v>343</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>525</v>
+        <v>344</v>
       </c>
       <c r="B254" t="s">
-        <v>525</v>
+        <v>344</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>526</v>
+        <v>345</v>
       </c>
       <c r="B255" t="s">
-        <v>526</v>
+        <v>345</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>527</v>
+        <v>346</v>
       </c>
       <c r="B256" t="s">
-        <v>527</v>
+        <v>346</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>528</v>
+        <v>347</v>
       </c>
       <c r="B257" t="s">
-        <v>528</v>
+        <v>347</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>529</v>
+        <v>348</v>
       </c>
       <c r="B258" t="s">
-        <v>529</v>
+        <v>348</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>530</v>
+        <v>349</v>
       </c>
       <c r="B259" t="s">
-        <v>530</v>
+        <v>349</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>531</v>
+        <v>350</v>
       </c>
       <c r="B260" t="s">
-        <v>531</v>
+        <v>350</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>532</v>
+        <v>351</v>
       </c>
       <c r="B261" t="s">
-        <v>532</v>
+        <v>351</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>533</v>
+        <v>352</v>
       </c>
       <c r="B262" t="s">
-        <v>533</v>
+        <v>352</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>534</v>
+        <v>353</v>
       </c>
       <c r="B263" t="s">
-        <v>534</v>
+        <v>353</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>535</v>
+        <v>354</v>
       </c>
       <c r="B264" t="s">
-        <v>535</v>
+        <v>354</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>536</v>
+        <v>355</v>
       </c>
       <c r="B265" t="s">
-        <v>536</v>
+        <v>355</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>537</v>
+        <v>356</v>
       </c>
       <c r="B266" t="s">
-        <v>537</v>
+        <v>356</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>538</v>
+        <v>357</v>
       </c>
       <c r="B267" t="s">
-        <v>538</v>
+        <v>357</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>539</v>
+        <v>358</v>
       </c>
       <c r="B268" t="s">
-        <v>539</v>
+        <v>358</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>540</v>
+        <v>359</v>
       </c>
       <c r="B269" t="s">
-        <v>540</v>
+        <v>359</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>541</v>
+        <v>360</v>
       </c>
       <c r="B270" t="s">
-        <v>541</v>
+        <v>360</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>542</v>
+        <v>361</v>
       </c>
       <c r="B271" t="s">
-        <v>542</v>
+        <v>361</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>543</v>
+        <v>362</v>
       </c>
       <c r="B272" t="s">
-        <v>543</v>
+        <v>362</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>544</v>
+        <v>363</v>
       </c>
       <c r="B273" t="s">
-        <v>544</v>
+        <v>363</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>545</v>
+        <v>364</v>
       </c>
       <c r="B274" t="s">
-        <v>545</v>
+        <v>364</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>546</v>
+        <v>365</v>
       </c>
       <c r="B275" t="s">
-        <v>546</v>
+        <v>365</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>547</v>
+        <v>466</v>
       </c>
       <c r="B276" t="s">
-        <v>547</v>
+        <v>466</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>548</v>
+        <v>467</v>
       </c>
       <c r="B277" t="s">
-        <v>548</v>
+        <v>467</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>549</v>
+        <v>468</v>
       </c>
       <c r="B278" t="s">
-        <v>549</v>
+        <v>468</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>550</v>
+        <v>469</v>
       </c>
       <c r="B279" t="s">
-        <v>550</v>
+        <v>469</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>551</v>
+        <v>470</v>
       </c>
       <c r="B280" t="s">
-        <v>551</v>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>471</v>
+      </c>
+      <c r="B281" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>472</v>
+      </c>
+      <c r="B282" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>473</v>
+      </c>
+      <c r="B283" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>474</v>
+      </c>
+      <c r="B284" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>475</v>
+      </c>
+      <c r="B285" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>476</v>
+      </c>
+      <c r="B286" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>477</v>
+      </c>
+      <c r="B287" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>478</v>
+      </c>
+      <c r="B288" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>479</v>
+      </c>
+      <c r="B289" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>480</v>
+      </c>
+      <c r="B290" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>481</v>
+      </c>
+      <c r="B291" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>482</v>
+      </c>
+      <c r="B292" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>483</v>
+      </c>
+      <c r="B293" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>484</v>
+      </c>
+      <c r="B294" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>485</v>
+      </c>
+      <c r="B295" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>486</v>
+      </c>
+      <c r="B296" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>487</v>
+      </c>
+      <c r="B297" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>488</v>
+      </c>
+      <c r="B298" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>489</v>
+      </c>
+      <c r="B299" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>490</v>
+      </c>
+      <c r="B300" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>491</v>
+      </c>
+      <c r="B301" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>492</v>
+      </c>
+      <c r="B302" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>493</v>
+      </c>
+      <c r="B303" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304" t="s">
+        <v>494</v>
+      </c>
+      <c r="B304" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>495</v>
+      </c>
+      <c r="B305" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A306" t="s">
+        <v>496</v>
+      </c>
+      <c r="B306" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>497</v>
+      </c>
+      <c r="B307" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A308" t="s">
+        <v>498</v>
+      </c>
+      <c r="B308" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>499</v>
+      </c>
+      <c r="B309" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A310" t="s">
+        <v>500</v>
+      </c>
+      <c r="B310" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>501</v>
+      </c>
+      <c r="B311" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A312" t="s">
+        <v>502</v>
+      </c>
+      <c r="B312" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>503</v>
+      </c>
+      <c r="B313" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A314" t="s">
+        <v>504</v>
+      </c>
+      <c r="B314" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>505</v>
+      </c>
+      <c r="B315" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316" t="s">
+        <v>506</v>
+      </c>
+      <c r="B316" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>507</v>
+      </c>
+      <c r="B317" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A318" t="s">
+        <v>508</v>
+      </c>
+      <c r="B318" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>509</v>
+      </c>
+      <c r="B319" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>510</v>
+      </c>
+      <c r="B320" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>511</v>
+      </c>
+      <c r="B321" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>512</v>
+      </c>
+      <c r="B322" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>513</v>
+      </c>
+      <c r="B323" t="s">
+        <v>513</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A215:A1048576 A1:A23 A25:A143">
-    <cfRule type="duplicateValues" dxfId="22" priority="38"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="40"/>
+  <conditionalFormatting sqref="A209:A1048576 A1:A23 A25:A84 A143">
+    <cfRule type="duplicateValues" dxfId="26" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
+    <cfRule type="duplicateValues" dxfId="24" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="33"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B23 B25 B28 B31:B83 B145:B1048576">
+    <cfRule type="duplicateValues" dxfId="22" priority="40"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="duplicateValues" dxfId="21" priority="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26">
     <cfRule type="duplicateValues" dxfId="20" priority="29"/>
     <cfRule type="duplicateValues" dxfId="19" priority="30"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B145:B1048576 B1:B23 B25 B28 B31:B83">
-    <cfRule type="duplicateValues" dxfId="18" priority="37"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24">
+  <conditionalFormatting sqref="B27">
+    <cfRule type="duplicateValues" dxfId="18" priority="27"/>
     <cfRule type="duplicateValues" dxfId="17" priority="28"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26">
-    <cfRule type="duplicateValues" dxfId="16" priority="26"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="27"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="14" priority="24"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="25"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="duplicateValues" dxfId="12" priority="22"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="duplicateValues" dxfId="10" priority="20"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A145:A214">
-    <cfRule type="duplicateValues" dxfId="6" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B143">
-    <cfRule type="duplicateValues" dxfId="3" priority="51"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="52"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84:B142">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A85:A142">
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A145:A208">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5771,532 +6402,820 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBE4172-FC39-45CE-BD67-BA23D6FB1A86}">
-  <dimension ref="A2:B66"/>
+  <dimension ref="A2:B102"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B66"/>
+      <selection activeCell="B2" sqref="B2:B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>422</v>
+        <v>365</v>
       </c>
       <c r="B2" t="s">
-        <v>487</v>
+        <v>365</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>423</v>
+        <v>366</v>
       </c>
       <c r="B3" t="s">
-        <v>488</v>
+        <v>466</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>424</v>
+        <v>367</v>
       </c>
       <c r="B4" t="s">
-        <v>489</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>425</v>
+        <v>368</v>
       </c>
       <c r="B5" t="s">
-        <v>490</v>
+        <v>467</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>426</v>
+        <v>369</v>
       </c>
       <c r="B6" t="s">
-        <v>491</v>
+        <v>468</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>427</v>
+        <v>370</v>
       </c>
       <c r="B7" t="s">
-        <v>492</v>
+        <v>469</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>428</v>
+        <v>371</v>
       </c>
       <c r="B8" t="s">
-        <v>493</v>
+        <v>470</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>429</v>
+        <v>372</v>
       </c>
       <c r="B9" t="s">
-        <v>494</v>
+        <v>471</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>430</v>
+        <v>373</v>
       </c>
       <c r="B10" t="s">
-        <v>495</v>
+        <v>470</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>431</v>
+        <v>374</v>
       </c>
       <c r="B11" t="s">
-        <v>496</v>
+        <v>472</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>432</v>
+        <v>375</v>
       </c>
       <c r="B12" t="s">
-        <v>497</v>
+        <v>473</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>433</v>
+        <v>376</v>
       </c>
       <c r="B13" t="s">
-        <v>498</v>
+        <v>474</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>434</v>
+        <v>377</v>
       </c>
       <c r="B14" t="s">
-        <v>499</v>
+        <v>475</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>435</v>
+        <v>378</v>
       </c>
       <c r="B15" t="s">
-        <v>500</v>
+        <v>476</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>436</v>
+        <v>379</v>
       </c>
       <c r="B16" t="s">
-        <v>501</v>
+        <v>477</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>437</v>
+        <v>380</v>
       </c>
       <c r="B17" t="s">
-        <v>502</v>
+        <v>478</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>438</v>
+        <v>381</v>
       </c>
       <c r="B18" t="s">
-        <v>503</v>
+        <v>479</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>439</v>
+        <v>382</v>
       </c>
       <c r="B19" t="s">
-        <v>504</v>
+        <v>480</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>440</v>
+        <v>383</v>
       </c>
       <c r="B20" t="s">
-        <v>505</v>
+        <v>481</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>441</v>
+        <v>384</v>
       </c>
       <c r="B21" t="s">
-        <v>506</v>
+        <v>482</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>442</v>
+        <v>385</v>
       </c>
       <c r="B22" t="s">
-        <v>507</v>
+        <v>483</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>443</v>
+        <v>386</v>
       </c>
       <c r="B23" t="s">
-        <v>508</v>
+        <v>301</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>444</v>
+        <v>387</v>
       </c>
       <c r="B24" t="s">
-        <v>509</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>445</v>
+        <v>388</v>
       </c>
       <c r="B25" t="s">
-        <v>510</v>
+        <v>303</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>446</v>
+        <v>389</v>
       </c>
       <c r="B26" t="s">
-        <v>511</v>
+        <v>304</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>447</v>
+        <v>390</v>
       </c>
       <c r="B27" t="s">
-        <v>512</v>
+        <v>305</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>448</v>
+        <v>391</v>
       </c>
       <c r="B28" t="s">
-        <v>513</v>
+        <v>484</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>449</v>
+        <v>392</v>
       </c>
       <c r="B29" t="s">
-        <v>514</v>
+        <v>485</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>450</v>
+        <v>393</v>
       </c>
       <c r="B30" t="s">
-        <v>515</v>
+        <v>486</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>451</v>
+        <v>394</v>
       </c>
       <c r="B31" t="s">
-        <v>516</v>
+        <v>306</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>452</v>
+        <v>395</v>
       </c>
       <c r="B32" t="s">
-        <v>517</v>
+        <v>307</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>453</v>
+        <v>396</v>
       </c>
       <c r="B33" t="s">
-        <v>518</v>
+        <v>308</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>454</v>
+        <v>397</v>
       </c>
       <c r="B34" t="s">
-        <v>519</v>
+        <v>309</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>455</v>
+        <v>398</v>
       </c>
       <c r="B35" t="s">
-        <v>520</v>
+        <v>310</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>456</v>
+        <v>399</v>
       </c>
       <c r="B36" t="s">
-        <v>521</v>
+        <v>487</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>457</v>
+        <v>400</v>
       </c>
       <c r="B37" t="s">
-        <v>522</v>
+        <v>488</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>458</v>
+        <v>401</v>
       </c>
       <c r="B38" t="s">
-        <v>523</v>
+        <v>489</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>459</v>
+        <v>402</v>
       </c>
       <c r="B39" t="s">
-        <v>524</v>
+        <v>311</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>460</v>
+        <v>403</v>
       </c>
       <c r="B40" t="s">
-        <v>525</v>
+        <v>312</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>461</v>
+        <v>404</v>
       </c>
       <c r="B41" t="s">
-        <v>526</v>
+        <v>313</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>462</v>
+        <v>405</v>
       </c>
       <c r="B42" t="s">
-        <v>527</v>
+        <v>314</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>463</v>
+        <v>406</v>
       </c>
       <c r="B43" t="s">
-        <v>528</v>
+        <v>315</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>464</v>
+        <v>407</v>
       </c>
       <c r="B44" t="s">
-        <v>529</v>
+        <v>490</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>465</v>
+        <v>408</v>
       </c>
       <c r="B45" t="s">
-        <v>530</v>
+        <v>491</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>466</v>
+        <v>409</v>
       </c>
       <c r="B46" t="s">
-        <v>531</v>
+        <v>492</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>467</v>
+        <v>410</v>
       </c>
       <c r="B47" t="s">
-        <v>532</v>
+        <v>316</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>468</v>
+        <v>411</v>
       </c>
       <c r="B48" t="s">
-        <v>533</v>
+        <v>317</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>469</v>
+        <v>412</v>
       </c>
       <c r="B49" t="s">
-        <v>534</v>
+        <v>318</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>470</v>
+        <v>413</v>
       </c>
       <c r="B50" t="s">
-        <v>535</v>
+        <v>319</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>471</v>
+        <v>414</v>
       </c>
       <c r="B51" t="s">
-        <v>536</v>
+        <v>320</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>472</v>
+        <v>415</v>
       </c>
       <c r="B52" t="s">
-        <v>537</v>
+        <v>493</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>473</v>
+        <v>416</v>
       </c>
       <c r="B53" t="s">
-        <v>538</v>
+        <v>494</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>474</v>
+        <v>417</v>
       </c>
       <c r="B54" t="s">
-        <v>539</v>
+        <v>495</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>475</v>
+        <v>418</v>
       </c>
       <c r="B55" t="s">
-        <v>540</v>
+        <v>321</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>476</v>
+        <v>419</v>
       </c>
       <c r="B56" t="s">
-        <v>541</v>
+        <v>322</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>477</v>
+        <v>420</v>
       </c>
       <c r="B57" t="s">
-        <v>542</v>
+        <v>323</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>478</v>
+        <v>421</v>
       </c>
       <c r="B58" t="s">
-        <v>543</v>
+        <v>324</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>479</v>
+        <v>422</v>
       </c>
       <c r="B59" t="s">
-        <v>544</v>
+        <v>325</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>480</v>
+        <v>423</v>
       </c>
       <c r="B60" t="s">
-        <v>545</v>
+        <v>496</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>481</v>
+        <v>424</v>
       </c>
       <c r="B61" t="s">
-        <v>546</v>
+        <v>497</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>482</v>
+        <v>425</v>
       </c>
       <c r="B62" t="s">
-        <v>547</v>
+        <v>498</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>483</v>
+        <v>426</v>
       </c>
       <c r="B63" t="s">
-        <v>548</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>484</v>
+        <v>427</v>
       </c>
       <c r="B64" t="s">
-        <v>549</v>
+        <v>327</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>485</v>
+        <v>428</v>
       </c>
       <c r="B65" t="s">
-        <v>550</v>
+        <v>328</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>486</v>
+        <v>429</v>
       </c>
       <c r="B66" t="s">
-        <v>551</v>
+        <v>329</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>430</v>
+      </c>
+      <c r="B67" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>431</v>
+      </c>
+      <c r="B68" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>432</v>
+      </c>
+      <c r="B69" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>433</v>
+      </c>
+      <c r="B70" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>434</v>
+      </c>
+      <c r="B71" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>435</v>
+      </c>
+      <c r="B72" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>436</v>
+      </c>
+      <c r="B73" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>437</v>
+      </c>
+      <c r="B74" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>438</v>
+      </c>
+      <c r="B75" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>439</v>
+      </c>
+      <c r="B76" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>440</v>
+      </c>
+      <c r="B77" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>441</v>
+      </c>
+      <c r="B78" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>442</v>
+      </c>
+      <c r="B79" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>443</v>
+      </c>
+      <c r="B80" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>444</v>
+      </c>
+      <c r="B81" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>445</v>
+      </c>
+      <c r="B82" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>446</v>
+      </c>
+      <c r="B83" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>447</v>
+      </c>
+      <c r="B84" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>448</v>
+      </c>
+      <c r="B85" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>449</v>
+      </c>
+      <c r="B86" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>450</v>
+      </c>
+      <c r="B87" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>451</v>
+      </c>
+      <c r="B88" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>452</v>
+      </c>
+      <c r="B89" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>453</v>
+      </c>
+      <c r="B90" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>454</v>
+      </c>
+      <c r="B91" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>455</v>
+      </c>
+      <c r="B92" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>456</v>
+      </c>
+      <c r="B93" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>457</v>
+      </c>
+      <c r="B94" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>458</v>
+      </c>
+      <c r="B95" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>459</v>
+      </c>
+      <c r="B96" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>460</v>
+      </c>
+      <c r="B97" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>461</v>
+      </c>
+      <c r="B98" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>462</v>
+      </c>
+      <c r="B99" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>463</v>
+      </c>
+      <c r="B100" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>464</v>
+      </c>
+      <c r="B101" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>465</v>
+      </c>
+      <c r="B102" t="s">
+        <v>513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Luận xong THái Dương
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{319D9890-F3C2-4F67-8C8F-DC61C1118924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E637207F-584E-443B-A955-982A2488F2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1263" uniqueCount="692">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -1136,306 +1136,6 @@
     <t>Vũ Khúc tọa thủ cung Mệnh ở Tỵ đồng cung Phá Quân</t>
   </si>
   <si>
-    <t>luanmenh.js:826 Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp Phá Quân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:830 Vũ Khúc tọa thủ cung Mệnh ở Tỵ đồng cung Phá Quân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:834 Vũ Khúc tọa thủ cung Mệnh ở Tỵ đồng cung Phá Quân gặp Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:840 Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp Kình Đà Quả Tú</t>
-  </si>
-  <si>
-    <t>luanmenh.js:845 Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp Kình Dương Kiếp Sát</t>
-  </si>
-  <si>
-    <t>luanmenh.js:822 Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:826 Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp Phá Quân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:830 Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:834 Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân gặp Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:840 Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp Kình Đà Quả Tú</t>
-  </si>
-  <si>
-    <t>luanmenh.js:845 Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp Kình Dương Kiếp Sát</t>
-  </si>
-  <si>
-    <t>luanmenh.js:854 Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân gặp Thái Âm, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:862 Người tuổi Giáp có Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân và Hỏa Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:862 Người tuổi Kỷ có Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân và Hỏa Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:862 Người tuổi Nhâm có Vũ Khúc tọa thủ cung Mệnh ở Hợi đồng cung Phá Quân và Hỏa Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:870 Vũ Khúc tọa thủ cung Mệnh đồng cung Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:877 Vũ Khúc tọa thủ cung Mệnh ở Sửu đồng cung Tham Lang, Kiếp Sát</t>
-  </si>
-  <si>
-    <t>luanmenh.js:877 Vũ Khúc tọa thủ cung Mệnh ở Mùi đồng cung Tham Lang, Kiếp Sát</t>
-  </si>
-  <si>
-    <t>luanmenh.js:884 Vũ Khúc tọa thủ cung Mệnh ở Dần gặp các sao cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền</t>
-  </si>
-  <si>
-    <t>luanmenh.js:884 Vũ Khúc tọa thủ cung Mệnh ở Thân gặp các sao cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền</t>
-  </si>
-  <si>
-    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Thìn đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Thìn đồng cung Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Thìn đồng cung Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Thìn gặp Thiên Mã, Hóa Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Tuất đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Tuất đồng cung Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Tuất đồng cung Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Tuất gặp Thiên Mã, Hóa Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Sửu đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Sửu đồng cung Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Sửu đồng cung Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Sửu gặp Thiên Mã, Hóa Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Mùi đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Mùi đồng cung Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Mùi đồng cung Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Mùi gặp Thiên Mã, Hóa Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Tý gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Tý gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Tý đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Tý đồng cung Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Tý đồng cung Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Tý gặp Thiên Mã, Hóa Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Ngọ đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Ngọ đồng cung Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Ngọ đồng cung Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Ngọ gặp Thiên Mã, Hóa Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Dần gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Dần đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Dần đồng cung Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Dần đồng cung Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Dần gặp Thiên Mã, Hóa Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Thân gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Thân gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Thân đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Thân đồng cung Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Thân đồng cung Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Thân gặp Thiên Mã, Hóa Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Mão gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Mão gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Mão đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Mão đồng cung Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Mão đồng cung Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Mão gặp Thiên Mã, Hóa Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:894 Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:899 Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh: Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:903 Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ: Thiên Hình, Hóa Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:907 Vũ Khúc tọa thủ cung Mệnh ở Dậu đồng cung Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:911 Quý Chị có Vũ Khúc tọa thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:915 Vũ Khúc tọa thủ cung Mệnh ở Dậu đồng cung Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:919 Vũ Khúc tọa thủ cung Mệnh ở Dậu đồng cung Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:924 Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp Thiên Mã, Hóa Lộc</t>
-  </si>
-  <si>
     <t>Vũ Khúc tọa thủ cung Mệnh ở Tỵ gặp Phá Quân</t>
   </si>
   <si>
@@ -1935,6 +1635,483 @@
   </si>
   <si>
     <t>Người tuổi C. có Thiên Đồng tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:990 Thái Dương tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:993 Thái Dương tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:996 Thái Dương tọa thủ cung Mệnh ở Tỵ gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1000 Quý Chị có Thái Dương tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:987 Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:990 Thái Dương tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:993 Thái Dương tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:996 Thái Dương tọa thủ cung Mệnh ở Ngọ gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1000 Quý Chị có Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:987 Thái Dương tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:990 Thái Dương tọa thủ cung Mệnh ở Dần gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:993 Thái Dương tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:996 Thái Dương tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1000 Quý Chị có Thái Dương tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:987 Thái Dương tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:990 Thái Dương tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:993 Thái Dương tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:996 Thái Dương tọa thủ cung Mệnh ở Mão gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1000 Quý Chị có Thái Dương tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:987 Thái Dương tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:990 Thái Dương tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:993 Thái Dương tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:996 Thái Dương tọa thủ cung Mệnh ở Thìn gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1000 Quý Chị có Thái Dương tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:987 Thái Dương tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:990 Thái Dương tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:993 Thái Dương tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:996 Thái Dương tọa thủ cung Mệnh ở Sửu gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1000 Quý Chị có Thái Dương tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:987 Thái Dương tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:990 Thái Dương tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:993 Thái Dương tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:996 Thái Dương tọa thủ cung Mệnh ở Mùi gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1000 Quý Chị có Thái Dương tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1009 Thái Dương tọa thủ cung Mệnh ở Sửu đồng cung Hóa Kỵ và không gặp Kình Đà Không Kiếp Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1009 Thái Dương tọa thủ cung Mệnh ở Mùi đồng cung Hóa Kỵ và không gặp Kình Đà Không Kiếp Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1015 Thái Dương tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1018 Thái Dương tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1021 Thái Dương tọa thủ cung Mệnh ở Thân gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1024 Thái Dương tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1015 Thái Dương tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1018 Thái Dương tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1021 Thái Dương tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1024 Thái Dương tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1015 Thái Dương tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1018 Thái Dương tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1021 Thái Dương tọa thủ cung Mệnh ở Tuất gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1024 Thái Dương tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1015 Thái Dương tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1018 Thái Dương tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1021 Thái Dương tọa thủ cung Mệnh ở Hợi gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1024 Thái Dương tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1015 Thái Dương tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1018 Thái Dương tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1021 Thái Dương tọa thủ cung Mệnh ở Tý gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1024 Thái Dương tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1034 Thái Dương tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1037 Thái Dương tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1034 Thái Dương tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1037 Thái Dương tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1047 Thái Dương tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1047 Thái Dương tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1047 Thái Dương tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1054 Thái Dương tọa thủ cung Mệnh đồng cung Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1061 Người tuổi Canh có Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1061 Người tuổi Tân có Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1061 Người tuổi Nhâm có Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1061 Người tuổi Kỷ có Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1067 Người tuổi Bính có Thái Dương tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1067 Người tuổi Đinh có Thái Dương tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1073 Thái Dương tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1073 Thái Dương tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1079 Thái Dương tọa thủ cung Mệnh đồng cung Thái Âm</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1085 Thái Dương Thái Âm đồng cung tại Mùi hội chiếu cung Mệnh tại Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1089 Thái Dương Thái Âm hội chiếu cung Mệnh tại Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1094 Thái Dương Thái Âm đồng cung tại Sửu hội chiếu cung Mệnh tại Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1099 Thái Dương Thái Âm hội chiếu cung Mệnh tại Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1103 Thái Dương tại Mão Thái Âm ở Hợi hội chiếu cung Mệnh tại Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1107 Cung Mệnh Vô Chính Diệu gặp Thái Dương, Thái Âm</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1112 Thái Dương tọa thủ cung Mệnh ở Sửu đồng cung Thái Âm gặp Văn Xương, Văn Khúc, Thiên Khôi, Đào Hồng</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1112 Thái Dương tọa thủ cung Mệnh ở Mùi đồng cung Thái Âm gặp Văn Xương, Văn Khúc, Thiên Khôi, Đào Hồng</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1118 Thái Dương tọa thủ cung Mệnh ở Sửu đồng cung Thái Âm gặp Khoa Lộc Quyền</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Tỵ gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Thái Dương tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Ngọ gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Dần gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Thái Dương tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Mão gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Thái Dương tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Thìn gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Thái Dương tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Sửu gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Thái Dương tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Mệnh ở Mùi gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Quý Chị có Thái Dương tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Sửu đồng cung Hóa Kỵ và không gặp Kình Đà Không Kiếp Thiên Riêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Mùi đồng cung Hóa Kỵ và không gặp Kình Đà Không Kiếp Thiên Riêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Thân gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Tuất gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Hợi gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Tý gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh đồng cung Thiên Hình</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Người tuổi Canh có Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Người tuổi Tân có Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Người tuổi Nhâm có Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Người tuổi Kỷ có Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Người tuổi Bính có Thái Dương tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Người tuổi Đinh có Thái Dương tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh đồng cung Thái Âm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương Thái Âm đồng cung tại Mùi hội chiếu cung Mệnh tại Sửu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương Thái Âm hội chiếu cung Mệnh tại Sửu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương Thái Âm đồng cung tại Sửu hội chiếu cung Mệnh tại Mùi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương Thái Âm hội chiếu cung Mệnh tại Mùi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tại Mão Thái Âm ở Hợi hội chiếu cung Mệnh tại Sửu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cung Mệnh Vô Chính Diệu gặp Thái Dương, Thái Âm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Sửu đồng cung Thái Âm gặp Văn Xương, Văn Khúc, Thiên Khôi, Đào Hồng</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Mùi đồng cung Thái Âm gặp Văn Xương, Văn Khúc, Thiên Khôi, Đào Hồng</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Sửu đồng cung Thái Âm gặp Khoa Lộc Quyền</t>
   </si>
 </sst>
 </file>
@@ -4015,10 +4192,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B323"/>
+  <dimension ref="A1:B407"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="B211" sqref="B211"/>
+    <sheetView tabSelected="1" topLeftCell="A319" workbookViewId="0">
+      <selection activeCell="B325" sqref="B325:B407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4446,274 +4623,274 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>514</v>
+        <v>414</v>
       </c>
       <c r="B85" t="s">
-        <v>514</v>
+        <v>414</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>515</v>
+        <v>415</v>
       </c>
       <c r="B86" t="s">
-        <v>515</v>
+        <v>415</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>516</v>
+        <v>416</v>
       </c>
       <c r="B87" t="s">
-        <v>516</v>
+        <v>416</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>517</v>
+        <v>417</v>
       </c>
       <c r="B88" t="s">
-        <v>517</v>
+        <v>417</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>518</v>
+        <v>418</v>
       </c>
       <c r="B89" t="s">
-        <v>518</v>
+        <v>418</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>519</v>
+        <v>419</v>
       </c>
       <c r="B90" t="s">
-        <v>519</v>
+        <v>419</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>520</v>
+        <v>420</v>
       </c>
       <c r="B91" t="s">
-        <v>520</v>
+        <v>420</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>521</v>
+        <v>421</v>
       </c>
       <c r="B92" t="s">
-        <v>521</v>
+        <v>421</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>522</v>
+        <v>422</v>
       </c>
       <c r="B93" t="s">
-        <v>522</v>
+        <v>422</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>523</v>
+        <v>423</v>
       </c>
       <c r="B94" t="s">
-        <v>523</v>
+        <v>423</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>524</v>
+        <v>424</v>
       </c>
       <c r="B95" t="s">
-        <v>524</v>
+        <v>424</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>525</v>
+        <v>425</v>
       </c>
       <c r="B96" t="s">
-        <v>525</v>
+        <v>425</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>526</v>
+        <v>426</v>
       </c>
       <c r="B97" t="s">
-        <v>526</v>
+        <v>426</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>527</v>
+        <v>427</v>
       </c>
       <c r="B98" t="s">
-        <v>527</v>
+        <v>427</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>528</v>
+        <v>428</v>
       </c>
       <c r="B99" t="s">
-        <v>528</v>
+        <v>428</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>529</v>
+        <v>429</v>
       </c>
       <c r="B100" t="s">
-        <v>529</v>
+        <v>429</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>530</v>
+        <v>430</v>
       </c>
       <c r="B101" t="s">
-        <v>530</v>
+        <v>430</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>531</v>
+        <v>431</v>
       </c>
       <c r="B102" t="s">
-        <v>531</v>
+        <v>431</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>532</v>
+        <v>432</v>
       </c>
       <c r="B103" t="s">
-        <v>532</v>
+        <v>432</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>533</v>
+        <v>433</v>
       </c>
       <c r="B104" t="s">
-        <v>533</v>
+        <v>433</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>534</v>
+        <v>434</v>
       </c>
       <c r="B105" t="s">
-        <v>534</v>
+        <v>434</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>535</v>
+        <v>435</v>
       </c>
       <c r="B106" t="s">
-        <v>535</v>
+        <v>435</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>536</v>
+        <v>436</v>
       </c>
       <c r="B107" t="s">
-        <v>536</v>
+        <v>436</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>537</v>
+        <v>437</v>
       </c>
       <c r="B108" t="s">
-        <v>537</v>
+        <v>437</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>538</v>
+        <v>438</v>
       </c>
       <c r="B109" t="s">
-        <v>538</v>
+        <v>438</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>539</v>
+        <v>439</v>
       </c>
       <c r="B110" t="s">
-        <v>539</v>
+        <v>439</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>540</v>
+        <v>440</v>
       </c>
       <c r="B111" t="s">
-        <v>540</v>
+        <v>440</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>541</v>
+        <v>441</v>
       </c>
       <c r="B112" t="s">
-        <v>541</v>
+        <v>441</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>542</v>
+        <v>442</v>
       </c>
       <c r="B113" t="s">
-        <v>542</v>
+        <v>442</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>543</v>
+        <v>443</v>
       </c>
       <c r="B114" t="s">
-        <v>543</v>
+        <v>443</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>544</v>
+        <v>444</v>
       </c>
       <c r="B115" t="s">
-        <v>544</v>
+        <v>444</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>545</v>
+        <v>445</v>
       </c>
       <c r="B116" t="s">
-        <v>545</v>
+        <v>445</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>546</v>
+        <v>446</v>
       </c>
       <c r="B117" t="s">
-        <v>546</v>
+        <v>446</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>547</v>
+        <v>447</v>
       </c>
       <c r="B118" t="s">
-        <v>547</v>
+        <v>447</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -4726,26 +4903,26 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>548</v>
+        <v>448</v>
       </c>
       <c r="B120" t="s">
-        <v>548</v>
+        <v>448</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>549</v>
+        <v>449</v>
       </c>
       <c r="B121" t="s">
-        <v>549</v>
+        <v>449</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>550</v>
+        <v>450</v>
       </c>
       <c r="B122" t="s">
-        <v>550</v>
+        <v>450</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -4758,26 +4935,26 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>551</v>
+        <v>451</v>
       </c>
       <c r="B124" t="s">
-        <v>551</v>
+        <v>451</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>552</v>
+        <v>452</v>
       </c>
       <c r="B125" t="s">
-        <v>552</v>
+        <v>452</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>553</v>
+        <v>453</v>
       </c>
       <c r="B126" t="s">
-        <v>553</v>
+        <v>453</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -4790,122 +4967,122 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>554</v>
+        <v>454</v>
       </c>
       <c r="B128" t="s">
-        <v>554</v>
+        <v>454</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>555</v>
+        <v>455</v>
       </c>
       <c r="B129" t="s">
-        <v>555</v>
+        <v>455</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>556</v>
+        <v>456</v>
       </c>
       <c r="B130" t="s">
-        <v>556</v>
+        <v>456</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>557</v>
+        <v>457</v>
       </c>
       <c r="B131" t="s">
-        <v>557</v>
+        <v>457</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>558</v>
+        <v>458</v>
       </c>
       <c r="B132" t="s">
-        <v>558</v>
+        <v>458</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>559</v>
+        <v>459</v>
       </c>
       <c r="B133" t="s">
-        <v>559</v>
+        <v>459</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>560</v>
+        <v>460</v>
       </c>
       <c r="B134" t="s">
-        <v>560</v>
+        <v>460</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>561</v>
+        <v>461</v>
       </c>
       <c r="B135" t="s">
-        <v>561</v>
+        <v>461</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>562</v>
+        <v>462</v>
       </c>
       <c r="B136" t="s">
-        <v>562</v>
+        <v>462</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>563</v>
+        <v>463</v>
       </c>
       <c r="B137" t="s">
-        <v>563</v>
+        <v>463</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>564</v>
+        <v>464</v>
       </c>
       <c r="B138" t="s">
-        <v>564</v>
+        <v>464</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>565</v>
+        <v>465</v>
       </c>
       <c r="B139" t="s">
-        <v>565</v>
+        <v>465</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>566</v>
+        <v>466</v>
       </c>
       <c r="B140" t="s">
-        <v>566</v>
+        <v>466</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>567</v>
+        <v>467</v>
       </c>
       <c r="B141" t="s">
-        <v>567</v>
+        <v>467</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>568</v>
+        <v>468</v>
       </c>
       <c r="B142" t="s">
-        <v>568</v>
+        <v>468</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
@@ -4918,514 +5095,514 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
-        <v>569</v>
+        <v>469</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>569</v>
+        <v>469</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
-        <v>570</v>
+        <v>470</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>570</v>
+        <v>470</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
-        <v>571</v>
+        <v>471</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>571</v>
+        <v>471</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
-        <v>572</v>
+        <v>472</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>572</v>
+        <v>472</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
-        <v>573</v>
+        <v>473</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>573</v>
+        <v>473</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
-        <v>574</v>
+        <v>474</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>574</v>
+        <v>474</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
-        <v>575</v>
+        <v>475</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>575</v>
+        <v>475</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
-        <v>576</v>
+        <v>476</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>576</v>
+        <v>476</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
-        <v>577</v>
+        <v>477</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>577</v>
+        <v>477</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
-        <v>578</v>
+        <v>478</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>578</v>
+        <v>478</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
-        <v>579</v>
+        <v>479</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>579</v>
+        <v>479</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
-        <v>580</v>
+        <v>480</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>580</v>
+        <v>480</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
-        <v>581</v>
+        <v>481</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>581</v>
+        <v>481</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
-        <v>582</v>
+        <v>482</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>582</v>
+        <v>482</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
-        <v>583</v>
+        <v>483</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>583</v>
+        <v>483</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
-        <v>584</v>
+        <v>484</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>584</v>
+        <v>484</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
-        <v>585</v>
+        <v>485</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>585</v>
+        <v>485</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
-        <v>586</v>
+        <v>486</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>586</v>
+        <v>486</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
-        <v>587</v>
+        <v>487</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>587</v>
+        <v>487</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
-        <v>588</v>
+        <v>488</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>588</v>
+        <v>488</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
-        <v>589</v>
+        <v>489</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>589</v>
+        <v>489</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
-        <v>590</v>
+        <v>490</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>590</v>
+        <v>490</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
-        <v>591</v>
+        <v>491</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>591</v>
+        <v>491</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
-        <v>592</v>
+        <v>492</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>592</v>
+        <v>492</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
-        <v>593</v>
+        <v>493</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>593</v>
+        <v>493</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
-        <v>594</v>
+        <v>494</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>594</v>
+        <v>494</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
-        <v>595</v>
+        <v>495</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>595</v>
+        <v>495</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="2" t="s">
-        <v>596</v>
+        <v>496</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>596</v>
+        <v>496</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
-        <v>597</v>
+        <v>497</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>597</v>
+        <v>497</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
-        <v>598</v>
+        <v>498</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>598</v>
+        <v>498</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
-        <v>599</v>
+        <v>499</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>599</v>
+        <v>499</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>600</v>
+        <v>500</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="2" t="s">
-        <v>601</v>
+        <v>501</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>601</v>
+        <v>501</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="2" t="s">
-        <v>602</v>
+        <v>502</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>602</v>
+        <v>502</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
-        <v>603</v>
+        <v>503</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>603</v>
+        <v>503</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
-        <v>604</v>
+        <v>504</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>604</v>
+        <v>504</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>605</v>
+        <v>505</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>605</v>
+        <v>505</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>606</v>
+        <v>506</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>606</v>
+        <v>506</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>607</v>
+        <v>507</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>607</v>
+        <v>507</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>608</v>
+        <v>508</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>608</v>
+        <v>508</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>609</v>
+        <v>509</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>609</v>
+        <v>509</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>610</v>
+        <v>510</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>610</v>
+        <v>510</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>611</v>
+        <v>511</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>611</v>
+        <v>511</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>612</v>
+        <v>512</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>612</v>
+        <v>512</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>613</v>
+        <v>513</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>613</v>
+        <v>513</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>614</v>
+        <v>514</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>614</v>
+        <v>514</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>615</v>
+        <v>515</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>615</v>
+        <v>515</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>616</v>
+        <v>516</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>616</v>
+        <v>516</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>617</v>
+        <v>517</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>617</v>
+        <v>517</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>618</v>
+        <v>518</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>618</v>
+        <v>518</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>619</v>
+        <v>519</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>619</v>
+        <v>519</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>620</v>
+        <v>520</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>620</v>
+        <v>520</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>621</v>
+        <v>521</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>621</v>
+        <v>521</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>622</v>
+        <v>522</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>622</v>
+        <v>522</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>623</v>
+        <v>523</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>623</v>
+        <v>523</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>624</v>
+        <v>524</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>624</v>
+        <v>524</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>625</v>
+        <v>525</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>625</v>
+        <v>525</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>626</v>
+        <v>526</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>626</v>
+        <v>526</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>627</v>
+        <v>527</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>627</v>
+        <v>527</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>628</v>
+        <v>528</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>628</v>
+        <v>528</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>629</v>
+        <v>529</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>629</v>
+        <v>529</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>630</v>
+        <v>530</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>630</v>
+        <v>530</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>631</v>
+        <v>531</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>631</v>
+        <v>531</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>632</v>
+        <v>532</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>632</v>
+        <v>532</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
@@ -5958,442 +6135,1110 @@
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>466</v>
+        <v>366</v>
       </c>
       <c r="B276" t="s">
-        <v>466</v>
+        <v>366</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>467</v>
+        <v>367</v>
       </c>
       <c r="B277" t="s">
-        <v>467</v>
+        <v>367</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>468</v>
+        <v>368</v>
       </c>
       <c r="B278" t="s">
-        <v>468</v>
+        <v>368</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>469</v>
+        <v>369</v>
       </c>
       <c r="B279" t="s">
-        <v>469</v>
+        <v>369</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>470</v>
+        <v>370</v>
       </c>
       <c r="B280" t="s">
-        <v>470</v>
+        <v>370</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>471</v>
+        <v>371</v>
       </c>
       <c r="B281" t="s">
-        <v>471</v>
+        <v>371</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>472</v>
+        <v>372</v>
       </c>
       <c r="B282" t="s">
-        <v>472</v>
+        <v>372</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>473</v>
+        <v>373</v>
       </c>
       <c r="B283" t="s">
-        <v>473</v>
+        <v>373</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>474</v>
+        <v>374</v>
       </c>
       <c r="B284" t="s">
-        <v>474</v>
+        <v>374</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>475</v>
+        <v>375</v>
       </c>
       <c r="B285" t="s">
-        <v>475</v>
+        <v>375</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>476</v>
+        <v>376</v>
       </c>
       <c r="B286" t="s">
-        <v>476</v>
+        <v>376</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>477</v>
+        <v>377</v>
       </c>
       <c r="B287" t="s">
-        <v>477</v>
+        <v>377</v>
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>478</v>
+        <v>378</v>
       </c>
       <c r="B288" t="s">
-        <v>478</v>
+        <v>378</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>479</v>
+        <v>379</v>
       </c>
       <c r="B289" t="s">
-        <v>479</v>
+        <v>379</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>480</v>
+        <v>380</v>
       </c>
       <c r="B290" t="s">
-        <v>480</v>
+        <v>380</v>
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>481</v>
+        <v>381</v>
       </c>
       <c r="B291" t="s">
-        <v>481</v>
+        <v>381</v>
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>482</v>
+        <v>382</v>
       </c>
       <c r="B292" t="s">
-        <v>482</v>
+        <v>382</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>483</v>
+        <v>383</v>
       </c>
       <c r="B293" t="s">
-        <v>483</v>
+        <v>383</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>484</v>
+        <v>384</v>
       </c>
       <c r="B294" t="s">
-        <v>484</v>
+        <v>384</v>
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>485</v>
+        <v>385</v>
       </c>
       <c r="B295" t="s">
-        <v>485</v>
+        <v>385</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>486</v>
+        <v>386</v>
       </c>
       <c r="B296" t="s">
-        <v>486</v>
+        <v>386</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>487</v>
+        <v>387</v>
       </c>
       <c r="B297" t="s">
-        <v>487</v>
+        <v>387</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>488</v>
+        <v>388</v>
       </c>
       <c r="B298" t="s">
-        <v>488</v>
+        <v>388</v>
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>489</v>
+        <v>389</v>
       </c>
       <c r="B299" t="s">
-        <v>489</v>
+        <v>389</v>
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>490</v>
+        <v>390</v>
       </c>
       <c r="B300" t="s">
-        <v>490</v>
+        <v>390</v>
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>491</v>
+        <v>391</v>
       </c>
       <c r="B301" t="s">
-        <v>491</v>
+        <v>391</v>
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>492</v>
+        <v>392</v>
       </c>
       <c r="B302" t="s">
-        <v>492</v>
+        <v>392</v>
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>493</v>
+        <v>393</v>
       </c>
       <c r="B303" t="s">
-        <v>493</v>
+        <v>393</v>
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>494</v>
+        <v>394</v>
       </c>
       <c r="B304" t="s">
-        <v>494</v>
+        <v>394</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>495</v>
+        <v>395</v>
       </c>
       <c r="B305" t="s">
-        <v>495</v>
+        <v>395</v>
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>496</v>
+        <v>396</v>
       </c>
       <c r="B306" t="s">
-        <v>496</v>
+        <v>396</v>
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>497</v>
+        <v>397</v>
       </c>
       <c r="B307" t="s">
-        <v>497</v>
+        <v>397</v>
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>498</v>
+        <v>398</v>
       </c>
       <c r="B308" t="s">
-        <v>498</v>
+        <v>398</v>
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>499</v>
+        <v>399</v>
       </c>
       <c r="B309" t="s">
-        <v>499</v>
+        <v>399</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="B310" t="s">
-        <v>500</v>
+        <v>400</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>501</v>
+        <v>401</v>
       </c>
       <c r="B311" t="s">
-        <v>501</v>
+        <v>401</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>502</v>
+        <v>402</v>
       </c>
       <c r="B312" t="s">
-        <v>502</v>
+        <v>402</v>
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>503</v>
+        <v>403</v>
       </c>
       <c r="B313" t="s">
-        <v>503</v>
+        <v>403</v>
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>504</v>
+        <v>404</v>
       </c>
       <c r="B314" t="s">
-        <v>504</v>
+        <v>404</v>
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>505</v>
+        <v>405</v>
       </c>
       <c r="B315" t="s">
-        <v>505</v>
+        <v>405</v>
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>506</v>
+        <v>406</v>
       </c>
       <c r="B316" t="s">
-        <v>506</v>
+        <v>406</v>
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>507</v>
+        <v>407</v>
       </c>
       <c r="B317" t="s">
-        <v>507</v>
+        <v>407</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>508</v>
+        <v>408</v>
       </c>
       <c r="B318" t="s">
-        <v>508</v>
+        <v>408</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>509</v>
+        <v>409</v>
       </c>
       <c r="B319" t="s">
-        <v>509</v>
+        <v>409</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>510</v>
+        <v>410</v>
       </c>
       <c r="B320" t="s">
-        <v>510</v>
+        <v>410</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>511</v>
+        <v>411</v>
       </c>
       <c r="B321" t="s">
-        <v>511</v>
+        <v>411</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>512</v>
+        <v>412</v>
       </c>
       <c r="B322" t="s">
-        <v>512</v>
+        <v>412</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>513</v>
+        <v>413</v>
       </c>
       <c r="B323" t="s">
-        <v>513</v>
+        <v>413</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>533</v>
+      </c>
+      <c r="B325" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>616</v>
+      </c>
+      <c r="B326" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>617</v>
+      </c>
+      <c r="B327" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>618</v>
+      </c>
+      <c r="B328" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>619</v>
+      </c>
+      <c r="B329" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>620</v>
+      </c>
+      <c r="B330" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>621</v>
+      </c>
+      <c r="B331" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>622</v>
+      </c>
+      <c r="B332" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>623</v>
+      </c>
+      <c r="B333" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>624</v>
+      </c>
+      <c r="B334" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>625</v>
+      </c>
+      <c r="B335" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>626</v>
+      </c>
+      <c r="B336" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>627</v>
+      </c>
+      <c r="B337" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>628</v>
+      </c>
+      <c r="B338" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>629</v>
+      </c>
+      <c r="B339" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>630</v>
+      </c>
+      <c r="B340" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A341" t="s">
+        <v>631</v>
+      </c>
+      <c r="B341" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A342" t="s">
+        <v>632</v>
+      </c>
+      <c r="B342" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>633</v>
+      </c>
+      <c r="B343" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>634</v>
+      </c>
+      <c r="B344" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>635</v>
+      </c>
+      <c r="B345" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>636</v>
+      </c>
+      <c r="B346" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>637</v>
+      </c>
+      <c r="B347" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>638</v>
+      </c>
+      <c r="B348" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>639</v>
+      </c>
+      <c r="B349" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>640</v>
+      </c>
+      <c r="B350" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>641</v>
+      </c>
+      <c r="B351" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>642</v>
+      </c>
+      <c r="B352" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>643</v>
+      </c>
+      <c r="B353" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>644</v>
+      </c>
+      <c r="B354" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>645</v>
+      </c>
+      <c r="B355" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>646</v>
+      </c>
+      <c r="B356" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>647</v>
+      </c>
+      <c r="B357" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>648</v>
+      </c>
+      <c r="B358" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>649</v>
+      </c>
+      <c r="B359" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>650</v>
+      </c>
+      <c r="B360" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>651</v>
+      </c>
+      <c r="B361" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>652</v>
+      </c>
+      <c r="B362" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>653</v>
+      </c>
+      <c r="B363" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>654</v>
+      </c>
+      <c r="B364" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>655</v>
+      </c>
+      <c r="B365" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>656</v>
+      </c>
+      <c r="B366" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>657</v>
+      </c>
+      <c r="B367" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>658</v>
+      </c>
+      <c r="B368" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>659</v>
+      </c>
+      <c r="B369" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>660</v>
+      </c>
+      <c r="B370" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>661</v>
+      </c>
+      <c r="B371" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>662</v>
+      </c>
+      <c r="B372" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>663</v>
+      </c>
+      <c r="B373" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>664</v>
+      </c>
+      <c r="B374" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>665</v>
+      </c>
+      <c r="B375" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>666</v>
+      </c>
+      <c r="B376" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>667</v>
+      </c>
+      <c r="B377" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>668</v>
+      </c>
+      <c r="B378" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>669</v>
+      </c>
+      <c r="B379" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>670</v>
+      </c>
+      <c r="B380" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>671</v>
+      </c>
+      <c r="B381" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>668</v>
+      </c>
+      <c r="B382" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>672</v>
+      </c>
+      <c r="B383" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>664</v>
+      </c>
+      <c r="B384" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>673</v>
+      </c>
+      <c r="B385" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>652</v>
+      </c>
+      <c r="B386" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>660</v>
+      </c>
+      <c r="B387" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>668</v>
+      </c>
+      <c r="B388" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>674</v>
+      </c>
+      <c r="B389" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>675</v>
+      </c>
+      <c r="B390" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>676</v>
+      </c>
+      <c r="B391" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>677</v>
+      </c>
+      <c r="B392" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>678</v>
+      </c>
+      <c r="B393" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>679</v>
+      </c>
+      <c r="B394" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>680</v>
+      </c>
+      <c r="B395" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>681</v>
+      </c>
+      <c r="B396" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>652</v>
+      </c>
+      <c r="B397" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>682</v>
+      </c>
+      <c r="B398" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>683</v>
+      </c>
+      <c r="B399" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>684</v>
+      </c>
+      <c r="B400" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="401" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>685</v>
+      </c>
+      <c r="B401" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>686</v>
+      </c>
+      <c r="B402" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>687</v>
+      </c>
+      <c r="B403" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>688</v>
+      </c>
+      <c r="B404" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>689</v>
+      </c>
+      <c r="B405" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>690</v>
+      </c>
+      <c r="B406" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>691</v>
+      </c>
+      <c r="B407" t="s">
+        <v>691</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A209:A1048576 A1:A23 A25:A84 A143">
-    <cfRule type="duplicateValues" dxfId="26" priority="41"/>
-    <cfRule type="duplicateValues" dxfId="25" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="24" priority="32"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="35"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B23 B25 B28 B31:B83 B145:B1048576">
-    <cfRule type="duplicateValues" dxfId="22" priority="40"/>
+  <conditionalFormatting sqref="B1:B23 B25 B28 B31:B83 B145:B324 B408:B1048576">
+    <cfRule type="duplicateValues" dxfId="22" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="21" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="duplicateValues" dxfId="20" priority="29"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="18" priority="27"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="duplicateValues" dxfId="16" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="duplicateValues" dxfId="14" priority="23"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="12" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="10" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B143">
-    <cfRule type="duplicateValues" dxfId="8" priority="54"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84:B142">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A145:A208">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A145:A208">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="B325:B407">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6402,820 +7247,676 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBE4172-FC39-45CE-BD67-BA23D6FB1A86}">
-  <dimension ref="A2:B102"/>
+  <dimension ref="A1:B83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B102"/>
+      <selection activeCell="B1" sqref="B1:B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B1" t="s">
+        <v>533</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>365</v>
+        <v>534</v>
       </c>
       <c r="B2" t="s">
-        <v>365</v>
+        <v>616</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>366</v>
+        <v>535</v>
       </c>
       <c r="B3" t="s">
-        <v>466</v>
+        <v>617</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>367</v>
+        <v>536</v>
       </c>
       <c r="B4" t="s">
-        <v>365</v>
+        <v>618</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>368</v>
+        <v>537</v>
       </c>
       <c r="B5" t="s">
-        <v>467</v>
+        <v>619</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>369</v>
+        <v>538</v>
       </c>
       <c r="B6" t="s">
-        <v>468</v>
+        <v>620</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>370</v>
+        <v>539</v>
       </c>
       <c r="B7" t="s">
-        <v>469</v>
+        <v>621</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>371</v>
+        <v>540</v>
       </c>
       <c r="B8" t="s">
-        <v>470</v>
+        <v>622</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>372</v>
+        <v>541</v>
       </c>
       <c r="B9" t="s">
-        <v>471</v>
+        <v>623</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>373</v>
+        <v>542</v>
       </c>
       <c r="B10" t="s">
-        <v>470</v>
+        <v>624</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>374</v>
+        <v>543</v>
       </c>
       <c r="B11" t="s">
-        <v>472</v>
+        <v>625</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>375</v>
+        <v>544</v>
       </c>
       <c r="B12" t="s">
-        <v>473</v>
+        <v>626</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>376</v>
+        <v>545</v>
       </c>
       <c r="B13" t="s">
-        <v>474</v>
+        <v>627</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>377</v>
+        <v>546</v>
       </c>
       <c r="B14" t="s">
-        <v>475</v>
+        <v>628</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>378</v>
+        <v>547</v>
       </c>
       <c r="B15" t="s">
-        <v>476</v>
+        <v>629</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>379</v>
+        <v>548</v>
       </c>
       <c r="B16" t="s">
-        <v>477</v>
+        <v>630</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>380</v>
+        <v>549</v>
       </c>
       <c r="B17" t="s">
-        <v>478</v>
+        <v>631</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>381</v>
+        <v>550</v>
       </c>
       <c r="B18" t="s">
-        <v>479</v>
+        <v>632</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>382</v>
+        <v>551</v>
       </c>
       <c r="B19" t="s">
-        <v>480</v>
+        <v>633</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>383</v>
+        <v>552</v>
       </c>
       <c r="B20" t="s">
-        <v>481</v>
+        <v>634</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>384</v>
+        <v>553</v>
       </c>
       <c r="B21" t="s">
-        <v>482</v>
+        <v>635</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>385</v>
+        <v>554</v>
       </c>
       <c r="B22" t="s">
-        <v>483</v>
+        <v>636</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>386</v>
+        <v>555</v>
       </c>
       <c r="B23" t="s">
-        <v>301</v>
+        <v>637</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>387</v>
+        <v>556</v>
       </c>
       <c r="B24" t="s">
-        <v>302</v>
+        <v>638</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>388</v>
+        <v>557</v>
       </c>
       <c r="B25" t="s">
-        <v>303</v>
+        <v>639</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>389</v>
+        <v>558</v>
       </c>
       <c r="B26" t="s">
-        <v>304</v>
+        <v>640</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>390</v>
+        <v>559</v>
       </c>
       <c r="B27" t="s">
-        <v>305</v>
+        <v>641</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>391</v>
+        <v>560</v>
       </c>
       <c r="B28" t="s">
-        <v>484</v>
+        <v>642</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>392</v>
+        <v>561</v>
       </c>
       <c r="B29" t="s">
-        <v>485</v>
+        <v>643</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>393</v>
+        <v>562</v>
       </c>
       <c r="B30" t="s">
-        <v>486</v>
+        <v>644</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>394</v>
+        <v>563</v>
       </c>
       <c r="B31" t="s">
-        <v>306</v>
+        <v>645</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>395</v>
+        <v>564</v>
       </c>
       <c r="B32" t="s">
-        <v>307</v>
+        <v>646</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>396</v>
+        <v>565</v>
       </c>
       <c r="B33" t="s">
-        <v>308</v>
+        <v>647</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>397</v>
+        <v>566</v>
       </c>
       <c r="B34" t="s">
-        <v>309</v>
+        <v>648</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>398</v>
+        <v>567</v>
       </c>
       <c r="B35" t="s">
-        <v>310</v>
+        <v>649</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>399</v>
+        <v>568</v>
       </c>
       <c r="B36" t="s">
-        <v>487</v>
+        <v>650</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>400</v>
+        <v>569</v>
       </c>
       <c r="B37" t="s">
-        <v>488</v>
+        <v>651</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>401</v>
+        <v>570</v>
       </c>
       <c r="B38" t="s">
-        <v>489</v>
+        <v>652</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>402</v>
+        <v>571</v>
       </c>
       <c r="B39" t="s">
-        <v>311</v>
+        <v>653</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>403</v>
+        <v>572</v>
       </c>
       <c r="B40" t="s">
-        <v>312</v>
+        <v>654</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>404</v>
+        <v>573</v>
       </c>
       <c r="B41" t="s">
-        <v>313</v>
+        <v>655</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>405</v>
+        <v>574</v>
       </c>
       <c r="B42" t="s">
-        <v>314</v>
+        <v>656</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>406</v>
+        <v>575</v>
       </c>
       <c r="B43" t="s">
-        <v>315</v>
+        <v>657</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>407</v>
+        <v>576</v>
       </c>
       <c r="B44" t="s">
-        <v>490</v>
+        <v>658</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>408</v>
+        <v>577</v>
       </c>
       <c r="B45" t="s">
-        <v>491</v>
+        <v>659</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>409</v>
+        <v>578</v>
       </c>
       <c r="B46" t="s">
-        <v>492</v>
+        <v>660</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>410</v>
+        <v>579</v>
       </c>
       <c r="B47" t="s">
-        <v>316</v>
+        <v>661</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>411</v>
+        <v>580</v>
       </c>
       <c r="B48" t="s">
-        <v>317</v>
+        <v>662</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>412</v>
+        <v>581</v>
       </c>
       <c r="B49" t="s">
-        <v>318</v>
+        <v>663</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>413</v>
+        <v>582</v>
       </c>
       <c r="B50" t="s">
-        <v>319</v>
+        <v>664</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>414</v>
+        <v>583</v>
       </c>
       <c r="B51" t="s">
-        <v>320</v>
+        <v>665</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>415</v>
+        <v>584</v>
       </c>
       <c r="B52" t="s">
-        <v>493</v>
+        <v>666</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>416</v>
+        <v>585</v>
       </c>
       <c r="B53" t="s">
-        <v>494</v>
+        <v>667</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>417</v>
+        <v>586</v>
       </c>
       <c r="B54" t="s">
-        <v>495</v>
+        <v>668</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>418</v>
+        <v>587</v>
       </c>
       <c r="B55" t="s">
-        <v>321</v>
+        <v>669</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>419</v>
+        <v>588</v>
       </c>
       <c r="B56" t="s">
-        <v>322</v>
+        <v>670</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>420</v>
+        <v>589</v>
       </c>
       <c r="B57" t="s">
-        <v>323</v>
+        <v>671</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>421</v>
+        <v>590</v>
       </c>
       <c r="B58" t="s">
-        <v>324</v>
+        <v>668</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>422</v>
+        <v>591</v>
       </c>
       <c r="B59" t="s">
-        <v>325</v>
+        <v>672</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>423</v>
+        <v>592</v>
       </c>
       <c r="B60" t="s">
-        <v>496</v>
+        <v>664</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>424</v>
+        <v>593</v>
       </c>
       <c r="B61" t="s">
-        <v>497</v>
+        <v>673</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>425</v>
+        <v>594</v>
       </c>
       <c r="B62" t="s">
-        <v>498</v>
+        <v>652</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>426</v>
+        <v>595</v>
       </c>
       <c r="B63" t="s">
-        <v>326</v>
+        <v>660</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>427</v>
+        <v>596</v>
       </c>
       <c r="B64" t="s">
-        <v>327</v>
+        <v>668</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>428</v>
+        <v>597</v>
       </c>
       <c r="B65" t="s">
-        <v>328</v>
+        <v>674</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>429</v>
+        <v>598</v>
       </c>
       <c r="B66" t="s">
-        <v>329</v>
+        <v>675</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>430</v>
+        <v>599</v>
       </c>
       <c r="B67" t="s">
-        <v>330</v>
+        <v>676</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>431</v>
+        <v>600</v>
       </c>
       <c r="B68" t="s">
-        <v>499</v>
+        <v>677</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>432</v>
+        <v>601</v>
       </c>
       <c r="B69" t="s">
-        <v>500</v>
+        <v>678</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>433</v>
+        <v>602</v>
       </c>
       <c r="B70" t="s">
-        <v>501</v>
+        <v>679</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>434</v>
+        <v>603</v>
       </c>
       <c r="B71" t="s">
-        <v>331</v>
+        <v>680</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>435</v>
+        <v>604</v>
       </c>
       <c r="B72" t="s">
-        <v>332</v>
+        <v>681</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>436</v>
+        <v>605</v>
       </c>
       <c r="B73" t="s">
-        <v>333</v>
+        <v>652</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>437</v>
+        <v>606</v>
       </c>
       <c r="B74" t="s">
-        <v>334</v>
+        <v>682</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>438</v>
+        <v>607</v>
       </c>
       <c r="B75" t="s">
-        <v>335</v>
+        <v>683</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>439</v>
+        <v>608</v>
       </c>
       <c r="B76" t="s">
-        <v>502</v>
+        <v>684</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>440</v>
+        <v>609</v>
       </c>
       <c r="B77" t="s">
-        <v>503</v>
+        <v>685</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>441</v>
+        <v>610</v>
       </c>
       <c r="B78" t="s">
-        <v>504</v>
+        <v>686</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>442</v>
+        <v>611</v>
       </c>
       <c r="B79" t="s">
-        <v>336</v>
+        <v>687</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>443</v>
+        <v>612</v>
       </c>
       <c r="B80" t="s">
-        <v>337</v>
+        <v>688</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>444</v>
+        <v>613</v>
       </c>
       <c r="B81" t="s">
-        <v>338</v>
+        <v>689</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>445</v>
+        <v>614</v>
       </c>
       <c r="B82" t="s">
-        <v>339</v>
+        <v>690</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>446</v>
+        <v>615</v>
       </c>
       <c r="B83" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>447</v>
-      </c>
-      <c r="B84" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>448</v>
-      </c>
-      <c r="B85" t="s">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>449</v>
-      </c>
-      <c r="B86" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>450</v>
-      </c>
-      <c r="B87" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>451</v>
-      </c>
-      <c r="B88" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>452</v>
-      </c>
-      <c r="B89" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>453</v>
-      </c>
-      <c r="B90" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>454</v>
-      </c>
-      <c r="B91" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>455</v>
-      </c>
-      <c r="B92" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>456</v>
-      </c>
-      <c r="B93" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>457</v>
-      </c>
-      <c r="B94" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>458</v>
-      </c>
-      <c r="B95" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>459</v>
-      </c>
-      <c r="B96" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>460</v>
-      </c>
-      <c r="B97" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>461</v>
-      </c>
-      <c r="B98" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>462</v>
-      </c>
-      <c r="B99" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>463</v>
-      </c>
-      <c r="B100" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>464</v>
-      </c>
-      <c r="B101" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>465</v>
-      </c>
-      <c r="B102" t="s">
-        <v>513</v>
+        <v>691</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Luan Menh thien co file excel
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667AAFA9-F1EB-429E-A95D-CA446C35B646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A57A37-8838-4922-87D2-96805862A2B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1433" uniqueCount="783">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -1640,252 +1640,6 @@
     <t>Thái Dương tọa thủ cung Mệnh ở Tỵ</t>
   </si>
   <si>
-    <t>luanmenh.js:990 Thái Dương tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:993 Thái Dương tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:996 Thái Dương tọa thủ cung Mệnh ở Tỵ gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1000 Quý Chị có Thái Dương tọa thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:987 Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:990 Thái Dương tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:993 Thái Dương tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:996 Thái Dương tọa thủ cung Mệnh ở Ngọ gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1000 Quý Chị có Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:987 Thái Dương tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:990 Thái Dương tọa thủ cung Mệnh ở Dần gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:993 Thái Dương tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:996 Thái Dương tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1000 Quý Chị có Thái Dương tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:987 Thái Dương tọa thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>luanmenh.js:990 Thái Dương tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:993 Thái Dương tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:996 Thái Dương tọa thủ cung Mệnh ở Mão gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1000 Quý Chị có Thái Dương tọa thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>luanmenh.js:987 Thái Dương tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:990 Thái Dương tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:993 Thái Dương tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:996 Thái Dương tọa thủ cung Mệnh ở Thìn gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1000 Quý Chị có Thái Dương tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:987 Thái Dương tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:990 Thái Dương tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:993 Thái Dương tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:996 Thái Dương tọa thủ cung Mệnh ở Sửu gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1000 Quý Chị có Thái Dương tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:987 Thái Dương tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:990 Thái Dương tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:993 Thái Dương tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:996 Thái Dương tọa thủ cung Mệnh ở Mùi gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1000 Quý Chị có Thái Dương tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1009 Thái Dương tọa thủ cung Mệnh ở Sửu đồng cung Hóa Kỵ và không gặp Kình Đà Không Kiếp Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1009 Thái Dương tọa thủ cung Mệnh ở Mùi đồng cung Hóa Kỵ và không gặp Kình Đà Không Kiếp Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1015 Thái Dương tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1018 Thái Dương tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1021 Thái Dương tọa thủ cung Mệnh ở Thân gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1024 Thái Dương tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1015 Thái Dương tọa thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1018 Thái Dương tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1021 Thái Dương tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1024 Thái Dương tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1015 Thái Dương tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1018 Thái Dương tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1021 Thái Dương tọa thủ cung Mệnh ở Tuất gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1024 Thái Dương tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1015 Thái Dương tọa thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1018 Thái Dương tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1021 Thái Dương tọa thủ cung Mệnh ở Hợi gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1024 Thái Dương tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1015 Thái Dương tọa thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1018 Thái Dương tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1021 Thái Dương tọa thủ cung Mệnh ở Tý gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1024 Thái Dương tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1034 Thái Dương tọa thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1037 Thái Dương tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1034 Thái Dương tọa thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1037 Thái Dương tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1047 Thái Dương tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1047 Thái Dương tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1047 Thái Dương tọa thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1054 Thái Dương tọa thủ cung Mệnh đồng cung Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1061 Người tuổi Canh có Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1061 Người tuổi Tân có Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1061 Người tuổi Nhâm có Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1061 Người tuổi Kỷ có Thái Dương tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1067 Người tuổi Bính có Thái Dương tọa thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1067 Người tuổi Đinh có Thái Dương tọa thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1073 Thái Dương tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1073 Thái Dương tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1079 Thái Dương tọa thủ cung Mệnh đồng cung Thái Âm</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1085 Thái Dương Thái Âm đồng cung tại Mùi hội chiếu cung Mệnh tại Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1089 Thái Dương Thái Âm hội chiếu cung Mệnh tại Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1094 Thái Dương Thái Âm đồng cung tại Sửu hội chiếu cung Mệnh tại Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1099 Thái Dương Thái Âm hội chiếu cung Mệnh tại Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1103 Thái Dương tại Mão Thái Âm ở Hợi hội chiếu cung Mệnh tại Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1107 Cung Mệnh Vô Chính Diệu gặp Thái Dương, Thái Âm</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1112 Thái Dương tọa thủ cung Mệnh ở Sửu đồng cung Thái Âm gặp Văn Xương, Văn Khúc, Thiên Khôi, Đào Hồng</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1112 Thái Dương tọa thủ cung Mệnh ở Mùi đồng cung Thái Âm gặp Văn Xương, Văn Khúc, Thiên Khôi, Đào Hồng</t>
-  </si>
-  <si>
-    <t>luanmenh.js:1118 Thái Dương tọa thủ cung Mệnh ở Sửu đồng cung Thái Âm gặp Khoa Lộc Quyền</t>
-  </si>
-  <si>
     <t>Thái Dương tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ</t>
   </si>
   <si>
@@ -2112,6 +1866,525 @@
   </si>
   <si>
     <t xml:space="preserve"> Thái Dương tọa thủ cung Mệnh ở Sửu đồng cung Thái Âm gặp Khoa Lộc Quyền</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1104 Thiên Cơ tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1107 Thiên Cơ tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1110 Thiên Cơ tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1113 Thiên Cơ tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1116 Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1101 Thiên Cơ tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1104 Thiên Cơ tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1107 Thiên Cơ tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1110 Thiên Cơ tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1113 Thiên Cơ tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1116 Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1101 Thiên Cơ tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1104 Thiên Cơ tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1107 Thiên Cơ tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1110 Thiên Cơ tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1113 Thiên Cơ tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1116 Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1101 Thiên Cơ tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1104 Thiên Cơ tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1107 Thiên Cơ tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1110 Thiên Cơ tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1113 Thiên Cơ tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1116 Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1101 Thiên Cơ tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1104 Thiên Cơ tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1107 Thiên Cơ tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1110 Thiên Cơ tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1113 Thiên Cơ tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1116 Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1101 Thiên Cơ tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1104 Thiên Cơ tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1107 Thiên Cơ tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1110 Thiên Cơ tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1113 Thiên Cơ tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1116 Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1101 Thiên Cơ tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1104 Thiên Cơ tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1107 Thiên Cơ tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1110 Thiên Cơ tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1113 Thiên Cơ tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1116 Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1101 Thiên Cơ tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1104 Thiên Cơ tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1107 Thiên Cơ tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1110 Thiên Cơ tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1113 Thiên Cơ tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1116 Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1101 Thiên Cơ tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1104 Thiên Cơ tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1107 Thiên Cơ tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1110 Thiên Cơ tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1113 Thiên Cơ tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1116 Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1101 Thiên Cơ tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1104 Thiên Cơ tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1107 Thiên Cơ tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1110 Thiên Cơ tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1113 Thiên Cơ tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1116 Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1124 Quý Anh có Thiên Cơ tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1127 Thiên Cơ tọa thủ cung Mệnh ở Thìn đồng cung Thiên Lương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1130 Thiên Cơ tọa thủ cung Mệnh ở Thìn đồng cung Thiên Lương gặp các sao Kình Đà Hỏa Linh Tướng</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1124 Quý Anh có Thiên Cơ tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1127 Thiên Cơ tọa thủ cung Mệnh ở Tuất đồng cung Thiên Lương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1130 Thiên Cơ tọa thủ cung Mệnh ở Tuất đồng cung Thiên Lương gặp các sao Kình Đà Hỏa Linh Tướng</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1145 Người tuổi Ất có Thiên Cơ tọa thủ cung Mệnh ở Mão gặp Song Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1145 Người tuổi Tân có Thiên Cơ tọa thủ cung Mệnh ở Mão gặp Song Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1145 Người tuổi Kỷ có Thiên Cơ tọa thủ cung Mệnh ở Mão gặp Song Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1145 Người tuổi Bính có Thiên Cơ tọa thủ cung Mệnh ở Mão gặp Song Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1145 Người tuổi Ất có Thiên Cơ tọa thủ cung Mệnh ở Dậu gặp Song Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1145 Người tuổi Tân có Thiên Cơ tọa thủ cung Mệnh ở Dậu gặp Song Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1145 Người tuổi Kỷ có Thiên Cơ tọa thủ cung Mệnh ở Dậu gặp Song Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1145 Người tuổi Bính có Thiên Cơ tọa thủ cung Mệnh ở Dậu gặp Song Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1157 Người tuổi Ất có Thiên Cơ tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1157 Người tuổi Bính có Thiên Cơ tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1157 Người tuổi Đinh có Thiên Cơ tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1157 Người tuổi Ất có Thiên Cơ tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1157 Người tuổi Bính có Thiên Cơ tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1157 Người tuổi Đinh có Thiên Cơ tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1168 Thiên Cơ tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1171 Thiên Cơ tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1174 Thiên Cơ tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1168 Thiên Cơ tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1171 Thiên Cơ tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1174 Thiên Cơ tọa thủ cung Mệnh ở Hợi gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:1181 Thiên Cơ tọa thủ cung Mệnh gặp Thiên Đồng, Thiên Lương, Thái Âm</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Tả Phù, Hữu Bật, Hóa Lộc, Thiên Hình, Thiên Y, Ân Quang, Thiên Quý</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Tả Phù, Hữu Bật, Linh Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>Quý Anh có Thiên Cơ tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Thìn đồng cung Thiên Lương</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Thìn đồng cung Thiên Lương gặp các sao Kình Đà Hỏa Linh Tướng</t>
+  </si>
+  <si>
+    <t>Quý Anh có Thiên Cơ tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tuất đồng cung Thiên Lương</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Tuất đồng cung Thiên Lương gặp các sao Kình Đà Hỏa Linh Tướng</t>
+  </si>
+  <si>
+    <t>Người tuổi Ất có Thiên Cơ tọa thủ cung Mệnh ở Mão gặp Song Hao</t>
+  </si>
+  <si>
+    <t>Người tuổi Tân có Thiên Cơ tọa thủ cung Mệnh ở Mão gặp Song Hao</t>
+  </si>
+  <si>
+    <t>Người tuổi Kỷ có Thiên Cơ tọa thủ cung Mệnh ở Mão gặp Song Hao</t>
+  </si>
+  <si>
+    <t>Người tuổi Bính có Thiên Cơ tọa thủ cung Mệnh ở Mão gặp Song Hao</t>
+  </si>
+  <si>
+    <t>Người tuổi Ất có Thiên Cơ tọa thủ cung Mệnh ở Dậu gặp Song Hao</t>
+  </si>
+  <si>
+    <t>Người tuổi Tân có Thiên Cơ tọa thủ cung Mệnh ở Dậu gặp Song Hao</t>
+  </si>
+  <si>
+    <t>Người tuổi Kỷ có Thiên Cơ tọa thủ cung Mệnh ở Dậu gặp Song Hao</t>
+  </si>
+  <si>
+    <t>Người tuổi Bính có Thiên Cơ tọa thủ cung Mệnh ở Dậu gặp Song Hao</t>
+  </si>
+  <si>
+    <t>Người tuổi Ất có Thiên Cơ tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Người tuổi Bính có Thiên Cơ tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Người tuổi Đinh có Thiên Cơ tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Người tuổi Ất có Thiên Cơ tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Người tuổi Bính có Thiên Cơ tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Người tuổi Đinh có Thiên Cơ tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh ở Hợi gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Mệnh gặp Thiên Đồng, Thiên Lương, Thái Âm</t>
   </si>
 </sst>
 </file>
@@ -4192,10 +4465,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B401"/>
+  <dimension ref="A1:B489"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A313" workbookViewId="0">
-      <selection activeCell="A383" sqref="A383:XFD383"/>
+    <sheetView tabSelected="1" topLeftCell="A382" workbookViewId="0">
+      <selection activeCell="B403" sqref="B403:B489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6527,610 +6800,1306 @@
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>616</v>
+        <v>534</v>
       </c>
       <c r="B326" t="s">
-        <v>616</v>
+        <v>534</v>
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>617</v>
+        <v>535</v>
       </c>
       <c r="B327" t="s">
-        <v>617</v>
+        <v>535</v>
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>618</v>
+        <v>536</v>
       </c>
       <c r="B328" t="s">
-        <v>618</v>
+        <v>536</v>
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>619</v>
+        <v>537</v>
       </c>
       <c r="B329" t="s">
-        <v>619</v>
+        <v>537</v>
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>620</v>
+        <v>538</v>
       </c>
       <c r="B330" t="s">
-        <v>620</v>
+        <v>538</v>
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>621</v>
+        <v>539</v>
       </c>
       <c r="B331" t="s">
-        <v>621</v>
+        <v>539</v>
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>622</v>
+        <v>540</v>
       </c>
       <c r="B332" t="s">
-        <v>622</v>
+        <v>540</v>
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>623</v>
+        <v>541</v>
       </c>
       <c r="B333" t="s">
-        <v>623</v>
+        <v>541</v>
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>624</v>
+        <v>542</v>
       </c>
       <c r="B334" t="s">
-        <v>624</v>
+        <v>542</v>
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>625</v>
+        <v>543</v>
       </c>
       <c r="B335" t="s">
-        <v>625</v>
+        <v>543</v>
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>626</v>
+        <v>544</v>
       </c>
       <c r="B336" t="s">
-        <v>626</v>
+        <v>544</v>
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>627</v>
+        <v>545</v>
       </c>
       <c r="B337" t="s">
-        <v>627</v>
+        <v>545</v>
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>628</v>
+        <v>546</v>
       </c>
       <c r="B338" t="s">
-        <v>628</v>
+        <v>546</v>
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>629</v>
+        <v>547</v>
       </c>
       <c r="B339" t="s">
-        <v>629</v>
+        <v>547</v>
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>630</v>
+        <v>548</v>
       </c>
       <c r="B340" t="s">
-        <v>630</v>
+        <v>548</v>
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>631</v>
+        <v>549</v>
       </c>
       <c r="B341" t="s">
-        <v>631</v>
+        <v>549</v>
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>632</v>
+        <v>550</v>
       </c>
       <c r="B342" t="s">
-        <v>632</v>
+        <v>550</v>
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>633</v>
+        <v>551</v>
       </c>
       <c r="B343" t="s">
-        <v>633</v>
+        <v>551</v>
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>634</v>
+        <v>552</v>
       </c>
       <c r="B344" t="s">
-        <v>634</v>
+        <v>552</v>
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>635</v>
+        <v>553</v>
       </c>
       <c r="B345" t="s">
-        <v>635</v>
+        <v>553</v>
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>636</v>
+        <v>554</v>
       </c>
       <c r="B346" t="s">
-        <v>636</v>
+        <v>554</v>
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>637</v>
+        <v>555</v>
       </c>
       <c r="B347" t="s">
-        <v>637</v>
+        <v>555</v>
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>638</v>
+        <v>556</v>
       </c>
       <c r="B348" t="s">
-        <v>638</v>
+        <v>556</v>
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>639</v>
+        <v>557</v>
       </c>
       <c r="B349" t="s">
-        <v>639</v>
+        <v>557</v>
       </c>
     </row>
     <row r="350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>640</v>
+        <v>558</v>
       </c>
       <c r="B350" t="s">
-        <v>640</v>
+        <v>558</v>
       </c>
     </row>
     <row r="351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>641</v>
+        <v>559</v>
       </c>
       <c r="B351" t="s">
-        <v>641</v>
+        <v>559</v>
       </c>
     </row>
     <row r="352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>642</v>
+        <v>560</v>
       </c>
       <c r="B352" t="s">
-        <v>642</v>
+        <v>560</v>
       </c>
     </row>
     <row r="353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>643</v>
+        <v>561</v>
       </c>
       <c r="B353" t="s">
-        <v>643</v>
+        <v>561</v>
       </c>
     </row>
     <row r="354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>644</v>
+        <v>562</v>
       </c>
       <c r="B354" t="s">
-        <v>644</v>
+        <v>562</v>
       </c>
     </row>
     <row r="355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>645</v>
+        <v>563</v>
       </c>
       <c r="B355" t="s">
-        <v>645</v>
+        <v>563</v>
       </c>
     </row>
     <row r="356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>646</v>
+        <v>564</v>
       </c>
       <c r="B356" t="s">
-        <v>646</v>
+        <v>564</v>
       </c>
     </row>
     <row r="357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>647</v>
+        <v>565</v>
       </c>
       <c r="B357" t="s">
-        <v>647</v>
+        <v>565</v>
       </c>
     </row>
     <row r="358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>648</v>
+        <v>566</v>
       </c>
       <c r="B358" t="s">
-        <v>648</v>
+        <v>566</v>
       </c>
     </row>
     <row r="359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>649</v>
+        <v>567</v>
       </c>
       <c r="B359" t="s">
-        <v>649</v>
+        <v>567</v>
       </c>
     </row>
     <row r="360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>650</v>
+        <v>568</v>
       </c>
       <c r="B360" t="s">
-        <v>650</v>
+        <v>568</v>
       </c>
     </row>
     <row r="361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>651</v>
+        <v>569</v>
       </c>
       <c r="B361" t="s">
-        <v>651</v>
+        <v>569</v>
       </c>
     </row>
     <row r="362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>652</v>
+        <v>570</v>
       </c>
       <c r="B362" t="s">
-        <v>652</v>
+        <v>570</v>
       </c>
     </row>
     <row r="363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>653</v>
+        <v>571</v>
       </c>
       <c r="B363" t="s">
-        <v>653</v>
+        <v>571</v>
       </c>
     </row>
     <row r="364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>654</v>
+        <v>572</v>
       </c>
       <c r="B364" t="s">
-        <v>654</v>
+        <v>572</v>
       </c>
     </row>
     <row r="365" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>655</v>
+        <v>573</v>
       </c>
       <c r="B365" t="s">
-        <v>655</v>
+        <v>573</v>
       </c>
     </row>
     <row r="366" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>656</v>
+        <v>574</v>
       </c>
       <c r="B366" t="s">
-        <v>656</v>
+        <v>574</v>
       </c>
     </row>
     <row r="367" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>657</v>
+        <v>575</v>
       </c>
       <c r="B367" t="s">
-        <v>657</v>
+        <v>575</v>
       </c>
     </row>
     <row r="368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>658</v>
+        <v>576</v>
       </c>
       <c r="B368" t="s">
-        <v>658</v>
+        <v>576</v>
       </c>
     </row>
     <row r="369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>659</v>
+        <v>577</v>
       </c>
       <c r="B369" t="s">
-        <v>659</v>
+        <v>577</v>
       </c>
     </row>
     <row r="370" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>660</v>
+        <v>578</v>
       </c>
       <c r="B370" t="s">
-        <v>660</v>
+        <v>578</v>
       </c>
     </row>
     <row r="371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>661</v>
+        <v>579</v>
       </c>
       <c r="B371" t="s">
-        <v>661</v>
+        <v>579</v>
       </c>
     </row>
     <row r="372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>662</v>
+        <v>580</v>
       </c>
       <c r="B372" t="s">
-        <v>662</v>
+        <v>580</v>
       </c>
     </row>
     <row r="373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>663</v>
+        <v>581</v>
       </c>
       <c r="B373" t="s">
-        <v>663</v>
+        <v>581</v>
       </c>
     </row>
     <row r="374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>664</v>
+        <v>582</v>
       </c>
       <c r="B374" t="s">
-        <v>664</v>
+        <v>582</v>
       </c>
     </row>
     <row r="375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>665</v>
+        <v>583</v>
       </c>
       <c r="B375" t="s">
-        <v>665</v>
+        <v>583</v>
       </c>
     </row>
     <row r="376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>666</v>
+        <v>584</v>
       </c>
       <c r="B376" t="s">
-        <v>666</v>
+        <v>584</v>
       </c>
     </row>
     <row r="377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>667</v>
+        <v>585</v>
       </c>
       <c r="B377" t="s">
-        <v>667</v>
+        <v>585</v>
       </c>
     </row>
     <row r="378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>668</v>
+        <v>586</v>
       </c>
       <c r="B378" t="s">
-        <v>668</v>
+        <v>586</v>
       </c>
     </row>
     <row r="379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>669</v>
+        <v>587</v>
       </c>
       <c r="B379" t="s">
-        <v>669</v>
+        <v>587</v>
       </c>
     </row>
     <row r="380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>670</v>
+        <v>588</v>
       </c>
       <c r="B380" t="s">
-        <v>670</v>
+        <v>588</v>
       </c>
     </row>
     <row r="381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>671</v>
+        <v>589</v>
       </c>
       <c r="B381" t="s">
-        <v>671</v>
+        <v>589</v>
       </c>
     </row>
     <row r="382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>672</v>
+        <v>590</v>
       </c>
       <c r="B382" t="s">
-        <v>672</v>
+        <v>590</v>
       </c>
     </row>
     <row r="383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>673</v>
+        <v>591</v>
       </c>
       <c r="B383" t="s">
-        <v>673</v>
+        <v>591</v>
       </c>
     </row>
     <row r="384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>674</v>
+        <v>592</v>
       </c>
       <c r="B384" t="s">
-        <v>674</v>
+        <v>592</v>
       </c>
     </row>
     <row r="385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>675</v>
+        <v>593</v>
       </c>
       <c r="B385" t="s">
-        <v>675</v>
+        <v>593</v>
       </c>
     </row>
     <row r="386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>676</v>
+        <v>594</v>
       </c>
       <c r="B386" t="s">
-        <v>676</v>
+        <v>594</v>
       </c>
     </row>
     <row r="387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>677</v>
+        <v>595</v>
       </c>
       <c r="B387" t="s">
-        <v>677</v>
+        <v>595</v>
       </c>
     </row>
     <row r="388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>678</v>
+        <v>596</v>
       </c>
       <c r="B388" t="s">
-        <v>678</v>
+        <v>596</v>
       </c>
     </row>
     <row r="389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>679</v>
+        <v>597</v>
       </c>
       <c r="B389" t="s">
-        <v>679</v>
+        <v>597</v>
       </c>
     </row>
     <row r="390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>680</v>
+        <v>598</v>
       </c>
       <c r="B390" t="s">
-        <v>680</v>
+        <v>598</v>
       </c>
     </row>
     <row r="391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>681</v>
+        <v>599</v>
       </c>
       <c r="B391" t="s">
-        <v>681</v>
+        <v>599</v>
       </c>
     </row>
     <row r="392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>682</v>
+        <v>600</v>
       </c>
       <c r="B392" t="s">
-        <v>682</v>
+        <v>600</v>
       </c>
     </row>
     <row r="393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>683</v>
+        <v>601</v>
       </c>
       <c r="B393" t="s">
-        <v>683</v>
+        <v>601</v>
       </c>
     </row>
     <row r="394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>684</v>
+        <v>602</v>
       </c>
       <c r="B394" t="s">
-        <v>684</v>
+        <v>602</v>
       </c>
     </row>
     <row r="395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>685</v>
+        <v>603</v>
       </c>
       <c r="B395" t="s">
-        <v>685</v>
+        <v>603</v>
       </c>
     </row>
     <row r="396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>686</v>
+        <v>604</v>
       </c>
       <c r="B396" t="s">
-        <v>686</v>
+        <v>604</v>
       </c>
     </row>
     <row r="397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>687</v>
+        <v>605</v>
       </c>
       <c r="B397" t="s">
-        <v>687</v>
+        <v>605</v>
       </c>
     </row>
     <row r="398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>688</v>
+        <v>606</v>
       </c>
       <c r="B398" t="s">
-        <v>688</v>
+        <v>606</v>
       </c>
     </row>
     <row r="399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>689</v>
+        <v>607</v>
       </c>
       <c r="B399" t="s">
-        <v>689</v>
+        <v>607</v>
       </c>
     </row>
     <row r="400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>690</v>
+        <v>608</v>
       </c>
       <c r="B400" t="s">
-        <v>690</v>
+        <v>608</v>
       </c>
     </row>
     <row r="401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>691</v>
+        <v>609</v>
       </c>
       <c r="B401" t="s">
-        <v>691</v>
+        <v>609</v>
+      </c>
+    </row>
+    <row r="403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>610</v>
+      </c>
+      <c r="B403" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>697</v>
+      </c>
+      <c r="B404" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>698</v>
+      </c>
+      <c r="B405" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>699</v>
+      </c>
+      <c r="B406" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="407" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>700</v>
+      </c>
+      <c r="B407" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="408" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>701</v>
+      </c>
+      <c r="B408" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="409" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>702</v>
+      </c>
+      <c r="B409" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="410" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>703</v>
+      </c>
+      <c r="B410" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="411" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>704</v>
+      </c>
+      <c r="B411" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="412" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A412" t="s">
+        <v>705</v>
+      </c>
+      <c r="B412" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="413" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>706</v>
+      </c>
+      <c r="B413" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="414" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
+        <v>707</v>
+      </c>
+      <c r="B414" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="415" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>708</v>
+      </c>
+      <c r="B415" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="416" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>709</v>
+      </c>
+      <c r="B416" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="417" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A417" t="s">
+        <v>710</v>
+      </c>
+      <c r="B417" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="418" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>711</v>
+      </c>
+      <c r="B418" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="419" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>712</v>
+      </c>
+      <c r="B419" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="420" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>713</v>
+      </c>
+      <c r="B420" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="421" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>714</v>
+      </c>
+      <c r="B421" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>715</v>
+      </c>
+      <c r="B422" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="423" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>716</v>
+      </c>
+      <c r="B423" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="424" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>717</v>
+      </c>
+      <c r="B424" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>718</v>
+      </c>
+      <c r="B425" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>719</v>
+      </c>
+      <c r="B426" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>720</v>
+      </c>
+      <c r="B427" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="428" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>721</v>
+      </c>
+      <c r="B428" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="429" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>722</v>
+      </c>
+      <c r="B429" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="430" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>723</v>
+      </c>
+      <c r="B430" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>724</v>
+      </c>
+      <c r="B431" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>725</v>
+      </c>
+      <c r="B432" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>726</v>
+      </c>
+      <c r="B433" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>727</v>
+      </c>
+      <c r="B434" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>728</v>
+      </c>
+      <c r="B435" t="s">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="436" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>729</v>
+      </c>
+      <c r="B436" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="437" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>730</v>
+      </c>
+      <c r="B437" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="438" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>731</v>
+      </c>
+      <c r="B438" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>732</v>
+      </c>
+      <c r="B439" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="440" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>733</v>
+      </c>
+      <c r="B440" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="441" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>734</v>
+      </c>
+      <c r="B441" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>735</v>
+      </c>
+      <c r="B442" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="443" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>736</v>
+      </c>
+      <c r="B443" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="444" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>737</v>
+      </c>
+      <c r="B444" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="445" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>738</v>
+      </c>
+      <c r="B445" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="446" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>739</v>
+      </c>
+      <c r="B446" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="447" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>740</v>
+      </c>
+      <c r="B447" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="448" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>741</v>
+      </c>
+      <c r="B448" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="449" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>742</v>
+      </c>
+      <c r="B449" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="450" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>743</v>
+      </c>
+      <c r="B450" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="451" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>744</v>
+      </c>
+      <c r="B451" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="452" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>745</v>
+      </c>
+      <c r="B452" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="453" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>746</v>
+      </c>
+      <c r="B453" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="454" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>747</v>
+      </c>
+      <c r="B454" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="455" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>748</v>
+      </c>
+      <c r="B455" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="456" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>749</v>
+      </c>
+      <c r="B456" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="457" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A457" t="s">
+        <v>750</v>
+      </c>
+      <c r="B457" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="458" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A458" t="s">
+        <v>751</v>
+      </c>
+      <c r="B458" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="459" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A459" t="s">
+        <v>752</v>
+      </c>
+      <c r="B459" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="460" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A460" t="s">
+        <v>753</v>
+      </c>
+      <c r="B460" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="461" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A461" t="s">
+        <v>754</v>
+      </c>
+      <c r="B461" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="462" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A462" t="s">
+        <v>755</v>
+      </c>
+      <c r="B462" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="463" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A463" t="s">
+        <v>756</v>
+      </c>
+      <c r="B463" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="464" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A464" t="s">
+        <v>757</v>
+      </c>
+      <c r="B464" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="465" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A465" t="s">
+        <v>758</v>
+      </c>
+      <c r="B465" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="466" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A466" t="s">
+        <v>759</v>
+      </c>
+      <c r="B466" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="467" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A467" t="s">
+        <v>760</v>
+      </c>
+      <c r="B467" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="468" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A468" t="s">
+        <v>761</v>
+      </c>
+      <c r="B468" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="469" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A469" t="s">
+        <v>762</v>
+      </c>
+      <c r="B469" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="470" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A470" t="s">
+        <v>763</v>
+      </c>
+      <c r="B470" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="471" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A471" t="s">
+        <v>764</v>
+      </c>
+      <c r="B471" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="472" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A472" t="s">
+        <v>765</v>
+      </c>
+      <c r="B472" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="473" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A473" t="s">
+        <v>766</v>
+      </c>
+      <c r="B473" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="474" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A474" t="s">
+        <v>767</v>
+      </c>
+      <c r="B474" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="475" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A475" t="s">
+        <v>768</v>
+      </c>
+      <c r="B475" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="476" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A476" t="s">
+        <v>769</v>
+      </c>
+      <c r="B476" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="477" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A477" t="s">
+        <v>770</v>
+      </c>
+      <c r="B477" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="478" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A478" t="s">
+        <v>771</v>
+      </c>
+      <c r="B478" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="479" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A479" t="s">
+        <v>772</v>
+      </c>
+      <c r="B479" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="480" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A480" t="s">
+        <v>773</v>
+      </c>
+      <c r="B480" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="481" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A481" t="s">
+        <v>774</v>
+      </c>
+      <c r="B481" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="482" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>775</v>
+      </c>
+      <c r="B482" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="483" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>776</v>
+      </c>
+      <c r="B483" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="484" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>777</v>
+      </c>
+      <c r="B484" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="485" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>778</v>
+      </c>
+      <c r="B485" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="486" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>779</v>
+      </c>
+      <c r="B486" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="487" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>780</v>
+      </c>
+      <c r="B487" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="488" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>781</v>
+      </c>
+      <c r="B488" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="489" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>782</v>
+      </c>
+      <c r="B489" t="s">
+        <v>782</v>
       </c>
     </row>
   </sheetData>
@@ -7199,676 +8168,708 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBE4172-FC39-45CE-BD67-BA23D6FB1A86}">
-  <dimension ref="A1:B83"/>
+  <dimension ref="A1:B87"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B83"/>
+      <selection activeCell="B1" sqref="B1:B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>533</v>
+        <v>610</v>
       </c>
       <c r="B1" t="s">
-        <v>533</v>
+        <v>610</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>534</v>
+        <v>611</v>
       </c>
       <c r="B2" t="s">
-        <v>616</v>
+        <v>697</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>535</v>
+        <v>612</v>
       </c>
       <c r="B3" t="s">
-        <v>617</v>
+        <v>698</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>536</v>
+        <v>613</v>
       </c>
       <c r="B4" t="s">
-        <v>618</v>
+        <v>699</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>537</v>
+        <v>614</v>
       </c>
       <c r="B5" t="s">
-        <v>619</v>
+        <v>700</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>538</v>
+        <v>615</v>
       </c>
       <c r="B6" t="s">
-        <v>620</v>
+        <v>701</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>539</v>
+        <v>616</v>
       </c>
       <c r="B7" t="s">
-        <v>621</v>
+        <v>702</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>540</v>
+        <v>617</v>
       </c>
       <c r="B8" t="s">
-        <v>622</v>
+        <v>703</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>541</v>
+        <v>618</v>
       </c>
       <c r="B9" t="s">
-        <v>623</v>
+        <v>704</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>542</v>
+        <v>619</v>
       </c>
       <c r="B10" t="s">
-        <v>624</v>
+        <v>705</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>543</v>
+        <v>620</v>
       </c>
       <c r="B11" t="s">
-        <v>625</v>
+        <v>706</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>544</v>
+        <v>621</v>
       </c>
       <c r="B12" t="s">
-        <v>626</v>
+        <v>707</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>545</v>
+        <v>622</v>
       </c>
       <c r="B13" t="s">
-        <v>627</v>
+        <v>708</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>546</v>
+        <v>623</v>
       </c>
       <c r="B14" t="s">
-        <v>628</v>
+        <v>709</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>547</v>
+        <v>624</v>
       </c>
       <c r="B15" t="s">
-        <v>629</v>
+        <v>710</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>548</v>
+        <v>625</v>
       </c>
       <c r="B16" t="s">
-        <v>630</v>
+        <v>711</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>549</v>
+        <v>626</v>
       </c>
       <c r="B17" t="s">
-        <v>631</v>
+        <v>712</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>550</v>
+        <v>627</v>
       </c>
       <c r="B18" t="s">
-        <v>632</v>
+        <v>713</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>551</v>
+        <v>628</v>
       </c>
       <c r="B19" t="s">
-        <v>633</v>
+        <v>714</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>552</v>
+        <v>629</v>
       </c>
       <c r="B20" t="s">
-        <v>634</v>
+        <v>715</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>553</v>
+        <v>630</v>
       </c>
       <c r="B21" t="s">
-        <v>635</v>
+        <v>716</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>554</v>
+        <v>631</v>
       </c>
       <c r="B22" t="s">
-        <v>636</v>
+        <v>717</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>555</v>
+        <v>632</v>
       </c>
       <c r="B23" t="s">
-        <v>637</v>
+        <v>718</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>556</v>
+        <v>633</v>
       </c>
       <c r="B24" t="s">
-        <v>638</v>
+        <v>719</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>557</v>
+        <v>634</v>
       </c>
       <c r="B25" t="s">
-        <v>639</v>
+        <v>720</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>558</v>
+        <v>635</v>
       </c>
       <c r="B26" t="s">
-        <v>640</v>
+        <v>721</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>559</v>
+        <v>636</v>
       </c>
       <c r="B27" t="s">
-        <v>641</v>
+        <v>722</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>560</v>
+        <v>637</v>
       </c>
       <c r="B28" t="s">
-        <v>642</v>
+        <v>723</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>561</v>
+        <v>638</v>
       </c>
       <c r="B29" t="s">
-        <v>643</v>
+        <v>724</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>562</v>
+        <v>639</v>
       </c>
       <c r="B30" t="s">
-        <v>644</v>
+        <v>725</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>563</v>
+        <v>640</v>
       </c>
       <c r="B31" t="s">
-        <v>645</v>
+        <v>726</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>564</v>
+        <v>641</v>
       </c>
       <c r="B32" t="s">
-        <v>646</v>
+        <v>727</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>565</v>
+        <v>642</v>
       </c>
       <c r="B33" t="s">
-        <v>647</v>
+        <v>728</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>566</v>
+        <v>643</v>
       </c>
       <c r="B34" t="s">
-        <v>648</v>
+        <v>729</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>567</v>
+        <v>644</v>
       </c>
       <c r="B35" t="s">
-        <v>649</v>
+        <v>730</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>568</v>
+        <v>645</v>
       </c>
       <c r="B36" t="s">
-        <v>650</v>
+        <v>731</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>569</v>
+        <v>646</v>
       </c>
       <c r="B37" t="s">
-        <v>651</v>
+        <v>732</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>570</v>
+        <v>647</v>
       </c>
       <c r="B38" t="s">
-        <v>652</v>
+        <v>733</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>571</v>
+        <v>648</v>
       </c>
       <c r="B39" t="s">
-        <v>653</v>
+        <v>734</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>572</v>
+        <v>649</v>
       </c>
       <c r="B40" t="s">
-        <v>654</v>
+        <v>735</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>573</v>
+        <v>650</v>
       </c>
       <c r="B41" t="s">
-        <v>655</v>
+        <v>736</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>574</v>
+        <v>651</v>
       </c>
       <c r="B42" t="s">
-        <v>656</v>
+        <v>737</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>575</v>
+        <v>652</v>
       </c>
       <c r="B43" t="s">
-        <v>657</v>
+        <v>738</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>576</v>
+        <v>653</v>
       </c>
       <c r="B44" t="s">
-        <v>658</v>
+        <v>739</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>577</v>
+        <v>654</v>
       </c>
       <c r="B45" t="s">
-        <v>659</v>
+        <v>740</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>578</v>
+        <v>655</v>
       </c>
       <c r="B46" t="s">
-        <v>660</v>
+        <v>741</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>579</v>
+        <v>656</v>
       </c>
       <c r="B47" t="s">
-        <v>661</v>
+        <v>742</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>580</v>
+        <v>657</v>
       </c>
       <c r="B48" t="s">
-        <v>662</v>
+        <v>743</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>581</v>
+        <v>658</v>
       </c>
       <c r="B49" t="s">
-        <v>663</v>
+        <v>744</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>582</v>
+        <v>659</v>
       </c>
       <c r="B50" t="s">
-        <v>664</v>
+        <v>745</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>583</v>
+        <v>660</v>
       </c>
       <c r="B51" t="s">
-        <v>665</v>
+        <v>746</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>584</v>
+        <v>661</v>
       </c>
       <c r="B52" t="s">
-        <v>666</v>
+        <v>747</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>585</v>
+        <v>662</v>
       </c>
       <c r="B53" t="s">
-        <v>667</v>
+        <v>748</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>586</v>
+        <v>663</v>
       </c>
       <c r="B54" t="s">
-        <v>668</v>
+        <v>749</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>587</v>
+        <v>664</v>
       </c>
       <c r="B55" t="s">
-        <v>669</v>
+        <v>750</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>588</v>
+        <v>665</v>
       </c>
       <c r="B56" t="s">
-        <v>670</v>
+        <v>751</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>589</v>
+        <v>666</v>
       </c>
       <c r="B57" t="s">
-        <v>671</v>
+        <v>752</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>590</v>
+        <v>667</v>
       </c>
       <c r="B58" t="s">
-        <v>668</v>
+        <v>753</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>591</v>
+        <v>668</v>
       </c>
       <c r="B59" t="s">
-        <v>672</v>
+        <v>754</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>592</v>
+        <v>669</v>
       </c>
       <c r="B60" t="s">
-        <v>664</v>
+        <v>755</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>593</v>
+        <v>670</v>
       </c>
       <c r="B61" t="s">
-        <v>673</v>
+        <v>756</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>594</v>
+        <v>671</v>
       </c>
       <c r="B62" t="s">
-        <v>652</v>
+        <v>757</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>595</v>
+        <v>672</v>
       </c>
       <c r="B63" t="s">
-        <v>660</v>
+        <v>758</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>596</v>
+        <v>673</v>
       </c>
       <c r="B64" t="s">
-        <v>668</v>
+        <v>759</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>597</v>
+        <v>674</v>
       </c>
       <c r="B65" t="s">
-        <v>674</v>
+        <v>760</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>598</v>
+        <v>675</v>
       </c>
       <c r="B66" t="s">
-        <v>675</v>
+        <v>761</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>599</v>
+        <v>676</v>
       </c>
       <c r="B67" t="s">
-        <v>676</v>
+        <v>762</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>600</v>
+        <v>677</v>
       </c>
       <c r="B68" t="s">
-        <v>677</v>
+        <v>763</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>601</v>
+        <v>678</v>
       </c>
       <c r="B69" t="s">
-        <v>678</v>
+        <v>764</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>602</v>
+        <v>679</v>
       </c>
       <c r="B70" t="s">
-        <v>679</v>
+        <v>765</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>603</v>
+        <v>680</v>
       </c>
       <c r="B71" t="s">
-        <v>680</v>
+        <v>766</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>604</v>
+        <v>681</v>
       </c>
       <c r="B72" t="s">
-        <v>681</v>
+        <v>767</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>605</v>
+        <v>682</v>
       </c>
       <c r="B73" t="s">
-        <v>652</v>
+        <v>768</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>606</v>
+        <v>683</v>
       </c>
       <c r="B74" t="s">
-        <v>682</v>
+        <v>769</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>607</v>
+        <v>684</v>
       </c>
       <c r="B75" t="s">
-        <v>683</v>
+        <v>770</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>608</v>
+        <v>685</v>
       </c>
       <c r="B76" t="s">
-        <v>684</v>
+        <v>771</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>609</v>
+        <v>686</v>
       </c>
       <c r="B77" t="s">
-        <v>685</v>
+        <v>772</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>610</v>
+        <v>687</v>
       </c>
       <c r="B78" t="s">
-        <v>686</v>
+        <v>773</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>611</v>
+        <v>688</v>
       </c>
       <c r="B79" t="s">
-        <v>687</v>
+        <v>774</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>612</v>
+        <v>689</v>
       </c>
       <c r="B80" t="s">
-        <v>688</v>
+        <v>775</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>613</v>
+        <v>690</v>
       </c>
       <c r="B81" t="s">
-        <v>689</v>
+        <v>776</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>614</v>
+        <v>691</v>
       </c>
       <c r="B82" t="s">
-        <v>690</v>
+        <v>777</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>615</v>
+        <v>692</v>
       </c>
       <c r="B83" t="s">
-        <v>691</v>
+        <v>778</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>693</v>
+      </c>
+      <c r="B84" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>694</v>
+      </c>
+      <c r="B85" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>695</v>
+      </c>
+      <c r="B86" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>696</v>
+      </c>
+      <c r="B87" t="s">
+        <v>782</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Luận Thiên Tướng hoàn thiện
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EADAF9D-1A3D-443A-9CFD-C962FAAAD82E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CDABEAF-E873-4EF4-91E9-93815E167F93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2224" uniqueCount="1207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2223" uniqueCount="1142">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -2738,468 +2738,6 @@
     <t>Cự Môn tọa thủ cung Mệnh</t>
   </si>
   <si>
-    <t>luanmenh.js:2112 Cự Môn tọa thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2115 Cự Môn tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2118 Cự Môn tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Thái Tuế, Thiên Hình, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2121 Cự Môn tọa thủ cung Mệnh ở Mão gặp Tuế Hổ Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2124 Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Lộc Tồn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2127 Cự Môn tọa thủ cung Mệnh ở Mão gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2130 Cự Môn tọa thủ cung Mệnh ở Mão gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2133 Cự Môn tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2112 Cự Môn tọa thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2115 Cự Môn tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2118 Cự Môn tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Thái Tuế, Thiên Hình, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2121 Cự Môn tọa thủ cung Mệnh ở Dậu gặp Tuế Hổ Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2124 Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Lộc Tồn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2127 Cự Môn tọa thủ cung Mệnh ở Dậu gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2130 Cự Môn tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2133 Cự Môn tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2112 Cự Môn tọa thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2115 Cự Môn tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2118 Cự Môn tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Thái Tuế, Thiên Hình, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2121 Cự Môn tọa thủ cung Mệnh ở Tý gặp Tuế Hổ Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2124 Cự Môn tọa thủ cung Mệnh ở Tý đồng cung Lộc Tồn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2127 Cự Môn tọa thủ cung Mệnh ở Tý gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2130 Cự Môn tọa thủ cung Mệnh ở Tý gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2133 Cự Môn tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2112 Cự Môn tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2115 Cự Môn tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2118 Cự Môn tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Thái Tuế, Thiên Hình, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2121 Cự Môn tọa thủ cung Mệnh ở Ngọ gặp Tuế Hổ Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2124 Cự Môn tọa thủ cung Mệnh ở Ngọ đồng cung Lộc Tồn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2127 Cự Môn tọa thủ cung Mệnh ở Ngọ gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2130 Cự Môn tọa thủ cung Mệnh ở Ngọ gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2133 Cự Môn tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2112 Cự Môn tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2115 Cự Môn tọa thủ cung Mệnh ở Dần gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2118 Cự Môn tọa thủ cung Mệnh ở Dần gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Thái Tuế, Thiên Hình, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2121 Cự Môn tọa thủ cung Mệnh ở Dần gặp Tuế Hổ Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2124 Cự Môn tọa thủ cung Mệnh ở Dần đồng cung Lộc Tồn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2127 Cự Môn tọa thủ cung Mệnh ở Dần gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2130 Cự Môn tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2133 Cự Môn tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2112 Cự Môn tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2115 Cự Môn tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2118 Cự Môn tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Thái Tuế, Thiên Hình, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2121 Cự Môn tọa thủ cung Mệnh ở Thân gặp Tuế Hổ Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2124 Cự Môn tọa thủ cung Mệnh ở Thân đồng cung Lộc Tồn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2127 Cự Môn tọa thủ cung Mệnh ở Thân gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2130 Cự Môn tọa thủ cung Mệnh ở Thân gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2133 Cự Môn tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2112 Cự Môn tọa thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2115 Cự Môn tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2118 Cự Môn tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Thái Tuế, Thiên Hình, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2121 Cự Môn tọa thủ cung Mệnh ở Hợi gặp Tuế Hổ Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2124 Cự Môn tọa thủ cung Mệnh ở Hợi đồng cung Lộc Tồn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2127 Cự Môn tọa thủ cung Mệnh ở Hợi gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2130 Cự Môn tọa thủ cung Mệnh ở Hợi gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2133 Cự Môn tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2142 Cự Môn tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2145 Cự Môn tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2148 Cự Môn tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Hóa Khoa, Thái Tuế, Thiên Hình, Tả Phù, Hữu Bật, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2151 Cự Môn tọa thủ cung Mệnh ở Sửu gặp Tuế Hổ Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2154 Cự Môn tọa thủ cung Mệnh ở Sửu đồng cung Lộc Tồn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2157 Cự Môn tọa thủ cung Mệnh ở Sửu gặp Hoá Lộc, Thái Tuế</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2160 Cự Môn tọa thủ cung Mệnh ở Sửu gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2163 Cự Môn tọa thủ cung Mệnh ở Sửu gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2166 Cự Môn tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">luanmenh.js:2169 Cự Môn tọa thủ cung Mệnh ở Sửu gặp Thiên Hư, Thiên Không, Địa Không, Địa Kiếp </t>
-  </si>
-  <si>
-    <t>luanmenh.js:2142 Cự Môn tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2145 Cự Môn tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2148 Cự Môn tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Hóa Khoa, Thái Tuế, Thiên Hình, Tả Phù, Hữu Bật, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2151 Cự Môn tọa thủ cung Mệnh ở Mùi gặp Tuế Hổ Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2154 Cự Môn tọa thủ cung Mệnh ở Mùi đồng cung Lộc Tồn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2157 Cự Môn tọa thủ cung Mệnh ở Mùi gặp Hoá Lộc, Thái Tuế</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2160 Cự Môn tọa thủ cung Mệnh ở Mùi gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2163 Cự Môn tọa thủ cung Mệnh ở Mùi gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2166 Cự Môn tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">luanmenh.js:2169 Cự Môn tọa thủ cung Mệnh ở Mùi gặp Thiên Hư, Thiên Không, Địa Không, Địa Kiếp </t>
-  </si>
-  <si>
-    <t>luanmenh.js:2142 Cự Môn tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2145 Cự Môn tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2148 Cự Môn tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Hóa Khoa, Thái Tuế, Thiên Hình, Tả Phù, Hữu Bật, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2151 Cự Môn tọa thủ cung Mệnh ở Thìn gặp Tuế Hổ Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2154 Cự Môn tọa thủ cung Mệnh ở Thìn đồng cung Lộc Tồn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2157 Cự Môn tọa thủ cung Mệnh ở Thìn gặp Hoá Lộc, Thái Tuế</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2160 Cự Môn tọa thủ cung Mệnh ở Thìn gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2163 Cự Môn tọa thủ cung Mệnh ở Thìn gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2166 Cự Môn tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">luanmenh.js:2169 Cự Môn tọa thủ cung Mệnh ở Thìn gặp Thiên Hư, Thiên Không, Địa Không, Địa Kiếp </t>
-  </si>
-  <si>
-    <t>luanmenh.js:2142 Cự Môn tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2145 Cự Môn tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2148 Cự Môn tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Hóa Khoa, Thái Tuế, Thiên Hình, Tả Phù, Hữu Bật, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2151 Cự Môn tọa thủ cung Mệnh ở Tuất gặp Tuế Hổ Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2154 Cự Môn tọa thủ cung Mệnh ở Tuất đồng cung Lộc Tồn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2157 Cự Môn tọa thủ cung Mệnh ở Tuất gặp Hoá Lộc, Thái Tuế</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2160 Cự Môn tọa thủ cung Mệnh ở Tuất gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2163 Cự Môn tọa thủ cung Mệnh ở Tuất gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2166 Cự Môn tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">luanmenh.js:2169 Cự Môn tọa thủ cung Mệnh ở Tuất gặp Thiên Hư, Thiên Không, Địa Không, Địa Kiếp </t>
-  </si>
-  <si>
-    <t>luanmenh.js:2142 Cự Môn tọa thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2145 Cự Môn tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2148 Cự Môn tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Hóa Khoa, Thái Tuế, Thiên Hình, Tả Phù, Hữu Bật, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2151 Cự Môn tọa thủ cung Mệnh ở Tỵ gặp Tuế Hổ Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2154 Cự Môn tọa thủ cung Mệnh ở Tỵ đồng cung Lộc Tồn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2157 Cự Môn tọa thủ cung Mệnh ở Tỵ gặp Hoá Lộc, Thái Tuế</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2160 Cự Môn tọa thủ cung Mệnh ở Tỵ gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2163 Cự Môn tọa thủ cung Mệnh ở Tỵ gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2166 Cự Môn tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">luanmenh.js:2169 Cự Môn tọa thủ cung Mệnh ở Tỵ gặp Thiên Hư, Thiên Không, Địa Không, Địa Kiếp </t>
-  </si>
-  <si>
-    <t>luanmenh.js:2180 Người tuổi Đ. có Cự Môn tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2180 Người tuổi C. có Cự Môn tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2186 Người tuổi Q. có Cự Môn tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2186 Người tuổi T. có Cự Môn tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2180 Người tuổi Đ. có Cự Môn tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2180 Người tuổi C. có Cự Môn tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2186 Người tuổi Q. có Cự Môn tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2186 Người tuổi T. có Cự Môn tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2195 Người tuổi Ất có Cự Môn tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2195 Người tuổi Bính có Cự Môn tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2195 Người tuổi Ất có Cự Môn tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2195 Người tuổi Bính có Cự Môn tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2204 Cự Môn tọa thủ cung Mệnh đồng cung Hoá Kỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2207 Cự Môn tọa thủ cung Mệnh đồng cung Thái Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2210 Cự Môn tọa thủ cung Mệnh ở Dần đồng cung Thái Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2213 Cự Môn tọa thủ cung Mệnh ở Thân đồng cung Thái Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2216 Cự Môn tọa thủ cung Mệnh ở Thân gặp Thái Dương, Thiên Di có Thái Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2219 Cự Môn tọa thủ cung Mệnh ở Dần gặp Thái Dương, Thiên Di có Thái Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2223 Cự Môn tọa thủ cung Thiên Di đồng cung Thái Dương xung chiếu cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2229 Cự Môn tọa thủ cung Mệnh ở Dần đồng cung Thái Dương gặp Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2229 Cự Môn tọa thủ cung Mệnh ở Thân đồng cung Thái Dương gặp Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2234 Cự Môn tọa thủ cung Mệnh ở Dần đồng cung Thiên Cơ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2243 Người tuổi Ất có Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2246 Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2249 Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ gặp Đại Hao, Tiểu Hao</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2252 Quý chị có Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2243 Người tuổi Ất có Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2246 Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2249 Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ gặp Đại Hao, Tiểu Hao</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2252 Quý chị có Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2243 Người tuổi Tân có Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2243 Người tuổi Tân có Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2243 Người tuổi Kỷ có Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2243 Người tuổi Kỷ có Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2243 Người tuổi Bính có Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2243 Người tuổi Bính có Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2260 Người tuổi Bính có Cự Môn tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2260 Người tuổi Tân có Cự Môn tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2268 Cự Môn tọa thủ cung Mệnh ở Tý đồng cung Lộc Tồn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2268 Cự Môn tọa thủ cung Mệnh ở Hợi đồng cung Lộc Tồn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2275 Cự Môn tọa thủ cung Mệnh ở Tý gặp Khoa Lộc Quyền</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2275 Cự Môn tọa thủ cung Mệnh ở Ngọ gặp Khoa Lộc Quyền</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2260 Người tuổi Bính có Cự Môn tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2260 Người tuổi Tân có Cự Môn tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2260 Người tuổi Bính có Cự Môn tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2260 Người tuổi Tân có Cự Môn tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2260 Người tuổi Bính có Cự Môn tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2260 Người tuổi Tân có Cự Môn tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
     <t>Cự Môn tọa thủ cung Mệnh ở Mão</t>
   </si>
   <si>
@@ -3648,6 +3186,273 @@
   </si>
   <si>
     <t>Người tuổi Tân có Cự Môn tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2393 Thiên Tướng tọa thủ cung Mệnh ở Dần gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2398 Thiên Tướng tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2390 Thiên Tướng tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2393 Thiên Tướng tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2398 Thiên Tướng tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2390 Thiên Tướng tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2393 Thiên Tướng tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2398 Thiên Tướng tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2390 Thiên Tướng tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2393 Thiên Tướng tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2398 Thiên Tướng tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2390 Thiên Tướng tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2393 Thiên Tướng tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2398 Thiên Tướng tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2390 Thiên Tướng tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2393 Thiên Tướng tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2398 Thiên Tướng tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2390 Thiên Tướng tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2393 Thiên Tướng tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2398 Thiên Tướng tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2390 Thiên Tướng tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2393 Thiên Tướng tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2398 Thiên Tướng tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2390 Thiên Tướng tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2393 Thiên Tướng tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2398 Thiên Tướng tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2390 Thiên Tướng tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2393 Thiên Tướng tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2398 Thiên Tướng tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2405 Thiên Tướng tọa thủ cung Mệnh ở Thìn gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2405 Thiên Tướng tọa thủ cung Mệnh ở Tuất gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2405 Thiên Tướng tọa thủ cung Mệnh ở Tý gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2405 Thiên Tướng tọa thủ cung Mệnh ở Ngọ gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2415 Thiên Tướng tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2419 Thiên Tướng tọa thủ cung Mệnh ở Mão gặp Hoá Lộc, Thái Tuế</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2422 Quý chị có Thiên Tướng tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2415 Thiên Tướng tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2419 Thiên Tướng tọa thủ cung Mệnh ở Dậu gặp Hoá Lộc, Thái Tuế</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2422 Quý chị có Thiên Tướng tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2428 Thiên Tướng tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2428 Thiên Tướng tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2435 Thiên Tướng tọa thủ cung Mệnh ở Tý đồng cung Liêm Trinh gặp Kình Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2435 Thiên Tướng tọa thủ cung Mệnh ở Ngọ đồng cung Liêm Trinh gặp Kình Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2441 Quý chị có Thiên Tướng tọa thủ cung Mệnh đồng cung Hồng Loan</t>
+  </si>
+  <si>
+    <t>luanmenh.js:2445 Quý chị có Thiên Tướng tọa thủ cung Mệnh gặp Đào Hoa, Hồng Loan, Hoa Cái, Vũ Khúc</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Dần gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Vũ Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Thìn gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Tuất gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Tý gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Ngọ gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Mão gặp Hoá Lộc, Thái Tuế</t>
+  </si>
+  <si>
+    <t>Quý chị có Thiên Tướng tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Dậu gặp Hoá Lộc, Thái Tuế</t>
+  </si>
+  <si>
+    <t>Quý chị có Thiên Tướng tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Tý đồng cung Liêm Trinh gặp Kình Dương</t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Mệnh ở Ngọ đồng cung Liêm Trinh gặp Kình Dương</t>
+  </si>
+  <si>
+    <t>Quý chị có Thiên Tướng tọa thủ cung Mệnh đồng cung Hồng Loan</t>
+  </si>
+  <si>
+    <t>Quý chị có Thiên Tướng tọa thủ cung Mệnh gặp Đào Hoa, Hồng Loan, Hoa Cái, Vũ Khúc</t>
   </si>
 </sst>
 </file>
@@ -5727,10 +5532,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B883"/>
+  <dimension ref="A1:B930"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A856" workbookViewId="0">
-      <selection activeCell="G882" sqref="G882"/>
+    <sheetView tabSelected="1" topLeftCell="A910" workbookViewId="0">
+      <selection activeCell="B885" sqref="B885:B930"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11014,1474 +10819,1842 @@
     </row>
     <row r="700" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A700" t="s">
-        <v>1057</v>
+        <v>903</v>
       </c>
       <c r="B700" t="s">
-        <v>1057</v>
+        <v>903</v>
       </c>
     </row>
     <row r="701" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A701" t="s">
-        <v>1058</v>
+        <v>904</v>
       </c>
       <c r="B701" t="s">
-        <v>1058</v>
+        <v>904</v>
       </c>
     </row>
     <row r="702" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A702" t="s">
-        <v>1059</v>
+        <v>905</v>
       </c>
       <c r="B702" t="s">
-        <v>1059</v>
+        <v>905</v>
       </c>
     </row>
     <row r="703" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
-        <v>1060</v>
+        <v>906</v>
       </c>
       <c r="B703" t="s">
-        <v>1060</v>
+        <v>906</v>
       </c>
     </row>
     <row r="704" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A704" t="s">
-        <v>1061</v>
+        <v>907</v>
       </c>
       <c r="B704" t="s">
-        <v>1061</v>
+        <v>907</v>
       </c>
     </row>
     <row r="705" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A705" t="s">
-        <v>1062</v>
+        <v>908</v>
       </c>
       <c r="B705" t="s">
-        <v>1062</v>
+        <v>908</v>
       </c>
     </row>
     <row r="706" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A706" t="s">
-        <v>1063</v>
+        <v>909</v>
       </c>
       <c r="B706" t="s">
-        <v>1063</v>
+        <v>909</v>
       </c>
     </row>
     <row r="707" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A707" t="s">
-        <v>1064</v>
+        <v>910</v>
       </c>
       <c r="B707" t="s">
-        <v>1064</v>
+        <v>910</v>
       </c>
     </row>
     <row r="708" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A708" t="s">
-        <v>1065</v>
+        <v>911</v>
       </c>
       <c r="B708" t="s">
-        <v>1065</v>
+        <v>911</v>
       </c>
     </row>
     <row r="709" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A709" t="s">
-        <v>1066</v>
+        <v>912</v>
       </c>
       <c r="B709" t="s">
-        <v>1066</v>
+        <v>912</v>
       </c>
     </row>
     <row r="710" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A710" t="s">
-        <v>1067</v>
+        <v>913</v>
       </c>
       <c r="B710" t="s">
-        <v>1067</v>
+        <v>913</v>
       </c>
     </row>
     <row r="711" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A711" t="s">
-        <v>1068</v>
+        <v>914</v>
       </c>
       <c r="B711" t="s">
-        <v>1068</v>
+        <v>914</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A712" t="s">
-        <v>1069</v>
+        <v>915</v>
       </c>
       <c r="B712" t="s">
-        <v>1069</v>
+        <v>915</v>
       </c>
     </row>
     <row r="713" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A713" t="s">
-        <v>1070</v>
+        <v>916</v>
       </c>
       <c r="B713" t="s">
-        <v>1070</v>
+        <v>916</v>
       </c>
     </row>
     <row r="714" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A714" t="s">
-        <v>1071</v>
+        <v>917</v>
       </c>
       <c r="B714" t="s">
-        <v>1071</v>
+        <v>917</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A715" t="s">
-        <v>1072</v>
+        <v>918</v>
       </c>
       <c r="B715" t="s">
-        <v>1072</v>
+        <v>918</v>
       </c>
     </row>
     <row r="716" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A716" t="s">
-        <v>1073</v>
+        <v>919</v>
       </c>
       <c r="B716" t="s">
-        <v>1073</v>
+        <v>919</v>
       </c>
     </row>
     <row r="717" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A717" t="s">
-        <v>1074</v>
+        <v>920</v>
       </c>
       <c r="B717" t="s">
-        <v>1074</v>
+        <v>920</v>
       </c>
     </row>
     <row r="718" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A718" t="s">
-        <v>1075</v>
+        <v>921</v>
       </c>
       <c r="B718" t="s">
-        <v>1075</v>
+        <v>921</v>
       </c>
     </row>
     <row r="719" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A719" t="s">
-        <v>1076</v>
+        <v>922</v>
       </c>
       <c r="B719" t="s">
-        <v>1076</v>
+        <v>922</v>
       </c>
     </row>
     <row r="720" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A720" t="s">
-        <v>1077</v>
+        <v>923</v>
       </c>
       <c r="B720" t="s">
-        <v>1077</v>
+        <v>923</v>
       </c>
     </row>
     <row r="721" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A721" t="s">
-        <v>1078</v>
+        <v>924</v>
       </c>
       <c r="B721" t="s">
-        <v>1078</v>
+        <v>924</v>
       </c>
     </row>
     <row r="722" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A722" t="s">
-        <v>1079</v>
+        <v>925</v>
       </c>
       <c r="B722" t="s">
-        <v>1079</v>
+        <v>925</v>
       </c>
     </row>
     <row r="723" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A723" t="s">
-        <v>1080</v>
+        <v>926</v>
       </c>
       <c r="B723" t="s">
-        <v>1080</v>
+        <v>926</v>
       </c>
     </row>
     <row r="724" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A724" t="s">
-        <v>1081</v>
+        <v>927</v>
       </c>
       <c r="B724" t="s">
-        <v>1081</v>
+        <v>927</v>
       </c>
     </row>
     <row r="725" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A725" t="s">
-        <v>1082</v>
+        <v>928</v>
       </c>
       <c r="B725" t="s">
-        <v>1082</v>
+        <v>928</v>
       </c>
     </row>
     <row r="726" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A726" t="s">
-        <v>1083</v>
+        <v>929</v>
       </c>
       <c r="B726" t="s">
-        <v>1083</v>
+        <v>929</v>
       </c>
     </row>
     <row r="727" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A727" t="s">
-        <v>1084</v>
+        <v>930</v>
       </c>
       <c r="B727" t="s">
-        <v>1084</v>
+        <v>930</v>
       </c>
     </row>
     <row r="728" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A728" t="s">
-        <v>1085</v>
+        <v>931</v>
       </c>
       <c r="B728" t="s">
-        <v>1085</v>
+        <v>931</v>
       </c>
     </row>
     <row r="729" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A729" t="s">
-        <v>1086</v>
+        <v>932</v>
       </c>
       <c r="B729" t="s">
-        <v>1086</v>
+        <v>932</v>
       </c>
     </row>
     <row r="730" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A730" t="s">
-        <v>1087</v>
+        <v>933</v>
       </c>
       <c r="B730" t="s">
-        <v>1087</v>
+        <v>933</v>
       </c>
     </row>
     <row r="731" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A731" t="s">
-        <v>1088</v>
+        <v>934</v>
       </c>
       <c r="B731" t="s">
-        <v>1088</v>
+        <v>934</v>
       </c>
     </row>
     <row r="732" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A732" t="s">
-        <v>1089</v>
+        <v>935</v>
       </c>
       <c r="B732" t="s">
-        <v>1089</v>
+        <v>935</v>
       </c>
     </row>
     <row r="733" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A733" t="s">
-        <v>1090</v>
+        <v>936</v>
       </c>
       <c r="B733" t="s">
-        <v>1090</v>
+        <v>936</v>
       </c>
     </row>
     <row r="734" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A734" t="s">
-        <v>1091</v>
+        <v>937</v>
       </c>
       <c r="B734" t="s">
-        <v>1091</v>
+        <v>937</v>
       </c>
     </row>
     <row r="735" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A735" t="s">
-        <v>1092</v>
+        <v>938</v>
       </c>
       <c r="B735" t="s">
-        <v>1092</v>
+        <v>938</v>
       </c>
     </row>
     <row r="736" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A736" t="s">
-        <v>1093</v>
+        <v>939</v>
       </c>
       <c r="B736" t="s">
-        <v>1093</v>
+        <v>939</v>
       </c>
     </row>
     <row r="737" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A737" t="s">
-        <v>1094</v>
+        <v>940</v>
       </c>
       <c r="B737" t="s">
-        <v>1094</v>
+        <v>940</v>
       </c>
     </row>
     <row r="738" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A738" t="s">
-        <v>1095</v>
+        <v>941</v>
       </c>
       <c r="B738" t="s">
-        <v>1095</v>
+        <v>941</v>
       </c>
     </row>
     <row r="739" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A739" t="s">
-        <v>1096</v>
+        <v>942</v>
       </c>
       <c r="B739" t="s">
-        <v>1096</v>
+        <v>942</v>
       </c>
     </row>
     <row r="740" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A740" t="s">
-        <v>1097</v>
+        <v>943</v>
       </c>
       <c r="B740" t="s">
-        <v>1097</v>
+        <v>943</v>
       </c>
     </row>
     <row r="741" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A741" t="s">
-        <v>1098</v>
+        <v>944</v>
       </c>
       <c r="B741" t="s">
-        <v>1098</v>
+        <v>944</v>
       </c>
     </row>
     <row r="742" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A742" t="s">
-        <v>1099</v>
+        <v>945</v>
       </c>
       <c r="B742" t="s">
-        <v>1099</v>
+        <v>945</v>
       </c>
     </row>
     <row r="743" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A743" t="s">
-        <v>1100</v>
+        <v>946</v>
       </c>
       <c r="B743" t="s">
-        <v>1100</v>
+        <v>946</v>
       </c>
     </row>
     <row r="744" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A744" t="s">
-        <v>1101</v>
+        <v>947</v>
       </c>
       <c r="B744" t="s">
-        <v>1101</v>
+        <v>947</v>
       </c>
     </row>
     <row r="745" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A745" t="s">
-        <v>1102</v>
+        <v>948</v>
       </c>
       <c r="B745" t="s">
-        <v>1102</v>
+        <v>948</v>
       </c>
     </row>
     <row r="746" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A746" t="s">
-        <v>1103</v>
+        <v>949</v>
       </c>
       <c r="B746" t="s">
-        <v>1103</v>
+        <v>949</v>
       </c>
     </row>
     <row r="747" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A747" t="s">
-        <v>1104</v>
+        <v>950</v>
       </c>
       <c r="B747" t="s">
-        <v>1104</v>
+        <v>950</v>
       </c>
     </row>
     <row r="748" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A748" t="s">
-        <v>1105</v>
+        <v>951</v>
       </c>
       <c r="B748" t="s">
-        <v>1105</v>
+        <v>951</v>
       </c>
     </row>
     <row r="749" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A749" t="s">
-        <v>1106</v>
+        <v>952</v>
       </c>
       <c r="B749" t="s">
-        <v>1106</v>
+        <v>952</v>
       </c>
     </row>
     <row r="750" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A750" t="s">
-        <v>1107</v>
+        <v>953</v>
       </c>
       <c r="B750" t="s">
-        <v>1107</v>
+        <v>953</v>
       </c>
     </row>
     <row r="751" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A751" t="s">
-        <v>1108</v>
+        <v>954</v>
       </c>
       <c r="B751" t="s">
-        <v>1108</v>
+        <v>954</v>
       </c>
     </row>
     <row r="752" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A752" t="s">
-        <v>1109</v>
+        <v>955</v>
       </c>
       <c r="B752" t="s">
-        <v>1109</v>
+        <v>955</v>
       </c>
     </row>
     <row r="753" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A753" t="s">
-        <v>1110</v>
+        <v>956</v>
       </c>
       <c r="B753" t="s">
-        <v>1110</v>
+        <v>956</v>
       </c>
     </row>
     <row r="754" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A754" t="s">
-        <v>1111</v>
+        <v>957</v>
       </c>
       <c r="B754" t="s">
-        <v>1111</v>
+        <v>957</v>
       </c>
     </row>
     <row r="755" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A755" t="s">
-        <v>1112</v>
+        <v>958</v>
       </c>
       <c r="B755" t="s">
-        <v>1112</v>
+        <v>958</v>
       </c>
     </row>
     <row r="756" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A756" t="s">
-        <v>1113</v>
+        <v>959</v>
       </c>
       <c r="B756" t="s">
-        <v>1113</v>
+        <v>959</v>
       </c>
     </row>
     <row r="757" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A757" t="s">
-        <v>1114</v>
+        <v>960</v>
       </c>
       <c r="B757" t="s">
-        <v>1114</v>
+        <v>960</v>
       </c>
     </row>
     <row r="758" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A758" t="s">
-        <v>1115</v>
+        <v>961</v>
       </c>
       <c r="B758" t="s">
-        <v>1115</v>
+        <v>961</v>
       </c>
     </row>
     <row r="759" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A759" t="s">
-        <v>1116</v>
+        <v>962</v>
       </c>
       <c r="B759" t="s">
-        <v>1116</v>
+        <v>962</v>
       </c>
     </row>
     <row r="760" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A760" t="s">
-        <v>1117</v>
+        <v>963</v>
       </c>
       <c r="B760" t="s">
-        <v>1117</v>
+        <v>963</v>
       </c>
     </row>
     <row r="761" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A761" t="s">
-        <v>1118</v>
+        <v>964</v>
       </c>
       <c r="B761" t="s">
-        <v>1118</v>
+        <v>964</v>
       </c>
     </row>
     <row r="762" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A762" t="s">
-        <v>1119</v>
+        <v>965</v>
       </c>
       <c r="B762" t="s">
-        <v>1119</v>
+        <v>965</v>
       </c>
     </row>
     <row r="763" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A763" t="s">
-        <v>1120</v>
+        <v>966</v>
       </c>
       <c r="B763" t="s">
-        <v>1120</v>
+        <v>966</v>
       </c>
     </row>
     <row r="764" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A764" t="s">
-        <v>1121</v>
+        <v>967</v>
       </c>
       <c r="B764" t="s">
-        <v>1121</v>
+        <v>967</v>
       </c>
     </row>
     <row r="765" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A765" t="s">
-        <v>1122</v>
+        <v>968</v>
       </c>
       <c r="B765" t="s">
-        <v>1122</v>
+        <v>968</v>
       </c>
     </row>
     <row r="766" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A766" t="s">
-        <v>1123</v>
+        <v>969</v>
       </c>
       <c r="B766" t="s">
-        <v>1123</v>
+        <v>969</v>
       </c>
     </row>
     <row r="767" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A767" t="s">
-        <v>1124</v>
+        <v>970</v>
       </c>
       <c r="B767" t="s">
-        <v>1124</v>
+        <v>970</v>
       </c>
     </row>
     <row r="768" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A768" t="s">
-        <v>1125</v>
+        <v>971</v>
       </c>
       <c r="B768" t="s">
-        <v>1125</v>
+        <v>971</v>
       </c>
     </row>
     <row r="769" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A769" t="s">
-        <v>1126</v>
+        <v>972</v>
       </c>
       <c r="B769" t="s">
-        <v>1126</v>
+        <v>972</v>
       </c>
     </row>
     <row r="770" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
-        <v>1127</v>
+        <v>973</v>
       </c>
       <c r="B770" t="s">
-        <v>1127</v>
+        <v>973</v>
       </c>
     </row>
     <row r="771" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
-        <v>1128</v>
+        <v>974</v>
       </c>
       <c r="B771" t="s">
-        <v>1128</v>
+        <v>974</v>
       </c>
     </row>
     <row r="772" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
-        <v>1129</v>
+        <v>975</v>
       </c>
       <c r="B772" t="s">
-        <v>1129</v>
+        <v>975</v>
       </c>
     </row>
     <row r="773" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
-        <v>1130</v>
+        <v>976</v>
       </c>
       <c r="B773" t="s">
-        <v>1130</v>
+        <v>976</v>
       </c>
     </row>
     <row r="774" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A774" t="s">
-        <v>1131</v>
+        <v>977</v>
       </c>
       <c r="B774" t="s">
-        <v>1131</v>
+        <v>977</v>
       </c>
     </row>
     <row r="775" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A775" t="s">
-        <v>1132</v>
+        <v>978</v>
       </c>
       <c r="B775" t="s">
-        <v>1132</v>
+        <v>978</v>
       </c>
     </row>
     <row r="776" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A776" t="s">
-        <v>1133</v>
+        <v>979</v>
       </c>
       <c r="B776" t="s">
-        <v>1133</v>
+        <v>979</v>
       </c>
     </row>
     <row r="777" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A777" t="s">
-        <v>1134</v>
+        <v>980</v>
       </c>
       <c r="B777" t="s">
-        <v>1134</v>
+        <v>980</v>
       </c>
     </row>
     <row r="778" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A778" t="s">
-        <v>1135</v>
+        <v>981</v>
       </c>
       <c r="B778" t="s">
-        <v>1135</v>
+        <v>981</v>
       </c>
     </row>
     <row r="779" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A779" t="s">
-        <v>1136</v>
+        <v>982</v>
       </c>
       <c r="B779" t="s">
-        <v>1136</v>
+        <v>982</v>
       </c>
     </row>
     <row r="780" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A780" t="s">
-        <v>1137</v>
+        <v>983</v>
       </c>
       <c r="B780" t="s">
-        <v>1137</v>
+        <v>983</v>
       </c>
     </row>
     <row r="781" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A781" t="s">
-        <v>1138</v>
+        <v>984</v>
       </c>
       <c r="B781" t="s">
-        <v>1138</v>
+        <v>984</v>
       </c>
     </row>
     <row r="782" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A782" t="s">
-        <v>1139</v>
+        <v>985</v>
       </c>
       <c r="B782" t="s">
-        <v>1139</v>
+        <v>985</v>
       </c>
     </row>
     <row r="783" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A783" t="s">
-        <v>1140</v>
+        <v>986</v>
       </c>
       <c r="B783" t="s">
-        <v>1140</v>
+        <v>986</v>
       </c>
     </row>
     <row r="784" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A784" t="s">
-        <v>1141</v>
+        <v>987</v>
       </c>
       <c r="B784" t="s">
-        <v>1141</v>
+        <v>987</v>
       </c>
     </row>
     <row r="785" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A785" t="s">
-        <v>1142</v>
+        <v>988</v>
       </c>
       <c r="B785" t="s">
-        <v>1142</v>
+        <v>988</v>
       </c>
     </row>
     <row r="786" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A786" t="s">
-        <v>1143</v>
+        <v>989</v>
       </c>
       <c r="B786" t="s">
-        <v>1143</v>
+        <v>989</v>
       </c>
     </row>
     <row r="787" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A787" t="s">
-        <v>1144</v>
+        <v>990</v>
       </c>
       <c r="B787" t="s">
-        <v>1144</v>
+        <v>990</v>
       </c>
     </row>
     <row r="788" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A788" t="s">
-        <v>1145</v>
+        <v>991</v>
       </c>
       <c r="B788" t="s">
-        <v>1145</v>
+        <v>991</v>
       </c>
     </row>
     <row r="789" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A789" t="s">
-        <v>1146</v>
+        <v>992</v>
       </c>
       <c r="B789" t="s">
-        <v>1146</v>
+        <v>992</v>
       </c>
     </row>
     <row r="790" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A790" t="s">
-        <v>1147</v>
+        <v>993</v>
       </c>
       <c r="B790" t="s">
-        <v>1147</v>
+        <v>993</v>
       </c>
     </row>
     <row r="791" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A791" t="s">
-        <v>1148</v>
+        <v>994</v>
       </c>
       <c r="B791" t="s">
-        <v>1148</v>
+        <v>994</v>
       </c>
     </row>
     <row r="792" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A792" t="s">
-        <v>1149</v>
+        <v>995</v>
       </c>
       <c r="B792" t="s">
-        <v>1149</v>
+        <v>995</v>
       </c>
     </row>
     <row r="793" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A793" t="s">
-        <v>1150</v>
+        <v>996</v>
       </c>
       <c r="B793" t="s">
-        <v>1150</v>
+        <v>996</v>
       </c>
     </row>
     <row r="794" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A794" t="s">
-        <v>1151</v>
+        <v>997</v>
       </c>
       <c r="B794" t="s">
-        <v>1151</v>
+        <v>997</v>
       </c>
     </row>
     <row r="795" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A795" t="s">
-        <v>1152</v>
+        <v>998</v>
       </c>
       <c r="B795" t="s">
-        <v>1152</v>
+        <v>998</v>
       </c>
     </row>
     <row r="796" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A796" t="s">
-        <v>1153</v>
+        <v>999</v>
       </c>
       <c r="B796" t="s">
-        <v>1153</v>
+        <v>999</v>
       </c>
     </row>
     <row r="797" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A797" t="s">
-        <v>1154</v>
+        <v>1000</v>
       </c>
       <c r="B797" t="s">
-        <v>1154</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="798" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A798" t="s">
-        <v>1155</v>
+        <v>1001</v>
       </c>
       <c r="B798" t="s">
-        <v>1155</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="799" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A799" t="s">
-        <v>1156</v>
+        <v>1002</v>
       </c>
       <c r="B799" t="s">
-        <v>1156</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A800" t="s">
-        <v>1157</v>
+        <v>1003</v>
       </c>
       <c r="B800" t="s">
-        <v>1157</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="801" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A801" t="s">
-        <v>1158</v>
+        <v>1004</v>
       </c>
       <c r="B801" t="s">
-        <v>1158</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="802" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A802" t="s">
-        <v>1159</v>
+        <v>1005</v>
       </c>
       <c r="B802" t="s">
-        <v>1159</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="803" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A803" t="s">
-        <v>1160</v>
+        <v>1006</v>
       </c>
       <c r="B803" t="s">
-        <v>1160</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="804" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A804" t="s">
-        <v>1161</v>
+        <v>1007</v>
       </c>
       <c r="B804" t="s">
-        <v>1161</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="805" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A805" t="s">
-        <v>1162</v>
+        <v>1008</v>
       </c>
       <c r="B805" t="s">
-        <v>1162</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="806" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A806" t="s">
-        <v>1163</v>
+        <v>1009</v>
       </c>
       <c r="B806" t="s">
-        <v>1163</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="807" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A807" t="s">
-        <v>1164</v>
+        <v>1010</v>
       </c>
       <c r="B807" t="s">
-        <v>1164</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="808" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A808" t="s">
-        <v>1165</v>
+        <v>1011</v>
       </c>
       <c r="B808" t="s">
-        <v>1165</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="809" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A809" t="s">
-        <v>1166</v>
+        <v>1012</v>
       </c>
       <c r="B809" t="s">
-        <v>1166</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="810" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A810" t="s">
-        <v>1167</v>
+        <v>1013</v>
       </c>
       <c r="B810" t="s">
-        <v>1167</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="811" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A811" t="s">
-        <v>1168</v>
+        <v>1014</v>
       </c>
       <c r="B811" t="s">
-        <v>1168</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="812" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A812" t="s">
-        <v>1169</v>
+        <v>1015</v>
       </c>
       <c r="B812" t="s">
-        <v>1169</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="813" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A813" t="s">
-        <v>1170</v>
+        <v>1016</v>
       </c>
       <c r="B813" t="s">
-        <v>1170</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="814" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A814" t="s">
-        <v>1171</v>
+        <v>1017</v>
       </c>
       <c r="B814" t="s">
-        <v>1171</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="815" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A815" t="s">
-        <v>1172</v>
+        <v>1018</v>
       </c>
       <c r="B815" t="s">
-        <v>1172</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="816" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A816" t="s">
-        <v>1173</v>
+        <v>1019</v>
       </c>
       <c r="B816" t="s">
-        <v>1173</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="817" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A817" t="s">
-        <v>1174</v>
+        <v>1020</v>
       </c>
       <c r="B817" t="s">
-        <v>1174</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="818" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A818" t="s">
-        <v>1175</v>
+        <v>1021</v>
       </c>
       <c r="B818" t="s">
-        <v>1175</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="819" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A819" t="s">
-        <v>1176</v>
+        <v>1022</v>
       </c>
       <c r="B819" t="s">
-        <v>1176</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="820" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A820" t="s">
-        <v>1177</v>
+        <v>1023</v>
       </c>
       <c r="B820" t="s">
-        <v>1177</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="821" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A821" t="s">
-        <v>1178</v>
+        <v>1024</v>
       </c>
       <c r="B821" t="s">
-        <v>1178</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="822" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A822" t="s">
-        <v>1179</v>
+        <v>1025</v>
       </c>
       <c r="B822" t="s">
-        <v>1179</v>
+        <v>1025</v>
       </c>
     </row>
     <row r="823" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A823" t="s">
-        <v>1180</v>
+        <v>1026</v>
       </c>
       <c r="B823" t="s">
-        <v>1180</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="824" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A824" t="s">
-        <v>1181</v>
+        <v>1027</v>
       </c>
       <c r="B824" t="s">
-        <v>1181</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="825" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A825" t="s">
-        <v>1182</v>
+        <v>1028</v>
       </c>
       <c r="B825" t="s">
-        <v>1182</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="826" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A826" t="s">
-        <v>1183</v>
+        <v>1029</v>
       </c>
       <c r="B826" t="s">
-        <v>1183</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="827" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A827" t="s">
-        <v>1184</v>
+        <v>1030</v>
       </c>
       <c r="B827" t="s">
-        <v>1184</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="828" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A828" t="s">
-        <v>1185</v>
+        <v>1031</v>
       </c>
       <c r="B828" t="s">
-        <v>1185</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="829" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A829" t="s">
-        <v>1186</v>
+        <v>1032</v>
       </c>
       <c r="B829" t="s">
-        <v>1186</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="830" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A830" t="s">
-        <v>1187</v>
+        <v>1033</v>
       </c>
       <c r="B830" t="s">
-        <v>1187</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="831" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A831" t="s">
-        <v>1188</v>
+        <v>1034</v>
       </c>
       <c r="B831" t="s">
-        <v>1188</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="832" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A832" t="s">
-        <v>1189</v>
+        <v>1035</v>
       </c>
       <c r="B832" t="s">
-        <v>1189</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="833" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A833" t="s">
-        <v>1190</v>
+        <v>1036</v>
       </c>
       <c r="B833" t="s">
-        <v>1190</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="834" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A834" t="s">
-        <v>1191</v>
+        <v>1037</v>
       </c>
       <c r="B834" t="s">
-        <v>1191</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="835" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A835" t="s">
-        <v>1192</v>
+        <v>1038</v>
       </c>
       <c r="B835" t="s">
-        <v>1192</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="836" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A836" t="s">
-        <v>1193</v>
+        <v>1039</v>
       </c>
       <c r="B836" t="s">
-        <v>1193</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="837" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A837" t="s">
-        <v>1186</v>
+        <v>1032</v>
       </c>
       <c r="B837" t="s">
-        <v>1186</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="838" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A838" t="s">
-        <v>1187</v>
+        <v>1033</v>
       </c>
       <c r="B838" t="s">
-        <v>1187</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="839" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A839" t="s">
-        <v>1188</v>
+        <v>1034</v>
       </c>
       <c r="B839" t="s">
-        <v>1188</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="840" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A840" t="s">
-        <v>1194</v>
+        <v>1040</v>
       </c>
       <c r="B840" t="s">
-        <v>1194</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="841" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A841" t="s">
-        <v>1190</v>
+        <v>1036</v>
       </c>
       <c r="B841" t="s">
-        <v>1190</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="842" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A842" t="s">
-        <v>1191</v>
+        <v>1037</v>
       </c>
       <c r="B842" t="s">
-        <v>1191</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="843" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A843" t="s">
-        <v>1192</v>
+        <v>1038</v>
       </c>
       <c r="B843" t="s">
-        <v>1192</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="844" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A844" t="s">
-        <v>1195</v>
+        <v>1041</v>
       </c>
       <c r="B844" t="s">
-        <v>1195</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="845" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A845" t="s">
-        <v>1186</v>
+        <v>1032</v>
       </c>
       <c r="B845" t="s">
-        <v>1186</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="846" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A846" t="s">
-        <v>1187</v>
+        <v>1033</v>
       </c>
       <c r="B846" t="s">
-        <v>1187</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="847" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A847" t="s">
-        <v>1188</v>
+        <v>1034</v>
       </c>
       <c r="B847" t="s">
-        <v>1188</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="848" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A848" t="s">
-        <v>1196</v>
+        <v>1042</v>
       </c>
       <c r="B848" t="s">
-        <v>1196</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="849" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A849" t="s">
-        <v>1190</v>
+        <v>1036</v>
       </c>
       <c r="B849" t="s">
-        <v>1190</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="850" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A850" t="s">
-        <v>1191</v>
+        <v>1037</v>
       </c>
       <c r="B850" t="s">
-        <v>1191</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="851" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A851" t="s">
-        <v>1192</v>
+        <v>1038</v>
       </c>
       <c r="B851" t="s">
-        <v>1192</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="852" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A852" t="s">
-        <v>1197</v>
+        <v>1043</v>
       </c>
       <c r="B852" t="s">
-        <v>1197</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="853" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A853" t="s">
-        <v>1186</v>
+        <v>1032</v>
       </c>
       <c r="B853" t="s">
-        <v>1186</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="854" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A854" t="s">
-        <v>1187</v>
+        <v>1033</v>
       </c>
       <c r="B854" t="s">
-        <v>1187</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="855" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A855" t="s">
-        <v>1188</v>
+        <v>1034</v>
       </c>
       <c r="B855" t="s">
-        <v>1188</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A856" t="s">
-        <v>1198</v>
+        <v>1044</v>
       </c>
       <c r="B856" t="s">
-        <v>1198</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="857" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A857" t="s">
-        <v>1190</v>
+        <v>1036</v>
       </c>
       <c r="B857" t="s">
-        <v>1190</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="858" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A858" t="s">
-        <v>1191</v>
+        <v>1037</v>
       </c>
       <c r="B858" t="s">
-        <v>1191</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="859" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A859" t="s">
-        <v>1192</v>
+        <v>1038</v>
       </c>
       <c r="B859" t="s">
-        <v>1192</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="860" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A860" t="s">
-        <v>1199</v>
+        <v>1045</v>
       </c>
       <c r="B860" t="s">
-        <v>1199</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="861" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A861" t="s">
-        <v>1200</v>
+        <v>1046</v>
       </c>
       <c r="B861" t="s">
-        <v>1200</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="862" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A862" t="s">
-        <v>1077</v>
+        <v>923</v>
       </c>
       <c r="B862" t="s">
-        <v>1077</v>
+        <v>923</v>
       </c>
     </row>
     <row r="863" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A863" t="s">
-        <v>1109</v>
+        <v>955</v>
       </c>
       <c r="B863" t="s">
-        <v>1109</v>
+        <v>955</v>
       </c>
     </row>
     <row r="864" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A864" t="s">
-        <v>1201</v>
+        <v>1047</v>
       </c>
       <c r="B864" t="s">
-        <v>1201</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="865" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A865" t="s">
-        <v>1202</v>
+        <v>1048</v>
       </c>
       <c r="B865" t="s">
-        <v>1202</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="866" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A866" t="s">
-        <v>1203</v>
+        <v>1049</v>
       </c>
       <c r="B866" t="s">
-        <v>1203</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="867" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A867" t="s">
-        <v>1204</v>
+        <v>1050</v>
       </c>
       <c r="B867" t="s">
-        <v>1204</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="868" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A868" t="s">
-        <v>1077</v>
+        <v>923</v>
       </c>
       <c r="B868" t="s">
-        <v>1077</v>
+        <v>923</v>
       </c>
     </row>
     <row r="869" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A869" t="s">
-        <v>1109</v>
+        <v>955</v>
       </c>
       <c r="B869" t="s">
-        <v>1109</v>
+        <v>955</v>
       </c>
     </row>
     <row r="870" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A870" t="s">
-        <v>1201</v>
+        <v>1047</v>
       </c>
       <c r="B870" t="s">
-        <v>1201</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="871" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A871" t="s">
-        <v>1202</v>
+        <v>1048</v>
       </c>
       <c r="B871" t="s">
-        <v>1202</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="872" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A872" t="s">
-        <v>1172</v>
+        <v>1018</v>
       </c>
       <c r="B872" t="s">
-        <v>1172</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="873" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A873" t="s">
-        <v>1205</v>
+        <v>1051</v>
       </c>
       <c r="B873" t="s">
-        <v>1205</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="874" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A874" t="s">
-        <v>1077</v>
+        <v>923</v>
       </c>
       <c r="B874" t="s">
-        <v>1077</v>
+        <v>923</v>
       </c>
     </row>
     <row r="875" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A875" t="s">
-        <v>1109</v>
+        <v>955</v>
       </c>
       <c r="B875" t="s">
-        <v>1109</v>
+        <v>955</v>
       </c>
     </row>
     <row r="876" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A876" t="s">
-        <v>1201</v>
+        <v>1047</v>
       </c>
       <c r="B876" t="s">
-        <v>1201</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="877" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A877" t="s">
-        <v>1202</v>
+        <v>1048</v>
       </c>
       <c r="B877" t="s">
-        <v>1202</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="878" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A878" t="s">
-        <v>1174</v>
+        <v>1020</v>
       </c>
       <c r="B878" t="s">
-        <v>1174</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="879" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A879" t="s">
-        <v>1206</v>
+        <v>1052</v>
       </c>
       <c r="B879" t="s">
-        <v>1206</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="880" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A880" t="s">
-        <v>1077</v>
+        <v>923</v>
       </c>
       <c r="B880" t="s">
-        <v>1077</v>
+        <v>923</v>
       </c>
     </row>
     <row r="881" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A881" t="s">
-        <v>1109</v>
+        <v>955</v>
       </c>
       <c r="B881" t="s">
-        <v>1109</v>
+        <v>955</v>
       </c>
     </row>
     <row r="882" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A882" t="s">
-        <v>1201</v>
+        <v>1047</v>
       </c>
       <c r="B882" t="s">
-        <v>1201</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="883" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A883" t="s">
-        <v>1202</v>
+        <v>1048</v>
       </c>
       <c r="B883" t="s">
-        <v>1202</v>
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="885" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A885" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B885" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="886" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A886" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B886" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="887" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A887" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B887" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="888" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A888" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B888" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="889" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A889" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B889" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="890" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A890" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B890" t="s">
+        <v>1103</v>
+      </c>
+    </row>
+    <row r="891" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A891" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B891" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="892" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A892" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B892" t="s">
+        <v>1105</v>
+      </c>
+    </row>
+    <row r="893" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A893" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B893" t="s">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="894" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A894" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B894" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="895" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A895" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B895" t="s">
+        <v>1108</v>
+      </c>
+    </row>
+    <row r="896" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A896" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B896" t="s">
+        <v>1109</v>
+      </c>
+    </row>
+    <row r="897" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A897" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B897" t="s">
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="898" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A898" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B898" t="s">
+        <v>1111</v>
+      </c>
+    </row>
+    <row r="899" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A899" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B899" t="s">
+        <v>1112</v>
+      </c>
+    </row>
+    <row r="900" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A900" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B900" t="s">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="901" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A901" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B901" t="s">
+        <v>1114</v>
+      </c>
+    </row>
+    <row r="902" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A902" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B902" t="s">
+        <v>1115</v>
+      </c>
+    </row>
+    <row r="903" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A903" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B903" t="s">
+        <v>1116</v>
+      </c>
+    </row>
+    <row r="904" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A904" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B904" t="s">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="905" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A905" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B905" t="s">
+        <v>1118</v>
+      </c>
+    </row>
+    <row r="906" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A906" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B906" t="s">
+        <v>1119</v>
+      </c>
+    </row>
+    <row r="907" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A907" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B907" t="s">
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="908" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A908" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B908" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="909" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A909" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B909" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="910" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A910" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B910" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="911" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A911" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B911" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="912" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A912" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B912" t="s">
+        <v>1125</v>
+      </c>
+    </row>
+    <row r="913" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A913" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B913" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="914" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A914" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B914" t="s">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="915" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A915" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B915" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="916" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A916" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B916" t="s">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="917" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A917" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B917" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="918" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A918" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B918" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="919" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A919" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B919" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="920" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A920" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B920" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="921" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A921" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B921" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="922" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A922" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B922" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="923" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A923" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B923" t="s">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="924" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A924" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B924" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="925" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A925" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B925" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="926" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A926" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B926" t="s">
+        <v>1107</v>
+      </c>
+    </row>
+    <row r="927" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A927" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B927" t="s">
+        <v>1138</v>
+      </c>
+    </row>
+    <row r="928" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A928" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B928" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="929" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A929" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B929" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="930" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A930" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B930" t="s">
+        <v>1141</v>
       </c>
     </row>
   </sheetData>
@@ -12550,1677 +12723,380 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBE4172-FC39-45CE-BD67-BA23D6FB1A86}">
-  <dimension ref="A3:B187"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B187"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1099</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>902</v>
-      </c>
-      <c r="B3" t="str">
-        <f>A3</f>
-        <v>Cự Môn tọa thủ cung Mệnh</v>
+        <v>1055</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>903</v>
-      </c>
-      <c r="B4" t="str">
-        <f>RIGHT(A4,LEN(A4)-17)</f>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mão</v>
+        <v>1056</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>904</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" ref="B5:B68" si="0">RIGHT(A5,LEN(A5)-17)</f>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</v>
+        <v>1057</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1102</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>905</v>
-      </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Thái Tuế, Thiên Hình, Thiên Khôi, Thiên Việt</v>
+        <v>1058</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1103</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>906</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mão gặp Tuế Hổ Phù</v>
+        <v>1059</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1104</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>907</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Lộc Tồn</v>
+        <v>1060</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1105</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>908</v>
-      </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mão gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</v>
+        <v>1061</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1106</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>909</v>
-      </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mão gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</v>
+        <v>1062</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1107</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>910</v>
-      </c>
-      <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</v>
+        <v>1063</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1108</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>911</v>
-      </c>
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dậu</v>
+        <v>1064</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1109</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>912</v>
-      </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</v>
+        <v>1065</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1110</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>913</v>
-      </c>
-      <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Thái Tuế, Thiên Hình, Thiên Khôi, Thiên Việt</v>
+        <v>1066</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1111</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>914</v>
-      </c>
-      <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dậu gặp Tuế Hổ Phù</v>
+        <v>1067</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1112</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>915</v>
-      </c>
-      <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Lộc Tồn</v>
+        <v>1068</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1113</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>916</v>
-      </c>
-      <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dậu gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</v>
+        <v>1069</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1114</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>917</v>
-      </c>
-      <c r="B18" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</v>
+        <v>1070</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1115</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>918</v>
-      </c>
-      <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</v>
+        <v>1071</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1116</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>919</v>
-      </c>
-      <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tý</v>
+        <v>1072</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1117</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>920</v>
-      </c>
-      <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</v>
+        <v>1073</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1118</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>921</v>
-      </c>
-      <c r="B22" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Thái Tuế, Thiên Hình, Thiên Khôi, Thiên Việt</v>
+        <v>1074</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1119</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>922</v>
-      </c>
-      <c r="B23" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tý gặp Tuế Hổ Phù</v>
+        <v>1075</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>923</v>
-      </c>
-      <c r="B24" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tý đồng cung Lộc Tồn</v>
+        <v>1076</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1121</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>924</v>
-      </c>
-      <c r="B25" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tý gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</v>
+        <v>1077</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1122</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>925</v>
-      </c>
-      <c r="B26" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tý gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</v>
+        <v>1078</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1123</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>926</v>
-      </c>
-      <c r="B27" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</v>
+        <v>1079</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1124</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>927</v>
-      </c>
-      <c r="B28" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Ngọ</v>
+        <v>1080</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1125</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>928</v>
-      </c>
-      <c r="B29" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</v>
+        <v>1081</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1126</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>929</v>
-      </c>
-      <c r="B30" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Thái Tuế, Thiên Hình, Thiên Khôi, Thiên Việt</v>
+        <v>1082</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1127</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>930</v>
-      </c>
-      <c r="B31" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Ngọ gặp Tuế Hổ Phù</v>
+        <v>1083</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1128</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>931</v>
-      </c>
-      <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Ngọ đồng cung Lộc Tồn</v>
+        <v>1084</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1129</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>932</v>
-      </c>
-      <c r="B33" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Ngọ gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</v>
+        <v>1085</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1130</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>933</v>
-      </c>
-      <c r="B34" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Ngọ gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</v>
+        <v>1086</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1131</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>934</v>
-      </c>
-      <c r="B35" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</v>
+        <v>1087</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1132</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>935</v>
-      </c>
-      <c r="B36" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dần</v>
+        <v>1088</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1133</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>936</v>
-      </c>
-      <c r="B37" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dần gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</v>
+        <v>1089</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1134</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>937</v>
-      </c>
-      <c r="B38" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dần gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Thái Tuế, Thiên Hình, Thiên Khôi, Thiên Việt</v>
+        <v>1090</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1135</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>938</v>
-      </c>
-      <c r="B39" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dần gặp Tuế Hổ Phù</v>
+        <v>1091</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1136</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>939</v>
-      </c>
-      <c r="B40" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dần đồng cung Lộc Tồn</v>
+        <v>1092</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1137</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>940</v>
-      </c>
-      <c r="B41" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dần gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</v>
+        <v>1093</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1104</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>941</v>
-      </c>
-      <c r="B42" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</v>
+        <v>1094</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1107</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>942</v>
-      </c>
-      <c r="B43" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</v>
+        <v>1095</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1138</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>943</v>
-      </c>
-      <c r="B44" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thân</v>
+        <v>1096</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1139</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>944</v>
-      </c>
-      <c r="B45" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</v>
+        <v>1097</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1140</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>945</v>
-      </c>
-      <c r="B46" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Thái Tuế, Thiên Hình, Thiên Khôi, Thiên Việt</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>946</v>
-      </c>
-      <c r="B47" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thân gặp Tuế Hổ Phù</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>947</v>
-      </c>
-      <c r="B48" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thân đồng cung Lộc Tồn</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>948</v>
-      </c>
-      <c r="B49" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thân gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>949</v>
-      </c>
-      <c r="B50" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thân gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>950</v>
-      </c>
-      <c r="B51" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>951</v>
-      </c>
-      <c r="B52" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Hợi</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>952</v>
-      </c>
-      <c r="B53" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>953</v>
-      </c>
-      <c r="B54" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Thái Tuế, Thiên Hình, Thiên Khôi, Thiên Việt</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>954</v>
-      </c>
-      <c r="B55" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Hợi gặp Tuế Hổ Phù</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>955</v>
-      </c>
-      <c r="B56" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Hợi đồng cung Lộc Tồn</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>956</v>
-      </c>
-      <c r="B57" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Hợi gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>957</v>
-      </c>
-      <c r="B58" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Hợi gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>958</v>
-      </c>
-      <c r="B59" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>959</v>
-      </c>
-      <c r="B60" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Sửu</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>960</v>
-      </c>
-      <c r="B61" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>961</v>
-      </c>
-      <c r="B62" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Hóa Khoa, Thái Tuế, Thiên Hình, Tả Phù, Hữu Bật, Hỏa Tinh, Linh Tinh</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>962</v>
-      </c>
-      <c r="B63" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Sửu gặp Tuế Hổ Phù</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>963</v>
-      </c>
-      <c r="B64" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Sửu đồng cung Lộc Tồn</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>964</v>
-      </c>
-      <c r="B65" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Sửu gặp Hoá Lộc, Thái Tuế</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>965</v>
-      </c>
-      <c r="B66" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Sửu gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>966</v>
-      </c>
-      <c r="B67" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Sửu gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>967</v>
-      </c>
-      <c r="B68" t="str">
-        <f t="shared" si="0"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>968</v>
-      </c>
-      <c r="B69" t="str">
-        <f t="shared" ref="B69:B132" si="1">RIGHT(A69,LEN(A69)-17)</f>
-        <v xml:space="preserve">Cự Môn tọa thủ cung Mệnh ở Sửu gặp Thiên Hư, Thiên Không, Địa Không, Địa Kiếp </v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>969</v>
-      </c>
-      <c r="B70" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mùi</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>970</v>
-      </c>
-      <c r="B71" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>971</v>
-      </c>
-      <c r="B72" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Hóa Khoa, Thái Tuế, Thiên Hình, Tả Phù, Hữu Bật, Hỏa Tinh, Linh Tinh</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>972</v>
-      </c>
-      <c r="B73" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mùi gặp Tuế Hổ Phù</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>973</v>
-      </c>
-      <c r="B74" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mùi đồng cung Lộc Tồn</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>974</v>
-      </c>
-      <c r="B75" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mùi gặp Hoá Lộc, Thái Tuế</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>975</v>
-      </c>
-      <c r="B76" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mùi gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>976</v>
-      </c>
-      <c r="B77" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mùi gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>977</v>
-      </c>
-      <c r="B78" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>978</v>
-      </c>
-      <c r="B79" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">Cự Môn tọa thủ cung Mệnh ở Mùi gặp Thiên Hư, Thiên Không, Địa Không, Địa Kiếp </v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>979</v>
-      </c>
-      <c r="B80" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thìn</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>980</v>
-      </c>
-      <c r="B81" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>981</v>
-      </c>
-      <c r="B82" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Hóa Khoa, Thái Tuế, Thiên Hình, Tả Phù, Hữu Bật, Hỏa Tinh, Linh Tinh</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>982</v>
-      </c>
-      <c r="B83" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thìn gặp Tuế Hổ Phù</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>983</v>
-      </c>
-      <c r="B84" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thìn đồng cung Lộc Tồn</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>984</v>
-      </c>
-      <c r="B85" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thìn gặp Hoá Lộc, Thái Tuế</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>985</v>
-      </c>
-      <c r="B86" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thìn gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>986</v>
-      </c>
-      <c r="B87" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thìn gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>987</v>
-      </c>
-      <c r="B88" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>988</v>
-      </c>
-      <c r="B89" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">Cự Môn tọa thủ cung Mệnh ở Thìn gặp Thiên Hư, Thiên Không, Địa Không, Địa Kiếp </v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>989</v>
-      </c>
-      <c r="B90" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tuất</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>990</v>
-      </c>
-      <c r="B91" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>991</v>
-      </c>
-      <c r="B92" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Hóa Khoa, Thái Tuế, Thiên Hình, Tả Phù, Hữu Bật, Hỏa Tinh, Linh Tinh</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>992</v>
-      </c>
-      <c r="B93" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tuất gặp Tuế Hổ Phù</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>993</v>
-      </c>
-      <c r="B94" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tuất đồng cung Lộc Tồn</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>994</v>
-      </c>
-      <c r="B95" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tuất gặp Hoá Lộc, Thái Tuế</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>995</v>
-      </c>
-      <c r="B96" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tuất gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>996</v>
-      </c>
-      <c r="B97" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tuất gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>997</v>
-      </c>
-      <c r="B98" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>998</v>
-      </c>
-      <c r="B99" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">Cự Môn tọa thủ cung Mệnh ở Tuất gặp Thiên Hư, Thiên Không, Địa Không, Địa Kiếp </v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>999</v>
-      </c>
-      <c r="B100" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tỵ</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B101" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>1001</v>
-      </c>
-      <c r="B102" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Hóa Khoa, Thái Tuế, Thiên Hình, Tả Phù, Hữu Bật, Hỏa Tinh, Linh Tinh</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>1002</v>
-      </c>
-      <c r="B103" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tỵ gặp Tuế Hổ Phù</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>1003</v>
-      </c>
-      <c r="B104" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tỵ đồng cung Lộc Tồn</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>1004</v>
-      </c>
-      <c r="B105" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tỵ gặp Hoá Lộc, Thái Tuế</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>1005</v>
-      </c>
-      <c r="B106" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tỵ gặp các sao:  Thiên Không, Địa Không, Địa Kiếp</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>1006</v>
-      </c>
-      <c r="B107" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tỵ gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>1007</v>
-      </c>
-      <c r="B108" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>1008</v>
-      </c>
-      <c r="B109" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">Cự Môn tọa thủ cung Mệnh ở Tỵ gặp Thiên Hư, Thiên Không, Địa Không, Địa Kiếp </v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>1009</v>
-      </c>
-      <c r="B110" t="str">
-        <f t="shared" si="1"/>
-        <v>Người tuổi Đ. có Cự Môn tọa thủ cung Mệnh ở Thìn</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>1010</v>
-      </c>
-      <c r="B111" t="str">
-        <f t="shared" si="1"/>
-        <v>Người tuổi C. có Cự Môn tọa thủ cung Mệnh ở Thìn</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>1011</v>
-      </c>
-      <c r="B112" t="str">
-        <f t="shared" si="1"/>
-        <v>Người tuổi Q. có Cự Môn tọa thủ cung Mệnh ở Thìn</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>1012</v>
-      </c>
-      <c r="B113" t="str">
-        <f t="shared" si="1"/>
-        <v>Người tuổi T. có Cự Môn tọa thủ cung Mệnh ở Thìn</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>1013</v>
-      </c>
-      <c r="B114" t="str">
-        <f t="shared" si="1"/>
-        <v>Người tuổi Đ. có Cự Môn tọa thủ cung Mệnh ở Tuất</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>1014</v>
-      </c>
-      <c r="B115" t="str">
-        <f t="shared" si="1"/>
-        <v>Người tuổi C. có Cự Môn tọa thủ cung Mệnh ở Tuất</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
-        <v>1015</v>
-      </c>
-      <c r="B116" t="str">
-        <f t="shared" si="1"/>
-        <v>Người tuổi Q. có Cự Môn tọa thủ cung Mệnh ở Tuất</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>1016</v>
-      </c>
-      <c r="B117" t="str">
-        <f t="shared" si="1"/>
-        <v>Người tuổi T. có Cự Môn tọa thủ cung Mệnh ở Tuất</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>1017</v>
-      </c>
-      <c r="B118" t="str">
-        <f t="shared" si="1"/>
-        <v>Người tuổi Ất có Cự Môn tọa thủ cung Mệnh ở Sửu</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>1018</v>
-      </c>
-      <c r="B119" t="str">
-        <f t="shared" si="1"/>
-        <v>Người tuổi Bính có Cự Môn tọa thủ cung Mệnh ở Sửu</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>1019</v>
-      </c>
-      <c r="B120" t="str">
-        <f t="shared" si="1"/>
-        <v>Người tuổi Ất có Cự Môn tọa thủ cung Mệnh ở Mùi</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>1020</v>
-      </c>
-      <c r="B121" t="str">
-        <f t="shared" si="1"/>
-        <v>Người tuổi Bính có Cự Môn tọa thủ cung Mệnh ở Mùi</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>1021</v>
-      </c>
-      <c r="B122" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh đồng cung Hoá Kỵ</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>1022</v>
-      </c>
-      <c r="B123" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh đồng cung Thái Dương</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>1023</v>
-      </c>
-      <c r="B124" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dần đồng cung Thái Dương</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>1024</v>
-      </c>
-      <c r="B125" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thân đồng cung Thái Dương</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>1025</v>
-      </c>
-      <c r="B126" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thân gặp Thái Dương, Thiên Di có Thái Dương</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>1026</v>
-      </c>
-      <c r="B127" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dần gặp Thái Dương, Thiên Di có Thái Dương</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>1027</v>
-      </c>
-      <c r="B128" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Thiên Di đồng cung Thái Dương xung chiếu cung Mệnh ở Dần</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>1028</v>
-      </c>
-      <c r="B129" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dần đồng cung Thái Dương gặp Hoá Lộc</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>1029</v>
-      </c>
-      <c r="B130" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Thân đồng cung Thái Dương gặp Hoá Lộc</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>1030</v>
-      </c>
-      <c r="B131" t="str">
-        <f t="shared" si="1"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dần đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>1031</v>
-      </c>
-      <c r="B132" t="str">
-        <f t="shared" si="1"/>
-        <v>Người tuổi Ất có Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>1032</v>
-      </c>
-      <c r="B133" t="str">
-        <f t="shared" ref="B133:B187" si="2">RIGHT(A133,LEN(A133)-17)</f>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B134" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ gặp Đại Hao, Tiểu Hao</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>1034</v>
-      </c>
-      <c r="B135" t="str">
-        <f t="shared" si="2"/>
-        <v>Quý chị có Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>1035</v>
-      </c>
-      <c r="B136" t="str">
-        <f t="shared" si="2"/>
-        <v>Người tuổi Ất có Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>1036</v>
-      </c>
-      <c r="B137" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>1037</v>
-      </c>
-      <c r="B138" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ gặp Đại Hao, Tiểu Hao</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>1038</v>
-      </c>
-      <c r="B139" t="str">
-        <f t="shared" si="2"/>
-        <v>Quý chị có Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>1039</v>
-      </c>
-      <c r="B140" t="str">
-        <f t="shared" si="2"/>
-        <v>Người tuổi Tân có Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>1032</v>
-      </c>
-      <c r="B141" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B142" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ gặp Đại Hao, Tiểu Hao</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>1034</v>
-      </c>
-      <c r="B143" t="str">
-        <f t="shared" si="2"/>
-        <v>Quý chị có Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>1040</v>
-      </c>
-      <c r="B144" t="str">
-        <f t="shared" si="2"/>
-        <v>Người tuổi Tân có Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>1036</v>
-      </c>
-      <c r="B145" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>1037</v>
-      </c>
-      <c r="B146" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ gặp Đại Hao, Tiểu Hao</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>1038</v>
-      </c>
-      <c r="B147" t="str">
-        <f t="shared" si="2"/>
-        <v>Quý chị có Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>1041</v>
-      </c>
-      <c r="B148" t="str">
-        <f t="shared" si="2"/>
-        <v>Người tuổi Kỷ có Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>1032</v>
-      </c>
-      <c r="B149" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B150" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ gặp Đại Hao, Tiểu Hao</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>1034</v>
-      </c>
-      <c r="B151" t="str">
-        <f t="shared" si="2"/>
-        <v>Quý chị có Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>1042</v>
-      </c>
-      <c r="B152" t="str">
-        <f t="shared" si="2"/>
-        <v>Người tuổi Kỷ có Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>1036</v>
-      </c>
-      <c r="B153" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>1037</v>
-      </c>
-      <c r="B154" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ gặp Đại Hao, Tiểu Hao</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>1038</v>
-      </c>
-      <c r="B155" t="str">
-        <f t="shared" si="2"/>
-        <v>Quý chị có Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>1043</v>
-      </c>
-      <c r="B156" t="str">
-        <f t="shared" si="2"/>
-        <v>Người tuổi Bính có Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>1032</v>
-      </c>
-      <c r="B157" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>1033</v>
-      </c>
-      <c r="B158" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ gặp Đại Hao, Tiểu Hao</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>1034</v>
-      </c>
-      <c r="B159" t="str">
-        <f t="shared" si="2"/>
-        <v>Quý chị có Cự Môn tọa thủ cung Mệnh ở Mão đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>1044</v>
-      </c>
-      <c r="B160" t="str">
-        <f t="shared" si="2"/>
-        <v>Người tuổi Bính có Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>1036</v>
-      </c>
-      <c r="B161" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>1037</v>
-      </c>
-      <c r="B162" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ gặp Đại Hao, Tiểu Hao</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>1038</v>
-      </c>
-      <c r="B163" t="str">
-        <f t="shared" si="2"/>
-        <v>Quý chị có Cự Môn tọa thủ cung Mệnh ở Dậu đồng cung Thiên Cơ</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>1045</v>
-      </c>
-      <c r="B164" t="str">
-        <f t="shared" si="2"/>
-        <v>Người tuổi Bính có Cự Môn tọa thủ cung Mệnh ở Thìn</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>1046</v>
-      </c>
-      <c r="B165" t="str">
-        <f t="shared" si="2"/>
-        <v>Người tuổi Tân có Cự Môn tọa thủ cung Mệnh ở Thìn</v>
-      </c>
-    </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>1047</v>
-      </c>
-      <c r="B166" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tý đồng cung Lộc Tồn</v>
-      </c>
-    </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>1048</v>
-      </c>
-      <c r="B167" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Hợi đồng cung Lộc Tồn</v>
-      </c>
-    </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>1049</v>
-      </c>
-      <c r="B168" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tý gặp Khoa Lộc Quyền</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>1050</v>
-      </c>
-      <c r="B169" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Ngọ gặp Khoa Lộc Quyền</v>
-      </c>
-    </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>1051</v>
-      </c>
-      <c r="B170" t="str">
-        <f t="shared" si="2"/>
-        <v>Người tuổi Bính có Cự Môn tọa thủ cung Mệnh ở Tuất</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>1052</v>
-      </c>
-      <c r="B171" t="str">
-        <f t="shared" si="2"/>
-        <v>Người tuổi Tân có Cự Môn tọa thủ cung Mệnh ở Tuất</v>
-      </c>
-    </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>1047</v>
-      </c>
-      <c r="B172" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tý đồng cung Lộc Tồn</v>
-      </c>
-    </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>1048</v>
-      </c>
-      <c r="B173" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Hợi đồng cung Lộc Tồn</v>
-      </c>
-    </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>1049</v>
-      </c>
-      <c r="B174" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tý gặp Khoa Lộc Quyền</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>1050</v>
-      </c>
-      <c r="B175" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Ngọ gặp Khoa Lộc Quyền</v>
-      </c>
-    </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>1053</v>
-      </c>
-      <c r="B176" t="str">
-        <f t="shared" si="2"/>
-        <v>Người tuổi Bính có Cự Môn tọa thủ cung Mệnh ở Sửu</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>1054</v>
-      </c>
-      <c r="B177" t="str">
-        <f t="shared" si="2"/>
-        <v>Người tuổi Tân có Cự Môn tọa thủ cung Mệnh ở Sửu</v>
-      </c>
-    </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>1047</v>
-      </c>
-      <c r="B178" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tý đồng cung Lộc Tồn</v>
-      </c>
-    </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>1048</v>
-      </c>
-      <c r="B179" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Hợi đồng cung Lộc Tồn</v>
-      </c>
-    </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>1049</v>
-      </c>
-      <c r="B180" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tý gặp Khoa Lộc Quyền</v>
-      </c>
-    </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>1050</v>
-      </c>
-      <c r="B181" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Ngọ gặp Khoa Lộc Quyền</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>1055</v>
-      </c>
-      <c r="B182" t="str">
-        <f t="shared" si="2"/>
-        <v>Người tuổi Bính có Cự Môn tọa thủ cung Mệnh ở Mùi</v>
-      </c>
-    </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>1056</v>
-      </c>
-      <c r="B183" t="str">
-        <f t="shared" si="2"/>
-        <v>Người tuổi Tân có Cự Môn tọa thủ cung Mệnh ở Mùi</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>1047</v>
-      </c>
-      <c r="B184" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tý đồng cung Lộc Tồn</v>
-      </c>
-    </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A185" t="s">
-        <v>1048</v>
-      </c>
-      <c r="B185" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Hợi đồng cung Lộc Tồn</v>
-      </c>
-    </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A186" t="s">
-        <v>1049</v>
-      </c>
-      <c r="B186" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Tý gặp Khoa Lộc Quyền</v>
-      </c>
-    </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A187" t="s">
-        <v>1050</v>
-      </c>
-      <c r="B187" t="str">
-        <f t="shared" si="2"/>
-        <v>Cự Môn tọa thủ cung Mệnh ở Ngọ gặp Khoa Lộc Quyền</v>
+        <v>1098</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
An Luận Mệnh Phá Quân
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -1,33 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308C2CE5-BD1B-4ECA-AC20-3F5BFC08443A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF544FCC-7FDE-4913-958D-D707B466B4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2635" uniqueCount="1344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2687" uniqueCount="1371">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -3521,276 +3530,6 @@
     <t>Thất Sát tọa thủ cung Mệnh</t>
   </si>
   <si>
-    <t>luanmenh.js:2883 Thất Sát tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2886 Quý chị có Thất Sát tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2892 Thất Sát tọa thủ cung Mệnh ở Dần gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc, Thiên Mã, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2897 Thất Sát tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2901 Thất Sát tọa thủ cung Mệnh ở Dần đồng cung Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2883 Thất Sát tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2886 Quý chị có Thất Sát tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2892 Thất Sát tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc, Thiên Mã, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2897 Thất Sát tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2901 Thất Sát tọa thủ cung Mệnh ở Thân đồng cung Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2883 Thất Sát tọa thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2886 Quý chị có Thất Sát tọa thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2892 Thất Sát tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc, Thiên Mã, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2897 Thất Sát tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2901 Thất Sát tọa thủ cung Mệnh ở Tý đồng cung Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2883 Thất Sát tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2886 Quý chị có Thất Sát tọa thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2892 Thất Sát tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc, Thiên Mã, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2897 Thất Sát tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2901 Thất Sát tọa thủ cung Mệnh ở Ngọ đồng cung Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2883 Thất Sát tọa thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2886 Quý chị có Thất Sát tọa thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2892 Thất Sát tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc, Thiên Mã, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2897 Thất Sát tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2901 Thất Sát tọa thủ cung Mệnh ở Tỵ đồng cung Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2883 Thất Sát tọa thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2886 Quý chị có Thất Sát tọa thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2892 Thất Sát tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc, Thiên Mã, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2897 Thất Sát tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2901 Thất Sát tọa thủ cung Mệnh ở Hợi đồng cung Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2883 Thất Sát tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2886 Quý chị có Thất Sát tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2892 Thất Sát tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc, Thiên Mã, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2897 Thất Sát tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2901 Thất Sát tọa thủ cung Mệnh ở Sửu đồng cung Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2883 Thất Sát tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2886 Quý chị có Thất Sát tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2892 Thất Sát tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc, Thiên Mã, Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2897 Thất Sát tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2901 Thất Sát tọa thủ cung Mệnh ở Mùi đồng cung Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2909 Người tuổi G. có Thất Sát tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2909 Người tuổi G. có Thất Sát tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2909 Người tuổi C. có Thất Sát tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2909 Người tuổi C. có Thất Sát tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2909 Người tuổi Đ. có Thất Sát tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2909 Người tuổi Đ. có Thất Sát tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2909 Người tuổi K. có Thất Sát tọa thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2909 Người tuổi K. có Thất Sát tọa thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2918 Thất Sát tọa thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2921 Thất Sát tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Tả Phù, Hữu Bật, Long Trì, Phượng Các, Ân Quang, Thiên Quý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2924 Thất Sát tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2927 Thất Sát tọa thủ cung Mệnh ở Mão đồng cung Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2930 Quý chị có Thất Sát tọa thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2918 Thất Sát tọa thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2921 Thất Sát tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Tả Phù, Hữu Bật, Long Trì, Phượng Các, Ân Quang, Thiên Quý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2924 Thất Sát tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2927 Thất Sát tọa thủ cung Mệnh ở Dậu đồng cung Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2930 Quý chị có Thất Sát tọa thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2918 Thất Sát tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2921 Thất Sát tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Tả Phù, Hữu Bật, Long Trì, Phượng Các, Ân Quang, Thiên Quý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2924 Thất Sát tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2927 Thất Sát tọa thủ cung Mệnh ở Thìn đồng cung Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2930 Quý chị có Thất Sát tọa thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2918 Thất Sát tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2921 Thất Sát tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Tả Phù, Hữu Bật, Long Trì, Phượng Các, Ân Quang, Thiên Quý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2924 Thất Sát tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2927 Thất Sát tọa thủ cung Mệnh ở Tuất đồng cung Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2930 Quý chị có Thất Sát tọa thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2938 Người tuổi Ất có Thất Sát tọa thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2938 Người tuổi Tân có Thất Sát tọa thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2938 Người tuổi Ất có Thất Sát tọa thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2938 Người tuổi Tân có Thất Sát tọa thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2944 Thất Sát tọa thủ cung Mệnh ở Tỵ đồng cung Tử Vi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2947 Thất Sát tọa thủ cung Mệnh ở Tỵ đồng cung Tử Vi gặp các sao cát tinh:  Hữu Bật, Hoá Khoa, Thiên Mã, Quốc Ấn, Hồng Loan</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2954 Thất Sát tọa thủ cung Mệnh ở Sửu đồng cung Liêm Trinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2959 Người tuổi Ất có Thất Sát tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2959 Người tuổi Kỷ có Thất Sát tọa thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2954 Thất Sát tọa thủ cung Mệnh ở Mùi đồng cung Liêm Trinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2959 Người tuổi Ất có Thất Sát tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2959 Người tuổi Kỷ có Thất Sát tọa thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2967 Thất Sát tọa thủ cung Mệnh gặp Phá Quân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2971 Quý chị tuổi Tân có Thất Sát tọa thủ cung Mệnh gặp Phá Quân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2971 Quý chị tuổi Đinh có Thất Sát tọa thủ cung Mệnh gặp Phá Quân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2967 Thất Sát tọa thủ cung Mệnh gặp Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2971 Quý chị tuổi Tân có Thất Sát tọa thủ cung Mệnh gặp Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2971 Quý chị tuổi Đinh có Thất Sát tọa thủ cung Mệnh gặp Tham Lang</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2978 Thất Sát tọa thủ cung Mệnh gặp Kình Dương, Đà La, Hoả Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2984 Người tuổi Bính có Thất Sát tọa thủ cung Mệnh đồng cung Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2988 Thất Sát tọa thủ cung Phu Thê Cuộc gặp Kình Dương, Đà La, Hoả Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:2984 Người tuổi Mậu có Thất Sát tọa thủ cung Mệnh đồng cung Kình Dương</t>
-  </si>
-  <si>
     <t>Thất Sát tọa thủ cung Mệnh ở Dần</t>
   </si>
   <si>
@@ -4059,6 +3798,357 @@
   </si>
   <si>
     <t>Người tuổi Mậu có Thất Sát tọa thủ cung Mệnh đồng cung Kình Dương</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3146 Phá Quân tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">luanmenh.js:3146 Phá Quân tọa thủ cung Mệnh ở Sửu </t>
+  </si>
+  <si>
+    <t>luanmenh.js:3146 Phá Quân tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3146 Phá Quân tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3146 Phá Quân tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3158 Người tuổi Đinh có Phá Quân tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3158 Người tuổi Kỷ có Phá Quân tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3158 Người tuổi Quý có Phá Quân tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3158 Người tuổi Đinh có Phá Quân tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3158 Người tuổi Kỷ có Phá Quân tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3158 Người tuổi Quý có Phá Quân tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3168 Phá Quân tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3172 Phá Quân tọa thủ cung Mệnh ở Dần có cách cục: Bạch Hổ, Thiên Hình, Hoá Kỵ, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3175 Phá Quân tọa thủ cung Mệnh ở Dần có cách cục: Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3178 Phá Quân tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3168 Phá Quân tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3172 Phá Quân tọa thủ cung Mệnh ở Thân có cách cục: Bạch Hổ, Thiên Hình, Hoá Kỵ, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3175 Phá Quân tọa thủ cung Mệnh ở Thân có cách cục: Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3178 Phá Quân tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3168 Phá Quân tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3172 Phá Quân tọa thủ cung Mệnh ở Mão có cách cục: Bạch Hổ, Thiên Hình, Hoá Kỵ, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3175 Phá Quân tọa thủ cung Mệnh ở Mão có cách cục: Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3178 Phá Quân tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3168 Phá Quân tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3172 Phá Quân tọa thủ cung Mệnh ở Dậu có cách cục: Bạch Hổ, Thiên Hình, Hoá Kỵ, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3175 Phá Quân tọa thủ cung Mệnh ở Dậu có cách cục: Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3178 Phá Quân tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3168 Phá Quân tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3172 Phá Quân tọa thủ cung Mệnh ở Tỵ có cách cục: Bạch Hổ, Thiên Hình, Hoá Kỵ, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3175 Phá Quân tọa thủ cung Mệnh ở Tỵ có cách cục: Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3178 Phá Quân tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">luanmenh.js:3168 Phá Quân tọa thủ cung Mệnh ở Hợi </t>
+  </si>
+  <si>
+    <t>luanmenh.js:3172 Phá Quân tọa thủ cung Mệnh ở Hợi  có cách cục: Bạch Hổ, Thiên Hình, Hoá Kỵ, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3175 Phá Quân tọa thủ cung Mệnh ở Hợi  có cách cục: Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3178 Phá Quân tọa thủ cung Mệnh ở Hợi  gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3189 Người tuổi Ất có Phá Quân tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3189 Người tuổi Tân có Phá Quân tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3189 Người tuổi Quý có Phá Quân tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3189 Người tuổi Ất có Phá Quân tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3189 Người tuổi Tân có Phá Quân tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3189 Người tuổi Quý có Phá Quân tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3198 Người tuổi Giáp có Phá Quân tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3198 Người tuổi Giáp có Phá Quân tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3198 Người tuổi Canh có Phá Quân tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3198 Người tuổi Canh có Phá Quân tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3198 Người tuổi Đinh có Phá Quân tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3198 Người tuổi Đinh có Phá Quân tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3198 Người tuổi Kỷ có Phá Quân tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3198 Người tuổi Kỷ có Phá Quân tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3206 Người tuổi Mậu có Phá Quân tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3206 Người tuổi Mậu có Phá Quân tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3212 Phá Quân tọa thủ cung Mệnh gặp Thiên Việt, Đại Hao, Tiểu Hao, Hoả Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3217 Phá Quân tọa thủ cung Mệnh gặp Hoả Tinh, Linh Tinh, Thiên Việt, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3222 Phá Quân tọa thủ cung Mệnh ở Ngọ đồng cung Lộc Tồn và gặp Thiếu Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3228 Phá Quân tọa thủ cung Mệnh ở Thìn gặp Hoá Lộc, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3228 Phá Quân tọa thủ cung Mệnh ở Tuất gặp Hoá Lộc, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3228 Phá Quân tọa thủ cung Mệnh ở Sửu gặp Hoá Lộc, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3228 Phá Quân tọa thủ cung Mệnh ở Mùi gặp Hoá Lộc, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phá Quân tọa thủ cung Mệnh ở Sửu </t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>Người tuổi Đinh có Phá Quân tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>Người tuổi Kỷ có Phá Quân tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>Người tuổi Quý có Phá Quân tọa thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>Người tuổi Đinh có Phá Quân tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Người tuổi Kỷ có Phá Quân tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Người tuổi Quý có Phá Quân tọa thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Dần có cách cục: Bạch Hổ, Thiên Hình, Hoá Kỵ, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Dần có cách cục: Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Thân có cách cục: Bạch Hổ, Thiên Hình, Hoá Kỵ, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Thân có cách cục: Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Mão có cách cục: Bạch Hổ, Thiên Hình, Hoá Kỵ, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Mão có cách cục: Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Dậu có cách cục: Bạch Hổ, Thiên Hình, Hoá Kỵ, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Dậu có cách cục: Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Tỵ có cách cục: Bạch Hổ, Thiên Hình, Hoá Kỵ, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Tỵ có cách cục: Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phá Quân tọa thủ cung Mệnh ở Hợi </t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Hợi  có cách cục: Bạch Hổ, Thiên Hình, Hoá Kỵ, Đại Hao, Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Hợi  có cách cục: Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Hợi  gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Người tuổi Ất có Phá Quân tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Người tuổi Tân có Phá Quân tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Người tuổi Quý có Phá Quân tọa thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Người tuổi Ất có Phá Quân tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Người tuổi Tân có Phá Quân tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Người tuổi Quý có Phá Quân tọa thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Người tuổi Giáp có Phá Quân tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Người tuổi Giáp có Phá Quân tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>Người tuổi Canh có Phá Quân tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Người tuổi Canh có Phá Quân tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>Người tuổi Đinh có Phá Quân tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Người tuổi Đinh có Phá Quân tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>Người tuổi Kỷ có Phá Quân tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Người tuổi Kỷ có Phá Quân tọa thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>Người tuổi Mậu có Phá Quân tọa thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Người tuổi Mậu có Phá Quân tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh gặp Thiên Việt, Đại Hao, Tiểu Hao, Hoả Tinh, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh gặp Hoả Tinh, Linh Tinh, Thiên Việt, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Ngọ đồng cung Lộc Tồn và gặp Thiếu Dương</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Thìn gặp Hoá Lộc, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Tuất gặp Hoá Lộc, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Sửu gặp Hoá Lộc, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Mùi gặp Hoá Lộc, Thiên Hình</t>
   </si>
 </sst>
 </file>
@@ -6138,10 +6228,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B1092"/>
+  <dimension ref="A1:B1152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A997" workbookViewId="0">
-      <selection activeCell="E1013" sqref="E1013"/>
+    <sheetView tabSelected="1" topLeftCell="A1075" workbookViewId="0">
+      <selection activeCell="B1094" sqref="B1094:B1152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13817,730 +13907,1202 @@
     </row>
     <row r="1002" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1002" t="s">
-        <v>1254</v>
+        <v>1164</v>
       </c>
       <c r="B1002" t="s">
-        <v>1254</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="1003" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1003" t="s">
-        <v>1255</v>
+        <v>1165</v>
       </c>
       <c r="B1003" t="s">
-        <v>1255</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="1004" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1004" t="s">
-        <v>1256</v>
+        <v>1166</v>
       </c>
       <c r="B1004" t="s">
-        <v>1256</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="1005" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1005" t="s">
-        <v>1257</v>
+        <v>1167</v>
       </c>
       <c r="B1005" t="s">
-        <v>1257</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="1006" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1006" t="s">
-        <v>1258</v>
+        <v>1168</v>
       </c>
       <c r="B1006" t="s">
-        <v>1258</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="1007" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1007" t="s">
-        <v>1259</v>
+        <v>1169</v>
       </c>
       <c r="B1007" t="s">
-        <v>1259</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="1008" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1008" t="s">
-        <v>1260</v>
+        <v>1170</v>
       </c>
       <c r="B1008" t="s">
-        <v>1260</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="1009" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1009" t="s">
-        <v>1261</v>
+        <v>1171</v>
       </c>
       <c r="B1009" t="s">
-        <v>1261</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="1010" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1010" t="s">
-        <v>1262</v>
+        <v>1172</v>
       </c>
       <c r="B1010" t="s">
-        <v>1262</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="1011" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1011" t="s">
-        <v>1263</v>
+        <v>1173</v>
       </c>
       <c r="B1011" t="s">
-        <v>1263</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="1012" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1012" t="s">
-        <v>1264</v>
+        <v>1174</v>
       </c>
       <c r="B1012" t="s">
-        <v>1264</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="1013" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1013" t="s">
-        <v>1265</v>
+        <v>1175</v>
       </c>
       <c r="B1013" t="s">
-        <v>1265</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="1014" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1014" t="s">
-        <v>1266</v>
+        <v>1176</v>
       </c>
       <c r="B1014" t="s">
-        <v>1266</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="1015" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1015" t="s">
-        <v>1267</v>
+        <v>1177</v>
       </c>
       <c r="B1015" t="s">
-        <v>1267</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="1016" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1016" t="s">
-        <v>1268</v>
+        <v>1178</v>
       </c>
       <c r="B1016" t="s">
-        <v>1268</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="1017" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1017" t="s">
-        <v>1269</v>
+        <v>1179</v>
       </c>
       <c r="B1017" t="s">
-        <v>1269</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="1018" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1018" t="s">
-        <v>1270</v>
+        <v>1180</v>
       </c>
       <c r="B1018" t="s">
-        <v>1270</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="1019" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1019" t="s">
-        <v>1271</v>
+        <v>1181</v>
       </c>
       <c r="B1019" t="s">
-        <v>1271</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="1020" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1020" t="s">
-        <v>1272</v>
+        <v>1182</v>
       </c>
       <c r="B1020" t="s">
-        <v>1272</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="1021" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1021" t="s">
-        <v>1273</v>
+        <v>1183</v>
       </c>
       <c r="B1021" t="s">
-        <v>1273</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="1022" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1022" t="s">
-        <v>1274</v>
+        <v>1184</v>
       </c>
       <c r="B1022" t="s">
-        <v>1274</v>
+        <v>1184</v>
       </c>
     </row>
     <row r="1023" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1023" t="s">
-        <v>1275</v>
+        <v>1185</v>
       </c>
       <c r="B1023" t="s">
-        <v>1275</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="1024" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1024" t="s">
-        <v>1276</v>
+        <v>1186</v>
       </c>
       <c r="B1024" t="s">
-        <v>1276</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="1025" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1025" t="s">
-        <v>1277</v>
+        <v>1187</v>
       </c>
       <c r="B1025" t="s">
-        <v>1277</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="1026" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1026" t="s">
-        <v>1278</v>
+        <v>1188</v>
       </c>
       <c r="B1026" t="s">
-        <v>1278</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="1027" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1027" t="s">
-        <v>1279</v>
+        <v>1189</v>
       </c>
       <c r="B1027" t="s">
-        <v>1279</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="1028" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1028" t="s">
-        <v>1280</v>
+        <v>1190</v>
       </c>
       <c r="B1028" t="s">
-        <v>1280</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="1029" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1029" t="s">
-        <v>1281</v>
+        <v>1191</v>
       </c>
       <c r="B1029" t="s">
-        <v>1281</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="1030" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1030" t="s">
-        <v>1282</v>
+        <v>1192</v>
       </c>
       <c r="B1030" t="s">
-        <v>1282</v>
+        <v>1192</v>
       </c>
     </row>
     <row r="1031" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1031" t="s">
-        <v>1283</v>
+        <v>1193</v>
       </c>
       <c r="B1031" t="s">
-        <v>1283</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="1032" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1032" t="s">
-        <v>1284</v>
+        <v>1194</v>
       </c>
       <c r="B1032" t="s">
-        <v>1284</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="1033" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1033" t="s">
-        <v>1285</v>
+        <v>1195</v>
       </c>
       <c r="B1033" t="s">
-        <v>1285</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="1034" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1034" t="s">
-        <v>1286</v>
+        <v>1196</v>
       </c>
       <c r="B1034" t="s">
-        <v>1286</v>
+        <v>1196</v>
       </c>
     </row>
     <row r="1035" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1035" t="s">
-        <v>1287</v>
+        <v>1197</v>
       </c>
       <c r="B1035" t="s">
-        <v>1287</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="1036" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1036" t="s">
-        <v>1288</v>
+        <v>1198</v>
       </c>
       <c r="B1036" t="s">
-        <v>1288</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="1037" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1037" t="s">
-        <v>1289</v>
+        <v>1199</v>
       </c>
       <c r="B1037" t="s">
-        <v>1289</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="1038" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1038" t="s">
-        <v>1290</v>
+        <v>1200</v>
       </c>
       <c r="B1038" t="s">
-        <v>1290</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="1039" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1039" t="s">
-        <v>1291</v>
+        <v>1201</v>
       </c>
       <c r="B1039" t="s">
-        <v>1291</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="1040" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1040" t="s">
-        <v>1292</v>
+        <v>1202</v>
       </c>
       <c r="B1040" t="s">
-        <v>1292</v>
+        <v>1202</v>
       </c>
     </row>
     <row r="1041" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1041" t="s">
-        <v>1293</v>
+        <v>1203</v>
       </c>
       <c r="B1041" t="s">
-        <v>1293</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="1042" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1042" t="s">
-        <v>1294</v>
+        <v>1204</v>
       </c>
       <c r="B1042" t="s">
-        <v>1294</v>
+        <v>1204</v>
       </c>
     </row>
     <row r="1043" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1043" t="s">
-        <v>1295</v>
+        <v>1205</v>
       </c>
       <c r="B1043" t="s">
-        <v>1295</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="1044" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1044" t="s">
-        <v>1296</v>
+        <v>1206</v>
       </c>
       <c r="B1044" t="s">
-        <v>1296</v>
+        <v>1206</v>
       </c>
     </row>
     <row r="1045" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1045" t="s">
-        <v>1297</v>
+        <v>1207</v>
       </c>
       <c r="B1045" t="s">
-        <v>1297</v>
+        <v>1207</v>
       </c>
     </row>
     <row r="1046" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1046" t="s">
-        <v>1298</v>
+        <v>1208</v>
       </c>
       <c r="B1046" t="s">
-        <v>1298</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="1047" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1047" t="s">
-        <v>1299</v>
+        <v>1209</v>
       </c>
       <c r="B1047" t="s">
-        <v>1299</v>
+        <v>1209</v>
       </c>
     </row>
     <row r="1048" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1048" t="s">
-        <v>1300</v>
+        <v>1210</v>
       </c>
       <c r="B1048" t="s">
-        <v>1300</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="1049" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1049" t="s">
-        <v>1301</v>
+        <v>1211</v>
       </c>
       <c r="B1049" t="s">
-        <v>1301</v>
+        <v>1211</v>
       </c>
     </row>
     <row r="1050" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1050" t="s">
-        <v>1302</v>
+        <v>1212</v>
       </c>
       <c r="B1050" t="s">
-        <v>1302</v>
+        <v>1212</v>
       </c>
     </row>
     <row r="1051" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1051" t="s">
-        <v>1303</v>
+        <v>1213</v>
       </c>
       <c r="B1051" t="s">
-        <v>1303</v>
+        <v>1213</v>
       </c>
     </row>
     <row r="1052" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1052" t="s">
-        <v>1304</v>
+        <v>1214</v>
       </c>
       <c r="B1052" t="s">
-        <v>1304</v>
+        <v>1214</v>
       </c>
     </row>
     <row r="1053" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1053" t="s">
-        <v>1305</v>
+        <v>1215</v>
       </c>
       <c r="B1053" t="s">
-        <v>1305</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="1054" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1054" t="s">
-        <v>1306</v>
+        <v>1216</v>
       </c>
       <c r="B1054" t="s">
-        <v>1306</v>
+        <v>1216</v>
       </c>
     </row>
     <row r="1055" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1055" t="s">
-        <v>1307</v>
+        <v>1217</v>
       </c>
       <c r="B1055" t="s">
-        <v>1307</v>
+        <v>1217</v>
       </c>
     </row>
     <row r="1056" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1056" t="s">
-        <v>1308</v>
+        <v>1218</v>
       </c>
       <c r="B1056" t="s">
-        <v>1308</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="1057" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1057" t="s">
-        <v>1309</v>
+        <v>1219</v>
       </c>
       <c r="B1057" t="s">
-        <v>1309</v>
+        <v>1219</v>
       </c>
     </row>
     <row r="1058" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1058" t="s">
-        <v>1310</v>
+        <v>1220</v>
       </c>
       <c r="B1058" t="s">
-        <v>1310</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="1059" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1059" t="s">
-        <v>1311</v>
+        <v>1221</v>
       </c>
       <c r="B1059" t="s">
-        <v>1311</v>
+        <v>1221</v>
       </c>
     </row>
     <row r="1060" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1060" t="s">
-        <v>1312</v>
+        <v>1222</v>
       </c>
       <c r="B1060" t="s">
-        <v>1312</v>
+        <v>1222</v>
       </c>
     </row>
     <row r="1061" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1061" t="s">
-        <v>1313</v>
+        <v>1223</v>
       </c>
       <c r="B1061" t="s">
-        <v>1313</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="1062" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1062" t="s">
-        <v>1314</v>
+        <v>1224</v>
       </c>
       <c r="B1062" t="s">
-        <v>1314</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="1063" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1063" t="s">
-        <v>1315</v>
+        <v>1225</v>
       </c>
       <c r="B1063" t="s">
-        <v>1315</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="1064" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1064" t="s">
-        <v>1316</v>
+        <v>1226</v>
       </c>
       <c r="B1064" t="s">
-        <v>1316</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="1065" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1065" t="s">
-        <v>1317</v>
+        <v>1227</v>
       </c>
       <c r="B1065" t="s">
-        <v>1317</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="1066" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1066" t="s">
-        <v>1318</v>
+        <v>1228</v>
       </c>
       <c r="B1066" t="s">
-        <v>1318</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="1067" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1067" t="s">
-        <v>1319</v>
+        <v>1229</v>
       </c>
       <c r="B1067" t="s">
-        <v>1319</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="1068" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1068" t="s">
-        <v>1320</v>
+        <v>1230</v>
       </c>
       <c r="B1068" t="s">
-        <v>1320</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="1069" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1069" t="s">
-        <v>1321</v>
+        <v>1231</v>
       </c>
       <c r="B1069" t="s">
-        <v>1321</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="1070" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1070" t="s">
-        <v>1322</v>
+        <v>1232</v>
       </c>
       <c r="B1070" t="s">
-        <v>1322</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="1071" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1071" t="s">
-        <v>1323</v>
+        <v>1233</v>
       </c>
       <c r="B1071" t="s">
-        <v>1323</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="1072" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1072" t="s">
-        <v>1324</v>
+        <v>1234</v>
       </c>
       <c r="B1072" t="s">
-        <v>1324</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="1073" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1073" t="s">
-        <v>1325</v>
+        <v>1235</v>
       </c>
       <c r="B1073" t="s">
-        <v>1325</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="1074" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1074" t="s">
-        <v>1326</v>
+        <v>1236</v>
       </c>
       <c r="B1074" t="s">
-        <v>1326</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="1075" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1075" t="s">
-        <v>1327</v>
+        <v>1237</v>
       </c>
       <c r="B1075" t="s">
-        <v>1327</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="1076" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1076" t="s">
-        <v>1328</v>
+        <v>1238</v>
       </c>
       <c r="B1076" t="s">
-        <v>1328</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="1077" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1077" t="s">
-        <v>1329</v>
+        <v>1239</v>
       </c>
       <c r="B1077" t="s">
-        <v>1329</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="1078" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1078" t="s">
-        <v>1330</v>
+        <v>1240</v>
       </c>
       <c r="B1078" t="s">
-        <v>1330</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="1079" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1079" t="s">
-        <v>1331</v>
+        <v>1241</v>
       </c>
       <c r="B1079" t="s">
-        <v>1331</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="1080" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1080" t="s">
-        <v>1332</v>
+        <v>1242</v>
       </c>
       <c r="B1080" t="s">
-        <v>1332</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="1081" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1081" t="s">
-        <v>1333</v>
+        <v>1243</v>
       </c>
       <c r="B1081" t="s">
-        <v>1333</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="1082" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1082" t="s">
-        <v>1334</v>
+        <v>1244</v>
       </c>
       <c r="B1082" t="s">
-        <v>1334</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="1083" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1083" t="s">
-        <v>1335</v>
+        <v>1245</v>
       </c>
       <c r="B1083" t="s">
-        <v>1335</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="1084" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1084" t="s">
-        <v>1336</v>
+        <v>1246</v>
       </c>
       <c r="B1084" t="s">
-        <v>1336</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="1085" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1085" t="s">
-        <v>1337</v>
+        <v>1247</v>
       </c>
       <c r="B1085" t="s">
-        <v>1337</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="1086" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1086" t="s">
-        <v>1338</v>
+        <v>1248</v>
       </c>
       <c r="B1086" t="s">
-        <v>1338</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="1087" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1087" t="s">
-        <v>1339</v>
+        <v>1249</v>
       </c>
       <c r="B1087" t="s">
-        <v>1339</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="1088" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1088" t="s">
-        <v>1340</v>
+        <v>1250</v>
       </c>
       <c r="B1088" t="s">
-        <v>1340</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="1089" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1089" t="s">
-        <v>1341</v>
+        <v>1251</v>
       </c>
       <c r="B1089" t="s">
-        <v>1341</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="1090" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1090" t="s">
-        <v>1342</v>
+        <v>1252</v>
       </c>
       <c r="B1090" t="s">
-        <v>1342</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="1091" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1091" t="s">
-        <v>1343</v>
+        <v>1253</v>
       </c>
       <c r="B1091" t="s">
-        <v>1343</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="1092" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1092" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B1092" t="s">
+        <v>1252</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1094" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B1094" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1095" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B1095" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1096" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B1096" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1097" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B1097" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1098" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B1098" t="s">
+        <v>1316</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1099" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B1099" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1100" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B1100" t="s">
+        <v>1318</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1101" t="s">
+        <v>1319</v>
+      </c>
+      <c r="B1101" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1102" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B1102" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1103" t="s">
+        <v>1321</v>
+      </c>
+      <c r="B1103" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1104" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B1104" t="s">
+        <v>1322</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1105" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B1105" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1106" t="s">
+        <v>1324</v>
+      </c>
+      <c r="B1106" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1107" t="s">
+        <v>1325</v>
+      </c>
+      <c r="B1107" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1108" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B1108" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1109" t="s">
+        <v>1327</v>
+      </c>
+      <c r="B1109" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1110" t="s">
+        <v>1328</v>
+      </c>
+      <c r="B1110" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1111" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B1111" t="s">
+        <v>1329</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1112" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B1112" t="s">
+        <v>1330</v>
+      </c>
+    </row>
+    <row r="1113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1113" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B1113" t="s">
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1114" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B1114" t="s">
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1115" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B1115" t="s">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1116" t="s">
+        <v>1334</v>
+      </c>
+      <c r="B1116" t="s">
+        <v>1334</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1117" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B1117" t="s">
+        <v>1335</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1118" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B1118" t="s">
+        <v>1336</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1119" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B1119" t="s">
+        <v>1337</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1120" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B1120" t="s">
+        <v>1338</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1121" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B1121" t="s">
+        <v>1339</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1122" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B1122" t="s">
+        <v>1340</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1123" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B1123" t="s">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1124" t="s">
         <v>1342</v>
       </c>
-      <c r="B1092" t="s">
+      <c r="B1124" t="s">
         <v>1342</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1125" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B1125" t="s">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1126" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B1126" t="s">
+        <v>1344</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1127" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B1127" t="s">
+        <v>1345</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1128" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B1128" t="s">
+        <v>1346</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1129" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B1129" t="s">
+        <v>1347</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1130" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B1130" t="s">
+        <v>1348</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1131" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B1131" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1132" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B1132" t="s">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="1133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1133" t="s">
+        <v>1351</v>
+      </c>
+      <c r="B1133" t="s">
+        <v>1351</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1134" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B1134" t="s">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1135" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B1135" t="s">
+        <v>1353</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1136" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B1136" t="s">
+        <v>1354</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1137" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B1137" t="s">
+        <v>1355</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1138" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B1138" t="s">
+        <v>1356</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1139" t="s">
+        <v>1357</v>
+      </c>
+      <c r="B1139" t="s">
+        <v>1357</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1140" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B1140" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1141" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B1141" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1142" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B1142" t="s">
+        <v>1360</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1143" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B1143" t="s">
+        <v>1361</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1144" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B1144" t="s">
+        <v>1362</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1145" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B1145" t="s">
+        <v>1363</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1146" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B1146" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1147" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B1147" t="s">
+        <v>1365</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1148" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B1148" t="s">
+        <v>1366</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1149" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B1149" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1150" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B1150" t="s">
+        <v>1368</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1151" t="s">
+        <v>1369</v>
+      </c>
+      <c r="B1151" t="s">
+        <v>1369</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1152" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B1152" t="s">
+        <v>1370</v>
       </c>
     </row>
   </sheetData>
@@ -14609,748 +15171,484 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBE4172-FC39-45CE-BD67-BA23D6FB1A86}">
-  <dimension ref="A1:B92"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B92"/>
+      <selection activeCell="B1" sqref="B1:B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1163</v>
+        <v>1254</v>
       </c>
       <c r="B1" t="s">
-        <v>1163</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1164</v>
+        <v>1255</v>
       </c>
       <c r="B2" t="s">
-        <v>1254</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1165</v>
+        <v>1256</v>
       </c>
       <c r="B3" t="s">
-        <v>1255</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1166</v>
+        <v>1257</v>
       </c>
       <c r="B4" t="s">
-        <v>1256</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1167</v>
+        <v>1258</v>
       </c>
       <c r="B5" t="s">
-        <v>1257</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1168</v>
+        <v>1259</v>
       </c>
       <c r="B6" t="s">
-        <v>1258</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1169</v>
+        <v>1260</v>
       </c>
       <c r="B7" t="s">
-        <v>1259</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1170</v>
+        <v>1261</v>
       </c>
       <c r="B8" t="s">
-        <v>1260</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1171</v>
+        <v>1262</v>
       </c>
       <c r="B9" t="s">
-        <v>1261</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1172</v>
+        <v>1263</v>
       </c>
       <c r="B10" t="s">
-        <v>1262</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1173</v>
+        <v>1264</v>
       </c>
       <c r="B11" t="s">
-        <v>1263</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1174</v>
+        <v>1265</v>
       </c>
       <c r="B12" t="s">
-        <v>1264</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1175</v>
+        <v>1266</v>
       </c>
       <c r="B13" t="s">
-        <v>1265</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1176</v>
+        <v>1267</v>
       </c>
       <c r="B14" t="s">
-        <v>1266</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1177</v>
+        <v>1268</v>
       </c>
       <c r="B15" t="s">
-        <v>1267</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1178</v>
+        <v>1269</v>
       </c>
       <c r="B16" t="s">
-        <v>1268</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1179</v>
+        <v>1270</v>
       </c>
       <c r="B17" t="s">
-        <v>1269</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1180</v>
+        <v>1271</v>
       </c>
       <c r="B18" t="s">
-        <v>1270</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1181</v>
+        <v>1272</v>
       </c>
       <c r="B19" t="s">
-        <v>1271</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1182</v>
+        <v>1273</v>
       </c>
       <c r="B20" t="s">
-        <v>1272</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1183</v>
+        <v>1274</v>
       </c>
       <c r="B21" t="s">
-        <v>1273</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1184</v>
+        <v>1275</v>
       </c>
       <c r="B22" t="s">
-        <v>1274</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1185</v>
+        <v>1276</v>
       </c>
       <c r="B23" t="s">
-        <v>1275</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1186</v>
+        <v>1277</v>
       </c>
       <c r="B24" t="s">
-        <v>1276</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1187</v>
+        <v>1278</v>
       </c>
       <c r="B25" t="s">
-        <v>1277</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1188</v>
+        <v>1279</v>
       </c>
       <c r="B26" t="s">
-        <v>1278</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1189</v>
+        <v>1280</v>
       </c>
       <c r="B27" t="s">
-        <v>1279</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1190</v>
+        <v>1281</v>
       </c>
       <c r="B28" t="s">
-        <v>1280</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1191</v>
+        <v>1282</v>
       </c>
       <c r="B29" t="s">
-        <v>1281</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1192</v>
+        <v>1283</v>
       </c>
       <c r="B30" t="s">
-        <v>1282</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1193</v>
+        <v>1284</v>
       </c>
       <c r="B31" t="s">
-        <v>1283</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1194</v>
+        <v>1285</v>
       </c>
       <c r="B32" t="s">
-        <v>1284</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1195</v>
+        <v>1286</v>
       </c>
       <c r="B33" t="s">
-        <v>1285</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1196</v>
+        <v>1287</v>
       </c>
       <c r="B34" t="s">
-        <v>1286</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1197</v>
+        <v>1288</v>
       </c>
       <c r="B35" t="s">
-        <v>1287</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1198</v>
+        <v>1289</v>
       </c>
       <c r="B36" t="s">
-        <v>1288</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1199</v>
+        <v>1290</v>
       </c>
       <c r="B37" t="s">
-        <v>1289</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1200</v>
+        <v>1291</v>
       </c>
       <c r="B38" t="s">
-        <v>1290</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1201</v>
+        <v>1292</v>
       </c>
       <c r="B39" t="s">
-        <v>1291</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1202</v>
+        <v>1293</v>
       </c>
       <c r="B40" t="s">
-        <v>1292</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1203</v>
+        <v>1294</v>
       </c>
       <c r="B41" t="s">
-        <v>1293</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1204</v>
+        <v>1295</v>
       </c>
       <c r="B42" t="s">
-        <v>1294</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1205</v>
+        <v>1296</v>
       </c>
       <c r="B43" t="s">
-        <v>1295</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1206</v>
+        <v>1297</v>
       </c>
       <c r="B44" t="s">
-        <v>1296</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1207</v>
+        <v>1298</v>
       </c>
       <c r="B45" t="s">
-        <v>1297</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1208</v>
+        <v>1299</v>
       </c>
       <c r="B46" t="s">
-        <v>1298</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1209</v>
+        <v>1300</v>
       </c>
       <c r="B47" t="s">
-        <v>1299</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1210</v>
+        <v>1301</v>
       </c>
       <c r="B48" t="s">
-        <v>1300</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1211</v>
+        <v>1302</v>
       </c>
       <c r="B49" t="s">
-        <v>1301</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1212</v>
+        <v>1303</v>
       </c>
       <c r="B50" t="s">
-        <v>1302</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1213</v>
+        <v>1304</v>
       </c>
       <c r="B51" t="s">
-        <v>1303</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1214</v>
+        <v>1305</v>
       </c>
       <c r="B52" t="s">
-        <v>1304</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1215</v>
+        <v>1306</v>
       </c>
       <c r="B53" t="s">
-        <v>1305</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1216</v>
+        <v>1307</v>
       </c>
       <c r="B54" t="s">
-        <v>1306</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1217</v>
+        <v>1308</v>
       </c>
       <c r="B55" t="s">
-        <v>1307</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1218</v>
+        <v>1309</v>
       </c>
       <c r="B56" t="s">
-        <v>1308</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1219</v>
+        <v>1310</v>
       </c>
       <c r="B57" t="s">
-        <v>1309</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1220</v>
+        <v>1311</v>
       </c>
       <c r="B58" t="s">
-        <v>1310</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1221</v>
+        <v>1312</v>
       </c>
       <c r="B59" t="s">
-        <v>1311</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>1222</v>
-      </c>
-      <c r="B60" t="s">
-        <v>1312</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>1223</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1313</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>1224</v>
-      </c>
-      <c r="B62" t="s">
-        <v>1314</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>1225</v>
-      </c>
-      <c r="B63" t="s">
-        <v>1315</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>1226</v>
-      </c>
-      <c r="B64" t="s">
-        <v>1316</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>1227</v>
-      </c>
-      <c r="B65" t="s">
-        <v>1317</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>1228</v>
-      </c>
-      <c r="B66" t="s">
-        <v>1318</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>1229</v>
-      </c>
-      <c r="B67" t="s">
-        <v>1319</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>1230</v>
-      </c>
-      <c r="B68" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>1231</v>
-      </c>
-      <c r="B69" t="s">
-        <v>1321</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>1232</v>
-      </c>
-      <c r="B70" t="s">
-        <v>1322</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>1233</v>
-      </c>
-      <c r="B71" t="s">
-        <v>1323</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>1234</v>
-      </c>
-      <c r="B72" t="s">
-        <v>1324</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>1235</v>
-      </c>
-      <c r="B73" t="s">
-        <v>1325</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>1236</v>
-      </c>
-      <c r="B74" t="s">
-        <v>1326</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>1237</v>
-      </c>
-      <c r="B75" t="s">
-        <v>1327</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>1238</v>
-      </c>
-      <c r="B76" t="s">
-        <v>1328</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>1239</v>
-      </c>
-      <c r="B77" t="s">
-        <v>1329</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>1240</v>
-      </c>
-      <c r="B78" t="s">
-        <v>1330</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>1241</v>
-      </c>
-      <c r="B79" t="s">
-        <v>1331</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>1242</v>
-      </c>
-      <c r="B80" t="s">
-        <v>1332</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>1243</v>
-      </c>
-      <c r="B81" t="s">
-        <v>1333</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>1244</v>
-      </c>
-      <c r="B82" t="s">
-        <v>1334</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>1245</v>
-      </c>
-      <c r="B83" t="s">
-        <v>1335</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>1246</v>
-      </c>
-      <c r="B84" t="s">
-        <v>1336</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>1247</v>
-      </c>
-      <c r="B85" t="s">
-        <v>1337</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>1248</v>
-      </c>
-      <c r="B86" t="s">
-        <v>1338</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>1249</v>
-      </c>
-      <c r="B87" t="s">
-        <v>1339</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>1250</v>
-      </c>
-      <c r="B88" t="s">
-        <v>1340</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>1251</v>
-      </c>
-      <c r="B89" t="s">
-        <v>1341</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>1252</v>
-      </c>
-      <c r="B90" t="s">
-        <v>1342</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>1253</v>
-      </c>
-      <c r="B91" t="s">
-        <v>1343</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>1252</v>
-      </c>
-      <c r="B92" t="s">
-        <v>1342</v>
+        <v>1370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Luận an Khôi Việt
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B87BBD3-12A1-4F7F-A9BC-FF142C459997}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FC1086-59CF-46E0-9FDB-A0F3CA49BF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2924" uniqueCount="1495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2813" uniqueCount="1434">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -3980,261 +3980,6 @@
     <t>Văn Xương toạ thủ cung Mệnh</t>
   </si>
   <si>
-    <t>luanmenh.js:3353 Văn Khúc toạ thủ cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3360 Văn Xương toạ thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3363 Văn Xương toạ thủ cung Mệnh ở Thìn gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3366 Văn Xương toạ thủ cung Mệnh ở Thìn gặp Thiên Lương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3369 Văn Xương toạ thủ cung Mệnh ở Thìn gặp Thiên Cơ, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3372 Văn Xương toạ thủ cung Mệnh ở Thìn đồng cung Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3375 Văn Xương toạ thủ cung Mệnh ở Thìn đồng cung Vũ Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3378 Văn Xương toạ thủ cung Mệnh ở Thìn đồng cung Tả Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3360 Văn Khúc toạ thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3363 Văn Khúc toạ thủ cung Mệnh ở Thìn gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3366 Văn Khúc toạ thủ cung Mệnh ở Thìn gặp Thiên Lương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3369 Văn Khúc toạ thủ cung Mệnh ở Thìn gặp Thiên Cơ, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3372 Văn Khúc toạ thủ cung Mệnh ở Thìn đồng cung Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3375 Văn Khúc toạ thủ cung Mệnh ở Thìn đồng cung Vũ Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3378 Văn Khúc toạ thủ cung Mệnh ở Thìn đồng cung Tả Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3360 Văn Xương toạ thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3363 Văn Xương toạ thủ cung Mệnh ở Tuất gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3366 Văn Xương toạ thủ cung Mệnh ở Tuất gặp Thiên Lương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3369 Văn Xương toạ thủ cung Mệnh ở Tuất gặp Thiên Cơ, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3372 Văn Xương toạ thủ cung Mệnh ở Tuất đồng cung Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3375 Văn Xương toạ thủ cung Mệnh ở Tuất đồng cung Vũ Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3378 Văn Xương toạ thủ cung Mệnh ở Tuất đồng cung Tả Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3360 Văn Khúc toạ thủ cung Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3363 Văn Khúc toạ thủ cung Mệnh ở Tuất gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3366 Văn Khúc toạ thủ cung Mệnh ở Tuất gặp Thiên Lương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3369 Văn Khúc toạ thủ cung Mệnh ở Tuất gặp Thiên Cơ, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3372 Văn Khúc toạ thủ cung Mệnh ở Tuất đồng cung Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3375 Văn Khúc toạ thủ cung Mệnh ở Tuất đồng cung Vũ Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3378 Văn Khúc toạ thủ cung Mệnh ở Tuất đồng cung Tả Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3360 Văn Xương toạ thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3363 Văn Xương toạ thủ cung Mệnh ở Sửu gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3366 Văn Xương toạ thủ cung Mệnh ở Sửu gặp Thiên Lương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3369 Văn Xương toạ thủ cung Mệnh ở Sửu gặp Thiên Cơ, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3372 Văn Xương toạ thủ cung Mệnh ở Sửu đồng cung Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3375 Văn Xương toạ thủ cung Mệnh ở Sửu đồng cung Vũ Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3378 Văn Xương toạ thủ cung Mệnh ở Sửu đồng cung Tả Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3360 Văn Khúc toạ thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3363 Văn Khúc toạ thủ cung Mệnh ở Sửu gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3366 Văn Khúc toạ thủ cung Mệnh ở Sửu gặp Thiên Lương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3369 Văn Khúc toạ thủ cung Mệnh ở Sửu gặp Thiên Cơ, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3372 Văn Khúc toạ thủ cung Mệnh ở Sửu đồng cung Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3375 Văn Khúc toạ thủ cung Mệnh ở Sửu đồng cung Vũ Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3378 Văn Khúc toạ thủ cung Mệnh ở Sửu đồng cung Tả Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3360 Văn Xương toạ thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3363 Văn Xương toạ thủ cung Mệnh ở Mùi gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3366 Văn Xương toạ thủ cung Mệnh ở Mùi gặp Thiên Lương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3369 Văn Xương toạ thủ cung Mệnh ở Mùi gặp Thiên Cơ, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3372 Văn Xương toạ thủ cung Mệnh ở Mùi đồng cung Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3375 Văn Xương toạ thủ cung Mệnh ở Mùi đồng cung Vũ Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3378 Văn Xương toạ thủ cung Mệnh ở Mùi đồng cung Tả Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3360 Văn Khúc toạ thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3363 Văn Khúc toạ thủ cung Mệnh ở Mùi gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3366 Văn Khúc toạ thủ cung Mệnh ở Mùi gặp Thiên Lương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3369 Văn Khúc toạ thủ cung Mệnh ở Mùi gặp Thiên Cơ, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3372 Văn Khúc toạ thủ cung Mệnh ở Mùi đồng cung Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3375 Văn Khúc toạ thủ cung Mệnh ở Mùi đồng cung Vũ Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3378 Văn Khúc toạ thủ cung Mệnh ở Mùi đồng cung Tả Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3360 Văn Xương toạ thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3363 Văn Xương toạ thủ cung Mệnh ở Tỵ gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3366 Văn Xương toạ thủ cung Mệnh ở Tỵ gặp Thiên Lương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3369 Văn Xương toạ thủ cung Mệnh ở Tỵ gặp Thiên Cơ, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3372 Văn Xương toạ thủ cung Mệnh ở Tỵ đồng cung Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3375 Văn Xương toạ thủ cung Mệnh ở Tỵ đồng cung Vũ Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3378 Văn Xương toạ thủ cung Mệnh ở Tỵ đồng cung Tả Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3360 Văn Khúc toạ thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3363 Văn Khúc toạ thủ cung Mệnh ở Tỵ gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3366 Văn Khúc toạ thủ cung Mệnh ở Tỵ gặp Thiên Lương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3369 Văn Khúc toạ thủ cung Mệnh ở Tỵ gặp Thiên Cơ, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3372 Văn Khúc toạ thủ cung Mệnh ở Tỵ đồng cung Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3375 Văn Khúc toạ thủ cung Mệnh ở Tỵ đồng cung Vũ Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3378 Văn Khúc toạ thủ cung Mệnh ở Tỵ đồng cung Tả Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3360 Văn Xương toạ thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3363 Văn Xương toạ thủ cung Mệnh ở Hợi gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3366 Văn Xương toạ thủ cung Mệnh ở Hợi gặp Thiên Lương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3369 Văn Xương toạ thủ cung Mệnh ở Hợi gặp Thiên Cơ, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3372 Văn Xương toạ thủ cung Mệnh ở Hợi đồng cung Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3375 Văn Xương toạ thủ cung Mệnh ở Hợi đồng cung Vũ Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3378 Văn Xương toạ thủ cung Mệnh ở Hợi đồng cung Tả Phù</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3360 Văn Khúc toạ thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3363 Văn Khúc toạ thủ cung Mệnh ở Hợi gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Thiên Khôi, Thiên Việt, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3366 Văn Khúc toạ thủ cung Mệnh ở Hợi gặp Thiên Lương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3369 Văn Khúc toạ thủ cung Mệnh ở Hợi gặp Thiên Cơ, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3372 Văn Khúc toạ thủ cung Mệnh ở Hợi đồng cung Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3375 Văn Khúc toạ thủ cung Mệnh ở Hợi đồng cung Vũ Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3378 Văn Khúc toạ thủ cung Mệnh ở Hợi đồng cung Tả Phù</t>
-  </si>
-  <si>
     <t>Văn Khúc toạ thủ cung Mệnh</t>
   </si>
   <si>
@@ -4490,37 +4235,109 @@
     <t>Văn Khúc toạ thủ cung Mệnh ở Hợi đồng cung Tả Phù</t>
   </si>
   <si>
-    <t>luanmenh.js:3390 Mệnh có Thái Dương giáp Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3395 Mệnh có Văn Xương hội chiếu Văn Khúc, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3399 Mệnh có Văn Khúc hội chiếu Văn Xương, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3406 Văn Xương toạ thủ cung Mệnh ở Tỵ đồng cung Liêm Trinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3406 Văn Khúc toạ thủ cung Mệnh ở Tỵ đồng cung Liêm Trinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3406 Văn Xương toạ thủ cung Mệnh ở Hợi đồng cung Liêm Trinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3406 Văn Khúc toạ thủ cung Mệnh ở Hợi đồng cung Liêm Trinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3417 Văn Xương toạ thủ cung Mệnh ở Dần đồng cung Phá Quân gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3417 Văn Khúc toạ thủ cung Mệnh ở Dần đồng cung Phá Quân gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3417 Văn Xương toạ thủ cung Mệnh ở Mão đồng cung Phá Quân gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3417 Văn Khúc toạ thủ cung Mệnh ở Mão đồng cung Phá Quân gặp Kình Dương</t>
+    <t>Thiên Khôi toạ thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3499 Thiên Khôi toạ thủ cung Mệnh gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3502 Thiên Khôi toạ thủ cung Mệnh gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3505 Thiên Khôi toạ thủ cung Mệnh gặp Hóa Kỵ, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3508 Thiên Khôi toạ thủ cung Mệnh gặp các sao Văn Xương, Văn Khúc, Tấu Thư, Thái Tuế</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3512 Thiên Khôi toạ thủ cung Mệnh gặp Thiên Lương, Thiên Cơ, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3515 Thiên Khôi toạ thủ cung Mệnh gặp Hóa Lộc mà không gặp các sao Sát tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3518 Thiên Khôi toạ thủ cung Mệnh ở Ngọ đồng cung Tử Vi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3496 Thiên Việt toạ thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3499 Thiên Việt toạ thủ cung Mệnh gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3502 Thiên Việt toạ thủ cung Mệnh gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3505 Thiên Việt toạ thủ cung Mệnh gặp Hóa Kỵ, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3508 Thiên Việt toạ thủ cung Mệnh gặp các sao Văn Xương, Văn Khúc, Tấu Thư, Thái Tuế</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3512 Thiên Việt toạ thủ cung Mệnh gặp Thiên Lương, Thiên Cơ, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3515 Thiên Việt toạ thủ cung Mệnh gặp Hóa Lộc mà không gặp các sao Sát tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3518 Thiên Việt toạ thủ cung Mệnh ở Ngọ đồng cung Tử Vi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3528 Mệnh có Thái Dương giáp Khôi Việt</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3531 Mệnh có Hóa Lộc giáp Khôi Việt</t>
+  </si>
+  <si>
+    <t>Thiên Khôi toạ thủ cung Mệnh gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>Thiên Khôi toạ thủ cung Mệnh gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Khôi toạ thủ cung Mệnh gặp Hóa Kỵ, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Thiên Khôi toạ thủ cung Mệnh gặp các sao Văn Xương, Văn Khúc, Tấu Thư, Thái Tuế</t>
+  </si>
+  <si>
+    <t>Thiên Khôi toạ thủ cung Mệnh gặp Thiên Lương, Thiên Cơ, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>Thiên Khôi toạ thủ cung Mệnh gặp Hóa Lộc mà không gặp các sao Sát tinh</t>
+  </si>
+  <si>
+    <t>Thiên Khôi toạ thủ cung Mệnh ở Ngọ đồng cung Tử Vi</t>
+  </si>
+  <si>
+    <t>Thiên Việt toạ thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>Thiên Việt toạ thủ cung Mệnh gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>Thiên Việt toạ thủ cung Mệnh gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Việt toạ thủ cung Mệnh gặp Hóa Kỵ, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Thiên Việt toạ thủ cung Mệnh gặp các sao Văn Xương, Văn Khúc, Tấu Thư, Thái Tuế</t>
+  </si>
+  <si>
+    <t>Thiên Việt toạ thủ cung Mệnh gặp Thiên Lương, Thiên Cơ, Hoá Lộc</t>
+  </si>
+  <si>
+    <t>Thiên Việt toạ thủ cung Mệnh gặp Hóa Lộc mà không gặp các sao Sát tinh</t>
+  </si>
+  <si>
+    <t>Thiên Việt toạ thủ cung Mệnh ở Ngọ đồng cung Tử Vi</t>
+  </si>
+  <si>
+    <t>Mệnh có Thái Dương giáp Khôi Việt</t>
+  </si>
+  <si>
+    <t>Mệnh có Hóa Lộc giáp Khôi Việt</t>
   </si>
 </sst>
 </file>
@@ -6600,10 +6417,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B1239"/>
+  <dimension ref="A1:B1258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1214" workbookViewId="0">
-      <selection activeCell="B1154" sqref="B1154:B1239"/>
+    <sheetView tabSelected="1" topLeftCell="A1238" workbookViewId="0">
+      <selection activeCell="G1259" sqref="G1259"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15487,682 +15304,826 @@
     </row>
     <row r="1155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1155" t="s">
-        <v>1399</v>
+        <v>1314</v>
       </c>
       <c r="B1155" t="s">
-        <v>1399</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="1156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1156" t="s">
-        <v>1400</v>
+        <v>1315</v>
       </c>
       <c r="B1156" t="s">
-        <v>1400</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="1157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1157" t="s">
-        <v>1401</v>
+        <v>1316</v>
       </c>
       <c r="B1157" t="s">
-        <v>1401</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="1158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1158" t="s">
-        <v>1402</v>
+        <v>1317</v>
       </c>
       <c r="B1158" t="s">
-        <v>1402</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="1159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1159" t="s">
-        <v>1403</v>
+        <v>1318</v>
       </c>
       <c r="B1159" t="s">
-        <v>1403</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="1160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1160" t="s">
-        <v>1404</v>
+        <v>1319</v>
       </c>
       <c r="B1160" t="s">
-        <v>1404</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="1161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1161" t="s">
-        <v>1405</v>
+        <v>1320</v>
       </c>
       <c r="B1161" t="s">
-        <v>1405</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="1162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1162" t="s">
-        <v>1406</v>
+        <v>1321</v>
       </c>
       <c r="B1162" t="s">
-        <v>1406</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="1163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1163" t="s">
-        <v>1407</v>
+        <v>1322</v>
       </c>
       <c r="B1163" t="s">
-        <v>1407</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="1164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1164" t="s">
-        <v>1408</v>
+        <v>1323</v>
       </c>
       <c r="B1164" t="s">
-        <v>1408</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="1165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1165" t="s">
-        <v>1409</v>
+        <v>1324</v>
       </c>
       <c r="B1165" t="s">
-        <v>1409</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="1166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1166" t="s">
-        <v>1410</v>
+        <v>1325</v>
       </c>
       <c r="B1166" t="s">
-        <v>1410</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="1167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1167" t="s">
-        <v>1411</v>
+        <v>1326</v>
       </c>
       <c r="B1167" t="s">
-        <v>1411</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="1168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1168" t="s">
-        <v>1412</v>
+        <v>1327</v>
       </c>
       <c r="B1168" t="s">
-        <v>1412</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="1169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1169" t="s">
-        <v>1413</v>
+        <v>1328</v>
       </c>
       <c r="B1169" t="s">
-        <v>1413</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="1170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1170" t="s">
-        <v>1414</v>
+        <v>1329</v>
       </c>
       <c r="B1170" t="s">
-        <v>1414</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="1171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1171" t="s">
-        <v>1415</v>
+        <v>1330</v>
       </c>
       <c r="B1171" t="s">
-        <v>1415</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="1172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1172" t="s">
-        <v>1416</v>
+        <v>1331</v>
       </c>
       <c r="B1172" t="s">
-        <v>1416</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="1173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1173" t="s">
-        <v>1417</v>
+        <v>1332</v>
       </c>
       <c r="B1173" t="s">
-        <v>1417</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="1174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1174" t="s">
-        <v>1418</v>
+        <v>1333</v>
       </c>
       <c r="B1174" t="s">
-        <v>1418</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="1175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1175" t="s">
-        <v>1419</v>
+        <v>1334</v>
       </c>
       <c r="B1175" t="s">
-        <v>1419</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="1176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1176" t="s">
-        <v>1420</v>
+        <v>1335</v>
       </c>
       <c r="B1176" t="s">
-        <v>1420</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="1177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1177" t="s">
-        <v>1421</v>
+        <v>1336</v>
       </c>
       <c r="B1177" t="s">
-        <v>1421</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="1178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1178" t="s">
-        <v>1422</v>
+        <v>1337</v>
       </c>
       <c r="B1178" t="s">
-        <v>1422</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="1179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1179" t="s">
-        <v>1423</v>
+        <v>1338</v>
       </c>
       <c r="B1179" t="s">
-        <v>1423</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="1180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1180" t="s">
-        <v>1424</v>
+        <v>1339</v>
       </c>
       <c r="B1180" t="s">
-        <v>1424</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="1181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1181" t="s">
-        <v>1425</v>
+        <v>1340</v>
       </c>
       <c r="B1181" t="s">
-        <v>1425</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="1182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1182" t="s">
-        <v>1426</v>
+        <v>1341</v>
       </c>
       <c r="B1182" t="s">
-        <v>1426</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="1183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1183" t="s">
-        <v>1427</v>
+        <v>1342</v>
       </c>
       <c r="B1183" t="s">
-        <v>1427</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="1184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1184" t="s">
-        <v>1428</v>
+        <v>1343</v>
       </c>
       <c r="B1184" t="s">
-        <v>1428</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="1185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1185" t="s">
-        <v>1429</v>
+        <v>1344</v>
       </c>
       <c r="B1185" t="s">
-        <v>1429</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="1186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1186" t="s">
-        <v>1430</v>
+        <v>1345</v>
       </c>
       <c r="B1186" t="s">
-        <v>1430</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="1187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1187" t="s">
-        <v>1431</v>
+        <v>1346</v>
       </c>
       <c r="B1187" t="s">
-        <v>1431</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="1188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1188" t="s">
-        <v>1432</v>
+        <v>1347</v>
       </c>
       <c r="B1188" t="s">
-        <v>1432</v>
+        <v>1347</v>
       </c>
     </row>
     <row r="1189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1189" t="s">
-        <v>1433</v>
+        <v>1348</v>
       </c>
       <c r="B1189" t="s">
-        <v>1433</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="1190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1190" t="s">
-        <v>1434</v>
+        <v>1349</v>
       </c>
       <c r="B1190" t="s">
-        <v>1434</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="1191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1191" t="s">
-        <v>1435</v>
+        <v>1350</v>
       </c>
       <c r="B1191" t="s">
-        <v>1435</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="1192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1192" t="s">
-        <v>1436</v>
+        <v>1351</v>
       </c>
       <c r="B1192" t="s">
-        <v>1436</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="1193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1193" t="s">
-        <v>1437</v>
+        <v>1352</v>
       </c>
       <c r="B1193" t="s">
-        <v>1437</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="1194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1194" t="s">
-        <v>1438</v>
+        <v>1353</v>
       </c>
       <c r="B1194" t="s">
-        <v>1438</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="1195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1195" t="s">
-        <v>1439</v>
+        <v>1354</v>
       </c>
       <c r="B1195" t="s">
-        <v>1439</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="1196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1196" t="s">
-        <v>1440</v>
+        <v>1355</v>
       </c>
       <c r="B1196" t="s">
-        <v>1440</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="1197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1197" t="s">
-        <v>1441</v>
+        <v>1356</v>
       </c>
       <c r="B1197" t="s">
-        <v>1441</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="1198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1198" t="s">
-        <v>1442</v>
+        <v>1357</v>
       </c>
       <c r="B1198" t="s">
-        <v>1442</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="1199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1199" t="s">
-        <v>1443</v>
+        <v>1358</v>
       </c>
       <c r="B1199" t="s">
-        <v>1443</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="1200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1200" t="s">
-        <v>1444</v>
+        <v>1359</v>
       </c>
       <c r="B1200" t="s">
-        <v>1444</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="1201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1201" t="s">
-        <v>1445</v>
+        <v>1360</v>
       </c>
       <c r="B1201" t="s">
-        <v>1445</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="1202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1202" t="s">
-        <v>1446</v>
+        <v>1361</v>
       </c>
       <c r="B1202" t="s">
-        <v>1446</v>
+        <v>1361</v>
       </c>
     </row>
     <row r="1203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1203" t="s">
-        <v>1447</v>
+        <v>1362</v>
       </c>
       <c r="B1203" t="s">
-        <v>1447</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="1204" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1204" t="s">
-        <v>1448</v>
+        <v>1363</v>
       </c>
       <c r="B1204" t="s">
-        <v>1448</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="1205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1205" t="s">
-        <v>1449</v>
+        <v>1364</v>
       </c>
       <c r="B1205" t="s">
-        <v>1449</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="1206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1206" t="s">
-        <v>1450</v>
+        <v>1365</v>
       </c>
       <c r="B1206" t="s">
-        <v>1450</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="1207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1207" t="s">
-        <v>1451</v>
+        <v>1366</v>
       </c>
       <c r="B1207" t="s">
-        <v>1451</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="1208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1208" t="s">
-        <v>1452</v>
+        <v>1367</v>
       </c>
       <c r="B1208" t="s">
-        <v>1452</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="1209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1209" t="s">
-        <v>1453</v>
+        <v>1368</v>
       </c>
       <c r="B1209" t="s">
-        <v>1453</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="1210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1210" t="s">
-        <v>1454</v>
+        <v>1369</v>
       </c>
       <c r="B1210" t="s">
-        <v>1454</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="1211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1211" t="s">
-        <v>1455</v>
+        <v>1370</v>
       </c>
       <c r="B1211" t="s">
-        <v>1455</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="1212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1212" t="s">
-        <v>1456</v>
+        <v>1371</v>
       </c>
       <c r="B1212" t="s">
-        <v>1456</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="1213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1213" t="s">
-        <v>1457</v>
+        <v>1372</v>
       </c>
       <c r="B1213" t="s">
-        <v>1457</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="1214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1214" t="s">
-        <v>1458</v>
+        <v>1373</v>
       </c>
       <c r="B1214" t="s">
-        <v>1458</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="1215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1215" t="s">
-        <v>1459</v>
+        <v>1374</v>
       </c>
       <c r="B1215" t="s">
-        <v>1459</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="1216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1216" t="s">
-        <v>1460</v>
+        <v>1375</v>
       </c>
       <c r="B1216" t="s">
-        <v>1460</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="1217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1217" t="s">
-        <v>1461</v>
+        <v>1376</v>
       </c>
       <c r="B1217" t="s">
-        <v>1461</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="1218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1218" t="s">
-        <v>1462</v>
+        <v>1377</v>
       </c>
       <c r="B1218" t="s">
-        <v>1462</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="1219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1219" t="s">
-        <v>1463</v>
+        <v>1378</v>
       </c>
       <c r="B1219" t="s">
-        <v>1463</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="1220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1220" t="s">
-        <v>1464</v>
+        <v>1379</v>
       </c>
       <c r="B1220" t="s">
-        <v>1464</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="1221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1221" t="s">
-        <v>1465</v>
+        <v>1380</v>
       </c>
       <c r="B1221" t="s">
-        <v>1465</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="1222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1222" t="s">
-        <v>1466</v>
+        <v>1381</v>
       </c>
       <c r="B1222" t="s">
-        <v>1466</v>
+        <v>1381</v>
       </c>
     </row>
     <row r="1223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1223" t="s">
-        <v>1467</v>
+        <v>1382</v>
       </c>
       <c r="B1223" t="s">
-        <v>1467</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="1224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1224" t="s">
-        <v>1468</v>
+        <v>1383</v>
       </c>
       <c r="B1224" t="s">
-        <v>1468</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="1225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1225" t="s">
-        <v>1469</v>
+        <v>1384</v>
       </c>
       <c r="B1225" t="s">
-        <v>1469</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="1226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1226" t="s">
-        <v>1470</v>
+        <v>1385</v>
       </c>
       <c r="B1226" t="s">
-        <v>1470</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="1227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1227" t="s">
-        <v>1471</v>
+        <v>1386</v>
       </c>
       <c r="B1227" t="s">
-        <v>1471</v>
+        <v>1386</v>
       </c>
     </row>
     <row r="1228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1228" t="s">
-        <v>1472</v>
+        <v>1387</v>
       </c>
       <c r="B1228" t="s">
-        <v>1472</v>
+        <v>1387</v>
       </c>
     </row>
     <row r="1229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1229" t="s">
-        <v>1473</v>
+        <v>1388</v>
       </c>
       <c r="B1229" t="s">
-        <v>1473</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="1230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1230" t="s">
-        <v>1474</v>
+        <v>1389</v>
       </c>
       <c r="B1230" t="s">
-        <v>1474</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="1231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1231" t="s">
-        <v>1475</v>
+        <v>1390</v>
       </c>
       <c r="B1231" t="s">
-        <v>1475</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="1232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1232" t="s">
-        <v>1476</v>
+        <v>1391</v>
       </c>
       <c r="B1232" t="s">
-        <v>1476</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="1233" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1233" t="s">
-        <v>1477</v>
+        <v>1392</v>
       </c>
       <c r="B1233" t="s">
-        <v>1477</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="1234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1234" t="s">
-        <v>1478</v>
+        <v>1393</v>
       </c>
       <c r="B1234" t="s">
-        <v>1478</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="1235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1235" t="s">
-        <v>1479</v>
+        <v>1394</v>
       </c>
       <c r="B1235" t="s">
-        <v>1479</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="1236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1236" t="s">
-        <v>1480</v>
+        <v>1395</v>
       </c>
       <c r="B1236" t="s">
-        <v>1480</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="1237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1237" t="s">
-        <v>1481</v>
+        <v>1396</v>
       </c>
       <c r="B1237" t="s">
-        <v>1481</v>
+        <v>1396</v>
       </c>
     </row>
     <row r="1238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1238" t="s">
-        <v>1482</v>
+        <v>1397</v>
       </c>
       <c r="B1238" t="s">
-        <v>1482</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="1239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1239" t="s">
-        <v>1483</v>
+        <v>1398</v>
       </c>
       <c r="B1239" t="s">
-        <v>1483</v>
+        <v>1398</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1241" t="s">
+        <v>1399</v>
+      </c>
+      <c r="B1241" t="s">
+        <v>1399</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1242" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B1242" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1243" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B1243" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1244" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B1244" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1245" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B1245" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1246" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B1246" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1247" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B1247" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1248" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B1248" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1249" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B1249" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1250" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B1250" t="s">
+        <v>1425</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1251" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B1251" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1252" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B1252" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1253" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B1253" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1254" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B1254" t="s">
+        <v>1429</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1255" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B1255" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1256" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B1256" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1257" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B1257" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1258" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B1258" t="s">
+        <v>1433</v>
       </c>
     </row>
   </sheetData>
@@ -16231,755 +16192,156 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBE4172-FC39-45CE-BD67-BA23D6FB1A86}">
-  <dimension ref="A1:B97"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B86"/>
+      <selection activeCell="B1" sqref="B1:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1313</v>
+        <v>1399</v>
       </c>
       <c r="B1" t="s">
-        <v>1313</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1314</v>
+        <v>1400</v>
       </c>
       <c r="B2" t="s">
-        <v>1399</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1315</v>
+        <v>1401</v>
       </c>
       <c r="B3" t="s">
-        <v>1400</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1316</v>
+        <v>1402</v>
       </c>
       <c r="B4" t="s">
-        <v>1401</v>
+        <v>1419</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1317</v>
+        <v>1403</v>
       </c>
       <c r="B5" t="s">
-        <v>1402</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1318</v>
+        <v>1404</v>
       </c>
       <c r="B6" t="s">
-        <v>1403</v>
+        <v>1421</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1319</v>
+        <v>1405</v>
       </c>
       <c r="B7" t="s">
-        <v>1404</v>
+        <v>1422</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1320</v>
+        <v>1406</v>
       </c>
       <c r="B8" t="s">
-        <v>1405</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1321</v>
+        <v>1407</v>
       </c>
       <c r="B9" t="s">
-        <v>1406</v>
+        <v>1424</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1322</v>
+        <v>1408</v>
       </c>
       <c r="B10" t="s">
-        <v>1407</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1323</v>
+        <v>1409</v>
       </c>
       <c r="B11" t="s">
-        <v>1408</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1324</v>
+        <v>1410</v>
       </c>
       <c r="B12" t="s">
-        <v>1409</v>
+        <v>1427</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1325</v>
+        <v>1411</v>
       </c>
       <c r="B13" t="s">
-        <v>1410</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1326</v>
+        <v>1412</v>
       </c>
       <c r="B14" t="s">
-        <v>1411</v>
+        <v>1429</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1327</v>
+        <v>1413</v>
       </c>
       <c r="B15" t="s">
-        <v>1412</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1328</v>
+        <v>1414</v>
       </c>
       <c r="B16" t="s">
-        <v>1413</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1329</v>
+        <v>1415</v>
       </c>
       <c r="B17" t="s">
-        <v>1414</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1330</v>
+        <v>1416</v>
       </c>
       <c r="B18" t="s">
-        <v>1415</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>1331</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1416</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>1332</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1417</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>1333</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1418</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>1334</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1419</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>1335</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1420</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>1336</v>
-      </c>
-      <c r="B24" t="s">
-        <v>1421</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>1337</v>
-      </c>
-      <c r="B25" t="s">
-        <v>1422</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>1338</v>
-      </c>
-      <c r="B26" t="s">
-        <v>1423</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>1339</v>
-      </c>
-      <c r="B27" t="s">
-        <v>1424</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>1340</v>
-      </c>
-      <c r="B28" t="s">
-        <v>1425</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>1341</v>
-      </c>
-      <c r="B29" t="s">
-        <v>1426</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>1342</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1427</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>1343</v>
-      </c>
-      <c r="B31" t="s">
-        <v>1428</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>1344</v>
-      </c>
-      <c r="B32" t="s">
-        <v>1429</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>1345</v>
-      </c>
-      <c r="B33" t="s">
-        <v>1430</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1346</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1431</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>1347</v>
-      </c>
-      <c r="B35" t="s">
-        <v>1432</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>1348</v>
-      </c>
-      <c r="B36" t="s">
         <v>1433</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>1349</v>
-      </c>
-      <c r="B37" t="s">
-        <v>1434</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>1350</v>
-      </c>
-      <c r="B38" t="s">
-        <v>1435</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>1351</v>
-      </c>
-      <c r="B39" t="s">
-        <v>1436</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>1352</v>
-      </c>
-      <c r="B40" t="s">
-        <v>1437</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>1353</v>
-      </c>
-      <c r="B41" t="s">
-        <v>1438</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>1354</v>
-      </c>
-      <c r="B42" t="s">
-        <v>1439</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>1355</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1440</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>1356</v>
-      </c>
-      <c r="B44" t="s">
-        <v>1441</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>1357</v>
-      </c>
-      <c r="B45" t="s">
-        <v>1442</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>1358</v>
-      </c>
-      <c r="B46" t="s">
-        <v>1443</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>1359</v>
-      </c>
-      <c r="B47" t="s">
-        <v>1444</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>1360</v>
-      </c>
-      <c r="B48" t="s">
-        <v>1445</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>1361</v>
-      </c>
-      <c r="B49" t="s">
-        <v>1446</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>1362</v>
-      </c>
-      <c r="B50" t="s">
-        <v>1447</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>1363</v>
-      </c>
-      <c r="B51" t="s">
-        <v>1448</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>1364</v>
-      </c>
-      <c r="B52" t="s">
-        <v>1449</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>1365</v>
-      </c>
-      <c r="B53" t="s">
-        <v>1450</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>1366</v>
-      </c>
-      <c r="B54" t="s">
-        <v>1451</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>1367</v>
-      </c>
-      <c r="B55" t="s">
-        <v>1452</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>1368</v>
-      </c>
-      <c r="B56" t="s">
-        <v>1453</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>1369</v>
-      </c>
-      <c r="B57" t="s">
-        <v>1454</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>1370</v>
-      </c>
-      <c r="B58" t="s">
-        <v>1455</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>1371</v>
-      </c>
-      <c r="B59" t="s">
-        <v>1456</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>1372</v>
-      </c>
-      <c r="B60" t="s">
-        <v>1457</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>1373</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1458</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>1374</v>
-      </c>
-      <c r="B62" t="s">
-        <v>1459</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>1375</v>
-      </c>
-      <c r="B63" t="s">
-        <v>1460</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>1376</v>
-      </c>
-      <c r="B64" t="s">
-        <v>1461</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>1377</v>
-      </c>
-      <c r="B65" t="s">
-        <v>1462</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>1378</v>
-      </c>
-      <c r="B66" t="s">
-        <v>1463</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>1379</v>
-      </c>
-      <c r="B67" t="s">
-        <v>1464</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>1380</v>
-      </c>
-      <c r="B68" t="s">
-        <v>1465</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>1381</v>
-      </c>
-      <c r="B69" t="s">
-        <v>1466</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>1382</v>
-      </c>
-      <c r="B70" t="s">
-        <v>1467</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>1383</v>
-      </c>
-      <c r="B71" t="s">
-        <v>1468</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>1384</v>
-      </c>
-      <c r="B72" t="s">
-        <v>1469</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>1385</v>
-      </c>
-      <c r="B73" t="s">
-        <v>1470</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>1386</v>
-      </c>
-      <c r="B74" t="s">
-        <v>1471</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>1387</v>
-      </c>
-      <c r="B75" t="s">
-        <v>1472</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>1388</v>
-      </c>
-      <c r="B76" t="s">
-        <v>1473</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>1389</v>
-      </c>
-      <c r="B77" t="s">
-        <v>1474</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>1390</v>
-      </c>
-      <c r="B78" t="s">
-        <v>1475</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>1391</v>
-      </c>
-      <c r="B79" t="s">
-        <v>1476</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>1392</v>
-      </c>
-      <c r="B80" t="s">
-        <v>1477</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>1393</v>
-      </c>
-      <c r="B81" t="s">
-        <v>1478</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>1394</v>
-      </c>
-      <c r="B82" t="s">
-        <v>1479</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>1395</v>
-      </c>
-      <c r="B83" t="s">
-        <v>1480</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>1396</v>
-      </c>
-      <c r="B84" t="s">
-        <v>1481</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>1397</v>
-      </c>
-      <c r="B85" t="s">
-        <v>1482</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>1398</v>
-      </c>
-      <c r="B86" t="s">
-        <v>1483</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>1484</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>1485</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>1486</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>1487</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>1488</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>1489</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>1490</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>1491</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>1492</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>1493</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>1494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Luận an Lộc tồn
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FC1086-59CF-46E0-9FDB-A0F3CA49BF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316EA4E6-B3CB-4BEA-9629-65914B6831B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2813" uniqueCount="1434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2822" uniqueCount="1446">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -4238,57 +4238,6 @@
     <t>Thiên Khôi toạ thủ cung Mệnh</t>
   </si>
   <si>
-    <t>luanmenh.js:3499 Thiên Khôi toạ thủ cung Mệnh gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3502 Thiên Khôi toạ thủ cung Mệnh gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3505 Thiên Khôi toạ thủ cung Mệnh gặp Hóa Kỵ, Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3508 Thiên Khôi toạ thủ cung Mệnh gặp các sao Văn Xương, Văn Khúc, Tấu Thư, Thái Tuế</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3512 Thiên Khôi toạ thủ cung Mệnh gặp Thiên Lương, Thiên Cơ, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3515 Thiên Khôi toạ thủ cung Mệnh gặp Hóa Lộc mà không gặp các sao Sát tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3518 Thiên Khôi toạ thủ cung Mệnh ở Ngọ đồng cung Tử Vi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3496 Thiên Việt toạ thủ cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3499 Thiên Việt toạ thủ cung Mệnh gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3502 Thiên Việt toạ thủ cung Mệnh gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3505 Thiên Việt toạ thủ cung Mệnh gặp Hóa Kỵ, Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3508 Thiên Việt toạ thủ cung Mệnh gặp các sao Văn Xương, Văn Khúc, Tấu Thư, Thái Tuế</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3512 Thiên Việt toạ thủ cung Mệnh gặp Thiên Lương, Thiên Cơ, Hoá Lộc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3515 Thiên Việt toạ thủ cung Mệnh gặp Hóa Lộc mà không gặp các sao Sát tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3518 Thiên Việt toạ thủ cung Mệnh ở Ngọ đồng cung Tử Vi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3528 Mệnh có Thái Dương giáp Khôi Việt</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3531 Mệnh có Hóa Lộc giáp Khôi Việt</t>
-  </si>
-  <si>
     <t>Thiên Khôi toạ thủ cung Mệnh gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hoá Khoa, Hoá Quyền, Hoá Lộc</t>
   </si>
   <si>
@@ -4338,6 +4287,93 @@
   </si>
   <si>
     <t>Mệnh có Hóa Lộc giáp Khôi Việt</t>
+  </si>
+  <si>
+    <t>Lộc Tồn toạ thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3616 Lộc Tồn toạ thủ cung Mệnh gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Thiên Mã</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3619 Lộc Tồn toạ thủ cung Mệnh gặp Ân Quang, Thiên Quý, Quan Phù, Thiên Y, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3622 Lộc Tồn toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp, Đại Hao, Tiểu Hao, Hóa Kỵ, Tuế Phá</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3625 Lộc Tồn toạ thủ cung Mệnh gặp Phá Quân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3629 Lộc Tồn toạ thủ cung Mệnh đồng cung Hoá Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3632 Song Lộc xung chiếu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3636 Lộc Tồn toạ thủ cung Mệnh đồng cung Thiên Mã</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3639 Lộc Mã giao trì không gặp Tuế Phá, Địa Kiếp, Thiên Không</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3645 Lộc Tồn toạ thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3649 Lộc Tồn toạ thủ cung Thiên Di ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3652 Lộc Tồn toạ thủ cung Phu Thê ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3645 Lộc Tồn toạ thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3649 Lộc Tồn toạ thủ cung Thiên Di ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:3652 Lộc Tồn toạ thủ cung Phu Thê ở Ngọ</t>
+  </si>
+  <si>
+    <t>Lộc Tồn toạ thủ cung Mệnh gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Thiên Mã</t>
+  </si>
+  <si>
+    <t>Lộc Tồn toạ thủ cung Mệnh gặp Ân Quang, Thiên Quý, Quan Phù, Thiên Y, Thiên Riêu</t>
+  </si>
+  <si>
+    <t>Lộc Tồn toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp, Đại Hao, Tiểu Hao, Hóa Kỵ, Tuế Phá</t>
+  </si>
+  <si>
+    <t>Lộc Tồn toạ thủ cung Mệnh gặp Phá Quân</t>
+  </si>
+  <si>
+    <t>Lộc Tồn toạ thủ cung Mệnh đồng cung Hoá Lộc</t>
+  </si>
+  <si>
+    <t>Song Lộc xung chiếu</t>
+  </si>
+  <si>
+    <t>Lộc Tồn toạ thủ cung Mệnh đồng cung Thiên Mã</t>
+  </si>
+  <si>
+    <t>Lộc Mã giao trì không gặp Tuế Phá, Địa Kiếp, Thiên Không</t>
+  </si>
+  <si>
+    <t>Lộc Tồn toạ thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>Lộc Tồn toạ thủ cung Thiên Di ở Tý</t>
+  </si>
+  <si>
+    <t>Lộc Tồn toạ thủ cung Phu Thê ở Tý</t>
+  </si>
+  <si>
+    <t>Lộc Tồn toạ thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Lộc Tồn toạ thủ cung Thiên Di ở Ngọ</t>
+  </si>
+  <si>
+    <t>Lộc Tồn toạ thủ cung Phu Thê ở Ngọ</t>
   </si>
 </sst>
 </file>
@@ -4386,7 +4422,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -6417,10 +6473,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B1258"/>
+  <dimension ref="A1:B1274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1238" workbookViewId="0">
-      <selection activeCell="G1259" sqref="G1259"/>
+    <sheetView tabSelected="1" topLeftCell="A1244" workbookViewId="0">
+      <selection activeCell="F1268" sqref="F1268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15992,198 +16048,322 @@
     </row>
     <row r="1242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1242" t="s">
-        <v>1417</v>
+        <v>1400</v>
       </c>
       <c r="B1242" t="s">
-        <v>1417</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="1243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1243" t="s">
-        <v>1418</v>
+        <v>1401</v>
       </c>
       <c r="B1243" t="s">
-        <v>1418</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="1244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1244" t="s">
-        <v>1419</v>
+        <v>1402</v>
       </c>
       <c r="B1244" t="s">
-        <v>1419</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="1245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1245" t="s">
-        <v>1420</v>
+        <v>1403</v>
       </c>
       <c r="B1245" t="s">
-        <v>1420</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="1246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1246" t="s">
-        <v>1421</v>
+        <v>1404</v>
       </c>
       <c r="B1246" t="s">
-        <v>1421</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="1247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1247" t="s">
-        <v>1422</v>
+        <v>1405</v>
       </c>
       <c r="B1247" t="s">
-        <v>1422</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="1248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1248" t="s">
-        <v>1423</v>
+        <v>1406</v>
       </c>
       <c r="B1248" t="s">
-        <v>1423</v>
+        <v>1406</v>
       </c>
     </row>
     <row r="1249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1249" t="s">
-        <v>1424</v>
+        <v>1407</v>
       </c>
       <c r="B1249" t="s">
-        <v>1424</v>
+        <v>1407</v>
       </c>
     </row>
     <row r="1250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1250" t="s">
-        <v>1425</v>
+        <v>1408</v>
       </c>
       <c r="B1250" t="s">
-        <v>1425</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="1251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1251" t="s">
-        <v>1426</v>
+        <v>1409</v>
       </c>
       <c r="B1251" t="s">
-        <v>1426</v>
+        <v>1409</v>
       </c>
     </row>
     <row r="1252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1252" t="s">
-        <v>1427</v>
+        <v>1410</v>
       </c>
       <c r="B1252" t="s">
-        <v>1427</v>
+        <v>1410</v>
       </c>
     </row>
     <row r="1253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1253" t="s">
-        <v>1428</v>
+        <v>1411</v>
       </c>
       <c r="B1253" t="s">
-        <v>1428</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="1254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1254" t="s">
-        <v>1429</v>
+        <v>1412</v>
       </c>
       <c r="B1254" t="s">
-        <v>1429</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="1255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1255" t="s">
-        <v>1430</v>
+        <v>1413</v>
       </c>
       <c r="B1255" t="s">
-        <v>1430</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="1256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1256" t="s">
-        <v>1431</v>
+        <v>1414</v>
       </c>
       <c r="B1256" t="s">
-        <v>1431</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="1257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1257" t="s">
-        <v>1432</v>
+        <v>1415</v>
       </c>
       <c r="B1257" t="s">
-        <v>1432</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="1258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1258" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B1258" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1260" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B1260" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1261" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B1261" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1262" t="s">
         <v>1433</v>
       </c>
-      <c r="B1258" t="s">
+      <c r="B1262" t="s">
         <v>1433</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1263" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B1263" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1264" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B1264" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1265" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B1265" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1266" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B1266" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1267" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B1267" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1268" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B1268" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1269" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B1269" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1270" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B1270" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1271" t="s">
+        <v>1442</v>
+      </c>
+      <c r="B1271" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1272" t="s">
+        <v>1443</v>
+      </c>
+      <c r="B1272" t="s">
+        <v>1443</v>
+      </c>
+    </row>
+    <row r="1273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1273" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B1273" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1274" t="s">
+        <v>1445</v>
+      </c>
+      <c r="B1274" t="s">
+        <v>1445</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="26" priority="34"/>
-    <cfRule type="duplicateValues" dxfId="25" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="24" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="22" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145:A208">
-    <cfRule type="duplicateValues" dxfId="20" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A209:A1048576 A1:A23 A25:A84 A143">
-    <cfRule type="duplicateValues" dxfId="19" priority="43"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="17" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
+    <cfRule type="duplicateValues" dxfId="18" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="34"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
     <cfRule type="duplicateValues" dxfId="16" priority="31"/>
     <cfRule type="duplicateValues" dxfId="15" priority="32"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
+  <conditionalFormatting sqref="B29">
     <cfRule type="duplicateValues" dxfId="14" priority="29"/>
     <cfRule type="duplicateValues" dxfId="13" priority="30"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
+  <conditionalFormatting sqref="B30">
     <cfRule type="duplicateValues" dxfId="12" priority="27"/>
     <cfRule type="duplicateValues" dxfId="11" priority="28"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="duplicateValues" dxfId="10" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="26"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B84:B142">
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B143">
-    <cfRule type="duplicateValues" dxfId="6" priority="56"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="4" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B325:B401">
-    <cfRule type="duplicateValues" dxfId="2" priority="132"/>
-    <cfRule type="duplicateValues" dxfId="1" priority="133"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="134"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="135"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B402:B1048576 B1:B23 B25 B28 B31:B83 B145:B324">
-    <cfRule type="duplicateValues" dxfId="0" priority="42"/>
+  <conditionalFormatting sqref="B402:B1259 B1:B23 B25 B28 B31:B83 B145:B324 B1275:B1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="44"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1260:B1274">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16192,156 +16372,147 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBE4172-FC39-45CE-BD67-BA23D6FB1A86}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B18"/>
+      <selection activeCell="B1" sqref="B1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1399</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1399</v>
+        <v>1417</v>
+      </c>
+      <c r="B1" t="str">
+        <f>A1</f>
+        <v>Lộc Tồn toạ thủ cung Mệnh</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1400</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1417</v>
+        <v>1418</v>
+      </c>
+      <c r="B2" t="str">
+        <f>RIGHT(A2,LEN(A2)-17)</f>
+        <v>Lộc Tồn toạ thủ cung Mệnh gặp Tử Vi, Thiên Phủ, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Thiên Mã</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1401</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1418</v>
+        <v>1419</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B15" si="0">RIGHT(A3,LEN(A3)-17)</f>
+        <v>Lộc Tồn toạ thủ cung Mệnh gặp Ân Quang, Thiên Quý, Quan Phù, Thiên Y, Thiên Riêu</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1402</v>
-      </c>
-      <c r="B4" t="s">
-        <v>1419</v>
+        <v>1420</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>Lộc Tồn toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp, Đại Hao, Tiểu Hao, Hóa Kỵ, Tuế Phá</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1403</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1420</v>
+        <v>1421</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Lộc Tồn toạ thủ cung Mệnh gặp Phá Quân</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1404</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1421</v>
+        <v>1422</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>Lộc Tồn toạ thủ cung Mệnh đồng cung Hoá Lộc</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1405</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1422</v>
+        <v>1423</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>Song Lộc xung chiếu</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1406</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1423</v>
+        <v>1424</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>Lộc Tồn toạ thủ cung Mệnh đồng cung Thiên Mã</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1407</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1424</v>
+        <v>1425</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>Lộc Mã giao trì không gặp Tuế Phá, Địa Kiếp, Thiên Không</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1408</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1425</v>
+        <v>1426</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>Lộc Tồn toạ thủ cung Mệnh ở Tý</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1409</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1426</v>
+        <v>1427</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>Lộc Tồn toạ thủ cung Thiên Di ở Tý</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1410</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1427</v>
+        <v>1428</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>Lộc Tồn toạ thủ cung Phu Thê ở Tý</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1411</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1428</v>
+        <v>1429</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>Lộc Tồn toạ thủ cung Mệnh ở Ngọ</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1412</v>
-      </c>
-      <c r="B14" t="s">
-        <v>1429</v>
+        <v>1430</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>Lộc Tồn toạ thủ cung Thiên Di ở Ngọ</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1413</v>
-      </c>
-      <c r="B15" t="s">
-        <v>1430</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>1414</v>
-      </c>
-      <c r="B16" t="s">
         <v>1431</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>1415</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1432</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>1416</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1433</v>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>Lộc Tồn toạ thủ cung Phu Thê ở Ngọ</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
An Hoả tinh Linh tinh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -1,42 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52EBEADF-05A9-41C0-9AA1-861A2CD9A790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69AE834-32A5-40AF-BB73-15D7E26FA0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3045" uniqueCount="1550">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3022" uniqueCount="1564">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -4427,265 +4418,307 @@
     <t>Mệnh có Tử Vi giáp Tả Phù Hữu Bật</t>
   </si>
   <si>
-    <t>Kình Dương toạ thủ cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3944 Kình Dương toạ thủ cung Mệnh gặp Hóa Kỵ, Liêm Trinh, Cự Môn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3947 Kình Dương, Cự Môn, Liêm Trinh, Hóa Kỵ đồng cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3954 Kình Dương toạ thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3954 Kình Dương toạ thủ cung Mệnh ở  Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3954 Kình Dương toạ thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3954 Kình Dương toạ thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3960 Kình Dương toạ thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3960 Kình Dương toạ thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3960 Kình Dương toạ thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3960 Kình Dương toạ thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3960 Kình Dương toạ thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3960 Kình Dương toạ thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3960 Kình Dương toạ thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3960 Kình Dương toạ thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3965 Thái Dương, Thái Âm đồng cung Mệnh gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3971 Thiên Phủ, Tử Vi đồng cung Mệnh ở Tỵ gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3971 Thiên Phủ, Tử Vi đồng cung Mệnh ở Mùi gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3977 Kình Dương toạ thủ cung Mệnh gặp Thiên Khôi, Hóa Quyền, Hóa Lộc, Thiên Mã</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3980 Kình Dương, Thái Âm, Thiên Đồng đồng cung Mệnh ở Ngọ gặp Địa Giải, Phượng Các</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3986 Tham Lang, Vũ Khúc đồng cung Mệnh ở Thìn gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3986 Tham Lang, Vũ Khúc đồng cung Mệnh ở Tuất gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3986 Tham Lang, Vũ Khúc đồng cung Mệnh ở Sửu gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3986 Tham Lang, Vũ Khúc đồng cung Mệnh ở Mùi gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3993 Kình Dương toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Đà La</t>
-  </si>
-  <si>
-    <t>luanmenh.js:3998 Kình Dương toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp, Đà La</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4002 Kình Dương, Đà La giáp mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4005 Mệnh có Hóa Kỵ giáp Kình Dương, Đà La</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4011 Kình Dương, Lực Sỹ đồng cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4016 Đà La toạ thủ cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4019 Đà La toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Kình Dương, Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4024 Đà La toạ thủ cung Mệnh gặp Hóa Kỵ, Liêm Trinh, Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4030 Đà La toạ thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4030 Đà La toạ thủ cung Mệnh ở  Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4030 Đà La toạ thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4030 Đà La toạ thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4036 Đà La toạ thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4036 Đà La toạ thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4036 Đà La toạ thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4036 Đà La toạ thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4036 Đà La toạ thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4036 Đà La toạ thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4036 Đà La toạ thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4036 Đà La toạ thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t>Kình Dương toạ thủ cung Mệnh gặp Hóa Kỵ, Liêm Trinh, Cự Môn</t>
-  </si>
-  <si>
-    <t>Kình Dương, Cự Môn, Liêm Trinh, Hóa Kỵ đồng cung Mệnh</t>
-  </si>
-  <si>
-    <t>Kình Dương toạ thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>Kình Dương toạ thủ cung Mệnh ở  Tuất</t>
-  </si>
-  <si>
-    <t>Kình Dương toạ thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>Kình Dương toạ thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>Kình Dương toạ thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t>Kình Dương toạ thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>Kình Dương toạ thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>Kình Dương toạ thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t>Kình Dương toạ thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>Kình Dương toạ thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>Kình Dương toạ thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t>Kình Dương toạ thủ cung Mệnh ở Hợi</t>
-  </si>
-  <si>
-    <t>Thái Dương, Thái Âm đồng cung Mệnh gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>Thiên Phủ, Tử Vi đồng cung Mệnh ở Tỵ gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>Thiên Phủ, Tử Vi đồng cung Mệnh ở Mùi gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>Kình Dương toạ thủ cung Mệnh gặp Thiên Khôi, Hóa Quyền, Hóa Lộc, Thiên Mã</t>
-  </si>
-  <si>
-    <t>Kình Dương, Thái Âm, Thiên Đồng đồng cung Mệnh ở Ngọ gặp Địa Giải, Phượng Các</t>
-  </si>
-  <si>
-    <t>Tham Lang, Vũ Khúc đồng cung Mệnh ở Thìn gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>Tham Lang, Vũ Khúc đồng cung Mệnh ở Tuất gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>Tham Lang, Vũ Khúc đồng cung Mệnh ở Sửu gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>Tham Lang, Vũ Khúc đồng cung Mệnh ở Mùi gặp Kình Dương</t>
-  </si>
-  <si>
-    <t>Kình Dương toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Đà La</t>
-  </si>
-  <si>
-    <t>Kình Dương toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp, Đà La</t>
-  </si>
-  <si>
-    <t>Kình Dương, Đà La giáp mệnh</t>
-  </si>
-  <si>
-    <t>Mệnh có Hóa Kỵ giáp Kình Dương, Đà La</t>
-  </si>
-  <si>
-    <t>Kình Dương, Lực Sỹ đồng cung Mệnh</t>
-  </si>
-  <si>
-    <t>Đà La toạ thủ cung Mệnh</t>
-  </si>
-  <si>
-    <t>Đà La toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Kình Dương, Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>Đà La toạ thủ cung Mệnh gặp Hóa Kỵ, Liêm Trinh, Thiên Hình</t>
-  </si>
-  <si>
-    <t>Đà La toạ thủ cung Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>Đà La toạ thủ cung Mệnh ở  Tuất</t>
-  </si>
-  <si>
-    <t>Đà La toạ thủ cung Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>Đà La toạ thủ cung Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>Đà La toạ thủ cung Mệnh ở Tý</t>
-  </si>
-  <si>
-    <t>Đà La toạ thủ cung Mệnh ở Dần</t>
-  </si>
-  <si>
-    <t>Đà La toạ thủ cung Mệnh ở Mão</t>
-  </si>
-  <si>
-    <t>Đà La toạ thủ cung Mệnh ở Tỵ</t>
-  </si>
-  <si>
-    <t>Đà La toạ thủ cung Mệnh ở Ngọ</t>
-  </si>
-  <si>
-    <t>Đà La toạ thủ cung Mệnh ở Thân</t>
-  </si>
-  <si>
-    <t>Đà La toạ thủ cung Mệnh ở Dậu</t>
-  </si>
-  <si>
-    <t>Đà La toạ thủ cung Mệnh ở Hợi</t>
+    <t>Hỏa Tinh toạ thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4148 Hỏa Tinh toạ thủ cung Mệnh gặp Hóa Kỵ, Liêm Trinh, Cự Môn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4145 Linh Tinh toạ thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4148 Linh Tinh toạ thủ cung Mệnh gặp Hóa Kỵ, Liêm Trinh, Cự Môn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4157 Hỏa Tinh toạ thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4157 Linh Tinh toạ thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4157 Hỏa Tinh toạ thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4157 Linh Tinh toạ thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4157 Hỏa Tinh toạ thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4157 Linh Tinh toạ thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4157 Hỏa Tinh toạ thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4157 Linh Tinh toạ thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4157 Hỏa Tinh toạ thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4157 Linh Tinh toạ thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4166 Hỏa Tinh toạ thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4166 Linh Tinh toạ thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4166 Hỏa Tinh toạ thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4166 Linh Tinh toạ thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4166 Hỏa Tinh toạ thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4166 Linh Tinh toạ thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4166 Hỏa Tinh toạ thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4166 Linh Tinh toạ thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4166 Hỏa Tinh toạ thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4166 Linh Tinh toạ thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4166 Hỏa Tinh toạ thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4166 Linh Tinh toạ thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4166 Hỏa Tinh toạ thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4166 Linh Tinh toạ thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4175 Tham Lang, Vũ Khúc đồng cung Mệnh ở Thìn gặp Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4178 Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Thìn gặp Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4175 Tham Lang, Vũ Khúc đồng cung Mệnh ở Thìn gặp Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4178 Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Thìn gặp Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4175 Tham Lang, Vũ Khúc đồng cung Mệnh ở Tuất gặp Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4178 Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Tuất gặp Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4175 Tham Lang, Vũ Khúc đồng cung Mệnh ở Tuất gặp Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4178 Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Tuất gặp Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4175 Tham Lang, Vũ Khúc đồng cung Mệnh ở Sửu gặp Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4178 Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Sửu gặp Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4175 Tham Lang, Vũ Khúc đồng cung Mệnh ở Sửu gặp Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4178 Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Sửu gặp Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4175 Tham Lang, Vũ Khúc đồng cung Mệnh ở Mùi gặp Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4178 Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Mùi gặp Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4175 Tham Lang, Vũ Khúc đồng cung Mệnh ở Mùi gặp Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4178 Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Mùi gặp Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4186 Hỏa Tinh toạ thủ cung Mệnh gặp Linh Tinh ở Thiên Di</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4189 Hỏa Tinh toạ thủ cung Mệnh đối xung Linh Tinh và gặp Kình Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4194 Linh Tinh toạ thủ cung Mệnh gặp Hỏa Tinh ở Thiên Di</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4197 Linh Tinh toạ thủ cung Mệnh đối xung Hỏa Tinh và gặp Kình Dương</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4202 Hỏa Tinh, Linh Tinh đồng cung Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4209 Hỏa Tinh toạ thủ cung Mệnh ở Hợi gặp Thiên Hình, Tham Lang</t>
+  </si>
+  <si>
+    <t>luanmenh.js:4213 Linh Tinh toạ thủ cung Mệnh gặp Thiên Mã, Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh toạ thủ cung Mệnh gặp Hóa Kỵ, Liêm Trinh, Cự Môn</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh gặp Hóa Kỵ, Liêm Trinh, Cự Môn</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh toạ thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh toạ thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh ở Mão</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh toạ thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh ở Thìn</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh toạ thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh ở Tỵ</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh toạ thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh ở Ngọ</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh toạ thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh ở Tý</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh toạ thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh toạ thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh ở Dậu</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh toạ thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh toạ thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh ở Tuất</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh toạ thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh ở Mùi</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh toạ thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh ở Thân</t>
+  </si>
+  <si>
+    <t>Tham Lang, Vũ Khúc đồng cung Mệnh ở Thìn gặp Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Thìn gặp Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>Tham Lang, Vũ Khúc đồng cung Mệnh ở Thìn gặp Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Thìn gặp Linh Tinh</t>
+  </si>
+  <si>
+    <t>Tham Lang, Vũ Khúc đồng cung Mệnh ở Tuất gặp Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Tuất gặp Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>Tham Lang, Vũ Khúc đồng cung Mệnh ở Tuất gặp Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Tuất gặp Linh Tinh</t>
+  </si>
+  <si>
+    <t>Tham Lang, Vũ Khúc đồng cung Mệnh ở Sửu gặp Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Sửu gặp Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>Tham Lang, Vũ Khúc đồng cung Mệnh ở Sửu gặp Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Sửu gặp Linh Tinh</t>
+  </si>
+  <si>
+    <t>Tham Lang, Vũ Khúc đồng cung Mệnh ở Mùi gặp Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Mùi gặp Hỏa Tinh</t>
+  </si>
+  <si>
+    <t>Tham Lang, Vũ Khúc đồng cung Mệnh ở Mùi gặp Linh Tinh</t>
+  </si>
+  <si>
+    <t>Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Mùi gặp Linh Tinh</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh toạ thủ cung Mệnh gặp Linh Tinh ở Thiên Di</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh toạ thủ cung Mệnh đối xung Linh Tinh và gặp Kình Dương</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh gặp Hỏa Tinh ở Thiên Di</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh đối xung Hỏa Tinh và gặp Kình Dương</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh, Linh Tinh đồng cung Mệnh</t>
+  </si>
+  <si>
+    <t>Hỏa Tinh toạ thủ cung Mệnh ở Hợi gặp Thiên Hình, Tham Lang</t>
+  </si>
+  <si>
+    <t>Linh Tinh toạ thủ cung Mệnh gặp Thiên Mã, Kình Dương, Đà La</t>
   </si>
 </sst>
 </file>
@@ -6785,10 +6818,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B1306"/>
+  <dimension ref="A1:B1358"/>
   <sheetViews>
-    <sheetView topLeftCell="A1292" workbookViewId="0">
-      <selection activeCell="I1266" sqref="I1266"/>
+    <sheetView tabSelected="1" topLeftCell="A1337" workbookViewId="0">
+      <selection activeCell="A1323" sqref="A1323"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16860,6 +16893,414 @@
       </c>
       <c r="B1306" t="s">
         <v>1462</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1308" t="s">
+        <v>1463</v>
+      </c>
+      <c r="B1308" t="s">
+        <v>1463</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1309" t="s">
+        <v>1514</v>
+      </c>
+      <c r="B1309" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1310" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B1310" t="s">
+        <v>1515</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1311" t="s">
+        <v>1516</v>
+      </c>
+      <c r="B1311" t="s">
+        <v>1516</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1312" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B1312" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1313" t="s">
+        <v>1518</v>
+      </c>
+      <c r="B1313" t="s">
+        <v>1518</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1314" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B1314" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1315" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B1315" t="s">
+        <v>1520</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1316" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B1316" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1317" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B1317" t="s">
+        <v>1522</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1318" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B1318" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1319" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B1319" t="s">
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1320" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B1320" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1321" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B1321" t="s">
+        <v>1526</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1322" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B1322" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1323" t="s">
+        <v>1528</v>
+      </c>
+      <c r="B1323" t="s">
+        <v>1528</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1324" t="s">
+        <v>1529</v>
+      </c>
+      <c r="B1324" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1325" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B1325" t="s">
+        <v>1530</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1326" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B1326" t="s">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1327" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B1327" t="s">
+        <v>1532</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1328" t="s">
+        <v>1533</v>
+      </c>
+      <c r="B1328" t="s">
+        <v>1533</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1329" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B1329" t="s">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1330" t="s">
+        <v>1535</v>
+      </c>
+      <c r="B1330" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1331" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B1331" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1332" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B1332" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="1333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1333" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B1333" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1334" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B1334" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1335" t="s">
+        <v>1540</v>
+      </c>
+      <c r="B1335" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1336" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B1336" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1337" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B1337" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1338" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B1338" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1339" t="s">
+        <v>1544</v>
+      </c>
+      <c r="B1339" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1340" t="s">
+        <v>1545</v>
+      </c>
+      <c r="B1340" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1341" t="s">
+        <v>1546</v>
+      </c>
+      <c r="B1341" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1342" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B1342" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1343" t="s">
+        <v>1548</v>
+      </c>
+      <c r="B1343" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1344" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B1344" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1345" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B1345" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1346" t="s">
+        <v>1551</v>
+      </c>
+      <c r="B1346" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1347" t="s">
+        <v>1552</v>
+      </c>
+      <c r="B1347" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1348" t="s">
+        <v>1553</v>
+      </c>
+      <c r="B1348" t="s">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1349" t="s">
+        <v>1554</v>
+      </c>
+      <c r="B1349" t="s">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1350" t="s">
+        <v>1555</v>
+      </c>
+      <c r="B1350" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1351" t="s">
+        <v>1556</v>
+      </c>
+      <c r="B1351" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1352" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B1352" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="1353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1353" t="s">
+        <v>1558</v>
+      </c>
+      <c r="B1353" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1354" t="s">
+        <v>1559</v>
+      </c>
+      <c r="B1354" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1355" t="s">
+        <v>1560</v>
+      </c>
+      <c r="B1355" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1356" t="s">
+        <v>1561</v>
+      </c>
+      <c r="B1356" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1357" t="s">
+        <v>1562</v>
+      </c>
+      <c r="B1357" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1358" t="s">
+        <v>1563</v>
+      </c>
+      <c r="B1358" t="s">
+        <v>1563</v>
       </c>
     </row>
   </sheetData>
@@ -16932,10 +17373,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBE4172-FC39-45CE-BD67-BA23D6FB1A86}">
-  <dimension ref="A1:B89"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16944,704 +17385,459 @@
       <c r="A1" t="s">
         <v>1463</v>
       </c>
-      <c r="B1" t="s">
-        <v>1463</v>
+      <c r="B1" t="str">
+        <f>A1</f>
+        <v>Hỏa Tinh toạ thủ cung Mệnh</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1464</v>
       </c>
-      <c r="B2" t="s">
-        <v>1507</v>
+      <c r="B2" t="str">
+        <f>RIGHT(A2,LEN(A2)-17)</f>
+        <v>Hỏa Tinh toạ thủ cung Mệnh gặp Hóa Kỵ, Liêm Trinh, Cự Môn</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1465</v>
       </c>
-      <c r="B3" t="s">
-        <v>1508</v>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B51" si="0">RIGHT(A3,LEN(A3)-17)</f>
+        <v>Linh Tinh toạ thủ cung Mệnh</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1466</v>
       </c>
-      <c r="B4" t="s">
-        <v>1509</v>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>Linh Tinh toạ thủ cung Mệnh gặp Hóa Kỵ, Liêm Trinh, Cự Môn</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1467</v>
       </c>
-      <c r="B5" t="s">
-        <v>1510</v>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Hỏa Tinh toạ thủ cung Mệnh ở Dần</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1468</v>
       </c>
-      <c r="B6" t="s">
-        <v>1511</v>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>Linh Tinh toạ thủ cung Mệnh ở Dần</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1469</v>
       </c>
-      <c r="B7" t="s">
-        <v>1512</v>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>Hỏa Tinh toạ thủ cung Mệnh ở Mão</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1470</v>
       </c>
-      <c r="B8" t="s">
-        <v>1513</v>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>Linh Tinh toạ thủ cung Mệnh ở Mão</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1471</v>
       </c>
-      <c r="B9" t="s">
-        <v>1514</v>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>Hỏa Tinh toạ thủ cung Mệnh ở Thìn</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1472</v>
       </c>
-      <c r="B10" t="s">
-        <v>1515</v>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>Linh Tinh toạ thủ cung Mệnh ở Thìn</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1473</v>
       </c>
-      <c r="B11" t="s">
-        <v>1516</v>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>Hỏa Tinh toạ thủ cung Mệnh ở Tỵ</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>1474</v>
       </c>
-      <c r="B12" t="s">
-        <v>1517</v>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>Linh Tinh toạ thủ cung Mệnh ở Tỵ</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1475</v>
       </c>
-      <c r="B13" t="s">
-        <v>1518</v>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>Hỏa Tinh toạ thủ cung Mệnh ở Ngọ</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1476</v>
       </c>
-      <c r="B14" t="s">
-        <v>1519</v>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>Linh Tinh toạ thủ cung Mệnh ở Ngọ</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1477</v>
       </c>
-      <c r="B15" t="s">
-        <v>1520</v>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>Hỏa Tinh toạ thủ cung Mệnh ở Tý</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1478</v>
       </c>
-      <c r="B16" t="s">
-        <v>1521</v>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>Linh Tinh toạ thủ cung Mệnh ở Tý</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1479</v>
       </c>
-      <c r="B17" t="s">
-        <v>1522</v>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>Hỏa Tinh toạ thủ cung Mệnh ở Sửu</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>1480</v>
       </c>
-      <c r="B18" t="s">
-        <v>1523</v>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>Linh Tinh toạ thủ cung Mệnh ở Sửu</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1481</v>
       </c>
-      <c r="B19" t="s">
-        <v>1524</v>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>Hỏa Tinh toạ thủ cung Mệnh ở Dậu</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1482</v>
       </c>
-      <c r="B20" t="s">
-        <v>1525</v>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>Linh Tinh toạ thủ cung Mệnh ở Dậu</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1483</v>
       </c>
-      <c r="B21" t="s">
-        <v>1526</v>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>Hỏa Tinh toạ thủ cung Mệnh ở Hợi</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>1484</v>
       </c>
-      <c r="B22" t="s">
-        <v>1527</v>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>Linh Tinh toạ thủ cung Mệnh ở Hợi</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1485</v>
       </c>
-      <c r="B23" t="s">
-        <v>1528</v>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>Hỏa Tinh toạ thủ cung Mệnh ở Tuất</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1486</v>
       </c>
-      <c r="B24" t="s">
-        <v>1529</v>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>Linh Tinh toạ thủ cung Mệnh ở Tuất</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1487</v>
       </c>
-      <c r="B25" t="s">
-        <v>1530</v>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>Hỏa Tinh toạ thủ cung Mệnh ở Mùi</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1488</v>
       </c>
-      <c r="B26" t="s">
-        <v>1531</v>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>Linh Tinh toạ thủ cung Mệnh ở Mùi</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1489</v>
       </c>
-      <c r="B27" t="s">
-        <v>1532</v>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>Hỏa Tinh toạ thủ cung Mệnh ở Thân</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1490</v>
       </c>
-      <c r="B28" t="s">
-        <v>1533</v>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>Linh Tinh toạ thủ cung Mệnh ở Thân</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1491</v>
       </c>
-      <c r="B29" t="s">
-        <v>1534</v>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>Tham Lang, Vũ Khúc đồng cung Mệnh ở Thìn gặp Hỏa Tinh</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1492</v>
       </c>
-      <c r="B30" t="s">
-        <v>1535</v>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Thìn gặp Hỏa Tinh</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1493</v>
       </c>
-      <c r="B31" t="s">
-        <v>1536</v>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>Tham Lang, Vũ Khúc đồng cung Mệnh ở Thìn gặp Linh Tinh</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1494</v>
       </c>
-      <c r="B32" t="s">
-        <v>1537</v>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Thìn gặp Linh Tinh</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1495</v>
       </c>
-      <c r="B33" t="s">
-        <v>1538</v>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>Tham Lang, Vũ Khúc đồng cung Mệnh ở Tuất gặp Hỏa Tinh</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1496</v>
       </c>
-      <c r="B34" t="s">
-        <v>1539</v>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Tuất gặp Hỏa Tinh</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1497</v>
       </c>
-      <c r="B35" t="s">
-        <v>1540</v>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>Tham Lang, Vũ Khúc đồng cung Mệnh ở Tuất gặp Linh Tinh</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>1498</v>
       </c>
-      <c r="B36" t="s">
-        <v>1541</v>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Tuất gặp Linh Tinh</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1499</v>
       </c>
-      <c r="B37" t="s">
-        <v>1542</v>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>Tham Lang, Vũ Khúc đồng cung Mệnh ở Sửu gặp Hỏa Tinh</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>1500</v>
       </c>
-      <c r="B38" t="s">
-        <v>1543</v>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Sửu gặp Hỏa Tinh</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1501</v>
       </c>
-      <c r="B39" t="s">
-        <v>1544</v>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>Tham Lang, Vũ Khúc đồng cung Mệnh ở Sửu gặp Linh Tinh</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>1502</v>
       </c>
-      <c r="B40" t="s">
-        <v>1545</v>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Sửu gặp Linh Tinh</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1503</v>
       </c>
-      <c r="B41" t="s">
-        <v>1546</v>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>Tham Lang, Vũ Khúc đồng cung Mệnh ở Mùi gặp Hỏa Tinh</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>1504</v>
       </c>
-      <c r="B42" t="s">
-        <v>1547</v>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Mùi gặp Hỏa Tinh</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1505</v>
       </c>
-      <c r="B43" t="s">
-        <v>1548</v>
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>Tham Lang, Vũ Khúc đồng cung Mệnh ở Mùi gặp Linh Tinh</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1506</v>
       </c>
-      <c r="B44" t="s">
-        <v>1549</v>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>Thiên Kiếp, Tham Lang, Vũ Khúc đồng cung Mệnh ở Mùi gặp Linh Tinh</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>1507</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>Hỏa Tinh toạ thủ cung Mệnh gặp Linh Tinh ở Thiên Di</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1463</v>
-      </c>
-      <c r="B46" t="s">
-        <v>1463</v>
+        <v>1508</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>Hỏa Tinh toạ thủ cung Mệnh đối xung Linh Tinh và gặp Kình Dương</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1507</v>
-      </c>
-      <c r="B47" t="s">
-        <v>1507</v>
+        <v>1509</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>Linh Tinh toạ thủ cung Mệnh gặp Hỏa Tinh ở Thiên Di</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1508</v>
-      </c>
-      <c r="B48" t="s">
-        <v>1508</v>
+        <v>1510</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>Linh Tinh toạ thủ cung Mệnh đối xung Hỏa Tinh và gặp Kình Dương</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1509</v>
-      </c>
-      <c r="B49" t="s">
-        <v>1509</v>
+        <v>1511</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>Hỏa Tinh, Linh Tinh đồng cung Mệnh</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1510</v>
-      </c>
-      <c r="B50" t="s">
-        <v>1510</v>
+        <v>1512</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>Hỏa Tinh toạ thủ cung Mệnh ở Hợi gặp Thiên Hình, Tham Lang</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1511</v>
-      </c>
-      <c r="B51" t="s">
-        <v>1511</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>1512</v>
-      </c>
-      <c r="B52" t="s">
-        <v>1512</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
         <v>1513</v>
       </c>
-      <c r="B53" t="s">
-        <v>1513</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>1514</v>
-      </c>
-      <c r="B54" t="s">
-        <v>1514</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>1515</v>
-      </c>
-      <c r="B55" t="s">
-        <v>1515</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>1516</v>
-      </c>
-      <c r="B56" t="s">
-        <v>1516</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>1517</v>
-      </c>
-      <c r="B57" t="s">
-        <v>1517</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>1518</v>
-      </c>
-      <c r="B58" t="s">
-        <v>1518</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>1519</v>
-      </c>
-      <c r="B59" t="s">
-        <v>1519</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>1520</v>
-      </c>
-      <c r="B60" t="s">
-        <v>1520</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>1521</v>
-      </c>
-      <c r="B61" t="s">
-        <v>1521</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>1522</v>
-      </c>
-      <c r="B62" t="s">
-        <v>1522</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>1523</v>
-      </c>
-      <c r="B63" t="s">
-        <v>1523</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>1524</v>
-      </c>
-      <c r="B64" t="s">
-        <v>1524</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>1525</v>
-      </c>
-      <c r="B65" t="s">
-        <v>1525</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>1526</v>
-      </c>
-      <c r="B66" t="s">
-        <v>1526</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>1527</v>
-      </c>
-      <c r="B67" t="s">
-        <v>1527</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>1528</v>
-      </c>
-      <c r="B68" t="s">
-        <v>1528</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>1529</v>
-      </c>
-      <c r="B69" t="s">
-        <v>1529</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>1530</v>
-      </c>
-      <c r="B70" t="s">
-        <v>1530</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>1531</v>
-      </c>
-      <c r="B71" t="s">
-        <v>1531</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>1532</v>
-      </c>
-      <c r="B72" t="s">
-        <v>1532</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>1533</v>
-      </c>
-      <c r="B73" t="s">
-        <v>1533</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>1534</v>
-      </c>
-      <c r="B74" t="s">
-        <v>1534</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>1535</v>
-      </c>
-      <c r="B75" t="s">
-        <v>1535</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>1536</v>
-      </c>
-      <c r="B76" t="s">
-        <v>1536</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>1537</v>
-      </c>
-      <c r="B77" t="s">
-        <v>1537</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>1538</v>
-      </c>
-      <c r="B78" t="s">
-        <v>1538</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>1539</v>
-      </c>
-      <c r="B79" t="s">
-        <v>1539</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>1540</v>
-      </c>
-      <c r="B80" t="s">
-        <v>1540</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>1541</v>
-      </c>
-      <c r="B81" t="s">
-        <v>1541</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>1542</v>
-      </c>
-      <c r="B82" t="s">
-        <v>1542</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>1543</v>
-      </c>
-      <c r="B83" t="s">
-        <v>1543</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>1544</v>
-      </c>
-      <c r="B84" t="s">
-        <v>1544</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>1545</v>
-      </c>
-      <c r="B85" t="s">
-        <v>1545</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>1546</v>
-      </c>
-      <c r="B86" t="s">
-        <v>1546</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>1547</v>
-      </c>
-      <c r="B87" t="s">
-        <v>1547</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>1548</v>
-      </c>
-      <c r="B88" t="s">
-        <v>1548</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>1549</v>
-      </c>
-      <c r="B89" t="s">
-        <v>1549</v>
+      <c r="B51" t="str">
+        <f t="shared" si="0"/>
+        <v>Linh Tinh toạ thủ cung Mệnh gặp Thiên Mã, Kình Dương, Đà La</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Luận An Lục đại bại tinh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE046B99-8A58-4C99-95FA-77F1611E56D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951F06FF-DC4E-4FAF-933B-583A98EAB127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3383" uniqueCount="1747">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3603" uniqueCount="1861">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -4916,189 +4916,6 @@
     <t>Hoá Lộc toạ thủ cung Mệnh</t>
   </si>
   <si>
-    <t>luanmenh.js:4737 Hoá Lộc toạ thủ cung Mệnh gặp Hóa Quyền, Hóa Khoa, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4740 Hoá Lộc toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Kình Dương, Đà La</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4743 Hoá Lộc toạ thủ cung Mệnh gặp Đào Hoa, Hồng Loan</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4746 Hoá Lộc toạ thủ cung Mệnh gặp Thiên Mã</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4749 Hoá Lộc toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4755 Hoá Quyền toạ thủ cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4758 Hoá Quyền toạ thủ cung Mệnh gặp Hóa Lộc, Hóa Khoa, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4761 Hoá Quyền toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Kình Dương, Đà La</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4764 Hoá Quyền toạ thủ cung Mệnh gặp Đào Hoa, Hồng Loan</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4767 Hoá Quyền toạ thủ cung Mệnh gặp Thiên Mã</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4770 Hoá Quyền toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4773 Hoá Quyền toạ thủ cung Mệnh gặp Tử Vi, Thiên Phủ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4776 Hoá Quyền toạ thủ cung Mệnh gặp Vũ Khúc, Cự Môn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4780 Hoá Quyền toạ thủ cung Mệnh gặp Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4785 Hoá Khoa toạ thủ cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4788 Hoá Khoa toạ thủ cung Mệnh gặp Hóa Lộc, Hóa Quyền, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4791 Hoá Khoa toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Kình Dương, Đà La</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4794 Hoá Khoa toạ thủ cung Mệnh gặp Đào Hoa, Hồng Loan</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4797 Hoá Khoa toạ thủ cung Mệnh gặp Thiên Mã</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4800 Hoá Khoa toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4804 Hoá Khoa toạ thủ cung Mệnh gặp Tử Vi, Thiên Phủ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4810 Hóa Kỵ toạ thủ cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4813 Hóa Kỵ toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Kình Dương, Đà La</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4816 Hóa Kỵ toạ thủ cung Mệnh gặp Đào Hoa, Hồng Loan</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4819 Hóa Kỵ toạ thủ cung Mệnh gặp Thiên Mã</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4822 Hóa Kỵ toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4825 Hóa Kỵ toạ thủ cung Mệnh gặp Thái Dương, Thái Âm</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4828 Hóa Kỵ toạ thủ cung Mệnh gặp Thái Dương, Thái Âm, Thiên Hình</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4831 Hóa Kỵ, Cự Môn đồng cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4834 Hóa Kỵ, Tham Lang đồng cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4837 Hóa Kỵ toạ thủ cung Mệnh gặp Tử Vi, Thiên Phủ</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4840 Hóa Kỵ toạ thủ cung Mệnh gặp Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4843 Hóa Kỵ toạ thủ cung Mệnh gặp Thiên Đồng, Thiên Lương</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4851 Hoá Lộc toạ thủ cung đồng cung Tham Lang, Vũ Khúc tại Mệnh ở Thìn</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4851 Hoá Lộc toạ thủ cung đồng cung Tham Lang, Vũ Khúc tại Mệnh ở Tuất</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4851 Hoá Lộc toạ thủ cung đồng cung Tham Lang, Vũ Khúc tại Mệnh ở Sửu</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4851 Hoá Lộc toạ thủ cung đồng cung Tham Lang, Vũ Khúc tại Mệnh ở Mùi</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4858 Người tuổiĐ. có Hoá Lộc toạ thủ cung Mệnh, Lộc Tồn toạ thủ cung Thiên Di</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4858 Người tuổiK. có Hoá Lộc toạ thủ cung Mệnh, Lộc Tồn toạ thủ cung Thiên Di</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4866 Người tuổiNgọ có Hoá Lộc, Thiên Lương đồng cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4866 Người tuổiThìn có Hoá Lộc, Thiên Lương đồng cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4866 Người tuổiTuất có Hoá Lộc, Thiên Lương đồng cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4873 Người tuổi Dần có Hoá Lộc toạ thủ cung Mệnh, Thiên Cơ, Thiên Lương, Lộc Tồn đồng cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4873 Người tuổi Thân có Hoá Lộc toạ thủ cung Mệnh, Thiên Cơ, Thiên Lương, Lộc Tồn đồng cung Mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4879 Hóa Quyền, Hóa Lộc đồng cung Mệnh không gặp Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4883 Hóa Quyền toạ thủ cung Mệnh gặp Hóa Lộc, không gặp Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4888 Hóa Lộc toạ thủ cung Mệnh gặp Hóa Quyền, không gặp Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4892 Hóa Quyền, Hóa Lộc giáp mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4896 Hóa Khoa toạ thủ cung Mệnh gặp Hóa Lộc, không gặp Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4900 Hóa Khoa, Hóa Lộc đồng cung Mệnh không gặp Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4904 Hóa Lộc toạ thủ cung Mệnh gặp Hóa Khoa, không gặp Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4908 Hóa Khoa, Hóa Lộc giáp mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4914 Hóa Khoa toạ thủ cung Mệnh gặp Hóa Lộc, không gặp Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4918 Hóa Khoa, Hóa Quyền đồng cung Mệnh không gặp Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4922 Hóa Khoa toạ thủ cung Mệnh gặp Hóa Quyền, không gặp Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4926 Hóa Khoa, Hóa Quyền giáp mệnh</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4931 Hóa Kỵ toạ thủ cung Mệnh gặp Hóa Lộc, Hóa Quyền, gặp Địa Không, Địa Kiếp</t>
-  </si>
-  <si>
-    <t>luanmenh.js:4935 Hóa Kỵ toạ thủ cung Mệnh gặp Hóa Lộc, Hóa Quyền, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">luanmenh.js:4941 Người tuổi Tý có Hóa Khoa toạ thủ cung Mệnh, gặp Thiên Đồng, Thiên Lương </t>
-  </si>
-  <si>
-    <t xml:space="preserve">luanmenh.js:4941 Người tuổi Ngọ có Hóa Khoa toạ thủ cung Mệnh, gặp Thiên Đồng, Thiên Lương </t>
-  </si>
-  <si>
-    <t>luanmenh.js:4947 Người tuổi Tý có Hóa Kỵ toạ thủ cung Mệnh, gặp Thiên Đồng, Thiên Lương</t>
-  </si>
-  <si>
     <t>Hoá Lộc toạ thủ cung Mệnh gặp Hóa Quyền, Hóa Khoa, Văn Xương, Văn Khúc</t>
   </si>
   <si>
@@ -5277,6 +5094,531 @@
   </si>
   <si>
     <t>Người tuổi Tý có Hóa Kỵ toạ thủ cung Mệnh, gặp Thiên Đồng, Thiên Lương</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Đại Hao tại Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5107 Người tuổi Dần có Đại Hao toạ thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5107 Người tuổi Thân có Tiểu Hao toạ thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5103 Cung Mệnh có Tiểu Hao tại Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5103 Cung Mệnh có undefined tại Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5103 Cung Mệnh có undefined tại Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5113 Cung Mệnh Vô Chính Diệu có Đại Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5113 Cung Mệnh Vô Chính Diệu có Tiểu Hao</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5121 Cung Mệnh có Tang Môn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5121 Cung Mệnh có Bạch Hổ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5130 Quý Chị có Tang Môn toạ thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5130 Quý Chị có Bạch Hổ toạ thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5137 Cung Mệnh có Tang Môn toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5140 Cung Mệnh có Tang Môn toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5143 Cung Mệnh có Tang Môn toạ thủ cung Mệnh gặp Kinh Dương, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5147 Cung Mệnh có Tang Môn đồng cung Tham Lang gặp Hỏa Tinh gặp Linh Tinh, Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5137 Cung Mệnh có Bạch Hổ toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5140 Cung Mệnh có Bạch Hổ toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5143 Cung Mệnh có Bạch Hổ toạ thủ cung Mệnh gặp Kinh Dương, Thiên Hình</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5147 Cung Mệnh có Bạch Hổ đồng cung Tham Lang gặp Hỏa Tinh gặp Linh Tinh, Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5154 Cung Mệnh có Bạch Hổ đồng cung Tấu Thư</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5157 Cung Mệnh có Bạch Hổ đồng cung Phi Liêm</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5171 Cung Mệnh có Thiên Khốc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5175 Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5178 Người tuổi Tý có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5175 Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5178 Người tuổi Ngọ có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5175 Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5178 Người tuổi Mão có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5175 Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5178 Người tuổi Dậu có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5175 Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5178 Người tuổi Sửu có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5175 Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5178 Người tuổi Mùi có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5171 Cung Mệnh có Thiên Hư</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5175 Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Tý</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5178 Người tuổi Tý có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5175 Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Ngọ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5178 Người tuổi Ngọ có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5175 Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Mão</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5178 Người tuổi Mão có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5175 Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Dậu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5178 Người tuổi Dậu có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5175 Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Sửu</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5178 Người tuổi Sửu có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5175 Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Mùi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5178 Người tuổi Mùi có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5188 Người tuổi Tý có Thiên Khốc toạ thủ cung Mệnh, gặp Kình Dương, Đà La, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5191 Người tuổi Tý có Thiên Khốc đồng cung Phá Quân tại Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5188 Người tuổi Ngọ có Thiên Khốc toạ thủ cung Mệnh, gặp Kình Dương, Đà La, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5191 Người tuổi Ngọ có Thiên Khốc đồng cung Phá Quân tại Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5188 Người tuổi Tý có Thiên Hư toạ thủ cung Mệnh, gặp Kình Dương, Đà La, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5191 Người tuổi Tý có Thiên Hư đồng cung Phá Quân tại Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5188 Người tuổi Ngọ có Thiên Hư toạ thủ cung Mệnh, gặp Kình Dương, Đà La, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5191 Người tuổi Ngọ có Thiên Hư đồng cung Phá Quân tại Mệnh</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5199 Cung Mệnh có Dần</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5203 Người tuổi Dần có Dần toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5206 Người tuổi Dần có Dần toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5203 Người tuổi Thân có Dần toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5206 Người tuổi Thân có Dần toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5199 Cung Mệnh có Thân</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5203 Người tuổi Dần có Thân toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5206 Người tuổi Dần có Thân toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5203 Người tuổi Thân có Thân toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5206 Người tuổi Thân có Thân toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5199 Cung Mệnh có Tỵ</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5203 Người tuổi Dần có Tỵ toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5206 Người tuổi Dần có Tỵ toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5203 Người tuổi Thân có Tỵ toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5206 Người tuổi Thân có Tỵ toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5199 Cung Mệnh có Hợi</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5203 Người tuổi Dần có Hợi toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5206 Người tuổi Dần có Hợi toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5203 Người tuổi Thân có Hợi toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5206 Người tuổi Thân có Hợi toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5199 Cung Mệnh có Thìn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5203 Người tuổi Dần có Thìn toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5206 Người tuổi Dần có Thìn toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5203 Người tuổi Thân có Thìn toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5206 Người tuổi Thân có Thìn toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5199 Cung Mệnh có Tuất</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5203 Người tuổi Dần có Tuất toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5206 Người tuổi Dần có Tuất toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5203 Người tuổi Thân có Tuất toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5206 Người tuổi Thân có Tuất toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5215 Cung Mệnh có Mão toạ thủ cung Mệnh gặp Thiên Cơ, Cự Môn</t>
+  </si>
+  <si>
+    <t>luanmenh.js:5215 Cung Mệnh có Dậu toạ thủ cung Mệnh gặp Thiên Cơ, Cự Môn</t>
+  </si>
+  <si>
+    <t>Người tuổi Dần có Đại Hao toạ thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>Người tuổi Thân có Tiểu Hao toạ thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Tiểu Hao tại Thân</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có undefined tại Mão</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có undefined tại Dậu</t>
+  </si>
+  <si>
+    <t>Cung Mệnh Vô Chính Diệu có Đại Hao</t>
+  </si>
+  <si>
+    <t>Cung Mệnh Vô Chính Diệu có Tiểu Hao</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Tang Môn</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Bạch Hổ</t>
+  </si>
+  <si>
+    <t>Quý Chị có Tang Môn toạ thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>Quý Chị có Bạch Hổ toạ thủ cung Mệnh</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Tang Môn toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Tang Môn toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Tang Môn toạ thủ cung Mệnh gặp Kinh Dương, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Tang Môn đồng cung Tham Lang gặp Hỏa Tinh gặp Linh Tinh, Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Bạch Hổ toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Bạch Hổ toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Bạch Hổ toạ thủ cung Mệnh gặp Kinh Dương, Thiên Hình</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Bạch Hổ đồng cung Tham Lang gặp Hỏa Tinh gặp Linh Tinh, Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Bạch Hổ đồng cung Tấu Thư</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Bạch Hổ đồng cung Phi Liêm</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Thiên Khốc</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Tý</t>
+  </si>
+  <si>
+    <t>Người tuổi Tý có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Ngọ</t>
+  </si>
+  <si>
+    <t>Người tuổi Ngọ có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Mão</t>
+  </si>
+  <si>
+    <t>Người tuổi Mão có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Dậu</t>
+  </si>
+  <si>
+    <t>Người tuổi Dậu có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Sửu</t>
+  </si>
+  <si>
+    <t>Người tuổi Sửu có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Mùi</t>
+  </si>
+  <si>
+    <t>Người tuổi Mùi có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Thiên Hư</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Tý</t>
+  </si>
+  <si>
+    <t>Người tuổi Tý có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Ngọ</t>
+  </si>
+  <si>
+    <t>Người tuổi Ngọ có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Mão</t>
+  </si>
+  <si>
+    <t>Người tuổi Mão có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Dậu</t>
+  </si>
+  <si>
+    <t>Người tuổi Dậu có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Sửu</t>
+  </si>
+  <si>
+    <t>Người tuổi Sửu có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Mùi</t>
+  </si>
+  <si>
+    <t>Người tuổi Mùi có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</t>
+  </si>
+  <si>
+    <t>Người tuổi Tý có Thiên Khốc toạ thủ cung Mệnh, gặp Kình Dương, Đà La, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Người tuổi Tý có Thiên Khốc đồng cung Phá Quân tại Mệnh</t>
+  </si>
+  <si>
+    <t>Người tuổi Ngọ có Thiên Khốc toạ thủ cung Mệnh, gặp Kình Dương, Đà La, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Người tuổi Ngọ có Thiên Khốc đồng cung Phá Quân tại Mệnh</t>
+  </si>
+  <si>
+    <t>Người tuổi Tý có Thiên Hư toạ thủ cung Mệnh, gặp Kình Dương, Đà La, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Người tuổi Tý có Thiên Hư đồng cung Phá Quân tại Mệnh</t>
+  </si>
+  <si>
+    <t>Người tuổi Ngọ có Thiên Hư toạ thủ cung Mệnh, gặp Kình Dương, Đà La, Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Người tuổi Ngọ có Thiên Hư đồng cung Phá Quân tại Mệnh</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Dần</t>
+  </si>
+  <si>
+    <t>Người tuổi Dần có Dần toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Người tuổi Dần có Dần toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>Người tuổi Thân có Dần toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Người tuổi Thân có Dần toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Thân</t>
+  </si>
+  <si>
+    <t>Người tuổi Dần có Thân toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Người tuổi Dần có Thân toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>Người tuổi Thân có Thân toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Người tuổi Thân có Thân toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Tỵ</t>
+  </si>
+  <si>
+    <t>Người tuổi Dần có Tỵ toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Người tuổi Dần có Tỵ toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>Người tuổi Thân có Tỵ toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Người tuổi Thân có Tỵ toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Hợi</t>
+  </si>
+  <si>
+    <t>Người tuổi Dần có Hợi toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Người tuổi Dần có Hợi toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>Người tuổi Thân có Hợi toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Người tuổi Thân có Hợi toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Thìn</t>
+  </si>
+  <si>
+    <t>Người tuổi Dần có Thìn toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Người tuổi Dần có Thìn toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>Người tuổi Thân có Thìn toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Người tuổi Thân có Thìn toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Tuất</t>
+  </si>
+  <si>
+    <t>Người tuổi Dần có Tuất toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Người tuổi Dần có Tuất toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>Người tuổi Thân có Tuất toạ thủ cung Mệnh, gặp Kình Dương, Đà La</t>
+  </si>
+  <si>
+    <t>Người tuổi Thân có Tuất toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Mão toạ thủ cung Mệnh gặp Thiên Cơ, Cự Môn</t>
+  </si>
+  <si>
+    <t>Cung Mệnh có Dậu toạ thủ cung Mệnh gặp Thiên Cơ, Cự Môn</t>
   </si>
 </sst>
 </file>
@@ -5325,7 +5667,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="31">
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -7396,10 +7758,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B1535"/>
+  <dimension ref="A1:B1630"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1468" workbookViewId="0">
-      <selection activeCell="B1474" sqref="B1474:B1535"/>
+    <sheetView tabSelected="1" topLeftCell="A1621" workbookViewId="0">
+      <selection activeCell="B1537" sqref="B1537:B1630"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18795,556 +19157,1312 @@
     </row>
     <row r="1475" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1475" t="s">
-        <v>1687</v>
+        <v>1626</v>
       </c>
       <c r="B1475" t="s">
-        <v>1687</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="1476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1476" t="s">
-        <v>1688</v>
+        <v>1627</v>
       </c>
       <c r="B1476" t="s">
-        <v>1688</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="1477" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1477" t="s">
-        <v>1689</v>
+        <v>1628</v>
       </c>
       <c r="B1477" t="s">
-        <v>1689</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="1478" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1478" t="s">
-        <v>1690</v>
+        <v>1629</v>
       </c>
       <c r="B1478" t="s">
-        <v>1690</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="1479" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1479" t="s">
-        <v>1691</v>
+        <v>1630</v>
       </c>
       <c r="B1479" t="s">
-        <v>1691</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="1480" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1480" t="s">
-        <v>1692</v>
+        <v>1631</v>
       </c>
       <c r="B1480" t="s">
-        <v>1692</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="1481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1481" t="s">
-        <v>1693</v>
+        <v>1632</v>
       </c>
       <c r="B1481" t="s">
-        <v>1693</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="1482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1482" t="s">
-        <v>1694</v>
+        <v>1633</v>
       </c>
       <c r="B1482" t="s">
-        <v>1694</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="1483" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1483" t="s">
-        <v>1695</v>
+        <v>1634</v>
       </c>
       <c r="B1483" t="s">
-        <v>1695</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="1484" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1484" t="s">
-        <v>1696</v>
+        <v>1635</v>
       </c>
       <c r="B1484" t="s">
-        <v>1696</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="1485" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1485" t="s">
-        <v>1697</v>
+        <v>1636</v>
       </c>
       <c r="B1485" t="s">
-        <v>1697</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="1486" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1486" t="s">
-        <v>1698</v>
+        <v>1637</v>
       </c>
       <c r="B1486" t="s">
-        <v>1698</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="1487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1487" t="s">
-        <v>1699</v>
+        <v>1638</v>
       </c>
       <c r="B1487" t="s">
-        <v>1699</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="1488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1488" t="s">
-        <v>1700</v>
+        <v>1639</v>
       </c>
       <c r="B1488" t="s">
-        <v>1700</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="1489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1489" t="s">
-        <v>1701</v>
+        <v>1640</v>
       </c>
       <c r="B1489" t="s">
-        <v>1701</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="1490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1490" t="s">
-        <v>1702</v>
+        <v>1641</v>
       </c>
       <c r="B1490" t="s">
-        <v>1702</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="1491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1491" t="s">
-        <v>1703</v>
+        <v>1642</v>
       </c>
       <c r="B1491" t="s">
-        <v>1703</v>
+        <v>1642</v>
       </c>
     </row>
     <row r="1492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1492" t="s">
-        <v>1704</v>
+        <v>1643</v>
       </c>
       <c r="B1492" t="s">
-        <v>1704</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="1493" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1493" t="s">
-        <v>1705</v>
+        <v>1644</v>
       </c>
       <c r="B1493" t="s">
-        <v>1705</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="1494" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1494" t="s">
-        <v>1706</v>
+        <v>1645</v>
       </c>
       <c r="B1494" t="s">
-        <v>1706</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="1495" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1495" t="s">
-        <v>1707</v>
+        <v>1646</v>
       </c>
       <c r="B1495" t="s">
-        <v>1707</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="1496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1496" t="s">
-        <v>1708</v>
+        <v>1647</v>
       </c>
       <c r="B1496" t="s">
-        <v>1708</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="1497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1497" t="s">
-        <v>1709</v>
+        <v>1648</v>
       </c>
       <c r="B1497" t="s">
-        <v>1709</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="1498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1498" t="s">
-        <v>1710</v>
+        <v>1649</v>
       </c>
       <c r="B1498" t="s">
-        <v>1710</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="1499" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1499" t="s">
-        <v>1711</v>
+        <v>1650</v>
       </c>
       <c r="B1499" t="s">
-        <v>1711</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="1500" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1500" t="s">
-        <v>1712</v>
+        <v>1651</v>
       </c>
       <c r="B1500" t="s">
-        <v>1712</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="1501" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1501" t="s">
-        <v>1713</v>
+        <v>1652</v>
       </c>
       <c r="B1501" t="s">
-        <v>1713</v>
+        <v>1652</v>
       </c>
     </row>
     <row r="1502" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1502" t="s">
-        <v>1714</v>
+        <v>1653</v>
       </c>
       <c r="B1502" t="s">
-        <v>1714</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="1503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1503" t="s">
-        <v>1715</v>
+        <v>1654</v>
       </c>
       <c r="B1503" t="s">
-        <v>1715</v>
+        <v>1654</v>
       </c>
     </row>
     <row r="1504" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1504" t="s">
-        <v>1716</v>
+        <v>1655</v>
       </c>
       <c r="B1504" t="s">
-        <v>1716</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="1505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1505" t="s">
-        <v>1717</v>
+        <v>1656</v>
       </c>
       <c r="B1505" t="s">
-        <v>1717</v>
+        <v>1656</v>
       </c>
     </row>
     <row r="1506" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1506" t="s">
-        <v>1718</v>
+        <v>1657</v>
       </c>
       <c r="B1506" t="s">
-        <v>1718</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="1507" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1507" t="s">
-        <v>1719</v>
+        <v>1658</v>
       </c>
       <c r="B1507" t="s">
-        <v>1719</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="1508" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1508" t="s">
-        <v>1720</v>
+        <v>1659</v>
       </c>
       <c r="B1508" t="s">
-        <v>1720</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="1509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1509" t="s">
-        <v>1721</v>
+        <v>1660</v>
       </c>
       <c r="B1509" t="s">
-        <v>1721</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="1510" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1510" t="s">
-        <v>1722</v>
+        <v>1661</v>
       </c>
       <c r="B1510" t="s">
-        <v>1722</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="1511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1511" t="s">
-        <v>1723</v>
+        <v>1662</v>
       </c>
       <c r="B1511" t="s">
-        <v>1723</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="1512" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1512" t="s">
-        <v>1724</v>
+        <v>1663</v>
       </c>
       <c r="B1512" t="s">
-        <v>1724</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="1513" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1513" t="s">
-        <v>1725</v>
+        <v>1664</v>
       </c>
       <c r="B1513" t="s">
-        <v>1725</v>
+        <v>1664</v>
       </c>
     </row>
     <row r="1514" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1514" t="s">
-        <v>1726</v>
+        <v>1665</v>
       </c>
       <c r="B1514" t="s">
-        <v>1726</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="1515" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1515" t="s">
-        <v>1727</v>
+        <v>1666</v>
       </c>
       <c r="B1515" t="s">
-        <v>1727</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="1516" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1516" t="s">
-        <v>1728</v>
+        <v>1667</v>
       </c>
       <c r="B1516" t="s">
-        <v>1728</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="1517" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1517" t="s">
-        <v>1729</v>
+        <v>1668</v>
       </c>
       <c r="B1517" t="s">
-        <v>1729</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="1518" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1518" t="s">
-        <v>1730</v>
+        <v>1669</v>
       </c>
       <c r="B1518" t="s">
-        <v>1730</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="1519" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1519" t="s">
-        <v>1731</v>
+        <v>1670</v>
       </c>
       <c r="B1519" t="s">
-        <v>1731</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="1520" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1520" t="s">
-        <v>1732</v>
+        <v>1671</v>
       </c>
       <c r="B1520" t="s">
-        <v>1732</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="1521" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1521" t="s">
-        <v>1733</v>
+        <v>1672</v>
       </c>
       <c r="B1521" t="s">
-        <v>1733</v>
+        <v>1672</v>
       </c>
     </row>
     <row r="1522" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1522" t="s">
-        <v>1734</v>
+        <v>1673</v>
       </c>
       <c r="B1522" t="s">
-        <v>1734</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="1523" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1523" t="s">
-        <v>1735</v>
+        <v>1674</v>
       </c>
       <c r="B1523" t="s">
-        <v>1735</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="1524" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1524" t="s">
-        <v>1736</v>
+        <v>1675</v>
       </c>
       <c r="B1524" t="s">
-        <v>1736</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="1525" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1525" t="s">
-        <v>1737</v>
+        <v>1676</v>
       </c>
       <c r="B1525" t="s">
-        <v>1737</v>
+        <v>1676</v>
       </c>
     </row>
     <row r="1526" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1526" t="s">
-        <v>1738</v>
+        <v>1677</v>
       </c>
       <c r="B1526" t="s">
-        <v>1738</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="1527" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1527" t="s">
-        <v>1735</v>
+        <v>1674</v>
       </c>
       <c r="B1527" t="s">
-        <v>1735</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="1528" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1528" t="s">
-        <v>1739</v>
+        <v>1678</v>
       </c>
       <c r="B1528" t="s">
-        <v>1739</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="1529" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1529" t="s">
-        <v>1740</v>
+        <v>1679</v>
       </c>
       <c r="B1529" t="s">
-        <v>1740</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="1530" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1530" t="s">
-        <v>1741</v>
+        <v>1680</v>
       </c>
       <c r="B1530" t="s">
-        <v>1741</v>
+        <v>1680</v>
       </c>
     </row>
     <row r="1531" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1531" t="s">
-        <v>1742</v>
+        <v>1681</v>
       </c>
       <c r="B1531" t="s">
-        <v>1742</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="1532" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1532" t="s">
-        <v>1743</v>
+        <v>1682</v>
       </c>
       <c r="B1532" t="s">
-        <v>1743</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="1533" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1533" t="s">
-        <v>1744</v>
+        <v>1683</v>
       </c>
       <c r="B1533" t="s">
-        <v>1744</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="1534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1534" t="s">
-        <v>1745</v>
+        <v>1684</v>
       </c>
       <c r="B1534" t="s">
-        <v>1745</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="1535" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1535" t="s">
-        <v>1746</v>
+        <v>1685</v>
       </c>
       <c r="B1535" t="s">
-        <v>1746</v>
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="1537" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1537" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B1537" t="s">
+        <v>1686</v>
+      </c>
+    </row>
+    <row r="1538" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1538" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B1538" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="1539" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1539" t="s">
+        <v>1775</v>
+      </c>
+      <c r="B1539" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="1540" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1540" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B1540" t="s">
+        <v>1776</v>
+      </c>
+    </row>
+    <row r="1541" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1541" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B1541" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="1542" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1542" t="s">
+        <v>1775</v>
+      </c>
+      <c r="B1542" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="1543" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1543" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B1543" t="s">
+        <v>1777</v>
+      </c>
+    </row>
+    <row r="1544" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1544" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B1544" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="1545" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1545" t="s">
+        <v>1775</v>
+      </c>
+      <c r="B1545" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="1546" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1546" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B1546" t="s">
+        <v>1778</v>
+      </c>
+    </row>
+    <row r="1547" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1547" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B1547" t="s">
+        <v>1774</v>
+      </c>
+    </row>
+    <row r="1548" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1548" t="s">
+        <v>1775</v>
+      </c>
+      <c r="B1548" t="s">
+        <v>1775</v>
+      </c>
+    </row>
+    <row r="1549" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1549" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B1549" t="s">
+        <v>1779</v>
+      </c>
+    </row>
+    <row r="1550" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1550" t="s">
+        <v>1780</v>
+      </c>
+      <c r="B1550" t="s">
+        <v>1780</v>
+      </c>
+    </row>
+    <row r="1551" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1551" t="s">
+        <v>1781</v>
+      </c>
+      <c r="B1551" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="1552" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1552" t="s">
+        <v>1782</v>
+      </c>
+      <c r="B1552" t="s">
+        <v>1782</v>
+      </c>
+    </row>
+    <row r="1553" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1553" t="s">
+        <v>1783</v>
+      </c>
+      <c r="B1553" t="s">
+        <v>1783</v>
+      </c>
+    </row>
+    <row r="1554" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1554" t="s">
+        <v>1784</v>
+      </c>
+      <c r="B1554" t="s">
+        <v>1784</v>
+      </c>
+    </row>
+    <row r="1555" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1555" t="s">
+        <v>1785</v>
+      </c>
+      <c r="B1555" t="s">
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="1556" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1556" t="s">
+        <v>1786</v>
+      </c>
+      <c r="B1556" t="s">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="1557" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1557" t="s">
+        <v>1787</v>
+      </c>
+      <c r="B1557" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="1558" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1558" t="s">
+        <v>1788</v>
+      </c>
+      <c r="B1558" t="s">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="1559" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1559" t="s">
+        <v>1789</v>
+      </c>
+      <c r="B1559" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1560" t="s">
+        <v>1790</v>
+      </c>
+      <c r="B1560" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1561" t="s">
+        <v>1791</v>
+      </c>
+      <c r="B1561" t="s">
+        <v>1791</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1562" t="s">
+        <v>1792</v>
+      </c>
+      <c r="B1562" t="s">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1563" t="s">
+        <v>1793</v>
+      </c>
+      <c r="B1563" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1564" t="s">
+        <v>1794</v>
+      </c>
+      <c r="B1564" t="s">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="1565" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1565" t="s">
+        <v>1795</v>
+      </c>
+      <c r="B1565" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="1566" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1566" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B1566" t="s">
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="1567" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1567" t="s">
+        <v>1797</v>
+      </c>
+      <c r="B1567" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="1568" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1568" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B1568" t="s">
+        <v>1798</v>
+      </c>
+    </row>
+    <row r="1569" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1569" t="s">
+        <v>1799</v>
+      </c>
+      <c r="B1569" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1570" t="s">
+        <v>1800</v>
+      </c>
+      <c r="B1570" t="s">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1571" t="s">
+        <v>1801</v>
+      </c>
+      <c r="B1571" t="s">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1572" t="s">
+        <v>1802</v>
+      </c>
+      <c r="B1572" t="s">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="1573" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1573" t="s">
+        <v>1803</v>
+      </c>
+      <c r="B1573" t="s">
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1574" t="s">
+        <v>1804</v>
+      </c>
+      <c r="B1574" t="s">
+        <v>1804</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1575" t="s">
+        <v>1805</v>
+      </c>
+      <c r="B1575" t="s">
+        <v>1805</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1576" t="s">
+        <v>1806</v>
+      </c>
+      <c r="B1576" t="s">
+        <v>1806</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1577" t="s">
+        <v>1807</v>
+      </c>
+      <c r="B1577" t="s">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="1578" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1578" t="s">
+        <v>1808</v>
+      </c>
+      <c r="B1578" t="s">
+        <v>1808</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1579" t="s">
+        <v>1809</v>
+      </c>
+      <c r="B1579" t="s">
+        <v>1809</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1580" t="s">
+        <v>1810</v>
+      </c>
+      <c r="B1580" t="s">
+        <v>1810</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1581" t="s">
+        <v>1811</v>
+      </c>
+      <c r="B1581" t="s">
+        <v>1811</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1582" t="s">
+        <v>1812</v>
+      </c>
+      <c r="B1582" t="s">
+        <v>1812</v>
+      </c>
+    </row>
+    <row r="1583" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1583" t="s">
+        <v>1813</v>
+      </c>
+      <c r="B1583" t="s">
+        <v>1813</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1584" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B1584" t="s">
+        <v>1814</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1585" t="s">
+        <v>1815</v>
+      </c>
+      <c r="B1585" t="s">
+        <v>1815</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1586" t="s">
+        <v>1816</v>
+      </c>
+      <c r="B1586" t="s">
+        <v>1816</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1587" t="s">
+        <v>1817</v>
+      </c>
+      <c r="B1587" t="s">
+        <v>1817</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1588" t="s">
+        <v>1818</v>
+      </c>
+      <c r="B1588" t="s">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="1589" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1589" t="s">
+        <v>1819</v>
+      </c>
+      <c r="B1589" t="s">
+        <v>1819</v>
+      </c>
+    </row>
+    <row r="1590" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1590" t="s">
+        <v>1820</v>
+      </c>
+      <c r="B1590" t="s">
+        <v>1820</v>
+      </c>
+    </row>
+    <row r="1591" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1591" t="s">
+        <v>1821</v>
+      </c>
+      <c r="B1591" t="s">
+        <v>1821</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1592" t="s">
+        <v>1822</v>
+      </c>
+      <c r="B1592" t="s">
+        <v>1822</v>
+      </c>
+    </row>
+    <row r="1593" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1593" t="s">
+        <v>1823</v>
+      </c>
+      <c r="B1593" t="s">
+        <v>1823</v>
+      </c>
+    </row>
+    <row r="1594" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1594" t="s">
+        <v>1824</v>
+      </c>
+      <c r="B1594" t="s">
+        <v>1824</v>
+      </c>
+    </row>
+    <row r="1595" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1595" t="s">
+        <v>1825</v>
+      </c>
+      <c r="B1595" t="s">
+        <v>1825</v>
+      </c>
+    </row>
+    <row r="1596" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1596" t="s">
+        <v>1826</v>
+      </c>
+      <c r="B1596" t="s">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="1597" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1597" t="s">
+        <v>1827</v>
+      </c>
+      <c r="B1597" t="s">
+        <v>1827</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1598" t="s">
+        <v>1828</v>
+      </c>
+      <c r="B1598" t="s">
+        <v>1828</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1599" t="s">
+        <v>1829</v>
+      </c>
+      <c r="B1599" t="s">
+        <v>1829</v>
+      </c>
+    </row>
+    <row r="1600" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1600" t="s">
+        <v>1830</v>
+      </c>
+      <c r="B1600" t="s">
+        <v>1830</v>
+      </c>
+    </row>
+    <row r="1601" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1601" t="s">
+        <v>1831</v>
+      </c>
+      <c r="B1601" t="s">
+        <v>1831</v>
+      </c>
+    </row>
+    <row r="1602" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1602" t="s">
+        <v>1832</v>
+      </c>
+      <c r="B1602" t="s">
+        <v>1832</v>
+      </c>
+    </row>
+    <row r="1603" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1603" t="s">
+        <v>1833</v>
+      </c>
+      <c r="B1603" t="s">
+        <v>1833</v>
+      </c>
+    </row>
+    <row r="1604" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1604" t="s">
+        <v>1834</v>
+      </c>
+      <c r="B1604" t="s">
+        <v>1834</v>
+      </c>
+    </row>
+    <row r="1605" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1605" t="s">
+        <v>1835</v>
+      </c>
+      <c r="B1605" t="s">
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="1606" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1606" t="s">
+        <v>1836</v>
+      </c>
+      <c r="B1606" t="s">
+        <v>1836</v>
+      </c>
+    </row>
+    <row r="1607" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1607" t="s">
+        <v>1837</v>
+      </c>
+      <c r="B1607" t="s">
+        <v>1837</v>
+      </c>
+    </row>
+    <row r="1608" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1608" t="s">
+        <v>1838</v>
+      </c>
+      <c r="B1608" t="s">
+        <v>1838</v>
+      </c>
+    </row>
+    <row r="1609" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1609" t="s">
+        <v>1839</v>
+      </c>
+      <c r="B1609" t="s">
+        <v>1839</v>
+      </c>
+    </row>
+    <row r="1610" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1610" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B1610" t="s">
+        <v>1840</v>
+      </c>
+    </row>
+    <row r="1611" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1611" t="s">
+        <v>1841</v>
+      </c>
+      <c r="B1611" t="s">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="1612" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1612" t="s">
+        <v>1842</v>
+      </c>
+      <c r="B1612" t="s">
+        <v>1842</v>
+      </c>
+    </row>
+    <row r="1613" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1613" t="s">
+        <v>1843</v>
+      </c>
+      <c r="B1613" t="s">
+        <v>1843</v>
+      </c>
+    </row>
+    <row r="1614" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1614" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B1614" t="s">
+        <v>1844</v>
+      </c>
+    </row>
+    <row r="1615" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1615" t="s">
+        <v>1845</v>
+      </c>
+      <c r="B1615" t="s">
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="1616" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1616" t="s">
+        <v>1846</v>
+      </c>
+      <c r="B1616" t="s">
+        <v>1846</v>
+      </c>
+    </row>
+    <row r="1617" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1617" t="s">
+        <v>1847</v>
+      </c>
+      <c r="B1617" t="s">
+        <v>1847</v>
+      </c>
+    </row>
+    <row r="1618" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1618" t="s">
+        <v>1848</v>
+      </c>
+      <c r="B1618" t="s">
+        <v>1848</v>
+      </c>
+    </row>
+    <row r="1619" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1619" t="s">
+        <v>1849</v>
+      </c>
+      <c r="B1619" t="s">
+        <v>1849</v>
+      </c>
+    </row>
+    <row r="1620" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1620" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B1620" t="s">
+        <v>1850</v>
+      </c>
+    </row>
+    <row r="1621" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1621" t="s">
+        <v>1851</v>
+      </c>
+      <c r="B1621" t="s">
+        <v>1851</v>
+      </c>
+    </row>
+    <row r="1622" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1622" t="s">
+        <v>1852</v>
+      </c>
+      <c r="B1622" t="s">
+        <v>1852</v>
+      </c>
+    </row>
+    <row r="1623" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1623" t="s">
+        <v>1853</v>
+      </c>
+      <c r="B1623" t="s">
+        <v>1853</v>
+      </c>
+    </row>
+    <row r="1624" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1624" t="s">
+        <v>1854</v>
+      </c>
+      <c r="B1624" t="s">
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="1625" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1625" t="s">
+        <v>1855</v>
+      </c>
+      <c r="B1625" t="s">
+        <v>1855</v>
+      </c>
+    </row>
+    <row r="1626" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1626" t="s">
+        <v>1856</v>
+      </c>
+      <c r="B1626" t="s">
+        <v>1856</v>
+      </c>
+    </row>
+    <row r="1627" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1627" t="s">
+        <v>1857</v>
+      </c>
+      <c r="B1627" t="s">
+        <v>1857</v>
+      </c>
+    </row>
+    <row r="1628" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1628" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B1628" t="s">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="1629" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1629" t="s">
+        <v>1859</v>
+      </c>
+      <c r="B1629" t="s">
+        <v>1859</v>
+      </c>
+    </row>
+    <row r="1630" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1630" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B1630" t="s">
+        <v>1860</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="30" priority="38"/>
-    <cfRule type="duplicateValues" dxfId="29" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="28" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="27" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="26" priority="12"/>
-    <cfRule type="duplicateValues" dxfId="25" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145:A208">
-    <cfRule type="duplicateValues" dxfId="24" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A209:A1048576 A1:A23 A25:A84 A143">
-    <cfRule type="duplicateValues" dxfId="23" priority="47"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="21" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
+    <cfRule type="duplicateValues" dxfId="22" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="38"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
     <cfRule type="duplicateValues" dxfId="20" priority="35"/>
     <cfRule type="duplicateValues" dxfId="19" priority="36"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
+  <conditionalFormatting sqref="B29">
     <cfRule type="duplicateValues" dxfId="18" priority="33"/>
     <cfRule type="duplicateValues" dxfId="17" priority="34"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
+  <conditionalFormatting sqref="B30">
     <cfRule type="duplicateValues" dxfId="16" priority="31"/>
     <cfRule type="duplicateValues" dxfId="15" priority="32"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30">
-    <cfRule type="duplicateValues" dxfId="14" priority="29"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="30"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B84:B142">
-    <cfRule type="duplicateValues" dxfId="12" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="11" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B143">
-    <cfRule type="duplicateValues" dxfId="10" priority="60"/>
-    <cfRule type="duplicateValues" dxfId="9" priority="61"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="62"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="8" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="7" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B325:B401">
-    <cfRule type="duplicateValues" dxfId="6" priority="136"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="137"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="138"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="139"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B402:B1259 B1:B23 B25 B28 B31:B83 B145:B324 B1275:B1473 B1536:B1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="46"/>
+  <conditionalFormatting sqref="B402:B1259 B1:B23 B25 B28 B31:B83 B145:B324 B1275:B1473 B1536 B1631:B1048576">
+    <cfRule type="duplicateValues" dxfId="6" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1260:B1274">
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1474:B1535">
     <cfRule type="duplicateValues" dxfId="3" priority="3"/>
     <cfRule type="duplicateValues" dxfId="2" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1474:B1535">
+  <conditionalFormatting sqref="B1537:B1630">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
@@ -19355,570 +20473,858 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FBE4172-FC39-45CE-BD67-BA23D6FB1A86}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:B94"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B62"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1625</v>
+        <v>1686</v>
       </c>
       <c r="B1" t="str">
         <f>A1</f>
-        <v>Hoá Lộc toạ thủ cung Mệnh</v>
+        <v>Cung Mệnh có Đại Hao tại Dần</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1626</v>
+        <v>1687</v>
       </c>
       <c r="B2" t="str">
         <f>RIGHT(A2,LEN(A2)-17)</f>
-        <v>Hoá Lộc toạ thủ cung Mệnh gặp Hóa Quyền, Hóa Khoa, Văn Xương, Văn Khúc</v>
+        <v>Người tuổi Dần có Đại Hao toạ thủ cung Mệnh</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1627</v>
+        <v>1688</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B62" si="0">RIGHT(A3,LEN(A3)-17)</f>
-        <v>Hoá Lộc toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Kình Dương, Đà La</v>
+        <f t="shared" ref="B3:B66" si="0">RIGHT(A3,LEN(A3)-17)</f>
+        <v>Người tuổi Thân có Tiểu Hao toạ thủ cung Mệnh</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1628</v>
+        <v>1689</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Lộc toạ thủ cung Mệnh gặp Đào Hoa, Hồng Loan</v>
+        <v>Cung Mệnh có Tiểu Hao tại Thân</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1629</v>
+        <v>1687</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Lộc toạ thủ cung Mệnh gặp Thiên Mã</v>
+        <v>Người tuổi Dần có Đại Hao toạ thủ cung Mệnh</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1630</v>
+        <v>1688</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Lộc toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp</v>
+        <v>Người tuổi Thân có Tiểu Hao toạ thủ cung Mệnh</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1631</v>
+        <v>1690</v>
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Quyền toạ thủ cung Mệnh</v>
+        <v>Cung Mệnh có undefined tại Mão</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>1632</v>
+        <v>1687</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Quyền toạ thủ cung Mệnh gặp Hóa Lộc, Hóa Khoa, Văn Xương, Văn Khúc</v>
+        <v>Người tuổi Dần có Đại Hao toạ thủ cung Mệnh</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1633</v>
+        <v>1688</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Quyền toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Kình Dương, Đà La</v>
+        <v>Người tuổi Thân có Tiểu Hao toạ thủ cung Mệnh</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>1634</v>
+        <v>1691</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Quyền toạ thủ cung Mệnh gặp Đào Hoa, Hồng Loan</v>
+        <v>Cung Mệnh có undefined tại Dậu</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1635</v>
+        <v>1687</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Quyền toạ thủ cung Mệnh gặp Thiên Mã</v>
+        <v>Người tuổi Dần có Đại Hao toạ thủ cung Mệnh</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>1636</v>
+        <v>1688</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Quyền toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp</v>
+        <v>Người tuổi Thân có Tiểu Hao toạ thủ cung Mệnh</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1637</v>
+        <v>1692</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Quyền toạ thủ cung Mệnh gặp Tử Vi, Thiên Phủ</v>
+        <v>Cung Mệnh Vô Chính Diệu có Đại Hao</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>1638</v>
+        <v>1693</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Quyền toạ thủ cung Mệnh gặp Vũ Khúc, Cự Môn</v>
+        <v>Cung Mệnh Vô Chính Diệu có Tiểu Hao</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1639</v>
+        <v>1694</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Quyền toạ thủ cung Mệnh gặp Kình Dương, Đà La, Địa Kiếp, Địa Không, Hỏa Tinh, Linh Tinh</v>
+        <v>Cung Mệnh có Tang Môn</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>1640</v>
+        <v>1695</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Khoa toạ thủ cung Mệnh</v>
+        <v>Cung Mệnh có Bạch Hổ</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1641</v>
+        <v>1696</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Khoa toạ thủ cung Mệnh gặp Hóa Lộc, Hóa Quyền, Văn Xương, Văn Khúc</v>
+        <v>Quý Chị có Tang Môn toạ thủ cung Mệnh</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1642</v>
+        <v>1697</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Khoa toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Kình Dương, Đà La</v>
+        <v>Quý Chị có Bạch Hổ toạ thủ cung Mệnh</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1643</v>
+        <v>1698</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Khoa toạ thủ cung Mệnh gặp Đào Hoa, Hồng Loan</v>
+        <v>Cung Mệnh có Tang Môn toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Kình Dương, Đà La</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>1644</v>
+        <v>1699</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Khoa toạ thủ cung Mệnh gặp Thiên Mã</v>
+        <v>Cung Mệnh có Tang Môn toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1645</v>
+        <v>1700</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Khoa toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp</v>
+        <v>Cung Mệnh có Tang Môn toạ thủ cung Mệnh gặp Kinh Dương, Thiên Hình</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>1646</v>
+        <v>1701</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Khoa toạ thủ cung Mệnh gặp Tử Vi, Thiên Phủ</v>
+        <v>Cung Mệnh có Tang Môn đồng cung Tham Lang gặp Hỏa Tinh gặp Linh Tinh, Kình Dương, Đà La</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>1647</v>
+        <v>1702</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Kỵ toạ thủ cung Mệnh</v>
+        <v>Cung Mệnh có Bạch Hổ toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Kình Dương, Đà La</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>1648</v>
+        <v>1703</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Kỵ toạ thủ cung Mệnh gặp Hỏa Tinh, Linh Tinh, Kình Dương, Đà La</v>
+        <v>Cung Mệnh có Bạch Hổ toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>1649</v>
+        <v>1704</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Kỵ toạ thủ cung Mệnh gặp Đào Hoa, Hồng Loan</v>
+        <v>Cung Mệnh có Bạch Hổ toạ thủ cung Mệnh gặp Kinh Dương, Thiên Hình</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>1650</v>
+        <v>1705</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Kỵ toạ thủ cung Mệnh gặp Thiên Mã</v>
+        <v>Cung Mệnh có Bạch Hổ đồng cung Tham Lang gặp Hỏa Tinh gặp Linh Tinh, Kình Dương, Đà La</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>1651</v>
+        <v>1706</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Kỵ toạ thủ cung Mệnh gặp Địa Không, Địa Kiếp</v>
+        <v>Cung Mệnh có Bạch Hổ đồng cung Tấu Thư</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>1652</v>
+        <v>1707</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Kỵ toạ thủ cung Mệnh gặp Thái Dương, Thái Âm</v>
+        <v>Cung Mệnh có Bạch Hổ đồng cung Phi Liêm</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>1653</v>
+        <v>1708</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Kỵ toạ thủ cung Mệnh gặp Thái Dương, Thái Âm, Thiên Hình</v>
+        <v>Cung Mệnh có Thiên Khốc</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>1654</v>
+        <v>1709</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Kỵ, Cự Môn đồng cung Mệnh</v>
+        <v>Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Tý</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>1655</v>
+        <v>1710</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Kỵ, Tham Lang đồng cung Mệnh</v>
+        <v>Người tuổi Tý có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>1656</v>
+        <v>1711</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Kỵ toạ thủ cung Mệnh gặp Tử Vi, Thiên Phủ</v>
+        <v>Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Ngọ</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>1657</v>
+        <v>1712</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Kỵ toạ thủ cung Mệnh gặp Thiên Khôi, Thiên Việt, Văn Xương, Văn Khúc</v>
+        <v>Người tuổi Ngọ có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1658</v>
+        <v>1713</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Kỵ toạ thủ cung Mệnh gặp Thiên Đồng, Thiên Lương</v>
+        <v>Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Mão</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>1659</v>
+        <v>1714</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Lộc toạ thủ cung đồng cung Tham Lang, Vũ Khúc tại Mệnh ở Thìn</v>
+        <v>Người tuổi Mão có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>1660</v>
+        <v>1715</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Lộc toạ thủ cung đồng cung Tham Lang, Vũ Khúc tại Mệnh ở Tuất</v>
+        <v>Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Dậu</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>1661</v>
+        <v>1716</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Lộc toạ thủ cung đồng cung Tham Lang, Vũ Khúc tại Mệnh ở Sửu</v>
+        <v>Người tuổi Dậu có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>1662</v>
+        <v>1717</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="0"/>
-        <v>Hoá Lộc toạ thủ cung đồng cung Tham Lang, Vũ Khúc tại Mệnh ở Mùi</v>
+        <v>Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Sửu</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>1663</v>
+        <v>1718</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="0"/>
-        <v>Người tuổiĐ. có Hoá Lộc toạ thủ cung Mệnh, Lộc Tồn toạ thủ cung Thiên Di</v>
+        <v>Người tuổi Sửu có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>1664</v>
+        <v>1719</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="0"/>
-        <v>Người tuổiK. có Hoá Lộc toạ thủ cung Mệnh, Lộc Tồn toạ thủ cung Thiên Di</v>
+        <v>Cung Mệnh có Thiên Khốc toạ thủ cung Mệnh tại Mùi</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1665</v>
+        <v>1720</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="0"/>
-        <v>Người tuổiNgọ có Hoá Lộc, Thiên Lương đồng cung Mệnh</v>
+        <v>Người tuổi Mùi có Thiên Khốc toạ thủ cung Mệnh, gặp Hóa Lộc</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>1666</v>
+        <v>1721</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="0"/>
-        <v>Người tuổiThìn có Hoá Lộc, Thiên Lương đồng cung Mệnh</v>
+        <v>Cung Mệnh có Thiên Hư</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>1667</v>
+        <v>1722</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="0"/>
-        <v>Người tuổiTuất có Hoá Lộc, Thiên Lương đồng cung Mệnh</v>
+        <v>Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Tý</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>1668</v>
+        <v>1723</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="0"/>
-        <v>Người tuổi Dần có Hoá Lộc toạ thủ cung Mệnh, Thiên Cơ, Thiên Lương, Lộc Tồn đồng cung Mệnh</v>
+        <v>Người tuổi Tý có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>1669</v>
+        <v>1724</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="0"/>
-        <v>Người tuổi Thân có Hoá Lộc toạ thủ cung Mệnh, Thiên Cơ, Thiên Lương, Lộc Tồn đồng cung Mệnh</v>
+        <v>Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Ngọ</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>1670</v>
+        <v>1725</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Quyền, Hóa Lộc đồng cung Mệnh không gặp Địa Không, Địa Kiếp</v>
+        <v>Người tuổi Ngọ có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>1671</v>
+        <v>1726</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Quyền toạ thủ cung Mệnh gặp Hóa Lộc, không gặp Địa Không, Địa Kiếp</v>
+        <v>Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Mão</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>1672</v>
+        <v>1727</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Lộc toạ thủ cung Mệnh gặp Hóa Quyền, không gặp Địa Không, Địa Kiếp</v>
+        <v>Người tuổi Mão có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1673</v>
+        <v>1728</v>
       </c>
       <c r="B49" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Quyền, Hóa Lộc giáp mệnh</v>
+        <v>Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Dậu</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>1674</v>
+        <v>1729</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Khoa toạ thủ cung Mệnh gặp Hóa Lộc, không gặp Địa Không, Địa Kiếp</v>
+        <v>Người tuổi Dậu có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>1675</v>
+        <v>1730</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Khoa, Hóa Lộc đồng cung Mệnh không gặp Địa Không, Địa Kiếp</v>
+        <v>Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Sửu</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>1676</v>
+        <v>1731</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Lộc toạ thủ cung Mệnh gặp Hóa Khoa, không gặp Địa Không, Địa Kiếp</v>
+        <v>Người tuổi Sửu có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>1677</v>
+        <v>1732</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Khoa, Hóa Lộc giáp mệnh</v>
+        <v>Cung Mệnh có Thiên Hư toạ thủ cung Mệnh tại Mùi</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>1678</v>
+        <v>1733</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Khoa toạ thủ cung Mệnh gặp Hóa Lộc, không gặp Địa Không, Địa Kiếp</v>
+        <v>Người tuổi Mùi có Thiên Hư toạ thủ cung Mệnh, gặp Hóa Lộc</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>1679</v>
+        <v>1734</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Khoa, Hóa Quyền đồng cung Mệnh không gặp Địa Không, Địa Kiếp</v>
+        <v>Người tuổi Tý có Thiên Khốc toạ thủ cung Mệnh, gặp Kình Dương, Đà La, Hỏa Tinh, Linh Tinh</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>1680</v>
+        <v>1735</v>
       </c>
       <c r="B56" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Khoa toạ thủ cung Mệnh gặp Hóa Quyền, không gặp Địa Không, Địa Kiếp</v>
+        <v>Người tuổi Tý có Thiên Khốc đồng cung Phá Quân tại Mệnh</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>1681</v>
+        <v>1736</v>
       </c>
       <c r="B57" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Khoa, Hóa Quyền giáp mệnh</v>
+        <v>Người tuổi Ngọ có Thiên Khốc toạ thủ cung Mệnh, gặp Kình Dương, Đà La, Hỏa Tinh, Linh Tinh</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>1682</v>
+        <v>1737</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Kỵ toạ thủ cung Mệnh gặp Hóa Lộc, Hóa Quyền, gặp Địa Không, Địa Kiếp</v>
+        <v>Người tuổi Ngọ có Thiên Khốc đồng cung Phá Quân tại Mệnh</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>1683</v>
+        <v>1738</v>
       </c>
       <c r="B59" t="str">
         <f t="shared" si="0"/>
-        <v>Hóa Kỵ toạ thủ cung Mệnh gặp Hóa Lộc, Hóa Quyền, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt</v>
+        <v>Người tuổi Tý có Thiên Hư toạ thủ cung Mệnh, gặp Kình Dương, Đà La, Hỏa Tinh, Linh Tinh</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>1684</v>
+        <v>1739</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Người tuổi Tý có Hóa Khoa toạ thủ cung Mệnh, gặp Thiên Đồng, Thiên Lương </v>
+        <v>Người tuổi Tý có Thiên Hư đồng cung Phá Quân tại Mệnh</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1685</v>
+        <v>1740</v>
       </c>
       <c r="B61" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">Người tuổi Ngọ có Hóa Khoa toạ thủ cung Mệnh, gặp Thiên Đồng, Thiên Lương </v>
+        <v>Người tuổi Ngọ có Thiên Hư toạ thủ cung Mệnh, gặp Kình Dương, Đà La, Hỏa Tinh, Linh Tinh</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>1686</v>
+        <v>1741</v>
       </c>
       <c r="B62" t="str">
         <f t="shared" si="0"/>
-        <v>Người tuổi Tý có Hóa Kỵ toạ thủ cung Mệnh, gặp Thiên Đồng, Thiên Lương</v>
+        <v>Người tuổi Ngọ có Thiên Hư đồng cung Phá Quân tại Mệnh</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>1742</v>
+      </c>
+      <c r="B63" t="str">
+        <f t="shared" si="0"/>
+        <v>Cung Mệnh có Dần</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>Người tuổi Dần có Dần toạ thủ cung Mệnh, gặp Kình Dương, Đà La</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>1744</v>
+      </c>
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>Người tuổi Dần có Dần toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>1745</v>
+      </c>
+      <c r="B66" t="str">
+        <f t="shared" si="0"/>
+        <v>Người tuổi Thân có Dần toạ thủ cung Mệnh, gặp Kình Dương, Đà La</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>1746</v>
+      </c>
+      <c r="B67" t="str">
+        <f t="shared" ref="B67:B94" si="1">RIGHT(A67,LEN(A67)-17)</f>
+        <v>Người tuổi Thân có Dần toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>1747</v>
+      </c>
+      <c r="B68" t="str">
+        <f t="shared" si="1"/>
+        <v>Cung Mệnh có Thân</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B69" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Dần có Thân toạ thủ cung Mệnh, gặp Kình Dương, Đà La</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>1749</v>
+      </c>
+      <c r="B70" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Dần có Thân toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>1750</v>
+      </c>
+      <c r="B71" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Thân có Thân toạ thủ cung Mệnh, gặp Kình Dương, Đà La</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B72" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Thân có Thân toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>1752</v>
+      </c>
+      <c r="B73" t="str">
+        <f t="shared" si="1"/>
+        <v>Cung Mệnh có Tỵ</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>1753</v>
+      </c>
+      <c r="B74" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Dần có Tỵ toạ thủ cung Mệnh, gặp Kình Dương, Đà La</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B75" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Dần có Tỵ toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>1755</v>
+      </c>
+      <c r="B76" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Thân có Tỵ toạ thủ cung Mệnh, gặp Kình Dương, Đà La</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>1756</v>
+      </c>
+      <c r="B77" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Thân có Tỵ toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>1757</v>
+      </c>
+      <c r="B78" t="str">
+        <f t="shared" si="1"/>
+        <v>Cung Mệnh có Hợi</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B79" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Dần có Hợi toạ thủ cung Mệnh, gặp Kình Dương, Đà La</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>1759</v>
+      </c>
+      <c r="B80" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Dần có Hợi toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>1760</v>
+      </c>
+      <c r="B81" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Thân có Hợi toạ thủ cung Mệnh, gặp Kình Dương, Đà La</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>1761</v>
+      </c>
+      <c r="B82" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Thân có Hợi toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>1762</v>
+      </c>
+      <c r="B83" t="str">
+        <f t="shared" si="1"/>
+        <v>Cung Mệnh có Thìn</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>1763</v>
+      </c>
+      <c r="B84" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Dần có Thìn toạ thủ cung Mệnh, gặp Kình Dương, Đà La</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>1764</v>
+      </c>
+      <c r="B85" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Dần có Thìn toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>1765</v>
+      </c>
+      <c r="B86" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Thân có Thìn toạ thủ cung Mệnh, gặp Kình Dương, Đà La</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>1766</v>
+      </c>
+      <c r="B87" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Thân có Thìn toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>1767</v>
+      </c>
+      <c r="B88" t="str">
+        <f t="shared" si="1"/>
+        <v>Cung Mệnh có Tuất</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B89" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Dần có Tuất toạ thủ cung Mệnh, gặp Kình Dương, Đà La</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B90" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Dần có Tuất toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B91" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Thân có Tuất toạ thủ cung Mệnh, gặp Kình Dương, Đà La</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>1771</v>
+      </c>
+      <c r="B92" t="str">
+        <f t="shared" si="1"/>
+        <v>Người tuổi Thân có Tuất toạ thủ cung Mệnh, gặp Thiên Hình, Thiên Mã</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>1772</v>
+      </c>
+      <c r="B93" t="str">
+        <f t="shared" si="1"/>
+        <v>Cung Mệnh có Mão toạ thủ cung Mệnh gặp Thiên Cơ, Cự Môn</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B94" t="str">
+        <f t="shared" si="1"/>
+        <v>Cung Mệnh có Dậu toạ thủ cung Mệnh gặp Thiên Cơ, Cự Môn</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Luận Sao Tử Vi
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95EF7944-127C-4962-8FC1-D6DC6256158D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B119C66-9547-4D27-8F46-224D0619A5F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3653" uniqueCount="1840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3655" uniqueCount="1841">
   <si>
     <t>Tử Vi</t>
   </si>
@@ -5555,6 +5555,9 @@
   </si>
   <si>
     <t>Cung Mệnh có Dậu toạ thủ cung Mệnh gặp Thiên Cơ, Cự Môn</t>
+  </si>
+  <si>
+    <t>Cung Mệnh Vô Chính Diệu</t>
   </si>
 </sst>
 </file>
@@ -5603,77 +5606,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -6270,10 +6203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B1804"/>
+  <dimension ref="A1:B1806"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1741" workbookViewId="0">
-      <selection activeCell="A1632" sqref="A1632:B1804"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20522,69 +20455,81 @@
         <v>181</v>
       </c>
     </row>
+    <row r="1806" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1806" t="s">
+        <v>1840</v>
+      </c>
+      <c r="B1806" t="s">
+        <v>1840</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="38" priority="46"/>
-    <cfRule type="duplicateValues" dxfId="37" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="36" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="35" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="34" priority="20"/>
-    <cfRule type="duplicateValues" dxfId="33" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145:A208">
-    <cfRule type="duplicateValues" dxfId="32" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A209:A1631 A1:A23 A25:A84 A143 A1805:A1048576">
-    <cfRule type="duplicateValues" dxfId="31" priority="55"/>
-    <cfRule type="duplicateValues" dxfId="30" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B84:B142">
-    <cfRule type="duplicateValues" dxfId="20" priority="18"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B143">
-    <cfRule type="duplicateValues" dxfId="18" priority="68"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="70"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="71"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="16" priority="23"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B325:B401">
-    <cfRule type="duplicateValues" dxfId="14" priority="144"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="145"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="146"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="147"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B402:B1259 B83 B145:B324 B1275:B1473 B1536 B1631 B1805:B1048576">
-    <cfRule type="duplicateValues" dxfId="12" priority="54"/>
+  <conditionalFormatting sqref="B402:B1259 B83 B145:B324 B1275:B1473 B1536 B1631 B1805:B1807 B1812:B1048576">
+    <cfRule type="duplicateValues" dxfId="14" priority="56"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1260:B1274">
+    <cfRule type="duplicateValues" dxfId="13" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1474:B1535">
     <cfRule type="duplicateValues" dxfId="11" priority="11"/>
     <cfRule type="duplicateValues" dxfId="10" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1474:B1535">
+  <conditionalFormatting sqref="B1537:B1630">
     <cfRule type="duplicateValues" dxfId="9" priority="9"/>
     <cfRule type="duplicateValues" dxfId="8" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1537:B1630">
+  <conditionalFormatting sqref="B1:B12">
     <cfRule type="duplicateValues" dxfId="7" priority="7"/>
     <cfRule type="duplicateValues" dxfId="6" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B12">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13:B23 B25:B82">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1808:B1811">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Luận cung quan lộc
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C43B0C-688F-4A89-9C6A-5A99C8BEF52A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1712B7A-4CC8-4494-97B6-3771E1C04988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -11776,8 +11776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
   <dimension ref="A1:B3812"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1655" workbookViewId="0">
-      <selection activeCell="Q1660" sqref="Q1660"/>
+    <sheetView tabSelected="1" topLeftCell="A1631" workbookViewId="0">
+      <selection activeCell="Q1657" sqref="Q1657"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Hoàn Thiện Luận theo file excel
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD879CBF-787F-40B3-918B-6170CA0930F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9BED4C-740D-4B7E-8858-AEC573F60A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7620" uniqueCount="3810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8454" uniqueCount="4226">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -11455,6 +11455,1254 @@
   </si>
   <si>
     <t>Tử Vi Tang Tả Hữu</t>
+  </si>
+  <si>
+    <t>Thiên Khôi (ĐV) tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Thiên Khôi (ĐV) tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Thiên Khôi (ĐV) tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Thiên Khôi (ĐV) tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Thiên Khôi (ĐV) tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Thiên Khôi (ĐV) tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Thiên Khôi (ĐV) tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Thiên Khôi (ĐV) tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thiên Khôi (ĐV) tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Thiên Khôi (ĐV) tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Khôi (ĐV) tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>L. Lộc Tồn tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>L. Lộc Tồn tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>L. Lộc Tồn tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>L. Lộc Tồn tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>L. Lộc Tồn tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>L. Lộc Tồn tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>L. Lộc Tồn tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>L. Lộc Tồn tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>L. Lộc Tồn tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>L. Lộc Tồn tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>L. Lộc Tồn tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Quan Phủ tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Quan Phủ tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Quan Phủ tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Quan Phủ tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Quan Phủ tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Quan Phủ tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Quan Phủ tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Quan Phủ tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Quan Phủ tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Quan Phủ tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Quan Phủ tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>L. Kình Dương tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>L. Kình Dương tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>L. Kình Dương tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>L. Kình Dương tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>L. Kình Dương tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>L. Kình Dương tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>L. Kình Dương tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>L. Kình Dương tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>L. Kình Dương tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>L. Kình Dương tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>L. Kình Dương tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Thiên Việt (ĐV) tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Thiên Việt (ĐV) tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Thiên Việt (ĐV) tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Thiên Việt (ĐV) tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Thiên Việt (ĐV) tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Thiên Việt (ĐV) tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Thiên Việt (ĐV) tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Thiên Việt (ĐV) tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Thiên Việt (ĐV) tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Việt (ĐV) tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Thiên Việt (ĐV) tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Phù tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Tử Phù tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Tử Phù tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Tử Phù tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tử Phù tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Tử Phù tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Tử Phù tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Tử Phù tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Tử Phù tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Tử Phù tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Tử Phù tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Kiếp Sát tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Kiếp Sát tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Kiếp Sát tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Kiếp Sát tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Kiếp Sát tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Kiếp Sát tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Kiếp Sát tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Kiếp Sát tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Kiếp Sát tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Kiếp Sát tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Kiếp Sát tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Phá Toái tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Phá Toái tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Phá Toái tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Phá Toái tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Phá Toái tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Phá Toái tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Phá Toái tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Phá Toái tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Phá Toái tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Phá Toái tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Phá Toái tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>L. Thái Tuế tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>L. Thái Tuế tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>L. Thái Tuế tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>L. Thái Tuế tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>L. Thái Tuế tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>L. Thái Tuế tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>L. Thái Tuế tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>L. Thái Tuế tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>L. Thái Tuế tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>L. Thái Tuế tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>L. Thái Tuế tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>L. Hóa Lộc tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>L. Hóa Lộc tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>L. Hóa Lộc tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>L. Hóa Lộc tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>L. Hóa Lộc tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>L. Hóa Lộc tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>L. Hóa Lộc tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>L. Hóa Lộc tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>L. Hóa Lộc tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>L. Hóa Lộc tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>L. Hóa Lộc tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tuế Phá tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Tuế Phá tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Tuế Phá tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Tuế Phá tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Tuế Phá tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Tuế Phá tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Tuế Phá tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Tuế Phá tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Tuế Phá tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Tuế Phá tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Tuế Phá tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Long Đức tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Long Đức tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Long Đức tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Long Đức tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Long Đức tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Long Đức tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Long Đức tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Long Đức tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Long Đức tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Long Đức tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Long Đức tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>L. Hóa Khoa tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>L. Hóa Khoa tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>L. Hóa Khoa tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>L. Hóa Khoa tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>L. Hóa Khoa tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>L. Hóa Khoa tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>L. Hóa Khoa tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>L. Hóa Khoa tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>L. Hóa Khoa tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>L. Hóa Khoa tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>L. Hóa Khoa tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>(Hóa Lộc - ĐV) tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>(Hóa Lộc - ĐV) tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>(Hóa Lộc - ĐV) tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>(Hóa Lộc - ĐV) tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>(Hóa Lộc - ĐV) tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>(Hóa Lộc - ĐV) tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>(Hóa Lộc - ĐV) tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>(Hóa Lộc - ĐV) tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>(Hóa Lộc - ĐV) tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>(Hóa Lộc - ĐV) tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>(Hóa Lộc - ĐV) tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>(Hóa Lộc - ĐV) tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>L. Tang Môn tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>L. Tang Môn tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>L. Tang Môn tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>L. Tang Môn tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>L. Tang Môn tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>L. Tang Môn tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>L. Tang Môn tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>L. Tang Môn tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>L. Tang Môn tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>L. Tang Môn tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>L. Tang Môn tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Văn Tinh tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Văn Tinh tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Văn Tinh tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Văn Tinh tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Văn Tinh tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Văn Tinh tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Văn Tinh tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Văn Tinh tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Văn Tinh tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Văn Tinh tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Văn Tinh tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Phúc Đức tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Phúc Đức tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Phúc Đức tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Phúc Đức tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Phúc Đức tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Phúc Đức tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Phúc Đức tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Phúc Đức tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Phúc Đức tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Phúc Đức tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Phúc Đức tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>(Hóa Khoa - ĐV) tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>(Hóa Khoa - ĐV) tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>(Hóa Khoa - ĐV) tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>(Hóa Khoa - ĐV) tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>(Hóa Khoa - ĐV) tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>(Hóa Khoa - ĐV) tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>(Hóa Khoa - ĐV) tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>(Hóa Khoa - ĐV) tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>(Hóa Khoa - ĐV) tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>(Hóa Khoa - ĐV) tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>(Hóa Khoa - ĐV) tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>(Hóa Khoa - ĐV) tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Điếu Khách tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Điếu Khách tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Điếu Khách tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Điếu Khách tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Điếu Khách tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Điếu Khách tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Điếu Khách tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Điếu Khách tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Điếu Khách tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Điếu Khách tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Điếu Khách tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Quả Tú tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Quả Tú tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Quả Tú tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Quả Tú tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Quả Tú tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Quả Tú tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Quả Tú tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Quả Tú tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Quả Tú tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Quả Tú tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Quả Tú tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>L. Hóa Kỵ tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>L. Hóa Kỵ tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>L. Hóa Kỵ tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>L. Hóa Kỵ tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>L. Hóa Kỵ tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>L. Hóa Kỵ tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>L. Hóa Kỵ tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>L. Hóa Kỵ tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>L. Hóa Kỵ tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>L. Hóa Kỵ tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>L. Hóa Kỵ tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Thiên Mã (ĐV) tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Thiên Mã (ĐV) tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Thiên Mã (ĐV) tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Thiên Mã (ĐV) tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Thiên Mã (ĐV) tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Thiên Mã (ĐV) tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Thiên Mã (ĐV) tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Thiên Mã (ĐV) tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thiên Mã (ĐV) tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Thiên Mã (ĐV) tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Thiên Mã (ĐV) tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Thiên Mã (ĐV) tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>L. Thiên Mã tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>L. Thiên Mã tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>L. Thiên Mã tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>L. Thiên Mã tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>L. Thiên Mã tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>L. Thiên Mã tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>L. Thiên Mã tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>L. Thiên Mã tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>L. Thiên Mã tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>L. Thiên Mã tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>L. Thiên Mã tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Đà La (ĐV) tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Đà La (ĐV) tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Đà La (ĐV) tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Đà La (ĐV) tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Đà La (ĐV) tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Đà La (ĐV) tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Đà La (ĐV) tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Đà La (ĐV) tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Đà La (ĐV) tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Đà La (ĐV) tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Đà La (ĐV) tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Trực Phù tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Trực Phù tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Trực Phù tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Trực Phù tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Trực Phù tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Trực Phù tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Trực Phù tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Trực Phù tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Trực Phù tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Trực Phù tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Trực Phù tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>L. Thiên Hư tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>L. Thiên Hư tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>L. Thiên Hư tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>L. Thiên Hư tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>L. Thiên Hư tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>L. Thiên Hư tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>L. Thiên Hư tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>L. Thiên Hư tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>L. Thiên Hư tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>L. Thiên Hư tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>L. Thiên Hư tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>(Hóa Kỵ - ĐV) tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>(Hóa Kỵ - ĐV) tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>(Hóa Kỵ - ĐV) tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>(Hóa Kỵ - ĐV) tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>(Hóa Kỵ - ĐV) tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>(Hóa Kỵ - ĐV) tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>(Hóa Kỵ - ĐV) tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>(Hóa Kỵ - ĐV) tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>(Hóa Kỵ - ĐV) tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>(Hóa Kỵ - ĐV) tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>(Hóa Kỵ - ĐV) tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>(Hóa Kỵ - ĐV) tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Lộc Tồn (ĐV) tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Lộc Tồn (ĐV) tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Lộc Tồn (ĐV) tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Lộc Tồn (ĐV) tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Lộc Tồn (ĐV) tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Lộc Tồn (ĐV) tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Lộc Tồn (ĐV) tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Lộc Tồn (ĐV) tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Lộc Tồn (ĐV) tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Lộc Tồn (ĐV) tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Lộc Tồn (ĐV) tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>(Hóa Quyền - ĐV) tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>(Hóa Quyền - ĐV) tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>(Hóa Quyền - ĐV) tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>(Hóa Quyền - ĐV) tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>(Hóa Quyền - ĐV) tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>(Hóa Quyền - ĐV) tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>(Hóa Quyền - ĐV) tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>(Hóa Quyền - ĐV) tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>(Hóa Quyền - ĐV) tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>(Hóa Quyền - ĐV) tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>(Hóa Quyền - ĐV) tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>(Hóa Quyền - ĐV) tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Thái Tuế tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Thái Tuế tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Thái Tuế tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Thái Tuế tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Thái Tuế tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Thái Tuế tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Thái Tuế tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Thái Tuế tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Thái Tuế tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Thái Tuế tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Thái Tuế tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Đẩu Quân tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Đẩu Quân tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Đẩu Quân tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Đẩu Quân tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Đẩu Quân tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Đẩu Quân tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Đẩu Quân tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Đẩu Quân tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Đẩu Quân tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Đẩu Quân tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Đẩu Quân tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Kình Dương (ĐV) tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Kình Dương (ĐV) tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Kình Dương (ĐV) tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Kình Dương (ĐV) tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Kình Dương (ĐV) tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Kình Dương (ĐV) tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Kình Dương (ĐV) tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>Kình Dương (ĐV) tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Kình Dương (ĐV) tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Kình Dương (ĐV) tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Kình Dương (ĐV) tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>L. Bạch Hổ tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>L. Bạch Hổ tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>L. Bạch Hổ tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>L. Bạch Hổ tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>L. Bạch Hổ tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>L. Bạch Hổ tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>L. Bạch Hổ tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>L. Bạch Hổ tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>L. Bạch Hổ tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>L. Bạch Hổ tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>L. Bạch Hổ tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>L. Thiên Khốc tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>L. Thiên Khốc tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>L. Thiên Khốc tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>L. Thiên Khốc tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>L. Thiên Khốc tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>L. Thiên Khốc tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>L. Thiên Khốc tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>L. Thiên Khốc tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>L. Thiên Khốc tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>L. Thiên Khốc tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>L. Thiên Khốc tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>L. Hóa Quyền tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>L. Hóa Quyền tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>L. Hóa Quyền tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>L. Hóa Quyền tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>L. Hóa Quyền tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>L. Hóa Quyền tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>L. Hóa Quyền tọa thủ tại Tật Ách</t>
+  </si>
+  <si>
+    <t>L. Hóa Quyền tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>L. Hóa Quyền tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>L. Hóa Quyền tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>L. Hóa Quyền tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Cô Thần tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Cô Thần tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Cô Thần tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>Cô Thần tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Cô Thần tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Cô Thần tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>Cô Thần tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>Cô Thần tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Cô Thần tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>Cô Thần tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>Cô Thần tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>L. Đà La tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>L. Đà La tọa thủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>L. Đà La tọa thủ tại Phúc Đức</t>
+  </si>
+  <si>
+    <t>L. Đà La tọa thủ tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>L. Đà La tọa thủ tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>L. Đà La tọa thủ tại Nô Bộc</t>
+  </si>
+  <si>
+    <t>L. Đà La tọa thủ tại Thiên Di</t>
+  </si>
+  <si>
+    <t>L. Đà La tọa thủ tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>L. Đà La tọa thủ tại Tử Tức</t>
+  </si>
+  <si>
+    <t>L. Đà La tọa thủ tại Phu Thê</t>
+  </si>
+  <si>
+    <t>L. Đà La tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tang Môn toạ thủ cung Mệnh tại Dần</t>
+  </si>
+  <si>
+    <t>Tang Môn toạ thủ cung Mệnh tại Thân</t>
+  </si>
+  <si>
+    <t>Tang Môn toạ thủ cung Mệnh tại Mão</t>
+  </si>
+  <si>
+    <t>Tang Môn toạ thủ cung Mệnh tại Dậu</t>
   </si>
 </sst>
 </file>
@@ -11496,7 +12744,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -11793,16 +13051,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B3811"/>
+  <dimension ref="A1:B4228"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3781" workbookViewId="0">
-      <selection activeCell="C3793" sqref="C3793"/>
+    <sheetView tabSelected="1" topLeftCell="A4203" workbookViewId="0">
+      <selection activeCell="O4212" sqref="O4212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -42285,16 +43542,3355 @@
         <v>3809</v>
       </c>
     </row>
+    <row r="3812" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3812" t="s">
+        <v>3810</v>
+      </c>
+      <c r="B3812" t="s">
+        <v>3810</v>
+      </c>
+    </row>
+    <row r="3813" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3813" t="s">
+        <v>3811</v>
+      </c>
+      <c r="B3813" t="s">
+        <v>3811</v>
+      </c>
+    </row>
+    <row r="3814" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3814" t="s">
+        <v>3812</v>
+      </c>
+      <c r="B3814" t="s">
+        <v>3812</v>
+      </c>
+    </row>
+    <row r="3815" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3815" t="s">
+        <v>3813</v>
+      </c>
+      <c r="B3815" t="s">
+        <v>3813</v>
+      </c>
+    </row>
+    <row r="3816" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3816" t="s">
+        <v>3814</v>
+      </c>
+      <c r="B3816" t="s">
+        <v>3814</v>
+      </c>
+    </row>
+    <row r="3817" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3817" t="s">
+        <v>3815</v>
+      </c>
+      <c r="B3817" t="s">
+        <v>3815</v>
+      </c>
+    </row>
+    <row r="3818" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3818" t="s">
+        <v>3816</v>
+      </c>
+      <c r="B3818" t="s">
+        <v>3816</v>
+      </c>
+    </row>
+    <row r="3819" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3819" t="s">
+        <v>3817</v>
+      </c>
+      <c r="B3819" t="s">
+        <v>3817</v>
+      </c>
+    </row>
+    <row r="3820" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3820" t="s">
+        <v>3818</v>
+      </c>
+      <c r="B3820" t="s">
+        <v>3818</v>
+      </c>
+    </row>
+    <row r="3821" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3821" t="s">
+        <v>3819</v>
+      </c>
+      <c r="B3821" t="s">
+        <v>3819</v>
+      </c>
+    </row>
+    <row r="3822" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3822" t="s">
+        <v>3820</v>
+      </c>
+      <c r="B3822" t="s">
+        <v>3820</v>
+      </c>
+    </row>
+    <row r="3823" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3823" t="s">
+        <v>3821</v>
+      </c>
+      <c r="B3823" t="s">
+        <v>3821</v>
+      </c>
+    </row>
+    <row r="3824" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3824" t="s">
+        <v>3822</v>
+      </c>
+      <c r="B3824" t="s">
+        <v>3822</v>
+      </c>
+    </row>
+    <row r="3825" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3825" t="s">
+        <v>3823</v>
+      </c>
+      <c r="B3825" t="s">
+        <v>3823</v>
+      </c>
+    </row>
+    <row r="3826" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3826" t="s">
+        <v>3824</v>
+      </c>
+      <c r="B3826" t="s">
+        <v>3824</v>
+      </c>
+    </row>
+    <row r="3827" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3827" t="s">
+        <v>3825</v>
+      </c>
+      <c r="B3827" t="s">
+        <v>3825</v>
+      </c>
+    </row>
+    <row r="3828" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3828" t="s">
+        <v>3826</v>
+      </c>
+      <c r="B3828" t="s">
+        <v>3826</v>
+      </c>
+    </row>
+    <row r="3829" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3829" t="s">
+        <v>3827</v>
+      </c>
+      <c r="B3829" t="s">
+        <v>3827</v>
+      </c>
+    </row>
+    <row r="3830" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3830" t="s">
+        <v>3828</v>
+      </c>
+      <c r="B3830" t="s">
+        <v>3828</v>
+      </c>
+    </row>
+    <row r="3831" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3831" t="s">
+        <v>3829</v>
+      </c>
+      <c r="B3831" t="s">
+        <v>3829</v>
+      </c>
+    </row>
+    <row r="3832" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3832" t="s">
+        <v>3830</v>
+      </c>
+      <c r="B3832" t="s">
+        <v>3830</v>
+      </c>
+    </row>
+    <row r="3833" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3833" t="s">
+        <v>3831</v>
+      </c>
+      <c r="B3833" t="s">
+        <v>3831</v>
+      </c>
+    </row>
+    <row r="3834" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3834" t="s">
+        <v>3832</v>
+      </c>
+      <c r="B3834" t="s">
+        <v>3832</v>
+      </c>
+    </row>
+    <row r="3835" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3835" t="s">
+        <v>3833</v>
+      </c>
+      <c r="B3835" t="s">
+        <v>3833</v>
+      </c>
+    </row>
+    <row r="3836" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3836" t="s">
+        <v>3834</v>
+      </c>
+      <c r="B3836" t="s">
+        <v>3834</v>
+      </c>
+    </row>
+    <row r="3837" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3837" t="s">
+        <v>3835</v>
+      </c>
+      <c r="B3837" t="s">
+        <v>3835</v>
+      </c>
+    </row>
+    <row r="3838" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3838" t="s">
+        <v>3836</v>
+      </c>
+      <c r="B3838" t="s">
+        <v>3836</v>
+      </c>
+    </row>
+    <row r="3839" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3839" t="s">
+        <v>3837</v>
+      </c>
+      <c r="B3839" t="s">
+        <v>3837</v>
+      </c>
+    </row>
+    <row r="3840" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3840" t="s">
+        <v>3838</v>
+      </c>
+      <c r="B3840" t="s">
+        <v>3838</v>
+      </c>
+    </row>
+    <row r="3841" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3841" t="s">
+        <v>3839</v>
+      </c>
+      <c r="B3841" t="s">
+        <v>3839</v>
+      </c>
+    </row>
+    <row r="3842" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3842" t="s">
+        <v>3840</v>
+      </c>
+      <c r="B3842" t="s">
+        <v>3840</v>
+      </c>
+    </row>
+    <row r="3843" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3843" t="s">
+        <v>3841</v>
+      </c>
+      <c r="B3843" t="s">
+        <v>3841</v>
+      </c>
+    </row>
+    <row r="3844" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3844" t="s">
+        <v>3842</v>
+      </c>
+      <c r="B3844" t="s">
+        <v>3842</v>
+      </c>
+    </row>
+    <row r="3845" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3845" t="s">
+        <v>3843</v>
+      </c>
+      <c r="B3845" t="s">
+        <v>3843</v>
+      </c>
+    </row>
+    <row r="3846" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3846" t="s">
+        <v>3844</v>
+      </c>
+      <c r="B3846" t="s">
+        <v>3844</v>
+      </c>
+    </row>
+    <row r="3847" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3847" t="s">
+        <v>3845</v>
+      </c>
+      <c r="B3847" t="s">
+        <v>3845</v>
+      </c>
+    </row>
+    <row r="3848" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3848" t="s">
+        <v>3846</v>
+      </c>
+      <c r="B3848" t="s">
+        <v>3846</v>
+      </c>
+    </row>
+    <row r="3849" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3849" t="s">
+        <v>3847</v>
+      </c>
+      <c r="B3849" t="s">
+        <v>3847</v>
+      </c>
+    </row>
+    <row r="3850" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3850" t="s">
+        <v>3848</v>
+      </c>
+      <c r="B3850" t="s">
+        <v>3848</v>
+      </c>
+    </row>
+    <row r="3851" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3851" t="s">
+        <v>3849</v>
+      </c>
+      <c r="B3851" t="s">
+        <v>3849</v>
+      </c>
+    </row>
+    <row r="3852" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3852" t="s">
+        <v>3850</v>
+      </c>
+      <c r="B3852" t="s">
+        <v>3850</v>
+      </c>
+    </row>
+    <row r="3853" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3853" t="s">
+        <v>3851</v>
+      </c>
+      <c r="B3853" t="s">
+        <v>3851</v>
+      </c>
+    </row>
+    <row r="3854" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3854" t="s">
+        <v>3852</v>
+      </c>
+      <c r="B3854" t="s">
+        <v>3852</v>
+      </c>
+    </row>
+    <row r="3855" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3855" t="s">
+        <v>3853</v>
+      </c>
+      <c r="B3855" t="s">
+        <v>3853</v>
+      </c>
+    </row>
+    <row r="3856" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3856" t="s">
+        <v>3854</v>
+      </c>
+      <c r="B3856" t="s">
+        <v>3854</v>
+      </c>
+    </row>
+    <row r="3857" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3857" t="s">
+        <v>3855</v>
+      </c>
+      <c r="B3857" t="s">
+        <v>3855</v>
+      </c>
+    </row>
+    <row r="3858" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3858" t="s">
+        <v>3856</v>
+      </c>
+      <c r="B3858" t="s">
+        <v>3856</v>
+      </c>
+    </row>
+    <row r="3859" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3859" t="s">
+        <v>3857</v>
+      </c>
+      <c r="B3859" t="s">
+        <v>3857</v>
+      </c>
+    </row>
+    <row r="3860" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3860" t="s">
+        <v>3858</v>
+      </c>
+      <c r="B3860" t="s">
+        <v>3858</v>
+      </c>
+    </row>
+    <row r="3861" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3861" t="s">
+        <v>3859</v>
+      </c>
+      <c r="B3861" t="s">
+        <v>3859</v>
+      </c>
+    </row>
+    <row r="3862" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3862" t="s">
+        <v>3860</v>
+      </c>
+      <c r="B3862" t="s">
+        <v>3860</v>
+      </c>
+    </row>
+    <row r="3863" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3863" t="s">
+        <v>3861</v>
+      </c>
+      <c r="B3863" t="s">
+        <v>3861</v>
+      </c>
+    </row>
+    <row r="3864" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3864" t="s">
+        <v>3862</v>
+      </c>
+      <c r="B3864" t="s">
+        <v>3862</v>
+      </c>
+    </row>
+    <row r="3865" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3865" t="s">
+        <v>3863</v>
+      </c>
+      <c r="B3865" t="s">
+        <v>3863</v>
+      </c>
+    </row>
+    <row r="3866" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3866" t="s">
+        <v>3864</v>
+      </c>
+      <c r="B3866" t="s">
+        <v>3864</v>
+      </c>
+    </row>
+    <row r="3867" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3867" t="s">
+        <v>3865</v>
+      </c>
+      <c r="B3867" t="s">
+        <v>3865</v>
+      </c>
+    </row>
+    <row r="3868" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3868" t="s">
+        <v>3866</v>
+      </c>
+      <c r="B3868" t="s">
+        <v>3866</v>
+      </c>
+    </row>
+    <row r="3869" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3869" t="s">
+        <v>3867</v>
+      </c>
+      <c r="B3869" t="s">
+        <v>3867</v>
+      </c>
+    </row>
+    <row r="3870" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3870" t="s">
+        <v>3868</v>
+      </c>
+      <c r="B3870" t="s">
+        <v>3868</v>
+      </c>
+    </row>
+    <row r="3871" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3871" t="s">
+        <v>3869</v>
+      </c>
+      <c r="B3871" t="s">
+        <v>3869</v>
+      </c>
+    </row>
+    <row r="3872" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3872" t="s">
+        <v>3870</v>
+      </c>
+      <c r="B3872" t="s">
+        <v>3870</v>
+      </c>
+    </row>
+    <row r="3873" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3873" t="s">
+        <v>3871</v>
+      </c>
+      <c r="B3873" t="s">
+        <v>3871</v>
+      </c>
+    </row>
+    <row r="3874" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3874" t="s">
+        <v>3872</v>
+      </c>
+      <c r="B3874" t="s">
+        <v>3872</v>
+      </c>
+    </row>
+    <row r="3875" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3875" t="s">
+        <v>3873</v>
+      </c>
+      <c r="B3875" t="s">
+        <v>3873</v>
+      </c>
+    </row>
+    <row r="3876" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3876" t="s">
+        <v>3874</v>
+      </c>
+      <c r="B3876" t="s">
+        <v>3874</v>
+      </c>
+    </row>
+    <row r="3877" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3877" t="s">
+        <v>3875</v>
+      </c>
+      <c r="B3877" t="s">
+        <v>3875</v>
+      </c>
+    </row>
+    <row r="3878" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3878" t="s">
+        <v>3876</v>
+      </c>
+      <c r="B3878" t="s">
+        <v>3876</v>
+      </c>
+    </row>
+    <row r="3879" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3879" t="s">
+        <v>3877</v>
+      </c>
+      <c r="B3879" t="s">
+        <v>3877</v>
+      </c>
+    </row>
+    <row r="3880" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3880" t="s">
+        <v>3878</v>
+      </c>
+      <c r="B3880" t="s">
+        <v>3878</v>
+      </c>
+    </row>
+    <row r="3881" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3881" t="s">
+        <v>3879</v>
+      </c>
+      <c r="B3881" t="s">
+        <v>3879</v>
+      </c>
+    </row>
+    <row r="3882" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3882" t="s">
+        <v>3880</v>
+      </c>
+      <c r="B3882" t="s">
+        <v>3880</v>
+      </c>
+    </row>
+    <row r="3883" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3883" t="s">
+        <v>3881</v>
+      </c>
+      <c r="B3883" t="s">
+        <v>3881</v>
+      </c>
+    </row>
+    <row r="3884" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3884" t="s">
+        <v>3882</v>
+      </c>
+      <c r="B3884" t="s">
+        <v>3882</v>
+      </c>
+    </row>
+    <row r="3885" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3885" t="s">
+        <v>3883</v>
+      </c>
+      <c r="B3885" t="s">
+        <v>3883</v>
+      </c>
+    </row>
+    <row r="3886" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3886" t="s">
+        <v>3884</v>
+      </c>
+      <c r="B3886" t="s">
+        <v>3884</v>
+      </c>
+    </row>
+    <row r="3887" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3887" t="s">
+        <v>3885</v>
+      </c>
+      <c r="B3887" t="s">
+        <v>3885</v>
+      </c>
+    </row>
+    <row r="3888" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3888" t="s">
+        <v>3886</v>
+      </c>
+      <c r="B3888" t="s">
+        <v>3886</v>
+      </c>
+    </row>
+    <row r="3889" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3889" t="s">
+        <v>3887</v>
+      </c>
+      <c r="B3889" t="s">
+        <v>3887</v>
+      </c>
+    </row>
+    <row r="3890" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3890" t="s">
+        <v>3888</v>
+      </c>
+      <c r="B3890" t="s">
+        <v>3888</v>
+      </c>
+    </row>
+    <row r="3891" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3891" t="s">
+        <v>3889</v>
+      </c>
+      <c r="B3891" t="s">
+        <v>3889</v>
+      </c>
+    </row>
+    <row r="3892" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3892" t="s">
+        <v>3890</v>
+      </c>
+      <c r="B3892" t="s">
+        <v>3890</v>
+      </c>
+    </row>
+    <row r="3893" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3893" t="s">
+        <v>3891</v>
+      </c>
+      <c r="B3893" t="s">
+        <v>3891</v>
+      </c>
+    </row>
+    <row r="3894" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3894" t="s">
+        <v>3892</v>
+      </c>
+      <c r="B3894" t="s">
+        <v>3892</v>
+      </c>
+    </row>
+    <row r="3895" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3895" t="s">
+        <v>3893</v>
+      </c>
+      <c r="B3895" t="s">
+        <v>3893</v>
+      </c>
+    </row>
+    <row r="3896" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3896" t="s">
+        <v>3894</v>
+      </c>
+      <c r="B3896" t="s">
+        <v>3894</v>
+      </c>
+    </row>
+    <row r="3897" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3897" t="s">
+        <v>3895</v>
+      </c>
+      <c r="B3897" t="s">
+        <v>3895</v>
+      </c>
+    </row>
+    <row r="3898" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3898" t="s">
+        <v>3896</v>
+      </c>
+      <c r="B3898" t="s">
+        <v>3896</v>
+      </c>
+    </row>
+    <row r="3899" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3899" t="s">
+        <v>3897</v>
+      </c>
+      <c r="B3899" t="s">
+        <v>3897</v>
+      </c>
+    </row>
+    <row r="3900" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3900" t="s">
+        <v>3898</v>
+      </c>
+      <c r="B3900" t="s">
+        <v>3898</v>
+      </c>
+    </row>
+    <row r="3901" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3901" t="s">
+        <v>3899</v>
+      </c>
+      <c r="B3901" t="s">
+        <v>3899</v>
+      </c>
+    </row>
+    <row r="3902" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3902" t="s">
+        <v>3900</v>
+      </c>
+      <c r="B3902" t="s">
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="3903" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3903" t="s">
+        <v>3901</v>
+      </c>
+      <c r="B3903" t="s">
+        <v>3901</v>
+      </c>
+    </row>
+    <row r="3904" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3904" t="s">
+        <v>3902</v>
+      </c>
+      <c r="B3904" t="s">
+        <v>3902</v>
+      </c>
+    </row>
+    <row r="3905" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3905" t="s">
+        <v>3903</v>
+      </c>
+      <c r="B3905" t="s">
+        <v>3903</v>
+      </c>
+    </row>
+    <row r="3906" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3906" t="s">
+        <v>3904</v>
+      </c>
+      <c r="B3906" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="3907" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3907" t="s">
+        <v>3905</v>
+      </c>
+      <c r="B3907" t="s">
+        <v>3905</v>
+      </c>
+    </row>
+    <row r="3908" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3908" t="s">
+        <v>3906</v>
+      </c>
+      <c r="B3908" t="s">
+        <v>3906</v>
+      </c>
+    </row>
+    <row r="3909" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3909" t="s">
+        <v>3907</v>
+      </c>
+      <c r="B3909" t="s">
+        <v>3907</v>
+      </c>
+    </row>
+    <row r="3910" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3910" t="s">
+        <v>3908</v>
+      </c>
+      <c r="B3910" t="s">
+        <v>3908</v>
+      </c>
+    </row>
+    <row r="3911" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3911" t="s">
+        <v>3909</v>
+      </c>
+      <c r="B3911" t="s">
+        <v>3909</v>
+      </c>
+    </row>
+    <row r="3912" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3912" t="s">
+        <v>3910</v>
+      </c>
+      <c r="B3912" t="s">
+        <v>3910</v>
+      </c>
+    </row>
+    <row r="3913" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3913" t="s">
+        <v>3911</v>
+      </c>
+      <c r="B3913" t="s">
+        <v>3911</v>
+      </c>
+    </row>
+    <row r="3914" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3914" t="s">
+        <v>3912</v>
+      </c>
+      <c r="B3914" t="s">
+        <v>3912</v>
+      </c>
+    </row>
+    <row r="3915" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3915" t="s">
+        <v>3913</v>
+      </c>
+      <c r="B3915" t="s">
+        <v>3913</v>
+      </c>
+    </row>
+    <row r="3916" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3916" t="s">
+        <v>3914</v>
+      </c>
+      <c r="B3916" t="s">
+        <v>3914</v>
+      </c>
+    </row>
+    <row r="3917" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3917" t="s">
+        <v>3915</v>
+      </c>
+      <c r="B3917" t="s">
+        <v>3915</v>
+      </c>
+    </row>
+    <row r="3918" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3918" t="s">
+        <v>3916</v>
+      </c>
+      <c r="B3918" t="s">
+        <v>3916</v>
+      </c>
+    </row>
+    <row r="3919" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3919" t="s">
+        <v>3917</v>
+      </c>
+      <c r="B3919" t="s">
+        <v>3917</v>
+      </c>
+    </row>
+    <row r="3920" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3920" t="s">
+        <v>3918</v>
+      </c>
+      <c r="B3920" t="s">
+        <v>3918</v>
+      </c>
+    </row>
+    <row r="3921" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3921" t="s">
+        <v>3919</v>
+      </c>
+      <c r="B3921" t="s">
+        <v>3919</v>
+      </c>
+    </row>
+    <row r="3922" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3922" t="s">
+        <v>3920</v>
+      </c>
+      <c r="B3922" t="s">
+        <v>3920</v>
+      </c>
+    </row>
+    <row r="3923" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3923" t="s">
+        <v>3921</v>
+      </c>
+      <c r="B3923" t="s">
+        <v>3921</v>
+      </c>
+    </row>
+    <row r="3924" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3924" t="s">
+        <v>3922</v>
+      </c>
+      <c r="B3924" t="s">
+        <v>3922</v>
+      </c>
+    </row>
+    <row r="3925" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3925" t="s">
+        <v>3923</v>
+      </c>
+      <c r="B3925" t="s">
+        <v>3923</v>
+      </c>
+    </row>
+    <row r="3926" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3926" t="s">
+        <v>3924</v>
+      </c>
+      <c r="B3926" t="s">
+        <v>3924</v>
+      </c>
+    </row>
+    <row r="3927" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3927" t="s">
+        <v>3925</v>
+      </c>
+      <c r="B3927" t="s">
+        <v>3925</v>
+      </c>
+    </row>
+    <row r="3928" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3928" t="s">
+        <v>3926</v>
+      </c>
+      <c r="B3928" t="s">
+        <v>3926</v>
+      </c>
+    </row>
+    <row r="3929" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3929" t="s">
+        <v>3927</v>
+      </c>
+      <c r="B3929" t="s">
+        <v>3927</v>
+      </c>
+    </row>
+    <row r="3930" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3930" t="s">
+        <v>3928</v>
+      </c>
+      <c r="B3930" t="s">
+        <v>3928</v>
+      </c>
+    </row>
+    <row r="3931" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3931" t="s">
+        <v>3929</v>
+      </c>
+      <c r="B3931" t="s">
+        <v>3929</v>
+      </c>
+    </row>
+    <row r="3932" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3932" t="s">
+        <v>3930</v>
+      </c>
+      <c r="B3932" t="s">
+        <v>3930</v>
+      </c>
+    </row>
+    <row r="3933" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3933" t="s">
+        <v>3931</v>
+      </c>
+      <c r="B3933" t="s">
+        <v>3931</v>
+      </c>
+    </row>
+    <row r="3934" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3934" t="s">
+        <v>3932</v>
+      </c>
+      <c r="B3934" t="s">
+        <v>3932</v>
+      </c>
+    </row>
+    <row r="3935" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3935" t="s">
+        <v>3933</v>
+      </c>
+      <c r="B3935" t="s">
+        <v>3933</v>
+      </c>
+    </row>
+    <row r="3936" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3936" t="s">
+        <v>3934</v>
+      </c>
+      <c r="B3936" t="s">
+        <v>3934</v>
+      </c>
+    </row>
+    <row r="3937" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3937" t="s">
+        <v>3935</v>
+      </c>
+      <c r="B3937" t="s">
+        <v>3935</v>
+      </c>
+    </row>
+    <row r="3938" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3938" t="s">
+        <v>3936</v>
+      </c>
+      <c r="B3938" t="s">
+        <v>3936</v>
+      </c>
+    </row>
+    <row r="3939" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3939" t="s">
+        <v>3937</v>
+      </c>
+      <c r="B3939" t="s">
+        <v>3937</v>
+      </c>
+    </row>
+    <row r="3940" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3940" t="s">
+        <v>3938</v>
+      </c>
+      <c r="B3940" t="s">
+        <v>3938</v>
+      </c>
+    </row>
+    <row r="3941" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3941" t="s">
+        <v>3939</v>
+      </c>
+      <c r="B3941" t="s">
+        <v>3939</v>
+      </c>
+    </row>
+    <row r="3942" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3942" t="s">
+        <v>3940</v>
+      </c>
+      <c r="B3942" t="s">
+        <v>3940</v>
+      </c>
+    </row>
+    <row r="3943" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3943" t="s">
+        <v>3941</v>
+      </c>
+      <c r="B3943" t="s">
+        <v>3941</v>
+      </c>
+    </row>
+    <row r="3944" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3944" t="s">
+        <v>3942</v>
+      </c>
+      <c r="B3944" t="s">
+        <v>3942</v>
+      </c>
+    </row>
+    <row r="3945" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3945" t="s">
+        <v>3943</v>
+      </c>
+      <c r="B3945" t="s">
+        <v>3943</v>
+      </c>
+    </row>
+    <row r="3946" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3946" t="s">
+        <v>3944</v>
+      </c>
+      <c r="B3946" t="s">
+        <v>3944</v>
+      </c>
+    </row>
+    <row r="3947" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3947" t="s">
+        <v>3945</v>
+      </c>
+      <c r="B3947" t="s">
+        <v>3945</v>
+      </c>
+    </row>
+    <row r="3948" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3948" t="s">
+        <v>3946</v>
+      </c>
+      <c r="B3948" t="s">
+        <v>3946</v>
+      </c>
+    </row>
+    <row r="3949" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3949" t="s">
+        <v>3947</v>
+      </c>
+      <c r="B3949" t="s">
+        <v>3947</v>
+      </c>
+    </row>
+    <row r="3950" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3950" t="s">
+        <v>3948</v>
+      </c>
+      <c r="B3950" t="s">
+        <v>3948</v>
+      </c>
+    </row>
+    <row r="3951" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3951" t="s">
+        <v>3949</v>
+      </c>
+      <c r="B3951" t="s">
+        <v>3949</v>
+      </c>
+    </row>
+    <row r="3952" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3952" t="s">
+        <v>3950</v>
+      </c>
+      <c r="B3952" t="s">
+        <v>3950</v>
+      </c>
+    </row>
+    <row r="3953" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3953" t="s">
+        <v>3951</v>
+      </c>
+      <c r="B3953" t="s">
+        <v>3951</v>
+      </c>
+    </row>
+    <row r="3954" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3954" t="s">
+        <v>3952</v>
+      </c>
+      <c r="B3954" t="s">
+        <v>3952</v>
+      </c>
+    </row>
+    <row r="3955" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3955" t="s">
+        <v>3953</v>
+      </c>
+      <c r="B3955" t="s">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="3956" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3956" t="s">
+        <v>3954</v>
+      </c>
+      <c r="B3956" t="s">
+        <v>3954</v>
+      </c>
+    </row>
+    <row r="3957" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3957" t="s">
+        <v>3955</v>
+      </c>
+      <c r="B3957" t="s">
+        <v>3955</v>
+      </c>
+    </row>
+    <row r="3958" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3958" t="s">
+        <v>3956</v>
+      </c>
+      <c r="B3958" t="s">
+        <v>3956</v>
+      </c>
+    </row>
+    <row r="3959" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3959" t="s">
+        <v>3957</v>
+      </c>
+      <c r="B3959" t="s">
+        <v>3957</v>
+      </c>
+    </row>
+    <row r="3960" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3960" t="s">
+        <v>3958</v>
+      </c>
+      <c r="B3960" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="3961" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3961" t="s">
+        <v>3959</v>
+      </c>
+      <c r="B3961" t="s">
+        <v>3959</v>
+      </c>
+    </row>
+    <row r="3962" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3962" t="s">
+        <v>3960</v>
+      </c>
+      <c r="B3962" t="s">
+        <v>3960</v>
+      </c>
+    </row>
+    <row r="3963" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3963" t="s">
+        <v>3961</v>
+      </c>
+      <c r="B3963" t="s">
+        <v>3961</v>
+      </c>
+    </row>
+    <row r="3964" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3964" t="s">
+        <v>3962</v>
+      </c>
+      <c r="B3964" t="s">
+        <v>3962</v>
+      </c>
+    </row>
+    <row r="3965" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3965" t="s">
+        <v>3963</v>
+      </c>
+      <c r="B3965" t="s">
+        <v>3963</v>
+      </c>
+    </row>
+    <row r="3966" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3966" t="s">
+        <v>3964</v>
+      </c>
+      <c r="B3966" t="s">
+        <v>3964</v>
+      </c>
+    </row>
+    <row r="3967" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3967" t="s">
+        <v>3965</v>
+      </c>
+      <c r="B3967" t="s">
+        <v>3965</v>
+      </c>
+    </row>
+    <row r="3968" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3968" t="s">
+        <v>3966</v>
+      </c>
+      <c r="B3968" t="s">
+        <v>3966</v>
+      </c>
+    </row>
+    <row r="3969" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3969" t="s">
+        <v>3967</v>
+      </c>
+      <c r="B3969" t="s">
+        <v>3967</v>
+      </c>
+    </row>
+    <row r="3970" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3970" t="s">
+        <v>3968</v>
+      </c>
+      <c r="B3970" t="s">
+        <v>3968</v>
+      </c>
+    </row>
+    <row r="3971" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3971" t="s">
+        <v>3969</v>
+      </c>
+      <c r="B3971" t="s">
+        <v>3969</v>
+      </c>
+    </row>
+    <row r="3972" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3972" t="s">
+        <v>3970</v>
+      </c>
+      <c r="B3972" t="s">
+        <v>3970</v>
+      </c>
+    </row>
+    <row r="3973" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3973" t="s">
+        <v>3971</v>
+      </c>
+      <c r="B3973" t="s">
+        <v>3971</v>
+      </c>
+    </row>
+    <row r="3974" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3974" t="s">
+        <v>3972</v>
+      </c>
+      <c r="B3974" t="s">
+        <v>3972</v>
+      </c>
+    </row>
+    <row r="3975" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3975" t="s">
+        <v>3973</v>
+      </c>
+      <c r="B3975" t="s">
+        <v>3973</v>
+      </c>
+    </row>
+    <row r="3976" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3976" t="s">
+        <v>3974</v>
+      </c>
+      <c r="B3976" t="s">
+        <v>3974</v>
+      </c>
+    </row>
+    <row r="3977" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3977" t="s">
+        <v>3975</v>
+      </c>
+      <c r="B3977" t="s">
+        <v>3975</v>
+      </c>
+    </row>
+    <row r="3978" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3978" t="s">
+        <v>3976</v>
+      </c>
+      <c r="B3978" t="s">
+        <v>3976</v>
+      </c>
+    </row>
+    <row r="3979" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3979" t="s">
+        <v>3977</v>
+      </c>
+      <c r="B3979" t="s">
+        <v>3977</v>
+      </c>
+    </row>
+    <row r="3980" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3980" t="s">
+        <v>3978</v>
+      </c>
+      <c r="B3980" t="s">
+        <v>3978</v>
+      </c>
+    </row>
+    <row r="3981" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3981" t="s">
+        <v>3979</v>
+      </c>
+      <c r="B3981" t="s">
+        <v>3979</v>
+      </c>
+    </row>
+    <row r="3982" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3982" t="s">
+        <v>3980</v>
+      </c>
+      <c r="B3982" t="s">
+        <v>3980</v>
+      </c>
+    </row>
+    <row r="3983" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3983" t="s">
+        <v>3981</v>
+      </c>
+      <c r="B3983" t="s">
+        <v>3981</v>
+      </c>
+    </row>
+    <row r="3984" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3984" t="s">
+        <v>3982</v>
+      </c>
+      <c r="B3984" t="s">
+        <v>3982</v>
+      </c>
+    </row>
+    <row r="3985" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3985" t="s">
+        <v>3983</v>
+      </c>
+      <c r="B3985" t="s">
+        <v>3983</v>
+      </c>
+    </row>
+    <row r="3986" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3986" t="s">
+        <v>3984</v>
+      </c>
+      <c r="B3986" t="s">
+        <v>3984</v>
+      </c>
+    </row>
+    <row r="3987" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3987" t="s">
+        <v>3985</v>
+      </c>
+      <c r="B3987" t="s">
+        <v>3985</v>
+      </c>
+    </row>
+    <row r="3988" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3988" t="s">
+        <v>3986</v>
+      </c>
+      <c r="B3988" t="s">
+        <v>3986</v>
+      </c>
+    </row>
+    <row r="3989" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3989" t="s">
+        <v>3987</v>
+      </c>
+      <c r="B3989" t="s">
+        <v>3987</v>
+      </c>
+    </row>
+    <row r="3990" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3990" t="s">
+        <v>3988</v>
+      </c>
+      <c r="B3990" t="s">
+        <v>3988</v>
+      </c>
+    </row>
+    <row r="3991" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3991" t="s">
+        <v>3989</v>
+      </c>
+      <c r="B3991" t="s">
+        <v>3989</v>
+      </c>
+    </row>
+    <row r="3992" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3992" t="s">
+        <v>3990</v>
+      </c>
+      <c r="B3992" t="s">
+        <v>3990</v>
+      </c>
+    </row>
+    <row r="3993" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3993" t="s">
+        <v>3991</v>
+      </c>
+      <c r="B3993" t="s">
+        <v>3991</v>
+      </c>
+    </row>
+    <row r="3994" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3994" t="s">
+        <v>3992</v>
+      </c>
+      <c r="B3994" t="s">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="3995" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3995" t="s">
+        <v>3993</v>
+      </c>
+      <c r="B3995" t="s">
+        <v>3993</v>
+      </c>
+    </row>
+    <row r="3996" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3996" t="s">
+        <v>3994</v>
+      </c>
+      <c r="B3996" t="s">
+        <v>3994</v>
+      </c>
+    </row>
+    <row r="3997" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3997" t="s">
+        <v>3995</v>
+      </c>
+      <c r="B3997" t="s">
+        <v>3995</v>
+      </c>
+    </row>
+    <row r="3998" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3998" t="s">
+        <v>3996</v>
+      </c>
+      <c r="B3998" t="s">
+        <v>3996</v>
+      </c>
+    </row>
+    <row r="3999" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3999" t="s">
+        <v>3997</v>
+      </c>
+      <c r="B3999" t="s">
+        <v>3997</v>
+      </c>
+    </row>
+    <row r="4000" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4000" t="s">
+        <v>3998</v>
+      </c>
+      <c r="B4000" t="s">
+        <v>3998</v>
+      </c>
+    </row>
+    <row r="4001" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4001" t="s">
+        <v>3999</v>
+      </c>
+      <c r="B4001" t="s">
+        <v>3999</v>
+      </c>
+    </row>
+    <row r="4002" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4002" t="s">
+        <v>4000</v>
+      </c>
+      <c r="B4002" t="s">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="4003" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4003" t="s">
+        <v>4001</v>
+      </c>
+      <c r="B4003" t="s">
+        <v>4001</v>
+      </c>
+    </row>
+    <row r="4004" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4004" t="s">
+        <v>4002</v>
+      </c>
+      <c r="B4004" t="s">
+        <v>4002</v>
+      </c>
+    </row>
+    <row r="4005" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4005" t="s">
+        <v>4003</v>
+      </c>
+      <c r="B4005" t="s">
+        <v>4003</v>
+      </c>
+    </row>
+    <row r="4006" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4006" t="s">
+        <v>4004</v>
+      </c>
+      <c r="B4006" t="s">
+        <v>4004</v>
+      </c>
+    </row>
+    <row r="4007" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4007" t="s">
+        <v>4005</v>
+      </c>
+      <c r="B4007" t="s">
+        <v>4005</v>
+      </c>
+    </row>
+    <row r="4008" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4008" t="s">
+        <v>4006</v>
+      </c>
+      <c r="B4008" t="s">
+        <v>4006</v>
+      </c>
+    </row>
+    <row r="4009" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4009" t="s">
+        <v>4007</v>
+      </c>
+      <c r="B4009" t="s">
+        <v>4007</v>
+      </c>
+    </row>
+    <row r="4010" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4010" t="s">
+        <v>4008</v>
+      </c>
+      <c r="B4010" t="s">
+        <v>4008</v>
+      </c>
+    </row>
+    <row r="4011" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4011" t="s">
+        <v>4009</v>
+      </c>
+      <c r="B4011" t="s">
+        <v>4009</v>
+      </c>
+    </row>
+    <row r="4012" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4012" t="s">
+        <v>4010</v>
+      </c>
+      <c r="B4012" t="s">
+        <v>4010</v>
+      </c>
+    </row>
+    <row r="4013" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4013" t="s">
+        <v>4011</v>
+      </c>
+      <c r="B4013" t="s">
+        <v>4011</v>
+      </c>
+    </row>
+    <row r="4014" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4014" t="s">
+        <v>4012</v>
+      </c>
+      <c r="B4014" t="s">
+        <v>4012</v>
+      </c>
+    </row>
+    <row r="4015" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4015" t="s">
+        <v>4013</v>
+      </c>
+      <c r="B4015" t="s">
+        <v>4013</v>
+      </c>
+    </row>
+    <row r="4016" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4016" t="s">
+        <v>4014</v>
+      </c>
+      <c r="B4016" t="s">
+        <v>4014</v>
+      </c>
+    </row>
+    <row r="4017" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4017" t="s">
+        <v>4015</v>
+      </c>
+      <c r="B4017" t="s">
+        <v>4015</v>
+      </c>
+    </row>
+    <row r="4018" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4018" t="s">
+        <v>4016</v>
+      </c>
+      <c r="B4018" t="s">
+        <v>4016</v>
+      </c>
+    </row>
+    <row r="4019" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4019" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B4019" t="s">
+        <v>4017</v>
+      </c>
+    </row>
+    <row r="4020" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4020" t="s">
+        <v>4018</v>
+      </c>
+      <c r="B4020" t="s">
+        <v>4018</v>
+      </c>
+    </row>
+    <row r="4021" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4021" t="s">
+        <v>4019</v>
+      </c>
+      <c r="B4021" t="s">
+        <v>4019</v>
+      </c>
+    </row>
+    <row r="4022" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4022" t="s">
+        <v>4020</v>
+      </c>
+      <c r="B4022" t="s">
+        <v>4020</v>
+      </c>
+    </row>
+    <row r="4023" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4023" t="s">
+        <v>4021</v>
+      </c>
+      <c r="B4023" t="s">
+        <v>4021</v>
+      </c>
+    </row>
+    <row r="4024" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4024" t="s">
+        <v>4022</v>
+      </c>
+      <c r="B4024" t="s">
+        <v>4022</v>
+      </c>
+    </row>
+    <row r="4025" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4025" t="s">
+        <v>4023</v>
+      </c>
+      <c r="B4025" t="s">
+        <v>4023</v>
+      </c>
+    </row>
+    <row r="4026" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4026" t="s">
+        <v>4024</v>
+      </c>
+      <c r="B4026" t="s">
+        <v>4024</v>
+      </c>
+    </row>
+    <row r="4027" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4027" t="s">
+        <v>4025</v>
+      </c>
+      <c r="B4027" t="s">
+        <v>4025</v>
+      </c>
+    </row>
+    <row r="4028" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4028" t="s">
+        <v>4026</v>
+      </c>
+      <c r="B4028" t="s">
+        <v>4026</v>
+      </c>
+    </row>
+    <row r="4029" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4029" t="s">
+        <v>4027</v>
+      </c>
+      <c r="B4029" t="s">
+        <v>4027</v>
+      </c>
+    </row>
+    <row r="4030" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4030" t="s">
+        <v>4028</v>
+      </c>
+      <c r="B4030" t="s">
+        <v>4028</v>
+      </c>
+    </row>
+    <row r="4031" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4031" t="s">
+        <v>4029</v>
+      </c>
+      <c r="B4031" t="s">
+        <v>4029</v>
+      </c>
+    </row>
+    <row r="4032" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4032" t="s">
+        <v>4030</v>
+      </c>
+      <c r="B4032" t="s">
+        <v>4030</v>
+      </c>
+    </row>
+    <row r="4033" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4033" t="s">
+        <v>4031</v>
+      </c>
+      <c r="B4033" t="s">
+        <v>4031</v>
+      </c>
+    </row>
+    <row r="4034" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4034" t="s">
+        <v>4032</v>
+      </c>
+      <c r="B4034" t="s">
+        <v>4032</v>
+      </c>
+    </row>
+    <row r="4035" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4035" t="s">
+        <v>4033</v>
+      </c>
+      <c r="B4035" t="s">
+        <v>4033</v>
+      </c>
+    </row>
+    <row r="4036" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4036" t="s">
+        <v>4034</v>
+      </c>
+      <c r="B4036" t="s">
+        <v>4034</v>
+      </c>
+    </row>
+    <row r="4037" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4037" t="s">
+        <v>4035</v>
+      </c>
+      <c r="B4037" t="s">
+        <v>4035</v>
+      </c>
+    </row>
+    <row r="4038" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4038" t="s">
+        <v>4036</v>
+      </c>
+      <c r="B4038" t="s">
+        <v>4036</v>
+      </c>
+    </row>
+    <row r="4039" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4039" t="s">
+        <v>4037</v>
+      </c>
+      <c r="B4039" t="s">
+        <v>4037</v>
+      </c>
+    </row>
+    <row r="4040" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4040" t="s">
+        <v>4038</v>
+      </c>
+      <c r="B4040" t="s">
+        <v>4038</v>
+      </c>
+    </row>
+    <row r="4041" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4041" t="s">
+        <v>4039</v>
+      </c>
+      <c r="B4041" t="s">
+        <v>4039</v>
+      </c>
+    </row>
+    <row r="4042" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4042" t="s">
+        <v>4040</v>
+      </c>
+      <c r="B4042" t="s">
+        <v>4040</v>
+      </c>
+    </row>
+    <row r="4043" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4043" t="s">
+        <v>4041</v>
+      </c>
+      <c r="B4043" t="s">
+        <v>4041</v>
+      </c>
+    </row>
+    <row r="4044" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4044" t="s">
+        <v>4042</v>
+      </c>
+      <c r="B4044" t="s">
+        <v>4042</v>
+      </c>
+    </row>
+    <row r="4045" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4045" t="s">
+        <v>4043</v>
+      </c>
+      <c r="B4045" t="s">
+        <v>4043</v>
+      </c>
+    </row>
+    <row r="4046" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4046" t="s">
+        <v>4044</v>
+      </c>
+      <c r="B4046" t="s">
+        <v>4044</v>
+      </c>
+    </row>
+    <row r="4047" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4047" t="s">
+        <v>4045</v>
+      </c>
+      <c r="B4047" t="s">
+        <v>4045</v>
+      </c>
+    </row>
+    <row r="4048" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4048" t="s">
+        <v>4046</v>
+      </c>
+      <c r="B4048" t="s">
+        <v>4046</v>
+      </c>
+    </row>
+    <row r="4049" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4049" t="s">
+        <v>4047</v>
+      </c>
+      <c r="B4049" t="s">
+        <v>4047</v>
+      </c>
+    </row>
+    <row r="4050" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4050" t="s">
+        <v>4048</v>
+      </c>
+      <c r="B4050" t="s">
+        <v>4048</v>
+      </c>
+    </row>
+    <row r="4051" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4051" t="s">
+        <v>4049</v>
+      </c>
+      <c r="B4051" t="s">
+        <v>4049</v>
+      </c>
+    </row>
+    <row r="4052" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4052" t="s">
+        <v>4050</v>
+      </c>
+      <c r="B4052" t="s">
+        <v>4050</v>
+      </c>
+    </row>
+    <row r="4053" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4053" t="s">
+        <v>4051</v>
+      </c>
+      <c r="B4053" t="s">
+        <v>4051</v>
+      </c>
+    </row>
+    <row r="4054" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4054" t="s">
+        <v>4052</v>
+      </c>
+      <c r="B4054" t="s">
+        <v>4052</v>
+      </c>
+    </row>
+    <row r="4055" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4055" t="s">
+        <v>4053</v>
+      </c>
+      <c r="B4055" t="s">
+        <v>4053</v>
+      </c>
+    </row>
+    <row r="4056" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4056" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B4056" t="s">
+        <v>4054</v>
+      </c>
+    </row>
+    <row r="4057" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4057" t="s">
+        <v>4055</v>
+      </c>
+      <c r="B4057" t="s">
+        <v>4055</v>
+      </c>
+    </row>
+    <row r="4058" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4058" t="s">
+        <v>4056</v>
+      </c>
+      <c r="B4058" t="s">
+        <v>4056</v>
+      </c>
+    </row>
+    <row r="4059" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4059" t="s">
+        <v>4057</v>
+      </c>
+      <c r="B4059" t="s">
+        <v>4057</v>
+      </c>
+    </row>
+    <row r="4060" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4060" t="s">
+        <v>4058</v>
+      </c>
+      <c r="B4060" t="s">
+        <v>4058</v>
+      </c>
+    </row>
+    <row r="4061" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4061" t="s">
+        <v>4059</v>
+      </c>
+      <c r="B4061" t="s">
+        <v>4059</v>
+      </c>
+    </row>
+    <row r="4062" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4062" t="s">
+        <v>4060</v>
+      </c>
+      <c r="B4062" t="s">
+        <v>4060</v>
+      </c>
+    </row>
+    <row r="4063" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4063" t="s">
+        <v>4061</v>
+      </c>
+      <c r="B4063" t="s">
+        <v>4061</v>
+      </c>
+    </row>
+    <row r="4064" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4064" t="s">
+        <v>4062</v>
+      </c>
+      <c r="B4064" t="s">
+        <v>4062</v>
+      </c>
+    </row>
+    <row r="4065" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4065" t="s">
+        <v>4063</v>
+      </c>
+      <c r="B4065" t="s">
+        <v>4063</v>
+      </c>
+    </row>
+    <row r="4066" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4066" t="s">
+        <v>4064</v>
+      </c>
+      <c r="B4066" t="s">
+        <v>4064</v>
+      </c>
+    </row>
+    <row r="4067" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4067" t="s">
+        <v>4065</v>
+      </c>
+      <c r="B4067" t="s">
+        <v>4065</v>
+      </c>
+    </row>
+    <row r="4068" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4068" t="s">
+        <v>4066</v>
+      </c>
+      <c r="B4068" t="s">
+        <v>4066</v>
+      </c>
+    </row>
+    <row r="4069" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4069" t="s">
+        <v>4067</v>
+      </c>
+      <c r="B4069" t="s">
+        <v>4067</v>
+      </c>
+    </row>
+    <row r="4070" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4070" t="s">
+        <v>4068</v>
+      </c>
+      <c r="B4070" t="s">
+        <v>4068</v>
+      </c>
+    </row>
+    <row r="4071" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4071" t="s">
+        <v>4069</v>
+      </c>
+      <c r="B4071" t="s">
+        <v>4069</v>
+      </c>
+    </row>
+    <row r="4072" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4072" t="s">
+        <v>4070</v>
+      </c>
+      <c r="B4072" t="s">
+        <v>4070</v>
+      </c>
+    </row>
+    <row r="4073" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4073" t="s">
+        <v>4071</v>
+      </c>
+      <c r="B4073" t="s">
+        <v>4071</v>
+      </c>
+    </row>
+    <row r="4074" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4074" t="s">
+        <v>4072</v>
+      </c>
+      <c r="B4074" t="s">
+        <v>4072</v>
+      </c>
+    </row>
+    <row r="4075" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4075" t="s">
+        <v>4073</v>
+      </c>
+      <c r="B4075" t="s">
+        <v>4073</v>
+      </c>
+    </row>
+    <row r="4076" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4076" t="s">
+        <v>4074</v>
+      </c>
+      <c r="B4076" t="s">
+        <v>4074</v>
+      </c>
+    </row>
+    <row r="4077" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4077" t="s">
+        <v>4075</v>
+      </c>
+      <c r="B4077" t="s">
+        <v>4075</v>
+      </c>
+    </row>
+    <row r="4078" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4078" t="s">
+        <v>4076</v>
+      </c>
+      <c r="B4078" t="s">
+        <v>4076</v>
+      </c>
+    </row>
+    <row r="4079" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4079" t="s">
+        <v>4077</v>
+      </c>
+      <c r="B4079" t="s">
+        <v>4077</v>
+      </c>
+    </row>
+    <row r="4080" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4080" t="s">
+        <v>4078</v>
+      </c>
+      <c r="B4080" t="s">
+        <v>4078</v>
+      </c>
+    </row>
+    <row r="4081" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4081" t="s">
+        <v>4079</v>
+      </c>
+      <c r="B4081" t="s">
+        <v>4079</v>
+      </c>
+    </row>
+    <row r="4082" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4082" t="s">
+        <v>4080</v>
+      </c>
+      <c r="B4082" t="s">
+        <v>4080</v>
+      </c>
+    </row>
+    <row r="4083" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4083" t="s">
+        <v>4081</v>
+      </c>
+      <c r="B4083" t="s">
+        <v>4081</v>
+      </c>
+    </row>
+    <row r="4084" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4084" t="s">
+        <v>4082</v>
+      </c>
+      <c r="B4084" t="s">
+        <v>4082</v>
+      </c>
+    </row>
+    <row r="4085" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4085" t="s">
+        <v>4083</v>
+      </c>
+      <c r="B4085" t="s">
+        <v>4083</v>
+      </c>
+    </row>
+    <row r="4086" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4086" t="s">
+        <v>4084</v>
+      </c>
+      <c r="B4086" t="s">
+        <v>4084</v>
+      </c>
+    </row>
+    <row r="4087" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4087" t="s">
+        <v>4085</v>
+      </c>
+      <c r="B4087" t="s">
+        <v>4085</v>
+      </c>
+    </row>
+    <row r="4088" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4088" t="s">
+        <v>4086</v>
+      </c>
+      <c r="B4088" t="s">
+        <v>4086</v>
+      </c>
+    </row>
+    <row r="4089" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4089" t="s">
+        <v>4087</v>
+      </c>
+      <c r="B4089" t="s">
+        <v>4087</v>
+      </c>
+    </row>
+    <row r="4090" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4090" t="s">
+        <v>4088</v>
+      </c>
+      <c r="B4090" t="s">
+        <v>4088</v>
+      </c>
+    </row>
+    <row r="4091" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4091" t="s">
+        <v>4089</v>
+      </c>
+      <c r="B4091" t="s">
+        <v>4089</v>
+      </c>
+    </row>
+    <row r="4092" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4092" t="s">
+        <v>4090</v>
+      </c>
+      <c r="B4092" t="s">
+        <v>4090</v>
+      </c>
+    </row>
+    <row r="4093" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4093" t="s">
+        <v>4091</v>
+      </c>
+      <c r="B4093" t="s">
+        <v>4091</v>
+      </c>
+    </row>
+    <row r="4094" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4094" t="s">
+        <v>4092</v>
+      </c>
+      <c r="B4094" t="s">
+        <v>4092</v>
+      </c>
+    </row>
+    <row r="4095" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4095" t="s">
+        <v>4093</v>
+      </c>
+      <c r="B4095" t="s">
+        <v>4093</v>
+      </c>
+    </row>
+    <row r="4096" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4096" t="s">
+        <v>4094</v>
+      </c>
+      <c r="B4096" t="s">
+        <v>4094</v>
+      </c>
+    </row>
+    <row r="4097" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4097" t="s">
+        <v>4095</v>
+      </c>
+      <c r="B4097" t="s">
+        <v>4095</v>
+      </c>
+    </row>
+    <row r="4098" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4098" t="s">
+        <v>4096</v>
+      </c>
+      <c r="B4098" t="s">
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="4099" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4099" t="s">
+        <v>4097</v>
+      </c>
+      <c r="B4099" t="s">
+        <v>4097</v>
+      </c>
+    </row>
+    <row r="4100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4100" t="s">
+        <v>4098</v>
+      </c>
+      <c r="B4100" t="s">
+        <v>4098</v>
+      </c>
+    </row>
+    <row r="4101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4101" t="s">
+        <v>4099</v>
+      </c>
+      <c r="B4101" t="s">
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="4102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4102" t="s">
+        <v>4100</v>
+      </c>
+      <c r="B4102" t="s">
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="4103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4103" t="s">
+        <v>4101</v>
+      </c>
+      <c r="B4103" t="s">
+        <v>4101</v>
+      </c>
+    </row>
+    <row r="4104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4104" t="s">
+        <v>4102</v>
+      </c>
+      <c r="B4104" t="s">
+        <v>4102</v>
+      </c>
+    </row>
+    <row r="4105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4105" t="s">
+        <v>4103</v>
+      </c>
+      <c r="B4105" t="s">
+        <v>4103</v>
+      </c>
+    </row>
+    <row r="4106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4106" t="s">
+        <v>4104</v>
+      </c>
+      <c r="B4106" t="s">
+        <v>4104</v>
+      </c>
+    </row>
+    <row r="4107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4107" t="s">
+        <v>4105</v>
+      </c>
+      <c r="B4107" t="s">
+        <v>4105</v>
+      </c>
+    </row>
+    <row r="4108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4108" t="s">
+        <v>4106</v>
+      </c>
+      <c r="B4108" t="s">
+        <v>4106</v>
+      </c>
+    </row>
+    <row r="4109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4109" t="s">
+        <v>4107</v>
+      </c>
+      <c r="B4109" t="s">
+        <v>4107</v>
+      </c>
+    </row>
+    <row r="4110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4110" t="s">
+        <v>4108</v>
+      </c>
+      <c r="B4110" t="s">
+        <v>4108</v>
+      </c>
+    </row>
+    <row r="4111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4111" t="s">
+        <v>4109</v>
+      </c>
+      <c r="B4111" t="s">
+        <v>4109</v>
+      </c>
+    </row>
+    <row r="4112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4112" t="s">
+        <v>4110</v>
+      </c>
+      <c r="B4112" t="s">
+        <v>4110</v>
+      </c>
+    </row>
+    <row r="4113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4113" t="s">
+        <v>4111</v>
+      </c>
+      <c r="B4113" t="s">
+        <v>4111</v>
+      </c>
+    </row>
+    <row r="4114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4114" t="s">
+        <v>4112</v>
+      </c>
+      <c r="B4114" t="s">
+        <v>4112</v>
+      </c>
+    </row>
+    <row r="4115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4115" t="s">
+        <v>4113</v>
+      </c>
+      <c r="B4115" t="s">
+        <v>4113</v>
+      </c>
+    </row>
+    <row r="4116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4116" t="s">
+        <v>4114</v>
+      </c>
+      <c r="B4116" t="s">
+        <v>4114</v>
+      </c>
+    </row>
+    <row r="4117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4117" t="s">
+        <v>4115</v>
+      </c>
+      <c r="B4117" t="s">
+        <v>4115</v>
+      </c>
+    </row>
+    <row r="4118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4118" t="s">
+        <v>4116</v>
+      </c>
+      <c r="B4118" t="s">
+        <v>4116</v>
+      </c>
+    </row>
+    <row r="4119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4119" t="s">
+        <v>4117</v>
+      </c>
+      <c r="B4119" t="s">
+        <v>4117</v>
+      </c>
+    </row>
+    <row r="4120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4120" t="s">
+        <v>4118</v>
+      </c>
+      <c r="B4120" t="s">
+        <v>4118</v>
+      </c>
+    </row>
+    <row r="4121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4121" t="s">
+        <v>4119</v>
+      </c>
+      <c r="B4121" t="s">
+        <v>4119</v>
+      </c>
+    </row>
+    <row r="4122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4122" t="s">
+        <v>4120</v>
+      </c>
+      <c r="B4122" t="s">
+        <v>4120</v>
+      </c>
+    </row>
+    <row r="4123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4123" t="s">
+        <v>4121</v>
+      </c>
+      <c r="B4123" t="s">
+        <v>4121</v>
+      </c>
+    </row>
+    <row r="4124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4124" t="s">
+        <v>4122</v>
+      </c>
+      <c r="B4124" t="s">
+        <v>4122</v>
+      </c>
+    </row>
+    <row r="4125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4125" t="s">
+        <v>4123</v>
+      </c>
+      <c r="B4125" t="s">
+        <v>4123</v>
+      </c>
+    </row>
+    <row r="4126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4126" t="s">
+        <v>4124</v>
+      </c>
+      <c r="B4126" t="s">
+        <v>4124</v>
+      </c>
+    </row>
+    <row r="4127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4127" t="s">
+        <v>4125</v>
+      </c>
+      <c r="B4127" t="s">
+        <v>4125</v>
+      </c>
+    </row>
+    <row r="4128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4128" t="s">
+        <v>4126</v>
+      </c>
+      <c r="B4128" t="s">
+        <v>4126</v>
+      </c>
+    </row>
+    <row r="4129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4129" t="s">
+        <v>4127</v>
+      </c>
+      <c r="B4129" t="s">
+        <v>4127</v>
+      </c>
+    </row>
+    <row r="4130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4130" t="s">
+        <v>4128</v>
+      </c>
+      <c r="B4130" t="s">
+        <v>4128</v>
+      </c>
+    </row>
+    <row r="4131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4131" t="s">
+        <v>4129</v>
+      </c>
+      <c r="B4131" t="s">
+        <v>4129</v>
+      </c>
+    </row>
+    <row r="4132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4132" t="s">
+        <v>4130</v>
+      </c>
+      <c r="B4132" t="s">
+        <v>4130</v>
+      </c>
+    </row>
+    <row r="4133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4133" t="s">
+        <v>4131</v>
+      </c>
+      <c r="B4133" t="s">
+        <v>4131</v>
+      </c>
+    </row>
+    <row r="4134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4134" t="s">
+        <v>4132</v>
+      </c>
+      <c r="B4134" t="s">
+        <v>4132</v>
+      </c>
+    </row>
+    <row r="4135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4135" t="s">
+        <v>4133</v>
+      </c>
+      <c r="B4135" t="s">
+        <v>4133</v>
+      </c>
+    </row>
+    <row r="4136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4136" t="s">
+        <v>4134</v>
+      </c>
+      <c r="B4136" t="s">
+        <v>4134</v>
+      </c>
+    </row>
+    <row r="4137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4137" t="s">
+        <v>4135</v>
+      </c>
+      <c r="B4137" t="s">
+        <v>4135</v>
+      </c>
+    </row>
+    <row r="4138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4138" t="s">
+        <v>4136</v>
+      </c>
+      <c r="B4138" t="s">
+        <v>4136</v>
+      </c>
+    </row>
+    <row r="4139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4139" t="s">
+        <v>4137</v>
+      </c>
+      <c r="B4139" t="s">
+        <v>4137</v>
+      </c>
+    </row>
+    <row r="4140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4140" t="s">
+        <v>4138</v>
+      </c>
+      <c r="B4140" t="s">
+        <v>4138</v>
+      </c>
+    </row>
+    <row r="4141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4141" t="s">
+        <v>4139</v>
+      </c>
+      <c r="B4141" t="s">
+        <v>4139</v>
+      </c>
+    </row>
+    <row r="4142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4142" t="s">
+        <v>4140</v>
+      </c>
+      <c r="B4142" t="s">
+        <v>4140</v>
+      </c>
+    </row>
+    <row r="4143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4143" t="s">
+        <v>4141</v>
+      </c>
+      <c r="B4143" t="s">
+        <v>4141</v>
+      </c>
+    </row>
+    <row r="4144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4144" t="s">
+        <v>4142</v>
+      </c>
+      <c r="B4144" t="s">
+        <v>4142</v>
+      </c>
+    </row>
+    <row r="4145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4145" t="s">
+        <v>4143</v>
+      </c>
+      <c r="B4145" t="s">
+        <v>4143</v>
+      </c>
+    </row>
+    <row r="4146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4146" t="s">
+        <v>4144</v>
+      </c>
+      <c r="B4146" t="s">
+        <v>4144</v>
+      </c>
+    </row>
+    <row r="4147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4147" t="s">
+        <v>4145</v>
+      </c>
+      <c r="B4147" t="s">
+        <v>4145</v>
+      </c>
+    </row>
+    <row r="4148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4148" t="s">
+        <v>4146</v>
+      </c>
+      <c r="B4148" t="s">
+        <v>4146</v>
+      </c>
+    </row>
+    <row r="4149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4149" t="s">
+        <v>4147</v>
+      </c>
+      <c r="B4149" t="s">
+        <v>4147</v>
+      </c>
+    </row>
+    <row r="4150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4150" t="s">
+        <v>4148</v>
+      </c>
+      <c r="B4150" t="s">
+        <v>4148</v>
+      </c>
+    </row>
+    <row r="4151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4151" t="s">
+        <v>4149</v>
+      </c>
+      <c r="B4151" t="s">
+        <v>4149</v>
+      </c>
+    </row>
+    <row r="4152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4152" t="s">
+        <v>4150</v>
+      </c>
+      <c r="B4152" t="s">
+        <v>4150</v>
+      </c>
+    </row>
+    <row r="4153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4153" t="s">
+        <v>4151</v>
+      </c>
+      <c r="B4153" t="s">
+        <v>4151</v>
+      </c>
+    </row>
+    <row r="4154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4154" t="s">
+        <v>4152</v>
+      </c>
+      <c r="B4154" t="s">
+        <v>4152</v>
+      </c>
+    </row>
+    <row r="4155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4155" t="s">
+        <v>4153</v>
+      </c>
+      <c r="B4155" t="s">
+        <v>4153</v>
+      </c>
+    </row>
+    <row r="4156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4156" t="s">
+        <v>4154</v>
+      </c>
+      <c r="B4156" t="s">
+        <v>4154</v>
+      </c>
+    </row>
+    <row r="4157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4157" t="s">
+        <v>4155</v>
+      </c>
+      <c r="B4157" t="s">
+        <v>4155</v>
+      </c>
+    </row>
+    <row r="4158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4158" t="s">
+        <v>4156</v>
+      </c>
+      <c r="B4158" t="s">
+        <v>4156</v>
+      </c>
+    </row>
+    <row r="4159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4159" t="s">
+        <v>4157</v>
+      </c>
+      <c r="B4159" t="s">
+        <v>4157</v>
+      </c>
+    </row>
+    <row r="4160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4160" t="s">
+        <v>4158</v>
+      </c>
+      <c r="B4160" t="s">
+        <v>4158</v>
+      </c>
+    </row>
+    <row r="4161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4161" t="s">
+        <v>4159</v>
+      </c>
+      <c r="B4161" t="s">
+        <v>4159</v>
+      </c>
+    </row>
+    <row r="4162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4162" t="s">
+        <v>4160</v>
+      </c>
+      <c r="B4162" t="s">
+        <v>4160</v>
+      </c>
+    </row>
+    <row r="4163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4163" t="s">
+        <v>4161</v>
+      </c>
+      <c r="B4163" t="s">
+        <v>4161</v>
+      </c>
+    </row>
+    <row r="4164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4164" t="s">
+        <v>4162</v>
+      </c>
+      <c r="B4164" t="s">
+        <v>4162</v>
+      </c>
+    </row>
+    <row r="4165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4165" t="s">
+        <v>4163</v>
+      </c>
+      <c r="B4165" t="s">
+        <v>4163</v>
+      </c>
+    </row>
+    <row r="4166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4166" t="s">
+        <v>4164</v>
+      </c>
+      <c r="B4166" t="s">
+        <v>4164</v>
+      </c>
+    </row>
+    <row r="4167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4167" t="s">
+        <v>4165</v>
+      </c>
+      <c r="B4167" t="s">
+        <v>4165</v>
+      </c>
+    </row>
+    <row r="4168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4168" t="s">
+        <v>4166</v>
+      </c>
+      <c r="B4168" t="s">
+        <v>4166</v>
+      </c>
+    </row>
+    <row r="4169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4169" t="s">
+        <v>4167</v>
+      </c>
+      <c r="B4169" t="s">
+        <v>4167</v>
+      </c>
+    </row>
+    <row r="4170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4170" t="s">
+        <v>4168</v>
+      </c>
+      <c r="B4170" t="s">
+        <v>4168</v>
+      </c>
+    </row>
+    <row r="4171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4171" t="s">
+        <v>4169</v>
+      </c>
+      <c r="B4171" t="s">
+        <v>4169</v>
+      </c>
+    </row>
+    <row r="4172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4172" t="s">
+        <v>4170</v>
+      </c>
+      <c r="B4172" t="s">
+        <v>4170</v>
+      </c>
+    </row>
+    <row r="4173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4173" t="s">
+        <v>4171</v>
+      </c>
+      <c r="B4173" t="s">
+        <v>4171</v>
+      </c>
+    </row>
+    <row r="4174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4174" t="s">
+        <v>4172</v>
+      </c>
+      <c r="B4174" t="s">
+        <v>4172</v>
+      </c>
+    </row>
+    <row r="4175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4175" t="s">
+        <v>4173</v>
+      </c>
+      <c r="B4175" t="s">
+        <v>4173</v>
+      </c>
+    </row>
+    <row r="4176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4176" t="s">
+        <v>4174</v>
+      </c>
+      <c r="B4176" t="s">
+        <v>4174</v>
+      </c>
+    </row>
+    <row r="4177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4177" t="s">
+        <v>4175</v>
+      </c>
+      <c r="B4177" t="s">
+        <v>4175</v>
+      </c>
+    </row>
+    <row r="4178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4178" t="s">
+        <v>4176</v>
+      </c>
+      <c r="B4178" t="s">
+        <v>4176</v>
+      </c>
+    </row>
+    <row r="4179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4179" t="s">
+        <v>4177</v>
+      </c>
+      <c r="B4179" t="s">
+        <v>4177</v>
+      </c>
+    </row>
+    <row r="4180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4180" t="s">
+        <v>4178</v>
+      </c>
+      <c r="B4180" t="s">
+        <v>4178</v>
+      </c>
+    </row>
+    <row r="4181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4181" t="s">
+        <v>4179</v>
+      </c>
+      <c r="B4181" t="s">
+        <v>4179</v>
+      </c>
+    </row>
+    <row r="4182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4182" t="s">
+        <v>4180</v>
+      </c>
+      <c r="B4182" t="s">
+        <v>4180</v>
+      </c>
+    </row>
+    <row r="4183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4183" t="s">
+        <v>4181</v>
+      </c>
+      <c r="B4183" t="s">
+        <v>4181</v>
+      </c>
+    </row>
+    <row r="4184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4184" t="s">
+        <v>4182</v>
+      </c>
+      <c r="B4184" t="s">
+        <v>4182</v>
+      </c>
+    </row>
+    <row r="4185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4185" t="s">
+        <v>4183</v>
+      </c>
+      <c r="B4185" t="s">
+        <v>4183</v>
+      </c>
+    </row>
+    <row r="4186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4186" t="s">
+        <v>4184</v>
+      </c>
+      <c r="B4186" t="s">
+        <v>4184</v>
+      </c>
+    </row>
+    <row r="4187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4187" t="s">
+        <v>4185</v>
+      </c>
+      <c r="B4187" t="s">
+        <v>4185</v>
+      </c>
+    </row>
+    <row r="4188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4188" t="s">
+        <v>4186</v>
+      </c>
+      <c r="B4188" t="s">
+        <v>4186</v>
+      </c>
+    </row>
+    <row r="4189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4189" t="s">
+        <v>4187</v>
+      </c>
+      <c r="B4189" t="s">
+        <v>4187</v>
+      </c>
+    </row>
+    <row r="4190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4190" t="s">
+        <v>4188</v>
+      </c>
+      <c r="B4190" t="s">
+        <v>4188</v>
+      </c>
+    </row>
+    <row r="4191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4191" t="s">
+        <v>4189</v>
+      </c>
+      <c r="B4191" t="s">
+        <v>4189</v>
+      </c>
+    </row>
+    <row r="4192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4192" t="s">
+        <v>4190</v>
+      </c>
+      <c r="B4192" t="s">
+        <v>4190</v>
+      </c>
+    </row>
+    <row r="4193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4193" t="s">
+        <v>4191</v>
+      </c>
+      <c r="B4193" t="s">
+        <v>4191</v>
+      </c>
+    </row>
+    <row r="4194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4194" t="s">
+        <v>4192</v>
+      </c>
+      <c r="B4194" t="s">
+        <v>4192</v>
+      </c>
+    </row>
+    <row r="4195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4195" t="s">
+        <v>4193</v>
+      </c>
+      <c r="B4195" t="s">
+        <v>4193</v>
+      </c>
+    </row>
+    <row r="4196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4196" t="s">
+        <v>4194</v>
+      </c>
+      <c r="B4196" t="s">
+        <v>4194</v>
+      </c>
+    </row>
+    <row r="4197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4197" t="s">
+        <v>4195</v>
+      </c>
+      <c r="B4197" t="s">
+        <v>4195</v>
+      </c>
+    </row>
+    <row r="4198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4198" t="s">
+        <v>4196</v>
+      </c>
+      <c r="B4198" t="s">
+        <v>4196</v>
+      </c>
+    </row>
+    <row r="4199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4199" t="s">
+        <v>4197</v>
+      </c>
+      <c r="B4199" t="s">
+        <v>4197</v>
+      </c>
+    </row>
+    <row r="4200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4200" t="s">
+        <v>4198</v>
+      </c>
+      <c r="B4200" t="s">
+        <v>4198</v>
+      </c>
+    </row>
+    <row r="4201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4201" t="s">
+        <v>4199</v>
+      </c>
+      <c r="B4201" t="s">
+        <v>4199</v>
+      </c>
+    </row>
+    <row r="4202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4202" t="s">
+        <v>4200</v>
+      </c>
+      <c r="B4202" t="s">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="4203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4203" t="s">
+        <v>4201</v>
+      </c>
+      <c r="B4203" t="s">
+        <v>4201</v>
+      </c>
+    </row>
+    <row r="4204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4204" t="s">
+        <v>4202</v>
+      </c>
+      <c r="B4204" t="s">
+        <v>4202</v>
+      </c>
+    </row>
+    <row r="4205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4205" t="s">
+        <v>4203</v>
+      </c>
+      <c r="B4205" t="s">
+        <v>4203</v>
+      </c>
+    </row>
+    <row r="4206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4206" t="s">
+        <v>4204</v>
+      </c>
+      <c r="B4206" t="s">
+        <v>4204</v>
+      </c>
+    </row>
+    <row r="4207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4207" t="s">
+        <v>4205</v>
+      </c>
+      <c r="B4207" t="s">
+        <v>4205</v>
+      </c>
+    </row>
+    <row r="4208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4208" t="s">
+        <v>4206</v>
+      </c>
+      <c r="B4208" t="s">
+        <v>4206</v>
+      </c>
+    </row>
+    <row r="4209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4209" t="s">
+        <v>4207</v>
+      </c>
+      <c r="B4209" t="s">
+        <v>4207</v>
+      </c>
+    </row>
+    <row r="4210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4210" t="s">
+        <v>4208</v>
+      </c>
+      <c r="B4210" t="s">
+        <v>4208</v>
+      </c>
+    </row>
+    <row r="4211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4211" t="s">
+        <v>4209</v>
+      </c>
+      <c r="B4211" t="s">
+        <v>4209</v>
+      </c>
+    </row>
+    <row r="4212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4212" t="s">
+        <v>4210</v>
+      </c>
+      <c r="B4212" t="s">
+        <v>4210</v>
+      </c>
+    </row>
+    <row r="4213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4213" t="s">
+        <v>4211</v>
+      </c>
+      <c r="B4213" t="s">
+        <v>4211</v>
+      </c>
+    </row>
+    <row r="4214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4214" t="s">
+        <v>4212</v>
+      </c>
+      <c r="B4214" t="s">
+        <v>4212</v>
+      </c>
+    </row>
+    <row r="4215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4215" t="s">
+        <v>4213</v>
+      </c>
+      <c r="B4215" t="s">
+        <v>4213</v>
+      </c>
+    </row>
+    <row r="4216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4216" t="s">
+        <v>4214</v>
+      </c>
+      <c r="B4216" t="s">
+        <v>4214</v>
+      </c>
+    </row>
+    <row r="4217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4217" t="s">
+        <v>4215</v>
+      </c>
+      <c r="B4217" t="s">
+        <v>4215</v>
+      </c>
+    </row>
+    <row r="4218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4218" t="s">
+        <v>4216</v>
+      </c>
+      <c r="B4218" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="4219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4219" t="s">
+        <v>4217</v>
+      </c>
+      <c r="B4219" t="s">
+        <v>4217</v>
+      </c>
+    </row>
+    <row r="4220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4220" t="s">
+        <v>4218</v>
+      </c>
+      <c r="B4220" t="s">
+        <v>4218</v>
+      </c>
+    </row>
+    <row r="4221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4221" t="s">
+        <v>4219</v>
+      </c>
+      <c r="B4221" t="s">
+        <v>4219</v>
+      </c>
+    </row>
+    <row r="4222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4222" t="s">
+        <v>4220</v>
+      </c>
+      <c r="B4222" t="s">
+        <v>4220</v>
+      </c>
+    </row>
+    <row r="4223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4223" t="s">
+        <v>4221</v>
+      </c>
+      <c r="B4223" t="s">
+        <v>4221</v>
+      </c>
+    </row>
+    <row r="4224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4224" t="s">
+        <v>4222</v>
+      </c>
+      <c r="B4224" t="s">
+        <v>4222</v>
+      </c>
+    </row>
+    <row r="4225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4225" t="s">
+        <v>4223</v>
+      </c>
+      <c r="B4225" t="s">
+        <v>4223</v>
+      </c>
+    </row>
+    <row r="4226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4226" t="s">
+        <v>4224</v>
+      </c>
+      <c r="B4226" t="s">
+        <v>4224</v>
+      </c>
+    </row>
+    <row r="4227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4227" t="s">
+        <v>4225</v>
+      </c>
+      <c r="B4227" t="s">
+        <v>4225</v>
+      </c>
+    </row>
+    <row r="4228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4228" t="s">
+        <v>981</v>
+      </c>
+      <c r="B4228" t="s">
+        <v>981</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:B3748">
     <sortCondition ref="A1:A3748"/>
   </sortState>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  <conditionalFormatting sqref="A1:A4190 A6736:A1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3741">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B4190 B6736:B1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Luận hoàn thiện giờ chỉ cần thêm các cách cục cho 12 cung
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9BED4C-740D-4B7E-8858-AEC573F60A39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A580F7E-BA28-4845-B6E3-724A1B04F669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8454" uniqueCount="4226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8458" uniqueCount="4229">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -12703,6 +12703,15 @@
   </si>
   <si>
     <t>Tang Môn toạ thủ cung Mệnh tại Dậu</t>
+  </si>
+  <si>
+    <t>Binh Hình Tướng Ấn hội chiếu tại Mệnh</t>
+  </si>
+  <si>
+    <t>Kình Đà hội chiếu tại Mệnh</t>
+  </si>
+  <si>
+    <t>Tang Hổ hội chiếu tại Mệnh</t>
   </si>
 </sst>
 </file>
@@ -13051,10 +13060,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B4228"/>
+  <dimension ref="A1:B4230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4203" workbookViewId="0">
-      <selection activeCell="O4212" sqref="O4212"/>
+    <sheetView tabSelected="1" topLeftCell="A4207" workbookViewId="0">
+      <selection activeCell="B4230" sqref="B4230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43144,7 +43153,7 @@
     </row>
     <row r="3762" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3762" t="s">
-        <v>3760</v>
+        <v>4226</v>
       </c>
       <c r="B3762" t="s">
         <v>3760</v>
@@ -46876,6 +46885,22 @@
       </c>
       <c r="B4228" t="s">
         <v>981</v>
+      </c>
+    </row>
+    <row r="4229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4229" t="s">
+        <v>4227</v>
+      </c>
+      <c r="B4229" t="s">
+        <v>4227</v>
+      </c>
+    </row>
+    <row r="4230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4230" t="s">
+        <v>4228</v>
+      </c>
+      <c r="B4230" t="s">
+        <v>4228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hoàn Thiện fiel excel luận
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A580F7E-BA28-4845-B6E3-724A1B04F669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E880F47F-A409-4C03-A9DC-C86BED50BF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8458" uniqueCount="4229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8462" uniqueCount="4231">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -12712,6 +12712,12 @@
   </si>
   <si>
     <t>Tang Hổ hội chiếu tại Mệnh</t>
+  </si>
+  <si>
+    <t>Hình Riêu Y hội chiếu tại Mệnh</t>
+  </si>
+  <si>
+    <t>Hình Riêu hội chiếu tại Mệnh</t>
   </si>
 </sst>
 </file>
@@ -13060,10 +13066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B4230"/>
+  <dimension ref="A1:B4232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4207" workbookViewId="0">
-      <selection activeCell="B4230" sqref="B4230"/>
+    <sheetView tabSelected="1" topLeftCell="A4209" workbookViewId="0">
+      <selection activeCell="B4232" sqref="B4232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46901,6 +46907,22 @@
       </c>
       <c r="B4230" t="s">
         <v>4228</v>
+      </c>
+    </row>
+    <row r="4231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4231" t="s">
+        <v>4229</v>
+      </c>
+      <c r="B4231" t="s">
+        <v>4229</v>
+      </c>
+    </row>
+    <row r="4232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4232" t="s">
+        <v>4230</v>
+      </c>
+      <c r="B4232" t="s">
+        <v>4230</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Luận thêm phần cung chính vô chính diệu
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1858A52B-0974-4067-B33A-294F87ADE4CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E86C37-4329-409F-87A1-3E978BBC2AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12978,67 +12978,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -13367,8 +13307,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
   <dimension ref="A1:B4305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4281" workbookViewId="0">
-      <selection activeCell="B4305" sqref="B4305"/>
+    <sheetView tabSelected="1" topLeftCell="A4293" workbookViewId="0">
+      <selection activeCell="A4307" sqref="A4307:A4320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -47814,13 +47754,13 @@
   </sortState>
   <dataConsolidate/>
   <conditionalFormatting sqref="A1:A4190 A6736:A1048576">
-    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3741">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A4305 A4313:A1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B4190 B6736:B1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>

</xml_diff>

<commit_message>
Giẩi thích Ân Quang tại mệnh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B323ADF7-F2C2-44CB-BB88-4B6502C3E204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB2539E-4F47-4FA5-9065-516069560B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8818" uniqueCount="4409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8835" uniqueCount="4437">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13252,6 +13252,90 @@
   </si>
   <si>
     <t>Thất Sát đồng cung Phá Quân tại cung đối Thiên Di</t>
+  </si>
+  <si>
+    <t>Bạn có diện mạo phúc hậu, hiền từ, mặt mũi thường sáng sủa, thông minh, khiến mọi người xung quanh luôn có thiện cảm, hành động luôn từ tốn, chừng mực, không bao giờ vội vàng hay hấp tấp.</t>
+  </si>
+  <si>
+    <t>Bạn là người có tính nhân hậu, lòng từ thiện, sự hên, may mắn, có sự thành tín với bạn bè, hiếu lễ đối với cha mẹ, chung thủy với vợ, chồng. Bạn là người điềm đạm, thông minh, ưa học hỏi. Người có thiện tâm, chính tâm, thiện lành, không hại ai cho nên ít bị người hại, tin tưởng vào phúc đức và nhân quả, được thần linh che chở cho một cách vô hình.</t>
+  </si>
+  <si>
+    <t>Bạn gặp nhiều may mắn và sống thọ. Có sự che chở của Trời Phật hay Linh Thiêng. Bạn là người làm nhiều phước báu để giúp đời, cứu người, vậy nên khi gặp họa thường được người trả ơn, người khác cứu, có bệnh thì gặp bác sĩ giỏi chữa, uống thuốc thang mau lành.</t>
+  </si>
+  <si>
+    <t>Cha mẹ là người hiền lương, tiết hạnh, được nhiều người kính mến. Cha mẹ là người thích tu tập, tìm hiểu tâm linh, Phật pháp, ưa làm việc thiện, Phật tánh cao. Cha mẹ là người có học thức, có chiều sâu, dạy dỗ con cái tốt, đáng để con cái noi theo và học tập.</t>
+  </si>
+  <si>
+    <t>Bạn có phúc dày, là người được thần linh che chở, ước gì được nấy, sống thọ. Họ hàng mọi người đoàn kết, đùm bọc nhau. Ông bà tổ tiên và dòng họ nhiều người hiền lương, tiết hạnh, ăn ở phúc đức, từ thiện được nhiều người nhớ ơn, nợ ân huệ, tới đời mình được hưởng</t>
+  </si>
+  <si>
+    <t>Gia đình người hôn phối là người lương thiện, hiền lành, nhiều phước đức, được người đời nể trọng.</t>
+  </si>
+  <si>
+    <t>Bạn làm từ thiện mà không mưu cầu danh lợi, từ bé đã có tính thương người, biết lo lắng quan tâm đến người khác, biết chăm sóc nơi thờ cúng, hiếu lễ với tổ tiên.</t>
+  </si>
+  <si>
+    <t>Mồ  yên mả đẹp, dòng họ có nhà thờ rất đẹp và linh thiêng.</t>
+  </si>
+  <si>
+    <t>Bạn gặp nhiều may mắn, sau này dễ kết hôn vào gia đình danh giá, được tổ tiên phù hộ, nâng đỡ rất nhiều, đương số được hưởng phước báu của tổ tiên để lại.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gia đình gia giáo, hạnh phúc, yên ấm, trên dưới rõ ràng, phép tắc, lễ độ.</t>
+  </si>
+  <si>
+    <t>Bạn được hưởng di sản (nhà, đất) của tổ phụ, của cha mẹ để lại. Bạn có thể dùng tài sản, đất đai nhà cửa để làm từ thiện, giúp đời.</t>
+  </si>
+  <si>
+    <t>Bạn là người hay giúp đỡ đồng nghiệp, lấy chí thành mà đãi người. Bạn cũng hay được nâng đỡ, người có chỗ làm, nghề nghiệp đúng sở thích, hay được may mắn trong quan trường, sự nghiệp.</t>
+  </si>
+  <si>
+    <t>Môi trường công việc thanh lương, trong sạch, không ưa cạnh tranh, kèn cựa, không bao giờ làm điều ác hay bất nhân để đạt được mục đích, do vậy nên rất được mọi người tin tưởng và ngưỡng mộ.</t>
+  </si>
+  <si>
+    <t>Bạn có người bạn, người phụ tá hợp tác đắc lực và trung tín. Bạn có bạn bè tốt quí mến, giúp đỡ tận tình, được nhiều thuộc quyền phò tá, nhiều nhân tình thương yêu.</t>
+  </si>
+  <si>
+    <t>Bạn ra ngoài thường thiện lương, điềm đạm, hay giúp người, từ thiện nên được nhiều người quý mến, kính trọng.</t>
+  </si>
+  <si>
+    <t>Bạn là người sinh phùng thời, được may mắn, hên ở xã hội, khi gặp vấn đề gì hay cầm trợ giúp gì luôn có quý nhân hỗ trợ, giúp đỡ.</t>
+  </si>
+  <si>
+    <t>Bạn ra ngoài hay có duyên gặp các vị cao nhân, người thầy quý giúp đỡ chỉ dạy.</t>
+  </si>
+  <si>
+    <t>Bạn luôn gặp giải trừ bệnh tật, tai họa, có bệnh thì chóng khỏi, gặp thầy giỏi, thuốc hay. Khi bệnh tật tai họa tới thường gặp may mắn mà thoát. Có thể tu tập, từ thiện để giảm bớt tai họa và bệnh tật cho mình.</t>
+  </si>
+  <si>
+    <t>Bạn thường được người giúp đỡ tiền bạc, của cải, người hay được nhiều may mắn về tiền bạc, có thể được hưởng di sản.</t>
+  </si>
+  <si>
+    <t>Cách kiếm tiền bằng sự lương thiện, không cạnh tranh hay làm việc trái với đạo lý.</t>
+  </si>
+  <si>
+    <t>Con cái có hiếu với cha mẹ và được cha mẹ thương yêu, về già con cái chăm sóc cha mẹ. Con cái là người tốt, hiếu lễ, thiện lương, thông minh, học cao hiểu rộng, có chiều sâu, được nhiều người kính trọng và quý mến.</t>
+  </si>
+  <si>
+    <t>Những duyên nghiệp tốt mà mình gieo thì sau này con cái sẽ được hưởng lại.</t>
+  </si>
+  <si>
+    <t>Vợ chồng yêu nhau trong một thời gian dài mới đến hôn nhân, vợ chồng xứng nứa vừa đôi, vợ chồng có ân tình, ân nghĩa với nhau, đây cũng là bộ sao hóa giải nghiệp của Vợ Chồng vì thế cho dù có xung khắc thế nào thì cuối cùng vợ chồng cũng ở với nhau đến già.</t>
+  </si>
+  <si>
+    <t>Người hôn phối là người thiện lương, ôn hòa, hay thích làm phúc, tu tập, mặt mũi thường phúc hậu. Người sẵn sàng chịu đựng khổ đau vất vả để đi cùng mình tới cuối đời.</t>
+  </si>
+  <si>
+    <t>Hôn nhân hạnh phúc, vợ chồng hòa thuận và thương yêu nhau, chịu đựng được nghịch cảnh mà lòng dạ sắt son, Tình nghĩa vợ chồng bền lâu, biết nhường nhịn nhau, ít khi cãi cọ, cưới nhau về rồi sống với nhau bằng tình nghĩa.</t>
+  </si>
+  <si>
+    <t>Người hôn phối là người hay làm phúc, giúp đời, được nhiều người kính mến, nể trọng. Có thể làm các ngành nghề liên quan tới thầy thuốc, bác sỹ, thầy giáo</t>
+  </si>
+  <si>
+    <t>Anh chị em tình cảm, hòa thuận và giúp đỡ lẫn nhau. Anh chị em sống tình nghĩa, thích tu tập, hay dang rộng vòng tay cứu người, được nhiều người mến mộ và kính trọng.</t>
+  </si>
+  <si>
+    <t>Ân Quang Thiên Quý Thai Cáo hội chiếu tại Mệnh</t>
   </si>
 </sst>
 </file>
@@ -13267,12 +13351,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -13287,8 +13377,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13620,114 +13711,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B4412"/>
+  <dimension ref="A1:F4413"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4293" workbookViewId="0">
-      <selection activeCell="B4322" sqref="B4322:B4412"/>
+    <sheetView tabSelected="1" topLeftCell="A4380" workbookViewId="0">
+      <selection activeCell="D4414" sqref="D4414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>2164</v>
       </c>
       <c r="B1" t="s">
-        <v>2164</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+        <v>4419</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4418</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2171</v>
       </c>
       <c r="B2" t="s">
-        <v>2171</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+        <v>4435</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2161</v>
       </c>
       <c r="B3" t="s">
-        <v>2161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+        <v>4409</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4410</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4411</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2166</v>
       </c>
       <c r="B4" t="s">
-        <v>2166</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+        <v>4422</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2162</v>
       </c>
       <c r="B5" t="s">
-        <v>2162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+        <v>4412</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>2170</v>
       </c>
       <c r="B6" t="s">
-        <v>2170</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <v>4433</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4431</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4432</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4434</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>2163</v>
       </c>
       <c r="B7" t="s">
-        <v>2163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+        <v>4413</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4414</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4415</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4416</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4417</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>2165</v>
       </c>
       <c r="B8" t="s">
-        <v>2165</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <v>4420</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4421</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>2168</v>
       </c>
       <c r="B9" t="s">
-        <v>2168</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+        <v>4427</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4428</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>2167</v>
       </c>
       <c r="B10" t="s">
-        <v>2167</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+        <v>4426</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>1594</v>
       </c>
       <c r="B11" t="s">
-        <v>1594</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+        <v>4424</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4423</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4425</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>2169</v>
       </c>
       <c r="B12" t="s">
-        <v>2169</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4429</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4430</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3741</v>
       </c>
@@ -13735,7 +13872,7 @@
         <v>3741</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3742</v>
       </c>
@@ -13743,7 +13880,7 @@
         <v>3742</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3743</v>
       </c>
@@ -13751,7 +13888,7 @@
         <v>3743</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3744</v>
       </c>
@@ -48901,6 +49038,14 @@
       </c>
       <c r="B4412" t="s">
         <v>4408</v>
+      </c>
+    </row>
+    <row r="4413" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4413" t="s">
+        <v>4436</v>
+      </c>
+      <c r="B4413" t="s">
+        <v>4436</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Giải thích về Thiên Quý tại các cung
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB2539E-4F47-4FA5-9065-516069560B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C530953-1DA4-446B-9423-2C50DDED305F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8835" uniqueCount="4437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8850" uniqueCount="4437">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13713,8 +13713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
   <dimension ref="A1:F4413"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4380" workbookViewId="0">
-      <selection activeCell="D4414" sqref="D4414"/>
+    <sheetView tabSelected="1" topLeftCell="A2977" workbookViewId="0">
+      <selection activeCell="F2996" sqref="F2996"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37576,7 +37576,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="2977" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2977" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2977" t="s">
         <v>2279</v>
       </c>
@@ -37584,7 +37584,7 @@
         <v>2279</v>
       </c>
     </row>
-    <row r="2978" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2978" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2978" t="s">
         <v>2278</v>
       </c>
@@ -37592,7 +37592,7 @@
         <v>2278</v>
       </c>
     </row>
-    <row r="2979" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2979" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2979" t="s">
         <v>2281</v>
       </c>
@@ -37600,103 +37600,148 @@
         <v>2281</v>
       </c>
     </row>
-    <row r="2980" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2980" t="s">
+    <row r="2980" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2980" s="1" t="s">
         <v>2153</v>
       </c>
       <c r="B2980" t="s">
-        <v>2153</v>
-      </c>
-    </row>
-    <row r="2981" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2981" t="s">
+        <v>4419</v>
+      </c>
+      <c r="C2980" t="s">
+        <v>4418</v>
+      </c>
+    </row>
+    <row r="2981" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2981" s="1" t="s">
         <v>2160</v>
       </c>
       <c r="B2981" t="s">
-        <v>2160</v>
-      </c>
-    </row>
-    <row r="2982" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2982" t="s">
+        <v>4435</v>
+      </c>
+    </row>
+    <row r="2982" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2982" s="1" t="s">
         <v>2150</v>
       </c>
       <c r="B2982" t="s">
-        <v>2150</v>
-      </c>
-    </row>
-    <row r="2983" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2983" t="s">
+        <v>4409</v>
+      </c>
+      <c r="C2982" t="s">
+        <v>4410</v>
+      </c>
+      <c r="D2982" t="s">
+        <v>4411</v>
+      </c>
+    </row>
+    <row r="2983" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2983" s="1" t="s">
         <v>2155</v>
       </c>
       <c r="B2983" t="s">
-        <v>2155</v>
-      </c>
-    </row>
-    <row r="2984" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2984" t="s">
+        <v>4422</v>
+      </c>
+    </row>
+    <row r="2984" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2984" s="1" t="s">
         <v>2151</v>
       </c>
       <c r="B2984" t="s">
-        <v>2151</v>
-      </c>
-    </row>
-    <row r="2985" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2985" t="s">
+        <v>4412</v>
+      </c>
+    </row>
+    <row r="2985" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2985" s="1" t="s">
         <v>2159</v>
       </c>
       <c r="B2985" t="s">
-        <v>2159</v>
-      </c>
-    </row>
-    <row r="2986" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2986" t="s">
+        <v>4433</v>
+      </c>
+      <c r="C2985" t="s">
+        <v>4431</v>
+      </c>
+      <c r="D2985" t="s">
+        <v>4432</v>
+      </c>
+      <c r="E2985" t="s">
+        <v>4434</v>
+      </c>
+    </row>
+    <row r="2986" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2986" s="1" t="s">
         <v>2152</v>
       </c>
       <c r="B2986" t="s">
-        <v>2152</v>
-      </c>
-    </row>
-    <row r="2987" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2987" t="s">
+        <v>4413</v>
+      </c>
+      <c r="C2986" t="s">
+        <v>4414</v>
+      </c>
+      <c r="D2986" t="s">
+        <v>4415</v>
+      </c>
+      <c r="E2986" t="s">
+        <v>4416</v>
+      </c>
+      <c r="F2986" t="s">
+        <v>4417</v>
+      </c>
+    </row>
+    <row r="2987" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2987" s="1" t="s">
         <v>2154</v>
       </c>
       <c r="B2987" t="s">
-        <v>2154</v>
-      </c>
-    </row>
-    <row r="2988" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2988" t="s">
+        <v>4420</v>
+      </c>
+      <c r="C2987" t="s">
+        <v>4421</v>
+      </c>
+    </row>
+    <row r="2988" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2988" s="1" t="s">
         <v>2157</v>
       </c>
       <c r="B2988" t="s">
-        <v>2157</v>
-      </c>
-    </row>
-    <row r="2989" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2989" t="s">
+        <v>4427</v>
+      </c>
+      <c r="C2988" t="s">
+        <v>4428</v>
+      </c>
+    </row>
+    <row r="2989" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2989" s="1" t="s">
         <v>2156</v>
       </c>
       <c r="B2989" t="s">
-        <v>2156</v>
-      </c>
-    </row>
-    <row r="2990" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2990" t="s">
+        <v>4426</v>
+      </c>
+    </row>
+    <row r="2990" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2990" s="1" t="s">
         <v>1593</v>
       </c>
       <c r="B2990" t="s">
-        <v>1593</v>
-      </c>
-    </row>
-    <row r="2991" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2991" t="s">
+        <v>4424</v>
+      </c>
+      <c r="C2990" t="s">
+        <v>4423</v>
+      </c>
+      <c r="D2990" t="s">
+        <v>4425</v>
+      </c>
+    </row>
+    <row r="2991" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2991" s="1" t="s">
         <v>2158</v>
       </c>
       <c r="B2991" t="s">
-        <v>2158</v>
-      </c>
-    </row>
-    <row r="2992" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4429</v>
+      </c>
+      <c r="C2991" t="s">
+        <v>4430</v>
+      </c>
+    </row>
+    <row r="2992" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2992" t="s">
         <v>1855</v>
       </c>
@@ -49059,10 +49104,10 @@
   <conditionalFormatting sqref="A1:A4305 A4313:A1048576">
     <cfRule type="duplicateValues" dxfId="3" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B4190 B6736:B1048576">
+  <conditionalFormatting sqref="B6736:B1048576 B1:B4190">
     <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B4305 B4313:B1048576">
+  <conditionalFormatting sqref="B4313:B1048576 B1:B4305">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3741">

</xml_diff>

<commit_message>
Giải thích Bác Sỹ tại 12 cung
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550CACDD-4DD3-4A60-9688-0520322F0955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C32E5BD-EA48-4918-B8D7-3EEAAF0C548F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17698" uniqueCount="4447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8865" uniqueCount="4475">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13366,6 +13366,90 @@
   </si>
   <si>
     <t>Bạn bớt được nhiều tai nạn chứ không phải là chẳng bao giờ bị tai nạn. Dễ thích ứng với hoàn cảnh.</t>
+  </si>
+  <si>
+    <t>Bạn là người có học, từ bi sáng suốt, tăng thọ trường. Người thông minh, có sự suy xét kín đáo, khôn ngoan, khéo léo trong ngôn ngữ, có khả năng giải trừ các bệnh tật nhỏ</t>
+  </si>
+  <si>
+    <t>Thể hiện cuộc sống no ấm giàu bền, người được nhiều may mắn, có của tiền người khác để lại cho.</t>
+  </si>
+  <si>
+    <t>Bác Sỹ Âm Dương Xương Khúc Khoa hội chiếu tại Mệnh</t>
+  </si>
+  <si>
+    <t>Bạn học hành đỗ đạt cao.</t>
+  </si>
+  <si>
+    <t>Bác Sỹ Lương Tướng Quang Quý Thiên Phúc hội chiếu tại Mệnh</t>
+  </si>
+  <si>
+    <t>Bạn có thể làm  thầy giáo hoặc thầy thuốc giỏi</t>
+  </si>
+  <si>
+    <t>Cha mẹ là người có học thức, điềm đạm. Hội nhiều cát tinh thì càng giàu mạnh, làm chủ doanh nghiệp, làm quan</t>
+  </si>
+  <si>
+    <t>Bạn sinh ra trong gia đình cha mẹ có điều kiện, bản thân dễ bị ốm đau tật bệnh trên người. Cha mẹ có của để lại cho sau này.</t>
+  </si>
+  <si>
+    <t>Trong dòng họ nhiều người có học thức, giỏi giang, thành đạt. Trong dòng họ dễ có mồ kết mả phát, con cháu được sung túc, phú quý. Bản thân được nhận nhiều may mắn từ phúc đức tổ tiên, dễ được nhận của cải từ ông bà tổ tiên truyền lại.</t>
+  </si>
+  <si>
+    <t>Gia đình nhà người hôn phối là những người thành đạt, giỏi giang. Người hôn phối là người có chức quyền, cầm con dấu.</t>
+  </si>
+  <si>
+    <t>Bạn có lộc đất cát, có của cải điền sản tổ tiên để lại cho sau này. Bạn biết quan tâm chăm chút ngôi nhà. Bản thân nhà cửa đẹp đẽ, gọn gàng, sạch sẽ, có thư phòng.</t>
+  </si>
+  <si>
+    <t>Bạn có thiên hướng nghệ thuật thì dễ làm kiến trúc sư, kỹ sư chuyên thiết kế nhà cửa.</t>
+  </si>
+  <si>
+    <t>Bác Sỹ Cơ Đồng Xương Khúc Đào Hoa hội chiếu tại Điền Trạch</t>
+  </si>
+  <si>
+    <t>Bạn gặp nhiều may mắn trong công việc, công danh. Bản thân là người có tác phong làm việc điềm đạm,cẩn thận, kĩ lưỡng, thường cực tin tưởng đảm nhận nhiều chức vụ cao hoặc không cũng làm chủ doanh nghiệp.</t>
+  </si>
+  <si>
+    <t>Bạn hay được bạn bè, đồng nghiệp, cấp dưới giúp đỡ, tặng quà. Bạn bè hay mời ăn uống, nhậu nhẹt.</t>
+  </si>
+  <si>
+    <t>Bạn có lộc khi làm ăn, chung vốn với bạn bè.</t>
+  </si>
+  <si>
+    <t>Bạn có bạn bè là những người có học, chuyên môn tốt</t>
+  </si>
+  <si>
+    <t>Bạn ra ngoài khôn ngoan, cẩn thận, khiêm nhường, gặp nhiều may mắn. Bạn ra ngoài hay được mời đi ăn, rủ đi chơi xa.</t>
+  </si>
+  <si>
+    <t>Sẽ giải trừ bớt bệnh tật từ thói quen chịu khó quan tâm cẩn thận sức khỏe của bản thân. Khi bệnh tật đến thường may mắn gặp thầy thuốc bác sỹ giỏi, mất tiền để giải trừ tật bệnh.</t>
+  </si>
+  <si>
+    <t>Dễ có cơ hội kiếm được của tiền khi xung quanh xảy ra tai họa, nạn dịch.</t>
+  </si>
+  <si>
+    <t>Bạn có kiến thức về tài chính, tiền bạc, tính toán kín kẽ, cẩn thận. Hội thêm nhiều tài tinh càng thể hiện rõ nghề nghiệp đương số liên quan tới ngành tài chính, là người kiếm tiền giỏi.</t>
+  </si>
+  <si>
+    <t>Bạn là người chi ly, có xu hướng kẹt xỉ, tính toán.</t>
+  </si>
+  <si>
+    <t>Bác Sỹ Cô Quả Đẩu Quân Vũ Khúc hội chiếu tại Tài Bạch</t>
+  </si>
+  <si>
+    <t>Có thể ít con, muộn con, chậm đường con cái, dễ phải có can thiệp của y học để hỗ trợ.</t>
+  </si>
+  <si>
+    <t>Con cái ngoan ngoãn và thành đạt.</t>
+  </si>
+  <si>
+    <t>Bạn kết hôn muộn vì đặt nhiều tiêu chuẩn nên dễ kết hôn muộn, người hôn phối nhiều tuổi hơn mình.</t>
+  </si>
+  <si>
+    <t>Người hôn phối là người điềm đạm, giỏi giang, có quyền chức và tiền tài.</t>
+  </si>
+  <si>
+    <t>Bạn ít anh chị em, bản thân thường chênh nhiều tuổi với anh chị em. Anh chị em là những người có học, thành đạt, giỏi giang, sau này hay giúp đỡ mình.</t>
   </si>
 </sst>
 </file>
@@ -13407,9 +13491,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13741,10 +13826,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:G4412"/>
+  <dimension ref="A1:G4416"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A994" workbookViewId="0">
-      <selection activeCell="I1005" sqref="I1005"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13754,7 +13839,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>2160</v>
       </c>
       <c r="B1" t="s">
@@ -13765,7 +13850,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2167</v>
       </c>
       <c r="B2" t="s">
@@ -13773,7 +13858,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>2157</v>
       </c>
       <c r="B3" t="s">
@@ -13787,7 +13872,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>2162</v>
       </c>
       <c r="B4" t="s">
@@ -13795,7 +13880,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>2158</v>
       </c>
       <c r="B5" t="s">
@@ -13803,7 +13888,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>2166</v>
       </c>
       <c r="B6" t="s">
@@ -13820,7 +13905,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>2159</v>
       </c>
       <c r="B7" t="s">
@@ -13840,7 +13925,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>2161</v>
       </c>
       <c r="B8" t="s">
@@ -13851,7 +13936,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>2164</v>
       </c>
       <c r="B9" t="s">
@@ -13862,7 +13947,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>2163</v>
       </c>
       <c r="B10" t="s">
@@ -13870,7 +13955,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>2165</v>
       </c>
       <c r="B11" t="s">
@@ -13881,7 +13966,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>3737</v>
       </c>
       <c r="B12" t="s">
@@ -13889,7 +13974,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>3738</v>
       </c>
       <c r="B13" t="s">
@@ -13897,7 +13982,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>3739</v>
       </c>
       <c r="B14" t="s">
@@ -13905,7 +13990,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>3740</v>
       </c>
       <c r="B15" t="s">
@@ -13917,98 +14002,122 @@
         <v>3658</v>
       </c>
       <c r="B16" t="s">
-        <v>3658</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4457</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3665</v>
       </c>
       <c r="B17" t="s">
-        <v>3665</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4474</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3655</v>
       </c>
       <c r="B18" t="s">
-        <v>3655</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4447</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4448</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3660</v>
       </c>
       <c r="B19" t="s">
-        <v>3660</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4461</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4462</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4463</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3656</v>
       </c>
       <c r="B20" t="s">
-        <v>3656</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4453</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4454</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3664</v>
       </c>
       <c r="B21" t="s">
-        <v>3664</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4472</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4473</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3657</v>
       </c>
       <c r="B22" t="s">
-        <v>3657</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4455</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4456</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>3659</v>
       </c>
       <c r="B23" t="s">
-        <v>3659</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4460</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>1608</v>
       </c>
       <c r="B24" t="s">
-        <v>1608</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4467</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>3662</v>
       </c>
       <c r="B25" t="s">
-        <v>3662</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4465</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4466</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3661</v>
       </c>
       <c r="B26" t="s">
-        <v>3661</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4464</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>3663</v>
       </c>
       <c r="B27" t="s">
-        <v>3663</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4470</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4471</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1319</v>
       </c>
@@ -14016,7 +14125,7 @@
         <v>1319</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1318</v>
       </c>
@@ -14024,7 +14133,7 @@
         <v>1318</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>1320</v>
       </c>
@@ -14032,7 +14141,7 @@
         <v>1320</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1648</v>
       </c>
@@ -14040,7 +14149,7 @@
         <v>1648</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>2126</v>
       </c>
@@ -49116,6 +49225,38 @@
       </c>
       <c r="B4412" t="s">
         <v>4436</v>
+      </c>
+    </row>
+    <row r="4413" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4413" s="1" t="s">
+        <v>4449</v>
+      </c>
+      <c r="B4413" t="s">
+        <v>4450</v>
+      </c>
+    </row>
+    <row r="4414" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4414" s="1" t="s">
+        <v>4451</v>
+      </c>
+      <c r="B4414" t="s">
+        <v>4452</v>
+      </c>
+    </row>
+    <row r="4415" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4415" s="1" t="s">
+        <v>4459</v>
+      </c>
+      <c r="B4415" t="s">
+        <v>4458</v>
+      </c>
+    </row>
+    <row r="4416" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4416" s="1" t="s">
+        <v>4469</v>
+      </c>
+      <c r="B4416" t="s">
+        <v>4468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Giải thích Bạch Hổ tại Mệnh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C32E5BD-EA48-4918-B8D7-3EEAAF0C548F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CD119FA-3D66-4B00-A090-08C20044C74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8865" uniqueCount="4475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8865" uniqueCount="4477">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13450,6 +13450,12 @@
   </si>
   <si>
     <t>Bạn ít anh chị em, bản thân thường chênh nhiều tuổi với anh chị em. Anh chị em là những người có học, thành đạt, giỏi giang, sau này hay giúp đỡ mình.</t>
+  </si>
+  <si>
+    <t>Bạn là người can đảm, quả cảm, có nghị lực, tài giỏi, quyền biến, ứng phó được với mọi nghịch cảnh, khả năng xét đoán, lý luận giỏi, có tài hùng biện</t>
+  </si>
+  <si>
+    <t>Quý Chị có khí phách, có ý chí mạnh như đàn ông, có tâm tính của nam giới.</t>
   </si>
 </sst>
 </file>
@@ -13828,8 +13834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
   <dimension ref="A1:G4416"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="O37" sqref="O37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14170,7 +14176,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>1</v>
+        <v>4475</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -24505,7 +24511,7 @@
         <v>980</v>
       </c>
       <c r="B1324" t="s">
-        <v>980</v>
+        <v>4476</v>
       </c>
     </row>
     <row r="1325" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Giải thích tử vi ở mệnh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828FF00B-2382-4029-BC6E-96129B2EE724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3007D8-CE2E-43B7-8483-5732AA8E32A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4260" yWindow="1875" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8932" uniqueCount="4563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8935" uniqueCount="4564">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13717,6 +13717,9 @@
   </si>
   <si>
     <t>Cuộc sống giàu sang phú quý, tuổi thọ cao. Có sự nghiệp nhiều thành tựu. Có nhiều người tin tưởng, tôn trọng nghe theo.</t>
+  </si>
+  <si>
+    <t>Cuộc sống bế tắc, vất vả, nhiều thử thách</t>
   </si>
 </sst>
 </file>
@@ -13732,7 +13735,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13742,6 +13745,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -13758,14 +13767,95 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -14105,8 +14195,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A2:G4424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3249" workbookViewId="0">
-      <selection activeCell="A3306" sqref="A3306"/>
+    <sheetView tabSelected="1" topLeftCell="A3288" workbookViewId="0">
+      <selection activeCell="G3299" sqref="G3299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40594,8 +40684,8 @@
       <c r="A3281" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B3281" t="s">
-        <v>4544</v>
+      <c r="B3281" s="2" t="s">
+        <v>4563</v>
       </c>
     </row>
     <row r="3282" spans="1:5" x14ac:dyDescent="0.25">
@@ -40629,11 +40719,11 @@
       </c>
     </row>
     <row r="3285" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3285" t="s">
+      <c r="A3285" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B3285" t="s">
-        <v>59</v>
+      <c r="B3285" s="2" t="s">
+        <v>4563</v>
       </c>
     </row>
     <row r="3286" spans="1:5" x14ac:dyDescent="0.25">
@@ -40654,59 +40744,68 @@
       </c>
     </row>
     <row r="3287" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3287" t="s">
+      <c r="A3287" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B3287" t="s">
-        <v>37</v>
+        <v>4544</v>
       </c>
     </row>
     <row r="3288" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3288" t="s">
+      <c r="A3288" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B3288" t="s">
-        <v>45</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="3289" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3289" t="s">
+      <c r="A3289" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B3289" t="s">
-        <v>53</v>
+      <c r="B3289" s="2" t="s">
+        <v>4563</v>
       </c>
     </row>
     <row r="3290" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3290" t="s">
+      <c r="A3290" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B3290" t="s">
-        <v>31</v>
+        <v>4525</v>
+      </c>
+      <c r="C3290" t="s">
+        <v>4528</v>
+      </c>
+      <c r="D3290" t="s">
+        <v>4548</v>
+      </c>
+      <c r="E3290" t="s">
+        <v>4553</v>
       </c>
     </row>
     <row r="3291" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3291" t="s">
+      <c r="A3291" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B3291" t="s">
-        <v>39</v>
+        <v>4544</v>
       </c>
     </row>
     <row r="3292" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3292" t="s">
+      <c r="A3292" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B3292" t="s">
-        <v>47</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="3293" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3293" t="s">
+      <c r="A3293" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B3293" t="s">
-        <v>55</v>
+      <c r="B3293" s="2" t="s">
+        <v>4563</v>
       </c>
     </row>
     <row r="3294" spans="1:5" x14ac:dyDescent="0.25">
@@ -49768,22 +49867,46 @@
   </sortState>
   <dataConsolidate/>
   <conditionalFormatting sqref="A4293:A1048576 A2:A4285">
-    <cfRule type="duplicateValues" dxfId="5" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6716:A1048576 A2:A4170">
-    <cfRule type="duplicateValues" dxfId="4" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4293:B4419 B4421:B1048576 B3265:B3266 B2:B3263 B3268:B4285">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  <conditionalFormatting sqref="B4293:B4419 B4421:B1048576 B3265:B3266 B2:B3263 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B3294:B4285">
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4420">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6716:B1048576 B4401:B4404 B3265:B3266 B2:B3263 B3268:B4170">
-    <cfRule type="duplicateValues" dxfId="1" priority="5"/>
+  <conditionalFormatting sqref="B6716:B1048576 B4401:B4404 B3265:B3266 B2:B3263 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B3294:B4170">
+    <cfRule type="duplicateValues" dxfId="9" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3721">
-    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3281">
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3281">
+    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3285">
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3285">
+    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3289">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3289">
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3293">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3293">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Giải thích Liêm trinh tại mệnh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD3007D8-CE2E-43B7-8483-5732AA8E32A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1103FB7-3322-4D4E-830A-FF845C6F383C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4260" yWindow="1875" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8935" uniqueCount="4564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9004" uniqueCount="4581">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13720,6 +13720,57 @@
   </si>
   <si>
     <t>Cuộc sống bế tắc, vất vả, nhiều thử thách</t>
+  </si>
+  <si>
+    <t>Thân hình to cao</t>
+  </si>
+  <si>
+    <t>Dễ gặp nạn bắt bớ, giam cầm, hãm hại.</t>
+  </si>
+  <si>
+    <t>Bạn là người thẳng thắn, liêm khiết.</t>
+  </si>
+  <si>
+    <t>Bạn có xuất thân khổ cực, suốt đời lao tâm khổ tứ</t>
+  </si>
+  <si>
+    <t>Công danh trắc trở, tiền tài khó kiếm, dễ gặp hoạ bắt bớ, giam cầm.</t>
+  </si>
+  <si>
+    <t>Bạn là người nghiêm nghị, tính tình nóng nảy</t>
+  </si>
+  <si>
+    <t>Bạn được hưởng cuộc sống giàu có phú quý, phúc thọ song toàn</t>
+  </si>
+  <si>
+    <t>Sức khoẻ bạn dễ ốm đau, bệnh tật.</t>
+  </si>
+  <si>
+    <t>Bạn có đầu óc kinh doanh, làm công việc kỹ thuật,  nhiều tính toán, nhiều phần phải xa quê để làm ăn</t>
+  </si>
+  <si>
+    <t>Bạn dễ gặp tai nạn tay chân</t>
+  </si>
+  <si>
+    <t>Cuộc sống phải đi xa nay đây mai đó, vất vả làm việc</t>
+  </si>
+  <si>
+    <t>Cuộc sống cô đơn, dễ có những suy nghĩ tiêu cực thái quá.</t>
+  </si>
+  <si>
+    <t>Cuộc sống ít tai nạn, cuộc sống vừa đủ mức trung bình</t>
+  </si>
+  <si>
+    <t>Bạn cũng là người có sự tinh toán chỉ lợi cho bản thân, dễ làm điều ác</t>
+  </si>
+  <si>
+    <t>Có nhiều bệnh tật khó chữa.</t>
+  </si>
+  <si>
+    <t>Tính tình nóng nảy cương nghị can đảm</t>
+  </si>
+  <si>
+    <t>Bạn là người có tài thao lược, cơ mưu  quyền biến</t>
   </si>
 </sst>
 </file>
@@ -13735,7 +13786,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13754,6 +13805,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -13767,15 +13824,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -14195,13 +14273,13 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A2:G4424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3288" workbookViewId="0">
-      <selection activeCell="G3299" sqref="G3299"/>
+    <sheetView tabSelected="1" topLeftCell="A786" workbookViewId="0">
+      <selection activeCell="A792" sqref="A792"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.7109375" customWidth="1"/>
+    <col min="1" max="1" width="53.140625" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -20410,7 +20488,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="769" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="769" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A769" t="s">
         <v>986</v>
       </c>
@@ -20418,7 +20496,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="770" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="770" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
         <v>1630</v>
       </c>
@@ -20426,7 +20504,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="771" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="771" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
         <v>1578</v>
       </c>
@@ -20434,7 +20512,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="772" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="772" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
         <v>1591</v>
       </c>
@@ -20442,7 +20520,7 @@
         <v>1591</v>
       </c>
     </row>
-    <row r="773" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="773" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
         <v>1574</v>
       </c>
@@ -20450,463 +20528,670 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="774" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A774" t="s">
+    <row r="774" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A774" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B774" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="775" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A775" t="s">
+        <v>4564</v>
+      </c>
+    </row>
+    <row r="775" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A775" s="3" t="s">
         <v>117</v>
       </c>
       <c r="B775" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="776" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A776" t="s">
+        <v>4565</v>
+      </c>
+    </row>
+    <row r="776" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A776" s="3" t="s">
         <v>118</v>
       </c>
       <c r="B776" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="777" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A777" t="s">
+        <v>4565</v>
+      </c>
+    </row>
+    <row r="777" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A777" s="3" t="s">
         <v>89</v>
       </c>
       <c r="B777" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="778" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A778" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C777" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="778" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A778" s="3" t="s">
         <v>1008</v>
       </c>
       <c r="B778" t="s">
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="779" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A779" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C778" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="779" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A779" s="3" t="s">
         <v>88</v>
       </c>
       <c r="B779" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="780" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A780" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C779" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D779" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="780" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A780" s="3" t="s">
         <v>108</v>
       </c>
       <c r="B780" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="781" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A781" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C780" t="s">
+        <v>4572</v>
+      </c>
+      <c r="D780" t="s">
+        <v>4571</v>
+      </c>
+    </row>
+    <row r="781" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A781" s="3" t="s">
         <v>109</v>
       </c>
       <c r="B781" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="782" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A782" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C781" t="s">
+        <v>4573</v>
+      </c>
+    </row>
+    <row r="782" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A782" s="3" t="s">
         <v>1181</v>
       </c>
       <c r="B782" t="s">
-        <v>1181</v>
-      </c>
-    </row>
-    <row r="783" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A783" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C782" t="s">
+        <v>4574</v>
+      </c>
+      <c r="D782" t="s">
+        <v>4578</v>
+      </c>
+    </row>
+    <row r="783" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A783" s="3" t="s">
         <v>116</v>
       </c>
       <c r="B783" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="784" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A784" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C783" t="s">
+        <v>4575</v>
+      </c>
+      <c r="D783" t="s">
+        <v>4577</v>
+      </c>
+    </row>
+    <row r="784" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A784" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B784" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="785" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A785" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C784" t="s">
+        <v>4572</v>
+      </c>
+      <c r="D784" t="s">
+        <v>4571</v>
+      </c>
+    </row>
+    <row r="785" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A785" s="3" t="s">
         <v>113</v>
       </c>
       <c r="B785" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="786" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A786" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C785" t="s">
+        <v>4576</v>
+      </c>
+    </row>
+    <row r="786" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A786" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B786" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="787" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A787" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C786" t="s">
+        <v>4573</v>
+      </c>
+    </row>
+    <row r="787" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A787" s="3" t="s">
         <v>1013</v>
       </c>
       <c r="B787" t="s">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="788" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A788" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C787" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="788" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A788" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B788" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="789" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A789" t="s">
+        <v>4567</v>
+      </c>
+    </row>
+    <row r="789" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A789" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B789" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="790" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A790" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C789" t="s">
+        <v>4573</v>
+      </c>
+    </row>
+    <row r="790" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A790" s="3" t="s">
         <v>1180</v>
       </c>
       <c r="B790" t="s">
-        <v>1180</v>
-      </c>
-    </row>
-    <row r="791" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A791" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C790" t="s">
+        <v>4574</v>
+      </c>
+      <c r="D790" t="s">
+        <v>4578</v>
+      </c>
+    </row>
+    <row r="791" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A791" s="3" t="s">
         <v>115</v>
       </c>
       <c r="B791" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="792" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A792" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C791" t="s">
+        <v>4575</v>
+      </c>
+      <c r="D791" t="s">
+        <v>4577</v>
+      </c>
+    </row>
+    <row r="792" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A792" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B792" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="793" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A793" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="793" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A793" s="3" t="s">
         <v>99</v>
       </c>
       <c r="B793" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="794" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A794" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C793" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="794" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A794" s="3" t="s">
         <v>1011</v>
       </c>
       <c r="B794" t="s">
-        <v>1011</v>
-      </c>
-    </row>
-    <row r="795" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A795" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C794" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="795" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A795" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B795" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="796" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A796" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C795" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D795" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="796" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A796" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B796" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="797" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A797" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C796" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="797" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A797" s="3" t="s">
         <v>1007</v>
       </c>
       <c r="B797" t="s">
-        <v>1007</v>
-      </c>
-    </row>
-    <row r="798" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A798" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C797" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="798" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A798" s="3" t="s">
         <v>85</v>
       </c>
       <c r="B798" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="799" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A799" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C798" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D798" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="799" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A799" s="3" t="s">
         <v>97</v>
       </c>
       <c r="B799" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="800" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A800" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="800" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A800" s="3" t="s">
         <v>95</v>
       </c>
       <c r="B800" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="801" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A801" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C800" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="801" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A801" s="3" t="s">
         <v>1010</v>
       </c>
       <c r="B801" t="s">
-        <v>1010</v>
-      </c>
-    </row>
-    <row r="802" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A802" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C801" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="802" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A802" s="3" t="s">
         <v>94</v>
       </c>
       <c r="B802" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="803" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A803" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C802" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D802" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="803" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A803" s="3" t="s">
         <v>92</v>
       </c>
       <c r="B803" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="804" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A804" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C803" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="804" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A804" s="3" t="s">
         <v>1009</v>
       </c>
       <c r="B804" t="s">
-        <v>1009</v>
-      </c>
-    </row>
-    <row r="805" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A805" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C804" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="805" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A805" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B805" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="806" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A806" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C805" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D805" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="806" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A806" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B806" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="807" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A807" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C806" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="807" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A807" s="3" t="s">
         <v>1004</v>
       </c>
       <c r="B807" t="s">
-        <v>1004</v>
-      </c>
-    </row>
-    <row r="808" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A808" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C807" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="808" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A808" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B808" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="809" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A809" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C808" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D808" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="809" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A809" s="3" t="s">
         <v>80</v>
       </c>
       <c r="B809" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="810" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A810" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C809" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="810" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A810" s="3" t="s">
         <v>1005</v>
       </c>
       <c r="B810" t="s">
-        <v>1005</v>
-      </c>
-    </row>
-    <row r="811" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A811" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C810" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="811" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A811" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B811" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="812" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A812" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C811" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D811" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="812" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A812" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B812" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="813" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A813" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C812" t="s">
+        <v>4572</v>
+      </c>
+      <c r="D812" t="s">
+        <v>4571</v>
+      </c>
+    </row>
+    <row r="813" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A813" s="3" t="s">
         <v>111</v>
       </c>
       <c r="B813" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="814" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A814" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C813" t="s">
+        <v>4576</v>
+      </c>
+    </row>
+    <row r="814" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A814" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B814" t="s">
+      <c r="B814" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="815" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A815" t="s">
+    <row r="815" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A815" s="3" t="s">
         <v>102</v>
       </c>
       <c r="B815" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="816" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A816" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C815" t="s">
+        <v>4573</v>
+      </c>
+    </row>
+    <row r="816" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A816" s="3" t="s">
         <v>1006</v>
       </c>
       <c r="B816" t="s">
-        <v>1006</v>
-      </c>
-    </row>
-    <row r="817" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A817" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C816" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="817" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A817" s="3" t="s">
         <v>1012</v>
       </c>
       <c r="B817" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="818" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A818" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C817" t="s">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="818" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A818" s="3" t="s">
         <v>82</v>
       </c>
       <c r="B818" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="819" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A819" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C818" t="s">
+        <v>4569</v>
+      </c>
+      <c r="D818" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="819" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A819" s="3" t="s">
         <v>2381</v>
       </c>
       <c r="B819" t="s">
-        <v>2381</v>
-      </c>
-    </row>
-    <row r="820" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A820" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C819" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="820" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A820" s="3" t="s">
         <v>2388</v>
       </c>
       <c r="B820" t="s">
-        <v>2388</v>
-      </c>
-    </row>
-    <row r="821" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A821" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C820" t="s">
+        <v>4572</v>
+      </c>
+      <c r="D820" t="s">
+        <v>4571</v>
+      </c>
+    </row>
+    <row r="821" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A821" s="3" t="s">
         <v>2390</v>
       </c>
       <c r="B821" t="s">
-        <v>2390</v>
-      </c>
-    </row>
-    <row r="822" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A822" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C821" t="s">
+        <v>4572</v>
+      </c>
+      <c r="D821" t="s">
+        <v>4571</v>
+      </c>
+    </row>
+    <row r="822" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A822" s="3" t="s">
         <v>2382</v>
       </c>
       <c r="B822" t="s">
-        <v>2382</v>
-      </c>
-    </row>
-    <row r="823" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A823" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C822" t="s">
+        <v>4572</v>
+      </c>
+      <c r="D822" t="s">
+        <v>4571</v>
+      </c>
+    </row>
+    <row r="823" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A823" s="3" t="s">
         <v>2386</v>
       </c>
       <c r="B823" t="s">
-        <v>2386</v>
-      </c>
-    </row>
-    <row r="824" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A824" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C823" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="824" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A824" s="3" t="s">
         <v>2385</v>
       </c>
       <c r="B824" t="s">
-        <v>2385</v>
-      </c>
-    </row>
-    <row r="825" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A825" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C824" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="825" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A825" s="3" t="s">
         <v>2380</v>
       </c>
       <c r="B825" t="s">
-        <v>2380</v>
-      </c>
-    </row>
-    <row r="826" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A826" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C825" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="826" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A826" s="3" t="s">
         <v>2387</v>
       </c>
       <c r="B826" t="s">
-        <v>2387</v>
-      </c>
-    </row>
-    <row r="827" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A827" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C826" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="827" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A827" s="3" t="s">
         <v>2383</v>
       </c>
       <c r="B827" t="s">
-        <v>2383</v>
-      </c>
-    </row>
-    <row r="828" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A828" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C827" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="828" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A828" s="3" t="s">
         <v>2389</v>
       </c>
       <c r="B828" t="s">
-        <v>2389</v>
-      </c>
-    </row>
-    <row r="829" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A829" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C828" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="829" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A829" s="3" t="s">
         <v>2379</v>
       </c>
       <c r="B829" t="s">
-        <v>2379</v>
-      </c>
-    </row>
-    <row r="830" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A830" t="s">
+        <v>4566</v>
+      </c>
+      <c r="C829" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="830" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A830" s="3" t="s">
         <v>2384</v>
       </c>
       <c r="B830" t="s">
-        <v>2384</v>
-      </c>
-    </row>
-    <row r="831" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4567</v>
+      </c>
+      <c r="C830" t="s">
+        <v>4572</v>
+      </c>
+      <c r="D830" t="s">
+        <v>4571</v>
+      </c>
+    </row>
+    <row r="831" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A831" t="s">
         <v>3178</v>
       </c>
@@ -20914,7 +21199,7 @@
         <v>3178</v>
       </c>
     </row>
-    <row r="832" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="832" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A832" t="s">
         <v>3185</v>
       </c>
@@ -20922,7 +21207,7 @@
         <v>3185</v>
       </c>
     </row>
-    <row r="833" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="833" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A833" t="s">
         <v>3187</v>
       </c>
@@ -20930,7 +21215,7 @@
         <v>3187</v>
       </c>
     </row>
-    <row r="834" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="834" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A834" t="s">
         <v>3179</v>
       </c>
@@ -20938,7 +21223,7 @@
         <v>3179</v>
       </c>
     </row>
-    <row r="835" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="835" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A835" t="s">
         <v>3183</v>
       </c>
@@ -20946,7 +21231,7 @@
         <v>3183</v>
       </c>
     </row>
-    <row r="836" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="836" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A836" t="s">
         <v>3182</v>
       </c>
@@ -20954,7 +21239,7 @@
         <v>3182</v>
       </c>
     </row>
-    <row r="837" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="837" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A837" t="s">
         <v>3177</v>
       </c>
@@ -20962,7 +21247,7 @@
         <v>3177</v>
       </c>
     </row>
-    <row r="838" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="838" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A838" t="s">
         <v>3184</v>
       </c>
@@ -20970,7 +21255,7 @@
         <v>3184</v>
       </c>
     </row>
-    <row r="839" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="839" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A839" t="s">
         <v>3180</v>
       </c>
@@ -20978,7 +21263,7 @@
         <v>3180</v>
       </c>
     </row>
-    <row r="840" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="840" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A840" t="s">
         <v>3186</v>
       </c>
@@ -20986,7 +21271,7 @@
         <v>3186</v>
       </c>
     </row>
-    <row r="841" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="841" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A841" t="s">
         <v>3176</v>
       </c>
@@ -20994,7 +21279,7 @@
         <v>3176</v>
       </c>
     </row>
-    <row r="842" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="842" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A842" t="s">
         <v>3181</v>
       </c>
@@ -21002,7 +21287,7 @@
         <v>3181</v>
       </c>
     </row>
-    <row r="843" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="843" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A843" t="s">
         <v>3226</v>
       </c>
@@ -21010,7 +21295,7 @@
         <v>3226</v>
       </c>
     </row>
-    <row r="844" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="844" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A844" t="s">
         <v>3232</v>
       </c>
@@ -21018,7 +21303,7 @@
         <v>3232</v>
       </c>
     </row>
-    <row r="845" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="845" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A845" t="s">
         <v>3234</v>
       </c>
@@ -21026,7 +21311,7 @@
         <v>3234</v>
       </c>
     </row>
-    <row r="846" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="846" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A846" t="s">
         <v>1602</v>
       </c>
@@ -21034,7 +21319,7 @@
         <v>1602</v>
       </c>
     </row>
-    <row r="847" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="847" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A847" t="s">
         <v>3230</v>
       </c>
@@ -21042,7 +21327,7 @@
         <v>3230</v>
       </c>
     </row>
-    <row r="848" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="848" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A848" t="s">
         <v>3229</v>
       </c>
@@ -21050,7 +21335,7 @@
         <v>3229</v>
       </c>
     </row>
-    <row r="849" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="849" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A849" t="s">
         <v>3225</v>
       </c>
@@ -21058,7 +21343,7 @@
         <v>3225</v>
       </c>
     </row>
-    <row r="850" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="850" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A850" t="s">
         <v>3231</v>
       </c>
@@ -21066,7 +21351,7 @@
         <v>3231</v>
       </c>
     </row>
-    <row r="851" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="851" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A851" t="s">
         <v>3227</v>
       </c>
@@ -21074,7 +21359,7 @@
         <v>3227</v>
       </c>
     </row>
-    <row r="852" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="852" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A852" t="s">
         <v>3233</v>
       </c>
@@ -21082,7 +21367,7 @@
         <v>3233</v>
       </c>
     </row>
-    <row r="853" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="853" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A853" t="s">
         <v>3224</v>
       </c>
@@ -21090,7 +21375,7 @@
         <v>3224</v>
       </c>
     </row>
-    <row r="854" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="854" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A854" t="s">
         <v>3228</v>
       </c>
@@ -21098,7 +21383,7 @@
         <v>3228</v>
       </c>
     </row>
-    <row r="855" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="855" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A855" t="s">
         <v>3154</v>
       </c>
@@ -21106,7 +21391,7 @@
         <v>3154</v>
       </c>
     </row>
-    <row r="856" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="856" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A856" t="s">
         <v>3161</v>
       </c>
@@ -21114,7 +21399,7 @@
         <v>3161</v>
       </c>
     </row>
-    <row r="857" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="857" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A857" t="s">
         <v>3163</v>
       </c>
@@ -21122,7 +21407,7 @@
         <v>3163</v>
       </c>
     </row>
-    <row r="858" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="858" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A858" t="s">
         <v>3155</v>
       </c>
@@ -21130,7 +21415,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="859" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="859" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A859" t="s">
         <v>3159</v>
       </c>
@@ -21138,7 +21423,7 @@
         <v>3159</v>
       </c>
     </row>
-    <row r="860" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="860" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A860" t="s">
         <v>3158</v>
       </c>
@@ -21146,7 +21431,7 @@
         <v>3158</v>
       </c>
     </row>
-    <row r="861" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="861" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A861" t="s">
         <v>3153</v>
       </c>
@@ -21154,7 +21439,7 @@
         <v>3153</v>
       </c>
     </row>
-    <row r="862" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="862" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A862" t="s">
         <v>3160</v>
       </c>
@@ -21162,7 +21447,7 @@
         <v>3160</v>
       </c>
     </row>
-    <row r="863" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="863" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A863" t="s">
         <v>3156</v>
       </c>
@@ -21170,7 +21455,7 @@
         <v>3156</v>
       </c>
     </row>
-    <row r="864" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="864" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A864" t="s">
         <v>3162</v>
       </c>
@@ -21178,7 +21463,7 @@
         <v>3162</v>
       </c>
     </row>
-    <row r="865" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="865" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A865" t="s">
         <v>3152</v>
       </c>
@@ -21186,7 +21471,7 @@
         <v>3152</v>
       </c>
     </row>
-    <row r="866" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="866" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A866" t="s">
         <v>3157</v>
       </c>
@@ -21194,7 +21479,7 @@
         <v>3157</v>
       </c>
     </row>
-    <row r="867" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="867" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A867" t="s">
         <v>3166</v>
       </c>
@@ -21202,7 +21487,7 @@
         <v>3166</v>
       </c>
     </row>
-    <row r="868" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="868" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A868" t="s">
         <v>3173</v>
       </c>
@@ -21210,7 +21495,7 @@
         <v>3173</v>
       </c>
     </row>
-    <row r="869" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="869" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A869" t="s">
         <v>3175</v>
       </c>
@@ -21218,7 +21503,7 @@
         <v>3175</v>
       </c>
     </row>
-    <row r="870" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="870" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A870" t="s">
         <v>3167</v>
       </c>
@@ -21226,7 +21511,7 @@
         <v>3167</v>
       </c>
     </row>
-    <row r="871" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="871" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A871" t="s">
         <v>3171</v>
       </c>
@@ -21234,7 +21519,7 @@
         <v>3171</v>
       </c>
     </row>
-    <row r="872" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="872" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A872" t="s">
         <v>3170</v>
       </c>
@@ -21242,7 +21527,7 @@
         <v>3170</v>
       </c>
     </row>
-    <row r="873" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="873" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A873" t="s">
         <v>3165</v>
       </c>
@@ -21250,7 +21535,7 @@
         <v>3165</v>
       </c>
     </row>
-    <row r="874" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="874" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A874" t="s">
         <v>3172</v>
       </c>
@@ -21258,7 +21543,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="875" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="875" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A875" t="s">
         <v>3168</v>
       </c>
@@ -21266,7 +21551,7 @@
         <v>3168</v>
       </c>
     </row>
-    <row r="876" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="876" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A876" t="s">
         <v>3174</v>
       </c>
@@ -21274,7 +21559,7 @@
         <v>3174</v>
       </c>
     </row>
-    <row r="877" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="877" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A877" t="s">
         <v>3164</v>
       </c>
@@ -21282,7 +21567,7 @@
         <v>3164</v>
       </c>
     </row>
-    <row r="878" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="878" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A878" t="s">
         <v>3169</v>
       </c>
@@ -21290,7 +21575,7 @@
         <v>3169</v>
       </c>
     </row>
-    <row r="879" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="879" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A879" t="s">
         <v>3214</v>
       </c>
@@ -21298,7 +21583,7 @@
         <v>3214</v>
       </c>
     </row>
-    <row r="880" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="880" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A880" t="s">
         <v>3221</v>
       </c>
@@ -21306,7 +21591,7 @@
         <v>3221</v>
       </c>
     </row>
-    <row r="881" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="881" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A881" t="s">
         <v>3223</v>
       </c>
@@ -21314,7 +21599,7 @@
         <v>3223</v>
       </c>
     </row>
-    <row r="882" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="882" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A882" t="s">
         <v>3215</v>
       </c>
@@ -21322,7 +21607,7 @@
         <v>3215</v>
       </c>
     </row>
-    <row r="883" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="883" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A883" t="s">
         <v>3219</v>
       </c>
@@ -21330,7 +21615,7 @@
         <v>3219</v>
       </c>
     </row>
-    <row r="884" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="884" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A884" t="s">
         <v>3218</v>
       </c>
@@ -21338,7 +21623,7 @@
         <v>3218</v>
       </c>
     </row>
-    <row r="885" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="885" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A885" t="s">
         <v>3213</v>
       </c>
@@ -21346,7 +21631,7 @@
         <v>3213</v>
       </c>
     </row>
-    <row r="886" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="886" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A886" t="s">
         <v>3220</v>
       </c>
@@ -21354,7 +21639,7 @@
         <v>3220</v>
       </c>
     </row>
-    <row r="887" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="887" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A887" t="s">
         <v>3216</v>
       </c>
@@ -21362,7 +21647,7 @@
         <v>3216</v>
       </c>
     </row>
-    <row r="888" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="888" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A888" t="s">
         <v>3222</v>
       </c>
@@ -21370,7 +21655,7 @@
         <v>3222</v>
       </c>
     </row>
-    <row r="889" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="889" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A889" t="s">
         <v>3212</v>
       </c>
@@ -21378,7 +21663,7 @@
         <v>3212</v>
       </c>
     </row>
-    <row r="890" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="890" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A890" t="s">
         <v>3217</v>
       </c>
@@ -21386,7 +21671,7 @@
         <v>3217</v>
       </c>
     </row>
-    <row r="891" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="891" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A891" t="s">
         <v>3202</v>
       </c>
@@ -21394,7 +21679,7 @@
         <v>3202</v>
       </c>
     </row>
-    <row r="892" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="892" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A892" t="s">
         <v>3209</v>
       </c>
@@ -21402,7 +21687,7 @@
         <v>3209</v>
       </c>
     </row>
-    <row r="893" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="893" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A893" t="s">
         <v>3211</v>
       </c>
@@ -21410,7 +21695,7 @@
         <v>3211</v>
       </c>
     </row>
-    <row r="894" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="894" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A894" t="s">
         <v>3203</v>
       </c>
@@ -21418,7 +21703,7 @@
         <v>3203</v>
       </c>
     </row>
-    <row r="895" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="895" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A895" t="s">
         <v>3207</v>
       </c>
@@ -21426,7 +21711,7 @@
         <v>3207</v>
       </c>
     </row>
-    <row r="896" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="896" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A896" t="s">
         <v>3206</v>
       </c>
@@ -21434,7 +21719,7 @@
         <v>3206</v>
       </c>
     </row>
-    <row r="897" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="897" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A897" t="s">
         <v>3201</v>
       </c>
@@ -21442,7 +21727,7 @@
         <v>3201</v>
       </c>
     </row>
-    <row r="898" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="898" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A898" t="s">
         <v>3208</v>
       </c>
@@ -21450,7 +21735,7 @@
         <v>3208</v>
       </c>
     </row>
-    <row r="899" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="899" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A899" t="s">
         <v>3204</v>
       </c>
@@ -21458,7 +21743,7 @@
         <v>3204</v>
       </c>
     </row>
-    <row r="900" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="900" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A900" t="s">
         <v>3210</v>
       </c>
@@ -21466,7 +21751,7 @@
         <v>3210</v>
       </c>
     </row>
-    <row r="901" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="901" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A901" t="s">
         <v>3200</v>
       </c>
@@ -21474,7 +21759,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="902" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="902" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A902" t="s">
         <v>3205</v>
       </c>
@@ -21482,7 +21767,7 @@
         <v>3205</v>
       </c>
     </row>
-    <row r="903" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="903" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A903" t="s">
         <v>3142</v>
       </c>
@@ -21490,7 +21775,7 @@
         <v>3142</v>
       </c>
     </row>
-    <row r="904" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="904" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A904" t="s">
         <v>3149</v>
       </c>
@@ -21498,7 +21783,7 @@
         <v>3149</v>
       </c>
     </row>
-    <row r="905" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="905" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A905" t="s">
         <v>3151</v>
       </c>
@@ -21506,7 +21791,7 @@
         <v>3151</v>
       </c>
     </row>
-    <row r="906" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="906" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A906" t="s">
         <v>3143</v>
       </c>
@@ -21514,7 +21799,7 @@
         <v>3143</v>
       </c>
     </row>
-    <row r="907" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="907" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A907" t="s">
         <v>3147</v>
       </c>
@@ -21522,7 +21807,7 @@
         <v>3147</v>
       </c>
     </row>
-    <row r="908" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="908" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A908" t="s">
         <v>3146</v>
       </c>
@@ -21530,7 +21815,7 @@
         <v>3146</v>
       </c>
     </row>
-    <row r="909" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="909" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A909" t="s">
         <v>3141</v>
       </c>
@@ -21538,7 +21823,7 @@
         <v>3141</v>
       </c>
     </row>
-    <row r="910" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="910" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A910" t="s">
         <v>3148</v>
       </c>
@@ -21546,7 +21831,7 @@
         <v>3148</v>
       </c>
     </row>
-    <row r="911" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="911" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A911" t="s">
         <v>3144</v>
       </c>
@@ -21554,7 +21839,7 @@
         <v>3144</v>
       </c>
     </row>
-    <row r="912" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="912" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A912" t="s">
         <v>3150</v>
       </c>
@@ -21562,7 +21847,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="913" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="913" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A913" t="s">
         <v>3140</v>
       </c>
@@ -21570,7 +21855,7 @@
         <v>3140</v>
       </c>
     </row>
-    <row r="914" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="914" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A914" t="s">
         <v>3145</v>
       </c>
@@ -21578,7 +21863,7 @@
         <v>3145</v>
       </c>
     </row>
-    <row r="915" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="915" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A915" t="s">
         <v>3190</v>
       </c>
@@ -21586,7 +21871,7 @@
         <v>3190</v>
       </c>
     </row>
-    <row r="916" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="916" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A916" t="s">
         <v>3197</v>
       </c>
@@ -21594,7 +21879,7 @@
         <v>3197</v>
       </c>
     </row>
-    <row r="917" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="917" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A917" t="s">
         <v>3199</v>
       </c>
@@ -21602,7 +21887,7 @@
         <v>3199</v>
       </c>
     </row>
-    <row r="918" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="918" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A918" t="s">
         <v>3191</v>
       </c>
@@ -21610,7 +21895,7 @@
         <v>3191</v>
       </c>
     </row>
-    <row r="919" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="919" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A919" t="s">
         <v>3195</v>
       </c>
@@ -21618,7 +21903,7 @@
         <v>3195</v>
       </c>
     </row>
-    <row r="920" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="920" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A920" t="s">
         <v>3194</v>
       </c>
@@ -21626,7 +21911,7 @@
         <v>3194</v>
       </c>
     </row>
-    <row r="921" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="921" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A921" t="s">
         <v>3189</v>
       </c>
@@ -21634,7 +21919,7 @@
         <v>3189</v>
       </c>
     </row>
-    <row r="922" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="922" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A922" t="s">
         <v>3196</v>
       </c>
@@ -21642,7 +21927,7 @@
         <v>3196</v>
       </c>
     </row>
-    <row r="923" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="923" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A923" t="s">
         <v>3192</v>
       </c>
@@ -21650,7 +21935,7 @@
         <v>3192</v>
       </c>
     </row>
-    <row r="924" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="924" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A924" t="s">
         <v>3198</v>
       </c>
@@ -21658,7 +21943,7 @@
         <v>3198</v>
       </c>
     </row>
-    <row r="925" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="925" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A925" t="s">
         <v>3188</v>
       </c>
@@ -21666,7 +21951,7 @@
         <v>3188</v>
       </c>
     </row>
-    <row r="926" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="926" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A926" t="s">
         <v>3193</v>
       </c>
@@ -40301,7 +40586,7 @@
         <v>3580</v>
       </c>
     </row>
-    <row r="3243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3243" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3243" s="1" t="s">
         <v>28</v>
       </c>
@@ -40309,7 +40594,7 @@
         <v>4550</v>
       </c>
     </row>
-    <row r="3244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3244" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3244" s="1" t="s">
         <v>990</v>
       </c>
@@ -40317,7 +40602,7 @@
         <v>4539</v>
       </c>
     </row>
-    <row r="3245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3245" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3245" s="1" t="s">
         <v>989</v>
       </c>
@@ -40325,7 +40610,7 @@
         <v>4539</v>
       </c>
     </row>
-    <row r="3246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3246" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3246" s="1" t="s">
         <v>26</v>
       </c>
@@ -40333,7 +40618,7 @@
         <v>4546</v>
       </c>
     </row>
-    <row r="3247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3247" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3247" s="1" t="s">
         <v>25</v>
       </c>
@@ -40341,7 +40626,7 @@
         <v>4546</v>
       </c>
     </row>
-    <row r="3248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3248" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3248" s="1" t="s">
         <v>999</v>
       </c>
@@ -40349,7 +40634,7 @@
         <v>4562</v>
       </c>
     </row>
-    <row r="3249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3249" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3249" s="1" t="s">
         <v>27</v>
       </c>
@@ -40357,7 +40642,7 @@
         <v>4549</v>
       </c>
     </row>
-    <row r="3250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3250" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3250" s="1" t="s">
         <v>987</v>
       </c>
@@ -40365,7 +40650,7 @@
         <v>4561</v>
       </c>
     </row>
-    <row r="3251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3251" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3251" t="s">
         <v>63</v>
       </c>
@@ -40373,7 +40658,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3252" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3252" s="1" t="s">
         <v>68</v>
       </c>
@@ -40381,7 +40666,7 @@
         <v>4560</v>
       </c>
     </row>
-    <row r="3253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3253" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3253" s="1" t="s">
         <v>21</v>
       </c>
@@ -40389,7 +40674,7 @@
         <v>4543</v>
       </c>
     </row>
-    <row r="3254" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3254" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3254" s="1" t="s">
         <v>64</v>
       </c>
@@ -40397,7 +40682,7 @@
         <v>4559</v>
       </c>
     </row>
-    <row r="3255" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3255" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3255" s="1" t="s">
         <v>1000</v>
       </c>
@@ -40405,7 +40690,7 @@
         <v>4545</v>
       </c>
     </row>
-    <row r="3256" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3256" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3256" s="1" t="s">
         <v>1002</v>
       </c>
@@ -40413,7 +40698,7 @@
         <v>4551</v>
       </c>
     </row>
-    <row r="3257" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3257" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3257" s="1" t="s">
         <v>23</v>
       </c>
@@ -40421,7 +40706,7 @@
         <v>4544</v>
       </c>
     </row>
-    <row r="3258" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3258" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3258" s="1" t="s">
         <v>24</v>
       </c>
@@ -40429,7 +40714,7 @@
         <v>4544</v>
       </c>
     </row>
-    <row r="3259" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3259" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3259" s="1" t="s">
         <v>67</v>
       </c>
@@ -40437,7 +40722,7 @@
         <v>4558</v>
       </c>
     </row>
-    <row r="3260" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3260" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3260" s="1" t="s">
         <v>19</v>
       </c>
@@ -40445,7 +40730,7 @@
         <v>4556</v>
       </c>
     </row>
-    <row r="3261" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3261" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3261" s="1" t="s">
         <v>69</v>
       </c>
@@ -40453,7 +40738,7 @@
         <v>4556</v>
       </c>
     </row>
-    <row r="3262" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3262" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3262" s="1" t="s">
         <v>6</v>
       </c>
@@ -40467,7 +40752,7 @@
         <v>4548</v>
       </c>
     </row>
-    <row r="3263" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3263" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3263" s="1" t="s">
         <v>13</v>
       </c>
@@ -40478,7 +40763,7 @@
         <v>4527</v>
       </c>
     </row>
-    <row r="3264" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3264" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3264" s="1" t="s">
         <v>62</v>
       </c>
@@ -40489,7 +40774,7 @@
         <v>4555</v>
       </c>
     </row>
-    <row r="3265" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3265" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3265" s="1" t="s">
         <v>11</v>
       </c>
@@ -40500,7 +40785,7 @@
         <v>4527</v>
       </c>
     </row>
-    <row r="3266" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3266" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3266" s="1" t="s">
         <v>12</v>
       </c>
@@ -40511,7 +40796,7 @@
         <v>4527</v>
       </c>
     </row>
-    <row r="3267" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3267" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3267" s="1" t="s">
         <v>61</v>
       </c>
@@ -40519,7 +40804,7 @@
         <v>4555</v>
       </c>
     </row>
-    <row r="3268" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3268" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3268" s="1" t="s">
         <v>2</v>
       </c>
@@ -40533,7 +40818,7 @@
         <v>4553</v>
       </c>
     </row>
-    <row r="3269" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3269" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3269" s="1" t="s">
         <v>5</v>
       </c>
@@ -40547,7 +40832,7 @@
         <v>4548</v>
       </c>
     </row>
-    <row r="3270" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3270" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3270" s="1" t="s">
         <v>66</v>
       </c>
@@ -40555,7 +40840,7 @@
         <v>4557</v>
       </c>
     </row>
-    <row r="3271" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3271" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3271" s="1" t="s">
         <v>3</v>
       </c>
@@ -40569,7 +40854,7 @@
         <v>4553</v>
       </c>
     </row>
-    <row r="3272" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3272" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3272" s="1" t="s">
         <v>7</v>
       </c>
@@ -40583,7 +40868,7 @@
         <v>4548</v>
       </c>
     </row>
-    <row r="3273" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3273" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3273" s="1" t="s">
         <v>9</v>
       </c>
@@ -40600,7 +40885,7 @@
         <v>4553</v>
       </c>
     </row>
-    <row r="3274" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3274" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3274" s="1" t="s">
         <v>8</v>
       </c>
@@ -40617,7 +40902,7 @@
         <v>4553</v>
       </c>
     </row>
-    <row r="3275" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3275" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3275" s="1" t="s">
         <v>10</v>
       </c>
@@ -40628,7 +40913,7 @@
         <v>4527</v>
       </c>
     </row>
-    <row r="3276" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3276" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3276" s="1" t="s">
         <v>4</v>
       </c>
@@ -40642,7 +40927,7 @@
         <v>4548</v>
       </c>
     </row>
-    <row r="3277" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3277" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3277" s="1" t="s">
         <v>65</v>
       </c>
@@ -40650,7 +40935,7 @@
         <v>4557</v>
       </c>
     </row>
-    <row r="3278" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3278" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3278" s="1" t="s">
         <v>33</v>
       </c>
@@ -40664,7 +40949,7 @@
         <v>4553</v>
       </c>
     </row>
-    <row r="3279" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3279" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3279" s="1" t="s">
         <v>41</v>
       </c>
@@ -40672,7 +40957,7 @@
         <v>4544</v>
       </c>
     </row>
-    <row r="3280" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3280" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3280" s="1" t="s">
         <v>49</v>
       </c>
@@ -40680,7 +40965,7 @@
         <v>4558</v>
       </c>
     </row>
-    <row r="3281" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3281" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3281" s="1" t="s">
         <v>57</v>
       </c>
@@ -40688,7 +40973,7 @@
         <v>4563</v>
       </c>
     </row>
-    <row r="3282" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3282" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3282" s="1" t="s">
         <v>35</v>
       </c>
@@ -40702,7 +40987,7 @@
         <v>4553</v>
       </c>
     </row>
-    <row r="3283" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3283" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3283" s="1" t="s">
         <v>43</v>
       </c>
@@ -40710,7 +40995,7 @@
         <v>4544</v>
       </c>
     </row>
-    <row r="3284" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3284" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3284" s="1" t="s">
         <v>51</v>
       </c>
@@ -40718,7 +41003,7 @@
         <v>4558</v>
       </c>
     </row>
-    <row r="3285" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3285" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3285" s="1" t="s">
         <v>59</v>
       </c>
@@ -40726,7 +41011,7 @@
         <v>4563</v>
       </c>
     </row>
-    <row r="3286" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3286" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3286" s="1" t="s">
         <v>29</v>
       </c>
@@ -40743,7 +41028,7 @@
         <v>4553</v>
       </c>
     </row>
-    <row r="3287" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3287" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3287" s="1" t="s">
         <v>37</v>
       </c>
@@ -40751,7 +41036,7 @@
         <v>4544</v>
       </c>
     </row>
-    <row r="3288" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3288" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3288" s="1" t="s">
         <v>45</v>
       </c>
@@ -40759,7 +41044,7 @@
         <v>4558</v>
       </c>
     </row>
-    <row r="3289" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3289" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3289" s="1" t="s">
         <v>53</v>
       </c>
@@ -40767,7 +41052,7 @@
         <v>4563</v>
       </c>
     </row>
-    <row r="3290" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3290" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3290" s="1" t="s">
         <v>31</v>
       </c>
@@ -40784,7 +41069,7 @@
         <v>4553</v>
       </c>
     </row>
-    <row r="3291" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3291" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3291" s="1" t="s">
         <v>39</v>
       </c>
@@ -40792,7 +41077,7 @@
         <v>4544</v>
       </c>
     </row>
-    <row r="3292" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3292" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3292" s="1" t="s">
         <v>47</v>
       </c>
@@ -40800,7 +41085,7 @@
         <v>4558</v>
       </c>
     </row>
-    <row r="3293" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3293" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3293" s="1" t="s">
         <v>55</v>
       </c>
@@ -40808,7 +41093,7 @@
         <v>4563</v>
       </c>
     </row>
-    <row r="3294" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3294" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3294" s="1" t="s">
         <v>72</v>
       </c>
@@ -40816,7 +41101,7 @@
         <v>4538</v>
       </c>
     </row>
-    <row r="3295" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3295" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3295" s="1" t="s">
         <v>988</v>
       </c>
@@ -40827,7 +41112,7 @@
         <v>4537</v>
       </c>
     </row>
-    <row r="3296" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3296" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3296" s="1" t="s">
         <v>18</v>
       </c>
@@ -40835,7 +41120,7 @@
         <v>4535</v>
       </c>
     </row>
-    <row r="3297" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3297" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3297" t="s">
         <v>2583</v>
       </c>
@@ -40843,7 +41128,7 @@
         <v>2583</v>
       </c>
     </row>
-    <row r="3298" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3298" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3298" t="s">
         <v>2590</v>
       </c>
@@ -40851,7 +41136,7 @@
         <v>2590</v>
       </c>
     </row>
-    <row r="3299" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3299" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3299" t="s">
         <v>2592</v>
       </c>
@@ -40859,7 +41144,7 @@
         <v>2592</v>
       </c>
     </row>
-    <row r="3300" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3300" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3300" t="s">
         <v>2584</v>
       </c>
@@ -40867,7 +41152,7 @@
         <v>2584</v>
       </c>
     </row>
-    <row r="3301" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3301" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3301" t="s">
         <v>2588</v>
       </c>
@@ -40875,7 +41160,7 @@
         <v>2588</v>
       </c>
     </row>
-    <row r="3302" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3302" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3302" t="s">
         <v>2587</v>
       </c>
@@ -40883,7 +41168,7 @@
         <v>2587</v>
       </c>
     </row>
-    <row r="3303" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3303" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3303" t="s">
         <v>2582</v>
       </c>
@@ -40891,7 +41176,7 @@
         <v>2582</v>
       </c>
     </row>
-    <row r="3304" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3304" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3304" t="s">
         <v>2589</v>
       </c>
@@ -40899,7 +41184,7 @@
         <v>2589</v>
       </c>
     </row>
-    <row r="3305" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3305" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3305" t="s">
         <v>2585</v>
       </c>
@@ -40907,7 +41192,7 @@
         <v>2585</v>
       </c>
     </row>
-    <row r="3306" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3306" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3306" t="s">
         <v>2591</v>
       </c>
@@ -40915,7 +41200,7 @@
         <v>2591</v>
       </c>
     </row>
-    <row r="3307" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3307" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3307" t="s">
         <v>2581</v>
       </c>
@@ -40923,7 +41208,7 @@
         <v>2581</v>
       </c>
     </row>
-    <row r="3308" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3308" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3308" t="s">
         <v>2586</v>
       </c>
@@ -40931,7 +41216,7 @@
         <v>2586</v>
       </c>
     </row>
-    <row r="3309" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3309" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3309" t="s">
         <v>2535</v>
       </c>
@@ -40939,7 +41224,7 @@
         <v>2535</v>
       </c>
     </row>
-    <row r="3310" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3310" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3310" t="s">
         <v>2542</v>
       </c>
@@ -40947,7 +41232,7 @@
         <v>2542</v>
       </c>
     </row>
-    <row r="3311" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3311" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3311" t="s">
         <v>2544</v>
       </c>
@@ -40955,7 +41240,7 @@
         <v>2544</v>
       </c>
     </row>
-    <row r="3312" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3312" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3312" t="s">
         <v>2536</v>
       </c>
@@ -40963,7 +41248,7 @@
         <v>2536</v>
       </c>
     </row>
-    <row r="3313" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3313" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3313" t="s">
         <v>2540</v>
       </c>
@@ -40971,7 +41256,7 @@
         <v>2540</v>
       </c>
     </row>
-    <row r="3314" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3314" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3314" t="s">
         <v>2539</v>
       </c>
@@ -40979,7 +41264,7 @@
         <v>2539</v>
       </c>
     </row>
-    <row r="3315" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3315" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3315" t="s">
         <v>2534</v>
       </c>
@@ -40987,7 +41272,7 @@
         <v>2534</v>
       </c>
     </row>
-    <row r="3316" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3316" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3316" t="s">
         <v>2541</v>
       </c>
@@ -40995,7 +41280,7 @@
         <v>2541</v>
       </c>
     </row>
-    <row r="3317" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3317" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3317" t="s">
         <v>2537</v>
       </c>
@@ -41003,7 +41288,7 @@
         <v>2537</v>
       </c>
     </row>
-    <row r="3318" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3318" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3318" t="s">
         <v>2543</v>
       </c>
@@ -41011,7 +41296,7 @@
         <v>2543</v>
       </c>
     </row>
-    <row r="3319" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3319" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3319" t="s">
         <v>2533</v>
       </c>
@@ -41019,7 +41304,7 @@
         <v>2533</v>
       </c>
     </row>
-    <row r="3320" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3320" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3320" t="s">
         <v>2538</v>
       </c>
@@ -41027,7 +41312,7 @@
         <v>2538</v>
       </c>
     </row>
-    <row r="3321" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3321" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3321" t="s">
         <v>2630</v>
       </c>
@@ -41035,7 +41320,7 @@
         <v>2630</v>
       </c>
     </row>
-    <row r="3322" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3322" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3322" t="s">
         <v>2637</v>
       </c>
@@ -41043,7 +41328,7 @@
         <v>2637</v>
       </c>
     </row>
-    <row r="3323" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3323" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3323" t="s">
         <v>2639</v>
       </c>
@@ -41051,7 +41336,7 @@
         <v>2639</v>
       </c>
     </row>
-    <row r="3324" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3324" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3324" t="s">
         <v>2631</v>
       </c>
@@ -41059,7 +41344,7 @@
         <v>2631</v>
       </c>
     </row>
-    <row r="3325" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3325" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3325" t="s">
         <v>2635</v>
       </c>
@@ -41067,7 +41352,7 @@
         <v>2635</v>
       </c>
     </row>
-    <row r="3326" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3326" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3326" t="s">
         <v>2634</v>
       </c>
@@ -41075,7 +41360,7 @@
         <v>2634</v>
       </c>
     </row>
-    <row r="3327" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3327" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3327" s="1" t="s">
         <v>2629</v>
       </c>
@@ -41083,7 +41368,7 @@
         <v>2629</v>
       </c>
     </row>
-    <row r="3328" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3328" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3328" t="s">
         <v>2636</v>
       </c>
@@ -41091,7 +41376,7 @@
         <v>2636</v>
       </c>
     </row>
-    <row r="3329" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3329" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3329" t="s">
         <v>2632</v>
       </c>
@@ -41099,7 +41384,7 @@
         <v>2632</v>
       </c>
     </row>
-    <row r="3330" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3330" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3330" t="s">
         <v>2638</v>
       </c>
@@ -41107,7 +41392,7 @@
         <v>2638</v>
       </c>
     </row>
-    <row r="3331" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3331" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3331" t="s">
         <v>2628</v>
       </c>
@@ -41115,7 +41400,7 @@
         <v>2628</v>
       </c>
     </row>
-    <row r="3332" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3332" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3332" t="s">
         <v>2633</v>
       </c>
@@ -41123,7 +41408,7 @@
         <v>2633</v>
       </c>
     </row>
-    <row r="3333" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3333" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3333" t="s">
         <v>2559</v>
       </c>
@@ -41131,7 +41416,7 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="3334" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3334" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3334" t="s">
         <v>2566</v>
       </c>
@@ -41139,7 +41424,7 @@
         <v>2566</v>
       </c>
     </row>
-    <row r="3335" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3335" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3335" t="s">
         <v>2568</v>
       </c>
@@ -41147,7 +41432,7 @@
         <v>2568</v>
       </c>
     </row>
-    <row r="3336" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3336" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3336" t="s">
         <v>2560</v>
       </c>
@@ -41155,7 +41440,7 @@
         <v>2560</v>
       </c>
     </row>
-    <row r="3337" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3337" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3337" t="s">
         <v>2564</v>
       </c>
@@ -41163,7 +41448,7 @@
         <v>2564</v>
       </c>
     </row>
-    <row r="3338" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3338" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3338" t="s">
         <v>2563</v>
       </c>
@@ -41171,7 +41456,7 @@
         <v>2563</v>
       </c>
     </row>
-    <row r="3339" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3339" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3339" t="s">
         <v>2558</v>
       </c>
@@ -41179,7 +41464,7 @@
         <v>2558</v>
       </c>
     </row>
-    <row r="3340" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3340" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3340" t="s">
         <v>2565</v>
       </c>
@@ -41187,7 +41472,7 @@
         <v>2565</v>
       </c>
     </row>
-    <row r="3341" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3341" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3341" t="s">
         <v>2561</v>
       </c>
@@ -41195,7 +41480,7 @@
         <v>2561</v>
       </c>
     </row>
-    <row r="3342" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3342" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3342" t="s">
         <v>2567</v>
       </c>
@@ -41203,7 +41488,7 @@
         <v>2567</v>
       </c>
     </row>
-    <row r="3343" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3343" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3343" t="s">
         <v>2557</v>
       </c>
@@ -41211,7 +41496,7 @@
         <v>2557</v>
       </c>
     </row>
-    <row r="3344" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3344" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3344" t="s">
         <v>2562</v>
       </c>
@@ -41219,7 +41504,7 @@
         <v>2562</v>
       </c>
     </row>
-    <row r="3345" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3345" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3345" t="s">
         <v>2499</v>
       </c>
@@ -41227,7 +41512,7 @@
         <v>2499</v>
       </c>
     </row>
-    <row r="3346" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3346" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3346" t="s">
         <v>2506</v>
       </c>
@@ -41235,7 +41520,7 @@
         <v>2506</v>
       </c>
     </row>
-    <row r="3347" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3347" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3347" t="s">
         <v>2508</v>
       </c>
@@ -41243,7 +41528,7 @@
         <v>2508</v>
       </c>
     </row>
-    <row r="3348" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3348" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3348" t="s">
         <v>2500</v>
       </c>
@@ -41251,7 +41536,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="3349" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3349" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3349" t="s">
         <v>2504</v>
       </c>
@@ -41259,7 +41544,7 @@
         <v>2504</v>
       </c>
     </row>
-    <row r="3350" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3350" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3350" t="s">
         <v>2503</v>
       </c>
@@ -41267,7 +41552,7 @@
         <v>2503</v>
       </c>
     </row>
-    <row r="3351" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3351" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3351" t="s">
         <v>2498</v>
       </c>
@@ -41275,7 +41560,7 @@
         <v>2498</v>
       </c>
     </row>
-    <row r="3352" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3352" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3352" t="s">
         <v>2505</v>
       </c>
@@ -41283,7 +41568,7 @@
         <v>2505</v>
       </c>
     </row>
-    <row r="3353" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3353" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3353" t="s">
         <v>2501</v>
       </c>
@@ -41291,7 +41576,7 @@
         <v>2501</v>
       </c>
     </row>
-    <row r="3354" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3354" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3354" t="s">
         <v>2507</v>
       </c>
@@ -41299,7 +41584,7 @@
         <v>2507</v>
       </c>
     </row>
-    <row r="3355" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3355" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3355" t="s">
         <v>2497</v>
       </c>
@@ -41307,7 +41592,7 @@
         <v>2497</v>
       </c>
     </row>
-    <row r="3356" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3356" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3356" t="s">
         <v>2502</v>
       </c>
@@ -41315,7 +41600,7 @@
         <v>2502</v>
       </c>
     </row>
-    <row r="3357" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3357" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3357" t="s">
         <v>2571</v>
       </c>
@@ -41323,7 +41608,7 @@
         <v>2571</v>
       </c>
     </row>
-    <row r="3358" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3358" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3358" t="s">
         <v>2578</v>
       </c>
@@ -41331,7 +41616,7 @@
         <v>2578</v>
       </c>
     </row>
-    <row r="3359" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3359" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3359" t="s">
         <v>2580</v>
       </c>
@@ -41339,7 +41624,7 @@
         <v>2580</v>
       </c>
     </row>
-    <row r="3360" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3360" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3360" t="s">
         <v>2572</v>
       </c>
@@ -41347,7 +41632,7 @@
         <v>2572</v>
       </c>
     </row>
-    <row r="3361" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3361" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3361" t="s">
         <v>2576</v>
       </c>
@@ -41355,7 +41640,7 @@
         <v>2576</v>
       </c>
     </row>
-    <row r="3362" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3362" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3362" t="s">
         <v>2575</v>
       </c>
@@ -41363,7 +41648,7 @@
         <v>2575</v>
       </c>
     </row>
-    <row r="3363" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3363" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3363" t="s">
         <v>2570</v>
       </c>
@@ -41371,7 +41656,7 @@
         <v>2570</v>
       </c>
     </row>
-    <row r="3364" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3364" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3364" t="s">
         <v>2577</v>
       </c>
@@ -41379,7 +41664,7 @@
         <v>2577</v>
       </c>
     </row>
-    <row r="3365" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3365" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3365" t="s">
         <v>2573</v>
       </c>
@@ -41387,7 +41672,7 @@
         <v>2573</v>
       </c>
     </row>
-    <row r="3366" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3366" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3366" t="s">
         <v>2579</v>
       </c>
@@ -41395,7 +41680,7 @@
         <v>2579</v>
       </c>
     </row>
-    <row r="3367" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3367" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3367" t="s">
         <v>2569</v>
       </c>
@@ -41403,7 +41688,7 @@
         <v>2569</v>
       </c>
     </row>
-    <row r="3368" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3368" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3368" t="s">
         <v>2574</v>
       </c>
@@ -41411,7 +41696,7 @@
         <v>2574</v>
       </c>
     </row>
-    <row r="3369" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3369" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3369" t="s">
         <v>2619</v>
       </c>
@@ -41419,7 +41704,7 @@
         <v>2619</v>
       </c>
     </row>
-    <row r="3370" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3370" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3370" t="s">
         <v>2626</v>
       </c>
@@ -41427,7 +41712,7 @@
         <v>2626</v>
       </c>
     </row>
-    <row r="3371" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3371" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3371" t="s">
         <v>1565</v>
       </c>
@@ -41435,7 +41720,7 @@
         <v>1565</v>
       </c>
     </row>
-    <row r="3372" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3372" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3372" t="s">
         <v>2620</v>
       </c>
@@ -41443,7 +41728,7 @@
         <v>2620</v>
       </c>
     </row>
-    <row r="3373" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3373" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3373" t="s">
         <v>2624</v>
       </c>
@@ -41451,7 +41736,7 @@
         <v>2624</v>
       </c>
     </row>
-    <row r="3374" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3374" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3374" t="s">
         <v>2623</v>
       </c>
@@ -41459,7 +41744,7 @@
         <v>2623</v>
       </c>
     </row>
-    <row r="3375" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3375" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3375" t="s">
         <v>2618</v>
       </c>
@@ -41467,7 +41752,7 @@
         <v>2618</v>
       </c>
     </row>
-    <row r="3376" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3376" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3376" t="s">
         <v>2625</v>
       </c>
@@ -41475,7 +41760,7 @@
         <v>2625</v>
       </c>
     </row>
-    <row r="3377" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3377" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3377" t="s">
         <v>2621</v>
       </c>
@@ -41483,7 +41768,7 @@
         <v>2621</v>
       </c>
     </row>
-    <row r="3378" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3378" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3378" t="s">
         <v>2627</v>
       </c>
@@ -41491,7 +41776,7 @@
         <v>2627</v>
       </c>
     </row>
-    <row r="3379" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3379" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3379" t="s">
         <v>2617</v>
       </c>
@@ -41499,7 +41784,7 @@
         <v>2617</v>
       </c>
     </row>
-    <row r="3380" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3380" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3380" t="s">
         <v>2622</v>
       </c>
@@ -41507,7 +41792,7 @@
         <v>2622</v>
       </c>
     </row>
-    <row r="3381" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3381" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3381" t="s">
         <v>2487</v>
       </c>
@@ -41515,7 +41800,7 @@
         <v>2487</v>
       </c>
     </row>
-    <row r="3382" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3382" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3382" t="s">
         <v>2494</v>
       </c>
@@ -41523,7 +41808,7 @@
         <v>2494</v>
       </c>
     </row>
-    <row r="3383" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3383" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3383" t="s">
         <v>2496</v>
       </c>
@@ -41531,7 +41816,7 @@
         <v>2496</v>
       </c>
     </row>
-    <row r="3384" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3384" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3384" t="s">
         <v>2488</v>
       </c>
@@ -41539,7 +41824,7 @@
         <v>2488</v>
       </c>
     </row>
-    <row r="3385" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3385" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3385" t="s">
         <v>2492</v>
       </c>
@@ -41547,7 +41832,7 @@
         <v>2492</v>
       </c>
     </row>
-    <row r="3386" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3386" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3386" t="s">
         <v>2491</v>
       </c>
@@ -41555,7 +41840,7 @@
         <v>2491</v>
       </c>
     </row>
-    <row r="3387" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3387" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3387" t="s">
         <v>2486</v>
       </c>
@@ -41563,7 +41848,7 @@
         <v>2486</v>
       </c>
     </row>
-    <row r="3388" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3388" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3388" t="s">
         <v>2493</v>
       </c>
@@ -41571,7 +41856,7 @@
         <v>2493</v>
       </c>
     </row>
-    <row r="3389" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3389" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3389" t="s">
         <v>2489</v>
       </c>
@@ -41579,7 +41864,7 @@
         <v>2489</v>
       </c>
     </row>
-    <row r="3390" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3390" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3390" t="s">
         <v>2495</v>
       </c>
@@ -41587,7 +41872,7 @@
         <v>2495</v>
       </c>
     </row>
-    <row r="3391" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3391" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3391" t="s">
         <v>2485</v>
       </c>
@@ -41595,7 +41880,7 @@
         <v>2485</v>
       </c>
     </row>
-    <row r="3392" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3392" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3392" t="s">
         <v>2490</v>
       </c>
@@ -41603,7 +41888,7 @@
         <v>2490</v>
       </c>
     </row>
-    <row r="3393" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3393" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3393" t="s">
         <v>2523</v>
       </c>
@@ -41611,7 +41896,7 @@
         <v>2523</v>
       </c>
     </row>
-    <row r="3394" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3394" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3394" t="s">
         <v>2530</v>
       </c>
@@ -41619,7 +41904,7 @@
         <v>2530</v>
       </c>
     </row>
-    <row r="3395" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3395" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3395" t="s">
         <v>2532</v>
       </c>
@@ -41627,7 +41912,7 @@
         <v>2532</v>
       </c>
     </row>
-    <row r="3396" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3396" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3396" t="s">
         <v>2524</v>
       </c>
@@ -41635,7 +41920,7 @@
         <v>2524</v>
       </c>
     </row>
-    <row r="3397" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3397" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3397" t="s">
         <v>2528</v>
       </c>
@@ -41643,7 +41928,7 @@
         <v>2528</v>
       </c>
     </row>
-    <row r="3398" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3398" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3398" t="s">
         <v>2527</v>
       </c>
@@ -41651,7 +41936,7 @@
         <v>2527</v>
       </c>
     </row>
-    <row r="3399" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3399" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3399" t="s">
         <v>2522</v>
       </c>
@@ -41659,7 +41944,7 @@
         <v>2522</v>
       </c>
     </row>
-    <row r="3400" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3400" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3400" t="s">
         <v>2529</v>
       </c>
@@ -41667,7 +41952,7 @@
         <v>2529</v>
       </c>
     </row>
-    <row r="3401" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3401" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3401" t="s">
         <v>2525</v>
       </c>
@@ -41675,7 +41960,7 @@
         <v>2525</v>
       </c>
     </row>
-    <row r="3402" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3402" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3402" t="s">
         <v>2531</v>
       </c>
@@ -41683,7 +41968,7 @@
         <v>2531</v>
       </c>
     </row>
-    <row r="3403" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3403" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3403" t="s">
         <v>2521</v>
       </c>
@@ -41691,7 +41976,7 @@
         <v>2521</v>
       </c>
     </row>
-    <row r="3404" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3404" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3404" t="s">
         <v>2526</v>
       </c>
@@ -41699,7 +41984,7 @@
         <v>2526</v>
       </c>
     </row>
-    <row r="3405" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3405" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3405" t="s">
         <v>2607</v>
       </c>
@@ -41707,7 +41992,7 @@
         <v>2607</v>
       </c>
     </row>
-    <row r="3406" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3406" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3406" t="s">
         <v>2614</v>
       </c>
@@ -41715,7 +42000,7 @@
         <v>2614</v>
       </c>
     </row>
-    <row r="3407" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3407" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3407" t="s">
         <v>2616</v>
       </c>
@@ -41723,7 +42008,7 @@
         <v>2616</v>
       </c>
     </row>
-    <row r="3408" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3408" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3408" t="s">
         <v>2608</v>
       </c>
@@ -41731,7 +42016,7 @@
         <v>2608</v>
       </c>
     </row>
-    <row r="3409" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3409" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3409" t="s">
         <v>2612</v>
       </c>
@@ -41739,7 +42024,7 @@
         <v>2612</v>
       </c>
     </row>
-    <row r="3410" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3410" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3410" t="s">
         <v>2611</v>
       </c>
@@ -41747,7 +42032,7 @@
         <v>2611</v>
       </c>
     </row>
-    <row r="3411" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3411" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3411" t="s">
         <v>2606</v>
       </c>
@@ -41755,7 +42040,7 @@
         <v>2606</v>
       </c>
     </row>
-    <row r="3412" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3412" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3412" t="s">
         <v>2613</v>
       </c>
@@ -41763,7 +42048,7 @@
         <v>2613</v>
       </c>
     </row>
-    <row r="3413" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3413" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3413" t="s">
         <v>2609</v>
       </c>
@@ -41771,7 +42056,7 @@
         <v>2609</v>
       </c>
     </row>
-    <row r="3414" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3414" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3414" t="s">
         <v>2615</v>
       </c>
@@ -41779,7 +42064,7 @@
         <v>2615</v>
       </c>
     </row>
-    <row r="3415" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3415" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3415" t="s">
         <v>2605</v>
       </c>
@@ -41787,7 +42072,7 @@
         <v>2605</v>
       </c>
     </row>
-    <row r="3416" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3416" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3416" t="s">
         <v>2610</v>
       </c>
@@ -41795,7 +42080,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="3417" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3417" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3417" t="s">
         <v>2547</v>
       </c>
@@ -41803,7 +42088,7 @@
         <v>2547</v>
       </c>
     </row>
-    <row r="3418" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3418" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3418" t="s">
         <v>2554</v>
       </c>
@@ -41811,7 +42096,7 @@
         <v>2554</v>
       </c>
     </row>
-    <row r="3419" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3419" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3419" t="s">
         <v>2556</v>
       </c>
@@ -41819,7 +42104,7 @@
         <v>2556</v>
       </c>
     </row>
-    <row r="3420" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3420" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3420" t="s">
         <v>2548</v>
       </c>
@@ -41827,7 +42112,7 @@
         <v>2548</v>
       </c>
     </row>
-    <row r="3421" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3421" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3421" t="s">
         <v>2552</v>
       </c>
@@ -41835,7 +42120,7 @@
         <v>2552</v>
       </c>
     </row>
-    <row r="3422" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3422" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3422" t="s">
         <v>2551</v>
       </c>
@@ -41843,7 +42128,7 @@
         <v>2551</v>
       </c>
     </row>
-    <row r="3423" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3423" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3423" t="s">
         <v>2546</v>
       </c>
@@ -41851,7 +42136,7 @@
         <v>2546</v>
       </c>
     </row>
-    <row r="3424" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3424" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3424" t="s">
         <v>2553</v>
       </c>
@@ -41859,7 +42144,7 @@
         <v>2553</v>
       </c>
     </row>
-    <row r="3425" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3425" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3425" t="s">
         <v>2549</v>
       </c>
@@ -41867,7 +42152,7 @@
         <v>2549</v>
       </c>
     </row>
-    <row r="3426" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3426" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3426" t="s">
         <v>2555</v>
       </c>
@@ -41875,7 +42160,7 @@
         <v>2555</v>
       </c>
     </row>
-    <row r="3427" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3427" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3427" t="s">
         <v>2545</v>
       </c>
@@ -41883,7 +42168,7 @@
         <v>2545</v>
       </c>
     </row>
-    <row r="3428" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3428" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3428" t="s">
         <v>2550</v>
       </c>
@@ -41891,7 +42176,7 @@
         <v>2550</v>
       </c>
     </row>
-    <row r="3429" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3429" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3429" t="s">
         <v>2595</v>
       </c>
@@ -41899,7 +42184,7 @@
         <v>2595</v>
       </c>
     </row>
-    <row r="3430" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3430" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3430" t="s">
         <v>2602</v>
       </c>
@@ -41907,7 +42192,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="3431" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3431" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3431" t="s">
         <v>2604</v>
       </c>
@@ -41915,7 +42200,7 @@
         <v>2604</v>
       </c>
     </row>
-    <row r="3432" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3432" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3432" t="s">
         <v>2596</v>
       </c>
@@ -41923,7 +42208,7 @@
         <v>2596</v>
       </c>
     </row>
-    <row r="3433" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3433" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3433" t="s">
         <v>2600</v>
       </c>
@@ -41931,7 +42216,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="3434" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3434" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3434" t="s">
         <v>2599</v>
       </c>
@@ -41939,7 +42224,7 @@
         <v>2599</v>
       </c>
     </row>
-    <row r="3435" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3435" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3435" t="s">
         <v>2594</v>
       </c>
@@ -41947,7 +42232,7 @@
         <v>2594</v>
       </c>
     </row>
-    <row r="3436" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3436" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3436" t="s">
         <v>2601</v>
       </c>
@@ -41955,7 +42240,7 @@
         <v>2601</v>
       </c>
     </row>
-    <row r="3437" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3437" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3437" t="s">
         <v>2597</v>
       </c>
@@ -41963,7 +42248,7 @@
         <v>2597</v>
       </c>
     </row>
-    <row r="3438" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3438" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3438" t="s">
         <v>2603</v>
       </c>
@@ -41971,7 +42256,7 @@
         <v>2603</v>
       </c>
     </row>
-    <row r="3439" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3439" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3439" t="s">
         <v>2593</v>
       </c>
@@ -41979,7 +42264,7 @@
         <v>2593</v>
       </c>
     </row>
-    <row r="3440" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3440" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3440" t="s">
         <v>2598</v>
       </c>
@@ -41987,7 +42272,7 @@
         <v>2598</v>
       </c>
     </row>
-    <row r="3441" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3441" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3441" t="s">
         <v>2511</v>
       </c>
@@ -41995,7 +42280,7 @@
         <v>2511</v>
       </c>
     </row>
-    <row r="3442" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3442" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3442" t="s">
         <v>2518</v>
       </c>
@@ -42003,7 +42288,7 @@
         <v>2518</v>
       </c>
     </row>
-    <row r="3443" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3443" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3443" t="s">
         <v>2520</v>
       </c>
@@ -42011,7 +42296,7 @@
         <v>2520</v>
       </c>
     </row>
-    <row r="3444" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3444" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3444" t="s">
         <v>2512</v>
       </c>
@@ -42019,7 +42304,7 @@
         <v>2512</v>
       </c>
     </row>
-    <row r="3445" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3445" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3445" t="s">
         <v>2516</v>
       </c>
@@ -42027,7 +42312,7 @@
         <v>2516</v>
       </c>
     </row>
-    <row r="3446" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3446" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3446" t="s">
         <v>2515</v>
       </c>
@@ -42035,7 +42320,7 @@
         <v>2515</v>
       </c>
     </row>
-    <row r="3447" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3447" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3447" t="s">
         <v>2510</v>
       </c>
@@ -42043,7 +42328,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="3448" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3448" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3448" t="s">
         <v>2517</v>
       </c>
@@ -42051,7 +42336,7 @@
         <v>2517</v>
       </c>
     </row>
-    <row r="3449" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3449" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3449" t="s">
         <v>2513</v>
       </c>
@@ -42059,7 +42344,7 @@
         <v>2513</v>
       </c>
     </row>
-    <row r="3450" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3450" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3450" t="s">
         <v>2519</v>
       </c>
@@ -42067,7 +42352,7 @@
         <v>2519</v>
       </c>
     </row>
-    <row r="3451" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3451" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3451" t="s">
         <v>2509</v>
       </c>
@@ -42075,7 +42360,7 @@
         <v>2509</v>
       </c>
     </row>
-    <row r="3452" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3452" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3452" t="s">
         <v>2514</v>
       </c>
@@ -42083,7 +42368,7 @@
         <v>2514</v>
       </c>
     </row>
-    <row r="3453" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3453" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3453" s="1" t="s">
         <v>1001</v>
       </c>
@@ -44772,7 +45057,7 @@
         <v>3785</v>
       </c>
     </row>
-    <row r="3790" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3790" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3790" t="s">
         <v>3786</v>
       </c>
@@ -44780,7 +45065,7 @@
         <v>3786</v>
       </c>
     </row>
-    <row r="3791" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3791" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3791" t="s">
         <v>3787</v>
       </c>
@@ -48724,7 +49009,7 @@
         <v>4280</v>
       </c>
     </row>
-    <row r="4284" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4284" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4284" t="s">
         <v>4281</v>
       </c>
@@ -48732,7 +49017,7 @@
         <v>4281</v>
       </c>
     </row>
-    <row r="4285" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4285" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4285" t="s">
         <v>4282</v>
       </c>
@@ -48741,7 +49026,7 @@
       </c>
     </row>
     <row r="4286" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="4287" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4287" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4287" t="s">
         <v>4283</v>
       </c>
@@ -48781,7 +49066,7 @@
         <v>4287</v>
       </c>
     </row>
-    <row r="4292" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4292" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4292" t="s">
         <v>4288</v>
       </c>
@@ -48854,7 +49139,7 @@
       </c>
     </row>
     <row r="4301" spans="1:2" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="4302" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4302" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4302" t="s">
         <v>4297</v>
       </c>
@@ -48862,7 +49147,7 @@
         <v>4297</v>
       </c>
     </row>
-    <row r="4303" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4303" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4303" t="s">
         <v>4298</v>
       </c>
@@ -48870,7 +49155,7 @@
         <v>4298</v>
       </c>
     </row>
-    <row r="4304" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4304" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4304" t="s">
         <v>4299</v>
       </c>
@@ -48878,7 +49163,7 @@
         <v>4299</v>
       </c>
     </row>
-    <row r="4305" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4305" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4305" t="s">
         <v>4300</v>
       </c>
@@ -48886,7 +49171,7 @@
         <v>4300</v>
       </c>
     </row>
-    <row r="4306" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4306" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4306" t="s">
         <v>4301</v>
       </c>
@@ -48894,7 +49179,7 @@
         <v>4301</v>
       </c>
     </row>
-    <row r="4307" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4307" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4307" t="s">
         <v>4302</v>
       </c>
@@ -48902,7 +49187,7 @@
         <v>4302</v>
       </c>
     </row>
-    <row r="4308" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4308" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4308" t="s">
         <v>4303</v>
       </c>
@@ -48910,7 +49195,7 @@
         <v>4303</v>
       </c>
     </row>
-    <row r="4309" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4309" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4309" t="s">
         <v>4304</v>
       </c>
@@ -48918,7 +49203,7 @@
         <v>4304</v>
       </c>
     </row>
-    <row r="4310" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4310" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4310" t="s">
         <v>4305</v>
       </c>
@@ -48926,7 +49211,7 @@
         <v>4305</v>
       </c>
     </row>
-    <row r="4311" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4311" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4311" t="s">
         <v>4306</v>
       </c>
@@ -48934,7 +49219,7 @@
         <v>4306</v>
       </c>
     </row>
-    <row r="4312" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4312" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4312" t="s">
         <v>4307</v>
       </c>
@@ -48942,7 +49227,7 @@
         <v>4307</v>
       </c>
     </row>
-    <row r="4313" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4313" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4313" t="s">
         <v>4308</v>
       </c>
@@ -48950,7 +49235,7 @@
         <v>4308</v>
       </c>
     </row>
-    <row r="4314" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4314" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4314" t="s">
         <v>4309</v>
       </c>
@@ -49294,7 +49579,7 @@
         <v>4351</v>
       </c>
     </row>
-    <row r="4357" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4357" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4357" t="s">
         <v>4352</v>
       </c>
@@ -49302,7 +49587,7 @@
         <v>4352</v>
       </c>
     </row>
-    <row r="4358" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4358" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4358" t="s">
         <v>4353</v>
       </c>
@@ -49310,7 +49595,7 @@
         <v>4353</v>
       </c>
     </row>
-    <row r="4359" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4359" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4359" t="s">
         <v>4354</v>
       </c>
@@ -49318,7 +49603,7 @@
         <v>4354</v>
       </c>
     </row>
-    <row r="4360" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4360" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4360" t="s">
         <v>4355</v>
       </c>
@@ -49326,7 +49611,7 @@
         <v>4355</v>
       </c>
     </row>
-    <row r="4361" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4361" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4361" t="s">
         <v>4356</v>
       </c>
@@ -49334,7 +49619,7 @@
         <v>4356</v>
       </c>
     </row>
-    <row r="4362" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4362" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4362" t="s">
         <v>4357</v>
       </c>
@@ -49342,7 +49627,7 @@
         <v>4357</v>
       </c>
     </row>
-    <row r="4363" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4363" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4363" t="s">
         <v>4358</v>
       </c>
@@ -49350,7 +49635,7 @@
         <v>4358</v>
       </c>
     </row>
-    <row r="4364" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4364" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4364" t="s">
         <v>4359</v>
       </c>
@@ -49858,7 +50143,7 @@
   <autoFilter ref="A1:G4424" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
     <filterColumn colId="0">
       <customFilters>
-        <customFilter val="Tử Vi*"/>
+        <customFilter val="Liêm Trinh*"/>
       </customFilters>
     </filterColumn>
   </autoFilter>
@@ -49867,45 +50152,43 @@
   </sortState>
   <dataConsolidate/>
   <conditionalFormatting sqref="A4293:A1048576 A2:A4285">
-    <cfRule type="duplicateValues" dxfId="13" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6716:A1048576 A2:A4170">
-    <cfRule type="duplicateValues" dxfId="12" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="21"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4293:B4419 B4421:B1048576 B3265:B3266 B2:B3263 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B3294:B4285">
-    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+  <conditionalFormatting sqref="B3281">
+    <cfRule type="duplicateValues" dxfId="13" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3285">
+    <cfRule type="duplicateValues" dxfId="11" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3289">
+    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3293">
+    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4293:B4419 B4421:B1048576 B3265:B3266 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B3294:B4285 B815:B3263 B2:B813">
+    <cfRule type="duplicateValues" dxfId="5" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4420">
-    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6716:B1048576 B4401:B4404 B3265:B3266 B2:B3263 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B3294:B4170">
-    <cfRule type="duplicateValues" dxfId="9" priority="13"/>
+  <conditionalFormatting sqref="B6716:B1048576 B4401:B4404 B3265:B3266 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B3294:B4170 B815:B3263 B2:B813">
+    <cfRule type="duplicateValues" dxfId="3" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3721">
-    <cfRule type="duplicateValues" dxfId="8" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3281">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3281">
-    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3285">
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3285">
-    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3289">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3289">
-    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3293">
+  <conditionalFormatting sqref="B814">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3293">
+  <conditionalFormatting sqref="B814">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Giải thích Thiên đồng tại Mệnh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1103FB7-3322-4D4E-830A-FF845C6F383C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C94E72-B22B-4EF4-8BD8-23502B9414E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4260" yWindow="1875" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9004" uniqueCount="4581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9006" uniqueCount="4584">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13771,6 +13771,15 @@
   </si>
   <si>
     <t>Bạn là người có tài thao lược, cơ mưu  quyền biến</t>
+  </si>
+  <si>
+    <t>Có thể kinh doanh hoặc làm kỹ thuật</t>
+  </si>
+  <si>
+    <t>Thân hình nở nang, da trắng, hơi thấp</t>
+  </si>
+  <si>
+    <t>Bạn là người thông minh, có tính khoan hoà, nhân hậu từ thiện, nhưng tính tình thiếu quả quyết. Nhưng sống hưởng trọn phúc thọ song toàn.</t>
   </si>
 </sst>
 </file>
@@ -13824,11 +13833,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14273,8 +14283,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A2:G4424"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A786" workbookViewId="0">
-      <selection activeCell="A792" sqref="A792"/>
+    <sheetView tabSelected="1" topLeftCell="A2412" workbookViewId="0">
+      <selection activeCell="A2425" sqref="A2425"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20488,7 +20498,7 @@
         <v>1607</v>
       </c>
     </row>
-    <row r="769" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="769" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A769" t="s">
         <v>986</v>
       </c>
@@ -20496,7 +20506,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="770" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="770" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A770" t="s">
         <v>1630</v>
       </c>
@@ -20504,7 +20514,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="771" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="771" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A771" t="s">
         <v>1578</v>
       </c>
@@ -20512,7 +20522,7 @@
         <v>1578</v>
       </c>
     </row>
-    <row r="772" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="772" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A772" t="s">
         <v>1591</v>
       </c>
@@ -20520,7 +20530,7 @@
         <v>1591</v>
       </c>
     </row>
-    <row r="773" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="773" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A773" t="s">
         <v>1574</v>
       </c>
@@ -20528,7 +20538,7 @@
         <v>1574</v>
       </c>
     </row>
-    <row r="774" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="774" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A774" s="3" t="s">
         <v>70</v>
       </c>
@@ -20536,7 +20546,7 @@
         <v>4564</v>
       </c>
     </row>
-    <row r="775" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="775" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A775" s="3" t="s">
         <v>117</v>
       </c>
@@ -20544,7 +20554,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="776" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="776" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A776" s="3" t="s">
         <v>118</v>
       </c>
@@ -20552,7 +20562,7 @@
         <v>4565</v>
       </c>
     </row>
-    <row r="777" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="777" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A777" s="3" t="s">
         <v>89</v>
       </c>
@@ -20563,7 +20573,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="778" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="778" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A778" s="3" t="s">
         <v>1008</v>
       </c>
@@ -20574,7 +20584,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="779" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="779" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A779" s="3" t="s">
         <v>88</v>
       </c>
@@ -20588,7 +20598,7 @@
         <v>4570</v>
       </c>
     </row>
-    <row r="780" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="780" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A780" s="3" t="s">
         <v>108</v>
       </c>
@@ -20602,7 +20612,7 @@
         <v>4571</v>
       </c>
     </row>
-    <row r="781" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="781" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A781" s="3" t="s">
         <v>109</v>
       </c>
@@ -20613,7 +20623,7 @@
         <v>4573</v>
       </c>
     </row>
-    <row r="782" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="782" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A782" s="3" t="s">
         <v>1181</v>
       </c>
@@ -20626,8 +20636,11 @@
       <c r="D782" t="s">
         <v>4578</v>
       </c>
-    </row>
-    <row r="783" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E782" t="s">
+        <v>4581</v>
+      </c>
+    </row>
+    <row r="783" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A783" s="3" t="s">
         <v>116</v>
       </c>
@@ -20641,7 +20654,7 @@
         <v>4577</v>
       </c>
     </row>
-    <row r="784" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="784" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A784" s="3" t="s">
         <v>16</v>
       </c>
@@ -20655,7 +20668,7 @@
         <v>4571</v>
       </c>
     </row>
-    <row r="785" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="785" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A785" s="3" t="s">
         <v>113</v>
       </c>
@@ -20666,7 +20679,7 @@
         <v>4576</v>
       </c>
     </row>
-    <row r="786" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="786" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A786" s="3" t="s">
         <v>104</v>
       </c>
@@ -20677,7 +20690,7 @@
         <v>4573</v>
       </c>
     </row>
-    <row r="787" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="787" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A787" s="3" t="s">
         <v>1013</v>
       </c>
@@ -20688,7 +20701,7 @@
         <v>4574</v>
       </c>
     </row>
-    <row r="788" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="788" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A788" s="3" t="s">
         <v>17</v>
       </c>
@@ -20696,7 +20709,7 @@
         <v>4567</v>
       </c>
     </row>
-    <row r="789" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="789" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A789" s="3" t="s">
         <v>106</v>
       </c>
@@ -20707,7 +20720,7 @@
         <v>4573</v>
       </c>
     </row>
-    <row r="790" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="790" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A790" s="3" t="s">
         <v>1180</v>
       </c>
@@ -20720,8 +20733,11 @@
       <c r="D790" t="s">
         <v>4578</v>
       </c>
-    </row>
-    <row r="791" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E790" t="s">
+        <v>4581</v>
+      </c>
+    </row>
+    <row r="791" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A791" s="3" t="s">
         <v>115</v>
       </c>
@@ -20735,7 +20751,7 @@
         <v>4577</v>
       </c>
     </row>
-    <row r="792" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="792" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A792" s="3" t="s">
         <v>101</v>
       </c>
@@ -20743,7 +20759,7 @@
         <v>4580</v>
       </c>
     </row>
-    <row r="793" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="793" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A793" s="3" t="s">
         <v>99</v>
       </c>
@@ -20754,7 +20770,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="794" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="794" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A794" s="3" t="s">
         <v>1011</v>
       </c>
@@ -20765,7 +20781,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="795" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="795" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A795" s="3" t="s">
         <v>98</v>
       </c>
@@ -20779,7 +20795,7 @@
         <v>4570</v>
       </c>
     </row>
-    <row r="796" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="796" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A796" s="3" t="s">
         <v>86</v>
       </c>
@@ -20790,7 +20806,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="797" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="797" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A797" s="3" t="s">
         <v>1007</v>
       </c>
@@ -20801,7 +20817,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="798" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="798" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A798" s="3" t="s">
         <v>85</v>
       </c>
@@ -20815,7 +20831,7 @@
         <v>4570</v>
       </c>
     </row>
-    <row r="799" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="799" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A799" s="3" t="s">
         <v>97</v>
       </c>
@@ -20823,7 +20839,7 @@
         <v>4580</v>
       </c>
     </row>
-    <row r="800" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="800" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A800" s="3" t="s">
         <v>95</v>
       </c>
@@ -20834,7 +20850,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="801" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="801" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A801" s="3" t="s">
         <v>1010</v>
       </c>
@@ -20845,7 +20861,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="802" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="802" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A802" s="3" t="s">
         <v>94</v>
       </c>
@@ -20859,7 +20875,7 @@
         <v>4570</v>
       </c>
     </row>
-    <row r="803" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="803" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A803" s="3" t="s">
         <v>92</v>
       </c>
@@ -20870,7 +20886,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="804" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="804" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A804" s="3" t="s">
         <v>1009</v>
       </c>
@@ -20881,7 +20897,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="805" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="805" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A805" s="3" t="s">
         <v>91</v>
       </c>
@@ -20895,7 +20911,7 @@
         <v>4570</v>
       </c>
     </row>
-    <row r="806" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="806" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A806" s="3" t="s">
         <v>77</v>
       </c>
@@ -20906,7 +20922,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="807" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="807" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A807" s="3" t="s">
         <v>1004</v>
       </c>
@@ -20917,7 +20933,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="808" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="808" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A808" s="3" t="s">
         <v>76</v>
       </c>
@@ -20931,7 +20947,7 @@
         <v>4570</v>
       </c>
     </row>
-    <row r="809" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="809" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A809" s="3" t="s">
         <v>80</v>
       </c>
@@ -20942,7 +20958,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="810" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="810" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A810" s="3" t="s">
         <v>1005</v>
       </c>
@@ -20953,7 +20969,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="811" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="811" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A811" s="3" t="s">
         <v>79</v>
       </c>
@@ -20967,7 +20983,7 @@
         <v>4570</v>
       </c>
     </row>
-    <row r="812" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="812" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A812" s="3" t="s">
         <v>15</v>
       </c>
@@ -20981,7 +20997,7 @@
         <v>4571</v>
       </c>
     </row>
-    <row r="813" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="813" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A813" s="3" t="s">
         <v>111</v>
       </c>
@@ -20992,7 +21008,7 @@
         <v>4576</v>
       </c>
     </row>
-    <row r="814" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="814" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A814" s="3" t="s">
         <v>83</v>
       </c>
@@ -21000,7 +21016,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="815" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="815" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A815" s="3" t="s">
         <v>102</v>
       </c>
@@ -21011,7 +21027,7 @@
         <v>4573</v>
       </c>
     </row>
-    <row r="816" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="816" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A816" s="3" t="s">
         <v>1006</v>
       </c>
@@ -21022,7 +21038,7 @@
         <v>4568</v>
       </c>
     </row>
-    <row r="817" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="817" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A817" s="3" t="s">
         <v>1012</v>
       </c>
@@ -21033,7 +21049,7 @@
         <v>4574</v>
       </c>
     </row>
-    <row r="818" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="818" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A818" s="3" t="s">
         <v>82</v>
       </c>
@@ -21047,7 +21063,7 @@
         <v>4570</v>
       </c>
     </row>
-    <row r="819" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="819" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A819" s="3" t="s">
         <v>2381</v>
       </c>
@@ -21058,7 +21074,7 @@
         <v>4579</v>
       </c>
     </row>
-    <row r="820" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="820" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A820" s="3" t="s">
         <v>2388</v>
       </c>
@@ -21072,7 +21088,7 @@
         <v>4571</v>
       </c>
     </row>
-    <row r="821" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="821" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A821" s="3" t="s">
         <v>2390</v>
       </c>
@@ -21086,7 +21102,7 @@
         <v>4571</v>
       </c>
     </row>
-    <row r="822" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="822" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A822" s="3" t="s">
         <v>2382</v>
       </c>
@@ -21100,7 +21116,7 @@
         <v>4571</v>
       </c>
     </row>
-    <row r="823" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="823" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A823" s="3" t="s">
         <v>2386</v>
       </c>
@@ -21111,7 +21127,7 @@
         <v>4579</v>
       </c>
     </row>
-    <row r="824" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="824" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A824" s="3" t="s">
         <v>2385</v>
       </c>
@@ -21122,7 +21138,7 @@
         <v>4579</v>
       </c>
     </row>
-    <row r="825" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="825" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A825" s="3" t="s">
         <v>2380</v>
       </c>
@@ -21133,7 +21149,7 @@
         <v>4579</v>
       </c>
     </row>
-    <row r="826" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="826" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A826" s="3" t="s">
         <v>2387</v>
       </c>
@@ -21144,7 +21160,7 @@
         <v>4579</v>
       </c>
     </row>
-    <row r="827" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="827" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A827" s="3" t="s">
         <v>2383</v>
       </c>
@@ -21155,7 +21171,7 @@
         <v>4579</v>
       </c>
     </row>
-    <row r="828" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="828" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A828" s="3" t="s">
         <v>2389</v>
       </c>
@@ -21166,7 +21182,7 @@
         <v>4579</v>
       </c>
     </row>
-    <row r="829" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="829" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A829" s="3" t="s">
         <v>2379</v>
       </c>
@@ -21177,7 +21193,7 @@
         <v>4579</v>
       </c>
     </row>
-    <row r="830" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="830" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A830" s="3" t="s">
         <v>2384</v>
       </c>
@@ -21191,7 +21207,7 @@
         <v>4571</v>
       </c>
     </row>
-    <row r="831" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="831" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A831" t="s">
         <v>3178</v>
       </c>
@@ -21199,7 +21215,7 @@
         <v>3178</v>
       </c>
     </row>
-    <row r="832" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="832" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A832" t="s">
         <v>3185</v>
       </c>
@@ -21207,7 +21223,7 @@
         <v>3185</v>
       </c>
     </row>
-    <row r="833" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="833" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A833" t="s">
         <v>3187</v>
       </c>
@@ -21215,7 +21231,7 @@
         <v>3187</v>
       </c>
     </row>
-    <row r="834" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="834" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A834" t="s">
         <v>3179</v>
       </c>
@@ -21223,7 +21239,7 @@
         <v>3179</v>
       </c>
     </row>
-    <row r="835" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="835" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A835" t="s">
         <v>3183</v>
       </c>
@@ -21231,7 +21247,7 @@
         <v>3183</v>
       </c>
     </row>
-    <row r="836" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="836" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A836" t="s">
         <v>3182</v>
       </c>
@@ -21239,7 +21255,7 @@
         <v>3182</v>
       </c>
     </row>
-    <row r="837" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="837" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A837" t="s">
         <v>3177</v>
       </c>
@@ -21247,7 +21263,7 @@
         <v>3177</v>
       </c>
     </row>
-    <row r="838" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="838" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A838" t="s">
         <v>3184</v>
       </c>
@@ -21255,7 +21271,7 @@
         <v>3184</v>
       </c>
     </row>
-    <row r="839" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="839" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A839" t="s">
         <v>3180</v>
       </c>
@@ -21263,7 +21279,7 @@
         <v>3180</v>
       </c>
     </row>
-    <row r="840" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="840" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A840" t="s">
         <v>3186</v>
       </c>
@@ -21271,7 +21287,7 @@
         <v>3186</v>
       </c>
     </row>
-    <row r="841" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="841" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A841" t="s">
         <v>3176</v>
       </c>
@@ -21279,7 +21295,7 @@
         <v>3176</v>
       </c>
     </row>
-    <row r="842" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="842" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A842" t="s">
         <v>3181</v>
       </c>
@@ -21287,7 +21303,7 @@
         <v>3181</v>
       </c>
     </row>
-    <row r="843" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="843" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A843" t="s">
         <v>3226</v>
       </c>
@@ -21295,7 +21311,7 @@
         <v>3226</v>
       </c>
     </row>
-    <row r="844" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="844" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A844" t="s">
         <v>3232</v>
       </c>
@@ -21303,7 +21319,7 @@
         <v>3232</v>
       </c>
     </row>
-    <row r="845" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="845" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A845" t="s">
         <v>3234</v>
       </c>
@@ -21311,7 +21327,7 @@
         <v>3234</v>
       </c>
     </row>
-    <row r="846" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="846" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A846" t="s">
         <v>1602</v>
       </c>
@@ -21319,7 +21335,7 @@
         <v>1602</v>
       </c>
     </row>
-    <row r="847" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="847" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A847" t="s">
         <v>3230</v>
       </c>
@@ -21327,7 +21343,7 @@
         <v>3230</v>
       </c>
     </row>
-    <row r="848" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="848" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A848" t="s">
         <v>3229</v>
       </c>
@@ -21335,7 +21351,7 @@
         <v>3229</v>
       </c>
     </row>
-    <row r="849" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="849" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A849" t="s">
         <v>3225</v>
       </c>
@@ -21343,7 +21359,7 @@
         <v>3225</v>
       </c>
     </row>
-    <row r="850" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="850" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A850" t="s">
         <v>3231</v>
       </c>
@@ -21351,7 +21367,7 @@
         <v>3231</v>
       </c>
     </row>
-    <row r="851" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="851" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A851" t="s">
         <v>3227</v>
       </c>
@@ -21359,7 +21375,7 @@
         <v>3227</v>
       </c>
     </row>
-    <row r="852" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="852" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A852" t="s">
         <v>3233</v>
       </c>
@@ -21367,7 +21383,7 @@
         <v>3233</v>
       </c>
     </row>
-    <row r="853" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="853" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A853" t="s">
         <v>3224</v>
       </c>
@@ -21375,7 +21391,7 @@
         <v>3224</v>
       </c>
     </row>
-    <row r="854" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="854" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A854" t="s">
         <v>3228</v>
       </c>
@@ -21383,7 +21399,7 @@
         <v>3228</v>
       </c>
     </row>
-    <row r="855" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="855" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A855" t="s">
         <v>3154</v>
       </c>
@@ -21391,7 +21407,7 @@
         <v>3154</v>
       </c>
     </row>
-    <row r="856" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="856" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A856" t="s">
         <v>3161</v>
       </c>
@@ -21399,7 +21415,7 @@
         <v>3161</v>
       </c>
     </row>
-    <row r="857" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="857" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A857" t="s">
         <v>3163</v>
       </c>
@@ -21407,7 +21423,7 @@
         <v>3163</v>
       </c>
     </row>
-    <row r="858" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="858" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A858" t="s">
         <v>3155</v>
       </c>
@@ -21415,7 +21431,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="859" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="859" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A859" t="s">
         <v>3159</v>
       </c>
@@ -21423,7 +21439,7 @@
         <v>3159</v>
       </c>
     </row>
-    <row r="860" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="860" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A860" t="s">
         <v>3158</v>
       </c>
@@ -21431,7 +21447,7 @@
         <v>3158</v>
       </c>
     </row>
-    <row r="861" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="861" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A861" t="s">
         <v>3153</v>
       </c>
@@ -21439,7 +21455,7 @@
         <v>3153</v>
       </c>
     </row>
-    <row r="862" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="862" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A862" t="s">
         <v>3160</v>
       </c>
@@ -21447,7 +21463,7 @@
         <v>3160</v>
       </c>
     </row>
-    <row r="863" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="863" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A863" t="s">
         <v>3156</v>
       </c>
@@ -21455,7 +21471,7 @@
         <v>3156</v>
       </c>
     </row>
-    <row r="864" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="864" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A864" t="s">
         <v>3162</v>
       </c>
@@ -21463,7 +21479,7 @@
         <v>3162</v>
       </c>
     </row>
-    <row r="865" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="865" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A865" t="s">
         <v>3152</v>
       </c>
@@ -21471,7 +21487,7 @@
         <v>3152</v>
       </c>
     </row>
-    <row r="866" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="866" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A866" t="s">
         <v>3157</v>
       </c>
@@ -21479,7 +21495,7 @@
         <v>3157</v>
       </c>
     </row>
-    <row r="867" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="867" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A867" t="s">
         <v>3166</v>
       </c>
@@ -21487,7 +21503,7 @@
         <v>3166</v>
       </c>
     </row>
-    <row r="868" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="868" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A868" t="s">
         <v>3173</v>
       </c>
@@ -21495,7 +21511,7 @@
         <v>3173</v>
       </c>
     </row>
-    <row r="869" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="869" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A869" t="s">
         <v>3175</v>
       </c>
@@ -21503,7 +21519,7 @@
         <v>3175</v>
       </c>
     </row>
-    <row r="870" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="870" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A870" t="s">
         <v>3167</v>
       </c>
@@ -21511,7 +21527,7 @@
         <v>3167</v>
       </c>
     </row>
-    <row r="871" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="871" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A871" t="s">
         <v>3171</v>
       </c>
@@ -21519,7 +21535,7 @@
         <v>3171</v>
       </c>
     </row>
-    <row r="872" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="872" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A872" t="s">
         <v>3170</v>
       </c>
@@ -21527,7 +21543,7 @@
         <v>3170</v>
       </c>
     </row>
-    <row r="873" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="873" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A873" t="s">
         <v>3165</v>
       </c>
@@ -21535,7 +21551,7 @@
         <v>3165</v>
       </c>
     </row>
-    <row r="874" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="874" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A874" t="s">
         <v>3172</v>
       </c>
@@ -21543,7 +21559,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="875" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="875" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A875" t="s">
         <v>3168</v>
       </c>
@@ -21551,7 +21567,7 @@
         <v>3168</v>
       </c>
     </row>
-    <row r="876" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="876" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A876" t="s">
         <v>3174</v>
       </c>
@@ -21559,7 +21575,7 @@
         <v>3174</v>
       </c>
     </row>
-    <row r="877" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="877" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A877" t="s">
         <v>3164</v>
       </c>
@@ -21567,7 +21583,7 @@
         <v>3164</v>
       </c>
     </row>
-    <row r="878" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="878" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A878" t="s">
         <v>3169</v>
       </c>
@@ -21575,7 +21591,7 @@
         <v>3169</v>
       </c>
     </row>
-    <row r="879" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="879" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A879" t="s">
         <v>3214</v>
       </c>
@@ -21583,7 +21599,7 @@
         <v>3214</v>
       </c>
     </row>
-    <row r="880" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="880" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A880" t="s">
         <v>3221</v>
       </c>
@@ -21591,7 +21607,7 @@
         <v>3221</v>
       </c>
     </row>
-    <row r="881" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="881" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A881" t="s">
         <v>3223</v>
       </c>
@@ -21599,7 +21615,7 @@
         <v>3223</v>
       </c>
     </row>
-    <row r="882" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="882" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A882" t="s">
         <v>3215</v>
       </c>
@@ -21607,7 +21623,7 @@
         <v>3215</v>
       </c>
     </row>
-    <row r="883" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="883" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A883" t="s">
         <v>3219</v>
       </c>
@@ -21615,7 +21631,7 @@
         <v>3219</v>
       </c>
     </row>
-    <row r="884" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="884" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A884" t="s">
         <v>3218</v>
       </c>
@@ -21623,7 +21639,7 @@
         <v>3218</v>
       </c>
     </row>
-    <row r="885" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="885" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A885" t="s">
         <v>3213</v>
       </c>
@@ -21631,7 +21647,7 @@
         <v>3213</v>
       </c>
     </row>
-    <row r="886" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="886" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A886" t="s">
         <v>3220</v>
       </c>
@@ -21639,7 +21655,7 @@
         <v>3220</v>
       </c>
     </row>
-    <row r="887" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="887" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A887" t="s">
         <v>3216</v>
       </c>
@@ -21647,7 +21663,7 @@
         <v>3216</v>
       </c>
     </row>
-    <row r="888" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="888" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A888" t="s">
         <v>3222</v>
       </c>
@@ -21655,7 +21671,7 @@
         <v>3222</v>
       </c>
     </row>
-    <row r="889" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="889" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A889" t="s">
         <v>3212</v>
       </c>
@@ -21663,7 +21679,7 @@
         <v>3212</v>
       </c>
     </row>
-    <row r="890" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="890" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A890" t="s">
         <v>3217</v>
       </c>
@@ -21671,7 +21687,7 @@
         <v>3217</v>
       </c>
     </row>
-    <row r="891" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="891" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A891" t="s">
         <v>3202</v>
       </c>
@@ -21679,7 +21695,7 @@
         <v>3202</v>
       </c>
     </row>
-    <row r="892" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="892" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A892" t="s">
         <v>3209</v>
       </c>
@@ -21687,7 +21703,7 @@
         <v>3209</v>
       </c>
     </row>
-    <row r="893" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="893" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A893" t="s">
         <v>3211</v>
       </c>
@@ -21695,7 +21711,7 @@
         <v>3211</v>
       </c>
     </row>
-    <row r="894" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="894" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A894" t="s">
         <v>3203</v>
       </c>
@@ -21703,7 +21719,7 @@
         <v>3203</v>
       </c>
     </row>
-    <row r="895" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="895" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A895" t="s">
         <v>3207</v>
       </c>
@@ -21711,7 +21727,7 @@
         <v>3207</v>
       </c>
     </row>
-    <row r="896" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="896" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A896" t="s">
         <v>3206</v>
       </c>
@@ -21719,7 +21735,7 @@
         <v>3206</v>
       </c>
     </row>
-    <row r="897" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="897" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A897" t="s">
         <v>3201</v>
       </c>
@@ -21727,7 +21743,7 @@
         <v>3201</v>
       </c>
     </row>
-    <row r="898" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="898" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A898" t="s">
         <v>3208</v>
       </c>
@@ -21735,7 +21751,7 @@
         <v>3208</v>
       </c>
     </row>
-    <row r="899" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="899" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A899" t="s">
         <v>3204</v>
       </c>
@@ -21743,7 +21759,7 @@
         <v>3204</v>
       </c>
     </row>
-    <row r="900" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="900" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A900" t="s">
         <v>3210</v>
       </c>
@@ -21751,7 +21767,7 @@
         <v>3210</v>
       </c>
     </row>
-    <row r="901" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="901" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A901" t="s">
         <v>3200</v>
       </c>
@@ -21759,7 +21775,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="902" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="902" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A902" t="s">
         <v>3205</v>
       </c>
@@ -21767,7 +21783,7 @@
         <v>3205</v>
       </c>
     </row>
-    <row r="903" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="903" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A903" t="s">
         <v>3142</v>
       </c>
@@ -21775,7 +21791,7 @@
         <v>3142</v>
       </c>
     </row>
-    <row r="904" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="904" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A904" t="s">
         <v>3149</v>
       </c>
@@ -21783,7 +21799,7 @@
         <v>3149</v>
       </c>
     </row>
-    <row r="905" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="905" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A905" t="s">
         <v>3151</v>
       </c>
@@ -21791,7 +21807,7 @@
         <v>3151</v>
       </c>
     </row>
-    <row r="906" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="906" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A906" t="s">
         <v>3143</v>
       </c>
@@ -21799,7 +21815,7 @@
         <v>3143</v>
       </c>
     </row>
-    <row r="907" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="907" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A907" t="s">
         <v>3147</v>
       </c>
@@ -21807,7 +21823,7 @@
         <v>3147</v>
       </c>
     </row>
-    <row r="908" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="908" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A908" t="s">
         <v>3146</v>
       </c>
@@ -21815,7 +21831,7 @@
         <v>3146</v>
       </c>
     </row>
-    <row r="909" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="909" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A909" t="s">
         <v>3141</v>
       </c>
@@ -21823,7 +21839,7 @@
         <v>3141</v>
       </c>
     </row>
-    <row r="910" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="910" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A910" t="s">
         <v>3148</v>
       </c>
@@ -21831,7 +21847,7 @@
         <v>3148</v>
       </c>
     </row>
-    <row r="911" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="911" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A911" t="s">
         <v>3144</v>
       </c>
@@ -21839,7 +21855,7 @@
         <v>3144</v>
       </c>
     </row>
-    <row r="912" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="912" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A912" t="s">
         <v>3150</v>
       </c>
@@ -21847,7 +21863,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="913" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="913" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A913" t="s">
         <v>3140</v>
       </c>
@@ -21855,7 +21871,7 @@
         <v>3140</v>
       </c>
     </row>
-    <row r="914" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="914" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A914" t="s">
         <v>3145</v>
       </c>
@@ -21863,7 +21879,7 @@
         <v>3145</v>
       </c>
     </row>
-    <row r="915" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="915" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A915" t="s">
         <v>3190</v>
       </c>
@@ -21871,7 +21887,7 @@
         <v>3190</v>
       </c>
     </row>
-    <row r="916" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="916" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A916" t="s">
         <v>3197</v>
       </c>
@@ -21879,7 +21895,7 @@
         <v>3197</v>
       </c>
     </row>
-    <row r="917" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="917" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A917" t="s">
         <v>3199</v>
       </c>
@@ -21887,7 +21903,7 @@
         <v>3199</v>
       </c>
     </row>
-    <row r="918" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="918" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A918" t="s">
         <v>3191</v>
       </c>
@@ -21895,7 +21911,7 @@
         <v>3191</v>
       </c>
     </row>
-    <row r="919" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="919" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A919" t="s">
         <v>3195</v>
       </c>
@@ -21903,7 +21919,7 @@
         <v>3195</v>
       </c>
     </row>
-    <row r="920" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="920" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A920" t="s">
         <v>3194</v>
       </c>
@@ -21911,7 +21927,7 @@
         <v>3194</v>
       </c>
     </row>
-    <row r="921" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="921" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A921" t="s">
         <v>3189</v>
       </c>
@@ -21919,7 +21935,7 @@
         <v>3189</v>
       </c>
     </row>
-    <row r="922" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="922" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A922" t="s">
         <v>3196</v>
       </c>
@@ -21927,7 +21943,7 @@
         <v>3196</v>
       </c>
     </row>
-    <row r="923" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="923" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A923" t="s">
         <v>3192</v>
       </c>
@@ -21935,7 +21951,7 @@
         <v>3192</v>
       </c>
     </row>
-    <row r="924" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="924" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A924" t="s">
         <v>3198</v>
       </c>
@@ -21943,7 +21959,7 @@
         <v>3198</v>
       </c>
     </row>
-    <row r="925" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="925" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A925" t="s">
         <v>3188</v>
       </c>
@@ -21951,7 +21967,7 @@
         <v>3188</v>
       </c>
     </row>
-    <row r="926" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="926" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A926" t="s">
         <v>3193</v>
       </c>
@@ -33539,15 +33555,15 @@
         <v>2118</v>
       </c>
     </row>
-    <row r="2367" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2367" t="s">
+    <row r="2367" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2367" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B2367" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2368" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4582</v>
+      </c>
+    </row>
+    <row r="2368" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2368" t="s">
         <v>143</v>
       </c>
@@ -33555,7 +33571,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2369" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2369" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2369" t="s">
         <v>144</v>
       </c>
@@ -33563,15 +33579,15 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2370" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2370" t="s">
+    <row r="2370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2370" s="4" t="s">
         <v>145</v>
       </c>
       <c r="B2370" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2371" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2371" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2371" t="s">
         <v>146</v>
       </c>
@@ -33579,7 +33595,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="2372" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2372" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2372" t="s">
         <v>147</v>
       </c>
@@ -33587,7 +33603,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2373" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2373" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2373" t="s">
         <v>1386</v>
       </c>
@@ -33595,15 +33611,15 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="2374" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2374" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2374" t="s">
         <v>119</v>
       </c>
       <c r="B2374" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2375" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="2375" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2375" t="s">
         <v>120</v>
       </c>
@@ -33611,7 +33627,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2376" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2376" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2376" t="s">
         <v>1233</v>
       </c>
@@ -33619,7 +33635,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="2377" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2377" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2377" t="s">
         <v>121</v>
       </c>
@@ -33627,7 +33643,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2378" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2378" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2378" t="s">
         <v>163</v>
       </c>
@@ -33635,7 +33651,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2379" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2379" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2379" t="s">
         <v>164</v>
       </c>
@@ -33643,7 +33659,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2380" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2380" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2380" t="s">
         <v>1118</v>
       </c>
@@ -33651,7 +33667,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="2381" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2381" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2381" t="s">
         <v>165</v>
       </c>
@@ -33659,15 +33675,15 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2382" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2382" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2382" t="s">
         <v>139</v>
       </c>
       <c r="B2382" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2383" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="2383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2383" t="s">
         <v>140</v>
       </c>
@@ -33675,7 +33691,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="2384" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2384" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2384" t="s">
         <v>1383</v>
       </c>
@@ -33683,7 +33699,7 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="2385" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2385" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2385" t="s">
         <v>141</v>
       </c>
@@ -33691,15 +33707,15 @@
         <v>141</v>
       </c>
     </row>
-    <row r="2386" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2386" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2386" t="s">
         <v>131</v>
       </c>
       <c r="B2386" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2387" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="2387" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2387" t="s">
         <v>132</v>
       </c>
@@ -33707,7 +33723,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2388" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2388" t="s">
         <v>1381</v>
       </c>
@@ -33715,7 +33731,7 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="2389" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2389" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2389" t="s">
         <v>133</v>
       </c>
@@ -33723,7 +33739,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2390" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2390" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2390" t="s">
         <v>154</v>
       </c>
@@ -33731,7 +33747,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="2391" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2391" t="s">
         <v>155</v>
       </c>
@@ -33739,7 +33755,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2392" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2392" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2392" t="s">
         <v>1115</v>
       </c>
@@ -33747,7 +33763,7 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="2393" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2393" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2393" t="s">
         <v>156</v>
       </c>
@@ -33755,7 +33771,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="2394" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2394" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2394" t="s">
         <v>148</v>
       </c>
@@ -33763,7 +33779,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="2395" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2395" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2395" t="s">
         <v>1384</v>
       </c>
@@ -33771,7 +33787,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="2396" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2396" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2396" t="s">
         <v>149</v>
       </c>
@@ -33779,7 +33795,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2397" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2397" t="s">
         <v>1387</v>
       </c>
@@ -33787,7 +33803,7 @@
         <v>1387</v>
       </c>
     </row>
-    <row r="2398" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2398" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2398" t="s">
         <v>150</v>
       </c>
@@ -33795,7 +33811,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2399" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2399" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2399" t="s">
         <v>151</v>
       </c>
@@ -33803,7 +33819,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="2400" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2400" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2400" t="s">
         <v>152</v>
       </c>
@@ -33811,7 +33827,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="2401" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2401" t="s">
         <v>1114</v>
       </c>
@@ -33819,7 +33835,7 @@
         <v>1114</v>
       </c>
     </row>
-    <row r="2402" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2402" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2402" t="s">
         <v>153</v>
       </c>
@@ -33827,15 +33843,15 @@
         <v>153</v>
       </c>
     </row>
-    <row r="2403" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2403" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2403" t="s">
         <v>123</v>
       </c>
       <c r="B2403" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="2404" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="2404" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2404" t="s">
         <v>124</v>
       </c>
@@ -33843,7 +33859,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2405" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2405" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2405" t="s">
         <v>1234</v>
       </c>
@@ -33851,7 +33867,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="2406" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2406" t="s">
         <v>125</v>
       </c>
@@ -33859,7 +33875,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2407" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2407" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2407" t="s">
         <v>160</v>
       </c>
@@ -33867,7 +33883,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2408" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2408" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2408" t="s">
         <v>161</v>
       </c>
@@ -33875,7 +33891,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2409" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2409" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2409" t="s">
         <v>1117</v>
       </c>
@@ -33883,7 +33899,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="2410" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2410" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2410" t="s">
         <v>162</v>
       </c>
@@ -33891,7 +33907,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="2411" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2411" t="s">
         <v>157</v>
       </c>
@@ -33899,7 +33915,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2412" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2412" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2412" t="s">
         <v>158</v>
       </c>
@@ -33907,7 +33923,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2413" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2413" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2413" t="s">
         <v>1116</v>
       </c>
@@ -33915,7 +33931,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="2414" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2414" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2414" t="s">
         <v>159</v>
       </c>
@@ -33923,23 +33939,23 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2415" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2415" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2415" t="s">
         <v>127</v>
       </c>
       <c r="B2415" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2416" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="2416" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2416" t="s">
         <v>135</v>
       </c>
       <c r="B2416" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2417" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="2417" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2417" t="s">
         <v>128</v>
       </c>
@@ -33947,7 +33963,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="2418" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2418" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2418" t="s">
         <v>136</v>
       </c>
@@ -33955,7 +33971,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2419" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2419" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2419" t="s">
         <v>1235</v>
       </c>
@@ -33963,7 +33979,7 @@
         <v>1235</v>
       </c>
     </row>
-    <row r="2420" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2420" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2420" t="s">
         <v>1382</v>
       </c>
@@ -33971,7 +33987,7 @@
         <v>1382</v>
       </c>
     </row>
-    <row r="2421" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2421" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2421" t="s">
         <v>129</v>
       </c>
@@ -33979,7 +33995,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2422" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2422" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2422" t="s">
         <v>137</v>
       </c>
@@ -33987,15 +34003,15 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2423" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2423" t="s">
         <v>2369</v>
       </c>
       <c r="B2423" t="s">
-        <v>2369</v>
-      </c>
-    </row>
-    <row r="2424" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="2424" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2424" t="s">
         <v>2376</v>
       </c>
@@ -34003,23 +34019,23 @@
         <v>2376</v>
       </c>
     </row>
-    <row r="2425" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2425" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2425" t="s">
         <v>2378</v>
       </c>
       <c r="B2425" t="s">
-        <v>2378</v>
-      </c>
-    </row>
-    <row r="2426" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="2426" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2426" t="s">
         <v>2370</v>
       </c>
       <c r="B2426" t="s">
-        <v>2370</v>
-      </c>
-    </row>
-    <row r="2427" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="2427" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2427" t="s">
         <v>2374</v>
       </c>
@@ -34027,7 +34043,7 @@
         <v>2374</v>
       </c>
     </row>
-    <row r="2428" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2428" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2428" t="s">
         <v>2373</v>
       </c>
@@ -34035,7 +34051,7 @@
         <v>2373</v>
       </c>
     </row>
-    <row r="2429" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2429" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2429" t="s">
         <v>2368</v>
       </c>
@@ -34043,15 +34059,15 @@
         <v>2368</v>
       </c>
     </row>
-    <row r="2430" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2430" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2430" t="s">
         <v>2375</v>
       </c>
       <c r="B2430" t="s">
-        <v>2375</v>
-      </c>
-    </row>
-    <row r="2431" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="2431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2431" t="s">
         <v>2371</v>
       </c>
@@ -34059,7 +34075,7 @@
         <v>2371</v>
       </c>
     </row>
-    <row r="2432" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2432" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2432" t="s">
         <v>2377</v>
       </c>
@@ -34067,23 +34083,23 @@
         <v>2377</v>
       </c>
     </row>
-    <row r="2433" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2433" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2433" t="s">
         <v>2367</v>
       </c>
       <c r="B2433" t="s">
-        <v>2367</v>
-      </c>
-    </row>
-    <row r="2434" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="2434" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2434" t="s">
         <v>2372</v>
       </c>
       <c r="B2434" t="s">
-        <v>2372</v>
-      </c>
-    </row>
-    <row r="2435" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="2435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2435" t="s">
         <v>3082</v>
       </c>
@@ -34091,7 +34107,7 @@
         <v>3082</v>
       </c>
     </row>
-    <row r="2436" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2436" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2436" t="s">
         <v>3089</v>
       </c>
@@ -34099,7 +34115,7 @@
         <v>3089</v>
       </c>
     </row>
-    <row r="2437" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2437" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2437" t="s">
         <v>3091</v>
       </c>
@@ -34107,7 +34123,7 @@
         <v>3091</v>
       </c>
     </row>
-    <row r="2438" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2438" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2438" t="s">
         <v>3083</v>
       </c>
@@ -34115,7 +34131,7 @@
         <v>3083</v>
       </c>
     </row>
-    <row r="2439" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2439" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2439" t="s">
         <v>3087</v>
       </c>
@@ -34123,7 +34139,7 @@
         <v>3087</v>
       </c>
     </row>
-    <row r="2440" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2440" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2440" t="s">
         <v>3086</v>
       </c>
@@ -34131,7 +34147,7 @@
         <v>3086</v>
       </c>
     </row>
-    <row r="2441" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2441" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2441" t="s">
         <v>3081</v>
       </c>
@@ -34139,7 +34155,7 @@
         <v>3081</v>
       </c>
     </row>
-    <row r="2442" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2442" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2442" t="s">
         <v>3088</v>
       </c>
@@ -34147,7 +34163,7 @@
         <v>3088</v>
       </c>
     </row>
-    <row r="2443" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2443" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2443" t="s">
         <v>3084</v>
       </c>
@@ -34155,7 +34171,7 @@
         <v>3084</v>
       </c>
     </row>
-    <row r="2444" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2444" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2444" t="s">
         <v>3090</v>
       </c>
@@ -34163,7 +34179,7 @@
         <v>3090</v>
       </c>
     </row>
-    <row r="2445" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2445" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2445" t="s">
         <v>3080</v>
       </c>
@@ -34171,7 +34187,7 @@
         <v>3080</v>
       </c>
     </row>
-    <row r="2446" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2446" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2446" t="s">
         <v>3085</v>
       </c>
@@ -34179,7 +34195,7 @@
         <v>3085</v>
       </c>
     </row>
-    <row r="2447" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2447" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2447" t="s">
         <v>3035</v>
       </c>
@@ -34187,7 +34203,7 @@
         <v>3035</v>
       </c>
     </row>
-    <row r="2448" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2448" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2448" t="s">
         <v>3042</v>
       </c>
@@ -34195,7 +34211,7 @@
         <v>3042</v>
       </c>
     </row>
-    <row r="2449" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2449" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2449" t="s">
         <v>3044</v>
       </c>
@@ -34203,7 +34219,7 @@
         <v>3044</v>
       </c>
     </row>
-    <row r="2450" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2450" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2450" t="s">
         <v>3036</v>
       </c>
@@ -34211,7 +34227,7 @@
         <v>3036</v>
       </c>
     </row>
-    <row r="2451" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2451" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2451" t="s">
         <v>3040</v>
       </c>
@@ -34219,7 +34235,7 @@
         <v>3040</v>
       </c>
     </row>
-    <row r="2452" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2452" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2452" t="s">
         <v>3039</v>
       </c>
@@ -34227,7 +34243,7 @@
         <v>3039</v>
       </c>
     </row>
-    <row r="2453" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2453" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2453" t="s">
         <v>3034</v>
       </c>
@@ -34235,7 +34251,7 @@
         <v>3034</v>
       </c>
     </row>
-    <row r="2454" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2454" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2454" t="s">
         <v>3041</v>
       </c>
@@ -34243,7 +34259,7 @@
         <v>3041</v>
       </c>
     </row>
-    <row r="2455" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2455" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2455" t="s">
         <v>3037</v>
       </c>
@@ -34251,7 +34267,7 @@
         <v>3037</v>
       </c>
     </row>
-    <row r="2456" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2456" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2456" t="s">
         <v>3043</v>
       </c>
@@ -34259,7 +34275,7 @@
         <v>3043</v>
       </c>
     </row>
-    <row r="2457" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2457" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2457" t="s">
         <v>3033</v>
       </c>
@@ -34267,7 +34283,7 @@
         <v>3033</v>
       </c>
     </row>
-    <row r="2458" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2458" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2458" t="s">
         <v>3038</v>
       </c>
@@ -34275,7 +34291,7 @@
         <v>3038</v>
       </c>
     </row>
-    <row r="2459" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2459" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2459" t="s">
         <v>3130</v>
       </c>
@@ -34283,7 +34299,7 @@
         <v>3130</v>
       </c>
     </row>
-    <row r="2460" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2460" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2460" t="s">
         <v>3137</v>
       </c>
@@ -34291,7 +34307,7 @@
         <v>3137</v>
       </c>
     </row>
-    <row r="2461" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2461" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2461" t="s">
         <v>3139</v>
       </c>
@@ -34299,7 +34315,7 @@
         <v>3139</v>
       </c>
     </row>
-    <row r="2462" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2462" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2462" t="s">
         <v>3131</v>
       </c>
@@ -34307,7 +34323,7 @@
         <v>3131</v>
       </c>
     </row>
-    <row r="2463" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2463" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2463" t="s">
         <v>3135</v>
       </c>
@@ -34315,7 +34331,7 @@
         <v>3135</v>
       </c>
     </row>
-    <row r="2464" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2464" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2464" t="s">
         <v>3134</v>
       </c>
@@ -34323,7 +34339,7 @@
         <v>3134</v>
       </c>
     </row>
-    <row r="2465" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2465" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2465" t="s">
         <v>3129</v>
       </c>
@@ -34331,7 +34347,7 @@
         <v>3129</v>
       </c>
     </row>
-    <row r="2466" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2466" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2466" t="s">
         <v>3136</v>
       </c>
@@ -34339,7 +34355,7 @@
         <v>3136</v>
       </c>
     </row>
-    <row r="2467" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2467" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2467" t="s">
         <v>3132</v>
       </c>
@@ -34347,7 +34363,7 @@
         <v>3132</v>
       </c>
     </row>
-    <row r="2468" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2468" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2468" t="s">
         <v>3138</v>
       </c>
@@ -34355,7 +34371,7 @@
         <v>3138</v>
       </c>
     </row>
-    <row r="2469" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2469" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2469" t="s">
         <v>3128</v>
       </c>
@@ -34363,7 +34379,7 @@
         <v>3128</v>
       </c>
     </row>
-    <row r="2470" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2470" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2470" t="s">
         <v>3133</v>
       </c>
@@ -34371,7 +34387,7 @@
         <v>3133</v>
       </c>
     </row>
-    <row r="2471" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2471" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2471" t="s">
         <v>3059</v>
       </c>
@@ -34379,7 +34395,7 @@
         <v>3059</v>
       </c>
     </row>
-    <row r="2472" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2472" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2472" t="s">
         <v>3065</v>
       </c>
@@ -34387,7 +34403,7 @@
         <v>3065</v>
       </c>
     </row>
-    <row r="2473" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2473" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2473" t="s">
         <v>3067</v>
       </c>
@@ -34395,7 +34411,7 @@
         <v>3067</v>
       </c>
     </row>
-    <row r="2474" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2474" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2474" t="s">
         <v>3060</v>
       </c>
@@ -34403,7 +34419,7 @@
         <v>3060</v>
       </c>
     </row>
-    <row r="2475" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2475" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2475" t="s">
         <v>3063</v>
       </c>
@@ -34411,7 +34427,7 @@
         <v>3063</v>
       </c>
     </row>
-    <row r="2476" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2476" t="s">
         <v>1632</v>
       </c>
@@ -34419,7 +34435,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="2477" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2477" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2477" t="s">
         <v>3058</v>
       </c>
@@ -34427,7 +34443,7 @@
         <v>3058</v>
       </c>
     </row>
-    <row r="2478" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2478" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2478" t="s">
         <v>3064</v>
       </c>
@@ -34435,7 +34451,7 @@
         <v>3064</v>
       </c>
     </row>
-    <row r="2479" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2479" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2479" t="s">
         <v>3061</v>
       </c>
@@ -34443,7 +34459,7 @@
         <v>3061</v>
       </c>
     </row>
-    <row r="2480" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2480" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2480" t="s">
         <v>3066</v>
       </c>
@@ -34451,7 +34467,7 @@
         <v>3066</v>
       </c>
     </row>
-    <row r="2481" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2481" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2481" t="s">
         <v>3057</v>
       </c>
@@ -34459,7 +34475,7 @@
         <v>3057</v>
       </c>
     </row>
-    <row r="2482" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2482" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2482" t="s">
         <v>3062</v>
       </c>
@@ -34467,7 +34483,7 @@
         <v>3062</v>
       </c>
     </row>
-    <row r="2483" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2483" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2483" t="s">
         <v>3070</v>
       </c>
@@ -34475,7 +34491,7 @@
         <v>3070</v>
       </c>
     </row>
-    <row r="2484" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2484" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2484" t="s">
         <v>3077</v>
       </c>
@@ -34483,7 +34499,7 @@
         <v>3077</v>
       </c>
     </row>
-    <row r="2485" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2485" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2485" t="s">
         <v>3079</v>
       </c>
@@ -34491,7 +34507,7 @@
         <v>3079</v>
       </c>
     </row>
-    <row r="2486" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2486" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2486" t="s">
         <v>3071</v>
       </c>
@@ -34499,7 +34515,7 @@
         <v>3071</v>
       </c>
     </row>
-    <row r="2487" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2487" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2487" t="s">
         <v>3075</v>
       </c>
@@ -34507,7 +34523,7 @@
         <v>3075</v>
       </c>
     </row>
-    <row r="2488" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2488" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2488" t="s">
         <v>3074</v>
       </c>
@@ -34515,7 +34531,7 @@
         <v>3074</v>
       </c>
     </row>
-    <row r="2489" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2489" t="s">
         <v>3069</v>
       </c>
@@ -34523,7 +34539,7 @@
         <v>3069</v>
       </c>
     </row>
-    <row r="2490" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2490" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2490" t="s">
         <v>3076</v>
       </c>
@@ -34531,7 +34547,7 @@
         <v>3076</v>
       </c>
     </row>
-    <row r="2491" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2491" t="s">
         <v>3072</v>
       </c>
@@ -34539,7 +34555,7 @@
         <v>3072</v>
       </c>
     </row>
-    <row r="2492" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2492" t="s">
         <v>3078</v>
       </c>
@@ -34547,7 +34563,7 @@
         <v>3078</v>
       </c>
     </row>
-    <row r="2493" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2493" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2493" t="s">
         <v>3068</v>
       </c>
@@ -34555,7 +34571,7 @@
         <v>3068</v>
       </c>
     </row>
-    <row r="2494" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2494" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2494" t="s">
         <v>3073</v>
       </c>
@@ -34563,7 +34579,7 @@
         <v>3073</v>
       </c>
     </row>
-    <row r="2495" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2495" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2495" t="s">
         <v>3118</v>
       </c>
@@ -34571,7 +34587,7 @@
         <v>3118</v>
       </c>
     </row>
-    <row r="2496" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2496" t="s">
         <v>3125</v>
       </c>
@@ -34579,7 +34595,7 @@
         <v>3125</v>
       </c>
     </row>
-    <row r="2497" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2497" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2497" t="s">
         <v>3127</v>
       </c>
@@ -34587,7 +34603,7 @@
         <v>3127</v>
       </c>
     </row>
-    <row r="2498" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2498" t="s">
         <v>3119</v>
       </c>
@@ -34595,7 +34611,7 @@
         <v>3119</v>
       </c>
     </row>
-    <row r="2499" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2499" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2499" t="s">
         <v>3123</v>
       </c>
@@ -34603,7 +34619,7 @@
         <v>3123</v>
       </c>
     </row>
-    <row r="2500" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2500" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2500" t="s">
         <v>3122</v>
       </c>
@@ -34611,7 +34627,7 @@
         <v>3122</v>
       </c>
     </row>
-    <row r="2501" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2501" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2501" t="s">
         <v>3117</v>
       </c>
@@ -34619,7 +34635,7 @@
         <v>3117</v>
       </c>
     </row>
-    <row r="2502" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2502" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2502" t="s">
         <v>3124</v>
       </c>
@@ -34627,7 +34643,7 @@
         <v>3124</v>
       </c>
     </row>
-    <row r="2503" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2503" t="s">
         <v>3120</v>
       </c>
@@ -34635,7 +34651,7 @@
         <v>3120</v>
       </c>
     </row>
-    <row r="2504" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2504" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2504" t="s">
         <v>3126</v>
       </c>
@@ -34643,7 +34659,7 @@
         <v>3126</v>
       </c>
     </row>
-    <row r="2505" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2505" t="s">
         <v>3116</v>
       </c>
@@ -34651,7 +34667,7 @@
         <v>3116</v>
       </c>
     </row>
-    <row r="2506" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2506" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2506" t="s">
         <v>3121</v>
       </c>
@@ -34659,7 +34675,7 @@
         <v>3121</v>
       </c>
     </row>
-    <row r="2507" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2507" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2507" t="s">
         <v>3106</v>
       </c>
@@ -34667,7 +34683,7 @@
         <v>3106</v>
       </c>
     </row>
-    <row r="2508" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2508" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2508" t="s">
         <v>3113</v>
       </c>
@@ -34675,7 +34691,7 @@
         <v>3113</v>
       </c>
     </row>
-    <row r="2509" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2509" t="s">
         <v>3115</v>
       </c>
@@ -34683,7 +34699,7 @@
         <v>3115</v>
       </c>
     </row>
-    <row r="2510" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2510" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2510" t="s">
         <v>3107</v>
       </c>
@@ -34691,7 +34707,7 @@
         <v>3107</v>
       </c>
     </row>
-    <row r="2511" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2511" t="s">
         <v>3111</v>
       </c>
@@ -34699,7 +34715,7 @@
         <v>3111</v>
       </c>
     </row>
-    <row r="2512" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2512" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2512" t="s">
         <v>3110</v>
       </c>
@@ -34707,7 +34723,7 @@
         <v>3110</v>
       </c>
     </row>
-    <row r="2513" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2513" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2513" t="s">
         <v>3105</v>
       </c>
@@ -34715,7 +34731,7 @@
         <v>3105</v>
       </c>
     </row>
-    <row r="2514" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2514" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2514" t="s">
         <v>3112</v>
       </c>
@@ -34723,7 +34739,7 @@
         <v>3112</v>
       </c>
     </row>
-    <row r="2515" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2515" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2515" t="s">
         <v>3108</v>
       </c>
@@ -34731,7 +34747,7 @@
         <v>3108</v>
       </c>
     </row>
-    <row r="2516" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2516" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2516" t="s">
         <v>3114</v>
       </c>
@@ -34739,7 +34755,7 @@
         <v>3114</v>
       </c>
     </row>
-    <row r="2517" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2517" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2517" t="s">
         <v>3104</v>
       </c>
@@ -34747,7 +34763,7 @@
         <v>3104</v>
       </c>
     </row>
-    <row r="2518" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2518" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2518" t="s">
         <v>3109</v>
       </c>
@@ -34755,7 +34771,7 @@
         <v>3109</v>
       </c>
     </row>
-    <row r="2519" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2519" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2519" t="s">
         <v>3047</v>
       </c>
@@ -34763,7 +34779,7 @@
         <v>3047</v>
       </c>
     </row>
-    <row r="2520" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2520" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2520" t="s">
         <v>3054</v>
       </c>
@@ -34771,7 +34787,7 @@
         <v>3054</v>
       </c>
     </row>
-    <row r="2521" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2521" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2521" t="s">
         <v>3056</v>
       </c>
@@ -34779,7 +34795,7 @@
         <v>3056</v>
       </c>
     </row>
-    <row r="2522" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2522" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2522" t="s">
         <v>3048</v>
       </c>
@@ -34787,7 +34803,7 @@
         <v>3048</v>
       </c>
     </row>
-    <row r="2523" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2523" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2523" t="s">
         <v>3052</v>
       </c>
@@ -34795,7 +34811,7 @@
         <v>3052</v>
       </c>
     </row>
-    <row r="2524" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2524" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2524" t="s">
         <v>3051</v>
       </c>
@@ -34803,7 +34819,7 @@
         <v>3051</v>
       </c>
     </row>
-    <row r="2525" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2525" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2525" t="s">
         <v>3046</v>
       </c>
@@ -34811,7 +34827,7 @@
         <v>3046</v>
       </c>
     </row>
-    <row r="2526" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2526" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2526" t="s">
         <v>3053</v>
       </c>
@@ -34819,7 +34835,7 @@
         <v>3053</v>
       </c>
     </row>
-    <row r="2527" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2527" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2527" t="s">
         <v>3049</v>
       </c>
@@ -34827,7 +34843,7 @@
         <v>3049</v>
       </c>
     </row>
-    <row r="2528" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2528" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2528" t="s">
         <v>3055</v>
       </c>
@@ -34835,7 +34851,7 @@
         <v>3055</v>
       </c>
     </row>
-    <row r="2529" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2529" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2529" t="s">
         <v>3045</v>
       </c>
@@ -34843,7 +34859,7 @@
         <v>3045</v>
       </c>
     </row>
-    <row r="2530" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2530" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2530" t="s">
         <v>3050</v>
       </c>
@@ -34851,7 +34867,7 @@
         <v>3050</v>
       </c>
     </row>
-    <row r="2531" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2531" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2531" t="s">
         <v>3094</v>
       </c>
@@ -34859,7 +34875,7 @@
         <v>3094</v>
       </c>
     </row>
-    <row r="2532" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2532" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2532" t="s">
         <v>3101</v>
       </c>
@@ -34867,7 +34883,7 @@
         <v>3101</v>
       </c>
     </row>
-    <row r="2533" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2533" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2533" t="s">
         <v>3103</v>
       </c>
@@ -34875,7 +34891,7 @@
         <v>3103</v>
       </c>
     </row>
-    <row r="2534" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2534" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2534" t="s">
         <v>3095</v>
       </c>
@@ -34883,7 +34899,7 @@
         <v>3095</v>
       </c>
     </row>
-    <row r="2535" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2535" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2535" t="s">
         <v>3099</v>
       </c>
@@ -34891,7 +34907,7 @@
         <v>3099</v>
       </c>
     </row>
-    <row r="2536" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2536" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2536" t="s">
         <v>3098</v>
       </c>
@@ -34899,7 +34915,7 @@
         <v>3098</v>
       </c>
     </row>
-    <row r="2537" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2537" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2537" t="s">
         <v>3093</v>
       </c>
@@ -34907,7 +34923,7 @@
         <v>3093</v>
       </c>
     </row>
-    <row r="2538" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2538" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2538" t="s">
         <v>3100</v>
       </c>
@@ -34915,7 +34931,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="2539" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2539" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2539" t="s">
         <v>3096</v>
       </c>
@@ -34923,7 +34939,7 @@
         <v>3096</v>
       </c>
     </row>
-    <row r="2540" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2540" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2540" t="s">
         <v>3102</v>
       </c>
@@ -34931,7 +34947,7 @@
         <v>3102</v>
       </c>
     </row>
-    <row r="2541" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2541" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2541" t="s">
         <v>3092</v>
       </c>
@@ -34939,7 +34955,7 @@
         <v>3092</v>
       </c>
     </row>
-    <row r="2542" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2542" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2542" t="s">
         <v>3097</v>
       </c>
@@ -49058,7 +49074,7 @@
         <v>4286</v>
       </c>
     </row>
-    <row r="4291" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4291" t="s">
         <v>4287</v>
       </c>
@@ -49066,7 +49082,7 @@
         <v>4287</v>
       </c>
     </row>
-    <row r="4292" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4292" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4292" t="s">
         <v>4288</v>
       </c>
@@ -49507,7 +49523,7 @@
         <v>4342</v>
       </c>
     </row>
-    <row r="4348" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4348" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4348" t="s">
         <v>4343</v>
       </c>
@@ -49515,7 +49531,7 @@
         <v>4343</v>
       </c>
     </row>
-    <row r="4349" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4349" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4349" t="s">
         <v>4344</v>
       </c>
@@ -49523,7 +49539,7 @@
         <v>4344</v>
       </c>
     </row>
-    <row r="4350" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4350" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4350" t="s">
         <v>4345</v>
       </c>
@@ -49531,7 +49547,7 @@
         <v>4345</v>
       </c>
     </row>
-    <row r="4351" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4351" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4351" t="s">
         <v>4346</v>
       </c>
@@ -49539,7 +49555,7 @@
         <v>4346</v>
       </c>
     </row>
-    <row r="4352" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4352" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4352" t="s">
         <v>4347</v>
       </c>
@@ -49547,7 +49563,7 @@
         <v>4347</v>
       </c>
     </row>
-    <row r="4353" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4353" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4353" t="s">
         <v>4348</v>
       </c>
@@ -49555,7 +49571,7 @@
         <v>4348</v>
       </c>
     </row>
-    <row r="4354" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4354" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4354" t="s">
         <v>4349</v>
       </c>
@@ -49563,7 +49579,7 @@
         <v>4349</v>
       </c>
     </row>
-    <row r="4355" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4355" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4355" t="s">
         <v>4350</v>
       </c>
@@ -49571,7 +49587,7 @@
         <v>4350</v>
       </c>
     </row>
-    <row r="4356" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4356" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4356" t="s">
         <v>4351</v>
       </c>
@@ -49579,7 +49595,7 @@
         <v>4351</v>
       </c>
     </row>
-    <row r="4357" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4357" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4357" t="s">
         <v>4352</v>
       </c>
@@ -49587,7 +49603,7 @@
         <v>4352</v>
       </c>
     </row>
-    <row r="4358" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4358" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4358" t="s">
         <v>4353</v>
       </c>
@@ -49595,7 +49611,7 @@
         <v>4353</v>
       </c>
     </row>
-    <row r="4359" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4359" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4359" t="s">
         <v>4354</v>
       </c>
@@ -49603,7 +49619,7 @@
         <v>4354</v>
       </c>
     </row>
-    <row r="4360" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4360" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4360" t="s">
         <v>4355</v>
       </c>
@@ -49611,7 +49627,7 @@
         <v>4355</v>
       </c>
     </row>
-    <row r="4361" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4361" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4361" t="s">
         <v>4356</v>
       </c>
@@ -49619,7 +49635,7 @@
         <v>4356</v>
       </c>
     </row>
-    <row r="4362" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4362" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4362" t="s">
         <v>4357</v>
       </c>
@@ -49627,7 +49643,7 @@
         <v>4357</v>
       </c>
     </row>
-    <row r="4363" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4363" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4363" t="s">
         <v>4358</v>
       </c>
@@ -49635,7 +49651,7 @@
         <v>4358</v>
       </c>
     </row>
-    <row r="4364" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4364" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4364" t="s">
         <v>4359</v>
       </c>
@@ -50143,7 +50159,7 @@
   <autoFilter ref="A1:G4424" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
     <filterColumn colId="0">
       <customFilters>
-        <customFilter val="Liêm Trinh*"/>
+        <customFilter val="Thiên Đồng*"/>
       </customFilters>
     </filterColumn>
   </autoFilter>
@@ -50157,39 +50173,37 @@
   <conditionalFormatting sqref="A6716:A1048576 A2:A4170">
     <cfRule type="duplicateValues" dxfId="14" priority="21"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B814">
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="2"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B3281">
-    <cfRule type="duplicateValues" dxfId="13" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3285">
-    <cfRule type="duplicateValues" dxfId="11" priority="7"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3289">
-    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3293">
-    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4293:B4419 B4421:B1048576 B3265:B3266 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B3294:B4285 B815:B3263 B2:B813">
-    <cfRule type="duplicateValues" dxfId="5" priority="14"/>
+  <conditionalFormatting sqref="B4293:B4419 B4421:B1048576 B3265:B3266 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B3294:B4285 B2:B813 B815:B3263">
+    <cfRule type="duplicateValues" dxfId="3" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4420">
-    <cfRule type="duplicateValues" dxfId="4" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6716:B1048576 B4401:B4404 B3265:B3266 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B3294:B4170 B815:B3263 B2:B813">
-    <cfRule type="duplicateValues" dxfId="3" priority="15"/>
+  <conditionalFormatting sqref="B6716:B1048576 B4401:B4404 B3265:B3266 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B3294:B4170 B2:B813 B815:B3263">
+    <cfRule type="duplicateValues" dxfId="1" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3721">
-    <cfRule type="duplicateValues" dxfId="2" priority="22"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B814">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B814">
-    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="22"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Giải thích VŨ khúc
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35BC34B0-1FB8-43E4-B869-5DBBB5BCAD08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5009AE42-95C4-4C99-BBC2-007294074230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13944,9 +13944,6 @@
     <t>Vũ Khúc tọa thủ cung Mệnh ở Dần gặp cát tinh: Hóa Khoa, Hóa Lộc, Hóa Quyền, Tả Phù, Hữu Bật, Văn Xương, Văn Khúc, Thiên Khôi, Thiên Việt, Tử Vi, Thiên Phủ, Thiên Tướng, Tham Lang</t>
   </si>
   <si>
-    <t xml:space="preserve">Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ: </t>
-  </si>
-  <si>
     <t>Vũ Khúc tọa thủ cung Mệnh ở Hợi gặp các sao Hình Kỵ:</t>
   </si>
   <si>
@@ -13978,6 +13975,9 @@
   </si>
   <si>
     <t>Vũ Khúc tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ:</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ: Thiên Hình, Hoá Kỵ</t>
   </si>
 </sst>
 </file>
@@ -14500,7 +14500,7 @@
   <dimension ref="A2:G4460"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4428" workbookViewId="0">
-      <selection activeCell="F4450" sqref="F4450"/>
+      <selection activeCell="A4449" sqref="A4449"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50696,62 +50696,62 @@
     </row>
     <row r="4449" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4449" s="3" t="s">
-        <v>4638</v>
+        <v>4649</v>
       </c>
     </row>
     <row r="4450" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4450" s="3" t="s">
-        <v>4639</v>
+        <v>4638</v>
       </c>
     </row>
     <row r="4451" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4451" s="3" t="s">
-        <v>4640</v>
+        <v>4639</v>
       </c>
     </row>
     <row r="4452" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4452" s="3" t="s">
-        <v>4641</v>
+        <v>4640</v>
       </c>
     </row>
     <row r="4453" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4453" s="3" t="s">
-        <v>4642</v>
+        <v>4641</v>
       </c>
     </row>
     <row r="4454" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4454" s="3" t="s">
-        <v>4643</v>
+        <v>4642</v>
       </c>
     </row>
     <row r="4455" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4455" s="3" t="s">
-        <v>4644</v>
+        <v>4643</v>
       </c>
     </row>
     <row r="4456" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4456" s="3" t="s">
-        <v>4645</v>
+        <v>4644</v>
       </c>
     </row>
     <row r="4457" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4457" s="3" t="s">
-        <v>4646</v>
+        <v>4645</v>
       </c>
     </row>
     <row r="4458" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4458" s="3" t="s">
-        <v>4647</v>
+        <v>4646</v>
       </c>
     </row>
     <row r="4459" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4459" s="3" t="s">
-        <v>4648</v>
+        <v>4647</v>
       </c>
     </row>
     <row r="4460" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4460" s="3" t="s">
-        <v>4649</v>
+        <v>4648</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
giai thich thai duong toa menh
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DD34E78-D265-4348-A9B7-6A1735A7A5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FFCEAA-5547-41F9-A0C8-CC9473B6D5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$G$4531</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9241" uniqueCount="4786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9250" uniqueCount="4786">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -14485,7 +14484,157 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="41">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -15025,8 +15174,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A2:G4531"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1654" workbookViewId="0">
-      <selection activeCell="D1655" sqref="D1655"/>
+    <sheetView tabSelected="1" topLeftCell="A4520" workbookViewId="0">
+      <selection activeCell="B1684" sqref="B1684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16092,7 +16241,7 @@
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
     </row>
-    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>516</v>
       </c>
@@ -16125,7 +16274,7 @@
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
     </row>
-    <row r="96" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>517</v>
       </c>
@@ -16136,7 +16285,7 @@
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
     </row>
-    <row r="97" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>522</v>
       </c>
@@ -16213,7 +16362,7 @@
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
     </row>
-    <row r="104" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>520</v>
       </c>
@@ -16840,7 +16989,7 @@
       <c r="F160" s="3"/>
       <c r="G160" s="3"/>
     </row>
-    <row r="161" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>518</v>
       </c>
@@ -16851,7 +17000,7 @@
       <c r="F161" s="3"/>
       <c r="G161" s="3"/>
     </row>
-    <row r="162" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>523</v>
       </c>
@@ -16917,7 +17066,7 @@
       <c r="F167" s="3"/>
       <c r="G167" s="3"/>
     </row>
-    <row r="168" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>519</v>
       </c>
@@ -17368,7 +17517,7 @@
       <c r="F208" s="3"/>
       <c r="G208" s="3"/>
     </row>
-    <row r="209" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
         <v>521</v>
       </c>
@@ -18127,7 +18276,7 @@
       <c r="F277" s="3"/>
       <c r="G277" s="3"/>
     </row>
-    <row r="278" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A278" s="9" t="s">
         <v>1397</v>
       </c>
@@ -19713,7 +19862,7 @@
       <c r="F421" s="3"/>
       <c r="G421" s="3"/>
     </row>
-    <row r="422" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A422" s="3" t="s">
         <v>935</v>
       </c>
@@ -21407,7 +21556,7 @@
       <c r="F575" s="3"/>
       <c r="G575" s="3"/>
     </row>
-    <row r="576" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A576" s="3" t="s">
         <v>962</v>
       </c>
@@ -21418,7 +21567,7 @@
       <c r="F576" s="3"/>
       <c r="G576" s="3"/>
     </row>
-    <row r="577" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="577" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A577" s="3" t="s">
         <v>963</v>
       </c>
@@ -26381,7 +26530,7 @@
       <c r="F1022" s="3"/>
       <c r="G1022" s="3"/>
     </row>
-    <row r="1023" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1023" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1023" s="3" t="s">
         <v>754</v>
       </c>
@@ -26392,7 +26541,7 @@
       <c r="F1023" s="3"/>
       <c r="G1023" s="3"/>
     </row>
-    <row r="1024" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1024" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1024" s="3" t="s">
         <v>1519</v>
       </c>
@@ -33265,7 +33414,7 @@
       <c r="F1646" s="3"/>
       <c r="G1646" s="3"/>
     </row>
-    <row r="1647" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1647" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A1647" s="9" t="s">
         <v>1396</v>
       </c>
@@ -33278,7 +33427,7 @@
       <c r="F1647" s="3"/>
       <c r="G1647" s="3"/>
     </row>
-    <row r="1648" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1648" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1648" s="9" t="s">
         <v>1393</v>
       </c>
@@ -33289,7 +33438,7 @@
       <c r="F1648" s="3"/>
       <c r="G1648" s="3"/>
     </row>
-    <row r="1649" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1649" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1649" s="9" t="s">
         <v>1395</v>
       </c>
@@ -33300,7 +33449,7 @@
       <c r="F1649" s="3"/>
       <c r="G1649" s="3"/>
     </row>
-    <row r="1650" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1650" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1650" s="9" t="s">
         <v>4763</v>
       </c>
@@ -33313,7 +33462,7 @@
       <c r="F1650" s="3"/>
       <c r="G1650" s="3"/>
     </row>
-    <row r="1651" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1651" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1651" s="9" t="s">
         <v>1394</v>
       </c>
@@ -33324,7 +33473,7 @@
       <c r="F1651" s="3"/>
       <c r="G1651" s="3"/>
     </row>
-    <row r="1652" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1652" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1652" s="3" t="s">
         <v>1060</v>
       </c>
@@ -33335,7 +33484,7 @@
       <c r="F1652" s="3"/>
       <c r="G1652" s="3"/>
     </row>
-    <row r="1653" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1653" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1653" s="9" t="s">
         <v>1054</v>
       </c>
@@ -33552,6 +33701,9 @@
       <c r="A1673" s="3" t="s">
         <v>1399</v>
       </c>
+      <c r="B1673" s="3" t="s">
+        <v>1399</v>
+      </c>
       <c r="F1673" s="3"/>
       <c r="G1673" s="3"/>
     </row>
@@ -33659,6 +33811,9 @@
       <c r="A1684" s="3" t="s">
         <v>1398</v>
       </c>
+      <c r="B1684" s="3" t="s">
+        <v>1398</v>
+      </c>
       <c r="F1684" s="3"/>
       <c r="G1684" s="3"/>
     </row>
@@ -33845,6 +34000,9 @@
       <c r="A1702" s="3" t="s">
         <v>1052</v>
       </c>
+      <c r="B1702" s="3" t="s">
+        <v>1052</v>
+      </c>
       <c r="F1702" s="3"/>
       <c r="G1702" s="3"/>
     </row>
@@ -33908,8 +34066,8 @@
       <c r="F1708" s="3"/>
       <c r="G1708" s="3"/>
     </row>
-    <row r="1709" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1709" s="3" t="s">
+    <row r="1709" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1709" s="9" t="s">
         <v>2343</v>
       </c>
       <c r="B1709" s="3" t="s">
@@ -33919,30 +34077,34 @@
       <c r="F1709" s="3"/>
       <c r="G1709" s="3"/>
     </row>
-    <row r="1710" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1710" s="3" t="s">
+    <row r="1710" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A1710" s="9" t="s">
         <v>2350</v>
       </c>
       <c r="B1710" s="3" t="s">
-        <v>2350</v>
-      </c>
-      <c r="C1710" s="3"/>
+        <v>4627</v>
+      </c>
+      <c r="C1710" s="10" t="s">
+        <v>4628</v>
+      </c>
       <c r="F1710" s="3"/>
       <c r="G1710" s="3"/>
     </row>
-    <row r="1711" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1711" s="3" t="s">
+    <row r="1711" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A1711" s="9" t="s">
         <v>2352</v>
       </c>
       <c r="B1711" s="3" t="s">
-        <v>2352</v>
-      </c>
-      <c r="C1711" s="3"/>
+        <v>4627</v>
+      </c>
+      <c r="C1711" s="10" t="s">
+        <v>4628</v>
+      </c>
       <c r="F1711" s="3"/>
       <c r="G1711" s="3"/>
     </row>
-    <row r="1712" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1712" s="3" t="s">
+    <row r="1712" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1712" s="9" t="s">
         <v>2344</v>
       </c>
       <c r="B1712" s="3" t="s">
@@ -33952,8 +34114,8 @@
       <c r="F1712" s="3"/>
       <c r="G1712" s="3"/>
     </row>
-    <row r="1713" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1713" s="3" t="s">
+    <row r="1713" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1713" s="9" t="s">
         <v>2348</v>
       </c>
       <c r="B1713" s="3" t="s">
@@ -33963,8 +34125,8 @@
       <c r="F1713" s="3"/>
       <c r="G1713" s="3"/>
     </row>
-    <row r="1714" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1714" s="3" t="s">
+    <row r="1714" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1714" s="9" t="s">
         <v>2347</v>
       </c>
       <c r="B1714" s="3" t="s">
@@ -33974,30 +34136,34 @@
       <c r="F1714" s="3"/>
       <c r="G1714" s="3"/>
     </row>
-    <row r="1715" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1715" s="3" t="s">
+    <row r="1715" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A1715" s="9" t="s">
         <v>2342</v>
       </c>
       <c r="B1715" s="3" t="s">
-        <v>2342</v>
-      </c>
-      <c r="C1715" s="3"/>
+        <v>4627</v>
+      </c>
+      <c r="C1715" s="10" t="s">
+        <v>4628</v>
+      </c>
       <c r="F1715" s="3"/>
       <c r="G1715" s="3"/>
     </row>
-    <row r="1716" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1716" s="3" t="s">
+    <row r="1716" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A1716" s="9" t="s">
         <v>2349</v>
       </c>
       <c r="B1716" s="3" t="s">
-        <v>2349</v>
-      </c>
-      <c r="C1716" s="3"/>
+        <v>4627</v>
+      </c>
+      <c r="C1716" s="10" t="s">
+        <v>4628</v>
+      </c>
       <c r="F1716" s="3"/>
       <c r="G1716" s="3"/>
     </row>
-    <row r="1717" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1717" s="3" t="s">
+    <row r="1717" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1717" s="9" t="s">
         <v>2345</v>
       </c>
       <c r="B1717" s="3" t="s">
@@ -34007,30 +34173,34 @@
       <c r="F1717" s="3"/>
       <c r="G1717" s="3"/>
     </row>
-    <row r="1718" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1718" s="3" t="s">
+    <row r="1718" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A1718" s="9" t="s">
         <v>2351</v>
       </c>
       <c r="B1718" s="3" t="s">
-        <v>2351</v>
-      </c>
-      <c r="C1718" s="3"/>
+        <v>4627</v>
+      </c>
+      <c r="C1718" s="10" t="s">
+        <v>4628</v>
+      </c>
       <c r="F1718" s="3"/>
       <c r="G1718" s="3"/>
     </row>
-    <row r="1719" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1719" s="3" t="s">
+    <row r="1719" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A1719" s="9" t="s">
         <v>2341</v>
       </c>
       <c r="B1719" s="3" t="s">
-        <v>2341</v>
-      </c>
-      <c r="C1719" s="3"/>
+        <v>4627</v>
+      </c>
+      <c r="C1719" s="10" t="s">
+        <v>4628</v>
+      </c>
       <c r="F1719" s="3"/>
       <c r="G1719" s="3"/>
     </row>
-    <row r="1720" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1720" s="3" t="s">
+    <row r="1720" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1720" s="9" t="s">
         <v>2346</v>
       </c>
       <c r="B1720" s="3" t="s">
@@ -34040,7 +34210,7 @@
       <c r="F1720" s="3"/>
       <c r="G1720" s="3"/>
     </row>
-    <row r="1721" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1721" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1721" s="3" t="s">
         <v>2855</v>
       </c>
@@ -34051,7 +34221,7 @@
       <c r="F1721" s="3"/>
       <c r="G1721" s="3"/>
     </row>
-    <row r="1722" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1722" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1722" s="3" t="s">
         <v>2861</v>
       </c>
@@ -34062,7 +34232,7 @@
       <c r="F1722" s="3"/>
       <c r="G1722" s="3"/>
     </row>
-    <row r="1723" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1723" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1723" s="3" t="s">
         <v>2863</v>
       </c>
@@ -34073,7 +34243,7 @@
       <c r="F1723" s="3"/>
       <c r="G1723" s="3"/>
     </row>
-    <row r="1724" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1724" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1724" s="3" t="s">
         <v>2856</v>
       </c>
@@ -34084,7 +34254,7 @@
       <c r="F1724" s="3"/>
       <c r="G1724" s="3"/>
     </row>
-    <row r="1725" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1725" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1725" s="3" t="s">
         <v>2860</v>
       </c>
@@ -34095,7 +34265,7 @@
       <c r="F1725" s="3"/>
       <c r="G1725" s="3"/>
     </row>
-    <row r="1726" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1726" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1726" s="3" t="s">
         <v>2859</v>
       </c>
@@ -34106,7 +34276,7 @@
       <c r="F1726" s="3"/>
       <c r="G1726" s="3"/>
     </row>
-    <row r="1727" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1727" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1727" s="3" t="s">
         <v>2854</v>
       </c>
@@ -34117,7 +34287,7 @@
       <c r="F1727" s="3"/>
       <c r="G1727" s="3"/>
     </row>
-    <row r="1728" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1728" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1728" s="3" t="s">
         <v>1533</v>
       </c>
@@ -34128,7 +34298,7 @@
       <c r="F1728" s="3"/>
       <c r="G1728" s="3"/>
     </row>
-    <row r="1729" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1729" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1729" s="3" t="s">
         <v>2857</v>
       </c>
@@ -34139,7 +34309,7 @@
       <c r="F1729" s="3"/>
       <c r="G1729" s="3"/>
     </row>
-    <row r="1730" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1730" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1730" s="3" t="s">
         <v>2862</v>
       </c>
@@ -34150,7 +34320,7 @@
       <c r="F1730" s="3"/>
       <c r="G1730" s="3"/>
     </row>
-    <row r="1731" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1731" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1731" s="3" t="s">
         <v>2853</v>
       </c>
@@ -34161,7 +34331,7 @@
       <c r="F1731" s="3"/>
       <c r="G1731" s="3"/>
     </row>
-    <row r="1732" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1732" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1732" s="3" t="s">
         <v>2858</v>
       </c>
@@ -34172,7 +34342,7 @@
       <c r="F1732" s="3"/>
       <c r="G1732" s="3"/>
     </row>
-    <row r="1733" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1733" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1733" s="3" t="s">
         <v>2807</v>
       </c>
@@ -34183,7 +34353,7 @@
       <c r="F1733" s="3"/>
       <c r="G1733" s="3"/>
     </row>
-    <row r="1734" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1734" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1734" s="3" t="s">
         <v>2814</v>
       </c>
@@ -34194,7 +34364,7 @@
       <c r="F1734" s="3"/>
       <c r="G1734" s="3"/>
     </row>
-    <row r="1735" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1735" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1735" s="3" t="s">
         <v>2816</v>
       </c>
@@ -34205,7 +34375,7 @@
       <c r="F1735" s="3"/>
       <c r="G1735" s="3"/>
     </row>
-    <row r="1736" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1736" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1736" s="3" t="s">
         <v>2808</v>
       </c>
@@ -34216,7 +34386,7 @@
       <c r="F1736" s="3"/>
       <c r="G1736" s="3"/>
     </row>
-    <row r="1737" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1737" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1737" s="3" t="s">
         <v>2812</v>
       </c>
@@ -34227,7 +34397,7 @@
       <c r="F1737" s="3"/>
       <c r="G1737" s="3"/>
     </row>
-    <row r="1738" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1738" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1738" s="3" t="s">
         <v>2811</v>
       </c>
@@ -34238,7 +34408,7 @@
       <c r="F1738" s="3"/>
       <c r="G1738" s="3"/>
     </row>
-    <row r="1739" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1739" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1739" s="3" t="s">
         <v>2806</v>
       </c>
@@ -34249,7 +34419,7 @@
       <c r="F1739" s="3"/>
       <c r="G1739" s="3"/>
     </row>
-    <row r="1740" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1740" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1740" s="3" t="s">
         <v>2813</v>
       </c>
@@ -34260,7 +34430,7 @@
       <c r="F1740" s="3"/>
       <c r="G1740" s="3"/>
     </row>
-    <row r="1741" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1741" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1741" s="3" t="s">
         <v>2809</v>
       </c>
@@ -34271,7 +34441,7 @@
       <c r="F1741" s="3"/>
       <c r="G1741" s="3"/>
     </row>
-    <row r="1742" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1742" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1742" s="3" t="s">
         <v>2815</v>
       </c>
@@ -34282,7 +34452,7 @@
       <c r="F1742" s="3"/>
       <c r="G1742" s="3"/>
     </row>
-    <row r="1743" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1743" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1743" s="3" t="s">
         <v>2805</v>
       </c>
@@ -34293,7 +34463,7 @@
       <c r="F1743" s="3"/>
       <c r="G1743" s="3"/>
     </row>
-    <row r="1744" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1744" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1744" s="3" t="s">
         <v>2810</v>
       </c>
@@ -34304,7 +34474,7 @@
       <c r="F1744" s="3"/>
       <c r="G1744" s="3"/>
     </row>
-    <row r="1745" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1745" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1745" s="3" t="s">
         <v>2902</v>
       </c>
@@ -34315,7 +34485,7 @@
       <c r="F1745" s="3"/>
       <c r="G1745" s="3"/>
     </row>
-    <row r="1746" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1746" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1746" s="3" t="s">
         <v>2909</v>
       </c>
@@ -34326,7 +34496,7 @@
       <c r="F1746" s="3"/>
       <c r="G1746" s="3"/>
     </row>
-    <row r="1747" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1747" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1747" s="3" t="s">
         <v>2911</v>
       </c>
@@ -34337,7 +34507,7 @@
       <c r="F1747" s="3"/>
       <c r="G1747" s="3"/>
     </row>
-    <row r="1748" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1748" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1748" s="3" t="s">
         <v>2903</v>
       </c>
@@ -34348,7 +34518,7 @@
       <c r="F1748" s="3"/>
       <c r="G1748" s="3"/>
     </row>
-    <row r="1749" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1749" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1749" s="3" t="s">
         <v>2907</v>
       </c>
@@ -34359,7 +34529,7 @@
       <c r="F1749" s="3"/>
       <c r="G1749" s="3"/>
     </row>
-    <row r="1750" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1750" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1750" s="3" t="s">
         <v>2906</v>
       </c>
@@ -34370,7 +34540,7 @@
       <c r="F1750" s="3"/>
       <c r="G1750" s="3"/>
     </row>
-    <row r="1751" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1751" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1751" s="3" t="s">
         <v>2901</v>
       </c>
@@ -34381,7 +34551,7 @@
       <c r="F1751" s="3"/>
       <c r="G1751" s="3"/>
     </row>
-    <row r="1752" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1752" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1752" s="3" t="s">
         <v>2908</v>
       </c>
@@ -34392,7 +34562,7 @@
       <c r="F1752" s="3"/>
       <c r="G1752" s="3"/>
     </row>
-    <row r="1753" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1753" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1753" s="3" t="s">
         <v>2904</v>
       </c>
@@ -34403,7 +34573,7 @@
       <c r="F1753" s="3"/>
       <c r="G1753" s="3"/>
     </row>
-    <row r="1754" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1754" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1754" s="3" t="s">
         <v>2910</v>
       </c>
@@ -34414,7 +34584,7 @@
       <c r="F1754" s="3"/>
       <c r="G1754" s="3"/>
     </row>
-    <row r="1755" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1755" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1755" s="3" t="s">
         <v>2900</v>
       </c>
@@ -34425,7 +34595,7 @@
       <c r="F1755" s="3"/>
       <c r="G1755" s="3"/>
     </row>
-    <row r="1756" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1756" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1756" s="3" t="s">
         <v>2905</v>
       </c>
@@ -34436,7 +34606,7 @@
       <c r="F1756" s="3"/>
       <c r="G1756" s="3"/>
     </row>
-    <row r="1757" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1757" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1757" s="3" t="s">
         <v>2831</v>
       </c>
@@ -34447,7 +34617,7 @@
       <c r="F1757" s="3"/>
       <c r="G1757" s="3"/>
     </row>
-    <row r="1758" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1758" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1758" s="3" t="s">
         <v>2838</v>
       </c>
@@ -34458,7 +34628,7 @@
       <c r="F1758" s="3"/>
       <c r="G1758" s="3"/>
     </row>
-    <row r="1759" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1759" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1759" s="3" t="s">
         <v>2840</v>
       </c>
@@ -34469,7 +34639,7 @@
       <c r="F1759" s="3"/>
       <c r="G1759" s="3"/>
     </row>
-    <row r="1760" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1760" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1760" s="3" t="s">
         <v>2832</v>
       </c>
@@ -34480,7 +34650,7 @@
       <c r="F1760" s="3"/>
       <c r="G1760" s="3"/>
     </row>
-    <row r="1761" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1761" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1761" s="3" t="s">
         <v>2836</v>
       </c>
@@ -34491,7 +34661,7 @@
       <c r="F1761" s="3"/>
       <c r="G1761" s="3"/>
     </row>
-    <row r="1762" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1762" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1762" s="3" t="s">
         <v>2835</v>
       </c>
@@ -34502,7 +34672,7 @@
       <c r="F1762" s="3"/>
       <c r="G1762" s="3"/>
     </row>
-    <row r="1763" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1763" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1763" s="3" t="s">
         <v>2830</v>
       </c>
@@ -34513,7 +34683,7 @@
       <c r="F1763" s="3"/>
       <c r="G1763" s="3"/>
     </row>
-    <row r="1764" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1764" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1764" s="3" t="s">
         <v>2837</v>
       </c>
@@ -34524,7 +34694,7 @@
       <c r="F1764" s="3"/>
       <c r="G1764" s="3"/>
     </row>
-    <row r="1765" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1765" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1765" s="3" t="s">
         <v>2833</v>
       </c>
@@ -34535,7 +34705,7 @@
       <c r="F1765" s="3"/>
       <c r="G1765" s="3"/>
     </row>
-    <row r="1766" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1766" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1766" s="3" t="s">
         <v>2839</v>
       </c>
@@ -34546,7 +34716,7 @@
       <c r="F1766" s="3"/>
       <c r="G1766" s="3"/>
     </row>
-    <row r="1767" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1767" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1767" s="3" t="s">
         <v>2829</v>
       </c>
@@ -34557,7 +34727,7 @@
       <c r="F1767" s="3"/>
       <c r="G1767" s="3"/>
     </row>
-    <row r="1768" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1768" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1768" s="3" t="s">
         <v>2834</v>
       </c>
@@ -34568,7 +34738,7 @@
       <c r="F1768" s="3"/>
       <c r="G1768" s="3"/>
     </row>
-    <row r="1769" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1769" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1769" s="3" t="s">
         <v>2843</v>
       </c>
@@ -34579,7 +34749,7 @@
       <c r="F1769" s="3"/>
       <c r="G1769" s="3"/>
     </row>
-    <row r="1770" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1770" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1770" s="3" t="s">
         <v>2850</v>
       </c>
@@ -34590,7 +34760,7 @@
       <c r="F1770" s="3"/>
       <c r="G1770" s="3"/>
     </row>
-    <row r="1771" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1771" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1771" s="3" t="s">
         <v>2852</v>
       </c>
@@ -34601,7 +34771,7 @@
       <c r="F1771" s="3"/>
       <c r="G1771" s="3"/>
     </row>
-    <row r="1772" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1772" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1772" s="3" t="s">
         <v>2844</v>
       </c>
@@ -34612,7 +34782,7 @@
       <c r="F1772" s="3"/>
       <c r="G1772" s="3"/>
     </row>
-    <row r="1773" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1773" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1773" s="3" t="s">
         <v>2848</v>
       </c>
@@ -34623,7 +34793,7 @@
       <c r="F1773" s="3"/>
       <c r="G1773" s="3"/>
     </row>
-    <row r="1774" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1774" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1774" s="3" t="s">
         <v>2847</v>
       </c>
@@ -34634,7 +34804,7 @@
       <c r="F1774" s="3"/>
       <c r="G1774" s="3"/>
     </row>
-    <row r="1775" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1775" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1775" s="3" t="s">
         <v>2842</v>
       </c>
@@ -34645,7 +34815,7 @@
       <c r="F1775" s="3"/>
       <c r="G1775" s="3"/>
     </row>
-    <row r="1776" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1776" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1776" s="3" t="s">
         <v>2849</v>
       </c>
@@ -34656,7 +34826,7 @@
       <c r="F1776" s="3"/>
       <c r="G1776" s="3"/>
     </row>
-    <row r="1777" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1777" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1777" s="3" t="s">
         <v>2845</v>
       </c>
@@ -34667,7 +34837,7 @@
       <c r="F1777" s="3"/>
       <c r="G1777" s="3"/>
     </row>
-    <row r="1778" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1778" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1778" s="3" t="s">
         <v>2851</v>
       </c>
@@ -34678,7 +34848,7 @@
       <c r="F1778" s="3"/>
       <c r="G1778" s="3"/>
     </row>
-    <row r="1779" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1779" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1779" s="3" t="s">
         <v>2841</v>
       </c>
@@ -34689,7 +34859,7 @@
       <c r="F1779" s="3"/>
       <c r="G1779" s="3"/>
     </row>
-    <row r="1780" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1780" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1780" s="3" t="s">
         <v>2846</v>
       </c>
@@ -34700,7 +34870,7 @@
       <c r="F1780" s="3"/>
       <c r="G1780" s="3"/>
     </row>
-    <row r="1781" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1781" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1781" s="3" t="s">
         <v>2890</v>
       </c>
@@ -34711,7 +34881,7 @@
       <c r="F1781" s="3"/>
       <c r="G1781" s="3"/>
     </row>
-    <row r="1782" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1782" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1782" s="3" t="s">
         <v>2897</v>
       </c>
@@ -34722,7 +34892,7 @@
       <c r="F1782" s="3"/>
       <c r="G1782" s="3"/>
     </row>
-    <row r="1783" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1783" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1783" s="3" t="s">
         <v>2899</v>
       </c>
@@ -34733,7 +34903,7 @@
       <c r="F1783" s="3"/>
       <c r="G1783" s="3"/>
     </row>
-    <row r="1784" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1784" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1784" s="3" t="s">
         <v>2891</v>
       </c>
@@ -34744,7 +34914,7 @@
       <c r="F1784" s="3"/>
       <c r="G1784" s="3"/>
     </row>
-    <row r="1785" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1785" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1785" s="3" t="s">
         <v>2895</v>
       </c>
@@ -34755,7 +34925,7 @@
       <c r="F1785" s="3"/>
       <c r="G1785" s="3"/>
     </row>
-    <row r="1786" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1786" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1786" s="3" t="s">
         <v>2894</v>
       </c>
@@ -34766,7 +34936,7 @@
       <c r="F1786" s="3"/>
       <c r="G1786" s="3"/>
     </row>
-    <row r="1787" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1787" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1787" s="3" t="s">
         <v>2889</v>
       </c>
@@ -34777,7 +34947,7 @@
       <c r="F1787" s="3"/>
       <c r="G1787" s="3"/>
     </row>
-    <row r="1788" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1788" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1788" s="3" t="s">
         <v>2896</v>
       </c>
@@ -34788,7 +34958,7 @@
       <c r="F1788" s="3"/>
       <c r="G1788" s="3"/>
     </row>
-    <row r="1789" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1789" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1789" s="3" t="s">
         <v>2892</v>
       </c>
@@ -34799,7 +34969,7 @@
       <c r="F1789" s="3"/>
       <c r="G1789" s="3"/>
     </row>
-    <row r="1790" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1790" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1790" s="3" t="s">
         <v>2898</v>
       </c>
@@ -34810,7 +34980,7 @@
       <c r="F1790" s="3"/>
       <c r="G1790" s="3"/>
     </row>
-    <row r="1791" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1791" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1791" s="3" t="s">
         <v>2888</v>
       </c>
@@ -34821,7 +34991,7 @@
       <c r="F1791" s="3"/>
       <c r="G1791" s="3"/>
     </row>
-    <row r="1792" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1792" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1792" s="3" t="s">
         <v>2893</v>
       </c>
@@ -34832,7 +35002,7 @@
       <c r="F1792" s="3"/>
       <c r="G1792" s="3"/>
     </row>
-    <row r="1793" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1793" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1793" s="3" t="s">
         <v>2795</v>
       </c>
@@ -34843,7 +35013,7 @@
       <c r="F1793" s="3"/>
       <c r="G1793" s="3"/>
     </row>
-    <row r="1794" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1794" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1794" s="3" t="s">
         <v>2802</v>
       </c>
@@ -34854,7 +35024,7 @@
       <c r="F1794" s="3"/>
       <c r="G1794" s="3"/>
     </row>
-    <row r="1795" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1795" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1795" s="3" t="s">
         <v>2804</v>
       </c>
@@ -34865,7 +35035,7 @@
       <c r="F1795" s="3"/>
       <c r="G1795" s="3"/>
     </row>
-    <row r="1796" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1796" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1796" s="3" t="s">
         <v>2796</v>
       </c>
@@ -34876,7 +35046,7 @@
       <c r="F1796" s="3"/>
       <c r="G1796" s="3"/>
     </row>
-    <row r="1797" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1797" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1797" s="3" t="s">
         <v>2800</v>
       </c>
@@ -34887,7 +35057,7 @@
       <c r="F1797" s="3"/>
       <c r="G1797" s="3"/>
     </row>
-    <row r="1798" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1798" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1798" s="3" t="s">
         <v>2799</v>
       </c>
@@ -34898,7 +35068,7 @@
       <c r="F1798" s="3"/>
       <c r="G1798" s="3"/>
     </row>
-    <row r="1799" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1799" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1799" s="3" t="s">
         <v>2794</v>
       </c>
@@ -34909,7 +35079,7 @@
       <c r="F1799" s="3"/>
       <c r="G1799" s="3"/>
     </row>
-    <row r="1800" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1800" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1800" s="3" t="s">
         <v>2801</v>
       </c>
@@ -34920,7 +35090,7 @@
       <c r="F1800" s="3"/>
       <c r="G1800" s="3"/>
     </row>
-    <row r="1801" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1801" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1801" s="3" t="s">
         <v>2797</v>
       </c>
@@ -34931,7 +35101,7 @@
       <c r="F1801" s="3"/>
       <c r="G1801" s="3"/>
     </row>
-    <row r="1802" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1802" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1802" s="3" t="s">
         <v>2803</v>
       </c>
@@ -34942,7 +35112,7 @@
       <c r="F1802" s="3"/>
       <c r="G1802" s="3"/>
     </row>
-    <row r="1803" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1803" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1803" s="3" t="s">
         <v>2793</v>
       </c>
@@ -34953,7 +35123,7 @@
       <c r="F1803" s="3"/>
       <c r="G1803" s="3"/>
     </row>
-    <row r="1804" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1804" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1804" s="3" t="s">
         <v>2798</v>
       </c>
@@ -34964,7 +35134,7 @@
       <c r="F1804" s="3"/>
       <c r="G1804" s="3"/>
     </row>
-    <row r="1805" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1805" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1805" s="3" t="s">
         <v>2878</v>
       </c>
@@ -34975,7 +35145,7 @@
       <c r="F1805" s="3"/>
       <c r="G1805" s="3"/>
     </row>
-    <row r="1806" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1806" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1806" s="3" t="s">
         <v>2885</v>
       </c>
@@ -34986,7 +35156,7 @@
       <c r="F1806" s="3"/>
       <c r="G1806" s="3"/>
     </row>
-    <row r="1807" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1807" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1807" s="3" t="s">
         <v>2887</v>
       </c>
@@ -34997,7 +35167,7 @@
       <c r="F1807" s="3"/>
       <c r="G1807" s="3"/>
     </row>
-    <row r="1808" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1808" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1808" s="3" t="s">
         <v>2879</v>
       </c>
@@ -35008,7 +35178,7 @@
       <c r="F1808" s="3"/>
       <c r="G1808" s="3"/>
     </row>
-    <row r="1809" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1809" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1809" s="3" t="s">
         <v>2883</v>
       </c>
@@ -35019,7 +35189,7 @@
       <c r="F1809" s="3"/>
       <c r="G1809" s="3"/>
     </row>
-    <row r="1810" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1810" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1810" s="3" t="s">
         <v>2882</v>
       </c>
@@ -35030,7 +35200,7 @@
       <c r="F1810" s="3"/>
       <c r="G1810" s="3"/>
     </row>
-    <row r="1811" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1811" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1811" s="3" t="s">
         <v>2877</v>
       </c>
@@ -35041,7 +35211,7 @@
       <c r="F1811" s="3"/>
       <c r="G1811" s="3"/>
     </row>
-    <row r="1812" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1812" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1812" s="3" t="s">
         <v>2884</v>
       </c>
@@ -35052,7 +35222,7 @@
       <c r="F1812" s="3"/>
       <c r="G1812" s="3"/>
     </row>
-    <row r="1813" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1813" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1813" s="3" t="s">
         <v>2880</v>
       </c>
@@ -35063,7 +35233,7 @@
       <c r="F1813" s="3"/>
       <c r="G1813" s="3"/>
     </row>
-    <row r="1814" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1814" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1814" s="3" t="s">
         <v>2886</v>
       </c>
@@ -35074,7 +35244,7 @@
       <c r="F1814" s="3"/>
       <c r="G1814" s="3"/>
     </row>
-    <row r="1815" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1815" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1815" s="3" t="s">
         <v>2876</v>
       </c>
@@ -35085,7 +35255,7 @@
       <c r="F1815" s="3"/>
       <c r="G1815" s="3"/>
     </row>
-    <row r="1816" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1816" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1816" s="3" t="s">
         <v>2881</v>
       </c>
@@ -35096,7 +35266,7 @@
       <c r="F1816" s="3"/>
       <c r="G1816" s="3"/>
     </row>
-    <row r="1817" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1817" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1817" s="3" t="s">
         <v>2819</v>
       </c>
@@ -35107,7 +35277,7 @@
       <c r="F1817" s="3"/>
       <c r="G1817" s="3"/>
     </row>
-    <row r="1818" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1818" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1818" s="3" t="s">
         <v>2826</v>
       </c>
@@ -35118,7 +35288,7 @@
       <c r="F1818" s="3"/>
       <c r="G1818" s="3"/>
     </row>
-    <row r="1819" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1819" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1819" s="3" t="s">
         <v>2828</v>
       </c>
@@ -35129,7 +35299,7 @@
       <c r="F1819" s="3"/>
       <c r="G1819" s="3"/>
     </row>
-    <row r="1820" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1820" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1820" s="3" t="s">
         <v>2820</v>
       </c>
@@ -35140,7 +35310,7 @@
       <c r="F1820" s="3"/>
       <c r="G1820" s="3"/>
     </row>
-    <row r="1821" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1821" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1821" s="3" t="s">
         <v>2824</v>
       </c>
@@ -35151,7 +35321,7 @@
       <c r="F1821" s="3"/>
       <c r="G1821" s="3"/>
     </row>
-    <row r="1822" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1822" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1822" s="3" t="s">
         <v>2823</v>
       </c>
@@ -35162,7 +35332,7 @@
       <c r="F1822" s="3"/>
       <c r="G1822" s="3"/>
     </row>
-    <row r="1823" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1823" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1823" s="3" t="s">
         <v>2818</v>
       </c>
@@ -35173,7 +35343,7 @@
       <c r="F1823" s="3"/>
       <c r="G1823" s="3"/>
     </row>
-    <row r="1824" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1824" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1824" s="3" t="s">
         <v>2825</v>
       </c>
@@ -35184,7 +35354,7 @@
       <c r="F1824" s="3"/>
       <c r="G1824" s="3"/>
     </row>
-    <row r="1825" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1825" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1825" s="3" t="s">
         <v>2821</v>
       </c>
@@ -35195,7 +35365,7 @@
       <c r="F1825" s="3"/>
       <c r="G1825" s="3"/>
     </row>
-    <row r="1826" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1826" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1826" s="3" t="s">
         <v>2827</v>
       </c>
@@ -35206,7 +35376,7 @@
       <c r="F1826" s="3"/>
       <c r="G1826" s="3"/>
     </row>
-    <row r="1827" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1827" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1827" s="3" t="s">
         <v>2817</v>
       </c>
@@ -35217,7 +35387,7 @@
       <c r="F1827" s="3"/>
       <c r="G1827" s="3"/>
     </row>
-    <row r="1828" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1828" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1828" s="3" t="s">
         <v>2822</v>
       </c>
@@ -35228,7 +35398,7 @@
       <c r="F1828" s="3"/>
       <c r="G1828" s="3"/>
     </row>
-    <row r="1829" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1829" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1829" s="3" t="s">
         <v>2866</v>
       </c>
@@ -35239,7 +35409,7 @@
       <c r="F1829" s="3"/>
       <c r="G1829" s="3"/>
     </row>
-    <row r="1830" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1830" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1830" s="3" t="s">
         <v>2873</v>
       </c>
@@ -35250,7 +35420,7 @@
       <c r="F1830" s="3"/>
       <c r="G1830" s="3"/>
     </row>
-    <row r="1831" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1831" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1831" s="3" t="s">
         <v>2875</v>
       </c>
@@ -35261,7 +35431,7 @@
       <c r="F1831" s="3"/>
       <c r="G1831" s="3"/>
     </row>
-    <row r="1832" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1832" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1832" s="3" t="s">
         <v>2867</v>
       </c>
@@ -35272,7 +35442,7 @@
       <c r="F1832" s="3"/>
       <c r="G1832" s="3"/>
     </row>
-    <row r="1833" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1833" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1833" s="3" t="s">
         <v>2871</v>
       </c>
@@ -35283,7 +35453,7 @@
       <c r="F1833" s="3"/>
       <c r="G1833" s="3"/>
     </row>
-    <row r="1834" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1834" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1834" s="3" t="s">
         <v>2870</v>
       </c>
@@ -35294,7 +35464,7 @@
       <c r="F1834" s="3"/>
       <c r="G1834" s="3"/>
     </row>
-    <row r="1835" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1835" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1835" s="3" t="s">
         <v>2865</v>
       </c>
@@ -35305,7 +35475,7 @@
       <c r="F1835" s="3"/>
       <c r="G1835" s="3"/>
     </row>
-    <row r="1836" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1836" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1836" s="3" t="s">
         <v>2872</v>
       </c>
@@ -35316,7 +35486,7 @@
       <c r="F1836" s="3"/>
       <c r="G1836" s="3"/>
     </row>
-    <row r="1837" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1837" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1837" s="3" t="s">
         <v>2868</v>
       </c>
@@ -35327,7 +35497,7 @@
       <c r="F1837" s="3"/>
       <c r="G1837" s="3"/>
     </row>
-    <row r="1838" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1838" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1838" s="3" t="s">
         <v>2874</v>
       </c>
@@ -35338,7 +35508,7 @@
       <c r="F1838" s="3"/>
       <c r="G1838" s="3"/>
     </row>
-    <row r="1839" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1839" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1839" s="3" t="s">
         <v>2864</v>
       </c>
@@ -35349,7 +35519,7 @@
       <c r="F1839" s="3"/>
       <c r="G1839" s="3"/>
     </row>
-    <row r="1840" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1840" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1840" s="3" t="s">
         <v>2869</v>
       </c>
@@ -35360,7 +35530,7 @@
       <c r="F1840" s="3"/>
       <c r="G1840" s="3"/>
     </row>
-    <row r="1841" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1841" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1841" s="3" t="s">
         <v>2783</v>
       </c>
@@ -35371,7 +35541,7 @@
       <c r="F1841" s="3"/>
       <c r="G1841" s="3"/>
     </row>
-    <row r="1842" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1842" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1842" s="3" t="s">
         <v>2790</v>
       </c>
@@ -35382,7 +35552,7 @@
       <c r="F1842" s="3"/>
       <c r="G1842" s="3"/>
     </row>
-    <row r="1843" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1843" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1843" s="3" t="s">
         <v>2792</v>
       </c>
@@ -35393,7 +35563,7 @@
       <c r="F1843" s="3"/>
       <c r="G1843" s="3"/>
     </row>
-    <row r="1844" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1844" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1844" s="3" t="s">
         <v>2784</v>
       </c>
@@ -35404,7 +35574,7 @@
       <c r="F1844" s="3"/>
       <c r="G1844" s="3"/>
     </row>
-    <row r="1845" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1845" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1845" s="3" t="s">
         <v>2788</v>
       </c>
@@ -35415,7 +35585,7 @@
       <c r="F1845" s="3"/>
       <c r="G1845" s="3"/>
     </row>
-    <row r="1846" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1846" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1846" s="3" t="s">
         <v>2787</v>
       </c>
@@ -35426,7 +35596,7 @@
       <c r="F1846" s="3"/>
       <c r="G1846" s="3"/>
     </row>
-    <row r="1847" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1847" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1847" s="3" t="s">
         <v>2782</v>
       </c>
@@ -35437,7 +35607,7 @@
       <c r="F1847" s="3"/>
       <c r="G1847" s="3"/>
     </row>
-    <row r="1848" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1848" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1848" s="3" t="s">
         <v>2789</v>
       </c>
@@ -35448,7 +35618,7 @@
       <c r="F1848" s="3"/>
       <c r="G1848" s="3"/>
     </row>
-    <row r="1849" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1849" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1849" s="3" t="s">
         <v>2785</v>
       </c>
@@ -35459,7 +35629,7 @@
       <c r="F1849" s="3"/>
       <c r="G1849" s="3"/>
     </row>
-    <row r="1850" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1850" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1850" s="3" t="s">
         <v>2791</v>
       </c>
@@ -35470,7 +35640,7 @@
       <c r="F1850" s="3"/>
       <c r="G1850" s="3"/>
     </row>
-    <row r="1851" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1851" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1851" s="3" t="s">
         <v>2781</v>
       </c>
@@ -35481,7 +35651,7 @@
       <c r="F1851" s="3"/>
       <c r="G1851" s="3"/>
     </row>
-    <row r="1852" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1852" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1852" s="3" t="s">
         <v>2786</v>
       </c>
@@ -35492,7 +35662,7 @@
       <c r="F1852" s="3"/>
       <c r="G1852" s="3"/>
     </row>
-    <row r="1853" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1853" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1853" s="3" t="s">
         <v>1077</v>
       </c>
@@ -39104,7 +39274,7 @@
       <c r="G2177" s="3"/>
     </row>
     <row r="2178" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2178" s="3" t="s">
+      <c r="A2178" s="9" t="s">
         <v>187</v>
       </c>
       <c r="B2178" s="3" t="s">
@@ -39983,7 +40153,7 @@
       <c r="F2257" s="3"/>
       <c r="G2257" s="3"/>
     </row>
-    <row r="2258" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2258" s="3" t="s">
         <v>2640</v>
       </c>
@@ -39994,7 +40164,7 @@
       <c r="F2258" s="3"/>
       <c r="G2258" s="3"/>
     </row>
-    <row r="2259" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2259" s="3" t="s">
         <v>2647</v>
       </c>
@@ -40005,7 +40175,7 @@
       <c r="F2259" s="3"/>
       <c r="G2259" s="3"/>
     </row>
-    <row r="2260" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2260" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2260" s="3" t="s">
         <v>2649</v>
       </c>
@@ -40016,7 +40186,7 @@
       <c r="F2260" s="3"/>
       <c r="G2260" s="3"/>
     </row>
-    <row r="2261" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2261" s="3" t="s">
         <v>2641</v>
       </c>
@@ -40027,7 +40197,7 @@
       <c r="F2261" s="3"/>
       <c r="G2261" s="3"/>
     </row>
-    <row r="2262" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2262" s="3" t="s">
         <v>2645</v>
       </c>
@@ -40038,7 +40208,7 @@
       <c r="F2262" s="3"/>
       <c r="G2262" s="3"/>
     </row>
-    <row r="2263" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2263" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2263" s="3" t="s">
         <v>2644</v>
       </c>
@@ -40049,7 +40219,7 @@
       <c r="F2263" s="3"/>
       <c r="G2263" s="3"/>
     </row>
-    <row r="2264" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2264" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2264" s="3" t="s">
         <v>2639</v>
       </c>
@@ -40060,7 +40230,7 @@
       <c r="F2264" s="3"/>
       <c r="G2264" s="3"/>
     </row>
-    <row r="2265" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2265" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2265" s="3" t="s">
         <v>2646</v>
       </c>
@@ -40071,7 +40241,7 @@
       <c r="F2265" s="3"/>
       <c r="G2265" s="3"/>
     </row>
-    <row r="2266" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2266" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2266" s="3" t="s">
         <v>2642</v>
       </c>
@@ -40082,7 +40252,7 @@
       <c r="F2266" s="3"/>
       <c r="G2266" s="3"/>
     </row>
-    <row r="2267" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2267" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2267" s="3" t="s">
         <v>2648</v>
       </c>
@@ -40093,7 +40263,7 @@
       <c r="F2267" s="3"/>
       <c r="G2267" s="3"/>
     </row>
-    <row r="2268" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2268" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2268" s="3" t="s">
         <v>2638</v>
       </c>
@@ -40104,7 +40274,7 @@
       <c r="F2268" s="3"/>
       <c r="G2268" s="3"/>
     </row>
-    <row r="2269" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2269" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2269" s="3" t="s">
         <v>2643</v>
       </c>
@@ -45064,7 +45234,7 @@
       <c r="F2713" s="3"/>
       <c r="G2713" s="3"/>
     </row>
-    <row r="2714" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2714" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2714" s="3" t="s">
         <v>1447</v>
       </c>
@@ -45438,7 +45608,7 @@
       <c r="F2747" s="3"/>
       <c r="G2747" s="3"/>
     </row>
-    <row r="2748" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2748" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2748" s="3" t="s">
         <v>592</v>
       </c>
@@ -45735,7 +45905,7 @@
       <c r="F2774" s="3"/>
       <c r="G2774" s="3"/>
     </row>
-    <row r="2775" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2775" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2775" s="3" t="s">
         <v>591</v>
       </c>
@@ -52120,7 +52290,7 @@
       <c r="F3344" s="3"/>
       <c r="G3344" s="3"/>
     </row>
-    <row r="3345" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3345" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3345" s="3" t="s">
         <v>2497</v>
       </c>
@@ -52131,7 +52301,7 @@
       <c r="F3345" s="3"/>
       <c r="G3345" s="3"/>
     </row>
-    <row r="3346" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3346" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3346" s="3" t="s">
         <v>2504</v>
       </c>
@@ -52142,7 +52312,7 @@
       <c r="F3346" s="3"/>
       <c r="G3346" s="3"/>
     </row>
-    <row r="3347" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3347" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3347" s="3" t="s">
         <v>2506</v>
       </c>
@@ -52153,7 +52323,7 @@
       <c r="F3347" s="3"/>
       <c r="G3347" s="3"/>
     </row>
-    <row r="3348" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3348" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3348" s="3" t="s">
         <v>2498</v>
       </c>
@@ -52164,7 +52334,7 @@
       <c r="F3348" s="3"/>
       <c r="G3348" s="3"/>
     </row>
-    <row r="3349" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3349" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3349" s="3" t="s">
         <v>2502</v>
       </c>
@@ -52175,7 +52345,7 @@
       <c r="F3349" s="3"/>
       <c r="G3349" s="3"/>
     </row>
-    <row r="3350" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3350" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3350" s="3" t="s">
         <v>2501</v>
       </c>
@@ -52186,7 +52356,7 @@
       <c r="F3350" s="3"/>
       <c r="G3350" s="3"/>
     </row>
-    <row r="3351" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3351" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3351" s="3" t="s">
         <v>2496</v>
       </c>
@@ -52197,7 +52367,7 @@
       <c r="F3351" s="3"/>
       <c r="G3351" s="3"/>
     </row>
-    <row r="3352" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3352" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3352" s="3" t="s">
         <v>2503</v>
       </c>
@@ -52208,7 +52378,7 @@
       <c r="F3352" s="3"/>
       <c r="G3352" s="3"/>
     </row>
-    <row r="3353" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3353" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3353" s="3" t="s">
         <v>2499</v>
       </c>
@@ -52219,7 +52389,7 @@
       <c r="F3353" s="3"/>
       <c r="G3353" s="3"/>
     </row>
-    <row r="3354" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3354" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3354" s="3" t="s">
         <v>2505</v>
       </c>
@@ -52230,7 +52400,7 @@
       <c r="F3354" s="3"/>
       <c r="G3354" s="3"/>
     </row>
-    <row r="3355" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3355" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3355" s="3" t="s">
         <v>2495</v>
       </c>
@@ -52241,7 +52411,7 @@
       <c r="F3355" s="3"/>
       <c r="G3355" s="3"/>
     </row>
-    <row r="3356" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3356" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3356" s="3" t="s">
         <v>2500</v>
       </c>
@@ -63070,7 +63240,7 @@
       <c r="E4287"/>
       <c r="F4287"/>
     </row>
-    <row r="4288" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4288" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4288" s="2" t="s">
         <v>4283</v>
       </c>
@@ -63233,7 +63403,7 @@
       <c r="E4301"/>
       <c r="F4301"/>
     </row>
-    <row r="4302" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4302" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4302" t="s">
         <v>4296</v>
       </c>
@@ -63377,7 +63547,7 @@
       <c r="E4313"/>
       <c r="F4313"/>
     </row>
-    <row r="4314" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4314" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4314" t="s">
         <v>4308</v>
       </c>
@@ -63521,7 +63691,7 @@
       <c r="E4325"/>
       <c r="F4325"/>
     </row>
-    <row r="4326" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4326" s="2" t="s">
         <v>4320</v>
       </c>
@@ -63533,7 +63703,7 @@
       <c r="E4326" s="2"/>
       <c r="F4326"/>
     </row>
-    <row r="4327" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4327" s="2" t="s">
         <v>4321</v>
       </c>
@@ -63545,7 +63715,7 @@
       <c r="E4327" s="2"/>
       <c r="F4327"/>
     </row>
-    <row r="4328" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4328" s="2" t="s">
         <v>4322</v>
       </c>
@@ -63557,7 +63727,7 @@
       <c r="E4328" s="2"/>
       <c r="F4328"/>
     </row>
-    <row r="4329" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4329" s="2" t="s">
         <v>4323</v>
       </c>
@@ -63569,7 +63739,7 @@
       <c r="E4329" s="2"/>
       <c r="F4329"/>
     </row>
-    <row r="4330" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4330" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4330" s="2" t="s">
         <v>4324</v>
       </c>
@@ -63581,7 +63751,7 @@
       <c r="E4330" s="2"/>
       <c r="F4330"/>
     </row>
-    <row r="4331" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4331" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4331" s="2" t="s">
         <v>4325</v>
       </c>
@@ -63593,7 +63763,7 @@
       <c r="E4331" s="2"/>
       <c r="F4331"/>
     </row>
-    <row r="4332" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4332" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4332" s="2" t="s">
         <v>4326</v>
       </c>
@@ -63605,7 +63775,7 @@
       <c r="E4332" s="2"/>
       <c r="F4332"/>
     </row>
-    <row r="4333" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4333" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4333" s="2" t="s">
         <v>4327</v>
       </c>
@@ -63617,7 +63787,7 @@
       <c r="E4333" s="2"/>
       <c r="F4333"/>
     </row>
-    <row r="4334" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4334" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4334" s="2" t="s">
         <v>4328</v>
       </c>
@@ -63629,7 +63799,7 @@
       <c r="E4334" s="2"/>
       <c r="F4334"/>
     </row>
-    <row r="4335" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4335" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4335" s="2" t="s">
         <v>4329</v>
       </c>
@@ -63641,7 +63811,7 @@
       <c r="E4335" s="2"/>
       <c r="F4335"/>
     </row>
-    <row r="4336" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4336" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4336" s="2" t="s">
         <v>4330</v>
       </c>
@@ -65682,7 +65852,7 @@
         <v>4753</v>
       </c>
     </row>
-    <row r="4522" spans="1:3" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4522" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4522" s="9" t="s">
         <v>4768</v>
       </c>
@@ -65690,7 +65860,7 @@
         <v>4766</v>
       </c>
     </row>
-    <row r="4523" spans="1:3" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4523" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4523" s="9" t="s">
         <v>4767</v>
       </c>
@@ -65765,88 +65935,9 @@
   </sheetData>
   <autoFilter ref="A1:G4531" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
     <filterColumn colId="0">
-      <filters>
-        <filter val="Người tuổi Bính có Thái Dương tọa thủ cung Mệnh ở Tý"/>
-        <filter val="Người tuổi Canh có Thái Dương tọa thủ cung Mệnh ở Ngọ"/>
-        <filter val="Người tuổi Đinh có Thái Dương tọa thủ cung Mệnh ở Ngọ"/>
-        <filter val="Người tuổi Đinh có Thái Dương tọa thủ cung Mệnh ở Tý"/>
-        <filter val="Người tuổi Kỷ có Thái Dương tọa thủ cung Mệnh ở Ngọ"/>
-        <filter val="Người tuổi Tân có Thái Dương tọa thủ cung Mệnh ở Ngọ"/>
-        <filter val="Quý Chị có Thái Dương tọa thủ cung Mệnh ở Dần"/>
-        <filter val="Quý Chị có Thái Dương tọa thủ cung Mệnh ở Dậu"/>
-        <filter val="Quý Chị có Thái Dương tọa thủ cung Mệnh ở Hợi"/>
-        <filter val="Quý Chị có Thái Dương tọa thủ cung Mệnh ở Mão"/>
-        <filter val="Quý Chị có Thái Dương tọa thủ cung Mệnh ở Mùi"/>
-        <filter val="Quý Chị có Thái Dương tọa thủ cung Mệnh ở Ngọ"/>
-        <filter val="Quý Chị có Thái Dương tọa thủ cung Mệnh ở Sửu"/>
-        <filter val="Quý Chị có Thái Dương tọa thủ cung Mệnh ở Thân"/>
-        <filter val="Quý Chị có Thái Dương tọa thủ cung Mệnh ở Thìn"/>
-        <filter val="Quý Chị có Thái Dương tọa thủ cung Mệnh ở Tuất"/>
-        <filter val="Quý Chị có Thái Dương tọa thủ cung Mệnh ở Tý"/>
-        <filter val="Quý Chị có Thái Dương tọa thủ cung Mệnh ở Tỵ"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Dần"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Dần gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Dần gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Dần gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Không, Địa Kiếp, Hỏa Tinh, Linh Tinh"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Dậu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Dậu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Dậu gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Dậu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Không, Địa Kiếp, Hỏa Tinh, Linh Tinh"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Hợi"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Hợi còn Cự Môn ở Tỵ chiếu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Hợi gặp Bạch Hổ, Long Trì, Phượng Các, Hoa Cái"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Văn Xương, Văn Khúc"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Hợi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Hợi gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Hợi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Không, Địa Kiếp, Hỏa Tinh, Linh Tinh"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Hợi gặp Khoa Lộc Quyền, Tả Hữu, Thiên Khôi Đào Hồng"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Mão"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Mão gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Mão gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Mão gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Không, Địa Kiếp, Hỏa Tinh, Linh Tinh"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Mùi"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Mùi đồng cung Hóa Kỵ và không gặp Kình Đà Không Kiếp Thiên Riêu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Mùi đồng cung Thái Âm gặp Văn Xương, Văn Khúc, Thiên Khôi, Đào Hồng"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Mùi gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Mùi gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Mùi gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Không, Địa Kiếp, Hỏa Tinh, Linh Tinh"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Ngọ"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Ngọ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Ngọ gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Ngọ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Không, Địa Kiếp, Hỏa Tinh, Linh Tinh"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Sửu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Sửu đồng cung Hóa Kỵ và không gặp Kình Đà Không Kiếp Thiên Riêu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Sửu đồng cung Thái Âm gặp Khoa Lộc Quyền"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Sửu đồng cung Thái Âm gặp Văn Xương, Văn Khúc, Thiên Khôi, Đào Hồng"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Sửu gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Sửu gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Sửu gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Không, Địa Kiếp, Hỏa Tinh, Linh Tinh"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Thân"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Thân gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Thân gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Thân gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Không, Địa Kiếp, Hỏa Tinh, Linh Tinh"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Thìn"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Thìn gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Thìn gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Thìn gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Không, Địa Kiếp, Hỏa Tinh, Linh Tinh"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Thìn gặp Thái Âm"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Tuất"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Tuất gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Tuất gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Tuất gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Không, Địa Kiếp, Hỏa Tinh, Linh Tinh"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Tý"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Tỵ"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Tỵ còn Cự Môn ở Hợi chiếu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Tý gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Tỵ gặp các sao cát tinh:  Văn Xương, Văn Khúc, Tả Phù, Hữu Bật, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt, Đào Hoa, Hồng Loan, Thiên Hỷ"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Tý gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Tỵ gặp các sao Hình Kỵ:  Thiên Hình, Hóa Kỵ, Thiên Riêu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Tý gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Không, Địa Kiếp, Hỏa Tinh, Linh Tinh"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Tỵ gặp các sao Sát tinh:  Kình Dương, Đà La, Địa Không, Địa Kiếp, Hỏa Tinh, Linh Tinh"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Tỵ gặp Lộc Mã Tả Hữu"/>
-        <filter val="Thái Dương tọa thủ cung Mệnh ở Tỵ gặp Thiên Tướng, Thiên Hình, Phục Binh, Quốc Ấn"/>
-      </filters>
+      <customFilters>
+        <customFilter val="*Thái Dương*"/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B3728">
@@ -65854,64 +65945,95 @@
   </sortState>
   <dataConsolidate/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="25" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A4284 A4292:A1048576">
-    <cfRule type="duplicateValues" dxfId="24" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6713:A1048576 A2:A4169">
-    <cfRule type="duplicateValues" dxfId="23" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B814">
-    <cfRule type="duplicateValues" dxfId="22" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="21" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="27"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3281">
+    <cfRule type="duplicateValues" dxfId="35" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="35"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3285">
+    <cfRule type="duplicateValues" dxfId="33" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="33"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3289">
+    <cfRule type="duplicateValues" dxfId="31" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3293">
+    <cfRule type="duplicateValues" dxfId="29" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="29"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4289">
+    <cfRule type="duplicateValues" dxfId="27" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="25"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4291">
+    <cfRule type="duplicateValues" dxfId="25" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4292:B4418 B3265:B3266 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B4420:B4424 B4426:B4433 B816 B2:B776 B798:B800 B802:B805 B808 B811:B812 B779:B780 B783:B784 B788 B3294:B4284 B791:B795 B818:B1672 B4435:B1048576 B1674:B1683 B1719:B3263 B1703:B1717 B1685:B1701">
+    <cfRule type="duplicateValues" dxfId="23" priority="39"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4419">
+    <cfRule type="duplicateValues" dxfId="22" priority="38"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4466">
+    <cfRule type="duplicateValues" dxfId="21" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6713:B1048576 B4400:B4403 B3265:B3266 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B816 B2:B776 B798:B800 B802:B805 B808 B811:B812 B779:B780 B783:B784 B788 B3294:B4169 B791:B795 B818:B1672 B1674:B1683 B1719:B3263 B1703:B1717 B1685:B1701">
+    <cfRule type="duplicateValues" dxfId="20" priority="40"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:W776 D777:W778 B777:B778 B798:W800 D796:W797 B796:B797 B808:W808 D806:W807 B806:B807 D809:W810 B809:B810 D801:W801 B801 B802:W805 B811:W812 B779:W780 C781:W782 B788:W788 B816:W816 C815:W815 C817:W817 B814:W814 C813:W813 C785:W787 C789:W790 B783:W784 B791:W795 B818:W1672 B1674:W1683 C1673:W1673 C1702:W1702 B1703:W1717 C1718:W1718 B1719:W1048576 B1685:W1701 C1684:W1684">
+    <cfRule type="duplicateValues" dxfId="19" priority="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3721">
+    <cfRule type="duplicateValues" dxfId="18" priority="47"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1673">
+    <cfRule type="duplicateValues" dxfId="17" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1673">
+    <cfRule type="duplicateValues" dxfId="16" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1673">
+    <cfRule type="duplicateValues" dxfId="15" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1702">
+    <cfRule type="duplicateValues" dxfId="14" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1702">
+    <cfRule type="duplicateValues" dxfId="13" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1702">
+    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1718">
-    <cfRule type="duplicateValues" dxfId="20" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="19" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3281">
-    <cfRule type="duplicateValues" dxfId="17" priority="19"/>
-    <cfRule type="duplicateValues" dxfId="16" priority="20"/>
+  <conditionalFormatting sqref="B1718">
+    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3285">
-    <cfRule type="duplicateValues" dxfId="15" priority="17"/>
-    <cfRule type="duplicateValues" dxfId="14" priority="18"/>
+  <conditionalFormatting sqref="B1718">
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3289">
-    <cfRule type="duplicateValues" dxfId="13" priority="15"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="16"/>
+  <conditionalFormatting sqref="B1684">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3293">
-    <cfRule type="duplicateValues" dxfId="11" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="14"/>
+  <conditionalFormatting sqref="B1684">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4289">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4291">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4292:B4418 B3265:B3266 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B4420:B4424 B4426:B4433 B1719:B3263 B816 B2:B776 B798:B800 B802:B805 B808 B811:B812 B779:B780 B783:B784 B788 B3294:B4284 B791:B795 B818:B1717 B4435:B1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="24"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4419">
-    <cfRule type="duplicateValues" dxfId="4" priority="23"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4466">
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6713:B1048576 B4400:B4403 B3265:B3266 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B1719:B3263 B816 B2:B776 B798:B800 B802:B805 B808 B811:B812 B779:B780 B783:B784 B788 B3294:B4169 B791:B795 B818:B1717">
-    <cfRule type="duplicateValues" dxfId="2" priority="25"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1718:W1718 B1:W776 D777:W778 B777:B778 B798:W800 D796:W797 B796:B797 B808:W808 D806:W807 B806:B807 D809:W810 B809:B810 D801:W801 B801 B802:W805 B811:W812 B779:W780 C781:W782 B788:W788 B816:W816 C815:W815 C817:W817 B814:W814 C813:W813 C785:W787 C789:W790 B783:W784 B791:W795 B818:W1717 B1719:W1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G3721">
-    <cfRule type="duplicateValues" dxfId="0" priority="32"/>
+  <conditionalFormatting sqref="B1684">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Giải thích về Thiên Cơ
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FFCEAA-5547-41F9-A0C8-CC9473B6D5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C511029-9A7A-42B0-8DCB-4CA87FBCFC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$G$4531</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$G$4535</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9250" uniqueCount="4786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9270" uniqueCount="4811">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -14397,6 +14397,83 @@
   </si>
   <si>
     <t>Lập kỳ công trong thời buổi ổn định</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thân hình cao, xương lộ, da trắng, mặt dài, nhưng đều đặn, rất thông minh, khôn ngoan, có óc kinh doanh, có mưu trí, biết quyền biến, tính nhân hậu, từ thiện, được
+hưởng giàu sang và sống lâu. </t>
+  </si>
+  <si>
+    <t>Tất được hưởng phú qúy song toàn và có uy danh lừng lẫy.</t>
+  </si>
+  <si>
+    <t>Chắc chắn phù hợp và trở thành danh y khoa, dược khoa</t>
+  </si>
+  <si>
+    <t>Bạn là người khéo tay, thường chuyên về kỹ nghệ, máy móc hay thủ công.</t>
+  </si>
+  <si>
+    <t>Cách cục là người đa tài, được hưởng phú qúy đến tột bực.</t>
+  </si>
+  <si>
+    <t>Cách cục lập được sự nghiệp lớn lao và được hưởng giàu sang trọn đời.</t>
+  </si>
+  <si>
+    <t>Thân hình nở nang, hơi thấp, da trắng, mặt tròn, kém thông minh hơn Thiên Cơ miếu vượng địa, cũng có óc kinh doanh, nhưng có tính gian xảo, thường phải buôn
+bán ngược xuôi hay làm nghề thủ công để kiếm ăn. Tuy vậy, vẫn được no cơm ấn áo và sống lâu.</t>
+  </si>
+  <si>
+    <t>Tất phải có tàn tật, nhất khó chữa, phải thường lang thang phiêu bạt, lại hay mắc những tai họa khủng khiếp, nếu không cùng khổ cô đơn,</t>
+  </si>
+  <si>
+    <t>Hay mắc phải tai nạn tay chân, mổ xẻ.</t>
+  </si>
+  <si>
+    <t>Quý Anh là người có mưu trí hay bàn xét về chính lược chiến lược.</t>
+  </si>
+  <si>
+    <t>Quý Chị  là người khôn ngoan tài giỏi, đảm đang, vượng phu ích tử, nhưng hưởng giàu sang và sống lâu.</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Dần</t>
+  </si>
+  <si>
+    <t>Quý Chị có Thiên Cơ tọa thủ cung Mệnh ở Hợi</t>
+  </si>
+  <si>
+    <t>Bạn là người đảm đang, suốt đời vất vả, hay tính toán lợi cho bản thân, phải muộn lập gia đình hay lấy kế, lấy lẽ mới tránh được những nỗi buồn thương, đau đớn vì chồng con.</t>
+  </si>
+  <si>
+    <t>Biểu thị bạn là người thích bàn luận đề tài mà người bình thường không rành, hơn nữa còn biểu hiện phong thái hùng tài vĩ lược, tất nhiên là giỏi biện luận, nhạy bén mưu trí và quyền biến. Thông thường không nên làm công việc kinh doanh buôn bán, có thể trở thành nhân tài tham mưu cố vấn.</t>
+  </si>
+  <si>
+    <t>Chủ về khéo léo, thông minh cơ trí, nhưng tính rất ham quyền bính, điều hành.</t>
+  </si>
+  <si>
+    <t>Bạn xử sự có mạch lạc, lớp lang, ngăn nắp, thứ tự, có thể dựa vào đó để định phương kế và kế hoạch làm việc, cho nên thích hợp làm công chức, hoặc đảm nhiệm chức vụ trong công ty. Xã hội hiện đại xem trọng việc quản lý công ty, rất thích hợp với người có mệnh cách này.</t>
+  </si>
+  <si>
+    <t>Cách cục là người qủy quyệt xảo trá, tính toán nhằm đem lợi ích cho bản thân.</t>
+  </si>
+  <si>
+    <t>Cách cục trộm cướp, bất lương.</t>
+  </si>
+  <si>
+    <t>Bạn nhân từ và chắc chắn là được hưởng phúc thọ song toàn. Bạn còn là người học rộng tài cao, hay bàn xét về chính lược, chiến lược</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thật chỉ có tu hành mới được yên thân, hưởng phúc và sống lâu. </t>
+  </si>
+  <si>
+    <t>Thiên Cơ Thiên Lương đồng cung tại Mệnh ở Thìn gặp các sao cát tinh: Văn Xương, Văn Khúc, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Chắc chắn là được hưởng giàu sang trọn đời.</t>
+  </si>
+  <si>
+    <t>Thiên Cơ Thiên Lương đồng cung tại Mệnh ở Tuất gặp các sao cát tinh: Văn Xương, Văn Khúc, Hóa Khoa, Hóa Lộc, Hóa Quyền, Thiên Khôi, Thiên Việt</t>
+  </si>
+  <si>
+    <t>Thường là công chức</t>
   </si>
 </sst>
 </file>
@@ -14484,7 +14561,427 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="83">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -15172,10 +15669,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A2:G4531"/>
+  <dimension ref="A2:G4535"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4520" workbookViewId="0">
-      <selection activeCell="B1684" sqref="B1684"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4540" sqref="A4540"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16241,7 +16738,7 @@
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>516</v>
       </c>
@@ -16274,7 +16771,7 @@
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
     </row>
-    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>517</v>
       </c>
@@ -16285,7 +16782,7 @@
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
     </row>
-    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>522</v>
       </c>
@@ -16362,7 +16859,7 @@
       <c r="F103" s="3"/>
       <c r="G103" s="3"/>
     </row>
-    <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>520</v>
       </c>
@@ -16989,7 +17486,7 @@
       <c r="F160" s="3"/>
       <c r="G160" s="3"/>
     </row>
-    <row r="161" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>518</v>
       </c>
@@ -17000,7 +17497,7 @@
       <c r="F161" s="3"/>
       <c r="G161" s="3"/>
     </row>
-    <row r="162" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>523</v>
       </c>
@@ -17066,7 +17563,7 @@
       <c r="F167" s="3"/>
       <c r="G167" s="3"/>
     </row>
-    <row r="168" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>519</v>
       </c>
@@ -17517,7 +18014,7 @@
       <c r="F208" s="3"/>
       <c r="G208" s="3"/>
     </row>
-    <row r="209" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="3" t="s">
         <v>521</v>
       </c>
@@ -18276,7 +18773,7 @@
       <c r="F277" s="3"/>
       <c r="G277" s="3"/>
     </row>
-    <row r="278" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" s="9" t="s">
         <v>1397</v>
       </c>
@@ -19862,7 +20359,7 @@
       <c r="F421" s="3"/>
       <c r="G421" s="3"/>
     </row>
-    <row r="422" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" s="3" t="s">
         <v>935</v>
       </c>
@@ -21556,7 +22053,7 @@
       <c r="F575" s="3"/>
       <c r="G575" s="3"/>
     </row>
-    <row r="576" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A576" s="3" t="s">
         <v>962</v>
       </c>
@@ -21567,7 +22064,7 @@
       <c r="F576" s="3"/>
       <c r="G576" s="3"/>
     </row>
-    <row r="577" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="577" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A577" s="3" t="s">
         <v>963</v>
       </c>
@@ -26530,7 +27027,7 @@
       <c r="F1022" s="3"/>
       <c r="G1022" s="3"/>
     </row>
-    <row r="1023" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1023" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1023" s="3" t="s">
         <v>754</v>
       </c>
@@ -26541,7 +27038,7 @@
       <c r="F1023" s="3"/>
       <c r="G1023" s="3"/>
     </row>
-    <row r="1024" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1024" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1024" s="3" t="s">
         <v>1519</v>
       </c>
@@ -26719,44 +27216,44 @@
       <c r="G1038" s="3"/>
     </row>
     <row r="1039" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1039" s="3" t="s">
+      <c r="A1039" s="9" t="s">
         <v>243</v>
       </c>
       <c r="B1039" s="3" t="s">
-        <v>243</v>
+        <v>4790</v>
       </c>
       <c r="C1039" s="3"/>
       <c r="F1039" s="3"/>
       <c r="G1039" s="3"/>
     </row>
     <row r="1040" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1040" s="3" t="s">
+      <c r="A1040" s="9" t="s">
         <v>239</v>
       </c>
       <c r="B1040" s="3" t="s">
-        <v>239</v>
+        <v>4790</v>
       </c>
       <c r="C1040" s="3"/>
       <c r="F1040" s="3"/>
       <c r="G1040" s="3"/>
     </row>
-    <row r="1041" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1041" s="3" t="s">
+    <row r="1041" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1041" s="9" t="s">
         <v>250</v>
       </c>
       <c r="B1041" s="3" t="s">
-        <v>250</v>
+        <v>4791</v>
       </c>
       <c r="C1041" s="3"/>
       <c r="F1041" s="3"/>
       <c r="G1041" s="3"/>
     </row>
-    <row r="1042" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1042" s="3" t="s">
+    <row r="1042" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1042" s="9" t="s">
         <v>247</v>
       </c>
       <c r="B1042" s="3" t="s">
-        <v>247</v>
+        <v>4791</v>
       </c>
       <c r="C1042" s="3"/>
       <c r="F1042" s="3"/>
@@ -26850,7 +27347,7 @@
       <c r="F1050" s="3"/>
       <c r="G1050" s="3"/>
     </row>
-    <row r="1051" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1051" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1051" s="9" t="s">
         <v>1058</v>
       </c>
@@ -26872,44 +27369,44 @@
       <c r="G1052" s="3"/>
     </row>
     <row r="1053" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1053" s="3" t="s">
+      <c r="A1053" s="9" t="s">
         <v>246</v>
       </c>
       <c r="B1053" s="3" t="s">
-        <v>246</v>
+        <v>4790</v>
       </c>
       <c r="C1053" s="3"/>
       <c r="F1053" s="3"/>
       <c r="G1053" s="3"/>
     </row>
     <row r="1054" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1054" s="3" t="s">
+      <c r="A1054" s="9" t="s">
         <v>242</v>
       </c>
       <c r="B1054" s="3" t="s">
-        <v>242</v>
+        <v>4790</v>
       </c>
       <c r="C1054" s="3"/>
       <c r="F1054" s="3"/>
       <c r="G1054" s="3"/>
     </row>
-    <row r="1055" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1055" s="3" t="s">
+    <row r="1055" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1055" s="9" t="s">
         <v>251</v>
       </c>
       <c r="B1055" s="3" t="s">
-        <v>251</v>
+        <v>4791</v>
       </c>
       <c r="C1055" s="3"/>
       <c r="F1055" s="3"/>
       <c r="G1055" s="3"/>
     </row>
-    <row r="1056" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1056" s="3" t="s">
+    <row r="1056" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1056" s="9" t="s">
         <v>248</v>
       </c>
       <c r="B1056" s="3" t="s">
-        <v>248</v>
+        <v>4791</v>
       </c>
       <c r="C1056" s="3"/>
       <c r="F1056" s="3"/>
@@ -26959,7 +27456,7 @@
       <c r="F1060" s="3"/>
       <c r="G1060" s="3"/>
     </row>
-    <row r="1061" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1061" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1061" s="9" t="s">
         <v>1055</v>
       </c>
@@ -27101,7 +27598,7 @@
       <c r="F1073" s="3"/>
       <c r="G1073" s="3"/>
     </row>
-    <row r="1074" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1074" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1074" s="9" t="s">
         <v>1059</v>
       </c>
@@ -27134,22 +27631,22 @@
       <c r="G1076" s="3"/>
     </row>
     <row r="1077" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1077" s="3" t="s">
+      <c r="A1077" s="9" t="s">
         <v>252</v>
       </c>
       <c r="B1077" s="3" t="s">
-        <v>252</v>
+        <v>4791</v>
       </c>
       <c r="C1077" s="3"/>
       <c r="F1077" s="3"/>
       <c r="G1077" s="3"/>
     </row>
-    <row r="1078" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1078" s="3" t="s">
+    <row r="1078" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1078" s="9" t="s">
         <v>249</v>
       </c>
       <c r="B1078" s="3" t="s">
-        <v>249</v>
+        <v>4791</v>
       </c>
       <c r="C1078" s="3"/>
       <c r="F1078" s="3"/>
@@ -27320,7 +27817,7 @@
       <c r="F1093" s="3"/>
       <c r="G1093" s="3"/>
     </row>
-    <row r="1094" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1094" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1094" s="9" t="s">
         <v>1057</v>
       </c>
@@ -27375,22 +27872,22 @@
       <c r="G1098" s="3"/>
     </row>
     <row r="1099" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1099" s="3" t="s">
+      <c r="A1099" s="9" t="s">
         <v>245</v>
       </c>
       <c r="B1099" s="3" t="s">
-        <v>245</v>
+        <v>4790</v>
       </c>
       <c r="C1099" s="3"/>
       <c r="F1099" s="3"/>
       <c r="G1099" s="3"/>
     </row>
     <row r="1100" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1100" s="3" t="s">
+      <c r="A1100" s="9" t="s">
         <v>241</v>
       </c>
       <c r="B1100" s="3" t="s">
-        <v>241</v>
+        <v>4790</v>
       </c>
       <c r="C1100" s="3"/>
       <c r="F1100" s="3"/>
@@ -27462,7 +27959,7 @@
       <c r="F1106" s="3"/>
       <c r="G1106" s="3"/>
     </row>
-    <row r="1107" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1107" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1107" s="9" t="s">
         <v>4756</v>
       </c>
@@ -27681,7 +28178,7 @@
       <c r="F1126" s="3"/>
       <c r="G1126" s="3"/>
     </row>
-    <row r="1127" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1127" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1127" s="9" t="s">
         <v>1056</v>
       </c>
@@ -27714,22 +28211,22 @@
       <c r="G1129" s="3"/>
     </row>
     <row r="1130" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1130" s="3" t="s">
+      <c r="A1130" s="9" t="s">
         <v>244</v>
       </c>
       <c r="B1130" s="3" t="s">
-        <v>244</v>
+        <v>4790</v>
       </c>
       <c r="C1130" s="3"/>
       <c r="F1130" s="3"/>
       <c r="G1130" s="3"/>
     </row>
     <row r="1131" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1131" s="3" t="s">
+      <c r="A1131" s="9" t="s">
         <v>240</v>
       </c>
       <c r="B1131" s="3" t="s">
-        <v>240</v>
+        <v>4790</v>
       </c>
       <c r="C1131" s="3"/>
       <c r="F1131" s="3"/>
@@ -29759,23 +30256,23 @@
       <c r="F1315" s="3"/>
       <c r="G1315" s="3"/>
     </row>
-    <row r="1316" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1316" s="3" t="s">
+    <row r="1316" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1316" s="9" t="s">
         <v>237</v>
       </c>
       <c r="B1316" s="3" t="s">
-        <v>237</v>
+        <v>4795</v>
       </c>
       <c r="C1316" s="3"/>
       <c r="F1316" s="3"/>
       <c r="G1316" s="3"/>
     </row>
-    <row r="1317" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1317" s="3" t="s">
+    <row r="1317" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1317" s="9" t="s">
         <v>238</v>
       </c>
       <c r="B1317" s="3" t="s">
-        <v>238</v>
+        <v>4795</v>
       </c>
       <c r="C1317" s="3"/>
       <c r="F1317" s="3"/>
@@ -29990,7 +30487,7 @@
       <c r="F1336" s="3"/>
       <c r="G1336" s="3"/>
     </row>
-    <row r="1337" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1337" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1337" s="9" t="s">
         <v>1021</v>
       </c>
@@ -30003,7 +30500,7 @@
       <c r="F1337" s="3"/>
       <c r="G1337" s="3"/>
     </row>
-    <row r="1338" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1338" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1338" s="9" t="s">
         <v>1023</v>
       </c>
@@ -30016,7 +30513,7 @@
       <c r="F1338" s="3"/>
       <c r="G1338" s="3"/>
     </row>
-    <row r="1339" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1339" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1339" s="9" t="s">
         <v>1029</v>
       </c>
@@ -30029,7 +30526,7 @@
       <c r="F1339" s="3"/>
       <c r="G1339" s="3"/>
     </row>
-    <row r="1340" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1340" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1340" s="9" t="s">
         <v>1019</v>
       </c>
@@ -30042,7 +30539,7 @@
       <c r="F1340" s="3"/>
       <c r="G1340" s="3"/>
     </row>
-    <row r="1341" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1341" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1341" s="9" t="s">
         <v>1027</v>
       </c>
@@ -30055,7 +30552,7 @@
       <c r="F1341" s="3"/>
       <c r="G1341" s="3"/>
     </row>
-    <row r="1342" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1342" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1342" s="9" t="s">
         <v>1025</v>
       </c>
@@ -30068,7 +30565,7 @@
       <c r="F1342" s="3"/>
       <c r="G1342" s="3"/>
     </row>
-    <row r="1343" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1343" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1343" s="9" t="s">
         <v>1017</v>
       </c>
@@ -30213,111 +30710,111 @@
       <c r="F1355" s="3"/>
       <c r="G1355" s="3"/>
     </row>
-    <row r="1356" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1356" s="3" t="s">
+    <row r="1356" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1356" s="9" t="s">
         <v>206</v>
       </c>
       <c r="B1356" s="3" t="s">
-        <v>206</v>
+        <v>4796</v>
       </c>
       <c r="C1356" s="3"/>
       <c r="F1356" s="3"/>
       <c r="G1356" s="3"/>
     </row>
-    <row r="1357" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1357" s="3" t="s">
+    <row r="1357" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1357" s="9" t="s">
         <v>201</v>
       </c>
       <c r="B1357" s="3" t="s">
-        <v>201</v>
+        <v>4796</v>
       </c>
       <c r="C1357" s="3"/>
       <c r="F1357" s="3"/>
       <c r="G1357" s="3"/>
     </row>
-    <row r="1358" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1358" s="3" t="s">
+    <row r="1358" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1358" s="9" t="s">
         <v>236</v>
       </c>
       <c r="B1358" s="3" t="s">
-        <v>236</v>
+        <v>4796</v>
       </c>
       <c r="C1358" s="3"/>
       <c r="F1358" s="3"/>
       <c r="G1358" s="3"/>
     </row>
-    <row r="1359" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1359" s="3" t="s">
+    <row r="1359" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1359" s="9" t="s">
         <v>226</v>
       </c>
       <c r="B1359" s="3" t="s">
-        <v>226</v>
+        <v>4796</v>
       </c>
       <c r="C1359" s="3"/>
       <c r="F1359" s="3"/>
       <c r="G1359" s="3"/>
     </row>
-    <row r="1360" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1360" s="3" t="s">
+    <row r="1360" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1360" s="9" t="s">
         <v>231</v>
       </c>
       <c r="B1360" s="3" t="s">
-        <v>231</v>
+        <v>4796</v>
       </c>
       <c r="C1360" s="3"/>
       <c r="F1360" s="3"/>
       <c r="G1360" s="3"/>
     </row>
-    <row r="1361" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1361" s="3" t="s">
+    <row r="1361" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1361" s="9" t="s">
         <v>216</v>
       </c>
       <c r="B1361" s="3" t="s">
-        <v>216</v>
+        <v>4796</v>
       </c>
       <c r="C1361" s="3"/>
       <c r="F1361" s="3"/>
       <c r="G1361" s="3"/>
     </row>
-    <row r="1362" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1362" s="3" t="s">
+    <row r="1362" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1362" s="9" t="s">
         <v>191</v>
       </c>
       <c r="B1362" s="3" t="s">
-        <v>191</v>
+        <v>4796</v>
       </c>
       <c r="C1362" s="3"/>
       <c r="F1362" s="3"/>
       <c r="G1362" s="3"/>
     </row>
-    <row r="1363" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1363" s="3" t="s">
+    <row r="1363" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1363" s="9" t="s">
         <v>196</v>
       </c>
       <c r="B1363" s="3" t="s">
-        <v>196</v>
+        <v>4796</v>
       </c>
       <c r="C1363" s="3"/>
       <c r="F1363" s="3"/>
       <c r="G1363" s="3"/>
     </row>
-    <row r="1364" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1364" s="3" t="s">
+    <row r="1364" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1364" s="9" t="s">
         <v>221</v>
       </c>
       <c r="B1364" s="3" t="s">
-        <v>221</v>
+        <v>4796</v>
       </c>
       <c r="C1364" s="3"/>
       <c r="F1364" s="3"/>
       <c r="G1364" s="3"/>
     </row>
-    <row r="1365" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A1365" s="3" t="s">
+    <row r="1365" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A1365" s="9" t="s">
         <v>211</v>
       </c>
       <c r="B1365" s="3" t="s">
-        <v>211</v>
+        <v>4796</v>
       </c>
       <c r="C1365" s="3"/>
       <c r="F1365" s="3"/>
@@ -33414,7 +33911,7 @@
       <c r="F1646" s="3"/>
       <c r="G1646" s="3"/>
     </row>
-    <row r="1647" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1647" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1647" s="9" t="s">
         <v>1396</v>
       </c>
@@ -33427,7 +33924,7 @@
       <c r="F1647" s="3"/>
       <c r="G1647" s="3"/>
     </row>
-    <row r="1648" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1648" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1648" s="9" t="s">
         <v>1393</v>
       </c>
@@ -33438,7 +33935,7 @@
       <c r="F1648" s="3"/>
       <c r="G1648" s="3"/>
     </row>
-    <row r="1649" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1649" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1649" s="9" t="s">
         <v>1395</v>
       </c>
@@ -33449,7 +33946,7 @@
       <c r="F1649" s="3"/>
       <c r="G1649" s="3"/>
     </row>
-    <row r="1650" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1650" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1650" s="9" t="s">
         <v>4763</v>
       </c>
@@ -33462,7 +33959,7 @@
       <c r="F1650" s="3"/>
       <c r="G1650" s="3"/>
     </row>
-    <row r="1651" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1651" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1651" s="9" t="s">
         <v>1394</v>
       </c>
@@ -33473,7 +33970,7 @@
       <c r="F1651" s="3"/>
       <c r="G1651" s="3"/>
     </row>
-    <row r="1652" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1652" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1652" s="3" t="s">
         <v>1060</v>
       </c>
@@ -33484,7 +33981,7 @@
       <c r="F1652" s="3"/>
       <c r="G1652" s="3"/>
     </row>
-    <row r="1653" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1653" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1653" s="9" t="s">
         <v>1054</v>
       </c>
@@ -33495,7 +33992,7 @@
       <c r="F1653" s="3"/>
       <c r="G1653" s="3"/>
     </row>
-    <row r="1654" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="1654" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1654" s="9" t="s">
         <v>172</v>
       </c>
@@ -33505,7 +34002,7 @@
       <c r="F1654" s="3"/>
       <c r="G1654" s="3"/>
     </row>
-    <row r="1655" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="1655" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1655" s="9" t="s">
         <v>173</v>
       </c>
@@ -33515,7 +34012,7 @@
       <c r="F1655" s="3"/>
       <c r="G1655" s="3"/>
     </row>
-    <row r="1656" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1656" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1656" s="9" t="s">
         <v>174</v>
       </c>
@@ -33525,7 +34022,7 @@
       <c r="F1656" s="3"/>
       <c r="G1656" s="3"/>
     </row>
-    <row r="1657" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1657" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1657" s="9" t="s">
         <v>1020</v>
       </c>
@@ -33535,7 +34032,7 @@
       <c r="F1657" s="3"/>
       <c r="G1657" s="3"/>
     </row>
-    <row r="1658" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="1658" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1658" s="9" t="s">
         <v>1036</v>
       </c>
@@ -33548,7 +34045,7 @@
       <c r="F1658" s="3"/>
       <c r="G1658" s="3"/>
     </row>
-    <row r="1659" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="1659" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1659" s="9" t="s">
         <v>1039</v>
       </c>
@@ -33558,7 +34055,7 @@
       <c r="F1659" s="3"/>
       <c r="G1659" s="3"/>
     </row>
-    <row r="1660" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1660" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1660" s="9" t="s">
         <v>1038</v>
       </c>
@@ -33568,7 +34065,7 @@
       <c r="F1660" s="3"/>
       <c r="G1660" s="3"/>
     </row>
-    <row r="1661" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1661" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1661" s="9" t="s">
         <v>1037</v>
       </c>
@@ -33578,7 +34075,7 @@
       <c r="F1661" s="3"/>
       <c r="G1661" s="3"/>
     </row>
-    <row r="1662" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="1662" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1662" s="9" t="s">
         <v>1044</v>
       </c>
@@ -33594,7 +34091,7 @@
       <c r="F1662" s="3"/>
       <c r="G1662" s="3"/>
     </row>
-    <row r="1663" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1663" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1663" s="9" t="s">
         <v>1053</v>
       </c>
@@ -33604,7 +34101,7 @@
       <c r="F1663" s="3"/>
       <c r="G1663" s="3"/>
     </row>
-    <row r="1664" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="1664" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1664" s="9" t="s">
         <v>1047</v>
       </c>
@@ -33614,7 +34111,7 @@
       <c r="F1664" s="3"/>
       <c r="G1664" s="3"/>
     </row>
-    <row r="1665" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1665" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1665" s="9" t="s">
         <v>1046</v>
       </c>
@@ -33624,7 +34121,7 @@
       <c r="F1665" s="3"/>
       <c r="G1665" s="3"/>
     </row>
-    <row r="1666" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1666" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1666" s="9" t="s">
         <v>1045</v>
       </c>
@@ -33634,7 +34131,7 @@
       <c r="F1666" s="3"/>
       <c r="G1666" s="3"/>
     </row>
-    <row r="1667" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="1667" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1667" s="9" t="s">
         <v>175</v>
       </c>
@@ -33644,7 +34141,7 @@
       <c r="F1667" s="3"/>
       <c r="G1667" s="3"/>
     </row>
-    <row r="1668" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="1668" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1668" s="9" t="s">
         <v>176</v>
       </c>
@@ -33654,7 +34151,7 @@
       <c r="F1668" s="3"/>
       <c r="G1668" s="3"/>
     </row>
-    <row r="1669" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1669" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1669" s="9" t="s">
         <v>177</v>
       </c>
@@ -33664,7 +34161,7 @@
       <c r="F1669" s="3"/>
       <c r="G1669" s="3"/>
     </row>
-    <row r="1670" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1670" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1670" s="9" t="s">
         <v>1022</v>
       </c>
@@ -33674,7 +34171,7 @@
       <c r="F1670" s="3"/>
       <c r="G1670" s="3"/>
     </row>
-    <row r="1671" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="1671" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1671" s="9" t="s">
         <v>184</v>
       </c>
@@ -33687,7 +34184,7 @@
       <c r="F1671" s="3"/>
       <c r="G1671" s="3"/>
     </row>
-    <row r="1672" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1672" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1672" s="9" t="s">
         <v>1031</v>
       </c>
@@ -33697,7 +34194,7 @@
       <c r="F1672" s="3"/>
       <c r="G1672" s="3"/>
     </row>
-    <row r="1673" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1673" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1673" s="3" t="s">
         <v>1399</v>
       </c>
@@ -33707,7 +34204,7 @@
       <c r="F1673" s="3"/>
       <c r="G1673" s="3"/>
     </row>
-    <row r="1674" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="1674" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1674" s="9" t="s">
         <v>185</v>
       </c>
@@ -33717,7 +34214,7 @@
       <c r="F1674" s="3"/>
       <c r="G1674" s="3"/>
     </row>
-    <row r="1675" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1675" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1675" s="9" t="s">
         <v>186</v>
       </c>
@@ -33727,7 +34224,7 @@
       <c r="F1675" s="3"/>
       <c r="G1675" s="3"/>
     </row>
-    <row r="1676" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1676" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1676" s="9" t="s">
         <v>1028</v>
       </c>
@@ -33737,7 +34234,7 @@
       <c r="F1676" s="3"/>
       <c r="G1676" s="3"/>
     </row>
-    <row r="1677" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="1677" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1677" s="9" t="s">
         <v>169</v>
       </c>
@@ -33747,7 +34244,7 @@
       <c r="F1677" s="3"/>
       <c r="G1677" s="3"/>
     </row>
-    <row r="1678" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="1678" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1678" s="9" t="s">
         <v>170</v>
       </c>
@@ -33757,7 +34254,7 @@
       <c r="F1678" s="3"/>
       <c r="G1678" s="3"/>
     </row>
-    <row r="1679" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1679" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1679" s="9" t="s">
         <v>171</v>
       </c>
@@ -33767,7 +34264,7 @@
       <c r="F1679" s="3"/>
       <c r="G1679" s="3"/>
     </row>
-    <row r="1680" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1680" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1680" s="9" t="s">
         <v>1018</v>
       </c>
@@ -33777,7 +34274,7 @@
       <c r="F1680" s="3"/>
       <c r="G1680" s="3"/>
     </row>
-    <row r="1681" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="1681" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1681" s="9" t="s">
         <v>181</v>
       </c>
@@ -33787,7 +34284,7 @@
       <c r="F1681" s="3"/>
       <c r="G1681" s="3"/>
     </row>
-    <row r="1682" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1682" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1682" s="9" t="s">
         <v>1030</v>
       </c>
@@ -33797,7 +34294,7 @@
       <c r="F1682" s="3"/>
       <c r="G1682" s="3"/>
     </row>
-    <row r="1683" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1683" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1683" s="9" t="s">
         <v>1400</v>
       </c>
@@ -33807,7 +34304,7 @@
       <c r="F1683" s="3"/>
       <c r="G1683" s="3"/>
     </row>
-    <row r="1684" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1684" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1684" s="3" t="s">
         <v>1398</v>
       </c>
@@ -33817,7 +34314,7 @@
       <c r="F1684" s="3"/>
       <c r="G1684" s="3"/>
     </row>
-    <row r="1685" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="1685" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1685" s="9" t="s">
         <v>182</v>
       </c>
@@ -33827,7 +34324,7 @@
       <c r="F1685" s="3"/>
       <c r="G1685" s="3"/>
     </row>
-    <row r="1686" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1686" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1686" s="9" t="s">
         <v>183</v>
       </c>
@@ -33837,7 +34334,7 @@
       <c r="F1686" s="3"/>
       <c r="G1686" s="3"/>
     </row>
-    <row r="1687" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1687" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1687" s="9" t="s">
         <v>1026</v>
       </c>
@@ -33847,7 +34344,7 @@
       <c r="F1687" s="3"/>
       <c r="G1687" s="3"/>
     </row>
-    <row r="1688" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="1688" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1688" s="9" t="s">
         <v>1032</v>
       </c>
@@ -33860,7 +34357,7 @@
       <c r="F1688" s="3"/>
       <c r="G1688" s="3"/>
     </row>
-    <row r="1689" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="1689" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1689" s="9" t="s">
         <v>1035</v>
       </c>
@@ -33870,7 +34367,7 @@
       <c r="F1689" s="3"/>
       <c r="G1689" s="3"/>
     </row>
-    <row r="1690" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1690" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1690" s="9" t="s">
         <v>1034</v>
       </c>
@@ -33880,7 +34377,7 @@
       <c r="F1690" s="3"/>
       <c r="G1690" s="3"/>
     </row>
-    <row r="1691" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1691" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1691" s="9" t="s">
         <v>1033</v>
       </c>
@@ -33890,7 +34387,7 @@
       <c r="F1691" s="3"/>
       <c r="G1691" s="3"/>
     </row>
-    <row r="1692" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="1692" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1692" s="9" t="s">
         <v>178</v>
       </c>
@@ -33900,7 +34397,7 @@
       <c r="F1692" s="3"/>
       <c r="G1692" s="3"/>
     </row>
-    <row r="1693" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="1693" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1693" s="9" t="s">
         <v>179</v>
       </c>
@@ -33910,7 +34407,7 @@
       <c r="F1693" s="3"/>
       <c r="G1693" s="3"/>
     </row>
-    <row r="1694" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1694" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1694" s="9" t="s">
         <v>180</v>
       </c>
@@ -33920,7 +34417,7 @@
       <c r="F1694" s="3"/>
       <c r="G1694" s="3"/>
     </row>
-    <row r="1695" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1695" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1695" s="9" t="s">
         <v>1024</v>
       </c>
@@ -33930,7 +34427,7 @@
       <c r="F1695" s="3"/>
       <c r="G1695" s="3"/>
     </row>
-    <row r="1696" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="1696" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1696" s="9" t="s">
         <v>1040</v>
       </c>
@@ -33940,7 +34437,7 @@
       <c r="F1696" s="3"/>
       <c r="G1696" s="3"/>
     </row>
-    <row r="1697" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="1697" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1697" s="9" t="s">
         <v>1043</v>
       </c>
@@ -33950,7 +34447,7 @@
       <c r="F1697" s="3"/>
       <c r="G1697" s="3"/>
     </row>
-    <row r="1698" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1698" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1698" s="9" t="s">
         <v>1042</v>
       </c>
@@ -33960,7 +34457,7 @@
       <c r="F1698" s="3"/>
       <c r="G1698" s="3"/>
     </row>
-    <row r="1699" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1699" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1699" s="9" t="s">
         <v>1041</v>
       </c>
@@ -33970,7 +34467,7 @@
       <c r="F1699" s="3"/>
       <c r="G1699" s="3"/>
     </row>
-    <row r="1700" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="1700" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1700" s="9" t="s">
         <v>1048</v>
       </c>
@@ -33986,7 +34483,7 @@
       <c r="F1700" s="3"/>
       <c r="G1700" s="3"/>
     </row>
-    <row r="1701" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="1701" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1701" s="9" t="s">
         <v>166</v>
       </c>
@@ -33996,7 +34493,7 @@
       <c r="F1701" s="3"/>
       <c r="G1701" s="3"/>
     </row>
-    <row r="1702" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1702" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1702" s="3" t="s">
         <v>1052</v>
       </c>
@@ -34006,7 +34503,7 @@
       <c r="F1702" s="3"/>
       <c r="G1702" s="3"/>
     </row>
-    <row r="1703" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="1703" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1703" s="9" t="s">
         <v>1051</v>
       </c>
@@ -34016,7 +34513,7 @@
       <c r="F1703" s="3"/>
       <c r="G1703" s="3"/>
     </row>
-    <row r="1704" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="1704" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1704" s="9" t="s">
         <v>167</v>
       </c>
@@ -34026,7 +34523,7 @@
       <c r="F1704" s="3"/>
       <c r="G1704" s="3"/>
     </row>
-    <row r="1705" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1705" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1705" s="9" t="s">
         <v>1050</v>
       </c>
@@ -34036,7 +34533,7 @@
       <c r="F1705" s="3"/>
       <c r="G1705" s="3"/>
     </row>
-    <row r="1706" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1706" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1706" s="9" t="s">
         <v>168</v>
       </c>
@@ -34046,7 +34543,7 @@
       <c r="F1706" s="3"/>
       <c r="G1706" s="3"/>
     </row>
-    <row r="1707" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1707" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1707" s="9" t="s">
         <v>1049</v>
       </c>
@@ -34056,7 +34553,7 @@
       <c r="F1707" s="3"/>
       <c r="G1707" s="3"/>
     </row>
-    <row r="1708" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1708" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1708" s="9" t="s">
         <v>1016</v>
       </c>
@@ -34066,7 +34563,7 @@
       <c r="F1708" s="3"/>
       <c r="G1708" s="3"/>
     </row>
-    <row r="1709" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="1709" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1709" s="9" t="s">
         <v>2343</v>
       </c>
@@ -34077,7 +34574,7 @@
       <c r="F1709" s="3"/>
       <c r="G1709" s="3"/>
     </row>
-    <row r="1710" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="1710" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1710" s="9" t="s">
         <v>2350</v>
       </c>
@@ -34090,7 +34587,7 @@
       <c r="F1710" s="3"/>
       <c r="G1710" s="3"/>
     </row>
-    <row r="1711" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="1711" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1711" s="9" t="s">
         <v>2352</v>
       </c>
@@ -34103,7 +34600,7 @@
       <c r="F1711" s="3"/>
       <c r="G1711" s="3"/>
     </row>
-    <row r="1712" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="1712" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1712" s="9" t="s">
         <v>2344</v>
       </c>
@@ -34114,7 +34611,7 @@
       <c r="F1712" s="3"/>
       <c r="G1712" s="3"/>
     </row>
-    <row r="1713" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="1713" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1713" s="9" t="s">
         <v>2348</v>
       </c>
@@ -34125,7 +34622,7 @@
       <c r="F1713" s="3"/>
       <c r="G1713" s="3"/>
     </row>
-    <row r="1714" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="1714" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1714" s="9" t="s">
         <v>2347</v>
       </c>
@@ -34136,7 +34633,7 @@
       <c r="F1714" s="3"/>
       <c r="G1714" s="3"/>
     </row>
-    <row r="1715" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="1715" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1715" s="9" t="s">
         <v>2342</v>
       </c>
@@ -34149,7 +34646,7 @@
       <c r="F1715" s="3"/>
       <c r="G1715" s="3"/>
     </row>
-    <row r="1716" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="1716" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1716" s="9" t="s">
         <v>2349</v>
       </c>
@@ -34162,7 +34659,7 @@
       <c r="F1716" s="3"/>
       <c r="G1716" s="3"/>
     </row>
-    <row r="1717" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="1717" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1717" s="9" t="s">
         <v>2345</v>
       </c>
@@ -34173,7 +34670,7 @@
       <c r="F1717" s="3"/>
       <c r="G1717" s="3"/>
     </row>
-    <row r="1718" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="1718" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1718" s="9" t="s">
         <v>2351</v>
       </c>
@@ -34186,7 +34683,7 @@
       <c r="F1718" s="3"/>
       <c r="G1718" s="3"/>
     </row>
-    <row r="1719" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="1719" spans="1:7" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1719" s="9" t="s">
         <v>2341</v>
       </c>
@@ -34199,7 +34696,7 @@
       <c r="F1719" s="3"/>
       <c r="G1719" s="3"/>
     </row>
-    <row r="1720" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="1720" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1720" s="9" t="s">
         <v>2346</v>
       </c>
@@ -34210,7 +34707,7 @@
       <c r="F1720" s="3"/>
       <c r="G1720" s="3"/>
     </row>
-    <row r="1721" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1721" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1721" s="3" t="s">
         <v>2855</v>
       </c>
@@ -34221,7 +34718,7 @@
       <c r="F1721" s="3"/>
       <c r="G1721" s="3"/>
     </row>
-    <row r="1722" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1722" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1722" s="3" t="s">
         <v>2861</v>
       </c>
@@ -34232,7 +34729,7 @@
       <c r="F1722" s="3"/>
       <c r="G1722" s="3"/>
     </row>
-    <row r="1723" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1723" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1723" s="3" t="s">
         <v>2863</v>
       </c>
@@ -34243,7 +34740,7 @@
       <c r="F1723" s="3"/>
       <c r="G1723" s="3"/>
     </row>
-    <row r="1724" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1724" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1724" s="3" t="s">
         <v>2856</v>
       </c>
@@ -34254,7 +34751,7 @@
       <c r="F1724" s="3"/>
       <c r="G1724" s="3"/>
     </row>
-    <row r="1725" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1725" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1725" s="3" t="s">
         <v>2860</v>
       </c>
@@ -34265,7 +34762,7 @@
       <c r="F1725" s="3"/>
       <c r="G1725" s="3"/>
     </row>
-    <row r="1726" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1726" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1726" s="3" t="s">
         <v>2859</v>
       </c>
@@ -34276,7 +34773,7 @@
       <c r="F1726" s="3"/>
       <c r="G1726" s="3"/>
     </row>
-    <row r="1727" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1727" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1727" s="3" t="s">
         <v>2854</v>
       </c>
@@ -34287,7 +34784,7 @@
       <c r="F1727" s="3"/>
       <c r="G1727" s="3"/>
     </row>
-    <row r="1728" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1728" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1728" s="3" t="s">
         <v>1533</v>
       </c>
@@ -34298,7 +34795,7 @@
       <c r="F1728" s="3"/>
       <c r="G1728" s="3"/>
     </row>
-    <row r="1729" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1729" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1729" s="3" t="s">
         <v>2857</v>
       </c>
@@ -34309,7 +34806,7 @@
       <c r="F1729" s="3"/>
       <c r="G1729" s="3"/>
     </row>
-    <row r="1730" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1730" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1730" s="3" t="s">
         <v>2862</v>
       </c>
@@ -34320,7 +34817,7 @@
       <c r="F1730" s="3"/>
       <c r="G1730" s="3"/>
     </row>
-    <row r="1731" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1731" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1731" s="3" t="s">
         <v>2853</v>
       </c>
@@ -34331,7 +34828,7 @@
       <c r="F1731" s="3"/>
       <c r="G1731" s="3"/>
     </row>
-    <row r="1732" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1732" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1732" s="3" t="s">
         <v>2858</v>
       </c>
@@ -34342,7 +34839,7 @@
       <c r="F1732" s="3"/>
       <c r="G1732" s="3"/>
     </row>
-    <row r="1733" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1733" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1733" s="3" t="s">
         <v>2807</v>
       </c>
@@ -34353,7 +34850,7 @@
       <c r="F1733" s="3"/>
       <c r="G1733" s="3"/>
     </row>
-    <row r="1734" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1734" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1734" s="3" t="s">
         <v>2814</v>
       </c>
@@ -34364,7 +34861,7 @@
       <c r="F1734" s="3"/>
       <c r="G1734" s="3"/>
     </row>
-    <row r="1735" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1735" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1735" s="3" t="s">
         <v>2816</v>
       </c>
@@ -34375,7 +34872,7 @@
       <c r="F1735" s="3"/>
       <c r="G1735" s="3"/>
     </row>
-    <row r="1736" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1736" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1736" s="3" t="s">
         <v>2808</v>
       </c>
@@ -34386,7 +34883,7 @@
       <c r="F1736" s="3"/>
       <c r="G1736" s="3"/>
     </row>
-    <row r="1737" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1737" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1737" s="3" t="s">
         <v>2812</v>
       </c>
@@ -34397,7 +34894,7 @@
       <c r="F1737" s="3"/>
       <c r="G1737" s="3"/>
     </row>
-    <row r="1738" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1738" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1738" s="3" t="s">
         <v>2811</v>
       </c>
@@ -34408,7 +34905,7 @@
       <c r="F1738" s="3"/>
       <c r="G1738" s="3"/>
     </row>
-    <row r="1739" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1739" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1739" s="3" t="s">
         <v>2806</v>
       </c>
@@ -34419,7 +34916,7 @@
       <c r="F1739" s="3"/>
       <c r="G1739" s="3"/>
     </row>
-    <row r="1740" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1740" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1740" s="3" t="s">
         <v>2813</v>
       </c>
@@ -34430,7 +34927,7 @@
       <c r="F1740" s="3"/>
       <c r="G1740" s="3"/>
     </row>
-    <row r="1741" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1741" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1741" s="3" t="s">
         <v>2809</v>
       </c>
@@ -34441,7 +34938,7 @@
       <c r="F1741" s="3"/>
       <c r="G1741" s="3"/>
     </row>
-    <row r="1742" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1742" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1742" s="3" t="s">
         <v>2815</v>
       </c>
@@ -34452,7 +34949,7 @@
       <c r="F1742" s="3"/>
       <c r="G1742" s="3"/>
     </row>
-    <row r="1743" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1743" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1743" s="3" t="s">
         <v>2805</v>
       </c>
@@ -34463,7 +34960,7 @@
       <c r="F1743" s="3"/>
       <c r="G1743" s="3"/>
     </row>
-    <row r="1744" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1744" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1744" s="3" t="s">
         <v>2810</v>
       </c>
@@ -34474,7 +34971,7 @@
       <c r="F1744" s="3"/>
       <c r="G1744" s="3"/>
     </row>
-    <row r="1745" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1745" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1745" s="3" t="s">
         <v>2902</v>
       </c>
@@ -34485,7 +34982,7 @@
       <c r="F1745" s="3"/>
       <c r="G1745" s="3"/>
     </row>
-    <row r="1746" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1746" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1746" s="3" t="s">
         <v>2909</v>
       </c>
@@ -34496,7 +34993,7 @@
       <c r="F1746" s="3"/>
       <c r="G1746" s="3"/>
     </row>
-    <row r="1747" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1747" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1747" s="3" t="s">
         <v>2911</v>
       </c>
@@ -34507,7 +35004,7 @@
       <c r="F1747" s="3"/>
       <c r="G1747" s="3"/>
     </row>
-    <row r="1748" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1748" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1748" s="3" t="s">
         <v>2903</v>
       </c>
@@ -34518,7 +35015,7 @@
       <c r="F1748" s="3"/>
       <c r="G1748" s="3"/>
     </row>
-    <row r="1749" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1749" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1749" s="3" t="s">
         <v>2907</v>
       </c>
@@ -34529,7 +35026,7 @@
       <c r="F1749" s="3"/>
       <c r="G1749" s="3"/>
     </row>
-    <row r="1750" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1750" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1750" s="3" t="s">
         <v>2906</v>
       </c>
@@ -34540,7 +35037,7 @@
       <c r="F1750" s="3"/>
       <c r="G1750" s="3"/>
     </row>
-    <row r="1751" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1751" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1751" s="3" t="s">
         <v>2901</v>
       </c>
@@ -34551,7 +35048,7 @@
       <c r="F1751" s="3"/>
       <c r="G1751" s="3"/>
     </row>
-    <row r="1752" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1752" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1752" s="3" t="s">
         <v>2908</v>
       </c>
@@ -34562,7 +35059,7 @@
       <c r="F1752" s="3"/>
       <c r="G1752" s="3"/>
     </row>
-    <row r="1753" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1753" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1753" s="3" t="s">
         <v>2904</v>
       </c>
@@ -34573,7 +35070,7 @@
       <c r="F1753" s="3"/>
       <c r="G1753" s="3"/>
     </row>
-    <row r="1754" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1754" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1754" s="3" t="s">
         <v>2910</v>
       </c>
@@ -34584,7 +35081,7 @@
       <c r="F1754" s="3"/>
       <c r="G1754" s="3"/>
     </row>
-    <row r="1755" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1755" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1755" s="3" t="s">
         <v>2900</v>
       </c>
@@ -34595,7 +35092,7 @@
       <c r="F1755" s="3"/>
       <c r="G1755" s="3"/>
     </row>
-    <row r="1756" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1756" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1756" s="3" t="s">
         <v>2905</v>
       </c>
@@ -34606,7 +35103,7 @@
       <c r="F1756" s="3"/>
       <c r="G1756" s="3"/>
     </row>
-    <row r="1757" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1757" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1757" s="3" t="s">
         <v>2831</v>
       </c>
@@ -34617,7 +35114,7 @@
       <c r="F1757" s="3"/>
       <c r="G1757" s="3"/>
     </row>
-    <row r="1758" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1758" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1758" s="3" t="s">
         <v>2838</v>
       </c>
@@ -34628,7 +35125,7 @@
       <c r="F1758" s="3"/>
       <c r="G1758" s="3"/>
     </row>
-    <row r="1759" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1759" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1759" s="3" t="s">
         <v>2840</v>
       </c>
@@ -34639,7 +35136,7 @@
       <c r="F1759" s="3"/>
       <c r="G1759" s="3"/>
     </row>
-    <row r="1760" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1760" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1760" s="3" t="s">
         <v>2832</v>
       </c>
@@ -34650,7 +35147,7 @@
       <c r="F1760" s="3"/>
       <c r="G1760" s="3"/>
     </row>
-    <row r="1761" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1761" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1761" s="3" t="s">
         <v>2836</v>
       </c>
@@ -34661,7 +35158,7 @@
       <c r="F1761" s="3"/>
       <c r="G1761" s="3"/>
     </row>
-    <row r="1762" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1762" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1762" s="3" t="s">
         <v>2835</v>
       </c>
@@ -34672,7 +35169,7 @@
       <c r="F1762" s="3"/>
       <c r="G1762" s="3"/>
     </row>
-    <row r="1763" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1763" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1763" s="3" t="s">
         <v>2830</v>
       </c>
@@ -34683,7 +35180,7 @@
       <c r="F1763" s="3"/>
       <c r="G1763" s="3"/>
     </row>
-    <row r="1764" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1764" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1764" s="3" t="s">
         <v>2837</v>
       </c>
@@ -34694,7 +35191,7 @@
       <c r="F1764" s="3"/>
       <c r="G1764" s="3"/>
     </row>
-    <row r="1765" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1765" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1765" s="3" t="s">
         <v>2833</v>
       </c>
@@ -34705,7 +35202,7 @@
       <c r="F1765" s="3"/>
       <c r="G1765" s="3"/>
     </row>
-    <row r="1766" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1766" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1766" s="3" t="s">
         <v>2839</v>
       </c>
@@ -34716,7 +35213,7 @@
       <c r="F1766" s="3"/>
       <c r="G1766" s="3"/>
     </row>
-    <row r="1767" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1767" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1767" s="3" t="s">
         <v>2829</v>
       </c>
@@ -34727,7 +35224,7 @@
       <c r="F1767" s="3"/>
       <c r="G1767" s="3"/>
     </row>
-    <row r="1768" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1768" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1768" s="3" t="s">
         <v>2834</v>
       </c>
@@ -34738,7 +35235,7 @@
       <c r="F1768" s="3"/>
       <c r="G1768" s="3"/>
     </row>
-    <row r="1769" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1769" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1769" s="3" t="s">
         <v>2843</v>
       </c>
@@ -34749,7 +35246,7 @@
       <c r="F1769" s="3"/>
       <c r="G1769" s="3"/>
     </row>
-    <row r="1770" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1770" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1770" s="3" t="s">
         <v>2850</v>
       </c>
@@ -34760,7 +35257,7 @@
       <c r="F1770" s="3"/>
       <c r="G1770" s="3"/>
     </row>
-    <row r="1771" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1771" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1771" s="3" t="s">
         <v>2852</v>
       </c>
@@ -34771,7 +35268,7 @@
       <c r="F1771" s="3"/>
       <c r="G1771" s="3"/>
     </row>
-    <row r="1772" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1772" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1772" s="3" t="s">
         <v>2844</v>
       </c>
@@ -34782,7 +35279,7 @@
       <c r="F1772" s="3"/>
       <c r="G1772" s="3"/>
     </row>
-    <row r="1773" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1773" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1773" s="3" t="s">
         <v>2848</v>
       </c>
@@ -34793,7 +35290,7 @@
       <c r="F1773" s="3"/>
       <c r="G1773" s="3"/>
     </row>
-    <row r="1774" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1774" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1774" s="3" t="s">
         <v>2847</v>
       </c>
@@ -34804,7 +35301,7 @@
       <c r="F1774" s="3"/>
       <c r="G1774" s="3"/>
     </row>
-    <row r="1775" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1775" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1775" s="3" t="s">
         <v>2842</v>
       </c>
@@ -34815,7 +35312,7 @@
       <c r="F1775" s="3"/>
       <c r="G1775" s="3"/>
     </row>
-    <row r="1776" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1776" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1776" s="3" t="s">
         <v>2849</v>
       </c>
@@ -34826,7 +35323,7 @@
       <c r="F1776" s="3"/>
       <c r="G1776" s="3"/>
     </row>
-    <row r="1777" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1777" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1777" s="3" t="s">
         <v>2845</v>
       </c>
@@ -34837,7 +35334,7 @@
       <c r="F1777" s="3"/>
       <c r="G1777" s="3"/>
     </row>
-    <row r="1778" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1778" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1778" s="3" t="s">
         <v>2851</v>
       </c>
@@ -34848,7 +35345,7 @@
       <c r="F1778" s="3"/>
       <c r="G1778" s="3"/>
     </row>
-    <row r="1779" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1779" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1779" s="3" t="s">
         <v>2841</v>
       </c>
@@ -34859,7 +35356,7 @@
       <c r="F1779" s="3"/>
       <c r="G1779" s="3"/>
     </row>
-    <row r="1780" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1780" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1780" s="3" t="s">
         <v>2846</v>
       </c>
@@ -34870,7 +35367,7 @@
       <c r="F1780" s="3"/>
       <c r="G1780" s="3"/>
     </row>
-    <row r="1781" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1781" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1781" s="3" t="s">
         <v>2890</v>
       </c>
@@ -34881,7 +35378,7 @@
       <c r="F1781" s="3"/>
       <c r="G1781" s="3"/>
     </row>
-    <row r="1782" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1782" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1782" s="3" t="s">
         <v>2897</v>
       </c>
@@ -34892,7 +35389,7 @@
       <c r="F1782" s="3"/>
       <c r="G1782" s="3"/>
     </row>
-    <row r="1783" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1783" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1783" s="3" t="s">
         <v>2899</v>
       </c>
@@ -34903,7 +35400,7 @@
       <c r="F1783" s="3"/>
       <c r="G1783" s="3"/>
     </row>
-    <row r="1784" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1784" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1784" s="3" t="s">
         <v>2891</v>
       </c>
@@ -34914,7 +35411,7 @@
       <c r="F1784" s="3"/>
       <c r="G1784" s="3"/>
     </row>
-    <row r="1785" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1785" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1785" s="3" t="s">
         <v>2895</v>
       </c>
@@ -34925,7 +35422,7 @@
       <c r="F1785" s="3"/>
       <c r="G1785" s="3"/>
     </row>
-    <row r="1786" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1786" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1786" s="3" t="s">
         <v>2894</v>
       </c>
@@ -34936,7 +35433,7 @@
       <c r="F1786" s="3"/>
       <c r="G1786" s="3"/>
     </row>
-    <row r="1787" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1787" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1787" s="3" t="s">
         <v>2889</v>
       </c>
@@ -34947,7 +35444,7 @@
       <c r="F1787" s="3"/>
       <c r="G1787" s="3"/>
     </row>
-    <row r="1788" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1788" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1788" s="3" t="s">
         <v>2896</v>
       </c>
@@ -34958,7 +35455,7 @@
       <c r="F1788" s="3"/>
       <c r="G1788" s="3"/>
     </row>
-    <row r="1789" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1789" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1789" s="3" t="s">
         <v>2892</v>
       </c>
@@ -34969,7 +35466,7 @@
       <c r="F1789" s="3"/>
       <c r="G1789" s="3"/>
     </row>
-    <row r="1790" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1790" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1790" s="3" t="s">
         <v>2898</v>
       </c>
@@ -34980,7 +35477,7 @@
       <c r="F1790" s="3"/>
       <c r="G1790" s="3"/>
     </row>
-    <row r="1791" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1791" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1791" s="3" t="s">
         <v>2888</v>
       </c>
@@ -34991,7 +35488,7 @@
       <c r="F1791" s="3"/>
       <c r="G1791" s="3"/>
     </row>
-    <row r="1792" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1792" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1792" s="3" t="s">
         <v>2893</v>
       </c>
@@ -35002,7 +35499,7 @@
       <c r="F1792" s="3"/>
       <c r="G1792" s="3"/>
     </row>
-    <row r="1793" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1793" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1793" s="3" t="s">
         <v>2795</v>
       </c>
@@ -35013,7 +35510,7 @@
       <c r="F1793" s="3"/>
       <c r="G1793" s="3"/>
     </row>
-    <row r="1794" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1794" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1794" s="3" t="s">
         <v>2802</v>
       </c>
@@ -35024,7 +35521,7 @@
       <c r="F1794" s="3"/>
       <c r="G1794" s="3"/>
     </row>
-    <row r="1795" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1795" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1795" s="3" t="s">
         <v>2804</v>
       </c>
@@ -35035,7 +35532,7 @@
       <c r="F1795" s="3"/>
       <c r="G1795" s="3"/>
     </row>
-    <row r="1796" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1796" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1796" s="3" t="s">
         <v>2796</v>
       </c>
@@ -35046,7 +35543,7 @@
       <c r="F1796" s="3"/>
       <c r="G1796" s="3"/>
     </row>
-    <row r="1797" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1797" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1797" s="3" t="s">
         <v>2800</v>
       </c>
@@ -35057,7 +35554,7 @@
       <c r="F1797" s="3"/>
       <c r="G1797" s="3"/>
     </row>
-    <row r="1798" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1798" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1798" s="3" t="s">
         <v>2799</v>
       </c>
@@ -35068,7 +35565,7 @@
       <c r="F1798" s="3"/>
       <c r="G1798" s="3"/>
     </row>
-    <row r="1799" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1799" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1799" s="3" t="s">
         <v>2794</v>
       </c>
@@ -35079,7 +35576,7 @@
       <c r="F1799" s="3"/>
       <c r="G1799" s="3"/>
     </row>
-    <row r="1800" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1800" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1800" s="3" t="s">
         <v>2801</v>
       </c>
@@ -35090,7 +35587,7 @@
       <c r="F1800" s="3"/>
       <c r="G1800" s="3"/>
     </row>
-    <row r="1801" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1801" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1801" s="3" t="s">
         <v>2797</v>
       </c>
@@ -35101,7 +35598,7 @@
       <c r="F1801" s="3"/>
       <c r="G1801" s="3"/>
     </row>
-    <row r="1802" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1802" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1802" s="3" t="s">
         <v>2803</v>
       </c>
@@ -35112,7 +35609,7 @@
       <c r="F1802" s="3"/>
       <c r="G1802" s="3"/>
     </row>
-    <row r="1803" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1803" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1803" s="3" t="s">
         <v>2793</v>
       </c>
@@ -35123,7 +35620,7 @@
       <c r="F1803" s="3"/>
       <c r="G1803" s="3"/>
     </row>
-    <row r="1804" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1804" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1804" s="3" t="s">
         <v>2798</v>
       </c>
@@ -35134,7 +35631,7 @@
       <c r="F1804" s="3"/>
       <c r="G1804" s="3"/>
     </row>
-    <row r="1805" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1805" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1805" s="3" t="s">
         <v>2878</v>
       </c>
@@ -35145,7 +35642,7 @@
       <c r="F1805" s="3"/>
       <c r="G1805" s="3"/>
     </row>
-    <row r="1806" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1806" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1806" s="3" t="s">
         <v>2885</v>
       </c>
@@ -35156,7 +35653,7 @@
       <c r="F1806" s="3"/>
       <c r="G1806" s="3"/>
     </row>
-    <row r="1807" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1807" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1807" s="3" t="s">
         <v>2887</v>
       </c>
@@ -35167,7 +35664,7 @@
       <c r="F1807" s="3"/>
       <c r="G1807" s="3"/>
     </row>
-    <row r="1808" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1808" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1808" s="3" t="s">
         <v>2879</v>
       </c>
@@ -35178,7 +35675,7 @@
       <c r="F1808" s="3"/>
       <c r="G1808" s="3"/>
     </row>
-    <row r="1809" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1809" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1809" s="3" t="s">
         <v>2883</v>
       </c>
@@ -35189,7 +35686,7 @@
       <c r="F1809" s="3"/>
       <c r="G1809" s="3"/>
     </row>
-    <row r="1810" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1810" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1810" s="3" t="s">
         <v>2882</v>
       </c>
@@ -35200,7 +35697,7 @@
       <c r="F1810" s="3"/>
       <c r="G1810" s="3"/>
     </row>
-    <row r="1811" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1811" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1811" s="3" t="s">
         <v>2877</v>
       </c>
@@ -35211,7 +35708,7 @@
       <c r="F1811" s="3"/>
       <c r="G1811" s="3"/>
     </row>
-    <row r="1812" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1812" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1812" s="3" t="s">
         <v>2884</v>
       </c>
@@ -35222,7 +35719,7 @@
       <c r="F1812" s="3"/>
       <c r="G1812" s="3"/>
     </row>
-    <row r="1813" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1813" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1813" s="3" t="s">
         <v>2880</v>
       </c>
@@ -35233,7 +35730,7 @@
       <c r="F1813" s="3"/>
       <c r="G1813" s="3"/>
     </row>
-    <row r="1814" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1814" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1814" s="3" t="s">
         <v>2886</v>
       </c>
@@ -35244,7 +35741,7 @@
       <c r="F1814" s="3"/>
       <c r="G1814" s="3"/>
     </row>
-    <row r="1815" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1815" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1815" s="3" t="s">
         <v>2876</v>
       </c>
@@ -35255,7 +35752,7 @@
       <c r="F1815" s="3"/>
       <c r="G1815" s="3"/>
     </row>
-    <row r="1816" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1816" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1816" s="3" t="s">
         <v>2881</v>
       </c>
@@ -35266,7 +35763,7 @@
       <c r="F1816" s="3"/>
       <c r="G1816" s="3"/>
     </row>
-    <row r="1817" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1817" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1817" s="3" t="s">
         <v>2819</v>
       </c>
@@ -35277,7 +35774,7 @@
       <c r="F1817" s="3"/>
       <c r="G1817" s="3"/>
     </row>
-    <row r="1818" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1818" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1818" s="3" t="s">
         <v>2826</v>
       </c>
@@ -35288,7 +35785,7 @@
       <c r="F1818" s="3"/>
       <c r="G1818" s="3"/>
     </row>
-    <row r="1819" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1819" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1819" s="3" t="s">
         <v>2828</v>
       </c>
@@ -35299,7 +35796,7 @@
       <c r="F1819" s="3"/>
       <c r="G1819" s="3"/>
     </row>
-    <row r="1820" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1820" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1820" s="3" t="s">
         <v>2820</v>
       </c>
@@ -35310,7 +35807,7 @@
       <c r="F1820" s="3"/>
       <c r="G1820" s="3"/>
     </row>
-    <row r="1821" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1821" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1821" s="3" t="s">
         <v>2824</v>
       </c>
@@ -35321,7 +35818,7 @@
       <c r="F1821" s="3"/>
       <c r="G1821" s="3"/>
     </row>
-    <row r="1822" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1822" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1822" s="3" t="s">
         <v>2823</v>
       </c>
@@ -35332,7 +35829,7 @@
       <c r="F1822" s="3"/>
       <c r="G1822" s="3"/>
     </row>
-    <row r="1823" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1823" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1823" s="3" t="s">
         <v>2818</v>
       </c>
@@ -35343,7 +35840,7 @@
       <c r="F1823" s="3"/>
       <c r="G1823" s="3"/>
     </row>
-    <row r="1824" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1824" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1824" s="3" t="s">
         <v>2825</v>
       </c>
@@ -35354,7 +35851,7 @@
       <c r="F1824" s="3"/>
       <c r="G1824" s="3"/>
     </row>
-    <row r="1825" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1825" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1825" s="3" t="s">
         <v>2821</v>
       </c>
@@ -35365,7 +35862,7 @@
       <c r="F1825" s="3"/>
       <c r="G1825" s="3"/>
     </row>
-    <row r="1826" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1826" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1826" s="3" t="s">
         <v>2827</v>
       </c>
@@ -35376,7 +35873,7 @@
       <c r="F1826" s="3"/>
       <c r="G1826" s="3"/>
     </row>
-    <row r="1827" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1827" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1827" s="3" t="s">
         <v>2817</v>
       </c>
@@ -35387,7 +35884,7 @@
       <c r="F1827" s="3"/>
       <c r="G1827" s="3"/>
     </row>
-    <row r="1828" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1828" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1828" s="3" t="s">
         <v>2822</v>
       </c>
@@ -35398,7 +35895,7 @@
       <c r="F1828" s="3"/>
       <c r="G1828" s="3"/>
     </row>
-    <row r="1829" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1829" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1829" s="3" t="s">
         <v>2866</v>
       </c>
@@ -35409,7 +35906,7 @@
       <c r="F1829" s="3"/>
       <c r="G1829" s="3"/>
     </row>
-    <row r="1830" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1830" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1830" s="3" t="s">
         <v>2873</v>
       </c>
@@ -35420,7 +35917,7 @@
       <c r="F1830" s="3"/>
       <c r="G1830" s="3"/>
     </row>
-    <row r="1831" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1831" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1831" s="3" t="s">
         <v>2875</v>
       </c>
@@ -35431,7 +35928,7 @@
       <c r="F1831" s="3"/>
       <c r="G1831" s="3"/>
     </row>
-    <row r="1832" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1832" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1832" s="3" t="s">
         <v>2867</v>
       </c>
@@ -35442,7 +35939,7 @@
       <c r="F1832" s="3"/>
       <c r="G1832" s="3"/>
     </row>
-    <row r="1833" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1833" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1833" s="3" t="s">
         <v>2871</v>
       </c>
@@ -35453,7 +35950,7 @@
       <c r="F1833" s="3"/>
       <c r="G1833" s="3"/>
     </row>
-    <row r="1834" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1834" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1834" s="3" t="s">
         <v>2870</v>
       </c>
@@ -35464,7 +35961,7 @@
       <c r="F1834" s="3"/>
       <c r="G1834" s="3"/>
     </row>
-    <row r="1835" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1835" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1835" s="3" t="s">
         <v>2865</v>
       </c>
@@ -35475,7 +35972,7 @@
       <c r="F1835" s="3"/>
       <c r="G1835" s="3"/>
     </row>
-    <row r="1836" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1836" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1836" s="3" t="s">
         <v>2872</v>
       </c>
@@ -35486,7 +35983,7 @@
       <c r="F1836" s="3"/>
       <c r="G1836" s="3"/>
     </row>
-    <row r="1837" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1837" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1837" s="3" t="s">
         <v>2868</v>
       </c>
@@ -35497,7 +35994,7 @@
       <c r="F1837" s="3"/>
       <c r="G1837" s="3"/>
     </row>
-    <row r="1838" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1838" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1838" s="3" t="s">
         <v>2874</v>
       </c>
@@ -35508,7 +36005,7 @@
       <c r="F1838" s="3"/>
       <c r="G1838" s="3"/>
     </row>
-    <row r="1839" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1839" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1839" s="3" t="s">
         <v>2864</v>
       </c>
@@ -35519,7 +36016,7 @@
       <c r="F1839" s="3"/>
       <c r="G1839" s="3"/>
     </row>
-    <row r="1840" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1840" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1840" s="3" t="s">
         <v>2869</v>
       </c>
@@ -35530,7 +36027,7 @@
       <c r="F1840" s="3"/>
       <c r="G1840" s="3"/>
     </row>
-    <row r="1841" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1841" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1841" s="3" t="s">
         <v>2783</v>
       </c>
@@ -35541,7 +36038,7 @@
       <c r="F1841" s="3"/>
       <c r="G1841" s="3"/>
     </row>
-    <row r="1842" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1842" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1842" s="3" t="s">
         <v>2790</v>
       </c>
@@ -35552,7 +36049,7 @@
       <c r="F1842" s="3"/>
       <c r="G1842" s="3"/>
     </row>
-    <row r="1843" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1843" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1843" s="3" t="s">
         <v>2792</v>
       </c>
@@ -35563,7 +36060,7 @@
       <c r="F1843" s="3"/>
       <c r="G1843" s="3"/>
     </row>
-    <row r="1844" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1844" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1844" s="3" t="s">
         <v>2784</v>
       </c>
@@ -35574,7 +36071,7 @@
       <c r="F1844" s="3"/>
       <c r="G1844" s="3"/>
     </row>
-    <row r="1845" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1845" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1845" s="3" t="s">
         <v>2788</v>
       </c>
@@ -35585,7 +36082,7 @@
       <c r="F1845" s="3"/>
       <c r="G1845" s="3"/>
     </row>
-    <row r="1846" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1846" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1846" s="3" t="s">
         <v>2787</v>
       </c>
@@ -35596,7 +36093,7 @@
       <c r="F1846" s="3"/>
       <c r="G1846" s="3"/>
     </row>
-    <row r="1847" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1847" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1847" s="3" t="s">
         <v>2782</v>
       </c>
@@ -35607,7 +36104,7 @@
       <c r="F1847" s="3"/>
       <c r="G1847" s="3"/>
     </row>
-    <row r="1848" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1848" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1848" s="3" t="s">
         <v>2789</v>
       </c>
@@ -35618,7 +36115,7 @@
       <c r="F1848" s="3"/>
       <c r="G1848" s="3"/>
     </row>
-    <row r="1849" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1849" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1849" s="3" t="s">
         <v>2785</v>
       </c>
@@ -35629,7 +36126,7 @@
       <c r="F1849" s="3"/>
       <c r="G1849" s="3"/>
     </row>
-    <row r="1850" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1850" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1850" s="3" t="s">
         <v>2791</v>
       </c>
@@ -35640,7 +36137,7 @@
       <c r="F1850" s="3"/>
       <c r="G1850" s="3"/>
     </row>
-    <row r="1851" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1851" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1851" s="3" t="s">
         <v>2781</v>
       </c>
@@ -35651,7 +36148,7 @@
       <c r="F1851" s="3"/>
       <c r="G1851" s="3"/>
     </row>
-    <row r="1852" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1852" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1852" s="3" t="s">
         <v>2786</v>
       </c>
@@ -35662,7 +36159,7 @@
       <c r="F1852" s="3"/>
       <c r="G1852" s="3"/>
     </row>
-    <row r="1853" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1853" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1853" s="3" t="s">
         <v>1077</v>
       </c>
@@ -38822,650 +39319,673 @@
       <c r="F2136" s="3"/>
       <c r="G2136" s="3"/>
     </row>
-    <row r="2137" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2137" s="3" t="s">
+    <row r="2137" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2137" s="9" t="s">
         <v>1173</v>
       </c>
       <c r="B2137" s="3" t="s">
-        <v>1173</v>
+        <v>4805</v>
       </c>
       <c r="C2137" s="3"/>
       <c r="F2137" s="3"/>
       <c r="G2137" s="3"/>
     </row>
     <row r="2138" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2138" s="3" t="s">
+      <c r="A2138" s="9" t="s">
         <v>1174</v>
       </c>
       <c r="B2138" s="3" t="s">
-        <v>1174</v>
+        <v>4806</v>
       </c>
       <c r="C2138" s="3"/>
       <c r="F2138" s="3"/>
       <c r="G2138" s="3"/>
     </row>
-    <row r="2139" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2139" s="3" t="s">
+    <row r="2139" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2139" s="9" t="s">
         <v>1175</v>
       </c>
       <c r="B2139" s="3" t="s">
-        <v>1175</v>
+        <v>4805</v>
       </c>
       <c r="C2139" s="3"/>
       <c r="F2139" s="3"/>
       <c r="G2139" s="3"/>
     </row>
     <row r="2140" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2140" s="3" t="s">
+      <c r="A2140" s="9" t="s">
         <v>1176</v>
       </c>
       <c r="B2140" s="3" t="s">
-        <v>1176</v>
+        <v>4806</v>
       </c>
       <c r="C2140" s="3"/>
       <c r="F2140" s="3"/>
       <c r="G2140" s="3"/>
     </row>
-    <row r="2141" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2141" s="3" t="s">
+    <row r="2141" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2141" s="9" t="s">
         <v>257</v>
       </c>
       <c r="B2141" s="3" t="s">
-        <v>257</v>
+        <v>4810</v>
       </c>
       <c r="C2141" s="3"/>
       <c r="F2141" s="3"/>
       <c r="G2141" s="3"/>
     </row>
-    <row r="2142" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2142" s="3" t="s">
+    <row r="2142" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2142" s="9" t="s">
         <v>253</v>
       </c>
       <c r="B2142" s="3" t="s">
-        <v>253</v>
+        <v>4792</v>
       </c>
       <c r="C2142" s="3"/>
       <c r="F2142" s="3"/>
       <c r="G2142" s="3"/>
     </row>
     <row r="2143" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2143" s="3" t="s">
+      <c r="A2143" s="9" t="s">
         <v>254</v>
       </c>
       <c r="B2143" s="3" t="s">
-        <v>254</v>
+        <v>4794</v>
       </c>
       <c r="C2143" s="3"/>
       <c r="F2143" s="3"/>
       <c r="G2143" s="3"/>
     </row>
     <row r="2144" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2144" s="3" t="s">
+      <c r="A2144" s="9" t="s">
         <v>1177</v>
       </c>
       <c r="B2144" s="3" t="s">
-        <v>1177</v>
-      </c>
-      <c r="C2144" s="3"/>
+        <v>4793</v>
+      </c>
+      <c r="C2144" s="3" t="s">
+        <v>4804</v>
+      </c>
       <c r="F2144" s="3"/>
       <c r="G2144" s="3"/>
     </row>
-    <row r="2145" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2145" s="3" t="s">
+    <row r="2145" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2145" s="9" t="s">
         <v>202</v>
       </c>
       <c r="B2145" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C2145" s="3"/>
+        <v>4786</v>
+      </c>
       <c r="F2145" s="3"/>
       <c r="G2145" s="3"/>
     </row>
     <row r="2146" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2146" s="3" t="s">
+      <c r="A2146" s="9" t="s">
         <v>204</v>
       </c>
       <c r="B2146" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="C2146" s="3"/>
+        <v>4787</v>
+      </c>
+      <c r="C2146" s="10" t="s">
+        <v>4788</v>
+      </c>
       <c r="F2146" s="3"/>
       <c r="G2146" s="3"/>
     </row>
     <row r="2147" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2147" s="3" t="s">
+      <c r="A2147" s="9" t="s">
         <v>205</v>
       </c>
       <c r="B2147" s="3" t="s">
-        <v>205</v>
+        <v>4789</v>
       </c>
       <c r="C2147" s="3"/>
       <c r="F2147" s="3"/>
       <c r="G2147" s="3"/>
     </row>
-    <row r="2148" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2148" s="3" t="s">
+    <row r="2148" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2148" s="9" t="s">
         <v>203</v>
       </c>
       <c r="B2148" s="3" t="s">
-        <v>203</v>
+        <v>4787</v>
       </c>
       <c r="C2148" s="3"/>
       <c r="F2148" s="3"/>
       <c r="G2148" s="3"/>
     </row>
     <row r="2149" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2149" s="3" t="s">
+      <c r="A2149" s="9" t="s">
         <v>1166</v>
       </c>
       <c r="B2149" s="3" t="s">
-        <v>1166</v>
+        <v>4803</v>
       </c>
       <c r="C2149" s="3"/>
       <c r="F2149" s="3"/>
       <c r="G2149" s="3"/>
     </row>
-    <row r="2150" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2150" s="3" t="s">
+    <row r="2150" spans="1:7" ht="75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2150" s="9" t="s">
         <v>255</v>
       </c>
       <c r="B2150" s="3" t="s">
-        <v>255</v>
+        <v>4792</v>
       </c>
       <c r="C2150" s="3"/>
       <c r="F2150" s="3"/>
       <c r="G2150" s="3"/>
     </row>
     <row r="2151" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2151" s="3" t="s">
+      <c r="A2151" s="9" t="s">
         <v>256</v>
       </c>
       <c r="B2151" s="3" t="s">
-        <v>256</v>
+        <v>4794</v>
       </c>
       <c r="C2151" s="3"/>
       <c r="F2151" s="3"/>
       <c r="G2151" s="3"/>
     </row>
     <row r="2152" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2152" s="3" t="s">
+      <c r="A2152" s="9" t="s">
         <v>1178</v>
       </c>
       <c r="B2152" s="3" t="s">
-        <v>1178</v>
-      </c>
-      <c r="C2152" s="3"/>
+        <v>4793</v>
+      </c>
+      <c r="C2152" s="3" t="s">
+        <v>4804</v>
+      </c>
       <c r="F2152" s="3"/>
       <c r="G2152" s="3"/>
     </row>
-    <row r="2153" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2153" s="3" t="s">
+    <row r="2153" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2153" s="9" t="s">
         <v>197</v>
       </c>
       <c r="B2153" s="3" t="s">
-        <v>197</v>
+        <v>4786</v>
       </c>
       <c r="C2153" s="3"/>
       <c r="F2153" s="3"/>
       <c r="G2153" s="3"/>
     </row>
     <row r="2154" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2154" s="3" t="s">
+      <c r="A2154" s="9" t="s">
         <v>199</v>
       </c>
       <c r="B2154" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2154" s="3"/>
+        <v>4787</v>
+      </c>
+      <c r="C2154" s="10" t="s">
+        <v>4788</v>
+      </c>
       <c r="F2154" s="3"/>
       <c r="G2154" s="3"/>
     </row>
     <row r="2155" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2155" s="3" t="s">
+      <c r="A2155" s="9" t="s">
         <v>200</v>
       </c>
       <c r="B2155" s="3" t="s">
-        <v>200</v>
+        <v>4789</v>
       </c>
       <c r="C2155" s="3"/>
       <c r="F2155" s="3"/>
       <c r="G2155" s="3"/>
     </row>
-    <row r="2156" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2156" s="3" t="s">
+    <row r="2156" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2156" s="9" t="s">
         <v>198</v>
       </c>
       <c r="B2156" s="3" t="s">
-        <v>198</v>
+        <v>4787</v>
       </c>
       <c r="C2156" s="3"/>
       <c r="F2156" s="3"/>
       <c r="G2156" s="3"/>
     </row>
     <row r="2157" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2157" s="3" t="s">
+      <c r="A2157" s="9" t="s">
         <v>1403</v>
       </c>
       <c r="B2157" s="3" t="s">
-        <v>1403</v>
+        <v>4803</v>
       </c>
       <c r="C2157" s="3"/>
       <c r="F2157" s="3"/>
       <c r="G2157" s="3"/>
     </row>
-    <row r="2158" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2158" s="3" t="s">
+    <row r="2158" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2158" s="9" t="s">
         <v>232</v>
       </c>
       <c r="B2158" s="3" t="s">
-        <v>232</v>
+        <v>4786</v>
       </c>
       <c r="C2158" s="3"/>
       <c r="F2158" s="3"/>
       <c r="G2158" s="3"/>
     </row>
     <row r="2159" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2159" s="3" t="s">
+      <c r="A2159" s="9" t="s">
         <v>234</v>
       </c>
       <c r="B2159" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="C2159" s="3"/>
+        <v>4787</v>
+      </c>
+      <c r="C2159" s="10" t="s">
+        <v>4788</v>
+      </c>
       <c r="F2159" s="3"/>
       <c r="G2159" s="3"/>
     </row>
     <row r="2160" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2160" s="3" t="s">
+      <c r="A2160" s="9" t="s">
         <v>235</v>
       </c>
       <c r="B2160" s="3" t="s">
-        <v>235</v>
+        <v>4789</v>
       </c>
       <c r="C2160" s="3"/>
       <c r="F2160" s="3"/>
       <c r="G2160" s="3"/>
     </row>
-    <row r="2161" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2161" s="3" t="s">
+    <row r="2161" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2161" s="9" t="s">
         <v>233</v>
       </c>
       <c r="B2161" s="3" t="s">
-        <v>233</v>
+        <v>4787</v>
       </c>
       <c r="C2161" s="3"/>
       <c r="F2161" s="3"/>
       <c r="G2161" s="3"/>
     </row>
     <row r="2162" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2162" s="3" t="s">
+      <c r="A2162" s="9" t="s">
         <v>1172</v>
       </c>
       <c r="B2162" s="3" t="s">
-        <v>1172</v>
+        <v>4803</v>
       </c>
       <c r="C2162" s="3"/>
       <c r="F2162" s="3"/>
       <c r="G2162" s="3"/>
     </row>
-    <row r="2163" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2163" s="3" t="s">
+    <row r="2163" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2163" s="9" t="s">
         <v>222</v>
       </c>
       <c r="B2163" s="3" t="s">
-        <v>222</v>
+        <v>4786</v>
       </c>
       <c r="C2163" s="3"/>
       <c r="F2163" s="3"/>
       <c r="G2163" s="3"/>
     </row>
     <row r="2164" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2164" s="3" t="s">
+      <c r="A2164" s="9" t="s">
         <v>224</v>
       </c>
       <c r="B2164" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C2164" s="3"/>
+        <v>4787</v>
+      </c>
+      <c r="C2164" s="10" t="s">
+        <v>4788</v>
+      </c>
       <c r="F2164" s="3"/>
       <c r="G2164" s="3"/>
     </row>
     <row r="2165" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2165" s="3" t="s">
+      <c r="A2165" s="9" t="s">
         <v>225</v>
       </c>
       <c r="B2165" s="3" t="s">
-        <v>225</v>
+        <v>4789</v>
       </c>
       <c r="C2165" s="3"/>
       <c r="F2165" s="3"/>
       <c r="G2165" s="3"/>
     </row>
-    <row r="2166" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2166" s="3" t="s">
+    <row r="2166" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2166" s="9" t="s">
         <v>223</v>
       </c>
       <c r="B2166" s="3" t="s">
-        <v>223</v>
+        <v>4787</v>
       </c>
       <c r="C2166" s="3"/>
       <c r="F2166" s="3"/>
       <c r="G2166" s="3"/>
     </row>
     <row r="2167" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2167" s="3" t="s">
+      <c r="A2167" s="9" t="s">
         <v>1170</v>
       </c>
       <c r="B2167" s="3" t="s">
-        <v>1170</v>
+        <v>4803</v>
       </c>
       <c r="C2167" s="3"/>
       <c r="F2167" s="3"/>
       <c r="G2167" s="3"/>
     </row>
-    <row r="2168" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2168" s="3" t="s">
+    <row r="2168" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2168" s="9" t="s">
         <v>227</v>
       </c>
       <c r="B2168" s="3" t="s">
-        <v>227</v>
+        <v>4786</v>
       </c>
       <c r="C2168" s="3"/>
       <c r="F2168" s="3"/>
       <c r="G2168" s="3"/>
     </row>
     <row r="2169" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2169" s="3" t="s">
+      <c r="A2169" s="9" t="s">
         <v>229</v>
       </c>
       <c r="B2169" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C2169" s="3"/>
+        <v>4787</v>
+      </c>
+      <c r="C2169" s="10" t="s">
+        <v>4788</v>
+      </c>
       <c r="F2169" s="3"/>
       <c r="G2169" s="3"/>
     </row>
     <row r="2170" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2170" s="3" t="s">
+      <c r="A2170" s="9" t="s">
         <v>230</v>
       </c>
       <c r="B2170" s="3" t="s">
-        <v>230</v>
+        <v>4789</v>
       </c>
       <c r="C2170" s="3"/>
       <c r="F2170" s="3"/>
       <c r="G2170" s="3"/>
     </row>
-    <row r="2171" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2171" s="3" t="s">
+    <row r="2171" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2171" s="9" t="s">
         <v>228</v>
       </c>
       <c r="B2171" s="3" t="s">
-        <v>228</v>
+        <v>4787</v>
       </c>
       <c r="C2171" s="3"/>
       <c r="F2171" s="3"/>
       <c r="G2171" s="3"/>
     </row>
     <row r="2172" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2172" s="3" t="s">
+      <c r="A2172" s="9" t="s">
         <v>1171</v>
       </c>
       <c r="B2172" s="3" t="s">
-        <v>1171</v>
+        <v>4803</v>
       </c>
       <c r="C2172" s="3"/>
       <c r="F2172" s="3"/>
       <c r="G2172" s="3"/>
     </row>
-    <row r="2173" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2173" s="3" t="s">
+    <row r="2173" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2173" s="9" t="s">
         <v>212</v>
       </c>
       <c r="B2173" s="3" t="s">
-        <v>212</v>
+        <v>4786</v>
       </c>
       <c r="C2173" s="3"/>
       <c r="F2173" s="3"/>
       <c r="G2173" s="3"/>
     </row>
     <row r="2174" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2174" s="3" t="s">
+      <c r="A2174" s="9" t="s">
         <v>214</v>
       </c>
       <c r="B2174" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="C2174" s="3"/>
+        <v>4787</v>
+      </c>
+      <c r="C2174" s="10" t="s">
+        <v>4788</v>
+      </c>
       <c r="F2174" s="3"/>
       <c r="G2174" s="3"/>
     </row>
     <row r="2175" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2175" s="3" t="s">
+      <c r="A2175" s="9" t="s">
         <v>215</v>
       </c>
       <c r="B2175" s="3" t="s">
-        <v>215</v>
+        <v>4789</v>
       </c>
       <c r="C2175" s="3"/>
       <c r="F2175" s="3"/>
       <c r="G2175" s="3"/>
     </row>
-    <row r="2176" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2176" s="3" t="s">
+    <row r="2176" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2176" s="9" t="s">
         <v>213</v>
       </c>
       <c r="B2176" s="3" t="s">
-        <v>213</v>
+        <v>4787</v>
       </c>
       <c r="C2176" s="3"/>
       <c r="F2176" s="3"/>
       <c r="G2176" s="3"/>
     </row>
     <row r="2177" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2177" s="3" t="s">
+      <c r="A2177" s="9" t="s">
         <v>1168</v>
       </c>
       <c r="B2177" s="3" t="s">
-        <v>1168</v>
+        <v>4803</v>
       </c>
       <c r="C2177" s="3"/>
       <c r="F2177" s="3"/>
       <c r="G2177" s="3"/>
     </row>
-    <row r="2178" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2178" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2178" s="9" t="s">
         <v>187</v>
       </c>
       <c r="B2178" s="3" t="s">
-        <v>187</v>
+        <v>4786</v>
       </c>
       <c r="C2178" s="3"/>
       <c r="F2178" s="3"/>
       <c r="G2178" s="3"/>
     </row>
     <row r="2179" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2179" s="3" t="s">
+      <c r="A2179" s="9" t="s">
         <v>189</v>
       </c>
       <c r="B2179" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2179" s="3"/>
+        <v>4787</v>
+      </c>
+      <c r="C2179" s="10" t="s">
+        <v>4788</v>
+      </c>
       <c r="F2179" s="3"/>
       <c r="G2179" s="3"/>
     </row>
     <row r="2180" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2180" s="3" t="s">
+      <c r="A2180" s="9" t="s">
         <v>190</v>
       </c>
       <c r="B2180" s="3" t="s">
-        <v>190</v>
+        <v>4789</v>
       </c>
       <c r="C2180" s="3"/>
       <c r="F2180" s="3"/>
       <c r="G2180" s="3"/>
     </row>
-    <row r="2181" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2181" s="3" t="s">
+    <row r="2181" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2181" s="9" t="s">
         <v>188</v>
       </c>
       <c r="B2181" s="3" t="s">
-        <v>188</v>
+        <v>4787</v>
       </c>
       <c r="C2181" s="3"/>
       <c r="F2181" s="3"/>
       <c r="G2181" s="3"/>
     </row>
     <row r="2182" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2182" s="3" t="s">
+      <c r="A2182" s="9" t="s">
         <v>1401</v>
       </c>
       <c r="B2182" s="3" t="s">
-        <v>1401</v>
+        <v>4803</v>
       </c>
       <c r="C2182" s="3"/>
       <c r="F2182" s="3"/>
       <c r="G2182" s="3"/>
     </row>
-    <row r="2183" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2183" s="3" t="s">
+    <row r="2183" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2183" s="9" t="s">
         <v>192</v>
       </c>
       <c r="B2183" s="3" t="s">
-        <v>192</v>
+        <v>4786</v>
       </c>
       <c r="C2183" s="3"/>
       <c r="F2183" s="3"/>
       <c r="G2183" s="3"/>
     </row>
     <row r="2184" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2184" s="3" t="s">
+      <c r="A2184" s="9" t="s">
         <v>194</v>
       </c>
       <c r="B2184" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="C2184" s="3"/>
+        <v>4787</v>
+      </c>
+      <c r="C2184" s="10" t="s">
+        <v>4788</v>
+      </c>
       <c r="F2184" s="3"/>
       <c r="G2184" s="3"/>
     </row>
     <row r="2185" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2185" s="3" t="s">
+      <c r="A2185" s="9" t="s">
         <v>195</v>
       </c>
       <c r="B2185" s="3" t="s">
-        <v>195</v>
+        <v>4789</v>
       </c>
       <c r="C2185" s="3"/>
       <c r="F2185" s="3"/>
       <c r="G2185" s="3"/>
     </row>
-    <row r="2186" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2186" s="3" t="s">
+    <row r="2186" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2186" s="9" t="s">
         <v>193</v>
       </c>
       <c r="B2186" s="3" t="s">
-        <v>193</v>
+        <v>4787</v>
       </c>
       <c r="C2186" s="3"/>
       <c r="F2186" s="3"/>
       <c r="G2186" s="3"/>
     </row>
     <row r="2187" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2187" s="3" t="s">
+      <c r="A2187" s="9" t="s">
         <v>1402</v>
       </c>
       <c r="B2187" s="3" t="s">
-        <v>1402</v>
+        <v>4803</v>
       </c>
       <c r="C2187" s="3"/>
       <c r="F2187" s="3"/>
       <c r="G2187" s="3"/>
     </row>
-    <row r="2188" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2188" s="3" t="s">
+    <row r="2188" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2188" s="9" t="s">
         <v>217</v>
       </c>
       <c r="B2188" s="3" t="s">
-        <v>217</v>
+        <v>4786</v>
       </c>
       <c r="C2188" s="3"/>
       <c r="F2188" s="3"/>
       <c r="G2188" s="3"/>
     </row>
-    <row r="2189" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2189" s="3" t="s">
+    <row r="2189" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2189" s="9" t="s">
         <v>207</v>
       </c>
       <c r="B2189" s="3" t="s">
-        <v>207</v>
+        <v>4786</v>
       </c>
       <c r="C2189" s="3"/>
       <c r="F2189" s="3"/>
       <c r="G2189" s="3"/>
     </row>
     <row r="2190" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2190" s="3" t="s">
+      <c r="A2190" s="9" t="s">
         <v>219</v>
       </c>
       <c r="B2190" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2190" s="3"/>
+        <v>4787</v>
+      </c>
+      <c r="C2190" s="10" t="s">
+        <v>4788</v>
+      </c>
       <c r="F2190" s="3"/>
       <c r="G2190" s="3"/>
     </row>
     <row r="2191" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2191" s="3" t="s">
+      <c r="A2191" s="9" t="s">
         <v>209</v>
       </c>
       <c r="B2191" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="C2191" s="3"/>
+        <v>4787</v>
+      </c>
+      <c r="C2191" s="10" t="s">
+        <v>4788</v>
+      </c>
       <c r="F2191" s="3"/>
       <c r="G2191" s="3"/>
     </row>
     <row r="2192" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2192" s="3" t="s">
+      <c r="A2192" s="9" t="s">
         <v>220</v>
       </c>
       <c r="B2192" s="3" t="s">
-        <v>220</v>
+        <v>4789</v>
       </c>
       <c r="C2192" s="3"/>
       <c r="F2192" s="3"/>
       <c r="G2192" s="3"/>
     </row>
     <row r="2193" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2193" s="3" t="s">
+      <c r="A2193" s="9" t="s">
         <v>210</v>
       </c>
       <c r="B2193" s="3" t="s">
-        <v>210</v>
+        <v>4789</v>
       </c>
       <c r="C2193" s="3"/>
       <c r="F2193" s="3"/>
       <c r="G2193" s="3"/>
     </row>
-    <row r="2194" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2194" s="3" t="s">
+    <row r="2194" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2194" s="9" t="s">
         <v>218</v>
       </c>
       <c r="B2194" s="3" t="s">
-        <v>218</v>
+        <v>4787</v>
       </c>
       <c r="C2194" s="3"/>
       <c r="F2194" s="3"/>
       <c r="G2194" s="3"/>
     </row>
-    <row r="2195" spans="1:7" ht="60" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2195" s="3" t="s">
+    <row r="2195" spans="1:7" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2195" s="9" t="s">
         <v>208</v>
       </c>
       <c r="B2195" s="3" t="s">
-        <v>208</v>
+        <v>4787</v>
       </c>
       <c r="C2195" s="3"/>
       <c r="F2195" s="3"/>
@@ -39537,34 +40057,34 @@
       <c r="F2201" s="3"/>
       <c r="G2201" s="3"/>
     </row>
-    <row r="2202" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2202" s="3" t="s">
+    <row r="2202" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2202" s="9" t="s">
         <v>2336</v>
       </c>
       <c r="B2202" s="3" t="s">
-        <v>2336</v>
+        <v>4800</v>
       </c>
       <c r="C2202" s="3"/>
       <c r="F2202" s="3"/>
       <c r="G2202" s="3"/>
     </row>
-    <row r="2203" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2203" s="3" t="s">
+    <row r="2203" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2203" s="9" t="s">
         <v>2335</v>
       </c>
       <c r="B2203" s="3" t="s">
-        <v>2335</v>
+        <v>4801</v>
       </c>
       <c r="C2203" s="3"/>
       <c r="F2203" s="3"/>
       <c r="G2203" s="3"/>
     </row>
-    <row r="2204" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2204" s="3" t="s">
+    <row r="2204" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2204" s="9" t="s">
         <v>2330</v>
       </c>
       <c r="B2204" s="3" t="s">
-        <v>2330</v>
+        <v>4800</v>
       </c>
       <c r="C2204" s="3"/>
       <c r="F2204" s="3"/>
@@ -39603,12 +40123,12 @@
       <c r="F2207" s="3"/>
       <c r="G2207" s="3"/>
     </row>
-    <row r="2208" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2208" s="3" t="s">
+    <row r="2208" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2208" s="9" t="s">
         <v>2329</v>
       </c>
       <c r="B2208" s="3" t="s">
-        <v>2329</v>
+        <v>4801</v>
       </c>
       <c r="C2208" s="3"/>
       <c r="F2208" s="3"/>
@@ -40021,139 +40541,139 @@
       <c r="F2245" s="3"/>
       <c r="G2245" s="3"/>
     </row>
-    <row r="2246" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2246" s="3" t="s">
+    <row r="2246" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2246" s="9" t="s">
         <v>2700</v>
       </c>
       <c r="B2246" s="3" t="s">
-        <v>2700</v>
+        <v>4802</v>
       </c>
       <c r="C2246" s="3"/>
       <c r="F2246" s="3"/>
       <c r="G2246" s="3"/>
     </row>
-    <row r="2247" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2247" s="3" t="s">
+    <row r="2247" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2247" s="9" t="s">
         <v>2707</v>
       </c>
       <c r="B2247" s="3" t="s">
-        <v>2707</v>
+        <v>4802</v>
       </c>
       <c r="C2247" s="3"/>
       <c r="F2247" s="3"/>
       <c r="G2247" s="3"/>
     </row>
-    <row r="2248" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2248" s="3" t="s">
+    <row r="2248" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2248" s="9" t="s">
         <v>2709</v>
       </c>
       <c r="B2248" s="3" t="s">
-        <v>2709</v>
+        <v>4802</v>
       </c>
       <c r="C2248" s="3"/>
       <c r="F2248" s="3"/>
       <c r="G2248" s="3"/>
     </row>
-    <row r="2249" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2249" s="3" t="s">
+    <row r="2249" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2249" s="9" t="s">
         <v>2701</v>
       </c>
       <c r="B2249" s="3" t="s">
-        <v>2701</v>
+        <v>4802</v>
       </c>
       <c r="C2249" s="3"/>
       <c r="F2249" s="3"/>
       <c r="G2249" s="3"/>
     </row>
-    <row r="2250" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2250" s="3" t="s">
+    <row r="2250" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2250" s="9" t="s">
         <v>2705</v>
       </c>
       <c r="B2250" s="3" t="s">
-        <v>2705</v>
+        <v>4802</v>
       </c>
       <c r="C2250" s="3"/>
       <c r="F2250" s="3"/>
       <c r="G2250" s="3"/>
     </row>
-    <row r="2251" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2251" s="3" t="s">
+    <row r="2251" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2251" s="9" t="s">
         <v>2704</v>
       </c>
       <c r="B2251" s="3" t="s">
-        <v>2704</v>
+        <v>4802</v>
       </c>
       <c r="C2251" s="3"/>
       <c r="F2251" s="3"/>
       <c r="G2251" s="3"/>
     </row>
-    <row r="2252" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2252" s="3" t="s">
+    <row r="2252" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2252" s="9" t="s">
         <v>2699</v>
       </c>
       <c r="B2252" s="3" t="s">
-        <v>2699</v>
+        <v>4802</v>
       </c>
       <c r="C2252" s="3"/>
       <c r="F2252" s="3"/>
       <c r="G2252" s="3"/>
     </row>
-    <row r="2253" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2253" s="3" t="s">
+    <row r="2253" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2253" s="9" t="s">
         <v>2706</v>
       </c>
       <c r="B2253" s="3" t="s">
-        <v>2706</v>
+        <v>4802</v>
       </c>
       <c r="C2253" s="3"/>
       <c r="F2253" s="3"/>
       <c r="G2253" s="3"/>
     </row>
-    <row r="2254" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2254" s="3" t="s">
+    <row r="2254" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2254" s="9" t="s">
         <v>2702</v>
       </c>
       <c r="B2254" s="3" t="s">
-        <v>2702</v>
+        <v>4802</v>
       </c>
       <c r="C2254" s="3"/>
       <c r="F2254" s="3"/>
       <c r="G2254" s="3"/>
     </row>
-    <row r="2255" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2255" s="3" t="s">
+    <row r="2255" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2255" s="9" t="s">
         <v>2708</v>
       </c>
       <c r="B2255" s="3" t="s">
-        <v>2708</v>
+        <v>4802</v>
       </c>
       <c r="C2255" s="3"/>
       <c r="F2255" s="3"/>
       <c r="G2255" s="3"/>
     </row>
-    <row r="2256" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2256" s="3" t="s">
+    <row r="2256" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2256" s="9" t="s">
         <v>2698</v>
       </c>
       <c r="B2256" s="3" t="s">
-        <v>2698</v>
+        <v>4802</v>
       </c>
       <c r="C2256" s="3"/>
       <c r="F2256" s="3"/>
       <c r="G2256" s="3"/>
     </row>
-    <row r="2257" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2257" s="3" t="s">
+    <row r="2257" spans="1:7" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2257" s="9" t="s">
         <v>2703</v>
       </c>
       <c r="B2257" s="3" t="s">
-        <v>2703</v>
+        <v>4802</v>
       </c>
       <c r="C2257" s="3"/>
       <c r="F2257" s="3"/>
       <c r="G2257" s="3"/>
     </row>
-    <row r="2258" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2258" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2258" s="3" t="s">
         <v>2640</v>
       </c>
@@ -40164,7 +40684,7 @@
       <c r="F2258" s="3"/>
       <c r="G2258" s="3"/>
     </row>
-    <row r="2259" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2259" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2259" s="3" t="s">
         <v>2647</v>
       </c>
@@ -40175,7 +40695,7 @@
       <c r="F2259" s="3"/>
       <c r="G2259" s="3"/>
     </row>
-    <row r="2260" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2260" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2260" s="3" t="s">
         <v>2649</v>
       </c>
@@ -40186,7 +40706,7 @@
       <c r="F2260" s="3"/>
       <c r="G2260" s="3"/>
     </row>
-    <row r="2261" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2261" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2261" s="3" t="s">
         <v>2641</v>
       </c>
@@ -40197,7 +40717,7 @@
       <c r="F2261" s="3"/>
       <c r="G2261" s="3"/>
     </row>
-    <row r="2262" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2262" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2262" s="3" t="s">
         <v>2645</v>
       </c>
@@ -40208,7 +40728,7 @@
       <c r="F2262" s="3"/>
       <c r="G2262" s="3"/>
     </row>
-    <row r="2263" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2263" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2263" s="3" t="s">
         <v>2644</v>
       </c>
@@ -40219,7 +40739,7 @@
       <c r="F2263" s="3"/>
       <c r="G2263" s="3"/>
     </row>
-    <row r="2264" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2264" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2264" s="3" t="s">
         <v>2639</v>
       </c>
@@ -40230,7 +40750,7 @@
       <c r="F2264" s="3"/>
       <c r="G2264" s="3"/>
     </row>
-    <row r="2265" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2265" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2265" s="3" t="s">
         <v>2646</v>
       </c>
@@ -40241,7 +40761,7 @@
       <c r="F2265" s="3"/>
       <c r="G2265" s="3"/>
     </row>
-    <row r="2266" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2266" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2266" s="3" t="s">
         <v>2642</v>
       </c>
@@ -40252,7 +40772,7 @@
       <c r="F2266" s="3"/>
       <c r="G2266" s="3"/>
     </row>
-    <row r="2267" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2267" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2267" s="3" t="s">
         <v>2648</v>
       </c>
@@ -40263,7 +40783,7 @@
       <c r="F2267" s="3"/>
       <c r="G2267" s="3"/>
     </row>
-    <row r="2268" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2268" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2268" s="3" t="s">
         <v>2638</v>
       </c>
@@ -40274,7 +40794,7 @@
       <c r="F2268" s="3"/>
       <c r="G2268" s="3"/>
     </row>
-    <row r="2269" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2269" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2269" s="3" t="s">
         <v>2643</v>
       </c>
@@ -45234,7 +45754,7 @@
       <c r="F2713" s="3"/>
       <c r="G2713" s="3"/>
     </row>
-    <row r="2714" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2714" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2714" s="3" t="s">
         <v>1447</v>
       </c>
@@ -45608,7 +46128,7 @@
       <c r="F2747" s="3"/>
       <c r="G2747" s="3"/>
     </row>
-    <row r="2748" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2748" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2748" s="3" t="s">
         <v>592</v>
       </c>
@@ -45905,7 +46425,7 @@
       <c r="F2774" s="3"/>
       <c r="G2774" s="3"/>
     </row>
-    <row r="2775" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2775" spans="1:7" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2775" s="3" t="s">
         <v>591</v>
       </c>
@@ -52290,7 +52810,7 @@
       <c r="F3344" s="3"/>
       <c r="G3344" s="3"/>
     </row>
-    <row r="3345" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3345" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3345" s="3" t="s">
         <v>2497</v>
       </c>
@@ -52301,7 +52821,7 @@
       <c r="F3345" s="3"/>
       <c r="G3345" s="3"/>
     </row>
-    <row r="3346" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3346" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3346" s="3" t="s">
         <v>2504</v>
       </c>
@@ -52312,7 +52832,7 @@
       <c r="F3346" s="3"/>
       <c r="G3346" s="3"/>
     </row>
-    <row r="3347" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3347" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3347" s="3" t="s">
         <v>2506</v>
       </c>
@@ -52323,7 +52843,7 @@
       <c r="F3347" s="3"/>
       <c r="G3347" s="3"/>
     </row>
-    <row r="3348" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3348" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3348" s="3" t="s">
         <v>2498</v>
       </c>
@@ -52334,7 +52854,7 @@
       <c r="F3348" s="3"/>
       <c r="G3348" s="3"/>
     </row>
-    <row r="3349" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3349" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3349" s="3" t="s">
         <v>2502</v>
       </c>
@@ -52345,7 +52865,7 @@
       <c r="F3349" s="3"/>
       <c r="G3349" s="3"/>
     </row>
-    <row r="3350" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3350" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3350" s="3" t="s">
         <v>2501</v>
       </c>
@@ -52356,7 +52876,7 @@
       <c r="F3350" s="3"/>
       <c r="G3350" s="3"/>
     </row>
-    <row r="3351" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3351" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3351" s="3" t="s">
         <v>2496</v>
       </c>
@@ -52367,7 +52887,7 @@
       <c r="F3351" s="3"/>
       <c r="G3351" s="3"/>
     </row>
-    <row r="3352" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3352" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3352" s="3" t="s">
         <v>2503</v>
       </c>
@@ -52378,7 +52898,7 @@
       <c r="F3352" s="3"/>
       <c r="G3352" s="3"/>
     </row>
-    <row r="3353" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3353" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3353" s="3" t="s">
         <v>2499</v>
       </c>
@@ -52389,7 +52909,7 @@
       <c r="F3353" s="3"/>
       <c r="G3353" s="3"/>
     </row>
-    <row r="3354" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3354" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3354" s="3" t="s">
         <v>2505</v>
       </c>
@@ -52400,7 +52920,7 @@
       <c r="F3354" s="3"/>
       <c r="G3354" s="3"/>
     </row>
-    <row r="3355" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3355" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3355" s="3" t="s">
         <v>2495</v>
       </c>
@@ -52411,7 +52931,7 @@
       <c r="F3355" s="3"/>
       <c r="G3355" s="3"/>
     </row>
-    <row r="3356" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3356" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3356" s="3" t="s">
         <v>2500</v>
       </c>
@@ -63240,7 +63760,7 @@
       <c r="E4287"/>
       <c r="F4287"/>
     </row>
-    <row r="4288" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4288" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4288" s="2" t="s">
         <v>4283</v>
       </c>
@@ -63403,7 +63923,7 @@
       <c r="E4301"/>
       <c r="F4301"/>
     </row>
-    <row r="4302" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4302" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4302" t="s">
         <v>4296</v>
       </c>
@@ -63547,7 +64067,7 @@
       <c r="E4313"/>
       <c r="F4313"/>
     </row>
-    <row r="4314" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4314" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4314" t="s">
         <v>4308</v>
       </c>
@@ -63691,7 +64211,7 @@
       <c r="E4325"/>
       <c r="F4325"/>
     </row>
-    <row r="4326" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4326" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4326" s="2" t="s">
         <v>4320</v>
       </c>
@@ -63703,7 +64223,7 @@
       <c r="E4326" s="2"/>
       <c r="F4326"/>
     </row>
-    <row r="4327" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4327" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4327" s="2" t="s">
         <v>4321</v>
       </c>
@@ -63715,7 +64235,7 @@
       <c r="E4327" s="2"/>
       <c r="F4327"/>
     </row>
-    <row r="4328" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4328" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4328" s="2" t="s">
         <v>4322</v>
       </c>
@@ -63727,7 +64247,7 @@
       <c r="E4328" s="2"/>
       <c r="F4328"/>
     </row>
-    <row r="4329" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4329" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4329" s="2" t="s">
         <v>4323</v>
       </c>
@@ -63739,7 +64259,7 @@
       <c r="E4329" s="2"/>
       <c r="F4329"/>
     </row>
-    <row r="4330" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4330" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4330" s="2" t="s">
         <v>4324</v>
       </c>
@@ -63751,7 +64271,7 @@
       <c r="E4330" s="2"/>
       <c r="F4330"/>
     </row>
-    <row r="4331" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4331" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4331" s="2" t="s">
         <v>4325</v>
       </c>
@@ -63763,7 +64283,7 @@
       <c r="E4331" s="2"/>
       <c r="F4331"/>
     </row>
-    <row r="4332" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4332" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4332" s="2" t="s">
         <v>4326</v>
       </c>
@@ -63775,7 +64295,7 @@
       <c r="E4332" s="2"/>
       <c r="F4332"/>
     </row>
-    <row r="4333" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4333" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4333" s="2" t="s">
         <v>4327</v>
       </c>
@@ -63787,7 +64307,7 @@
       <c r="E4333" s="2"/>
       <c r="F4333"/>
     </row>
-    <row r="4334" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4334" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4334" s="2" t="s">
         <v>4328</v>
       </c>
@@ -63799,7 +64319,7 @@
       <c r="E4334" s="2"/>
       <c r="F4334"/>
     </row>
-    <row r="4335" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4335" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4335" s="2" t="s">
         <v>4329</v>
       </c>
@@ -63811,7 +64331,7 @@
       <c r="E4335" s="2"/>
       <c r="F4335"/>
     </row>
-    <row r="4336" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4336" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4336" s="2" t="s">
         <v>4330</v>
       </c>
@@ -65812,7 +66332,7 @@
       </c>
       <c r="C4516" s="3"/>
     </row>
-    <row r="4517" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="4517" spans="1:3" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4517" s="9" t="s">
         <v>4748</v>
       </c>
@@ -65820,7 +66340,7 @@
         <v>4753</v>
       </c>
     </row>
-    <row r="4518" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="4518" spans="1:3" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4518" s="9" t="s">
         <v>4749</v>
       </c>
@@ -65828,7 +66348,7 @@
         <v>4753</v>
       </c>
     </row>
-    <row r="4519" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="4519" spans="1:3" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4519" s="9" t="s">
         <v>4750</v>
       </c>
@@ -65836,7 +66356,7 @@
         <v>4753</v>
       </c>
     </row>
-    <row r="4520" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="4520" spans="1:3" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4520" s="9" t="s">
         <v>4751</v>
       </c>
@@ -65844,7 +66364,7 @@
         <v>4753</v>
       </c>
     </row>
-    <row r="4521" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="4521" spans="1:3" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4521" s="9" t="s">
         <v>4752</v>
       </c>
@@ -65852,7 +66372,7 @@
         <v>4753</v>
       </c>
     </row>
-    <row r="4522" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="4522" spans="1:3" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4522" s="9" t="s">
         <v>4768</v>
       </c>
@@ -65860,7 +66380,7 @@
         <v>4766</v>
       </c>
     </row>
-    <row r="4523" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="4523" spans="1:3" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4523" s="9" t="s">
         <v>4767</v>
       </c>
@@ -65868,7 +66388,7 @@
         <v>4766</v>
       </c>
     </row>
-    <row r="4524" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4524" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4524" s="9" t="s">
         <v>4770</v>
       </c>
@@ -65884,7 +66404,7 @@
         <v>4773</v>
       </c>
     </row>
-    <row r="4526" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4526" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4526" s="9" t="s">
         <v>4774</v>
       </c>
@@ -65892,7 +66412,7 @@
         <v>4776</v>
       </c>
     </row>
-    <row r="4527" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4527" spans="1:3" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4527" s="9" t="s">
         <v>4775</v>
       </c>
@@ -65900,7 +66420,7 @@
         <v>4777</v>
       </c>
     </row>
-    <row r="4528" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4528" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4528" s="9" t="s">
         <v>4778</v>
       </c>
@@ -65908,7 +66428,7 @@
         <v>4779</v>
       </c>
     </row>
-    <row r="4529" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4529" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4529" s="9" t="s">
         <v>4780</v>
       </c>
@@ -65916,7 +66436,7 @@
         <v>4781</v>
       </c>
     </row>
-    <row r="4530" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4530" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4530" s="9" t="s">
         <v>4782</v>
       </c>
@@ -65924,7 +66444,7 @@
         <v>4783</v>
       </c>
     </row>
-    <row r="4531" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4531" spans="1:2" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4531" s="9" t="s">
         <v>4784</v>
       </c>
@@ -65932,12 +66452,44 @@
         <v>4785</v>
       </c>
     </row>
+    <row r="4532" spans="1:2" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4532" s="3" t="s">
+        <v>4797</v>
+      </c>
+      <c r="B4532" s="3" t="s">
+        <v>4799</v>
+      </c>
+    </row>
+    <row r="4533" spans="1:2" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4533" s="3" t="s">
+        <v>4798</v>
+      </c>
+      <c r="B4533" s="3" t="s">
+        <v>4799</v>
+      </c>
+    </row>
+    <row r="4534" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4534" s="9" t="s">
+        <v>4807</v>
+      </c>
+      <c r="B4534" s="3" t="s">
+        <v>4808</v>
+      </c>
+    </row>
+    <row r="4535" spans="1:2" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4535" s="9" t="s">
+        <v>4809</v>
+      </c>
+      <c r="B4535" s="3" t="s">
+        <v>4808</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G4531" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
+  <autoFilter ref="A1:G4535" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
     <filterColumn colId="0">
-      <customFilters>
-        <customFilter val="*Thái Dương*"/>
-      </customFilters>
+      <filters>
+        <filter val="Thiên Cơ tọa thủ cung Mệnh gặp Thiên Đồng, Thiên Lương, Thái Âm"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B3728">
@@ -65945,95 +66497,107 @@
   </sortState>
   <dataConsolidate/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A4284 A4292:A1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="81" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6713:A1048576 A2:A4169">
-    <cfRule type="duplicateValues" dxfId="3" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="56"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B814">
-    <cfRule type="duplicateValues" dxfId="40" priority="26"/>
-    <cfRule type="duplicateValues" dxfId="39" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="79" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3281">
-    <cfRule type="duplicateValues" dxfId="35" priority="34"/>
-    <cfRule type="duplicateValues" dxfId="34" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3285">
-    <cfRule type="duplicateValues" dxfId="33" priority="32"/>
-    <cfRule type="duplicateValues" dxfId="32" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3289">
-    <cfRule type="duplicateValues" dxfId="31" priority="30"/>
-    <cfRule type="duplicateValues" dxfId="30" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3293">
-    <cfRule type="duplicateValues" dxfId="29" priority="28"/>
-    <cfRule type="duplicateValues" dxfId="28" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4289">
-    <cfRule type="duplicateValues" dxfId="27" priority="24"/>
-    <cfRule type="duplicateValues" dxfId="26" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4291">
-    <cfRule type="duplicateValues" dxfId="25" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="27"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4292:B4418 B3265:B3266 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B4420:B4424 B4426:B4433 B816 B2:B776 B798:B800 B802:B805 B808 B811:B812 B779:B780 B783:B784 B788 B3294:B4284 B791:B795 B818:B1672 B4435:B1048576 B1674:B1683 B1719:B3263 B1703:B1717 B1685:B1701">
-    <cfRule type="duplicateValues" dxfId="23" priority="39"/>
+  <conditionalFormatting sqref="B4292:B4418 B3265:B3266 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B4420:B4424 B4426:B4433 B816 B2:B776 B798:B800 B802:B805 B808 B811:B812 B779:B780 B783:B784 B788 B3294:B4284 B791:B795 B1674:B1683 B1703:B1717 B1685:B1701 B818:B1672 B2147:B2181 B2183:B3263 B1719:B2145 B4435:B1048576">
+    <cfRule type="duplicateValues" dxfId="65" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4419">
-    <cfRule type="duplicateValues" dxfId="22" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4466">
-    <cfRule type="duplicateValues" dxfId="21" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="28"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6713:B1048576 B4400:B4403 B3265:B3266 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B816 B2:B776 B798:B800 B802:B805 B808 B811:B812 B779:B780 B783:B784 B788 B3294:B4169 B791:B795 B818:B1672 B1674:B1683 B1719:B3263 B1703:B1717 B1685:B1701">
-    <cfRule type="duplicateValues" dxfId="20" priority="40"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:W776 D777:W778 B777:B778 B798:W800 D796:W797 B796:B797 B808:W808 D806:W807 B806:B807 D809:W810 B809:B810 D801:W801 B801 B802:W805 B811:W812 B779:W780 C781:W782 B788:W788 B816:W816 C815:W815 C817:W817 B814:W814 C813:W813 C785:W787 C789:W790 B783:W784 B791:W795 B818:W1672 B1674:W1683 C1673:W1673 C1702:W1702 B1703:W1717 C1718:W1718 B1719:W1048576 B1685:W1701 C1684:W1684">
-    <cfRule type="duplicateValues" dxfId="19" priority="23"/>
+  <conditionalFormatting sqref="B6713:B1048576 B4400:B4403 B3265:B3266 B3268:B3280 B3282:B3284 B3286:B3288 B3290:B3292 B816 B2:B776 B798:B800 B802:B805 B808 B811:B812 B779:B780 B783:B784 B788 B3294:B4169 B791:B795 B1674:B1683 B1703:B1717 B1685:B1701 B818:B1672 B2147:B2181 B2183:B3263 B1719:B2145">
+    <cfRule type="duplicateValues" dxfId="62" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3721">
-    <cfRule type="duplicateValues" dxfId="18" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1673">
-    <cfRule type="duplicateValues" dxfId="17" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1673">
-    <cfRule type="duplicateValues" dxfId="16" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1673">
-    <cfRule type="duplicateValues" dxfId="15" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1702">
-    <cfRule type="duplicateValues" dxfId="14" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1702">
-    <cfRule type="duplicateValues" dxfId="13" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1702">
-    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1718">
-    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1718">
-    <cfRule type="duplicateValues" dxfId="7" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1718">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1684">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1684">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1684">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:W776 D777:W778 B777:B778 B798:W800 D796:W797 B796:B797 B808:W808 D806:W807 B806:B807 D809:W810 B809:B810 D801:W801 B801 B802:W805 B811:W812 B779:W780 C781:W782 B788:W788 B816:W816 C815:W815 C817:W817 B814:W814 C813:W813 C785:W787 C789:W790 B783:W784 B791:W795 B1674:W1683 C1673:W1673 C1702:W1702 B1703:W1717 C1718:W1718 B1685:W1701 C1684:W1684 D2145:W2146 B2145:B2146 D2154:W2154 D2159:W2159 D2164:W2164 D2169:W2169 D2174:W2174 B2179 D2179:W2179 D2184:W2184 D2190:W2191 B2154:B2155 B2159:B2160 B2164:B2165 B2169:B2170 B2174:B2175 B2183:W2183 C2182:W2182 B2180:W2181 B2184:B2185 B2190:B2193 B2147:W2153 B818:W1672 B2155:W2158 B2160:W2163 B2165:W2168 B2170:W2173 B2175:W2178 B2185:W2189 B1719:W2144 B2192:W1048576">
+    <cfRule type="duplicateValues" dxfId="48" priority="106"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2182">
+    <cfRule type="duplicateValues" dxfId="47" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2182">
+    <cfRule type="duplicateValues" dxfId="46" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2182">
+    <cfRule type="duplicateValues" dxfId="45" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Giải thích thất sát tại mệnh đến phần luận nam
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEA1293-814B-47F5-8258-E2262EDD3F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883583A1-C506-492C-B471-7DCA55915491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9645" uniqueCount="5107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9645" uniqueCount="5119">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -15374,6 +15374,42 @@
   </si>
   <si>
     <t>Thiên Lương tọa thủ cung Mệnh ở Hợi gặp Thiên Mã ở Thiên Di</t>
+  </si>
+  <si>
+    <t>Thân hình nở nang, hơi cao, nhưng thô xấu, da xám hây đen dòn, mặt thường có vết, mắt to và lồi, tính ương ngạnh, nóng nảy, làm việc gì cũng muốn cho chóng xong.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bạn là người rất can đảm, dũng mãnh, thông minh, có nhiều mưu cơ, lại thêm tánh cương nghị, hiếu thắng, và hay nói đại ngôn, nhưng được nhiều người tin phục, tuy được hưởng giàu sang, sống lâu, nhưng trên đường đời gặp nhiều bước thăng trầm. </t>
+  </si>
+  <si>
+    <t>Bạn có cách cục được hưởng giàu sang phú quý tột bậc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tất được hưởng phú qúy đến tột bậc, có uy quyền hiển hách và danh tiếng lừng lẫy. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cách cục là người tàn nhẫn, đa sát, tuy được hưởng giàu sang, nhưng chẳng được lâu bề, lại có tật bênh, thường hay mắc tai nạn xe cộ, đao súng, hay bị bắt bớ, giam giữ và chắc chắn giảm thọ. </t>
+  </si>
+  <si>
+    <t>Cách cục là người tàn nhẫn, đa sát, tuy được hưởng giàu sang, nhưng chẳng được lâu bề, lại có tật bênh, thường hay mắc tai nạn xe cộ, đao súng, hay bị bắt bớ, giam giữ và chắc chắn giảm thọ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cách cục là người hung bạo gian quyệt, hay nói khoác lác, thường làm đồ tể, hàng thịt, thợ rèn, nếu giàu có, tất không thể sống lâu được. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cách cục tuy có xấu nhưng cũng như được hưởngphú qúy và tuổi thọ cũng gia tăng. </t>
+  </si>
+  <si>
+    <t>Thường làm thợ vàng hay thợ bạc cũng làm cách cục trở nên đẹp.</t>
+  </si>
+  <si>
+    <t>Suốt đời cùng khổ cô đơn, phải loang thang phiêu bạt, thường có bệnh tật khó chữa, lại hay bị bắt bớ giam cầm, hay mắc tia nạn khủng khiếp, nhất là về xe cộ, dao súng và dĩ nhiên là yểu tử,</t>
+  </si>
+  <si>
+    <t>Nếu không mắc tù tội, tất cũng bị giết chết, hay chết vì tai nạn xe cộ.</t>
+  </si>
+  <si>
+    <t>Bạn là người có biệt tài về quân sự và có oai phong lẫm liệt.</t>
   </si>
 </sst>
 </file>
@@ -15454,7 +15490,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -15883,8 +15939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
   <dimension ref="A2:G4686"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2747" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C2753" sqref="C2753"/>
+    <sheetView tabSelected="1" topLeftCell="A2061" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C2067" sqref="C2067"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27387,45 +27443,45 @@
       <c r="F1034" s="2"/>
       <c r="G1034" s="2"/>
     </row>
-    <row r="1035" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1035" s="2" t="s">
+    <row r="1035" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1035" s="6" t="s">
         <v>4742</v>
       </c>
       <c r="B1035" s="2" t="s">
-        <v>4742</v>
+        <v>5114</v>
       </c>
       <c r="C1035" s="2"/>
       <c r="F1035" s="2"/>
       <c r="G1035" s="2"/>
     </row>
-    <row r="1036" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1036" s="2" t="s">
+    <row r="1036" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1036" s="6" t="s">
         <v>4743</v>
       </c>
       <c r="B1036" s="2" t="s">
-        <v>4743</v>
+        <v>5114</v>
       </c>
       <c r="C1036" s="2"/>
       <c r="F1036" s="2"/>
       <c r="G1036" s="2"/>
     </row>
-    <row r="1037" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1037" s="2" t="s">
+    <row r="1037" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1037" s="6" t="s">
         <v>4744</v>
       </c>
       <c r="B1037" s="2" t="s">
-        <v>4744</v>
+        <v>5108</v>
       </c>
       <c r="C1037" s="2"/>
       <c r="F1037" s="2"/>
       <c r="G1037" s="2"/>
     </row>
-    <row r="1038" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1038" s="2" t="s">
+    <row r="1038" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1038" s="6" t="s">
         <v>4745</v>
       </c>
       <c r="B1038" s="2" t="s">
-        <v>4745</v>
+        <v>5108</v>
       </c>
       <c r="C1038" s="2"/>
       <c r="F1038" s="2"/>
@@ -27705,22 +27761,22 @@
       <c r="G1063" s="2"/>
     </row>
     <row r="1064" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1064" s="2" t="s">
+      <c r="A1064" s="6" t="s">
         <v>4810</v>
       </c>
       <c r="B1064" s="2" t="s">
-        <v>4810</v>
+        <v>5109</v>
       </c>
       <c r="C1064" s="2"/>
       <c r="F1064" s="2"/>
       <c r="G1064" s="2"/>
     </row>
     <row r="1065" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1065" s="2" t="s">
+      <c r="A1065" s="6" t="s">
         <v>4811</v>
       </c>
       <c r="B1065" s="2" t="s">
-        <v>4811</v>
+        <v>5109</v>
       </c>
       <c r="C1065" s="2"/>
       <c r="F1065" s="2"/>
@@ -27847,22 +27903,22 @@
       <c r="G1076" s="2"/>
     </row>
     <row r="1077" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1077" s="2" t="s">
+      <c r="A1077" s="6" t="s">
         <v>4823</v>
       </c>
       <c r="B1077" s="2" t="s">
-        <v>4823</v>
+        <v>5109</v>
       </c>
       <c r="C1077" s="2"/>
       <c r="F1077" s="2"/>
       <c r="G1077" s="2"/>
     </row>
     <row r="1078" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1078" s="2" t="s">
+      <c r="A1078" s="6" t="s">
         <v>4824</v>
       </c>
       <c r="B1078" s="2" t="s">
-        <v>4824</v>
+        <v>5109</v>
       </c>
       <c r="C1078" s="2"/>
       <c r="F1078" s="2"/>
@@ -27935,22 +27991,22 @@
       <c r="G1084" s="2"/>
     </row>
     <row r="1085" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1085" s="2" t="s">
+      <c r="A1085" s="6" t="s">
         <v>4831</v>
       </c>
       <c r="B1085" s="2" t="s">
-        <v>4831</v>
+        <v>5109</v>
       </c>
       <c r="C1085" s="2"/>
       <c r="F1085" s="2"/>
       <c r="G1085" s="2"/>
     </row>
     <row r="1086" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1086" s="2" t="s">
+      <c r="A1086" s="6" t="s">
         <v>4832</v>
       </c>
       <c r="B1086" s="2" t="s">
-        <v>4832</v>
+        <v>5109</v>
       </c>
       <c r="C1086" s="2"/>
       <c r="F1086" s="2"/>
@@ -28066,11 +28122,11 @@
       <c r="G1096" s="2"/>
     </row>
     <row r="1097" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1097" s="2" t="s">
+      <c r="A1097" s="6" t="s">
         <v>4843</v>
       </c>
       <c r="B1097" s="2" t="s">
-        <v>4843</v>
+        <v>5109</v>
       </c>
       <c r="C1097" s="2"/>
       <c r="F1097" s="2"/>
@@ -28081,7 +28137,7 @@
         <v>4844</v>
       </c>
       <c r="B1098" s="2" t="s">
-        <v>4844</v>
+        <v>5109</v>
       </c>
       <c r="C1098" s="2"/>
       <c r="F1098" s="2"/>
@@ -28099,11 +28155,11 @@
       <c r="G1099" s="2"/>
     </row>
     <row r="1100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1100" s="2" t="s">
+      <c r="A1100" s="6" t="s">
         <v>4846</v>
       </c>
       <c r="B1100" s="2" t="s">
-        <v>4846</v>
+        <v>5109</v>
       </c>
       <c r="C1100" s="2"/>
       <c r="F1100" s="2"/>
@@ -28426,23 +28482,23 @@
       <c r="F1129" s="2"/>
       <c r="G1129" s="2"/>
     </row>
-    <row r="1130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1130" s="2" t="s">
+    <row r="1130" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1130" s="6" t="s">
         <v>4865</v>
       </c>
       <c r="B1130" s="2" t="s">
-        <v>4865</v>
+        <v>5114</v>
       </c>
       <c r="C1130" s="2"/>
       <c r="F1130" s="2"/>
       <c r="G1130" s="2"/>
     </row>
-    <row r="1131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1131" s="2" t="s">
+    <row r="1131" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1131" s="6" t="s">
         <v>4866</v>
       </c>
       <c r="B1131" s="2" t="s">
-        <v>4866</v>
+        <v>5114</v>
       </c>
       <c r="C1131" s="2"/>
       <c r="F1131" s="2"/>
@@ -30850,10 +30906,10 @@
       <c r="G1348" s="2"/>
     </row>
     <row r="1349" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1349" s="2" t="s">
+      <c r="A1349" s="6" t="s">
         <v>589</v>
       </c>
-      <c r="B1349" s="2" t="s">
+      <c r="B1349" s="6" t="s">
         <v>589</v>
       </c>
       <c r="C1349" s="2"/>
@@ -30882,12 +30938,12 @@
       <c r="F1351" s="2"/>
       <c r="G1351" s="2"/>
     </row>
-    <row r="1352" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1352" s="2" t="s">
+    <row r="1352" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1352" s="6" t="s">
         <v>583</v>
       </c>
       <c r="B1352" s="2" t="s">
-        <v>583</v>
+        <v>5108</v>
       </c>
       <c r="C1352" s="2"/>
       <c r="F1352" s="2"/>
@@ -30937,23 +30993,23 @@
       <c r="F1356" s="2"/>
       <c r="G1356" s="2"/>
     </row>
-    <row r="1357" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1357" s="2" t="s">
+    <row r="1357" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1357" s="6" t="s">
         <v>580</v>
       </c>
       <c r="B1357" s="2" t="s">
-        <v>580</v>
+        <v>5108</v>
       </c>
       <c r="C1357" s="2"/>
       <c r="F1357" s="2"/>
       <c r="G1357" s="2"/>
     </row>
-    <row r="1358" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1358" s="2" t="s">
+    <row r="1358" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1358" s="6" t="s">
         <v>586</v>
       </c>
       <c r="B1358" s="2" t="s">
-        <v>586</v>
+        <v>5108</v>
       </c>
       <c r="C1358" s="2"/>
       <c r="F1358" s="2"/>
@@ -38745,122 +38801,122 @@
       <c r="F2060" s="2"/>
       <c r="G2060" s="2"/>
     </row>
-    <row r="2061" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2061" s="2" t="s">
+    <row r="2061" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2061" s="6" t="s">
         <v>1130</v>
       </c>
       <c r="B2061" s="2" t="s">
-        <v>1130</v>
+        <v>5117</v>
       </c>
       <c r="C2061" s="2"/>
       <c r="F2061" s="2"/>
       <c r="G2061" s="2"/>
     </row>
-    <row r="2062" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2062" s="2" t="s">
+    <row r="2062" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2062" s="6" t="s">
         <v>1122</v>
       </c>
       <c r="B2062" s="2" t="s">
-        <v>1122</v>
+        <v>5118</v>
       </c>
       <c r="C2062" s="2"/>
       <c r="F2062" s="2"/>
       <c r="G2062" s="2"/>
     </row>
-    <row r="2063" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2063" s="2" t="s">
+    <row r="2063" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2063" s="6" t="s">
         <v>1128</v>
       </c>
       <c r="B2063" s="2" t="s">
-        <v>1128</v>
+        <v>5117</v>
       </c>
       <c r="C2063" s="2"/>
       <c r="F2063" s="2"/>
       <c r="G2063" s="2"/>
     </row>
-    <row r="2064" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2064" s="2" t="s">
+    <row r="2064" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2064" s="6" t="s">
         <v>1126</v>
       </c>
       <c r="B2064" s="2" t="s">
-        <v>1126</v>
+        <v>5118</v>
       </c>
       <c r="C2064" s="2"/>
       <c r="F2064" s="2"/>
       <c r="G2064" s="2"/>
     </row>
-    <row r="2065" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2065" s="2" t="s">
+    <row r="2065" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2065" s="6" t="s">
         <v>1118</v>
       </c>
       <c r="B2065" s="2" t="s">
-        <v>1118</v>
+        <v>5118</v>
       </c>
       <c r="C2065" s="2"/>
       <c r="F2065" s="2"/>
       <c r="G2065" s="2"/>
     </row>
-    <row r="2066" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2066" s="2" t="s">
+    <row r="2066" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2066" s="6" t="s">
         <v>1124</v>
       </c>
       <c r="B2066" s="2" t="s">
-        <v>1124</v>
+        <v>5118</v>
       </c>
       <c r="C2066" s="2"/>
       <c r="F2066" s="2"/>
       <c r="G2066" s="2"/>
     </row>
-    <row r="2067" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2067" s="2" t="s">
+    <row r="2067" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2067" s="6" t="s">
         <v>1345</v>
       </c>
       <c r="B2067" s="2" t="s">
-        <v>1345</v>
+        <v>5118</v>
       </c>
       <c r="C2067" s="2"/>
       <c r="F2067" s="2"/>
       <c r="G2067" s="2"/>
     </row>
-    <row r="2068" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2068" s="2" t="s">
+    <row r="2068" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2068" s="6" t="s">
         <v>1132</v>
       </c>
       <c r="B2068" s="2" t="s">
-        <v>1132</v>
+        <v>5117</v>
       </c>
       <c r="C2068" s="2"/>
       <c r="F2068" s="2"/>
       <c r="G2068" s="2"/>
     </row>
-    <row r="2069" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2069" s="2" t="s">
+    <row r="2069" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2069" s="6" t="s">
         <v>1134</v>
       </c>
       <c r="B2069" s="2" t="s">
-        <v>1134</v>
+        <v>5117</v>
       </c>
       <c r="C2069" s="2"/>
       <c r="F2069" s="2"/>
       <c r="G2069" s="2"/>
     </row>
-    <row r="2070" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2070" s="2" t="s">
+    <row r="2070" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2070" s="6" t="s">
         <v>1347</v>
       </c>
       <c r="B2070" s="2" t="s">
-        <v>1347</v>
+        <v>5118</v>
       </c>
       <c r="C2070" s="2"/>
       <c r="F2070" s="2"/>
       <c r="G2070" s="2"/>
     </row>
-    <row r="2071" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2071" s="2" t="s">
+    <row r="2071" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2071" s="6" t="s">
         <v>1120</v>
       </c>
       <c r="B2071" s="2" t="s">
-        <v>1120</v>
+        <v>5118</v>
       </c>
       <c r="C2071" s="2"/>
       <c r="F2071" s="2"/>
@@ -38888,12 +38944,12 @@
       <c r="F2073" s="2"/>
       <c r="G2073" s="2"/>
     </row>
-    <row r="2074" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2074" s="2" t="s">
+    <row r="2074" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2074" s="6" t="s">
         <v>572</v>
       </c>
       <c r="B2074" s="2" t="s">
-        <v>572</v>
+        <v>5107</v>
       </c>
       <c r="C2074" s="2"/>
       <c r="F2074" s="2"/>
@@ -38921,331 +38977,331 @@
       <c r="F2076" s="2"/>
       <c r="G2076" s="2"/>
     </row>
-    <row r="2077" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2077" s="2" t="s">
+    <row r="2077" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2077" s="6" t="s">
         <v>573</v>
       </c>
       <c r="B2077" s="2" t="s">
-        <v>573</v>
+        <v>5108</v>
       </c>
       <c r="C2077" s="2"/>
       <c r="F2077" s="2"/>
       <c r="G2077" s="2"/>
     </row>
     <row r="2078" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2078" s="2" t="s">
+      <c r="A2078" s="6" t="s">
         <v>575</v>
       </c>
       <c r="B2078" s="2" t="s">
-        <v>575</v>
+        <v>5110</v>
       </c>
       <c r="C2078" s="2"/>
       <c r="F2078" s="2"/>
       <c r="G2078" s="2"/>
     </row>
-    <row r="2079" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2079" s="2" t="s">
+    <row r="2079" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2079" s="6" t="s">
         <v>1342</v>
       </c>
       <c r="B2079" s="2" t="s">
-        <v>1342</v>
+        <v>5112</v>
       </c>
       <c r="C2079" s="2"/>
       <c r="F2079" s="2"/>
       <c r="G2079" s="2"/>
     </row>
-    <row r="2080" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2080" s="2" t="s">
+    <row r="2080" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2080" s="6" t="s">
         <v>600</v>
       </c>
       <c r="B2080" s="2" t="s">
-        <v>600</v>
+        <v>5113</v>
       </c>
       <c r="C2080" s="2"/>
       <c r="F2080" s="2"/>
       <c r="G2080" s="2"/>
     </row>
-    <row r="2081" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2081" s="2" t="s">
+    <row r="2081" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2081" s="6" t="s">
         <v>601</v>
       </c>
       <c r="B2081" s="2" t="s">
-        <v>601</v>
+        <v>5115</v>
       </c>
       <c r="C2081" s="2"/>
       <c r="F2081" s="2"/>
       <c r="G2081" s="2"/>
     </row>
-    <row r="2082" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2082" s="2" t="s">
+    <row r="2082" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2082" s="6" t="s">
         <v>1129</v>
       </c>
       <c r="B2082" s="2" t="s">
-        <v>1129</v>
+        <v>5116</v>
       </c>
       <c r="C2082" s="2"/>
       <c r="F2082" s="2"/>
       <c r="G2082" s="2"/>
     </row>
-    <row r="2083" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2083" s="2" t="s">
+    <row r="2083" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2083" s="6" t="s">
         <v>588</v>
       </c>
       <c r="B2083" s="2" t="s">
-        <v>588</v>
+        <v>5108</v>
       </c>
       <c r="C2083" s="2"/>
       <c r="F2083" s="2"/>
       <c r="G2083" s="2"/>
     </row>
     <row r="2084" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2084" s="2" t="s">
+      <c r="A2084" s="6" t="s">
         <v>590</v>
       </c>
       <c r="B2084" s="2" t="s">
-        <v>590</v>
+        <v>5110</v>
       </c>
       <c r="C2084" s="2"/>
       <c r="F2084" s="2"/>
       <c r="G2084" s="2"/>
     </row>
-    <row r="2085" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2085" s="2" t="s">
+    <row r="2085" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2085" s="6" t="s">
         <v>1121</v>
       </c>
       <c r="B2085" s="2" t="s">
-        <v>1121</v>
+        <v>5112</v>
       </c>
       <c r="C2085" s="2"/>
       <c r="F2085" s="2"/>
       <c r="G2085" s="2"/>
     </row>
-    <row r="2086" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2086" s="2" t="s">
+    <row r="2086" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2086" s="6" t="s">
         <v>597</v>
       </c>
       <c r="B2086" s="2" t="s">
-        <v>597</v>
+        <v>5113</v>
       </c>
       <c r="C2086" s="2"/>
       <c r="F2086" s="2"/>
       <c r="G2086" s="2"/>
     </row>
-    <row r="2087" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2087" s="2" t="s">
+    <row r="2087" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2087" s="6" t="s">
         <v>598</v>
       </c>
       <c r="B2087" s="2" t="s">
-        <v>598</v>
+        <v>5115</v>
       </c>
       <c r="C2087" s="2"/>
       <c r="F2087" s="2"/>
       <c r="G2087" s="2"/>
     </row>
-    <row r="2088" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2088" s="2" t="s">
+    <row r="2088" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2088" s="6" t="s">
         <v>1127</v>
       </c>
       <c r="B2088" s="2" t="s">
-        <v>1127</v>
+        <v>5116</v>
       </c>
       <c r="C2088" s="2"/>
       <c r="F2088" s="2"/>
       <c r="G2088" s="2"/>
     </row>
-    <row r="2089" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2089" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A2089" s="2" t="s">
         <v>594</v>
       </c>
       <c r="B2089" s="2" t="s">
-        <v>594</v>
+        <v>5108</v>
       </c>
       <c r="C2089" s="2"/>
       <c r="F2089" s="2"/>
       <c r="G2089" s="2"/>
     </row>
     <row r="2090" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2090" s="2" t="s">
+      <c r="A2090" s="6" t="s">
         <v>596</v>
       </c>
       <c r="B2090" s="2" t="s">
-        <v>596</v>
+        <v>5110</v>
       </c>
       <c r="C2090" s="2"/>
       <c r="F2090" s="2"/>
       <c r="G2090" s="2"/>
     </row>
-    <row r="2091" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2091" s="2" t="s">
+    <row r="2091" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2091" s="6" t="s">
         <v>1125</v>
       </c>
       <c r="B2091" s="2" t="s">
-        <v>1125</v>
+        <v>5111</v>
       </c>
       <c r="C2091" s="2"/>
       <c r="F2091" s="2"/>
       <c r="G2091" s="2"/>
     </row>
-    <row r="2092" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2092" s="2" t="s">
+    <row r="2092" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2092" s="6" t="s">
         <v>582</v>
       </c>
       <c r="B2092" s="2" t="s">
-        <v>582</v>
+        <v>5108</v>
       </c>
       <c r="C2092" s="2"/>
       <c r="F2092" s="2"/>
       <c r="G2092" s="2"/>
     </row>
     <row r="2093" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2093" s="2" t="s">
+      <c r="A2093" s="6" t="s">
         <v>584</v>
       </c>
       <c r="B2093" s="2" t="s">
-        <v>584</v>
+        <v>5110</v>
       </c>
       <c r="C2093" s="2"/>
       <c r="F2093" s="2"/>
       <c r="G2093" s="2"/>
     </row>
-    <row r="2094" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2094" s="2" t="s">
+    <row r="2094" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2094" s="6" t="s">
         <v>1117</v>
       </c>
       <c r="B2094" s="2" t="s">
-        <v>1117</v>
+        <v>5112</v>
       </c>
       <c r="C2094" s="2"/>
       <c r="F2094" s="2"/>
       <c r="G2094" s="2"/>
     </row>
-    <row r="2095" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2095" s="2" t="s">
+    <row r="2095" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2095" s="6" t="s">
         <v>591</v>
       </c>
       <c r="B2095" s="2" t="s">
-        <v>591</v>
+        <v>5108</v>
       </c>
       <c r="C2095" s="2"/>
       <c r="F2095" s="2"/>
       <c r="G2095" s="2"/>
     </row>
     <row r="2096" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2096" s="2" t="s">
+      <c r="A2096" s="6" t="s">
         <v>593</v>
       </c>
       <c r="B2096" s="2" t="s">
-        <v>593</v>
+        <v>5110</v>
       </c>
       <c r="C2096" s="2"/>
       <c r="F2096" s="2"/>
       <c r="G2096" s="2"/>
     </row>
-    <row r="2097" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2097" s="2" t="s">
+    <row r="2097" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2097" s="6" t="s">
         <v>1123</v>
       </c>
       <c r="B2097" s="2" t="s">
-        <v>1123</v>
+        <v>5112</v>
       </c>
       <c r="C2097" s="2"/>
       <c r="F2097" s="2"/>
       <c r="G2097" s="2"/>
     </row>
-    <row r="2098" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2098" s="2" t="s">
+    <row r="2098" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2098" s="6" t="s">
         <v>576</v>
       </c>
       <c r="B2098" s="2" t="s">
-        <v>576</v>
+        <v>5108</v>
       </c>
       <c r="C2098" s="2"/>
       <c r="F2098" s="2"/>
       <c r="G2098" s="2"/>
     </row>
     <row r="2099" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2099" s="2" t="s">
+      <c r="A2099" s="6" t="s">
         <v>578</v>
       </c>
       <c r="B2099" s="2" t="s">
-        <v>578</v>
+        <v>5110</v>
       </c>
       <c r="C2099" s="2"/>
       <c r="F2099" s="2"/>
       <c r="G2099" s="2"/>
     </row>
-    <row r="2100" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2100" s="2" t="s">
+    <row r="2100" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2100" s="6" t="s">
         <v>1344</v>
       </c>
       <c r="B2100" s="2" t="s">
-        <v>1344</v>
+        <v>5112</v>
       </c>
       <c r="C2100" s="2"/>
       <c r="F2100" s="2"/>
       <c r="G2100" s="2"/>
     </row>
-    <row r="2101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2101" s="2" t="s">
+    <row r="2101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2101" s="6" t="s">
         <v>603</v>
       </c>
       <c r="B2101" s="2" t="s">
-        <v>603</v>
+        <v>5113</v>
       </c>
       <c r="C2101" s="2"/>
       <c r="F2101" s="2"/>
       <c r="G2101" s="2"/>
     </row>
-    <row r="2102" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2102" s="2" t="s">
+    <row r="2102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2102" s="6" t="s">
         <v>604</v>
       </c>
       <c r="B2102" s="2" t="s">
-        <v>604</v>
+        <v>5115</v>
       </c>
       <c r="C2102" s="2"/>
       <c r="F2102" s="2"/>
       <c r="G2102" s="2"/>
     </row>
-    <row r="2103" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2103" s="2" t="s">
+    <row r="2103" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2103" s="6" t="s">
         <v>1131</v>
       </c>
       <c r="B2103" s="2" t="s">
-        <v>1131</v>
+        <v>5116</v>
       </c>
       <c r="C2103" s="2"/>
       <c r="F2103" s="2"/>
       <c r="G2103" s="2"/>
     </row>
-    <row r="2104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2104" s="2" t="s">
+    <row r="2104" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2104" s="6" t="s">
         <v>606</v>
       </c>
       <c r="B2104" s="2" t="s">
-        <v>606</v>
+        <v>5113</v>
       </c>
       <c r="C2104" s="2"/>
       <c r="F2104" s="2"/>
       <c r="G2104" s="2"/>
     </row>
-    <row r="2105" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2105" s="2" t="s">
+    <row r="2105" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2105" s="6" t="s">
         <v>607</v>
       </c>
       <c r="B2105" s="2" t="s">
-        <v>607</v>
+        <v>5115</v>
       </c>
       <c r="C2105" s="2"/>
       <c r="F2105" s="2"/>
       <c r="G2105" s="2"/>
     </row>
-    <row r="2106" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2106" s="2" t="s">
+    <row r="2106" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2106" s="6" t="s">
         <v>1133</v>
       </c>
       <c r="B2106" s="2" t="s">
-        <v>1133</v>
+        <v>5116</v>
       </c>
       <c r="C2106" s="2"/>
       <c r="F2106" s="2"/>
@@ -39274,44 +39330,44 @@
       <c r="G2108" s="2"/>
     </row>
     <row r="2109" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2109" s="2" t="s">
+      <c r="A2109" s="6" t="s">
         <v>581</v>
       </c>
       <c r="B2109" s="2" t="s">
-        <v>581</v>
+        <v>5110</v>
       </c>
       <c r="C2109" s="2"/>
       <c r="F2109" s="2"/>
       <c r="G2109" s="2"/>
     </row>
     <row r="2110" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2110" s="2" t="s">
+      <c r="A2110" s="6" t="s">
         <v>587</v>
       </c>
       <c r="B2110" s="2" t="s">
-        <v>587</v>
+        <v>5110</v>
       </c>
       <c r="C2110" s="2"/>
       <c r="F2110" s="2"/>
       <c r="G2110" s="2"/>
     </row>
-    <row r="2111" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2111" s="2" t="s">
+    <row r="2111" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2111" s="6" t="s">
         <v>1346</v>
       </c>
       <c r="B2111" s="2" t="s">
-        <v>1346</v>
+        <v>5112</v>
       </c>
       <c r="C2111" s="2"/>
       <c r="F2111" s="2"/>
       <c r="G2111" s="2"/>
     </row>
-    <row r="2112" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2112" s="2" t="s">
+    <row r="2112" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2112" s="6" t="s">
         <v>1119</v>
       </c>
       <c r="B2112" s="2" t="s">
-        <v>1119</v>
+        <v>5112</v>
       </c>
       <c r="C2112" s="2"/>
       <c r="F2112" s="2"/>
@@ -67602,49 +67658,52 @@
   </sortState>
   <dataConsolidate/>
   <conditionalFormatting sqref="G3720">
-    <cfRule type="duplicateValues" dxfId="14" priority="70"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="72"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G1049:W1324 G1:W1044 G1046:W1047 G1326:W2774 G2776:W1048576">
-    <cfRule type="duplicateValues" dxfId="13" priority="119"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="121"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4557:A4602 A1049:A1324 A1046:A1047 A1326:A2774 A1:A1044 A4607:A4664 A4667:A1048576 A2776:A4555">
+    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4556">
+    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4603:A4606">
     <cfRule type="duplicateValues" dxfId="12" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4556">
+  <conditionalFormatting sqref="G1048:W1048">
     <cfRule type="duplicateValues" dxfId="11" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4603:A4606">
+  <conditionalFormatting sqref="A1048">
     <cfRule type="duplicateValues" dxfId="10" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1048:W1048">
+  <conditionalFormatting sqref="G1045:W1045">
     <cfRule type="duplicateValues" dxfId="9" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1048">
+  <conditionalFormatting sqref="A1045">
     <cfRule type="duplicateValues" dxfId="8" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1045:W1045">
+  <conditionalFormatting sqref="G1325:W1325">
     <cfRule type="duplicateValues" dxfId="7" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1045">
+  <conditionalFormatting sqref="A1325">
     <cfRule type="duplicateValues" dxfId="6" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1325:W1325">
+  <conditionalFormatting sqref="A4665">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1325">
+  <conditionalFormatting sqref="A4666">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4665">
+  <conditionalFormatting sqref="G2775:W2775">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4666">
+  <conditionalFormatting sqref="A2775">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2775:W2775">
+  <conditionalFormatting sqref="B1349">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2775">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Giải thích Phá quân đắc địa
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{ECBC450F-FB0C-4264-990D-97DFE20165CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93ECAE1-72EF-493A-A139-7921F56E82F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$G$4606</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9673" uniqueCount="5145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9681" uniqueCount="5148">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -15489,6 +15488,15 @@
   </si>
   <si>
     <t>Thân cư Quan Lộc có Thất Sát tọa thủ và gặp Kình Dương, Đà La, Hoả Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Bạn là Bạn có cuộc sống sang giàu, quyền uy. Thân hình đẫy đà, cao vừa tầm da hồng hào, mặt đầy đặn, mắt lộ, hầu lộ, lông mày thưa.</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Mệnh ở Sửu</t>
+  </si>
+  <si>
+    <t>Bạn là người thông minh, cương quả, hiếu thắng, tự đắc, có thủ đoạn, có tài thao lược, lại can đảm, dũng mãnh, ưa hoạt động, thích đi xa, thể thao cảm giác mạnh.</t>
   </si>
 </sst>
 </file>
@@ -15569,7 +15577,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -16056,10 +16074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A2:G4698"/>
+  <dimension ref="A2:G4699"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4618" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B4695" sqref="B4695"/>
+    <sheetView tabSelected="1" topLeftCell="A1178" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C1180" sqref="C1180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29129,14 +29147,16 @@
       <c r="F1177" s="2"/>
       <c r="G1177" s="2"/>
     </row>
-    <row r="1178" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1178" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A1178" s="2" t="s">
         <v>613</v>
       </c>
       <c r="B1178" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="C1178" s="2"/>
+        <v>5145</v>
+      </c>
+      <c r="C1178" s="2" t="s">
+        <v>5147</v>
+      </c>
       <c r="F1178" s="2"/>
       <c r="G1178" s="2"/>
     </row>
@@ -29173,14 +29193,16 @@
       <c r="F1181" s="2"/>
       <c r="G1181" s="2"/>
     </row>
-    <row r="1182" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1182" s="2" t="s">
+    <row r="1182" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1182" s="6" t="s">
         <v>611</v>
       </c>
       <c r="B1182" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="C1182" s="2"/>
+        <v>5145</v>
+      </c>
+      <c r="C1182" s="2" t="s">
+        <v>5147</v>
+      </c>
       <c r="F1182" s="2"/>
       <c r="G1182" s="2"/>
     </row>
@@ -29206,14 +29228,16 @@
       <c r="F1184" s="2"/>
       <c r="G1184" s="2"/>
     </row>
-    <row r="1185" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1185" s="2" t="s">
+    <row r="1185" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1185" s="6" t="s">
         <v>612</v>
       </c>
       <c r="B1185" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="C1185" s="2"/>
+        <v>5145</v>
+      </c>
+      <c r="C1185" s="2" t="s">
+        <v>5147</v>
+      </c>
       <c r="F1185" s="2"/>
       <c r="G1185" s="2"/>
     </row>
@@ -29294,14 +29318,16 @@
       <c r="F1192" s="2"/>
       <c r="G1192" s="2"/>
     </row>
-    <row r="1193" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1193" s="2" t="s">
+    <row r="1193" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1193" s="6" t="s">
         <v>614</v>
       </c>
       <c r="B1193" s="2" t="s">
-        <v>4880</v>
-      </c>
-      <c r="C1193" s="2"/>
+        <v>5145</v>
+      </c>
+      <c r="C1193" s="2" t="s">
+        <v>5147</v>
+      </c>
       <c r="F1193" s="2"/>
       <c r="G1193" s="2"/>
     </row>
@@ -29338,14 +29364,16 @@
       <c r="F1196" s="2"/>
       <c r="G1196" s="2"/>
     </row>
-    <row r="1197" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1197" s="2" t="s">
+    <row r="1197" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1197" s="6" t="s">
         <v>615</v>
       </c>
       <c r="B1197" s="2" t="s">
-        <v>4880</v>
-      </c>
-      <c r="C1197" s="2"/>
+        <v>5145</v>
+      </c>
+      <c r="C1197" s="2" t="s">
+        <v>5147</v>
+      </c>
       <c r="F1197" s="2"/>
       <c r="G1197" s="2"/>
     </row>
@@ -29382,14 +29410,16 @@
       <c r="F1200" s="2"/>
       <c r="G1200" s="2"/>
     </row>
-    <row r="1201" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1201" s="2" t="s">
+    <row r="1201" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A1201" s="6" t="s">
         <v>610</v>
       </c>
       <c r="B1201" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="C1201" s="2"/>
+        <v>5145</v>
+      </c>
+      <c r="C1201" s="2" t="s">
+        <v>5147</v>
+      </c>
       <c r="F1201" s="2"/>
       <c r="G1201" s="2"/>
     </row>
@@ -67872,6 +67902,14 @@
       </c>
       <c r="B4698" s="2" t="s">
         <v>5138</v>
+      </c>
+    </row>
+    <row r="4699" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4699" s="6" t="s">
+        <v>5146</v>
+      </c>
+      <c r="B4699" s="2" t="s">
+        <v>5145</v>
       </c>
     </row>
   </sheetData>
@@ -67881,66 +67919,69 @@
   </sortState>
   <dataConsolidate/>
   <conditionalFormatting sqref="G3720">
-    <cfRule type="duplicateValues" dxfId="20" priority="79"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="80"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2776:W1048576 G1049:W1324 G1:W1044 G1046:W1047 G1326:W2774">
-    <cfRule type="duplicateValues" dxfId="19" priority="128"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="129"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4556">
+    <cfRule type="duplicateValues" dxfId="19" priority="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4603:A4606">
     <cfRule type="duplicateValues" dxfId="18" priority="21"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4603:A4606">
+  <conditionalFormatting sqref="G1048:W1048">
     <cfRule type="duplicateValues" dxfId="17" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1048:W1048">
+  <conditionalFormatting sqref="A1048">
     <cfRule type="duplicateValues" dxfId="16" priority="19"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1048">
+  <conditionalFormatting sqref="G1045:W1045">
     <cfRule type="duplicateValues" dxfId="15" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1045:W1045">
+  <conditionalFormatting sqref="A1045">
     <cfRule type="duplicateValues" dxfId="14" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1045">
+  <conditionalFormatting sqref="G1325:W1325">
     <cfRule type="duplicateValues" dxfId="13" priority="16"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G1325:W1325">
+  <conditionalFormatting sqref="A1325">
     <cfRule type="duplicateValues" dxfId="12" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1325">
+  <conditionalFormatting sqref="A4665">
     <cfRule type="duplicateValues" dxfId="11" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4665">
+  <conditionalFormatting sqref="A4666">
     <cfRule type="duplicateValues" dxfId="10" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4666">
+  <conditionalFormatting sqref="G2775:W2775">
     <cfRule type="duplicateValues" dxfId="9" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2775:W2775">
+  <conditionalFormatting sqref="A2775">
     <cfRule type="duplicateValues" dxfId="8" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2775">
-    <cfRule type="duplicateValues" dxfId="7" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4557:A4602 A1049:A1324 A1046:A1047 A1:A1044 A4607:A4664 A2776:A4555 A4667:A4693 A2114:A2774 A1326:A2112 A4699:A1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="142"/>
+  <conditionalFormatting sqref="A4557:A4602 A1049:A1324 A1046:A1047 A1:A1044 A4607:A4664 A2776:A4555 A4667:A4693 A2114:A2774 A1326:A2112 A4700:A1048576">
+    <cfRule type="duplicateValues" dxfId="7" priority="143"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2113">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4694">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4694">
+  <conditionalFormatting sqref="A4695">
     <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4695">
+  <conditionalFormatting sqref="A4696">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4696">
+  <conditionalFormatting sqref="A4697">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4697">
+  <conditionalFormatting sqref="A4698">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A4698">
+  <conditionalFormatting sqref="A4699">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Giải thích xong tài bạch
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App_Tuvi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8105C39A-1275-4825-9F86-555EA956D413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455E2E20-A23B-46F1-8A80-F759F82E038D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13656,8 +13656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
   <dimension ref="A2:G3697"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B236" sqref="B236"/>
+    <sheetView tabSelected="1" topLeftCell="A2333" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C2336" sqref="C2336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Giải thích quan lộc
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App_Tuvi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C914EF15-15C7-45CE-9541-D701E5484DB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE144C0-F874-44CE-AAAA-7256B237AEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13804,8 +13804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
   <dimension ref="A2:H3612"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A665" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C669" sqref="C669"/>
+    <sheetView tabSelected="1" topLeftCell="A880" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C884" sqref="C884"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Sửa lại Tả phù
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App_Tuvi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE144C0-F874-44CE-AAAA-7256B237AEE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B91AAB9-0990-45D6-BEFB-DE210B726414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13804,8 +13804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
   <dimension ref="A2:H3612"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A880" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C884" sqref="C884"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50689,7 +50689,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G3612" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B2867">
     <sortCondition ref="A2:A2867"/>
   </sortState>

</xml_diff>

<commit_message>
Giải thích vô chính diệu
</commit_message>
<xml_diff>
--- a/LuanMenh.xlsx
+++ b/LuanMenh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B5B40F-D130-4979-B67A-1B8233D4705C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8171D6D-BF75-4698-A32A-3B92A7A44B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10457,7 +10457,7 @@
   <dimension ref="A2:H2476"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2473" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2464" sqref="A2464:K2477"/>
+      <selection activeCell="B2480" sqref="B2480"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>